<commit_message>
GH ACTION Headlines Mon Nov 28 01:39:01 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,22 +473,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SSG 블랙 프라이데이</t>
+          <t>대한민국을 응원합니다</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>초강력 블프세일, 오늘은 득템 하는 날! ~12% 쿠폰</t>
+          <t>축구 국가대표팀 경기 당일, 10% 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002683</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003009</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[11/21-27] SSG 블랙프라이데이 - 인기 상품 최대의 혜택으로</t>
+          <t>대한민국을 응원합니다</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -498,76 +498,76 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-04</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [11/21-27] SSG 블랙프라이데이 - 인기 상품 최대의 혜택으로', '스마일클럽', '최대 ~80% 초강력 세일, 오늘은 득템하는 날!', '01. 선착순 최대 12% 블랙 쿠폰', '05. 최대 80% 초강력 클리어런스', '01. 선착순 블랙 쿠폰 최대 12% 쿠폰 최대 2만원 할인', '쿠폰 사용 전 꼭 확인하세요!', '        쿠폰 발급 기간', '        쿠폰 사용 기간', '        쿠폰 발급 후 11/27(일)까지', '        쿠폰 사용 조건', '        쿠폰 발급 대상', '스마일클럽 회원은 1장 더! 스마일클럽 전용 최대 2만원 쿠폰', '12% 장바구니 쿠폰 - 7만원 이상 구매시, 최대 2만원 할인(매일 오전 9시 선착순 8천명, Smile Club 전용)', '        2022년 11/21(월) ~ 11/27(일) (선착순 수량 종료시 쿠폰 마감될 수 있습니다)', '        본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '+PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '05. 매일매일 SSG에서 득템하세요 최대 80% 초강력 클리어런스', '80% 클리어런스 상품 더보기', 'SSG 스포츠 박람회 스포츠 전용 쿠폰으로 등산/아웃도어/캠핑/골프 스포츠웨어부터 용품까지! 자세히 보기', '건강식품 전문관 바이오퍼블릭 그랜드 오픈 ~20% 쿠폰, 1+1 오픈 특가! 이제는 SSG.COM에서 건강식품을 구매하세요 자세히 보기', '스마일클럽 가입 고객에게만 제공되는 혜택입니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 대한민국을 응원합니다', '스마일클럽', '국가대표팀 경기 당일 오전 9시 선착순 쿠폰 제공', '10% 장바구니 쿠폰 - 선착순 3만장', '10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰이 마감되었습니다', '발급 방식 : 기간 내 ID당 1회씩 발급 (선착순 3만장)', "발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다."]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>29th 창립기념 오반장 위시리스트</t>
+          <t>공공남매가 SSG.COM 인스타그램을 해킹했다!</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11월 위시템 최대 50%! 10만원 장보기 지원금까지</t>
+          <t>무물 질문하고 친필 사인, 다이슨 에어랩, 하만카돈 스피커도 받아가세요.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002932</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[11/17-27] 창립기념 오반장 위시리스트</t>
+          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-11-17</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [11/17-27] 창립기념 오반장 위시리스트', '스마일클럽', '11월 위시템 최대50% 최대 10만원 장보기 지원금까지!', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '쓱- 무물 SNS 댓글 이벤트', '                  모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.', '쓱배송, 만사오케이']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>대한민국, 승리를 위해</t>
+          <t>패피혁님들</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>축구 국가대표팀 경기 당일, 10% 할인쿠폰 제공</t>
+          <t>핏 터지는 1:1 스타일링 배틀</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003009</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003140</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>대한민국, 승리를 위해!</t>
+          <t>[1128~1204] 패피혁님들 EP.5 '연말 파티 스타일링 대결'</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -577,29 +577,29 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 대한민국, 승리를 위해!', '스마일클럽', '승리 기원 쿠폰', 'SSGMONEY 제공', '응원 댓글 이벤트', '국가대표팀 경기 당일 오전 9시 선착순 쿠폰 제공', '10% 장바구니 쿠폰 - 선착순 3만장', '10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰이 마감되었습니다', '발급 방식 : 기간 내 ID당 1회씩 발급 (선착순 3만장)', "발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '에어랩, 기본 배럴보다 50% 더 긴 롱 배럴', '실감나는 VR로 본다, 피코4 다양한 이벤트', '커피머신 판촉할인 앵콜행사', '승리 기원 응원 댓글 이벤트', '사용 대상 : SSG.COM 전체 상품 (단, 일부 특가, 여행/쿠폰 등 서비스 상품, 환금성 카테고리 제외)', 'SSGMONEY는 당첨 즉시 지급되어 지급일로부터 30일간 사용 가능하며, 기간 경과 후 자동 소멸됩니다.', '전용 쿠폰으로 겨울 스포츠 즐길 준비!']</t>
+          <t>["이벤트/쿠폰 &gt; [1128~1204] 패피혁님들 EP.5 '연말 파티 스타일링 대결'", '스마일클럽', "그 동안의 소감을 담아 댓글을 남겨 주시면 추첨을 통해 영상 속 스타일링 제품을 드립니다 +♥사심 가득♥ 혁님의 특별 애장품과 폴라로이드 사진은 보너스!(자세한 이벤트 내용은 '패피혁님들 5화 유튜브 영상 더보기란'에서 확인하세요)"]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SSG 스포츠 박람회</t>
+          <t>신세계 리빙 셀렉샵 오픈</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>역대급 할인에 쿠폰 받아 ~2만원 추가 할인까지!</t>
+          <t>백화점 리빙 7% 쿠폰 + 뱅앤올룹슨/아르떼미데 外 경품 이벤트</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003013</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003007</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[11/21~27] SSG 스포츠 박람회</t>
+          <t>Shinsegae Living Select Shop</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -609,602 +609,380 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-04</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [11/21~27] SSG 스포츠 박람회', '스마일클럽', '#1. 스포츠 카테고리 최대 2만원 할인', '#1. 매일 오전 9시, 10% 쿠폰 다운받아 최대 2만원 할인! 스포츠 박람회 전용 쿠폰', '선착순 1만명', '오늘의 쿠폰은 마감되었습니다.', '      쿠폰 발급 기간', '      쿠폰 사용 기간', '      쿠폰 발급 후 11/27(일)까지', '      쿠폰 사용 조건', '      본 쿠폰은 신세계몰, 신세계백화점 스포츠 카테고리 상품에만 적용되는 카테고리 쿠폰입니다.', '      쿠폰 발급 대상', '나이키 NIKE - FW 스포츠웨어/슈즈 인기상품 모음전! UP TO 44%', '블랙야크 스페셜 위크 - 아이유 착용 상품 FW 아우터 최대 70% 할인', '스위스 프리미엄 스포츠 브랜드 ON - 이월상품 최대 50% 할인', '데카트론 FW 야외스포츠 - 트래킹/자전거/캠핑 등 최대 40% 할인', 'SSG 블랙 프라이데이 최대 12% 쿠폰으로 SSG에서 인기 상품을 저렴하게!']</t>
+          <t>['이벤트/쿠폰 &gt; Shinsegae Living Select Shop', '스마일클럽', '백화점 리빙 7% 쿠폰 바로보기', 'SNS 소문내기 경품 이벤트 바로보기', '할인으로 더 가깝게 만나는 프리미엄 리빙 7% COUPON', '      7% 장바구니 쿠폰', '      선착순 1,500명', '      7만원 이상 결제 시, 최대 1만 5천원 할인', '쿠폰 발급 및 사용기간: 2022년 11월 21일 (월) 00:00 ~ 12월 4일 (일) 23:59', '쿠폰 발급 후 MY SSG &gt; 쿠폰 &gt; 보유쿠폰에서 확인 가능', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '리빙 셀렉샵 소문내기 이벤트', '이벤트 참여 방법', '1. 이벤트 페이지 캡쳐 및 URL을 복사해서 SNS에 공유해주세요.', '       이벤트 기간', "       SSG.COM 이벤트&amp;쿠폰 '당첨자 발표' 게시판", '본 이벤트는 ID별로 1회 참여할 수 있으며, 부정한 방법으로 참여한 것이 발견될 경우 당첨이 취소될 수 있습니다.', '댓글 입력 후 SNS 공유글을 삭제한 경우 이벤트 당첨자 명단에서 자동 제외됩니다.', '이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다. (개인 정보 위탁업체 : (주)젤라블루코리아, 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호, 주소)', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>W컨셉 브랜드 쇼케이스</t>
+          <t>캡틴쓱 : 게임 체인저</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Welcome W컨셉 To SSG, 12% 쿠폰 혜택 찬스!</t>
+          <t>친환경 인식 개선 캠페인</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003008</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003079</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(11/21~27) W컨셉 브랜드 쇼케이스</t>
+          <t>친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (11/21~27) W컨셉 브랜드 쇼케이스', '스마일클럽', '01 #SPECIAL OFFER 12% 쿠폰 바로보기', '#SPECIAL OFFER 12% 상품 쿠폰', '1만원 이상 구매시 최대 3만원 할인 기간 내 ID당 4장 발급 가능', '쿠폰 사용 전 꼭 확인하세요(레이어팝업 열기)', '쿠폰 사용 전 꼭 확인하세요!', '        쿠폰 발급 및 사용 기간', '        1만원 이상 상품 구매 시 12% 할인, 최대 3만원(기간내 ID당 발급수량 4장)', '        쿠폰 적용 방법', '        상품 상세에서 쿠폰 적용 여부를 확인하실 수 있습니다.', '        쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)']</t>
+          <t>['이벤트/쿠폰 &gt; 친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;', '스마일클럽', '전기차 쓱배송 차량 캐릭터 - 전기차 쓱카', '쓱배송 차량의 전기차 브로! 착실하고 우직한 성격으로 쓱배송을 전담하고 있다. 명석한 두뇌로 최적의 루트를 빠르게 분석한다.', '첫 번째 이벤트 - 메타버스 캡틴쓱 본부 내 모든 스테이지 참여 시 추첨을 통해 친환경 키트 혹은 신세계 모바일 상품권 5천원권', '두 번째 이벤트 - 스테이지 4에서 최단 기록 10명 대상으로 날마다 신세계 모바일 상품권 5천원권 증정', '세 번째 이벤트 - 보너스 스테이지 참여자 대상으로 추첨을 통해 스타벅스 기프트카드 1만원권 증정', ' 미션 종료 후 이벤트 참여 및 리워드 제공을 위해 테라사이클 코리아에서 개인정보를 수집할 수 있습니다. 자세한 이벤트 내용은 해당 스테이지 내 안내 문구를 참고해주세요. PC로 참여하시는 경우, 크롬 브라우저를 통해 입장해주시길 바랍니다. ', '       인스타그램 이벤트 계정에 들어가서 게시글을 눌러가며 힌트를 얻어 곰인형을 구해주세요. 마지막 단계에서 댓글 작성 시, 댓글 수에 따라 기부가 진행됩니다.', '자세한 이벤트 내용은 해당 게시글 내 안내 문구를 참고해주세요.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>건강전문관 바이오퍼블릭 오픈</t>
+          <t>2022 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>쏜리서치 1+1 오픈특가 /~ 20% 쿠폰 /  ~ 50% 브랜드별 할인</t>
+          <t>연말 이벤트전</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002986</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003149</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>건강 관리의 신세계- 바이오퍼블릭 전문관 OPEN! 1+1 부터 체험팩까지</t>
+          <t>(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-24</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 건강 관리의 신세계- 바이오퍼블릭 전문관 OPEN! 1+1 부터 체험팩까지', '스마일클럽', '#최대 20% 할인 쿠폰', '#~50% 브랜드별 할인', '#03 최대 20% 할인쿠폰 바로보기', '#05 최대 50% 브랜드별 할인 바로보기', '#06 체험팩 이벤트 바로보기', '#03. 쇼핑찬스 건강식품 최대 20% 할인', '매일 오전 9시 선착순 5천명 상품쿠폰 10% 1만 5천원 이상 구매시 최대 1만원 할인', '상품쿠폰 10% 다운 받기 (기간내 ID당 1회)', '오늘의 쿠폰은 마감되었습니다.', '매일 오전 9시 선착순 5천명 장바구니 쿠폰 15% 5만원 이상 구매시 최대 2만원 할인', '장바구니 쿠폰 15% 다운 받기 (기간내 ID당 1회)', '쿠폰 발급 및 유효기간: 22/11/21(월) ~ 22/11/27(일)', '쿠폰 사용 조건 : ', '상품쿠폰은 상품 1개 단품으로 적용 가능', '스마일클럽 멤버십 전용 쿠폰은 스마일클럽 회원만 발급 가능', '스마일클럽 회원은 더 큰 혜택! 20% 쿠폰', '매일 오전 9시 선착순 2천명, SmlieClub 전용', '장바구니 쿠폰 20% 다운 받기 (기간내 ID당 1회)', '본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '7만원 이상 구매 시 카드할인까지 잊지 말고 꼭 챙기세요!', '[SSGPAY전용] 신한카드 7만이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 7만이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 7만이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 7만이상 5% 청구할인 (일 5만원 한) 자세히 보기', '#05 최대 50% 브랜드별 할인 Biopublic', '누적판매 150만개 돌파! 이마트 건강식품 대표 브랜드 바이오퍼블릭 최대 50% 구매찬스', '최대 15% 할인 GNM 금액대별 &amp; 신상품 런칭 증정+할인 보러가기', '최대 50% 할인 덴프스 유산균부터 트루바이타민까지 보러가기', '최대 30% 할인 듀오락 베스트 유산균 슈퍼위크 보러가기', '최대 50% 할인 안국건강 루테인 4천원대 부터/비타민D 3천원대 부터 보러가기', '최대 37% 할인 CJ웰케어 건강 가을 특가 찬스 보러가기', '최대 15% 할인 종근당건강 다운 쿠폰 제공 보러가기', '최대 20% 할인 휴온스 박미선의 갱년기 유산균 보러가기', '최대 50% 할인 뉴트리원 오픈 축하 특가 보러가기', '최대 30% 할인 우리가족 맞춤형 비타민 세노비스 보러가기', '최대 30%할인! 듀오랩 입점 기념 브랜드위크 보러가기', '최대 50%할인! 농협헬스케어 체험팩 3일분 1,900원 외 보러가기', '#06. 오픈 기념 이벤트 체험팩 무료 증정', '이벤트 당첨 시, 기본배송지의 주소지와 연락처로 상품이 발송될 예정이오니, 기본배송지 정보를 반드시 확인하여 주시기 바랍니다.', '제공받은 상품으로 리뷰 용도 외 재판매 등은 엄격하게 제한되며, 적발 시 추후 이벤트 응모 및 당첨이 제한될 수 있습니다.', '법인회원 및 간편가입회원은 이벤트 응모 및 당첨이 제한될 수 있습니다.', '이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '이벤트 응모에 따른 개인정보 제공 동의 및 운영 방침 동의 안내입니다.', "본 이벤트에 응모하시는 경우 '회원 아이디, 성함, 이메일 주소, 휴대폰 번호, 기본 주소'가 제공되며, 제공된 개인 정보는 경품 제공의 목적 외에 사용되지 않음을 알려드립니다.", '제공된 개인 정보의 보유 및 이용 기간은 이벤트 종료 후 3개월입니다.', '[체험단] 이벤트 당첨자 발표 공지 후 개인 정보에 기재된 휴대폰 번호로 공지 및 연락을 드립니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '스마일클럽', '(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>패피위크: 니트웨어 A to Z</t>
+          <t>SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>따뜻한 니트웨어로 겨울 준비, SSG머니+ 럭키드로우 혜택까지!</t>
+          <t>이건 진짜 드라마다! WE ARE SSG랜더스!!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002909</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002943</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>(11/21~27) 패피위크: 니트웨어 A to Z</t>
+          <t>SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-09</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-11-30</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (11/21~27) 패피위크: 니트웨어 A to Z', '스마일클럽', 'SSG머니부터 경품까지! 더블 이벤트 바로보기', '11월에는 혜택도 1+1 더블 이벤트', '페이백 이벤트 참여 브랜드 상품 7만원 이상 구매 시 5천원 페이백! 참여 브랜드는 패션전문관 SSG STYLE 내 STYLE과 TREND 매장에서 확인하실 수있습니다.', '경품은 이벤트 응모 시 사용한 ID 회원정보 상의 휴대폰 번호와 기본 주소지 기준으로 발송되오니, 개인정보를 꼭 확인해 주세요.', '이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료 될 수 있습니다.', '대상 상품은 상품 상세 페이지 내 이벤트 엠블럼으로 확인 가능하며, STYLE 및 TREND 매장 내 브랜드 중에서 일부 브랜드 및 상품은 제외될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
+          <t>['이벤트/쿠폰 &gt; SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트', '스마일클럽', 'SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트', 'SSG닷컴 X SSG랜더스 첫 통합 우승 랜딩 축하 댓글 이벤트', '랜더스 팬 여러분들을 위해 준비한 이벤트 참여하고 다양한 경품 받아가세요!', '       이벤트 기간', '       이벤트 대상', '       이벤트 참여 방법', '       이벤트 페이지 하단에서 축하 댓글 작성 완료 시, 자동 응모됩니다.', "       2022년 12월 9일(금) * 'MY SSG - 이벤트 참여내역' 메뉴를 통해 확인 가능", '      이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '      부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '      이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '      SSG MONEY 지급안내', '      당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 30일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', '      SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>신세계 리빙 셀렉샵 오픈</t>
+          <t>스마일클럽의 스마트한 장보기</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>백화점 리빙 7% 쿠폰 + 뱅앤올룹슨/아르떼미데 外 경품 이벤트</t>
+          <t>월요일마다 최대 10% 더블적립!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003007</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Shinsegae Living Select Shop</t>
+          <t>[스마일클럽] 11월 내내 매일매일 스마일</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-14</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-12-04</t>
+          <t>2022-11-30</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Shinsegae Living Select Shop', '스마일클럽', '백화점 리빙 7% 쿠폰 바로보기', 'SNS 소문내기 경품 이벤트 바로보기', '할인으로 더 가깝게 만나는 프리미엄 리빙 7% COUPON', '      7% 장바구니 쿠폰', '      선착순 1,500명', '      7만원 이상 결제 시, 최대 1만 5천원 할인', '쿠폰 발급 및 사용기간: 2022년 11월 21일 (월) 00:00 ~ 12월 4일 (일) 23:59', '쿠폰 발급 후 MY SSG &gt; 쿠폰 &gt; 보유쿠폰에서 확인 가능', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '리빙 셀렉샵 소문내기 이벤트', '이벤트 참여 방법', '1. 이벤트 페이지 캡쳐 및 URL을 복사해서 SNS에 공유해주세요.', '       이벤트 기간', "       SSG.COM 이벤트&amp;쿠폰 '당첨자 발표' 게시판", '본 이벤트는 ID별로 1회 참여할 수 있으며, 부정한 방법으로 참여한 것이 발견될 경우 당첨이 취소될 수 있습니다.', '댓글 입력 후 SNS 공유글을 삭제한 경우 이벤트 당첨자 명단에서 자동 제외됩니다.', '이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다. (개인 정보 위탁업체 : (주)젤라블루코리아, 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호, 주소)', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 11월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 11월 내내 매일매일 스마일', '지금 스마일클럽 가입하고 모든 혜택 받기', '한달 내내 막강한 스마일클럽 혜택', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 즉시 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '2. 매주 월요일마다 장보기 최대 10% 더블적립 DAY', '스마일클럽 기본적립 + 월요일마다 추가 적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>먼데이문 컬러 포인트 메이크업</t>
+          <t>오르시떼 11/28(월) 11AM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>연말을 준비하는 뷰티 팁! SSG머니 1만원 페이백 혜택</t>
+          <t>패밀리 파자마 최대 65%OFF! SSG단독 다크체크/조이 선착순 핫딜</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002948</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003135</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>먼데이문 컬러 포인트 메이크업</t>
+          <t>[SSG.LIVE]11/28 오르시떼</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 먼데이문 컬러 포인트 메이크업', '스마일클럽', '[홀리데이 한정판][57% OFF] 치크 파티 패키지', 'SSG MONEY 페이백 응모하기', '신청방법 : 행사기간 중 대상 상품 2만원 이상 구매 후, 이벤트 페이지 신청하기 버튼 신청', '구매사은 대상금액은 지정된 구매사은의 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다.', "이벤트 참여 후 'MY SSG &gt; 이벤트 참여현황' 에서 참여 여부 확인이 가능합니다. ", '이벤트는 당사의 사정에 따라 변경/중단될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]11/28 오르시떼', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트</t>
+          <t>캐논 11/28(월) 8PM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>이건 진짜 드라마다! WE ARE SSG랜더스!!</t>
+          <t>EOS R6 MARK II 출시기념 최초공개 LIVE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002943</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003169</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트</t>
+          <t>캐논 @SSG.LIVE 11/28(월) 8PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-11-09</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트', '스마일클럽', 'SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트', 'SSG닷컴 X SSG랜더스 첫 통합 우승 랜딩 축하 댓글 이벤트', '랜더스 팬 여러분들을 위해 준비한 이벤트 참여하고 다양한 경품 받아가세요!', '       이벤트 기간', '       이벤트 대상', '       이벤트 참여 방법', '       이벤트 페이지 하단에서 축하 댓글 작성 완료 시, 자동 응모됩니다.', "       2022년 12월 9일(금) * 'MY SSG - 이벤트 참여내역' 메뉴를 통해 확인 가능", '      이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '      부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '      이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '      SSG MONEY 지급안내', '      당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 30일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', '      SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 캐논 @SSG.LIVE 11/28(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>창립기념 민지의 장바구니</t>
+          <t>플라스틱아일랜드 11/29(화) 7PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>장보기 꿀템 추천하고 SSG머니 받아가세요!</t>
+          <t>최대 66%↓인플루언서 젤라비PICK 겨울 아우터 6만원~</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003076</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003168</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>창립기념 민지의 장바구니 (11/21~11/27)</t>
+          <t>플라스틱 아일랜드 @SSG.LIVE 11/29(화) 7PM</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 창립기념 민지의 장바구니 (11/21~11/27)', '스마일클럽', '#최대 50%부터 n+1까지 해피해피 이마특가! 바로보기', '#최대 50%부터 n+1 특가까지', ' 2건 꼭 9매 해야지! 생각하는 장보기 꿀템을 민지들에게 추천해줘 ex) 이마트하면 피코크고 피코크는 역시 초콜릿 샌드위치 아니겠어? 한때 품절대란까지 났었던 슈스 그 잡채였다구... 지금은 쓱배송으로 클릭 한번이면 간편하게~ 쓱배송 9(고)마워 ', '        추첨을 통하여 민지 용돈 3천원 증정 - SSG MONEY 3천원 (300명)', "       'my SSG&gt;이벤트 현황&gt;이벤트 참여내역'에서 확인해주세요", '       ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '창립기념 장보기 구매지원금 증정 이벤트']</t>
+          <t>['이벤트/쿠폰 &gt; 플라스틱 아일랜드 @SSG.LIVE 11/29(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2022 대한민국 수산대전</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>연말 이벤트전</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003149</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-11-24</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '스마일클럽', '(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 3만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>스마일클럽은 SSG 블프에 더 큰 혜택!</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>바이오퍼블릭 오픈 기념 ~20% 선착순 쿠폰까지</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인 + ~68,900원 이달의 혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002938</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[스마일클럽] 11월 내내 매일매일 스마일</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-11-14</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 11월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 11월 내내 매일매일 스마일', '지금 스마일클럽 가입하고 모든 혜택 받기', '한달 내내 막강한 스마일클럽 혜택', '매주 달라지는 카테고리 할인 쿠폰', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 즉시 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '2. 매주 월요일마다 장보기 최대 10% 더블적립 DAY', '스마일클럽 기본적립 + 월요일마다 추가 적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', '3. 매주 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '쿠폰 받으러 가기', '오픈 기념 스마일클럽 추가 혜택', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.11.01 ~ 2022.11.30', '쿠폰 사용기간 : 2022.11.01 ~ 2022.11.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛 위크</t>
+          <t>11월 유행하는 유아동 상품</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11월 할인대전</t>
+          <t>잡지로 만나는 유아동소식 With 스타일러</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003096&amp;siteNo=7008</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002682</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[1121-1127] 프리미엄 아울렛 위크</t>
+          <t>[11/01-30] 11월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-01</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-11-30</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [1121-1127] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 11월 할인 대전', '최대 10% 할인 쿠폰 혜택', 'EVENT 03 아울렛 가격에 추가 할인이 더 카테고리별 특가전', '[여성 패션 - 최대 80% 할인] 쟈딕앤볼테르 브랜드 위크 외 특가 &amp; BEST 보러가기', '[언더웨어 - 최대 70% 할인] 노와이어 BEST 모음전, 남성 드로즈 특가 외 보러가기', '[스포츠 - 최대 73% 할인] 아울렛 스포츠 BEST SELECTION 보러가기', '[키즈 패션 - 최대 80% 할인] 오프라벨 게스키즈 외 특가 보러가기', '[리빙 - 최대 75% 할인] 아울렛 리빙 BEST ITEM 최대 75% 보러가기', '[패션 슈즈 - 최대 70% 할인] SHOES&amp;BAGS&amp;ACC FESTIVAL 보러가기', '[패션 잡화 - 최대 30% 할인] RAWROW 아울렛 단독 물량 입고 보러가기', '[명품 잡화 - 최대 50% 할인] 미우미우/톰브라운/프라다 등 일주일 특가 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 신상 입고 보러가기', '[유니섹스 / 캐주얼 - 최대 81% 할인] 아울렛 캐주얼 의류 BEST SELECTION 보러가기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>블랙 프라이데이 여행 BIG SALE</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>패키지 최대 ~15만원 할인 &amp; 항공권 ~7만원 특가</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002946</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>블랙프라이데이 11월 여행 BIG SALE</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2022-11-21</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2022-11-27</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 블랙프라이데이 11월 여행 BIG SALE', '스마일클럽', '캐세이퍼시픽 ~7만원 할인', '여행상품 ~15만원 할인', '실시간 호텔 5% 할인', '카드 청구할인', '홍콩행 항공권 핫딜', '추가 2만원 즉시 할인', '      선착순 50명', '선착순 할인이 종료되었습니다. 성원에 감사드립니다.', '국제선 캐세이퍼시픽 홍콩노선 왕복 항공권 선착순 50명 2만원 할인 (10만원 이상 결제 시)', '행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', '선착순 20명 한정 블랙프라이데이 깜짝 딜!', 'BEST 4 해외여행지 최대 15만원 즉시 할인', '한진관광 SSG 블프 초특가 &amp; 선물 증정 이벤트가고시마 &amp; 달랏 패키지 구매자 1인당 1장씩 스타벅스 커피쿠폰 증정!', '[대한항공 전세기][백수관/LA VISTA] 가고시마 설레임 온천 4일 최초가 2,190,000원 &gt; 할인가 2,040,000원부터 (15만원 할인 / 한진관광 구매자 스타벅스 커피쿠폰 인당 1장 증정)', '[대한항공 전세기/파격특가+삼미 호텔] 4계절 봄의 도시 베트남(달랏) 관광 6일 최초가 999,000원 &gt; 할인가 899,000원부터 (10만원 할인 / 한진관광 구매자 스타벅스 커피쿠폰 인당 1장 증정)', '보홀 솔레아리조트 릴라 고래상어 + 나팔링 자유일정 4일 최초가 589,000원 &gt; 539,000원부터 (5만원 할인 / SSG단독특전: 보홀 현지 망고주스 1잔 증정)', '그리스+튀르키예 10일 - 터키직항+중간 항공 이동1회+특급호텔+11대 특식 최초가 1,299,000원 &gt; 1,119,000원부터 (10만원 할인)', '국내/해외 패키지 전 상품 최대 2만원 즉시 할인', '블프 특가 구매 전, 즉시 할인 혜택을 꼭 챙기세요. 여행 일반상품 결제 시 할인액이 바로 적용됩니다.', '      즉시할인', '여행 상품 즉시할인이 종료되었습니다! 성원에 감사드립니다.', "1) 프로모션 내용: SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 5천원/1만원/2만원 즉시할인", 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '야놀자 실시간 호텔 5% 할인', '실시간 호텔 상품 상세페이지에서 쿠폰을 다운받아 주세요.', '      야놀자 실시간 호텔 5%', '      1원 이상 결제시 최대 3만원 할인', '할인이 종료되었습니다. 감사합니다.', '2) 사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '3) 쿠폰 내용: 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 (최대 3만원)', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '글래드 강남 코엑스센터 정상가 : 132,000원 &gt; 할인가 : 125,400원', '글래드 마포 정상가 : 99,000원 &gt; 할인가 : 94,050원', '라마다용인호텔 정상가 : 109,000원 &gt; 할인가 : 103,550원', '제이앤파크 호텔 정상가 : 166,500원 &gt; 할인가 : 158,175원', '파라다이스 호텔 부산 정상가 : 333,830원 &gt; 할인가 : 317,139원', '라한셀렉트 경주 정상가 : 252,000원 &gt; 할인가 : 239,400원', '통영 스탠포드 호텔앤리조트 정상가 : 145,000원 &gt; 할인가 : 137,750원', '봄그리고가을 호텔&amp;리조트 정상가 : 62,000원 &gt; 할인가 : 58,900원', '호텔 뉴브 정상가 : 99,000원 &gt; 할인가 : 94,050원', '나인트리 호텔 동대문 정상가 : 105,000원 &gt; 할인가 : 99,750원', '서머셋 팰리스 정상가 : 111,620원 &gt; 할인가 : 106,039원', '광명 테이크 호텔 정상가 : 128,250원 &gt; 할인가 : 121,838원', '오라카이 송도파크 호텔 정상가 : 110,000원 &gt; 할인가 : 104,500원', '롯데시티호텔 대전 정상가 : 139,590원 &gt; 할인가 : 132,611원', '호텔 오노마 대전 오토그래프 컬랙션 정상가 : 220,000원 &gt; 할인가 : 209,000원', '호텔 토스카나 정상가 : 240,800원 &gt; 할인가 : 228,760원', '인터컨티넨탈 알펜시아 평창 정상가 : 113,660원 &gt; 할인가 : 107,977원', '오크밸리리조트 정상가 : 138,000원 &gt; 할인가 : 131,100원', '소노벨 비발디파크 B , C (구 오크 , 파인) 정상가 : 115,000원 &gt; 할인가 : 109,250원', '한화리조트 설악 쏘라노 본관 정상가 : 98,000원 &gt; 할인가 : 93,100원', '하이원 리조트 정상가 : 145,000원 &gt; 할인가 : 137,750원', '메이힐스 리조트 정상가 : 55,800원 &gt; 할인가 : 53,010원', '한화리조트 평창 정상가 : 105,001원 &gt; 할인가 : 99,751원', '휘닉스평창 스카이 프리미엄 정상가 : 119,000원 &gt; 할인가 : 113,050원', '포항 네이처풀빌라펜션 정상가 : 190,000원 &gt; 할인가 : 180,500원', '여수 해랑호스텔펜션 정상가 : 140,000원 &gt; 할인가 : 133,000원', '포천 포레스트풀빌라(키즈풀빌라보유) 정상가 : 129,000원 &gt; 할인가 : 122,550원', '고성(속초) 코스트하우스펜션 정상가 : 55,000원 &gt; 할인가 : 52,250원', '강릉 더원펜션,더클래식펜션(신축펜션) 정상가 : 80,000원 &gt; 할인가 : 76,000원', '남양주 코지힐펜션(워터슬라이드,무료 스파) 정상가 : 109,000원 &gt; 할인가 : 103,550원', '가평 에이스펜션(대형수영장,스파) 정상가 : 69,000원 &gt; 할인가 : 65,550원', '서귀포 성산오채풀빌라 정상가 : 420,000원 &gt; 할인가 : 399,000원', '강릉 세인트존스호텔 정상가 : 97,000원 &gt; 할인가 : 92,150원', '체스터톤스 속초 정상가 : 81,250원 &gt; 할인가 : 77,188원', '호텔 탑스텐 정동진 정상가 : 94,910원 &gt; 할인가 : 90,165원', '호텔 센트럴베이 광안리 정상가 : 109,000원 &gt; 할인가 : 103,550원', '코모도호텔 부산 정상가 : 67,000원 &gt; 할인가 : 63,650원', '여수 유탑 마리나 호텔&amp;리조트 정상가 : 99,000원 &gt; 할인가 : 94,050원', '여수 호텔 JCS 정상가 : 175,000원 &gt; 할인가 : 166,250원', '여수 라마다플라자 호텔 정상가 : 80,000원 &gt; 할인가 : 76,000원', '[SSGPAY전용] 신한 7만원이상 7% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] 삼성 7만원이상 7%청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>오르시떼 11/28(월) 11AM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>패밀리 파자마 최대 65%OFF! SSG단독 다크체크/조이 선착순 핫딜</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003135</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]11/28 오르시떼</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2022-11-22</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2022-11-28</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]11/28 오르시떼', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>캐논 11/28(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>EOS R6 MARK II 출시기념 최초공개 LIVE</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003169</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>캐논 @SSG.LIVE 11/28(월) 8PM</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2022-11-22</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2022-11-28</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 캐논 @SSG.LIVE 11/28(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>최대 8만원 혜택</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2022-07-08</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2023-06-28</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 3만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인 + ~68,900원 이달의 혜택</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2022-10-26</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2025-10-25</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.11.01 ~ 2022.11.30', '쿠폰 사용기간 : 2022.11.01 ~ 2022.11.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>11월 유행하는 유아동 상품</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>잡지로 만나는 유아동소식 With 스타일러</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002682</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>[11/01-30] 11월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2022-11-01</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2022-11-30</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; [11/01-30] 11월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '“설레는 마음으로 겨울 룩을 준비하는 시즌, 스타일러맘과 함께하는 퀵 월간 쇼핑, ‘리틀 쓱’과 함께해요!” 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 ‘유아동 전문관’에서 ‘리틀 쓱(Little SSG)’으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!', '근육과 뼈가 쑥쑥 자라는 폭풍 성장기 아이의 겨울옷은 보온성과 활동성을 두루 살펴야 한다. 여기, 어디에 받쳐 입어도 깔끔하게 어울릴 베이식한 디자인의 패딩 아우터 2종을 고르고 골랐다. 물에 강한 것이 특징으로 발수 처리한 자연스러운 크링클 원단에 빠른 복원력을 자랑하는 덕다운 소재라 보관까지 용이하다. 겨울 아우터의 장점은 빠뜨리지 않고 두루 갖춘 셈이다. 여기 팁 하나 더! 덕다운의 혼합 비율을 체크해볼 것. 포근한 보온성의 솜털 80%와 깃털 20% 비율이 패딩 아우터로는 가장 적절해 구매하면 후회 없을 듯.', '순한 유기농 제품만을 선택하는 똑똑한 엄마들에게 전폭적 지지를 받고 있는 브랜드 ‘갸마르드 베이비 by 온뜨레’는 예비맘들 사이에서 꼭 챙겨야 할 육아템으로 손꼽히고 있다. 신생아부터 사용 가능한 100% 천연 성분의 유기농 인증을 받은 갸마르드 베이비 라인이 특별한 이유는 바로 원료에 있다. 미네랄과 유황 함량이 높은 프랑스 2대 온천 지역인 갸마르드의 온천수를 기본 원료로 사용해 진정 효과에 집중한다. 클렌징 젤부터 크림 등 전 라인이 프랑스 정부 산하 유기농 인증 기관인 ‘깔리떼 프랑스’와 에코서트가 설립한 유기농 화장품 인증기관 ‘코스메비오’의 인증을 받아 연약한 아기 피부에 안심하고 사용할 수 있다.']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Dec  1 01:51:11 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,7 +510,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>공공남매가 SSG.COM 인스타그램을 해킹했다!</t>
+          <t>공유, 공효진 SSG.COM 인스타그램을 해킹하다!</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '쓱- 무물 SNS 댓글 이벤트', '                  모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.', '쓱배송, 만사오케이']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.', '쓱배송, 만사오케이']</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; [1128~1204] 패피혁님들 EP.5 '연말 파티 스타일링 대결'", '스마일클럽', "그 동안의 소감을 담아 댓글을 남겨 주시면 추첨을 통해 영상 속 스타일링 제품을 드립니다 +♥사심 가득♥ 혁님의 특별 애장품과 폴라로이드 사진은 보너스!(자세한 이벤트 내용은 '패피혁님들 5화 유튜브 영상 더보기란'에서 확인하세요)"]</t>
+          <t>["이벤트/쿠폰 &gt; [1128~1204] 패피혁님들 EP.5 '연말 파티 스타일링 대결'", '스마일클럽', "그 동안의 소감을 담아 댓글을 남겨 주시면 추첨을 통해 영상 속 스타일링 제품을 드립니다 +♥사심 가득♥ 혁님의 특별 애장품과 폴라로이드 사진은 보너스!(자세한 이벤트 내용은 '패피혁님들 5화 유튜브 영상 더보기란'에서 확인하세요)", '이벤트 기간 : 2022.11.28(월) 18:00 ~ 12.04(일) 23:59', '본 이벤트 조건에 모두 충족되었을 경우에만 이벤트 참여로 간주됩니다.', '이벤트 상세 내용은 SSG.COM 패피혁님들 5화 유튜브 영상 더보기란에서 확인할 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
@@ -695,96 +695,96 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트</t>
+          <t>모두의 야식을 응원합니다</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>이건 진짜 드라마다! WE ARE SSG랜더스!!</t>
+          <t>아침에 주문해 저녁에 받는 쓱배송 야식</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002943</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003209</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트</t>
+          <t>(12/1~7) 모두의 야식을 응원합니다</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-11-09</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트', '스마일클럽', 'SSG닷컴 X SSG랜더스 통합 우승 랜딩 축하 댓글 이벤트', 'SSG닷컴 X SSG랜더스 첫 통합 우승 랜딩 축하 댓글 이벤트', '랜더스 팬 여러분들을 위해 준비한 이벤트 참여하고 다양한 경품 받아가세요!', '       이벤트 기간', '       이벤트 대상', '       이벤트 참여 방법', '       이벤트 페이지 하단에서 축하 댓글 작성 완료 시, 자동 응모됩니다.', "       2022년 12월 9일(금) * 'MY SSG - 이벤트 참여내역' 메뉴를 통해 확인 가능", '      이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '      부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '      이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '      SSG MONEY 지급안내', '      당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 30일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', '      SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (12/1~7) 모두의 야식을 응원합니다', '스마일클럽', '대한민국 경기당일 최대 1.5만원 할인쿠폰', '대한민국 경기 당일 최대 1.5만원 할인쿠폰 바로보기', '국가대표급 쓱배송 야식 바로보기', '아침에 주문하면 저녁에 딱 쓱배송으로 즐기는 야식 바로보기', '아침에 주문해서 저녁에 받는 쓱배송으로 야식을 즐겨요', '최대 1.5만원 할인쿠폰', '12월 3일 경기 딩일 오전 9시 승리 기원 선착순 쿠폰 제공', '         10% 장바구니 쿠폰', '         10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 받으러 가기', '국가대표급 야식 야식에 딱! 쓱배송 상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>스마일클럽의 스마트한 장보기</t>
+          <t>한국금거래소 12/1(목) 7PM</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>월요일마다 최대 10% 더블적립!</t>
+          <t>순금 22년 굿바이 특가/ 순금 주얼리 전제품 8% 쿠폰</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002938</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003199</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[스마일클럽] 11월 내내 매일매일 스마일</t>
+          <t>한국금거래소 @SSG.LIVE 12/1(목)19:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-11-14</t>
+          <t>2022-11-24</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 11월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 11월 내내 매일매일 스마일', '지금 스마일클럽 가입하고 모든 혜택 받기', '한달 내내 막강한 스마일클럽 혜택', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 즉시 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '2. 매주 월요일마다 장보기 최대 10% 더블적립 DAY', '스마일클럽 기본적립 + 월요일마다 추가 적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 한국금거래소 @SSG.LIVE 12/1(목)19:00', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>오르시떼 11/28(월) 11AM</t>
+          <t>에어서울 12/1(목) 8PM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>패밀리 파자마 최대 65%OFF! SSG단독 다크체크/조이 선착순 핫딜</t>
+          <t>일본 편도 항공권 최저 7만원대~, 동남아 편도 항공권 최저 11만원대~</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003135</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003167</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]11/28 오르시떼</t>
+          <t>에어서울 @SSG.LIVE 12/1(목) 8PM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -794,197 +794,123 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]11/28 오르시떼', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 에어서울 @SSG.LIVE 12/1(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>캐논 11/28(월) 8PM</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EOS R6 MARK II 출시기념 최초공개 LIVE</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003169</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>캐논 @SSG.LIVE 11/28(월) 8PM</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-11-22</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 캐논 @SSG.LIVE 11/28(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 3만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>플라스틱아일랜드 11/29(화) 7PM</t>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>최대 66%↓인플루언서 젤라비PICK 겨울 아우터 6만원~</t>
+          <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003168</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>플라스틱 아일랜드 @SSG.LIVE 11/29(화) 7PM</t>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-11-22</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 플라스틱 아일랜드 @SSG.LIVE 11/29(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>12월 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>지금 할인 중! ~50% 할인 혜택</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 3만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인 + ~68,900원 이달의 혜택</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2022-10-26</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2025-10-25</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.11.01 ~ 2022.11.30', '쿠폰 사용기간 : 2022.11.01 ~ 2022.11.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>11월 유행하는 유아동 상품</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>잡지로 만나는 유아동소식 With 스타일러</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002682</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[11/01-30] 11월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2022-11-01</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2022-11-30</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [11/01-30] 11월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '“설레는 마음으로 겨울 룩을 준비하는 시즌, 스타일러맘과 함께하는 퀵 월간 쇼핑, ‘리틀 쓱’과 함께해요!” 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 ‘유아동 전문관’에서 ‘리틀 쓱(Little SSG)’으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!', '근육과 뼈가 쑥쑥 자라는 폭풍 성장기 아이의 겨울옷은 보온성과 활동성을 두루 살펴야 한다. 여기, 어디에 받쳐 입어도 깔끔하게 어울릴 베이식한 디자인의 패딩 아우터 2종을 고르고 골랐다. 물에 강한 것이 특징으로 발수 처리한 자연스러운 크링클 원단에 빠른 복원력을 자랑하는 덕다운 소재라 보관까지 용이하다. 겨울 아우터의 장점은 빠뜨리지 않고 두루 갖춘 셈이다. 여기 팁 하나 더! 덕다운의 혼합 비율을 체크해볼 것. 포근한 보온성의 솜털 80%와 깃털 20% 비율이 패딩 아우터로는 가장 적절해 구매하면 후회 없을 듯.', '순한 유기농 제품만을 선택하는 똑똑한 엄마들에게 전폭적 지지를 받고 있는 브랜드 ‘갸마르드 베이비 by 온뜨레’는 예비맘들 사이에서 꼭 챙겨야 할 육아템으로 손꼽히고 있다. 신생아부터 사용 가능한 100% 천연 성분의 유기농 인증을 받은 갸마르드 베이비 라인이 특별한 이유는 바로 원료에 있다. 미네랄과 유황 함량이 높은 프랑스 2대 온천 지역인 갸마르드의 온천수를 기본 원료로 사용해 진정 효과에 집중한다. 클렌징 젤부터 크림 등 전 라인이 프랑스 정부 산하 유기농 인증 기관인 ‘깔리떼 프랑스’와 에코서트가 설립한 유기농 화장품 인증기관 ‘코스메비오’의 인증을 받아 연약한 아기 피부에 안심하고 사용할 수 있다.']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~50% 쿠폰상품', '지금 할인 중 !', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 50% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 50%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '[맘키즈25%][일동] 프리미엄하이키드/하이키드초코 2종 택1', '[파스퇴르] 올곧게만든 위드맘 100일 750g (NEO2 쓱배송, 그외지역 택배)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '5無과일 100% 유기농 스퀴즈 오렌지 400ml (100ml×4포)', '(알뜰쇼핑 기념 28일 단하루 타임딜)헬로카봇 펜타스톰X', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Dec  5 01:26:13 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,444 +473,777 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>대한민국을 응원합니다</t>
+          <t>SSG 쇼핑 익스프레스</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>축구 국가대표팀 경기 당일, 10% 할인쿠폰 제공</t>
+          <t>~12% 3종 쿠폰팩 + BEST 브랜드 + 카드혜택까지</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003009</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003211</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>대한민국을 응원합니다</t>
+          <t>(1205-07) SSG 쇼핑 익스프레스</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-12-04</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 대한민국을 응원합니다', '스마일클럽', '국가대표팀 경기 당일 오전 9시 선착순 쿠폰 제공', '10% 장바구니 쿠폰 - 선착순 3만장', '10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰이 마감되었습니다', '발급 방식 : 기간 내 ID당 1회씩 발급 (선착순 3만장)', "발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다."]</t>
+          <t>['이벤트/쿠폰 &gt; (1205-07) SSG 쇼핑 익스프레스', '스마일클럽', '최대 12% 할인 쿠폰팩 + 카드청구할인 혜택까지', '쿠폰팩 받고 쇼핑열차 출발!', '#1 최대 12% 장바구니 쿠폰', '쿠폰 적용 몰: 신세계몰, 신세계백화점몰 (일부 카테고리/상품제외)', '       7% 장바구니 쿠폰', '       5만원 이상 구매시 최대 5천원 할인', '       10% 장바구니 쿠폰', '       7만원 이상 구매시 최대 1만원 할인', '       12% 장바구니 쿠폰', '       10만원 이상 구매시 최대 2만원 할인', '#5 카드할인', '삼성카드[SSGPAY전용] 7만원 이상 결제 시 7% 청구할인 (일 30만원 限, 라이프스타일 CAT 대상)', '삼성카드[SSGPAY전용] 7만원 이상 결제 시 7% 청구할인 (일 20만원 限, 라이프스타일 CAT 대상)', '삼성카드[SSGPAY전용] 7만원 이상 결제 시 7% 청구할인 (일 10만원 限, 라이프스타일 CAT 대상)', '베스트 패션 어워즈2022년 BEST 브랜드&amp;아이템 + 선착순 장바구니 쿠폰', '먼데이문 위크2022년 BEST 브랜드&amp;아이템 + 선착순 장바구니 쿠폰', 'SSG Luxury Gift Week최대 15만원 할인 쿠폰 + 매일 오전 10시 타임딜', '쿠폰 발급 및 사용기간: 2022년 12월 5일 (월) 00:00 ~ 12월 7일 (수) 23:59', '쿠폰은 ID당 기간 내 1회 발급 가능하며, 발급된 쿠폰은 ‘My SSG &gt; 쿠폰 &gt; 보유쿠폰’ 에서 확인 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점몰 상품 대상이며 동일 주문건 내 대상상품 전체에 적용 가능합니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '쿠폰 발급 및 사용기간: 2022년 12월 5일 (월) ~ 12월 7일 (수) 매일 오전 9시부터 발급, 기간 내 사용', '본 쿠폰은 스마일클럽 가입회원 전용으로 발급되는 쿠폰입니다.']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>공유, 공효진 SSG.COM 인스타그램을 해킹하다!</t>
+          <t>베스트 패션 어워즈</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>무물 질문하고 친필 사인, 다이슨 에어랩, 하만카돈 스피커도 받아가세요.</t>
+          <t>10% 쿠폰으로 2022년 인기 브랜드 쇼핑!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003198</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
+          <t>(12/5~11) 베스트 패션 어워즈</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.', '쓱배송, 만사오케이']</t>
+          <t>['이벤트/쿠폰 &gt; (12/5~11) 베스트 패션 어워즈', '스마일클럽', '10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매시 최대 1.2만원 할인(매일 오전 9시,선착순 1만명)', '선착순 쿠폰 sold out!', '쿠폰 발급 받기(ID당 1회 발급)', '쿠폰 발급 기간:  2022년 12월 5일(월) ~ 12월 11(일), 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간 : 2022년 12월 5일(월) ~ 12월 11(일), 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '[온앤온.올리브데올리브] 패밀리세일! 윈터 인기 아이템 ~70% OFF', '22F/W 헤지스 여성 겨울 베스트 신상 +최대 15%쿠폰', '♥사은품증정♥ FW 베스트 아우터 추가 쿠폰 헤택!', '겨울 남성 코디 제안! ! 최대 15% 할인 + 무배', '[MD추천] 지금 핫한 아우터 BEST 50 ★ 쿠폰 혜택!', 'WINTER 골프의류 및 용품 단독 ~50% OFF', '22 WINTER CAMPAIGN 오픈 + 신세계 단독 최대 30%', '★키플링BEST★ 데일리백 특가찬스 +추가할인쿠폰', '신세계 광주점 단독 특가! 핸드백&amp;지갑 ~35% OFF + 양말 사은품', '[카렌화이트] 22FW 신상&amp;베스트 특가 + 쿠폰혜택', '부츠 베스트 어워즈 ~70%+추가쿠폰', '[TUMI] 손흥민 PICK! 럭셔리백팩~30%OFF + 10% 쿠폰!', 'BEST 모음전! 추가 쿠폰 혜택까지', '[워치스테이션] 아르마니 BEST 시계 SALE 69%', 'BEST SELLER / 추가쿠폰혜택!', '[자주]WINTER SALE 파자마 특집전 +10%OFF']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>패피혁님들</t>
+          <t>SSG Luxury Gift Week</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>핏 터지는 1:1 스타일링 배틀</t>
+          <t>최대 15만원 할인 쿠폰 + 연말 BEST 기프트 추천</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003140</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003212&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[1128~1204] 패피혁님들 EP.5 '연말 파티 스타일링 대결'</t>
+          <t>(1205-11) SSG Luxury Gift Week</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2022-12-04</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; [1128~1204] 패피혁님들 EP.5 '연말 파티 스타일링 대결'", '스마일클럽', "그 동안의 소감을 담아 댓글을 남겨 주시면 추첨을 통해 영상 속 스타일링 제품을 드립니다 +♥사심 가득♥ 혁님의 특별 애장품과 폴라로이드 사진은 보너스!(자세한 이벤트 내용은 '패피혁님들 5화 유튜브 영상 더보기란'에서 확인하세요)", '이벤트 기간 : 2022.11.28(월) 18:00 ~ 12.04(일) 23:59', '본 이벤트 조건에 모두 충족되었을 경우에만 이벤트 참여로 간주됩니다.', '이벤트 상세 내용은 SSG.COM 패피혁님들 5화 유튜브 영상 더보기란에서 확인할 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (1205-11) SSG Luxury Gift Week', '스마일클럽', '# 최대 15만원 할인 쿠폰', '# 매일 오전 10시 타임딜', '01. 매일 오전 10시 럭셔리 타임딜', '02. 명품 쇼핑찬스 최대 15만원 할인쿠폰', '01. 지금만 이 가격! 매일 오전 10시 SSG Luxury 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다.', '상품쿠폰 7% - 15만원 이상 상품 구매 시, 최대 7만원 할인(선착순 5천명)', '상품쿠폰 10% - 30만원 이상 상품 구매 시, 최대 15만원 할인(선착순 5천명)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요!', '쿠폰 발급 및 유효기간: 22/12/05(월) ~ 22/12/11(일)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '본 쿠폰은 이마트몰, 신세계몰, 신세계백화점 특정 카테고리 상품 중 SSG Luxury club 상품에 적용되는 쿠폰입니다.', '쿠폰 대상 상품은 상품 상세에서 SSG Luxury club 상세 배너 확인 부탁드립니다.', '명품 상품 중에 판매가 5천원 이상 상품 구매하시고 스페셜 리뷰를 작성하면 SSG MONEY 1,000원 적립 가능!(리뷰 작성은 MY SSG &gt; 나의 활동 관리 &gt; 마이리뷰 내 ‘스페셜’ Tab에서 ‘작성 가능한 리뷰’ 에서 하실 수 있습니다.)']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>신세계 리빙 셀렉샵 오픈</t>
+          <t>신세계백화점 Holiday Gift</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>백화점 리빙 7% 쿠폰 + 뱅앤올룹슨/아르떼미데 外 경품 이벤트</t>
+          <t>럭셔리 기프트 제안</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003007</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003163</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Shinsegae Living Select Shop</t>
+          <t>[12/5-25] Magical Winter Fantasy</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-12-04</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Shinsegae Living Select Shop', '스마일클럽', '백화점 리빙 7% 쿠폰 바로보기', 'SNS 소문내기 경품 이벤트 바로보기', '할인으로 더 가깝게 만나는 프리미엄 리빙 7% COUPON', '      7% 장바구니 쿠폰', '      선착순 1,500명', '      7만원 이상 결제 시, 최대 1만 5천원 할인', '쿠폰 발급 및 사용기간: 2022년 11월 21일 (월) 00:00 ~ 12월 4일 (일) 23:59', '쿠폰 발급 후 MY SSG &gt; 쿠폰 &gt; 보유쿠폰에서 확인 가능', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '리빙 셀렉샵 소문내기 이벤트', '이벤트 참여 방법', '1. 이벤트 페이지 캡쳐 및 URL을 복사해서 SNS에 공유해주세요.', '       이벤트 기간', "       SSG.COM 이벤트&amp;쿠폰 '당첨자 발표' 게시판", '본 이벤트는 ID별로 1회 참여할 수 있으며, 부정한 방법으로 참여한 것이 발견될 경우 당첨이 취소될 수 있습니다.', '댓글 입력 후 SNS 공유글을 삭제한 경우 이벤트 당첨자 명단에서 자동 제외됩니다.', '이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다. (개인 정보 위탁업체 : (주)젤라블루코리아, 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호, 주소)', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [12/5-25] Magical Winter Fantasy', '스마일클럽', '따뜻한 연말을 위한 네스프레소 선물 기획전 - 에센자미니 10% 할인 및 사은품 증정 보러가기', '바오밥컬렉션 신제품 출시 기념 팝업 - 마이퍼스트바오밥 신상품 최대 20%할인 &amp; 선물용 기프트포장 혜택 보러가기', 'SENNHEISSER NEW YEAR PROMOTION - CX PLUS TW SE/HD-600 최대 10% 할인 혜택 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>캡틴쓱 : 게임 체인저</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>친환경 인식 개선 캠페인</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003079</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;', '스마일클럽', '전기차 쓱배송 차량 캐릭터 - 전기차 쓱카', '쓱배송 차량의 전기차 브로! 착실하고 우직한 성격으로 쓱배송을 전담하고 있다. 명석한 두뇌로 최적의 루트를 빠르게 분석한다.', '첫 번째 이벤트 - 메타버스 캡틴쓱 본부 내 모든 스테이지 참여 시 추첨을 통해 친환경 키트 혹은 신세계 모바일 상품권 5천원권', '두 번째 이벤트 - 스테이지 4에서 최단 기록 10명 대상으로 날마다 신세계 모바일 상품권 5천원권 증정', '세 번째 이벤트 - 보너스 스테이지 참여자 대상으로 추첨을 통해 스타벅스 기프트카드 1만원권 증정', ' 미션 종료 후 이벤트 참여 및 리워드 제공을 위해 테라사이클 코리아에서 개인정보를 수집할 수 있습니다. 자세한 이벤트 내용은 해당 스테이지 내 안내 문구를 참고해주세요. PC로 참여하시는 경우, 크롬 브라우저를 통해 입장해주시길 바랍니다. ', '       인스타그램 이벤트 계정에 들어가서 게시글을 눌러가며 힌트를 얻어 곰인형을 구해주세요. 마지막 단계에서 댓글 작성 시, 댓글 수에 따라 기부가 진행됩니다.', '자세한 이벤트 내용은 해당 게시글 내 안내 문구를 참고해주세요.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2022 대한민국 수산대전</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>연말 이벤트전</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003149</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-11-24</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '스마일클럽', '(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>모두의 야식을 응원합니다</t>
+          <t>공유 &amp; 공효진 무물 대공개</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>아침에 주문해 저녁에 받는 쓱배송 야식</t>
+          <t>궁금증을 쓱-풀어보세요</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003209</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>(12/1~7) 모두의 야식을 응원합니다</t>
+          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (12/1~7) 모두의 야식을 응원합니다', '스마일클럽', '대한민국 경기당일 최대 1.5만원 할인쿠폰', '대한민국 경기 당일 최대 1.5만원 할인쿠폰 바로보기', '국가대표급 쓱배송 야식 바로보기', '아침에 주문하면 저녁에 딱 쓱배송으로 즐기는 야식 바로보기', '아침에 주문해서 저녁에 받는 쓱배송으로 야식을 즐겨요', '최대 1.5만원 할인쿠폰', '12월 3일 경기 딩일 오전 9시 승리 기원 선착순 쿠폰 제공', '         10% 장바구니 쿠폰', '         10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 받으러 가기', '국가대표급 야식 야식에 딱! 쓱배송 상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>한국금거래소 12/1(목) 7PM</t>
+          <t>캡틴쓱 : 게임 체인저</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>순금 22년 굿바이 특가/ 순금 주얼리 전제품 8% 쿠폰</t>
+          <t>친환경 인식 개선 캠페인</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003199</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003079</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>한국금거래소 @SSG.LIVE 12/1(목)19:00</t>
+          <t>친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-11-24</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 한국금거래소 @SSG.LIVE 12/1(목)19:00', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; 친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;', '스마일클럽', '전기차 쓱배송 차량 캐릭터 - 전기차 쓱카', '쓱배송 차량의 전기차 브로! 착실하고 우직한 성격으로 쓱배송을 전담하고 있다. 명석한 두뇌로 최적의 루트를 빠르게 분석한다.', '첫 번째 이벤트 - 메타버스 캡틴쓱 본부 내 모든 스테이지 참여 시 추첨을 통해 친환경 키트 혹은 신세계 모바일 상품권 5천원권', '두 번째 이벤트 - 스테이지 4에서 최단 기록 10명 대상으로 날마다 신세계 모바일 상품권 5천원권 증정', '세 번째 이벤트 - 보너스 스테이지 참여자 대상으로 추첨을 통해 스타벅스 기프트카드 1만원권 증정', ' 미션 종료 후 이벤트 참여 및 리워드 제공을 위해 테라사이클 코리아에서 개인정보를 수집할 수 있습니다. 자세한 이벤트 내용은 해당 스테이지 내 안내 문구를 참고해주세요. PC로 참여하시는 경우, 크롬 브라우저를 통해 입장해주시길 바랍니다. ', '       인스타그램 이벤트 계정에 들어가서 게시글을 눌러가며 힌트를 얻어 곰인형을 구해주세요. 마지막 단계에서 댓글 작성 시, 댓글 수에 따라 기부가 진행됩니다.', '자세한 이벤트 내용은 해당 게시글 내 안내 문구를 참고해주세요.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>에어서울 12/1(목) 8PM</t>
+          <t>2022 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>일본 편도 항공권 최저 7만원대~, 동남아 편도 항공권 최저 11만원대~</t>
+          <t>연말 이벤트전</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003167</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003149</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>에어서울 @SSG.LIVE 12/1(목) 8PM</t>
+          <t>(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-11-22</t>
+          <t>2022-11-24</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 에어서울 @SSG.LIVE 12/1(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; (11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '스마일클럽', '(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>모두의 야식을 응원합니다</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>아침에 주문해 저녁에 받는 쓱배송 야식</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003209</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>(12/1~7) 모두의 야식을 응원합니다</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 3만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; (12/1~7) 모두의 야식을 응원합니다', '스마일클럽', '대한민국 경기당일 최대 1.5만원 할인쿠폰', '대한민국 경기 당일 최대 1.5만원 할인쿠폰 바로보기', '국가대표급 쓱배송 야식 바로보기', '아침에 주문하면 저녁에 딱 쓱배송으로 즐기는 야식 바로보기', '아침에 주문해서 저녁에 받는 쓱배송으로 야식을 즐겨요', '최대 1.5만원 할인쿠폰', '12월 3일 경기 딩일 오전 9시 승리 기원 선착순 쿠폰 제공', '         10% 장바구니 쿠폰', '         10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 받으러 가기', '국가대표급 야식 야식에 딱! 쓱배송 상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
+          <t>홀리데이 뷰티 기프트</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
+          <t>럭셔리&amp;트랜드뷰티 ~15%쿠폰 SSG머니 혜택까지!</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003234</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
+          <t>[1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
+          <t>["이벤트/쿠폰 &gt; [1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'", '스마일클럽', '뷰티 ~15% 쿠폰', '모두의 홀리데이 뷰티 ~15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '상품쿠폰 12% 선착순 - 3만원 이상 상품 구매시 최대 1만원 2천원 할인', '쿠폰은 09시부터 선착순 발급 됩니다', '트렌드뷰티 최대 5% 상품쿠폰', '상품쿠폰 5% 선착순 - 2만원 이상 상품 구매시 최대 5천원 할인', '발급 수량 : 럭셔리뷰티 12% 상품쿠폰 - 선착순 4만장, 트렌드뷰티 5% 상품쿠폰 - 선착순 3만장', '12% 상품쿠폰은 신세계백화점몰, 시코르몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용 됩니다.', '5% 상품쿠폰은 신세계몰, 이마트몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용됩니다. ', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', ' 본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다. ', 'SSG 단독 ~17% + 정품증정 구성', '피테라 에센스 리미티드 에디션 구매시', 'SSG 단독 사은 이벤트', '쿠션/섀도우/치크 외 최대 55%할인', '~45%+3만원 이상 구매시 바닐라부티크 핸드크림 증정 + 쿠폰 15% 발급', '6가지 컬러로 최대 63컬러까지 조합 가능한 아이 팔레트 UP TO 53% 특가', '[특별선물] 캐스키드슨 바디세트/핸드크림/향수/핸드클렌저 등 ~56%할인', '뷰티 어워즈 구매사은+무료배송 (토일렛페이퍼,멀티아이팔레트,페이스블러쉬,블러워터틴트,벨벳틴트,소프트매트립,뉴테이크 외)', 'SSG단독 블룸쿠션 럭키박스 (55%할인)', '신상품 출시 기념 홀리데이 이벤트+구매 사은품', '[바이오오일 브랜드 기획전] BEST 위너 뷰티템 단독 특가~56% + 9900원 특가 + 무료배송 + 15% 추가쿠폰혜택', '★구찌경품★ 2022 연말결산! 크나이프/지아자 연중최대할인!', '기프트 세트 20% 할인 &amp; 럭셔리 케어 증정', '핸드크림 신규츌시! 라이프 프래그런스 최대 59% 할인! (+쇼핑백 증정)', '■ 당첨 조건 및 당첨 인원 : 이벤트 기간 내 뷰티 1개 이상 구매 후 응모한 고객  중 500명 추첨 후 SSG머니 2,000원 지급', '- 해당 조건 1개 이상 구매 후 이벤트페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한하여 당첨자 추첨 후 해당 ID로 적립됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12월 맘키즈 PLUS</t>
+          <t>2022 펫페어 어워즈</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>지금 할인 중! ~50% 할인 혜택</t>
+          <t>20% 장바구니 쿠폰</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003136</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>이달의 맘키즈 PLUS</t>
+          <t>2022 펫페어 어워즈</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2999-12-13</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~50% 쿠폰상품', '지금 할인 중 !', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 50% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 50%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '[맘키즈25%][일동] 프리미엄하이키드/하이키드초코 2종 택1', '[파스퇴르] 올곧게만든 위드맘 100일 750g (NEO2 쓱배송, 그외지역 택배)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '5無과일 100% 유기농 스퀴즈 오렌지 400ml (100ml×4포)', '(알뜰쇼핑 기념 28일 단하루 타임딜)헬로카봇 펜타스톰X', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
+          <t>['이벤트/쿠폰 &gt; 2022 펫페어 어워즈', '스마일클럽', '선착순 혜택', '20% 할인 쿠폰', '20% 장바구니 쿠폰', '매일 600명 선착순', '20% 장바구니 쿠폰 - 4만원 이상 구매시 적용 (최대 1만원 할인)', '      쿠폰 발급 및 사용기간', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '[선착순핫딜]본사직영_붐펫드라이룸 K100', '[쓱배송] 몰리스 고양이 사료 15kg', '[무료배송]모래혁명 무향 가는입자 6kg*3개(박스)', '[무료배송] 에버크린 무향 19kg_2개이상구매시 분할발송', '[무료배송/빠른출고] 에버크린 무향 19kg_2개이상구매시 분할발송']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>스마일클럽 12월의 가입 혜택</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2022-12-05</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2022-12-31</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>프리미엄 아울렛 위크</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12월 할인대전</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003270</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>[1205-1211] 프리미엄 아울렛 위크</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-12-05</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2022-12-11</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [1205-1211] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 12월 할인 대전', '최대 10% 할인 쿠폰 혜택', '혜택에 할인을 더 10% 카드청구 할인', '       10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 가격에 추가 할인이 더 12월 주요 행사', '[여성 패션 - 최대 70% 할인] 지컷/ 시슬리/ 랩 外 여성패션 특가 &amp; BEST 보러가기', '[언더웨어 - 최대 75% 할인] 노와이어 BEST 모음전, 남성 드로즈 특가 외 보러가기', '[스포츠 - 최대 70% 할인] 내셔널/ 노스페이스 등 겨울 아웃도어 BEST 보러가기', '[키즈 패션 - 최대 75% 할인] 스키복/아우터 外 겨울 상품 입고 보러가기', '[리빙 - 최대 70% 할인] 아울렛 리빙 BEST 보러가기', '[패션 슈즈 - 최대 80% 할인] 아울렛 슈즈 GIFT 전 보러가기', '[패션 잡화 - 최대 44% 할인] 골든듀/ 로제도르 30% OFF 보러가기', '[명품 잡화 - 최대 50% 할인] 미우미우/톰브라운/프라다 등 일주일 특가 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 신상 입고 보러가기', '[유니섹스 / 캐주얼 - 최대 80% 할인] 경량베스트, 점퍼 등 최고 80% OFF 보러가기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>지라프 12/5(월) 7PM</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>구이바다 핫딜 10만원대 + 역대급 LIVE이벤트까지</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003243</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>지라프 @SSG.LIVE 12/5(월) 19:00PM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022-11-28</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2022-12-05</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 지라프 @SSG.LIVE 12/5(월) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>에고이스트 12/5(월) 9PM</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>구스 다운 핫딜가 99천원 찬스! 캐리어&amp;카드지갑 증정 이벤트</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003222</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>[SSG.LIVE]12/5 에고이스트</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2022-11-29</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2022-12-05</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]12/5 에고이스트', '스마일클럽', '                    SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>블랑101 12/6(화) 11AM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>세탁세제 4개세트 5.8만원대+멀티클리너 본품 증정</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003252&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>[쓱라이브] 블랑101 12/6(화) 11AM</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2022-11-28</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2022-12-08</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 블랑101 12/6(화) 11AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SK-II  12/6(화) 7PM</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SK-II 에센스 최대 30%할인 + 홀리데이 리미티드 에디션 공개</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003284</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SK-II @SSG.LIVE 12/6(화) 7PM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2022-11-30</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2022-12-06</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SK-II @SSG.LIVE 12/6(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>휘닉스평창 12/6(화) 8PM</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>겨울 액티비티 성지, 휘닉스평창 올인클루시브 패키지</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003250</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>[월간호캉쓱] 휘닉스평창 @SSG.LIVE 12/6(화) 20:00PM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2022-11-28</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2022-12-06</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [월간호캉쓱] 휘닉스평창 @SSG.LIVE 12/6(화) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>아늑한 꿀잠을 위한 숙면테리어</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>침구부터 인테리어까지, 우리집 침실 새단장 프로젝트</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003110</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>숙면테리어</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2022-12-05</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2022-12-12</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 숙면테리어', '스마일클럽', '원데이 타임딜 바로보기', '할인 상품 모아보기 바로보기', '하루에 하나씩 득템! 원데이 숙면 타임딜', '[타임딜] 클래식패브릭 헝가리 구스 SS/Q', '할인상품 모아보기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>산타가 골라준 홀리데이 장난감</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2022-12-01</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2022-12-31</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Dec  8 01:26:43 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,22 +473,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SSG 쇼핑 익스프레스</t>
+          <t>베스트 패션 어워즈</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>~12% 3종 쿠폰팩 + BEST 브랜드 + 카드혜택까지</t>
+          <t>10% 쿠폰으로 2022년 인기 브랜드 쇼핑!</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003211</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003198</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(1205-07) SSG 쇼핑 익스프레스</t>
+          <t>(12/5~11) 베스트 패션 어워즈</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -498,34 +498,34 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1205-07) SSG 쇼핑 익스프레스', '스마일클럽', '최대 12% 할인 쿠폰팩 + 카드청구할인 혜택까지', '쿠폰팩 받고 쇼핑열차 출발!', '#1 최대 12% 장바구니 쿠폰', '쿠폰 적용 몰: 신세계몰, 신세계백화점몰 (일부 카테고리/상품제외)', '       7% 장바구니 쿠폰', '       5만원 이상 구매시 최대 5천원 할인', '       10% 장바구니 쿠폰', '       7만원 이상 구매시 최대 1만원 할인', '       12% 장바구니 쿠폰', '       10만원 이상 구매시 최대 2만원 할인', '#5 카드할인', '삼성카드[SSGPAY전용] 7만원 이상 결제 시 7% 청구할인 (일 30만원 限, 라이프스타일 CAT 대상)', '삼성카드[SSGPAY전용] 7만원 이상 결제 시 7% 청구할인 (일 20만원 限, 라이프스타일 CAT 대상)', '삼성카드[SSGPAY전용] 7만원 이상 결제 시 7% 청구할인 (일 10만원 限, 라이프스타일 CAT 대상)', '베스트 패션 어워즈2022년 BEST 브랜드&amp;아이템 + 선착순 장바구니 쿠폰', '먼데이문 위크2022년 BEST 브랜드&amp;아이템 + 선착순 장바구니 쿠폰', 'SSG Luxury Gift Week최대 15만원 할인 쿠폰 + 매일 오전 10시 타임딜', '쿠폰 발급 및 사용기간: 2022년 12월 5일 (월) 00:00 ~ 12월 7일 (수) 23:59', '쿠폰은 ID당 기간 내 1회 발급 가능하며, 발급된 쿠폰은 ‘My SSG &gt; 쿠폰 &gt; 보유쿠폰’ 에서 확인 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점몰 상품 대상이며 동일 주문건 내 대상상품 전체에 적용 가능합니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '쿠폰 발급 및 사용기간: 2022년 12월 5일 (월) ~ 12월 7일 (수) 매일 오전 9시부터 발급, 기간 내 사용', '본 쿠폰은 스마일클럽 가입회원 전용으로 발급되는 쿠폰입니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (12/5~11) 베스트 패션 어워즈', '스마일클럽', '10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매시 최대 1.2만원 할인(매일 오전 9시,선착순 1만명)', '선착순 쿠폰 sold out!', '쿠폰 발급 받기(ID당 1회 발급)', '쿠폰 발급 기간:  2022년 12월 5일(월) ~ 12월 11(일), 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간 : 2022년 12월 5일(월) ~ 12월 11(일), 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '[온앤온.올리브데올리브] 패밀리세일! 윈터 인기 아이템 ~70% OFF', '22F/W 헤지스 여성 겨울 베스트 신상 +최대 15%쿠폰', '♥사은품증정♥ FW 베스트 아우터 추가 쿠폰 헤택!', '겨울 남성 코디 제안! ! 최대 15% 할인 + 무배', '[MD추천] 지금 핫한 아우터 BEST 50 ★ 쿠폰 혜택!', 'WINTER 골프의류 및 용품 단독 ~50% OFF', '22 WINTER CAMPAIGN 오픈 + 신세계 단독 최대 30%', '★키플링BEST★ 데일리백 특가찬스 +추가할인쿠폰', '신세계 광주점 단독 특가! 핸드백&amp;지갑 ~35% OFF + 양말 사은품', '[카렌화이트] 22FW 신상&amp;베스트 특가 + 쿠폰혜택', '부츠 베스트 어워즈 ~70%+추가쿠폰', '[LUXURY WEEK] 급! 추워진 날씨도 물리칠 럭셔리 의류50종, 몽클레어/톰브라운 外 + 추가쿠폰적용가능', '[TUMI] 손흥민 PICK! 럭셔리백팩~30%OFF + 10% 쿠폰!', 'BEST 모음전! 추가 쿠폰 혜택까지', '[워치스테이션] 아르마니 BEST 시계 SALE 69%', 'BEST SELLER / 추가쿠폰혜택!', '[자주]WINTER SALE 파자마 특집전 +10%OFF']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>베스트 패션 어워즈</t>
+          <t>SSG Luxury Gift Week</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10% 쿠폰으로 2022년 인기 브랜드 쇼핑!</t>
+          <t>최대 15만원 할인 쿠폰 + 연말 BEST 기프트 추천</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003198</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003212&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(12/5~11) 베스트 패션 어워즈</t>
+          <t>(1205-11) SSG Luxury Gift Week</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -540,29 +540,29 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (12/5~11) 베스트 패션 어워즈', '스마일클럽', '10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매시 최대 1.2만원 할인(매일 오전 9시,선착순 1만명)', '선착순 쿠폰 sold out!', '쿠폰 발급 받기(ID당 1회 발급)', '쿠폰 발급 기간:  2022년 12월 5일(월) ~ 12월 11(일), 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간 : 2022년 12월 5일(월) ~ 12월 11(일), 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '[온앤온.올리브데올리브] 패밀리세일! 윈터 인기 아이템 ~70% OFF', '22F/W 헤지스 여성 겨울 베스트 신상 +최대 15%쿠폰', '♥사은품증정♥ FW 베스트 아우터 추가 쿠폰 헤택!', '겨울 남성 코디 제안! ! 최대 15% 할인 + 무배', '[MD추천] 지금 핫한 아우터 BEST 50 ★ 쿠폰 혜택!', 'WINTER 골프의류 및 용품 단독 ~50% OFF', '22 WINTER CAMPAIGN 오픈 + 신세계 단독 최대 30%', '★키플링BEST★ 데일리백 특가찬스 +추가할인쿠폰', '신세계 광주점 단독 특가! 핸드백&amp;지갑 ~35% OFF + 양말 사은품', '[카렌화이트] 22FW 신상&amp;베스트 특가 + 쿠폰혜택', '부츠 베스트 어워즈 ~70%+추가쿠폰', '[TUMI] 손흥민 PICK! 럭셔리백팩~30%OFF + 10% 쿠폰!', 'BEST 모음전! 추가 쿠폰 혜택까지', '[워치스테이션] 아르마니 BEST 시계 SALE 69%', 'BEST SELLER / 추가쿠폰혜택!', '[자주]WINTER SALE 파자마 특집전 +10%OFF']</t>
+          <t>['이벤트/쿠폰 &gt; (1205-11) SSG Luxury Gift Week', '스마일클럽', '# 최대 15만원 할인 쿠폰', '# 매일 오전 10시 타임딜', '01. 매일 오전 10시 럭셔리 타임딜', '02. 명품 쇼핑찬스 최대 15만원 할인쿠폰', '01. 지금만 이 가격! 매일 오전 10시 SSG Luxury 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다.', '상품쿠폰 7% - 15만원 이상 상품 구매 시, 최대 7만원 할인(선착순 5천명)', '상품쿠폰 10% - 30만원 이상 상품 구매 시, 최대 15만원 할인(선착순 5천명)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요!', '쿠폰 발급 및 유효기간: 22/12/05(월) ~ 22/12/11(일)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '본 쿠폰은 이마트몰, 신세계몰, 신세계백화점 특정 카테고리 상품 중 SSG Luxury club 상품에 적용되는 쿠폰입니다.', '쿠폰 대상 상품은 상품 상세에서 SSG Luxury club 상세 배너 확인 부탁드립니다.', '명품 상품 중에 판매가 5천원 이상 상품 구매하시고 스페셜 리뷰를 작성하면 SSG MONEY 1,000원 적립 가능!(리뷰 작성은 MY SSG &gt; 나의 활동 관리 &gt; 마이리뷰 내 ‘스페셜’ Tab에서 ‘작성 가능한 리뷰’ 에서 하실 수 있습니다.)']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SSG Luxury Gift Week</t>
+          <t>신세계백화점 Holiday Gift</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>최대 15만원 할인 쿠폰 + 연말 BEST 기프트 추천</t>
+          <t>럭셔리 기프트 제안</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003212&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003163</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(1205-11) SSG Luxury Gift Week</t>
+          <t>[12/5-25] Magical Winter Fantasy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,49 +572,49 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1205-11) SSG Luxury Gift Week', '스마일클럽', '# 최대 15만원 할인 쿠폰', '# 매일 오전 10시 타임딜', '01. 매일 오전 10시 럭셔리 타임딜', '02. 명품 쇼핑찬스 최대 15만원 할인쿠폰', '01. 지금만 이 가격! 매일 오전 10시 SSG Luxury 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다.', '상품쿠폰 7% - 15만원 이상 상품 구매 시, 최대 7만원 할인(선착순 5천명)', '상품쿠폰 10% - 30만원 이상 상품 구매 시, 최대 15만원 할인(선착순 5천명)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요!', '쿠폰 발급 및 유효기간: 22/12/05(월) ~ 22/12/11(일)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '본 쿠폰은 이마트몰, 신세계몰, 신세계백화점 특정 카테고리 상품 중 SSG Luxury club 상품에 적용되는 쿠폰입니다.', '쿠폰 대상 상품은 상품 상세에서 SSG Luxury club 상세 배너 확인 부탁드립니다.', '명품 상품 중에 판매가 5천원 이상 상품 구매하시고 스페셜 리뷰를 작성하면 SSG MONEY 1,000원 적립 가능!(리뷰 작성은 MY SSG &gt; 나의 활동 관리 &gt; 마이리뷰 내 ‘스페셜’ Tab에서 ‘작성 가능한 리뷰’ 에서 하실 수 있습니다.)']</t>
+          <t>['이벤트/쿠폰 &gt; [12/5-25] Magical Winter Fantasy', '스마일클럽', '따뜻한 연말을 위한 네스프레소 선물 기획전 - 에센자미니 10% 할인 및 사은품 증정 보러가기', '바오밥컬렉션 신제품 출시 기념 팝업 - 마이퍼스트바오밥 신상품 최대 20%할인 &amp; 선물용 기프트포장 혜택 보러가기', 'SENNHEISSER NEW YEAR PROMOTION - CX PLUS TW SE/HD-600 최대 10% 할인 혜택 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>신세계백화점 Holiday Gift</t>
+          <t>랜더스 우승기념 쓱닷컴 우승챌린지</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>럭셔리 기프트 제안</t>
+          <t>우승의 기쁨을 쓱닷컴과 한번더!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003163</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003137</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[12/5-25] Magical Winter Fantasy</t>
+          <t>[SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/5-25] Magical Winter Fantasy', '스마일클럽', '따뜻한 연말을 위한 네스프레소 선물 기획전 - 에센자미니 10% 할인 및 사은품 증정 보러가기', '바오밥컬렉션 신제품 출시 기념 팝업 - 마이퍼스트바오밥 신상품 최대 20%할인 &amp; 선물용 기프트포장 혜택 보러가기', 'SENNHEISSER NEW YEAR PROMOTION - CX PLUS TW SE/HD-600 최대 10% 할인 혜택 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내', '스마일클럽', '       이벤트경품', '       이벤트 기간', '       이벤트 참여 방법', '이벤트 기간 내 인스타그램을 통해 #쓱닷컴우승챌린지 에 참여한 경우 자동 응모', '이벤트 기간', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', 'SSG MONEY 지급안내', '당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 180일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', 'SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
@@ -769,96 +769,96 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2022 대한민국 수산대전</t>
+          <t>홀리데이 뷰티 기프트</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>연말 이벤트전</t>
+          <t>럭셔리&amp;트랜드뷰티 ~15%쿠폰 SSG머니 혜택까지!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003149</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003234</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전</t>
+          <t>[1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-11-24</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '스마일클럽', '(11/24~12/7) 2022 대한민국 수산대전 - 연말 이벤트전', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>["이벤트/쿠폰 &gt; [1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'", '스마일클럽', '뷰티 ~15% 쿠폰', '모두의 홀리데이 뷰티 ~15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '상품쿠폰 12% 선착순 - 3만원 이상 상품 구매시 최대 1만원 2천원 할인', '쿠폰은 09시부터 선착순 발급 됩니다', '트렌드뷰티 최대 5% 상품쿠폰', '상품쿠폰 5% 선착순 - 2만원 이상 상품 구매시 최대 5천원 할인', '발급 수량 : 럭셔리뷰티 12% 상품쿠폰 - 선착순 4만장, 트렌드뷰티 5% 상품쿠폰 - 선착순 3만장', '12% 상품쿠폰은 신세계백화점몰, 시코르몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용 됩니다.', '5% 상품쿠폰은 신세계몰, 이마트몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용됩니다. ', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', ' 본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다. ', 'SSG 단독 ~17% + 정품증정 구성', '피테라 에센스 리미티드 에디션 구매시', 'SSG 단독 사은 이벤트', '쿠션/섀도우/치크 외 최대 55%할인', '크리스마스 에디션 UP TO 15%', '~45%+3만원 이상 구매시 바닐라부티크 핸드크림 증정 + 쿠폰 15% 발급', '6가지 컬러로 최대 63컬러까지 조합 가능한 아이 팔레트 UP TO 53% 특가', '[특별선물] 캐스키드슨 2022 홀리데이 에디션 ~56%할인', '뷰티 어워즈 구매사은+무료배송 (토일렛페이퍼,멀티아이팔레트,페이스블러쉬,블러워터틴트,벨벳틴트,소프트매트립,뉴테이크 외)', 'SSG단독 블룸쿠션 럭키박스 (55%할인)', '신상품 출시 기념 홀리데이 이벤트+구매 사은품', '[바이오오일 브랜드 기획전] BEST 위너 뷰티템 단독 특가~56% + 9900원 특가 + 무료배송 + 15% 추가쿠폰혜택', '★구찌경품★ 2022 연말결산! 크나이프/지아자 연중최대할인!', '기프트 세트 20% 할인 &amp; 럭셔리 케어 증정', '핸드크림 신규츌시! 라이프 프래그런스 최대 59% 할인! (+쇼핑백 증정)', '■ 당첨 조건 및 당첨 인원 : 이벤트 기간 내 뷰티 1개 이상 구매 후 응모한 고객  중 500명 추첨 후 SSG머니 2,000원 지급', '- 해당 조건 1개 이상 구매 후 이벤트페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한하여 당첨자 추첨 후 해당 ID로 적립됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>모두의 야식을 응원합니다</t>
+          <t>2022 펫페어 어워즈</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>아침에 주문해 저녁에 받는 쓱배송 야식</t>
+          <t>20% 장바구니 쿠폰</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003209</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003136</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>(12/1~7) 모두의 야식을 응원합니다</t>
+          <t>2022 펫페어 어워즈</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (12/1~7) 모두의 야식을 응원합니다', '스마일클럽', '대한민국 경기당일 최대 1.5만원 할인쿠폰', '대한민국 경기 당일 최대 1.5만원 할인쿠폰 바로보기', '국가대표급 쓱배송 야식 바로보기', '아침에 주문하면 저녁에 딱 쓱배송으로 즐기는 야식 바로보기', '아침에 주문해서 저녁에 받는 쓱배송으로 야식을 즐겨요', '최대 1.5만원 할인쿠폰', '12월 3일 경기 딩일 오전 9시 승리 기원 선착순 쿠폰 제공', '         10% 장바구니 쿠폰', '         10만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 받으러 가기', '국가대표급 야식 야식에 딱! 쓱배송 상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; 2022 펫페어 어워즈', '스마일클럽', '선착순 혜택', '20% 할인 쿠폰', '20% 장바구니 쿠폰', '매일 600명 선착순', '20% 장바구니 쿠폰 - 4만원 이상 구매시 적용 (최대 1만원 할인)', '      쿠폰 발급 및 사용기간', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '[쓱배송] 몰리스 고양이 사료 15kg', '[무료배송]모래혁명 무향 가는입자 6kg*3개(박스)', '[무료배송/빠른출고] 에버크린 무향 19kg_2개이상구매시 분할발송', '[쓱배송] 우리와 ANF 반려견 사료 특가모음', '[로그인쿠폰] 하림펫푸드 더리얼 밥이보약 사료 모음', '[쓱배송] 강아지 오리젠,아카나 사료', '점포/네오에서 쓱배송으로! 펫프렌즈 최대 1+1 특가!', '럭셔리 애견 용품 Boooh 15% mark-down 단독', '[쓱배송] 챠오츄르 SSG 단독상품 출시! 캣 간식 행사 모음', '[고양이] 캐츠랑/프로베스트/이즈칸 대포장사료 ~40%_신세계몰 직발송', '[로그인시 최대20%]하림펫푸드 더리얼/밥이보약 고양이사료', '[쓱배송/새벽배송]프로베스트/ANF/이즈칸 캣 사료 행사', '[쓱배송] 캣간식 1+1 , 2+1 한정수량 하나더 증정!', '집사들 주목! 뽀떼/그린웨일 스크래쳐/캣타워/캣워크 할인', '[고양이 왕국] 펫페어 고양이 모래/캣타워/스크래쳐1+1/장난감 할인특가']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>홀리데이 뷰티 기프트</t>
+          <t>스마일클럽 12월의 가입 혜택</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>럭셔리&amp;트랜드뷰티 ~15%쿠폰 SSG머니 혜택까지!</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003234</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'</t>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -868,34 +868,34 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; [1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'", '스마일클럽', '뷰티 ~15% 쿠폰', '모두의 홀리데이 뷰티 ~15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '상품쿠폰 12% 선착순 - 3만원 이상 상품 구매시 최대 1만원 2천원 할인', '쿠폰은 09시부터 선착순 발급 됩니다', '트렌드뷰티 최대 5% 상품쿠폰', '상품쿠폰 5% 선착순 - 2만원 이상 상품 구매시 최대 5천원 할인', '발급 수량 : 럭셔리뷰티 12% 상품쿠폰 - 선착순 4만장, 트렌드뷰티 5% 상품쿠폰 - 선착순 3만장', '12% 상품쿠폰은 신세계백화점몰, 시코르몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용 됩니다.', '5% 상품쿠폰은 신세계몰, 이마트몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용됩니다. ', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', ' 본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다. ', 'SSG 단독 ~17% + 정품증정 구성', '피테라 에센스 리미티드 에디션 구매시', 'SSG 단독 사은 이벤트', '쿠션/섀도우/치크 외 최대 55%할인', '~45%+3만원 이상 구매시 바닐라부티크 핸드크림 증정 + 쿠폰 15% 발급', '6가지 컬러로 최대 63컬러까지 조합 가능한 아이 팔레트 UP TO 53% 특가', '[특별선물] 캐스키드슨 바디세트/핸드크림/향수/핸드클렌저 등 ~56%할인', '뷰티 어워즈 구매사은+무료배송 (토일렛페이퍼,멀티아이팔레트,페이스블러쉬,블러워터틴트,벨벳틴트,소프트매트립,뉴테이크 외)', 'SSG단독 블룸쿠션 럭키박스 (55%할인)', '신상품 출시 기념 홀리데이 이벤트+구매 사은품', '[바이오오일 브랜드 기획전] BEST 위너 뷰티템 단독 특가~56% + 9900원 특가 + 무료배송 + 15% 추가쿠폰혜택', '★구찌경품★ 2022 연말결산! 크나이프/지아자 연중최대할인!', '기프트 세트 20% 할인 &amp; 럭셔리 케어 증정', '핸드크림 신규츌시! 라이프 프래그런스 최대 59% 할인! (+쇼핑백 증정)', '■ 당첨 조건 및 당첨 인원 : 이벤트 기간 내 뷰티 1개 이상 구매 후 응모한 고객  중 500명 추첨 후 SSG머니 2,000원 지급', '- 해당 조건 1개 이상 구매 후 이벤트페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한하여 당첨자 추첨 후 해당 ID로 적립됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2022 펫페어 어워즈</t>
+          <t>프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>20% 장바구니 쿠폰</t>
+          <t>12월 할인대전</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003136</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003270</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2022 펫페어 어워즈</t>
+          <t>[1205-1211] 프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -910,66 +910,66 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2022 펫페어 어워즈', '스마일클럽', '선착순 혜택', '20% 할인 쿠폰', '20% 장바구니 쿠폰', '매일 600명 선착순', '20% 장바구니 쿠폰 - 4만원 이상 구매시 적용 (최대 1만원 할인)', '      쿠폰 발급 및 사용기간', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '[선착순핫딜]본사직영_붐펫드라이룸 K100', '[쓱배송] 몰리스 고양이 사료 15kg', '[무료배송]모래혁명 무향 가는입자 6kg*3개(박스)', '[무료배송] 에버크린 무향 19kg_2개이상구매시 분할발송', '[무료배송/빠른출고] 에버크린 무향 19kg_2개이상구매시 분할발송']</t>
+          <t>['이벤트/쿠폰 &gt; [1205-1211] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 12월 할인 대전', '최대 10% 할인 쿠폰 혜택', '혜택에 할인을 더 10% 카드청구 할인', '       10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 가격에 추가 할인이 더 12월 주요 행사', '[여성 패션 - 최대 70% 할인] 지컷/ 시슬리/ 랩 外 여성패션 특가 &amp; BEST 보러가기', '[언더웨어 - 최대 75% 할인] 노와이어 BEST 모음전, 남성 드로즈 특가 외 보러가기', '[스포츠 - 최대 70% 할인] 내셔널/ 노스페이스 등 겨울 아웃도어 BEST 보러가기', '[키즈 패션 - 최대 75% 할인] 스키복/아우터 外 겨울 상품 입고 보러가기', '[리빙 - 최대 70% 할인] 아울렛 리빙 BEST 보러가기', '[패션 슈즈 - 최대 80% 할인] 아울렛 슈즈 GIFT 전 보러가기', '[패션 잡화 - 최대 44% 할인] 골든듀/ 로제도르 30% OFF 보러가기', '[명품 잡화 - 최대 50% 할인] 미우미우/톰브라운/프라다 등 일주일 특가 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 신상 입고 보러가기', '[유니섹스 / 캐주얼 - 최대 80% 할인] 경량베스트, 점퍼 등 최고 80% OFF 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>모두투어(일본) 12/8(목) 8PM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>오사카 여행 최저가 도전! 최저 29만원~</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003279</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>모두투어(일본) @SSG.LIVE 12/8(목) 8PM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-08</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 모두투어(일본) @SSG.LIVE 12/8(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛 위크</t>
+          <t>아늑한 꿀잠을 위한 숙면테리어</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12월 할인대전</t>
+          <t>침구부터 인테리어까지, 우리집 침실 새단장 프로젝트</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003270</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003110</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[1205-1211] 프리미엄 아울렛 위크</t>
+          <t>숙면테리어</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -979,269 +979,47 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [1205-1211] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 12월 할인 대전', '최대 10% 할인 쿠폰 혜택', '혜택에 할인을 더 10% 카드청구 할인', '       10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 가격에 추가 할인이 더 12월 주요 행사', '[여성 패션 - 최대 70% 할인] 지컷/ 시슬리/ 랩 外 여성패션 특가 &amp; BEST 보러가기', '[언더웨어 - 최대 75% 할인] 노와이어 BEST 모음전, 남성 드로즈 특가 외 보러가기', '[스포츠 - 최대 70% 할인] 내셔널/ 노스페이스 등 겨울 아웃도어 BEST 보러가기', '[키즈 패션 - 최대 75% 할인] 스키복/아우터 外 겨울 상품 입고 보러가기', '[리빙 - 최대 70% 할인] 아울렛 리빙 BEST 보러가기', '[패션 슈즈 - 최대 80% 할인] 아울렛 슈즈 GIFT 전 보러가기', '[패션 잡화 - 최대 44% 할인] 골든듀/ 로제도르 30% OFF 보러가기', '[명품 잡화 - 최대 50% 할인] 미우미우/톰브라운/프라다 등 일주일 특가 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 신상 입고 보러가기', '[유니섹스 / 캐주얼 - 최대 80% 할인] 경량베스트, 점퍼 등 최고 80% OFF 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 숙면테리어', '스마일클럽', '원데이 타임딜 바로보기', '할인 상품 모아보기 바로보기', '하루에 하나씩 득템! 원데이 숙면 타임딜', '[타임딜] 클래식패브릭 헝가리 구스 SS/Q', '할인상품 모아보기']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>지라프 12/5(월) 7PM</t>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>구이바다 핫딜 10만원대 + 역대급 LIVE이벤트까지</t>
+          <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003243</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>지라프 @SSG.LIVE 12/5(월) 19:00PM</t>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 지라프 @SSG.LIVE 12/5(월) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>에고이스트 12/5(월) 9PM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>구스 다운 핫딜가 99천원 찬스! 캐리어&amp;카드지갑 증정 이벤트</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003222</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]12/5 에고이스트</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2022-11-29</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2022-12-05</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]12/5 에고이스트', '스마일클럽', '                    SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>블랑101 12/6(화) 11AM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>세탁세제 4개세트 5.8만원대+멀티클리너 본품 증정</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003252&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>[쓱라이브] 블랑101 12/6(화) 11AM</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2022-11-28</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2022-12-08</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 블랑101 12/6(화) 11AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>SK-II  12/6(화) 7PM</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>SK-II 에센스 최대 30%할인 + 홀리데이 리미티드 에디션 공개</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003284</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>SK-II @SSG.LIVE 12/6(화) 7PM</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2022-11-30</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2022-12-06</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SK-II @SSG.LIVE 12/6(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>휘닉스평창 12/6(화) 8PM</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>겨울 액티비티 성지, 휘닉스평창 올인클루시브 패키지</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003250</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>[월간호캉쓱] 휘닉스평창 @SSG.LIVE 12/6(화) 20:00PM</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2022-11-28</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2022-12-06</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [월간호캉쓱] 휘닉스평창 @SSG.LIVE 12/6(화) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>아늑한 꿀잠을 위한 숙면테리어</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>침구부터 인테리어까지, 우리집 침실 새단장 프로젝트</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003110</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>숙면테리어</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2022-12-05</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2022-12-12</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 숙면테리어', '스마일클럽', '원데이 타임딜 바로보기', '할인 상품 모아보기 바로보기', '하루에 하나씩 득템! 원데이 숙면 타임딜', '[타임딜] 클래식패브릭 헝가리 구스 SS/Q', '할인상품 모아보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2022-12-01</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Dec 12 01:36:22 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,101 +473,101 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>베스트 패션 어워즈</t>
+          <t>Wonderful Holiday</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10% 쿠폰으로 2022년 인기 브랜드 쇼핑!</t>
+          <t>기프트부터 홈파티까지 연말의 모든 것 기프트 쇼핑 10% 선착순 쿠폰</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003198</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003336</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(12/5~11) 베스트 패션 어워즈</t>
+          <t>Wonderfull Holiday 원더풀 홀리데이</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (12/5~11) 베스트 패션 어워즈', '스마일클럽', '10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매시 최대 1.2만원 할인(매일 오전 9시,선착순 1만명)', '선착순 쿠폰 sold out!', '쿠폰 발급 받기(ID당 1회 발급)', '쿠폰 발급 기간:  2022년 12월 5일(월) ~ 12월 11(일), 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간 : 2022년 12월 5일(월) ~ 12월 11(일), 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '[온앤온.올리브데올리브] 패밀리세일! 윈터 인기 아이템 ~70% OFF', '22F/W 헤지스 여성 겨울 베스트 신상 +최대 15%쿠폰', '♥사은품증정♥ FW 베스트 아우터 추가 쿠폰 헤택!', '겨울 남성 코디 제안! ! 최대 15% 할인 + 무배', '[MD추천] 지금 핫한 아우터 BEST 50 ★ 쿠폰 혜택!', 'WINTER 골프의류 및 용품 단독 ~50% OFF', '22 WINTER CAMPAIGN 오픈 + 신세계 단독 최대 30%', '★키플링BEST★ 데일리백 특가찬스 +추가할인쿠폰', '신세계 광주점 단독 특가! 핸드백&amp;지갑 ~35% OFF + 양말 사은품', '[카렌화이트] 22FW 신상&amp;베스트 특가 + 쿠폰혜택', '부츠 베스트 어워즈 ~70%+추가쿠폰', '[LUXURY WEEK] 급! 추워진 날씨도 물리칠 럭셔리 의류50종, 몽클레어/톰브라운 外 + 추가쿠폰적용가능', '[TUMI] 손흥민 PICK! 럭셔리백팩~30%OFF + 10% 쿠폰!', 'BEST 모음전! 추가 쿠폰 혜택까지', '[워치스테이션] 아르마니 BEST 시계 SALE 69%', 'BEST SELLER / 추가쿠폰혜택!', '[자주]WINTER SALE 파자마 특집전 +10%OFF']</t>
+          <t>['이벤트/쿠폰 &gt; Wonderfull Holiday 원더풀 홀리데이', '스마일클럽', '쓱배송 홈파티 먹거리', '연말 기프트 쇼핑을 도와줄 10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 1만장)', '쿠폰 발급 받기 (기간내 ID당 1회 발급)', '쿠폰 발급 기간 : 2022년 12월 12일(월) ~ 12월 18(일), 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간 : 2022년 11월 12일(월) ~ 11월 18(일), 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 상품에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니쿠폰으로 구매 건 내 대상상품 전체에 적용되며, 5만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', ' 아래 미션 중 하나 이상을 달성하고, 응모하기 버튼을 클릭하여 이벤트에 응모하세요. 추첨을 통해 당첨된 분들께 특별한 홀리데이 선물을 드립니다. 미션 2개를 모두 완료하시면 더욱 특별한 경품 찬스! ', 'Misson1. 쓱배송/새벽배송 15만원이상 구매', '쓱배송 미션 응모하기', '쓱배송에는 트레이더스 주문건도 포함됩니다.', '미션을 달성하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다.', '선물하기 또는 이벤트 해당 주문 취소 시 해당 내역은 집계 제외됩니다.', '부당한 방법으로 이벤트에 응모하였을 경우 당첨에서 제외될 수 있습니다.', '당첨자는 1월 6일(금) 이벤트 당첨자 발표 게시판을 통해 공지됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SSG Luxury Gift Week</t>
+          <t>THE GIFT GUIDE MAGICAL CHRISTMAS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 15만원 할인 쿠폰 + 연말 BEST 기프트 추천</t>
+          <t>연말 선물 추천+홀리데이 10%쿠폰</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003212&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003120</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(1205-11) SSG Luxury Gift Week</t>
+          <t>THE GIFT GUIDE Magical Christmas</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1205-11) SSG Luxury Gift Week', '스마일클럽', '# 최대 15만원 할인 쿠폰', '# 매일 오전 10시 타임딜', '01. 매일 오전 10시 럭셔리 타임딜', '02. 명품 쇼핑찬스 최대 15만원 할인쿠폰', '01. 지금만 이 가격! 매일 오전 10시 SSG Luxury 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다.', '상품쿠폰 7% - 15만원 이상 상품 구매 시, 최대 7만원 할인(선착순 5천명)', '상품쿠폰 10% - 30만원 이상 상품 구매 시, 최대 15만원 할인(선착순 5천명)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요!', '쿠폰 발급 및 유효기간: 22/12/05(월) ~ 22/12/11(일)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '본 쿠폰은 이마트몰, 신세계몰, 신세계백화점 특정 카테고리 상품 중 SSG Luxury club 상품에 적용되는 쿠폰입니다.', '쿠폰 대상 상품은 상품 상세에서 SSG Luxury club 상세 배너 확인 부탁드립니다.', '명품 상품 중에 판매가 5천원 이상 상품 구매하시고 스페셜 리뷰를 작성하면 SSG MONEY 1,000원 적립 가능!(리뷰 작성은 MY SSG &gt; 나의 활동 관리 &gt; 마이리뷰 내 ‘스페셜’ Tab에서 ‘작성 가능한 리뷰’ 에서 하실 수 있습니다.)']</t>
+          <t>['이벤트/쿠폰 &gt; THE GIFT GUIDE Magical Christmas', '스마일클럽', '01 - 홀리데이 12% 쿠폰', "발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '03 - 홀리데이 뷰티박스 이벤트', '        - 경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다.', '        - 이벤트 기간 내 경품 응모 후 주문 후 취소/반품하신 고객은 경품 응모 대상에서 제외됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '홀리데이 쇼핑은 시마을에서! 최대 15% 쿠폰 &amp; e포인트 선물하기 보너스 혜택까지 - shop']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>신세계백화점 Holiday Gift</t>
+          <t>MAGICAL CHRISTMAS</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>럭셔리 기프트 제안</t>
+          <t>프리미엄 아울렛에서 준비한 크리스마스 기프트</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003163</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003230</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[12/5-25] Magical Winter Fantasy</t>
+          <t>[12/12~25] MAGICAL CHRISTMAS - 프리미엄 아울렛</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -577,34 +577,34 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/5-25] Magical Winter Fantasy', '스마일클럽', '따뜻한 연말을 위한 네스프레소 선물 기획전 - 에센자미니 10% 할인 및 사은품 증정 보러가기', '바오밥컬렉션 신제품 출시 기념 팝업 - 마이퍼스트바오밥 신상품 최대 20%할인 &amp; 선물용 기프트포장 혜택 보러가기', 'SENNHEISSER NEW YEAR PROMOTION - CX PLUS TW SE/HD-600 최대 10% 할인 혜택 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; [12/12~25] MAGICAL CHRISTMAS - 프리미엄 아울렛', '스마일클럽', '최대 10% 할인 쿠폰 혜택', '[해외 명품 - 최대 50% 할인] 연말 맞이 나에게 주는 명품 선물 BEST 모음 보러가기', '[패션/잡화 - 최대 44% 할인] 골든듀/로제도르 30% OFF 보러가기', '[키즈 패션 - 최대 75% 할인] 아디다스키즈/게스키즈 외 BEST 보러가기', '[언더웨어 - 최대 70% 할인] 연말 맞이 언더/이지웨어 특가 &amp; BEST 모음 보러가기', '[여성 패션 - 최대 70% 할인] 연말 맞이 여성패션 특가 &amp; BEST 모음 보러가기', '[패션 슈즈 - 최대 80% 할인] 아울렛 슈즈 GIFT 전 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 상품 입고 OFF 보러가기', '[유니섹스 - 최대 80% 할인] 경량베스트, 점퍼 등 최고 80% OFF 보러가기', '[스포츠 - 최대 70% 할인] 내셔널지오그래픽/노스페이스 등 겨울 BEST 보러가기', '[리빙 - 최대 75% 할인] 웨지우드 BEST 아이템 특가 보러가기', '홀리데이 쇼핑은 시마을에서! 최대 15% 쿠폰 &amp; e포인트 선물하기 보너스 혜택까지 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>랜더스 우승기념 쓱닷컴 우승챌린지</t>
+          <t>12월 유아동 Merry Little SSG</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>우승의 기쁨을 쓱닷컴과 한번더!</t>
+          <t>유아동 ~ 2만원 쿠폰 + 크리스마스 선물가이드</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003137</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003074</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내</t>
+          <t>[12/12-18] 12월의 Merry Little SSG</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-12-06</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -614,229 +614,229 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내', '스마일클럽', '       이벤트경품', '       이벤트 기간', '       이벤트 참여 방법', '이벤트 기간 내 인스타그램을 통해 #쓱닷컴우승챌린지 에 참여한 경우 자동 응모', '이벤트 기간', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', 'SSG MONEY 지급안내', '당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 180일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', 'SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [12/12-18] 12월의 Merry Little SSG', '스마일클럽', '(현재페이지) 유아동 2만원 쿠폰받고 쇼핑 GO!', '+ 크리스마스 유아동 최대 2만원 쿠폰', '크리스마스 유아동 전용 쿠폰 최대 2만원 할인', '5% 상품쿠폰 - 1만 5천원 이상 상품 구매 시, 최대 1만원 할인', '10% 결제쿠폰 - 5만원 이상 상품 구매 시, 최대 2만원 할인', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 발급 후 12/18(일)까지', '       쿠폰 사용 조건', '       상품 쿠폰은 상품 1개 단품으로 적용 가능', '       쿠폰 발급 대상', '+PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히보기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>FW트렌드 패피위크</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>유튜버 '연우'의 연말 코디 추천 12% 쿠폰으로 트렌드지수 UP</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003338</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>FW 트렌드 패피위크</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; FW 트렌드 패피위크', '스마일클럽', "패션유튜버 '연우'와 함께 짚어보는 FW 트렌드 12% 선착순 쿠폰으로 트렌드 지수 UP", '스타일UP 12% 쿠폰찬스 바로보기', '매일 오전 9시, 트렌드 UP 찬스 12% 상품 쿠폰', '       12% 상품쿠폰', '       선착순 3천명', '       5만원 이상 구매시 최대 1만원 5천원 할인', '쿠폰 다운 받기', '오늘의 쿠폰이 소진되었습니다!', '쿠폰 사용 전 꼭 확인하세요! (레이어팝업 열기)', "대상 상품은 상품상세에서 FW트렌드 패피위크 패션유튜버 '연우' 추천상품 코디 12% 패션 상품 쿠폰까지 배너를 확인해주세요", '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 발급 기간', '      2022년 12월 12일 월요일 부터 12월 18일 일요일, 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용조건', '      적용 상품은 상품 상세에서 이벤트 엠블럼으로 확인하실 수 있습니다.', '      패피위크 참여 브랜드의 상품 중 일부 상품은 쿠폰 적용에서 제외될 수 있습니다.', '      쿠폰 사용 가능 대상']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>랜더스 우승기념 쓱닷컴 우승챌린지</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>우승의 기쁨을 쓱닷컴과 한번더!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003137</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-12-06</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내', '스마일클럽', '       이벤트경품', '       이벤트 기간', '       이벤트 참여 방법', '이벤트 기간 내 인스타그램을 통해 #쓱닷컴우승챌린지 에 참여한 경우 자동 응모', '이벤트 기간', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', 'SSG MONEY 지급안내', '당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 180일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', 'SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>공유 &amp; 공효진 무물 대공개</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>궁금증을 쓱-풀어보세요</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>캡틴쓱 : 게임 체인저</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>친환경 인식 개선 캠페인</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003079</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 친환경 캠페인 &lt;캡틴쓱 : 게임 체인저&gt;', '스마일클럽', '전기차 쓱배송 차량 캐릭터 - 전기차 쓱카', '쓱배송 차량의 전기차 브로! 착실하고 우직한 성격으로 쓱배송을 전담하고 있다. 명석한 두뇌로 최적의 루트를 빠르게 분석한다.', '첫 번째 이벤트 - 메타버스 캡틴쓱 본부 내 모든 스테이지 참여 시 추첨을 통해 친환경 키트 혹은 신세계 모바일 상품권 5천원권', '두 번째 이벤트 - 스테이지 4에서 최단 기록 10명 대상으로 날마다 신세계 모바일 상품권 5천원권 증정', '세 번째 이벤트 - 보너스 스테이지 참여자 대상으로 추첨을 통해 스타벅스 기프트카드 1만원권 증정', ' 미션 종료 후 이벤트 참여 및 리워드 제공을 위해 테라사이클 코리아에서 개인정보를 수집할 수 있습니다. 자세한 이벤트 내용은 해당 스테이지 내 안내 문구를 참고해주세요. PC로 참여하시는 경우, 크롬 브라우저를 통해 입장해주시길 바랍니다. ', '       인스타그램 이벤트 계정에 들어가서 게시글을 눌러가며 힌트를 얻어 곰인형을 구해주세요. 마지막 단계에서 댓글 작성 시, 댓글 수에 따라 기부가 진행됩니다.', '자세한 이벤트 내용은 해당 게시글 내 안내 문구를 참고해주세요.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>홀리데이 뷰티 기프트</t>
+          <t>오반장위크 2022 연말결산</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>럭셔리&amp;트랜드뷰티 ~15%쿠폰 SSG머니 혜택까지!</t>
+          <t>BEST ITEM 앵콜특가 + 연말 추천 필수템</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003234</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003385</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'</t>
+          <t>(12/12~18) 오반장위크_2022 연말결산</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; [1205~1211] 12월 먼데이문 위크 '홀리데이 뷰티 기프트'", '스마일클럽', '뷰티 ~15% 쿠폰', '모두의 홀리데이 뷰티 ~15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '상품쿠폰 12% 선착순 - 3만원 이상 상품 구매시 최대 1만원 2천원 할인', '쿠폰은 09시부터 선착순 발급 됩니다', '트렌드뷰티 최대 5% 상품쿠폰', '상품쿠폰 5% 선착순 - 2만원 이상 상품 구매시 최대 5천원 할인', '발급 수량 : 럭셔리뷰티 12% 상품쿠폰 - 선착순 4만장, 트렌드뷰티 5% 상품쿠폰 - 선착순 3만장', '12% 상품쿠폰은 신세계백화점몰, 시코르몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용 됩니다.', '5% 상품쿠폰은 신세계몰, 이마트몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용됩니다. ', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', ' 본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다. ', 'SSG 단독 ~17% + 정품증정 구성', '피테라 에센스 리미티드 에디션 구매시', 'SSG 단독 사은 이벤트', '쿠션/섀도우/치크 외 최대 55%할인', '크리스마스 에디션 UP TO 15%', '~45%+3만원 이상 구매시 바닐라부티크 핸드크림 증정 + 쿠폰 15% 발급', '6가지 컬러로 최대 63컬러까지 조합 가능한 아이 팔레트 UP TO 53% 특가', '[특별선물] 캐스키드슨 2022 홀리데이 에디션 ~56%할인', '뷰티 어워즈 구매사은+무료배송 (토일렛페이퍼,멀티아이팔레트,페이스블러쉬,블러워터틴트,벨벳틴트,소프트매트립,뉴테이크 외)', 'SSG단독 블룸쿠션 럭키박스 (55%할인)', '신상품 출시 기념 홀리데이 이벤트+구매 사은품', '[바이오오일 브랜드 기획전] BEST 위너 뷰티템 단독 특가~56% + 9900원 특가 + 무료배송 + 15% 추가쿠폰혜택', '★구찌경품★ 2022 연말결산! 크나이프/지아자 연중최대할인!', '기프트 세트 20% 할인 &amp; 럭셔리 케어 증정', '핸드크림 신규츌시! 라이프 프래그런스 최대 59% 할인! (+쇼핑백 증정)', '■ 당첨 조건 및 당첨 인원 : 이벤트 기간 내 뷰티 1개 이상 구매 후 응모한 고객  중 500명 추첨 후 SSG머니 2,000원 지급', '- 해당 조건 1개 이상 구매 후 이벤트페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한하여 당첨자 추첨 후 해당 ID로 적립됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (12/12~18) 오반장위크_2022 연말결산', '스마일클럽', 'NEW 이마트몰 앱 다운받으면 SSG머니 5천원 증정! 이벤트까지']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2022 펫페어 어워즈</t>
+          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>20% 장바구니 쿠폰</t>
+          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003136</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022 펫페어 어워즈</t>
+          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2022 펫페어 어워즈', '스마일클럽', '선착순 혜택', '20% 할인 쿠폰', '20% 장바구니 쿠폰', '매일 600명 선착순', '20% 장바구니 쿠폰 - 4만원 이상 구매시 적용 (최대 1만원 할인)', '      쿠폰 발급 및 사용기간', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '[쓱배송] 몰리스 고양이 사료 15kg', '[무료배송]모래혁명 무향 가는입자 6kg*3개(박스)', '[무료배송/빠른출고] 에버크린 무향 19kg_2개이상구매시 분할발송', '[쓱배송] 우리와 ANF 반려견 사료 특가모음', '[로그인쿠폰] 하림펫푸드 더리얼 밥이보약 사료 모음', '[쓱배송] 강아지 오리젠,아카나 사료', '점포/네오에서 쓱배송으로! 펫프렌즈 최대 1+1 특가!', '럭셔리 애견 용품 Boooh 15% mark-down 단독', '[쓱배송] 챠오츄르 SSG 단독상품 출시! 캣 간식 행사 모음', '[고양이] 캐츠랑/프로베스트/이즈칸 대포장사료 ~40%_신세계몰 직발송', '[로그인시 최대20%]하림펫푸드 더리얼/밥이보약 고양이사료', '[쓱배송/새벽배송]프로베스트/ANF/이즈칸 캣 사료 행사', '[쓱배송] 캣간식 1+1 , 2+1 한정수량 하나더 증정!', '집사들 주목! 뽀떼/그린웨일 스크래쳐/캣타워/캣워크 할인', '[고양이 왕국] 펫페어 고양이 모래/캣타워/스크래쳐1+1/장난감 할인특가']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
         </is>
       </c>
     </row>
@@ -873,66 +873,66 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM X MEGABOX 스마일클럽은 더욱 특별한 가격으로! 메가박스 2D/3D 영화 관람권 &amp; 팝콘 핫딜', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛 위크</t>
+          <t>홀리데이 주얼리 12/13(화) 8PM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12월 할인대전</t>
+          <t>골든듀/디디에두보/제이에스티나 ~79% OFF!</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003270</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003318</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[1205-1211] 프리미엄 아울렛 위크</t>
+          <t>[SSG.LIVE]골든듀/디디에두보/제이에스티나</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-13</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [1205-1211] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 12월 할인 대전', '최대 10% 할인 쿠폰 혜택', '혜택에 할인을 더 10% 카드청구 할인', '       10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 가격에 추가 할인이 더 12월 주요 행사', '[여성 패션 - 최대 70% 할인] 지컷/ 시슬리/ 랩 外 여성패션 특가 &amp; BEST 보러가기', '[언더웨어 - 최대 75% 할인] 노와이어 BEST 모음전, 남성 드로즈 특가 외 보러가기', '[스포츠 - 최대 70% 할인] 내셔널/ 노스페이스 등 겨울 아웃도어 BEST 보러가기', '[키즈 패션 - 최대 75% 할인] 스키복/아우터 外 겨울 상품 입고 보러가기', '[리빙 - 최대 70% 할인] 아울렛 리빙 BEST 보러가기', '[패션 슈즈 - 최대 80% 할인] 아울렛 슈즈 GIFT 전 보러가기', '[패션 잡화 - 최대 44% 할인] 골든듀/ 로제도르 30% OFF 보러가기', '[명품 잡화 - 최대 50% 할인] 미우미우/톰브라운/프라다 등 일주일 특가 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 신상 입고 보러가기', '[유니섹스 / 캐주얼 - 최대 80% 할인] 경량베스트, 점퍼 등 최고 80% OFF 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]골든듀/디디에두보/제이에스티나', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>모두투어(일본) 12/8(목) 8PM</t>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>오사카 여행 최저가 도전! 최저 29만원~</t>
+          <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003279</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>모두투어(일본) @SSG.LIVE 12/8(목) 8PM</t>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -942,84 +942,10 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-12-08</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 모두투어(일본) @SSG.LIVE 12/8(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>아늑한 꿀잠을 위한 숙면테리어</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>침구부터 인테리어까지, 우리집 침실 새단장 프로젝트</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003110</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>숙면테리어</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2022-12-05</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2022-12-12</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 숙면테리어', '스마일클럽', '원데이 타임딜 바로보기', '할인 상품 모아보기 바로보기', '하루에 하나씩 득템! 원데이 숙면 타임딜', '[타임딜] 클래식패브릭 헝가리 구스 SS/Q', '할인상품 모아보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2022-12-01</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Dec 15 01:36:55 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Wonderfull Holiday 원더풀 홀리데이', '스마일클럽', '쓱배송 홈파티 먹거리', '연말 기프트 쇼핑을 도와줄 10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 1만장)', '쿠폰 발급 받기 (기간내 ID당 1회 발급)', '쿠폰 발급 기간 : 2022년 12월 12일(월) ~ 12월 18(일), 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간 : 2022년 11월 12일(월) ~ 11월 18(일), 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 상품에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니쿠폰으로 구매 건 내 대상상품 전체에 적용되며, 5만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', ' 아래 미션 중 하나 이상을 달성하고, 응모하기 버튼을 클릭하여 이벤트에 응모하세요. 추첨을 통해 당첨된 분들께 특별한 홀리데이 선물을 드립니다. 미션 2개를 모두 완료하시면 더욱 특별한 경품 찬스! ', 'Misson1. 쓱배송/새벽배송 15만원이상 구매', '쓱배송 미션 응모하기', '쓱배송에는 트레이더스 주문건도 포함됩니다.', '미션을 달성하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다.', '선물하기 또는 이벤트 해당 주문 취소 시 해당 내역은 집계 제외됩니다.', '부당한 방법으로 이벤트에 응모하였을 경우 당첨에서 제외될 수 있습니다.', '당첨자는 1월 6일(금) 이벤트 당첨자 발표 게시판을 통해 공지됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다']</t>
+          <t>['이벤트/쿠폰 &gt; Wonderfull Holiday 원더풀 홀리데이', '스마일클럽', '쓱배송 홈파티 먹거리', '연말 기프트 쇼핑을 도와줄 10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 1만장)', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 2만장)', '쿠폰 발급 받기 (기간내 ID당 1회 발급)', '       쿠폰 발급 기간', '       2022년 12월 12일(월) ~ 12월 18(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '쿠폰은 매일 선착순 2만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 상품에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니쿠폰으로 구매 건 내 대상상품 전체에 적용되며, 5만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', ' 아래 미션 중 하나 이상을 달성하고, 응모하기 버튼을 클릭하여 이벤트에 응모하세요. 추첨을 통해 당첨된 분들께 특별한 홀리데이 선물을 드립니다. 미션 2개를 모두 완료하시면 더욱 특별한 경품 찬스! ', 'Misson1. 쓱배송/새벽배송 15만원이상 구매', '쓱배송 미션 응모하기', '쓱배송에는 트레이더스 주문건도 포함됩니다.', '미션을 달성하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다.', '선물하기 또는 이벤트 해당 주문 취소 시 해당 내역은 집계 제외됩니다.', '부당한 방법으로 이벤트에 응모하였을 경우 당첨에서 제외될 수 있습니다.', '당첨자는 1월 6일(금) 이벤트 당첨자 발표 게시판을 통해 공지됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다']</t>
         </is>
       </c>
     </row>
@@ -584,59 +584,59 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>12월 유아동 Merry Little SSG</t>
+          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>유아동 ~ 2만원 쿠폰 + 크리스마스 선물가이드</t>
+          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003074</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[12/12-18] 12월의 Merry Little SSG</t>
+          <t>선물하기로 쓱- 마음을 전하세요</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/12-18] 12월의 Merry Little SSG', '스마일클럽', '(현재페이지) 유아동 2만원 쿠폰받고 쇼핑 GO!', '+ 크리스마스 유아동 최대 2만원 쿠폰', '크리스마스 유아동 전용 쿠폰 최대 2만원 할인', '5% 상품쿠폰 - 1만 5천원 이상 상품 구매 시, 최대 1만원 할인', '10% 결제쿠폰 - 5만원 이상 상품 구매 시, 최대 2만원 할인', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 발급 후 12/18(일)까지', '       쿠폰 사용 조건', '       상품 쿠폰은 상품 1개 단품으로 적용 가능', '       쿠폰 발급 대상', '+PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히보기']</t>
+          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FW트렌드 패피위크</t>
+          <t>12월 유아동 Merry Little SSG</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>유튜버 '연우'의 연말 코디 추천 12% 쿠폰으로 트렌드지수 UP</t>
+          <t>유아동 ~ 2만원 쿠폰 + 크리스마스 선물가이드</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003338</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003074</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FW 트렌드 패피위크</t>
+          <t>[12/12-18] 12월의 Merry Little SSG</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -651,34 +651,34 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; FW 트렌드 패피위크', '스마일클럽', "패션유튜버 '연우'와 함께 짚어보는 FW 트렌드 12% 선착순 쿠폰으로 트렌드 지수 UP", '스타일UP 12% 쿠폰찬스 바로보기', '매일 오전 9시, 트렌드 UP 찬스 12% 상품 쿠폰', '       12% 상품쿠폰', '       선착순 3천명', '       5만원 이상 구매시 최대 1만원 5천원 할인', '쿠폰 다운 받기', '오늘의 쿠폰이 소진되었습니다!', '쿠폰 사용 전 꼭 확인하세요! (레이어팝업 열기)', "대상 상품은 상품상세에서 FW트렌드 패피위크 패션유튜버 '연우' 추천상품 코디 12% 패션 상품 쿠폰까지 배너를 확인해주세요", '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 발급 기간', '      2022년 12월 12일 월요일 부터 12월 18일 일요일, 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용조건', '      적용 상품은 상품 상세에서 이벤트 엠블럼으로 확인하실 수 있습니다.', '      패피위크 참여 브랜드의 상품 중 일부 상품은 쿠폰 적용에서 제외될 수 있습니다.', '      쿠폰 사용 가능 대상']</t>
+          <t>['이벤트/쿠폰 &gt; [12/12-18] 12월의 Merry Little SSG', '스마일클럽', '(현재페이지) 유아동 2만원 쿠폰받고 쇼핑 GO!', '+ 크리스마스 유아동 최대 2만원 쿠폰', '크리스마스 유아동 전용 쿠폰 최대 2만원 할인', '5% 상품쿠폰 - 1만 5천원 이상 상품 구매 시, 최대 1만원 할인', '10% 결제쿠폰 - 5만원 이상 상품 구매 시, 최대 2만원 할인', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 발급 후 12/18(일)까지', '       쿠폰 사용 조건', '       상품 쿠폰은 상품 1개 단품으로 적용 가능', '       쿠폰 발급 대상', '+PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히보기']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>랜더스 우승기념 쓱닷컴 우승챌린지</t>
+          <t>FW트렌드 패피위크</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>우승의 기쁨을 쓱닷컴과 한번더!</t>
+          <t>유튜버 '연우'의 연말 코디 추천 12% 쿠폰으로 트렌드지수 UP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003137</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003338</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내</t>
+          <t>FW 트렌드 패피위크</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-12-06</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,264 +688,375 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내', '스마일클럽', '       이벤트경품', '       이벤트 기간', '       이벤트 참여 방법', '이벤트 기간 내 인스타그램을 통해 #쓱닷컴우승챌린지 에 참여한 경우 자동 응모', '이벤트 기간', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', 'SSG MONEY 지급안내', '당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 180일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', 'SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; FW 트렌드 패피위크', '스마일클럽', "패션유튜버 '연우'와 함께 짚어보는 FW 트렌드 12% 선착순 쿠폰으로 트렌드 지수 UP", '스타일UP 12% 쿠폰찬스 바로보기', '매일 오전 9시, 트렌드 UP 찬스 12% 상품 쿠폰', '       12% 상품쿠폰', '       선착순 3천명', '       5만원 이상 구매시 최대 1만원 5천원 할인', '쿠폰 다운 받기', '오늘의 쿠폰이 소진되었습니다!', '쿠폰 사용 전 꼭 확인하세요! (레이어팝업 열기)', "대상 상품은 상품상세에서 FW트렌드 패피위크 패션유튜버 '연우' 추천상품 코디 12% 패션 상품 쿠폰까지 배너를 확인해주세요", '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 발급 기간', '      2022년 12월 12일 월요일 부터 12월 18일 일요일, 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용조건', '      적용 상품은 상품 상세에서 이벤트 엠블럼으로 확인하실 수 있습니다.', '      패피위크 참여 브랜드의 상품 중 일부 상품은 쿠폰 적용에서 제외될 수 있습니다.', '      쿠폰 사용 가능 대상']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>랜더스 우승기념 쓱닷컴 우승챌린지</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>우승의 기쁨을 쓱닷컴과 한번더!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003137</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-12-06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내', '스마일클럽', '       이벤트경품', '       이벤트 기간', '       이벤트 참여 방법', '이벤트 기간 내 인스타그램을 통해 #쓱닷컴우승챌린지 에 참여한 경우 자동 응모', '이벤트 기간', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', 'SSG MONEY 지급안내', '당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 180일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', 'SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>오반장위크 2022 연말결산</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BEST ITEM 앵콜특가 + 연말 추천 필수템</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003385</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(12/12~18) 오반장위크_2022 연말결산</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (12/12~18) 오반장위크_2022 연말결산', '스마일클럽', 'NEW 이마트몰 앱 다운받으면 SSG머니 5천원 증정! 이벤트까지']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
+          <t>오반장위크 2022 연말결산</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
+          <t>BEST ITEM 앵콜특가 + 연말 추천 필수템</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003385</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
+          <t>(12/12~18) 오반장위크_2022 연말결산</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
+          <t>['이벤트/쿠폰 &gt; (12/12~18) 오반장위크_2022 연말결산', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>All About Strawberries</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>제철딸기 ~50% 도레도레 케이크 20% 쿠폰까지</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003408</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>All About Strawberries 올 어바웃 스트로베리 ♥</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-21</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM X MEGABOX 스마일클럽은 더욱 특별한 가격으로! 메가박스 2D/3D 영화 관람권 &amp; 팝콘 핫딜', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; All About Strawberries 올 어바웃 스트로베리 ♥', '스마일클럽', '딸기 단품 구매 시 최대 50% 할인', '딸기 베이커리 신상품 구매 시 20% 할인', 'BENEFIT 딸기가 가장 맛있는 지금, 최대 50% 할인 혜택', '#달달상큼 #풍부한과즙 눈 속에서 맛보는 봄의 맛, 베스트셀러 설향딸기 정상가 : 17,800원 &gt; 할인가 : 10,680원 보러가기', '#SNS하얀딸기 #알프스딸기 #이색과일 눈꽃처럼 하얀 속살의 달콤함, 설희딸기 정상가 : 21,800원 &gt; 할인가 : 15,260원 보러가기', '#고당도 #진한향기 새콤달콤 풍부한 향, 한단딸기 정상가 : 16,800원 &gt; 할인가 : 8,400원 보러가기', '#왕크왕맛 #풍부한과즙 #복숭아향 과즙도 단맛도 풍성한 왕의 딸기, 킹스베리 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#부드러워요 #쉐이크용 #잼용 날씬한 몸매를 뽐내는, 장희딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#단단해요 #새콤달콤 달큰한 비타민 C의 여왕, 금실딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', 'BENEFIT 도레도레부터 몽상클레르까지 딸기 베이커리 신상품 20% 할인 쿠폰', '푸드마켓 딸기 베이커리 신상품 20% 쿠폰할인(22.12.15 ~ 22.12.21)', '#홀리데이 #홈파티 #딸기요거트 도레도레와 함께하는 크리스마스 ♥ 산타요정 딸기요거트생크림 케이크 정상가 : 39,000원 &gt; 할인가 : 28,080원 보러가기', '#딸기우유맛 #산뜻달달 유크림과 딸기잼으로 가득 채운 오르�逼＠箝옇� 딸기크러핀 정상가 : 4,800원 &gt; 할인가 : 3,840원 보러가기', '#바삭달콤 #티타임 #64겹파이 바삭한 식감 뒤로 전해지는 진한 풍미 몽상클레르 딸기팔미에 정상가 : 5,000원 &gt; 할인가 : 4,000원 보러가기', '할인 적용 기간 : 2022년 12월 15일(목)~21일(수)', 'BENEFIT SSG 푸드마켓 딸기 페어링 EVENT 추천푸드 20% 할인!', '상품 상세에서 SSG 푸드마켓과 할인 혜택을 확인해주세요 :)', '엠블럼으로도 확인 가능! (SSG 푸드마켓 딸기 동시 구매 시 20% 할인 대상 상품)', '       할인 적용 기간', '       할인 조건', '       - 본 이벤트페이지에서 소개하는 SSG 푸드마켓 딸기 동시구매 이벤트에 적용되는 혜택입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → O', '       ex) 푸드마켓 브랜드가 아닌 딸기 + 20% 할인 배너 구매시 → X', '       - 딸기와 함께 구매 시 전체금액의 20%가 아닌 동시구매되는 푸드 상품에 대한 20% 할인입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → 할인배너 상품 20% 할인']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>홀리데이 주얼리 12/13(화) 8PM</t>
+          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>골든듀/디디에두보/제이에스티나 ~79% OFF!</t>
+          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003318</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]골든듀/디디에두보/제이에스티나</t>
+          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2022-12-13</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]골든듀/디디에두보/제이에스티나', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>스마일클럽 12월의 가입 혜택</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2022-12-05</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2022-12-31</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM X MEGABOX 스마일클럽은 더욱 특별한 가격으로! 메가박스 2D/3D 영화 관람권 &amp; 팝콘 핫딜', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>메가박스 영화예매권 핫딜</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>스마일클럽 전용 Exclusive Price !</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003308</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>[SSG.COM x 메가박스] 영화관람권 &amp; 팝콘 스페셜 할인 혜택</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-12-14</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2022-12-18</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [SSG.COM x 메가박스] 영화관람권 &amp; 팝콘 스페셜 할인 혜택', '스마일클럽', '[SSG.COM x 메가박스] 영화관람권 &amp; 팝콘 스페셜 할인 혜택', ' 스마일클럽 무료 가입하기 ', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 소중한 사람과 함께하는 연말을 더욱 즐겁게!', '영화 관람권 &amp; 팝콘 스페셜 할인 혜택', '       기존금액 : 13,000원 / 할인금액 : 8,500원', '       기존금액 : 5,500원 / 할인금액 : 2,500원', '영화 관람권 스페셜 할인 혜택', '       기존금액 : 13,000원 / 할인금액 : 9,100원', '3D 영화 관람권 스페셜 할인 혜택', '       기존금액 : 16,000원 / 할인금액 : 11,000원']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>비발디파크 12/15(목) 8PM</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>발디파크 1박 + 스노위랜드 3인 종일권 선착순 핫딜</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003372&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>[쓱라이브] 비발디파크 12/15(목) 8PM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022-12-07</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2022-12-17</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 비발디파크 12/15(목) 8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>2022-12-01</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>2022-12-31</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Dec 19 01:21:01 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Wonderfull Holiday 원더풀 홀리데이', '스마일클럽', '쓱배송 홈파티 먹거리', '연말 기프트 쇼핑을 도와줄 10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 1만장)', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 2만장)', '쿠폰 발급 받기 (기간내 ID당 1회 발급)', '       쿠폰 발급 기간', '       2022년 12월 12일(월) ~ 12월 18(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '쿠폰은 매일 선착순 2만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 상품에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니쿠폰으로 구매 건 내 대상상품 전체에 적용되며, 5만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', ' 아래 미션 중 하나 이상을 달성하고, 응모하기 버튼을 클릭하여 이벤트에 응모하세요. 추첨을 통해 당첨된 분들께 특별한 홀리데이 선물을 드립니다. 미션 2개를 모두 완료하시면 더욱 특별한 경품 찬스! ', 'Misson1. 쓱배송/새벽배송 15만원이상 구매', '쓱배송 미션 응모하기', '쓱배송에는 트레이더스 주문건도 포함됩니다.', '미션을 달성하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다.', '선물하기 또는 이벤트 해당 주문 취소 시 해당 내역은 집계 제외됩니다.', '부당한 방법으로 이벤트에 응모하였을 경우 당첨에서 제외될 수 있습니다.', '당첨자는 1월 6일(금) 이벤트 당첨자 발표 게시판을 통해 공지됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다']</t>
+          <t>['이벤트/쿠폰 &gt; Wonderfull Holiday 원더풀 홀리데이', '스마일클럽', '쓱배송 파티 푸드', '연말 기프트 쇼핑을 도와줄 10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 1만장)', '쿠폰 발급 받기 (기간내 ID당 1회 발급)', '       쿠폰 발급 기간', '       2022년 12월 19일(월) ~ 12월 25(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 상품에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니쿠폰으로 구매 건 내 대상상품 전체에 적용되며, 5만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '아래 미션 중 하나 이상을 달성하고, 응모하기 버튼을 클릭하여 이벤트에 응모하세요. 추첨을 통해 당첨된 분들께 특별한 홀리데이 선물을 드립니다. 미션 2개를 모두 완료하시면 더욱 특별한 경품 찬스!', 'Misson1. 쓱배송/새벽배송 15만원이상 구매', '쓱배송 미션 응모하기', '쓱배송에는 트레이더스 주문건도 포함됩니다.', '미션을 달성하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다.', '선물하기 또는 이벤트 해당 주문 취소 시 해당 내역은 집계 제외됩니다.', '부당한 방법으로 이벤트에 응모하였을 경우 당첨에서 제외될 수 있습니다.', '당첨자는 1월 6일(금) 이벤트 당첨자 발표 게시판을 통해 공지됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다']</t>
         </is>
       </c>
     </row>
@@ -584,323 +584,323 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
+          <t>반값다~딜</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
+          <t>첫구매는 네개 다 반값!  + 무료배송 쿠폰</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003404&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>선물하기로 쓱- 마음을 전하세요</t>
+          <t>첫구매는 네개다 반값! 반값다딜</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 첫구매는 네개다 반값! 반값다딜', '스마일클럽', '첫구매는 네개다 반값! 반값다딜', '첫구매는 네개 다 반값! 게다가 무료배송', '반값다 딜 50%', '반값다딜 쿠폰이 모두 소진되었습니다. 더 좋은 이벤트로 찾아뵙겠습니다.', '첫구매는 네개 모두 다 반값!', '오늘의 반값쿠폰', '       이마트몰, 쓱배송/새벽배송', '       딸기 50% 할인 (첫 구매 전용)', '       딸기 cat 최대 5천원 할인', '       흰우유 50% 할인 (첫 구매 전용)', '       흰우유 cat 최대 2천원 할인', '       봉지라면 50% 할인 (첫 구매 전용)', '       봉지라면 cat 최대 2천원 할인', '       식빵 50% 할인 (첫 구매 전용)', '       식빵 cat 최대 2천원 할인', '       쓱배송 첫구매 무료배송 (첫 구매 전용)', '       2만원 이상 구매시 사용 가능', '첫구매 쿠폰 모두 한번에 받기', '       2021년 12월 18일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매이력이 없는 고객 한정', '       쿠폰 발급 기간', '       쿠폰 사용기간', '       상품할인 쿠폰 : 2022년 12월 19일(월) 부터 25일(일) 까지', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용대상', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 우유 1개, 딸기 1개, 라면 1개, 식빵 1개 적용 가능! 딸기 2개 구매시 1개에만 적용 가능합니다', '첫구매 쿠폰 CAT', '       딸기 50% cat', '       우유 50% cat', '       식빵 50% cat', '       봉지라면 50% cat', '       쿠폰 발급 대상', '첫구매 전용 오늘의 상품 보기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>12월 유아동 Merry Little SSG</t>
+          <t>SSG 브랜드 스포트라이트: 레고</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>유아동 ~ 2만원 쿠폰 + 크리스마스 선물가이드</t>
+          <t>크리스마스 특별 할인부터 사은품SET 증정까지!</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003074</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003346</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[12/12-18] 12월의 Merry Little SSG</t>
+          <t>SSG 브랜드 스포트라이트 - 레고</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/12-18] 12월의 Merry Little SSG', '스마일클럽', '(현재페이지) 유아동 2만원 쿠폰받고 쇼핑 GO!', '+ 크리스마스 유아동 최대 2만원 쿠폰', '크리스마스 유아동 전용 쿠폰 최대 2만원 할인', '5% 상품쿠폰 - 1만 5천원 이상 상품 구매 시, 최대 1만원 할인', '10% 결제쿠폰 - 5만원 이상 상품 구매 시, 최대 2만원 할인', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 발급 후 12/18(일)까지', '       쿠폰 사용 조건', '       상품 쿠폰은 상품 1개 단품으로 적용 가능', '       쿠폰 발급 대상', '+PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 레고', '스마일클럽', " 01. '레고 아바타 시리즈' 행사상품 구매 시, SSG MONEY 10% 적립 ※ 이벤트 페이지 내 레고 아바타 시리즈 4개 상품에만 해당됩니다. ", " 02. '레고 BEST 시리즈' 행사상품 20% 할인 ※ 이벤트 페이지 내 레고 BEST 시리즈 4개 상품에만 해당됩니다. "]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FW트렌드 패피위크</t>
+          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>유튜버 '연우'의 연말 코디 추천 12% 쿠폰으로 트렌드지수 UP</t>
+          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003338</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FW 트렌드 패피위크</t>
+          <t>선물하기로 쓱- 마음을 전하세요</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; FW 트렌드 패피위크', '스마일클럽', "패션유튜버 '연우'와 함께 짚어보는 FW 트렌드 12% 선착순 쿠폰으로 트렌드 지수 UP", '스타일UP 12% 쿠폰찬스 바로보기', '매일 오전 9시, 트렌드 UP 찬스 12% 상품 쿠폰', '       12% 상품쿠폰', '       선착순 3천명', '       5만원 이상 구매시 최대 1만원 5천원 할인', '쿠폰 다운 받기', '오늘의 쿠폰이 소진되었습니다!', '쿠폰 사용 전 꼭 확인하세요! (레이어팝업 열기)', "대상 상품은 상품상세에서 FW트렌드 패피위크 패션유튜버 '연우' 추천상품 코디 12% 패션 상품 쿠폰까지 배너를 확인해주세요", '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 발급 기간', '      2022년 12월 12일 월요일 부터 12월 18일 일요일, 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용조건', '      적용 상품은 상품 상세에서 이벤트 엠블럼으로 확인하실 수 있습니다.', '      패피위크 참여 브랜드의 상품 중 일부 상품은 쿠폰 적용에서 제외될 수 있습니다.', '      쿠폰 사용 가능 대상']</t>
+          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>랜더스 우승기념 쓱닷컴 우승챌린지</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>우승의 기쁨을 쓱닷컴과 한번더!</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003137</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-12-06</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG랜더스 통합우승 기념]쓱닷컴 우승 챌린지 안내', '스마일클럽', '       이벤트경품', '       이벤트 기간', '       이벤트 참여 방법', '이벤트 기간 내 인스타그램을 통해 #쓱닷컴우승챌린지 에 참여한 경우 자동 응모', '이벤트 기간', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품안내 완료 후 즉시 파기됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '이벤트에 대한 세부사항 및 경품내용은 당사 및 제휴관계사 사정에 의해 조기 종료 및 변경될 수 있습니다.', 'SSG MONEY 지급안내', '당첨된 SSG MONEY는 당첨 즉시 응모하신 계정으로 지급되며, 지급일로부터 180일동안 사용 가능합니다.(유효기간 경과 시 자동 소멸)', 'SSG MONEY 사용가능 대상상품은 이마트몰, 트레이더스몰, 새벽배송 쓱배송 상품을 비롯한 SSG.COM 전체 상품에 해당되며, 일부 브랜드 및 특가상품, 여행/쿠폰 등의 서비스 상품은 제외됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>All About Strawberries</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>제철딸기 ~50% 도레도레 케이크 20% 쿠폰까지</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003408</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>All About Strawberries 올 어바웃 스트로베리 ♥</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2022-12-21</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; All About Strawberries 올 어바웃 스트로베리 ♥', '스마일클럽', '딸기 단품 구매 시 최대 50% 할인', '딸기 베이커리 신상품 구매 시 20% 할인', 'BENEFIT 딸기가 가장 맛있는 지금, 최대 50% 할인 혜택', '#달달상큼 #풍부한과즙 눈 속에서 맛보는 봄의 맛, 베스트셀러 설향딸기 정상가 : 17,800원 &gt; 할인가 : 10,680원 보러가기', '#SNS하얀딸기 #알프스딸기 #이색과일 눈꽃처럼 하얀 속살의 달콤함, 설희딸기 정상가 : 21,800원 &gt; 할인가 : 15,260원 보러가기', '#고당도 #진한향기 새콤달콤 풍부한 향, 한단딸기 정상가 : 16,800원 &gt; 할인가 : 8,400원 보러가기', '#왕크왕맛 #풍부한과즙 #복숭아향 과즙도 단맛도 풍성한 왕의 딸기, 킹스베리 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#부드러워요 #쉐이크용 #잼용 날씬한 몸매를 뽐내는, 장희딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#단단해요 #새콤달콤 달큰한 비타민 C의 여왕, 금실딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '눈 속에서 맛보는 봄의 맛, 베스트셀러 설향딸기 정상가 : 12,900원~ &gt; 할인가 : 10,900원~ 보러가기', '날씬한 몸매를 뽐내는, 장희딸기 정상가 : 20,900원~ &gt; 할인가 : 19,900원~ 보러가기', '달큰한 비타민 C의 여왕, 금실딸기 정상가 : 17,900원 &gt; 할인가 : 15,900원 보러가기', 'BENEFIT 도레도레부터 몽상클레르까지 딸기 베이커리 신상품 20% 할인 쿠폰', '푸드마켓 딸기 베이커리 신상품 20% 쿠폰할인(22.12.15 ~ 22.12.21)', '#홀리데이 #홈파티 #딸기요거트 도레도레와 함께하는 크리스마스 ♥ 산타요정 딸기요거트생크림 케이크 정상가 : 39,000원 &gt; 할인가 : 28,080원 보러가기', '#딸기우유맛 #산뜻달달 유크림과 딸기잼으로 가득 채운 오르�逼＠箝옇� 딸기크러핀 정상가 : 4,800원 &gt; 할인가 : 3,840원 보러가기', '#바삭달콤 #티타임 #64겹파이 바삭한 식감 뒤로 전해지는 진한 풍미 몽상클레르 딸기팔미에 정상가 : 5,000원 &gt; 할인가 : 4,000원 보러가기', '할인 적용 기간 : 2022년 12월 15일(목)~21일(수)', 'BENEFIT SSG 푸드마켓 딸기 페어링 EVENT 추천푸드 20% 할인!', '상품 상세에서 SSG 푸드마켓과 할인 혜택을 확인해주세요 :)', '엠블럼으로도 확인 가능! (SSG 푸드마켓 딸기 동시 구매 시 20% 할인 대상 상품)', '       할인 적용 기간', '       할인 조건', '       - 본 이벤트페이지에서 소개하는 SSG 푸드마켓 딸기 동시구매 이벤트에 적용되는 혜택입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → O', '       ex) 푸드마켓 브랜드가 아닌 딸기 + 20% 할인 배너 구매시 → X', '       - 딸기와 함께 구매 시 전체금액의 20%가 아닌 동시구매되는 푸드 상품에 대한 20% 할인입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → 할인배너 상품 20% 할인']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>오반장위크 2022 연말결산</t>
+          <t>연말 홈파티 메뉴 추천</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BEST ITEM 앵콜특가 + 연말 추천 필수템</t>
+          <t>최대 30% 할인부터 페이백 이벤트까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003385</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>(12/12~18) 오반장위크_2022 연말결산</t>
+          <t>Holiday at Home</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (12/12~18) 오반장위크_2022 연말결산', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>All About Strawberries</t>
+          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>제철딸기 ~50% 도레도레 케이크 20% 쿠폰까지</t>
+          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003408</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>All About Strawberries 올 어바웃 스트로베리 ♥</t>
+          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-12-21</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; All About Strawberries 올 어바웃 스트로베리 ♥', '스마일클럽', '딸기 단품 구매 시 최대 50% 할인', '딸기 베이커리 신상품 구매 시 20% 할인', 'BENEFIT 딸기가 가장 맛있는 지금, 최대 50% 할인 혜택', '#달달상큼 #풍부한과즙 눈 속에서 맛보는 봄의 맛, 베스트셀러 설향딸기 정상가 : 17,800원 &gt; 할인가 : 10,680원 보러가기', '#SNS하얀딸기 #알프스딸기 #이색과일 눈꽃처럼 하얀 속살의 달콤함, 설희딸기 정상가 : 21,800원 &gt; 할인가 : 15,260원 보러가기', '#고당도 #진한향기 새콤달콤 풍부한 향, 한단딸기 정상가 : 16,800원 &gt; 할인가 : 8,400원 보러가기', '#왕크왕맛 #풍부한과즙 #복숭아향 과즙도 단맛도 풍성한 왕의 딸기, 킹스베리 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#부드러워요 #쉐이크용 #잼용 날씬한 몸매를 뽐내는, 장희딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#단단해요 #새콤달콤 달큰한 비타민 C의 여왕, 금실딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', 'BENEFIT 도레도레부터 몽상클레르까지 딸기 베이커리 신상품 20% 할인 쿠폰', '푸드마켓 딸기 베이커리 신상품 20% 쿠폰할인(22.12.15 ~ 22.12.21)', '#홀리데이 #홈파티 #딸기요거트 도레도레와 함께하는 크리스마스 ♥ 산타요정 딸기요거트생크림 케이크 정상가 : 39,000원 &gt; 할인가 : 28,080원 보러가기', '#딸기우유맛 #산뜻달달 유크림과 딸기잼으로 가득 채운 오르�逼＠箝옇� 딸기크러핀 정상가 : 4,800원 &gt; 할인가 : 3,840원 보러가기', '#바삭달콤 #티타임 #64겹파이 바삭한 식감 뒤로 전해지는 진한 풍미 몽상클레르 딸기팔미에 정상가 : 5,000원 &gt; 할인가 : 4,000원 보러가기', '할인 적용 기간 : 2022년 12월 15일(목)~21일(수)', 'BENEFIT SSG 푸드마켓 딸기 페어링 EVENT 추천푸드 20% 할인!', '상품 상세에서 SSG 푸드마켓과 할인 혜택을 확인해주세요 :)', '엠블럼으로도 확인 가능! (SSG 푸드마켓 딸기 동시 구매 시 20% 할인 대상 상품)', '       할인 적용 기간', '       할인 조건', '       - 본 이벤트페이지에서 소개하는 SSG 푸드마켓 딸기 동시구매 이벤트에 적용되는 혜택입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → O', '       ex) 푸드마켓 브랜드가 아닌 딸기 + 20% 할인 배너 구매시 → X', '       - 딸기와 함께 구매 시 전체금액의 20%가 아닌 동시구매되는 푸드 상품에 대한 20% 할인입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → 할인배너 상품 20% 할인']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
+          <t>스마일클럽 12월의 가입 혜택</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -910,34 +910,34 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>인기브랜드 15% 쿠폰 혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -947,118 +947,266 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '1. 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급(5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', 'SSG.COM X MEGABOX 스마일클럽은 더욱 특별한 가격으로! 메가박스 2D/3D 영화 관람권 &amp; 팝콘 핫딜', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '명절 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '쿠폰 대상 상품은 상품상세에서 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '런칭 할인', '겨울맞이 多품목 多증정 이벤트!★원더풀 홀리데이 10% 장바구니 쿠폰 적용★', '★15%할인쿠폰★ 종근당건강 BEST 행사 상품']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>메가박스 영화예매권 핫딜</t>
+          <t>Winter Vacation 여행 위크</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>스마일클럽 전용 Exclusive Price !</t>
+          <t>투어2000 패키지 5만원 즉시할인 특가</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003308</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003228</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[SSG.COM x 메가박스] 영화관람권 &amp; 팝콘 스페셜 할인 혜택</t>
+          <t>WINTER VACATION 여행 특가 위크</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-12-14</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.COM x 메가박스] 영화관람권 &amp; 팝콘 스페셜 할인 혜택', '스마일클럽', '[SSG.COM x 메가박스] 영화관람권 &amp; 팝콘 스페셜 할인 혜택', ' 스마일클럽 무료 가입하기 ', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 소중한 사람과 함께하는 연말을 더욱 즐겁게!', '영화 관람권 &amp; 팝콘 스페셜 할인 혜택', '       기존금액 : 13,000원 / 할인금액 : 8,500원', '       기존금액 : 5,500원 / 할인금액 : 2,500원', '영화 관람권 스페셜 할인 혜택', '       기존금액 : 13,000원 / 할인금액 : 9,100원', '3D 영화 관람권 스페셜 할인 혜택', '       기존금액 : 16,000원 / 할인금액 : 11,000원']</t>
+          <t>['이벤트/쿠폰 &gt; WINTER VACATION 여행 특가 위크', '스마일클럽', '여행상품 ~2만원 할인', '실시간 숙소 5% 할인', '카드 청구할인', 'NEW! SSG 입점기념 빅세일 패키지 투어 2000 5만원 할인 특가(*선착순 60명 한정 할인)', '알짜배기 해외&amp;국내 패키지 즉시 할인!', '혜택 받아 구매하고 쓱 떠나보세요.(*선착순 60명 한정 할인)', '[다낭/호이안] 미케비치 투본강 투어 바나산 국립공원 4/5일 최초가 448,000원 &gt; 할인가 398,000원부터 (5만원 즉시할인)', '[전국출발] 제주 힐링투어 초특가 3박4일 (카멜리아힐 + 여미지식물원 + 에코랜드 + 족욕) 최초가 159,000원 &gt; 할인가 109,000원부터 (5만원 즉시할인)', '[인기NO.1 그리스+튀르키예 10일] 터키직항 + 중간항공이동 1회 + 5성특급호텔 최초가 1,399,000원 &gt; 할인가 1,349,000원부터 (5만원 즉시할인)', '[서유럽 3국8일] 만족도 1위! 이태리남부 나/폼/쏘 + 파리/로마 전일관광 + 베니스 최초가 1,699,000원 &gt; 할인가 1,649,000원부터 (5만원 즉시할인)', '선착순 할인이 종료되었습니다. 성원에 감사드립니다.', 'SSG.COM/신세계몰/이마트몰/트립몰 내  &lt;투어2000&gt; 국내/외 여행상품 구매 시 5만원 즉시할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '국내/해외 여행 전 상품 ~2만원 즉시할인', '윈터 베케이션 특가 구매 전, 즉시 할인 혜택을 꼭 챙기세요. 여행 일반상품 결제 시 할인액이 바로 적용됩니다.', '      즉시할인', '여행 상품 즉시할인이 종료되었습니다! 성원에 감사드립니다.', "SSG.COM/신세계몰/이마트몰/트립몰 내 '여행' 일반 상품 구매 시 금액대별 5천원/1만원/2만원 즉시할인", '여기어때 전 상품 5% 할인', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '여기어때 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '파인아트라벨 정상가 : 59,900원 &gt; 할인가 : 56,905원', '파크마린호텔 정상가 : 72,000원 &gt; 할인가 : 68,400원', '곤지암 리조트 정상가 : 155,250원 &gt; 할인가 : 147,488원', '소노캄 델피노 AB동 정상가 : 168,000원 &gt; 할인가 : 159,600원', '남해 베네치아 리조트 정상가 : 140,000원 &gt; 할인가 : 133,000원', '마이다스 호텔&amp;리조트 정상가 : 159,000원 &gt; 할인가 : 151,050원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 92,565원 &gt; 할인가 : 87,937원', '소노벨 변산 호텔 정상가 : 130,000원 &gt; 할인가 : 123,500원', '르네블루 바이 워커힐 정상가 : 160,000원 &gt; 할인가 : 152,000원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 329,175원', '한라궁 호텔 정상가 : 74,000원 &gt; 할인가 : 70,300원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 213,180원', '그랜드 워커힐 서울 호텔 정상가 : 170,000원 &gt; 할인가 : 161,500원', '파라다이스시티 정상가 : 418,000원 &gt; 할인가 : 397,100원', '제주신라호텔 정상가 : 375,100원 &gt; 할인가 : 356,345원', '메종 글래드 제주 정상가 : 94,000원 &gt; 할인가 : 89,300원', '소노벨 비발디파크 E (펫동반가능) 정상가 : 388,300원 &gt; 할인가 : 368,885원', '소노펠리체 빌리지 비발디파크 정상가 : 414,000원 &gt; 할인가 : 393,000원', '소노펠리체 비발디파크 정상가 : 374,000원 &gt; 할인가 : 355,300원', '메이힐스 리조트 정상가 : 90,250원 &gt; 할인가 : 85,738원', '인터컨티넨탈 알펜시아 정상가 : 174,191원 &gt; 할인가 : 165,481원', '소노벨 비발디파크 B.C 정상가 : 207,000원 &gt; 할인가 : 196,650원', '하이캐슬리조트 정상가 : 77,280원 &gt; 할인가 : 73,416원', '정선 인투라온 정상가 : 149,900원 &gt; 할인가 : 142,405원', '풀빌라 아마레 정상가 : 320,000원 &gt; 할인가 : 304,000원', '경주 비클래시 키즈풀빌라 불국사점 정상가 : 239,000원 &gt; 할인가 : 277,050원', '가평 코지 키즈 가족 풀빌라 펜션 정상가 : 161,100원 &gt; 할인가 : 153,045원', '포항 그랑모던풀빌라 정상가 : 90,300원 &gt; 할인가 : 85,785원', '경주 머물다풀빌라 정상가 : 179,000원 &gt; 할인가 : 170,050원', '가평 도도키즈풀빌라 정상가 : 130,000원 &gt; 할인가 : 123,500원', '경주 JS애견풀빌라 정상가 : 69,000원 &gt; 할인가 : 65,550원', '남해 파인트리키즈스파펜션 정상가 : 230,000원 &gt; 할인가 : 218,500원', '제이앤파크 호텔 정상가 : 157,000원 &gt; 할인가 : 149,150원', '속초 호텔 더 블루테라 정상가 : 63,049원 &gt; 할인가 : 59,897원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 64,125원', '더클래스300 호텔 정상가 : 92,000원 &gt; 할인가 : 87,400원', '여수 하이락리조트 정상가 : 94,000원 &gt; 할인가 : 89,300원', '디그니티 호텔 정상가 : 89,096원 &gt; 할인가 : 84,641원', '라마다 속초 정상가 : 104,900원 &gt; 할인가 : 99,655원', '오션스위츠 제주 정상가 : 79,001원 &gt; 할인가 : 75,051원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', 'KB국민카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY 전용] NH농협카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>비발디파크 12/15(목) 8PM</t>
+          <t>[e득라이브] 토이킹덤 12/20(화) 11AM</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>발디파크 1박 + 스노위랜드 3인 종일권 선착순 핫딜</t>
+          <t>인기상품 총집합! 레고 AT-AT/미미프렌즈 마법항아리 外 ~50% OFF</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003372&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003442</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[쓱라이브] 비발디파크 12/15(목) 8PM</t>
+          <t>[SSG.LIVE]12/20 토이킹덤</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-12-17</t>
+          <t>2022-12-20</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 비발디파크 12/15(목) 8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]12/20 토이킹덤', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>P&amp;G 12/20(화) 19시</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>다우니/오랄비/헤드앤숄더 인기상품 최대 33% 즉시할인 + 손흥민 싸인볼 c</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003464</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>P&amp;G @SSG.LIVE 12/20(화) 7PM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2022-12-14</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2022-12-20</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; P&amp;G @SSG.LIVE 12/20(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>레고 12/19(월) 11AM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>최대 30% + 특정카드 1만원 추가할인</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003422</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>레고 @SSG.LIVE 12/19(월) 11:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2022-12-13</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2022-12-19</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 레고 @SSG.LIVE 12/19(월) 11:00', '스마일클럽']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>에스트라 홀리데이 기프트 특집 LIVE 12/19(월) 8PM</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>역대급 핫딜4종 포함 최대49%할인 + 홀리데이 굿즈 증정</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003443</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>에스트라 @SSG.LIVE 12/19(월) 20:00PM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2022-12-14</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2022-12-19</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 에스트라 @SSG.LIVE 12/19(월) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>2022-12-01</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>2022-12-31</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>12월 맘키즈 PLUS</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>지금 할인 중! ~50% 할인 혜택</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>이달의 맘키즈 PLUS</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2022-09-01</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2999-12-13</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~50% 쿠폰상품', '지금 할인 중 !', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 50% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 50%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '(카드사할인 12/8-25) 헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Dec 22 01:23:32 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -762,71 +762,71 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>All About Strawberries</t>
+          <t>연말 홈파티 메뉴 추천</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>제철딸기 ~50% 도레도레 케이크 20% 쿠폰까지</t>
+          <t>최대 30% 할인부터 페이백 이벤트까지</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003408</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>All About Strawberries 올 어바웃 스트로베리 ♥</t>
+          <t>Holiday at Home</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-21</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; All About Strawberries 올 어바웃 스트로베리 ♥', '스마일클럽', '딸기 단품 구매 시 최대 50% 할인', '딸기 베이커리 신상품 구매 시 20% 할인', 'BENEFIT 딸기가 가장 맛있는 지금, 최대 50% 할인 혜택', '#달달상큼 #풍부한과즙 눈 속에서 맛보는 봄의 맛, 베스트셀러 설향딸기 정상가 : 17,800원 &gt; 할인가 : 10,680원 보러가기', '#SNS하얀딸기 #알프스딸기 #이색과일 눈꽃처럼 하얀 속살의 달콤함, 설희딸기 정상가 : 21,800원 &gt; 할인가 : 15,260원 보러가기', '#고당도 #진한향기 새콤달콤 풍부한 향, 한단딸기 정상가 : 16,800원 &gt; 할인가 : 8,400원 보러가기', '#왕크왕맛 #풍부한과즙 #복숭아향 과즙도 단맛도 풍성한 왕의 딸기, 킹스베리 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#부드러워요 #쉐이크용 #잼용 날씬한 몸매를 뽐내는, 장희딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '#단단해요 #새콤달콤 달큰한 비타민 C의 여왕, 금실딸기 정상가 : 19,800원 &gt; 할인가 : 11,800원 보러가기', '눈 속에서 맛보는 봄의 맛, 베스트셀러 설향딸기 정상가 : 12,900원~ &gt; 할인가 : 10,900원~ 보러가기', '날씬한 몸매를 뽐내는, 장희딸기 정상가 : 20,900원~ &gt; 할인가 : 19,900원~ 보러가기', '달큰한 비타민 C의 여왕, 금실딸기 정상가 : 17,900원 &gt; 할인가 : 15,900원 보러가기', 'BENEFIT 도레도레부터 몽상클레르까지 딸기 베이커리 신상품 20% 할인 쿠폰', '푸드마켓 딸기 베이커리 신상품 20% 쿠폰할인(22.12.15 ~ 22.12.21)', '#홀리데이 #홈파티 #딸기요거트 도레도레와 함께하는 크리스마스 ♥ 산타요정 딸기요거트생크림 케이크 정상가 : 39,000원 &gt; 할인가 : 28,080원 보러가기', '#딸기우유맛 #산뜻달달 유크림과 딸기잼으로 가득 채운 오르�逼＠箝옇� 딸기크러핀 정상가 : 4,800원 &gt; 할인가 : 3,840원 보러가기', '#바삭달콤 #티타임 #64겹파이 바삭한 식감 뒤로 전해지는 진한 풍미 몽상클레르 딸기팔미에 정상가 : 5,000원 &gt; 할인가 : 4,000원 보러가기', '할인 적용 기간 : 2022년 12월 15일(목)~21일(수)', 'BENEFIT SSG 푸드마켓 딸기 페어링 EVENT 추천푸드 20% 할인!', '상품 상세에서 SSG 푸드마켓과 할인 혜택을 확인해주세요 :)', '엠블럼으로도 확인 가능! (SSG 푸드마켓 딸기 동시 구매 시 20% 할인 대상 상품)', '       할인 적용 기간', '       할인 조건', '       - 본 이벤트페이지에서 소개하는 SSG 푸드마켓 딸기 동시구매 이벤트에 적용되는 혜택입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → O', '       ex) 푸드마켓 브랜드가 아닌 딸기 + 20% 할인 배너 구매시 → X', '       - 딸기와 함께 구매 시 전체금액의 20%가 아닌 동시구매되는 푸드 상품에 대한 20% 할인입니다.', '       ex) 푸드마켓 딸기 + 20% 할인 배너 상품 동시 구매시 → 할인배너 상품 20% 할인']</t>
+          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>연말 홈파티 메뉴 추천</t>
+          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>최대 30% 할인부터 페이백 이벤트까지</t>
+          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Holiday at Home</t>
+          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -836,34 +836,34 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
+          <t>스마일클럽 12월의 가입 혜택</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -873,34 +873,34 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>인기브랜드 15% 쿠폰 혜택</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -910,29 +910,29 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '명절 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '쿠폰 대상 상품은 상품상세에서 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '겨울맞이 10% 즉시 할인중♥', '★15%할인쿠폰★ 종근당건강 BEST 행사 상품']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>Winter Vacation 여행 위크</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>인기브랜드 15% 쿠폰 혜택</t>
+          <t>투어2000 패키지 5만원 즉시할인 특가</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003228</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>WINTER VACATION 여행 특가 위크</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -942,271 +942,123 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '명절 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '쿠폰 대상 상품은 상품상세에서 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '런칭 할인', '겨울맞이 多품목 多증정 이벤트!★원더풀 홀리데이 10% 장바구니 쿠폰 적용★', '★15%할인쿠폰★ 종근당건강 BEST 행사 상품']</t>
+          <t>['이벤트/쿠폰 &gt; WINTER VACATION 여행 특가 위크', '스마일클럽', '여행상품 ~2만원 할인', '실시간 숙소 5% 할인', '카드 청구할인', 'NEW! SSG 입점기념 빅세일 패키지 투어 2000 5만원 할인 특가(*선착순 60명 한정 할인)', '알짜배기 해외&amp;국내 패키지 즉시 할인!', '혜택 받아 구매하고 쓱 떠나보세요.(*선착순 60명 한정 할인)', '[다낭/호이안] 미케비치 투본강 투어 바나산 국립공원 4/5일 최초가 448,000원 &gt; 할인가 398,000원부터 (5만원 즉시할인)', '[전국출발] 제주 힐링투어 초특가 3박4일 (카멜리아힐 + 여미지식물원 + 에코랜드 + 족욕) 최초가 159,000원 &gt; 할인가 109,000원부터 (5만원 즉시할인)', '[인기NO.1 그리스+튀르키예 10일] 터키직항 + 중간항공이동 1회 + 5성특급호텔 최초가 1,399,000원 &gt; 할인가 1,349,000원부터 (5만원 즉시할인)', '[서유럽 3국8일] 만족도 1위! 이태리남부 나/폼/쏘 + 파리/로마 전일관광 + 베니스 최초가 1,699,000원 &gt; 할인가 1,649,000원부터 (5만원 즉시할인)', '선착순 할인이 종료되었습니다. 성원에 감사드립니다.', 'SSG.COM/신세계몰/이마트몰/트립몰 내  &lt;투어2000&gt; 국내/외 여행상품 구매 시 5만원 즉시할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '국내/해외 여행 전 상품 ~2만원 즉시할인', '윈터 베케이션 특가 구매 전, 즉시 할인 혜택을 꼭 챙기세요. 여행 일반상품 결제 시 할인액이 바로 적용됩니다.', '      즉시할인', '여행 상품 즉시할인이 종료되었습니다! 성원에 감사드립니다.', "SSG.COM/신세계몰/이마트몰/트립몰 내 '여행' 일반 상품 구매 시 금액대별 5천원/1만원/2만원 즉시할인", '여기어때 전 상품 5% 할인', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '여기어때 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '파인아트라벨 정상가 : 59,900원 &gt; 할인가 : 56,905원', '파크마린호텔 정상가 : 72,000원 &gt; 할인가 : 68,400원', '곤지암 리조트 정상가 : 155,250원 &gt; 할인가 : 147,488원', '소노캄 델피노 AB동 정상가 : 168,000원 &gt; 할인가 : 159,600원', '남해 베네치아 리조트 정상가 : 140,000원 &gt; 할인가 : 133,000원', '마이다스 호텔&amp;리조트 정상가 : 159,000원 &gt; 할인가 : 151,050원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 92,565원 &gt; 할인가 : 87,937원', '소노벨 변산 호텔 정상가 : 130,000원 &gt; 할인가 : 123,500원', '르네블루 바이 워커힐 정상가 : 160,000원 &gt; 할인가 : 152,000원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 329,175원', '한라궁 호텔 정상가 : 74,000원 &gt; 할인가 : 70,300원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 213,180원', '그랜드 워커힐 서울 호텔 정상가 : 170,000원 &gt; 할인가 : 161,500원', '파라다이스시티 정상가 : 418,000원 &gt; 할인가 : 397,100원', '제주신라호텔 정상가 : 375,100원 &gt; 할인가 : 356,345원', '메종 글래드 제주 정상가 : 94,000원 &gt; 할인가 : 89,300원', '소노벨 비발디파크 E (펫동반가능) 정상가 : 388,300원 &gt; 할인가 : 368,885원', '소노펠리체 빌리지 비발디파크 정상가 : 414,000원 &gt; 할인가 : 393,000원', '소노펠리체 비발디파크 정상가 : 374,000원 &gt; 할인가 : 355,300원', '메이힐스 리조트 정상가 : 90,250원 &gt; 할인가 : 85,738원', '인터컨티넨탈 알펜시아 정상가 : 174,191원 &gt; 할인가 : 165,481원', '소노벨 비발디파크 B.C 정상가 : 207,000원 &gt; 할인가 : 196,650원', '하이캐슬리조트 정상가 : 77,280원 &gt; 할인가 : 73,416원', '정선 인투라온 정상가 : 149,900원 &gt; 할인가 : 142,405원', '풀빌라 아마레 정상가 : 320,000원 &gt; 할인가 : 304,000원', '경주 비클래시 키즈풀빌라 불국사점 정상가 : 239,000원 &gt; 할인가 : 277,050원', '가평 코지 키즈 가족 풀빌라 펜션 정상가 : 161,100원 &gt; 할인가 : 153,045원', '포항 그랑모던풀빌라 정상가 : 90,300원 &gt; 할인가 : 85,785원', '경주 머물다풀빌라 정상가 : 179,000원 &gt; 할인가 : 170,050원', '가평 도도키즈풀빌라 정상가 : 130,000원 &gt; 할인가 : 123,500원', '경주 JS애견풀빌라 정상가 : 69,000원 &gt; 할인가 : 65,550원', '남해 파인트리키즈스파펜션 정상가 : 230,000원 &gt; 할인가 : 218,500원', '제이앤파크 호텔 정상가 : 157,000원 &gt; 할인가 : 149,150원', '속초 호텔 더 블루테라 정상가 : 63,049원 &gt; 할인가 : 59,897원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 64,125원', '더클래스300 호텔 정상가 : 92,000원 &gt; 할인가 : 87,400원', '여수 하이락리조트 정상가 : 94,000원 &gt; 할인가 : 89,300원', '디그니티 호텔 정상가 : 89,096원 &gt; 할인가 : 84,641원', '라마다 속초 정상가 : 104,900원 &gt; 할인가 : 99,655원', '오션스위츠 제주 정상가 : 79,001원 &gt; 할인가 : 75,051원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', 'KB국민카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY 전용] NH농협카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Winter Vacation 여행 위크</t>
+          <t>피코크 12/22(목) 8PM</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>투어2000 패키지 5만원 즉시할인 특가</t>
+          <t>피코크/프레시지 최대 30% 크리스마스 홈파티!</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003228</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003421&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>WINTER VACATION 여행 특가 위크</t>
+          <t>피코크@SSG.LIVE 12/22(목)20:00PM</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-12-13</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2022-12-24</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; WINTER VACATION 여행 특가 위크', '스마일클럽', '여행상품 ~2만원 할인', '실시간 숙소 5% 할인', '카드 청구할인', 'NEW! SSG 입점기념 빅세일 패키지 투어 2000 5만원 할인 특가(*선착순 60명 한정 할인)', '알짜배기 해외&amp;국내 패키지 즉시 할인!', '혜택 받아 구매하고 쓱 떠나보세요.(*선착순 60명 한정 할인)', '[다낭/호이안] 미케비치 투본강 투어 바나산 국립공원 4/5일 최초가 448,000원 &gt; 할인가 398,000원부터 (5만원 즉시할인)', '[전국출발] 제주 힐링투어 초특가 3박4일 (카멜리아힐 + 여미지식물원 + 에코랜드 + 족욕) 최초가 159,000원 &gt; 할인가 109,000원부터 (5만원 즉시할인)', '[인기NO.1 그리스+튀르키예 10일] 터키직항 + 중간항공이동 1회 + 5성특급호텔 최초가 1,399,000원 &gt; 할인가 1,349,000원부터 (5만원 즉시할인)', '[서유럽 3국8일] 만족도 1위! 이태리남부 나/폼/쏘 + 파리/로마 전일관광 + 베니스 최초가 1,699,000원 &gt; 할인가 1,649,000원부터 (5만원 즉시할인)', '선착순 할인이 종료되었습니다. 성원에 감사드립니다.', 'SSG.COM/신세계몰/이마트몰/트립몰 내  &lt;투어2000&gt; 국내/외 여행상품 구매 시 5만원 즉시할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '국내/해외 여행 전 상품 ~2만원 즉시할인', '윈터 베케이션 특가 구매 전, 즉시 할인 혜택을 꼭 챙기세요. 여행 일반상품 결제 시 할인액이 바로 적용됩니다.', '      즉시할인', '여행 상품 즉시할인이 종료되었습니다! 성원에 감사드립니다.', "SSG.COM/신세계몰/이마트몰/트립몰 내 '여행' 일반 상품 구매 시 금액대별 5천원/1만원/2만원 즉시할인", '여기어때 전 상품 5% 할인', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '여기어때 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '파인아트라벨 정상가 : 59,900원 &gt; 할인가 : 56,905원', '파크마린호텔 정상가 : 72,000원 &gt; 할인가 : 68,400원', '곤지암 리조트 정상가 : 155,250원 &gt; 할인가 : 147,488원', '소노캄 델피노 AB동 정상가 : 168,000원 &gt; 할인가 : 159,600원', '남해 베네치아 리조트 정상가 : 140,000원 &gt; 할인가 : 133,000원', '마이다스 호텔&amp;리조트 정상가 : 159,000원 &gt; 할인가 : 151,050원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 92,565원 &gt; 할인가 : 87,937원', '소노벨 변산 호텔 정상가 : 130,000원 &gt; 할인가 : 123,500원', '르네블루 바이 워커힐 정상가 : 160,000원 &gt; 할인가 : 152,000원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 329,175원', '한라궁 호텔 정상가 : 74,000원 &gt; 할인가 : 70,300원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 213,180원', '그랜드 워커힐 서울 호텔 정상가 : 170,000원 &gt; 할인가 : 161,500원', '파라다이스시티 정상가 : 418,000원 &gt; 할인가 : 397,100원', '제주신라호텔 정상가 : 375,100원 &gt; 할인가 : 356,345원', '메종 글래드 제주 정상가 : 94,000원 &gt; 할인가 : 89,300원', '소노벨 비발디파크 E (펫동반가능) 정상가 : 388,300원 &gt; 할인가 : 368,885원', '소노펠리체 빌리지 비발디파크 정상가 : 414,000원 &gt; 할인가 : 393,000원', '소노펠리체 비발디파크 정상가 : 374,000원 &gt; 할인가 : 355,300원', '메이힐스 리조트 정상가 : 90,250원 &gt; 할인가 : 85,738원', '인터컨티넨탈 알펜시아 정상가 : 174,191원 &gt; 할인가 : 165,481원', '소노벨 비발디파크 B.C 정상가 : 207,000원 &gt; 할인가 : 196,650원', '하이캐슬리조트 정상가 : 77,280원 &gt; 할인가 : 73,416원', '정선 인투라온 정상가 : 149,900원 &gt; 할인가 : 142,405원', '풀빌라 아마레 정상가 : 320,000원 &gt; 할인가 : 304,000원', '경주 비클래시 키즈풀빌라 불국사점 정상가 : 239,000원 &gt; 할인가 : 277,050원', '가평 코지 키즈 가족 풀빌라 펜션 정상가 : 161,100원 &gt; 할인가 : 153,045원', '포항 그랑모던풀빌라 정상가 : 90,300원 &gt; 할인가 : 85,785원', '경주 머물다풀빌라 정상가 : 179,000원 &gt; 할인가 : 170,050원', '가평 도도키즈풀빌라 정상가 : 130,000원 &gt; 할인가 : 123,500원', '경주 JS애견풀빌라 정상가 : 69,000원 &gt; 할인가 : 65,550원', '남해 파인트리키즈스파펜션 정상가 : 230,000원 &gt; 할인가 : 218,500원', '제이앤파크 호텔 정상가 : 157,000원 &gt; 할인가 : 149,150원', '속초 호텔 더 블루테라 정상가 : 63,049원 &gt; 할인가 : 59,897원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 64,125원', '더클래스300 호텔 정상가 : 92,000원 &gt; 할인가 : 87,400원', '여수 하이락리조트 정상가 : 94,000원 &gt; 할인가 : 89,300원', '디그니티 호텔 정상가 : 89,096원 &gt; 할인가 : 84,641원', '라마다 속초 정상가 : 104,900원 &gt; 할인가 : 99,655원', '오션스위츠 제주 정상가 : 79,001원 &gt; 할인가 : 75,051원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', 'KB국민카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY 전용] NH농협카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 피코크@SSG.LIVE 12/22(목)20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[e득라이브] 토이킹덤 12/20(화) 11AM</t>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>인기상품 총집합! 레고 AT-AT/미미프렌즈 마법항아리 外 ~50% OFF</t>
+          <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003442</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]12/20 토이킹덤</t>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-12-20</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]12/20 토이킹덤', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>P&amp;G 12/20(화) 19시</t>
+          <t>12월 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>다우니/오랄비/헤드앤숄더 인기상품 최대 33% 즉시할인 + 손흥민 싸인볼 c</t>
+          <t>지금 할인 중! ~50% 할인 혜택</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003464</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>P&amp;G @SSG.LIVE 12/20(화) 7PM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2022-12-14</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-12-20</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; P&amp;G @SSG.LIVE 12/20(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>레고 12/19(월) 11AM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>최대 30% + 특정카드 1만원 추가할인</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003422</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>레고 @SSG.LIVE 12/19(월) 11:00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2022-12-13</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2022-12-19</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 레고 @SSG.LIVE 12/19(월) 11:00', '스마일클럽']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>에스트라 홀리데이 기프트 특집 LIVE 12/19(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>역대급 핫딜4종 포함 최대49%할인 + 홀리데이 굿즈 증정</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003443</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>에스트라 @SSG.LIVE 12/19(월) 20:00PM</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2022-12-14</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2022-12-19</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 에스트라 @SSG.LIVE 12/19(월) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2022-12-01</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>12월 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~50% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~50% 쿠폰상품', '지금 할인 중 !', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 50% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 50%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '(카드사할인 12/8-25) 헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '(카드사할인 12/8-25) 헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Dec 26 01:23:41 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,318 +473,318 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wonderful Holiday</t>
+          <t>2023 설 스페셜 혜택전</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기프트부터 홈파티까지 연말의 모든 것 기프트 쇼핑 10% 선착순 쿠폰</t>
+          <t>단 3일간, 최대 3만원 선물세트 전용쿠폰</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003336</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003554</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Wonderfull Holiday 원더풀 홀리데이</t>
+          <t>2023 설 스페셜 혜택전</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-26</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2022-12-28</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Wonderfull Holiday 원더풀 홀리데이', '스마일클럽', '쓱배송 파티 푸드', '연말 기프트 쇼핑을 도와줄 10% 장바구니 쿠폰', '10% 장바구니쿠폰 - 5만원 이상 구매 시, 최대 1만원 할인 (매일 오전 9시 1만장)', '쿠폰 발급 받기 (기간내 ID당 1회 발급)', '       쿠폰 발급 기간', '       2022년 12월 19일(월) ~ 12월 25(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 상품에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니쿠폰으로 구매 건 내 대상상품 전체에 적용되며, 5만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '아래 미션 중 하나 이상을 달성하고, 응모하기 버튼을 클릭하여 이벤트에 응모하세요. 추첨을 통해 당첨된 분들께 특별한 홀리데이 선물을 드립니다. 미션 2개를 모두 완료하시면 더욱 특별한 경품 찬스!', 'Misson1. 쓱배송/새벽배송 15만원이상 구매', '쓱배송 미션 응모하기', '쓱배송에는 트레이더스 주문건도 포함됩니다.', '미션을 달성하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다.', '선물하기 또는 이벤트 해당 주문 취소 시 해당 내역은 집계 제외됩니다.', '부당한 방법으로 이벤트에 응모하였을 경우 당첨에서 제외될 수 있습니다.', '당첨자는 1월 6일(금) 이벤트 당첨자 발표 게시판을 통해 공지됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 설 스페셜 혜택전', '스마일클럽', '4종쿠폰', '카드사 청구할인', '명절 종합 선물세트 4종 쿠폰', '      명절 선물 전용 3,000원 쿠폰 (점포명절, 명절)', '      명절 선물 전용 7,000원 쿠폰 (점포명절, 명절)', '      명절 선물 전용 15,000원 쿠폰 (점포명절, 명절)', '      명절 선물 전용 30,000원 쿠폰 (점포명절, 명절)', '쿠폰 발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '[명절] [점포 명절] 엠블렘이 있는 설 명절 기프트 상품 전용 쿠폰입니다.', '[카드 50% 할인]LG 선물 세트)리튠 녹용진액 골드 3종 기획세트', '[SSGPAY머니 증정][1/5(목)이후 순차출고][냉동][오늘의소] 꽃갈비를 품은 블랙앵거스 LA갈비 선물세트 3kg', '[20만원↑구매시3만원쓱머니증정][배송일 해피콜][직접배송][SSG정담][과일愛]프라이빗 과일선물세트 후룻디니뜨 혼합 9호 (샤인머스켓3 / 사과2 / 배2 / 자몽2 - 4.8kg) - 보자기포장', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가', '최대 57% 할인! GC녹십자 설 명절 건강 선물세트', '[백화점라인/국내배송] 폴로 랄프로렌 이태리산 울 100% 시그니처 멀티로고 폴로 머플러 (6color)', '[해외직구] 포켓몬 몬스터볼 변신 피규어 6종세트 무료배송 빠른 출고', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '새해맞이 댕댕이 한복/배변패드/유모차 할인 구경하시개!', '설맞이 설레는 고양이 모래/캣타워/스크래쳐 용품 할인전', '- 삼성카드 청구할인 -']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>THE GIFT GUIDE MAGICAL CHRISTMAS</t>
+          <t>설 선물세트 다함께 공동구매 1탄 _프리미엄</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>연말 선물 추천+홀리데이 10%쿠폰</t>
+          <t>최대 40%할인 + 목표달성하면 SSG머니 최대 6만원 혜택</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003120</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003545</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>THE GIFT GUIDE Magical Christmas</t>
+          <t>[명절]설 공동구매 1탄</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-26</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; THE GIFT GUIDE Magical Christmas', '스마일클럽', '01 - 홀리데이 12% 쿠폰', "발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '03 - 홀리데이 뷰티박스 이벤트', '        - 경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다.', '        - 이벤트 기간 내 경품 응모 후 주문 후 취소/반품하신 고객은 경품 응모 대상에서 제외됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '홀리데이 쇼핑은 시마을에서! 최대 15% 쿠폰 &amp; e포인트 선물하기 보너스 혜택까지 - shop']</t>
+          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 1탄', '스마일클럽', '명절 선물세트 7종 최대 40% 할인 + 공동구매 혜택 최대 6만원 적립', '공구 이벤트 기간 : 12월 26일 ~ 1월 1일', '[오메드] 오일 비네거 세트 30% 할인 + 최대 8천원 적립!', '[꽁피튀르] 파리지엥잼 선물세트 30% 할인 + 최대 8천원 적립!', '[SSG 정담] 프리미엄 선물세트 33% 할인 + 최대 8천원 적립!', '프리미엄 망고혼합 선물세트 17% 할인 + 최대 1만원 적립!', '[종근당건강] 6년근 홍삼정업 세트 20% 할인 + 최대 1만원 적립!', '[고려천홍삼] 프리미엄 녹용홍삼 37% 할인 + 최대 8천원 적립!', '호주산 LA갈비 선물세트 28% 할인 + 최대 8천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MAGICAL CHRISTMAS</t>
+          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛에서 준비한 크리스마스 기프트</t>
+          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003230</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[12/12~25] MAGICAL CHRISTMAS - 프리미엄 아울렛</t>
+          <t>선물하기로 쓱- 마음을 전하세요</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/12~25] MAGICAL CHRISTMAS - 프리미엄 아울렛', '스마일클럽', '최대 10% 할인 쿠폰 혜택', '[해외 명품 - 최대 50% 할인] 연말 맞이 나에게 주는 명품 선물 BEST 모음 보러가기', '[패션/잡화 - 최대 44% 할인] 골든듀/로제도르 30% OFF 보러가기', '[키즈 패션 - 최대 75% 할인] 아디다스키즈/게스키즈 외 BEST 보러가기', '[언더웨어 - 최대 70% 할인] 연말 맞이 언더/이지웨어 특가 &amp; BEST 모음 보러가기', '[여성 패션 - 최대 70% 할인] 연말 맞이 여성패션 특가 &amp; BEST 모음 보러가기', '[패션 슈즈 - 최대 80% 할인] 아울렛 슈즈 GIFT 전 보러가기', '[남성 패션 - 최대 80% 할인] 브룩스브라더스 외 남성 겨울 상품 입고 OFF 보러가기', '[유니섹스 - 최대 80% 할인] 경량베스트, 점퍼 등 최고 80% OFF 보러가기', '[스포츠 - 최대 70% 할인] 내셔널지오그래픽/노스페이스 등 겨울 BEST 보러가기', '[리빙 - 최대 75% 할인] 웨지우드 BEST 아이템 특가 보러가기', '홀리데이 쇼핑은 시마을에서! 최대 15% 쿠폰 &amp; e포인트 선물하기 보너스 혜택까지 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>반값다~딜</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>첫구매는 네개 다 반값!  + 무료배송 쿠폰</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003404&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>첫구매는 네개다 반값! 반값다딜</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫구매는 네개다 반값! 반값다딜', '스마일클럽', '첫구매는 네개다 반값! 반값다딜', '첫구매는 네개 다 반값! 게다가 무료배송', '반값다 딜 50%', '반값다딜 쿠폰이 모두 소진되었습니다. 더 좋은 이벤트로 찾아뵙겠습니다.', '첫구매는 네개 모두 다 반값!', '오늘의 반값쿠폰', '       이마트몰, 쓱배송/새벽배송', '       딸기 50% 할인 (첫 구매 전용)', '       딸기 cat 최대 5천원 할인', '       흰우유 50% 할인 (첫 구매 전용)', '       흰우유 cat 최대 2천원 할인', '       봉지라면 50% 할인 (첫 구매 전용)', '       봉지라면 cat 최대 2천원 할인', '       식빵 50% 할인 (첫 구매 전용)', '       식빵 cat 최대 2천원 할인', '       쓱배송 첫구매 무료배송 (첫 구매 전용)', '       2만원 이상 구매시 사용 가능', '첫구매 쿠폰 모두 한번에 받기', '       2021년 12월 18일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매이력이 없는 고객 한정', '       쿠폰 발급 기간', '       쿠폰 사용기간', '       상품할인 쿠폰 : 2022년 12월 19일(월) 부터 25일(일) 까지', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용대상', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 우유 1개, 딸기 1개, 라면 1개, 식빵 1개 적용 가능! 딸기 2개 구매시 1개에만 적용 가능합니다', '첫구매 쿠폰 CAT', '       딸기 50% cat', '       우유 50% cat', '       식빵 50% cat', '       봉지라면 50% cat', '       쿠폰 발급 대상', '첫구매 전용 오늘의 상품 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 레고</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>크리스마스 특별 할인부터 사은품SET 증정까지!</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003346</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 레고</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 레고', '스마일클럽', " 01. '레고 아바타 시리즈' 행사상품 구매 시, SSG MONEY 10% 적립 ※ 이벤트 페이지 내 레고 아바타 시리즈 4개 상품에만 해당됩니다. ", " 02. '레고 BEST 시리즈' 행사상품 20% 할인 ※ 이벤트 페이지 내 레고 BEST 시리즈 4개 상품에만 해당됩니다. "]</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
+          <t>연말 홈파티 메뉴 추천</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
+          <t>최대 30% 할인부터 페이백 이벤트까지</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>선물하기로 쓱- 마음을 전하세요</t>
+          <t>Holiday at Home</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>W컨셉 베스트 브랜드 셀렉션</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>13% 쿠폰+모두가 사랑한 브랜드를 한 자리에!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003454</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-12-26</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION', '스마일클럽', '01) SPECIAL OFFER 13% 쿠폰 바로보기', '01) SPECIAL OFFER 13% 쿠폰 상품 쿠폰', '1만원 이상 구매시 최대 2만원 할인 -기간 내 ID당 4장 발급 가능-', '         쿠폰 발급 및 사용 기간', '         - 1만원 이상 상품 구매 시 13% 할인, 최대 2만원 (기간내 ID당 발급수량 4장)', '         쿠폰 적용 방법', '- 쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>스마일클럽 12월의 가입 혜택</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>연말 홈파티 메뉴 추천</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>최대 30% 할인부터 페이백 이벤트까지</t>
+          <t>인기브랜드 15% 쿠폰 혜택</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Holiday at Home</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -799,34 +799,34 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '건강 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', '      쿠폰발급 및 사용 기간', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰은 기간 내 ID당 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점, 이마트몰, 새벽배송, 트레이더스몰에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니 쿠폰으로 구매 건 내 해당 브랜드에 적용되며, 3만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '겨울맞이 10% 즉시 할인중♥', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '해피라운지★올인원 이뮨 액상 비타민 구매시 콜라겐 구미 증정★', '이마트 선물세트 할인 및 적립 상품권 증정까지 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 쓱-잘 사는 이야기  with 공유, 공효진</t>
+          <t>[월간캠핑쇼]  이타카 12/26(월) 7PM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>영상 보고 댓글 달면 푸짐한 경품이~</t>
+          <t>그랑데 스테이션 38만원+코베아 3웨이 구이바다 6.9만원대 핫딜</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003174</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003558&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진</t>
+          <t>[쓱라이브] 이타카 12/26(월) 7PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-21</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -836,34 +836,34 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Good Buy! 2022 : 쓱- 잘 사는 이야기 with 공유, 공효진', '스마일클럽', '신선 식품은 역시 쓱배송!', '풍성한 연말을 위한 댓글 이벤트', ' 영상 더보기란에 기재된 인증 폼까지 참여하면 응모 완료! 영상 확인하고 댓글 쓰러 가기! ※ 응모 조건 및 자세한 이벤트 내용은 영상 내 더보기란에서 확인하세요 ', '            모델 친필 사인은 모델별 영상 기준으로 당첨자 선정 진행됩니다. 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정합니다', '쓱- 무물 SNS 댓글 이벤트', '배스킨라빈스 아빠왔다팩 모바일쿠폰 (50명)', '               모델 친필 사인은 모델 피드 기준으로 당첨자 선정 진행 됩니다. (e.g. 공유님 무물 이벤트 피드 댓글 작성 → 당첨 시 공유님 사인 증정) 그 외 경품은 본 이벤트 참여자 전원 대상으로 당첨자 선정 진행됩니다', '응모 조건 및 자세한 이벤트 내용은 SSG.COM 인스타그램에서 확인하세요.']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 이타카 12/26(월) 7PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>포레오 12/27(화) 8PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>라이브중에만 추가 10% 쿠폰! 쏟아지는 구매인증 선물까지</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003559&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>[신세계라이브쇼핑] 포레오 12/27(화) 8PM</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-21</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -873,34 +873,34 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; [신세계라이브쇼핑] 포레오 12/27(화) 8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>인기브랜드 15% 쿠폰 혜택</t>
+          <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -910,155 +910,44 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '명절 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '쿠폰 대상 상품은 상품상세에서 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '겨울맞이 10% 즉시 할인중♥', '★15%할인쿠폰★ 종근당건강 BEST 행사 상품']</t>
+          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Winter Vacation 여행 위크</t>
+          <t>12월 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>투어2000 패키지 5만원 즉시할인 특가</t>
+          <t>지금 할인 중! ~50% 할인 혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003228</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>WINTER VACATION 여행 특가 위크</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-12-25</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; WINTER VACATION 여행 특가 위크', '스마일클럽', '여행상품 ~2만원 할인', '실시간 숙소 5% 할인', '카드 청구할인', 'NEW! SSG 입점기념 빅세일 패키지 투어 2000 5만원 할인 특가(*선착순 60명 한정 할인)', '알짜배기 해외&amp;국내 패키지 즉시 할인!', '혜택 받아 구매하고 쓱 떠나보세요.(*선착순 60명 한정 할인)', '[다낭/호이안] 미케비치 투본강 투어 바나산 국립공원 4/5일 최초가 448,000원 &gt; 할인가 398,000원부터 (5만원 즉시할인)', '[전국출발] 제주 힐링투어 초특가 3박4일 (카멜리아힐 + 여미지식물원 + 에코랜드 + 족욕) 최초가 159,000원 &gt; 할인가 109,000원부터 (5만원 즉시할인)', '[인기NO.1 그리스+튀르키예 10일] 터키직항 + 중간항공이동 1회 + 5성특급호텔 최초가 1,399,000원 &gt; 할인가 1,349,000원부터 (5만원 즉시할인)', '[서유럽 3국8일] 만족도 1위! 이태리남부 나/폼/쏘 + 파리/로마 전일관광 + 베니스 최초가 1,699,000원 &gt; 할인가 1,649,000원부터 (5만원 즉시할인)', '선착순 할인이 종료되었습니다. 성원에 감사드립니다.', 'SSG.COM/신세계몰/이마트몰/트립몰 내  &lt;투어2000&gt; 국내/외 여행상품 구매 시 5만원 즉시할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '국내/해외 여행 전 상품 ~2만원 즉시할인', '윈터 베케이션 특가 구매 전, 즉시 할인 혜택을 꼭 챙기세요. 여행 일반상품 결제 시 할인액이 바로 적용됩니다.', '      즉시할인', '여행 상품 즉시할인이 종료되었습니다! 성원에 감사드립니다.', "SSG.COM/신세계몰/이마트몰/트립몰 내 '여행' 일반 상품 구매 시 금액대별 5천원/1만원/2만원 즉시할인", '여기어때 전 상품 5% 할인', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '여기어때 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '파인아트라벨 정상가 : 59,900원 &gt; 할인가 : 56,905원', '파크마린호텔 정상가 : 72,000원 &gt; 할인가 : 68,400원', '곤지암 리조트 정상가 : 155,250원 &gt; 할인가 : 147,488원', '소노캄 델피노 AB동 정상가 : 168,000원 &gt; 할인가 : 159,600원', '남해 베네치아 리조트 정상가 : 140,000원 &gt; 할인가 : 133,000원', '마이다스 호텔&amp;리조트 정상가 : 159,000원 &gt; 할인가 : 151,050원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 92,565원 &gt; 할인가 : 87,937원', '소노벨 변산 호텔 정상가 : 130,000원 &gt; 할인가 : 123,500원', '르네블루 바이 워커힐 정상가 : 160,000원 &gt; 할인가 : 152,000원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 329,175원', '한라궁 호텔 정상가 : 74,000원 &gt; 할인가 : 70,300원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 213,180원', '그랜드 워커힐 서울 호텔 정상가 : 170,000원 &gt; 할인가 : 161,500원', '파라다이스시티 정상가 : 418,000원 &gt; 할인가 : 397,100원', '제주신라호텔 정상가 : 375,100원 &gt; 할인가 : 356,345원', '메종 글래드 제주 정상가 : 94,000원 &gt; 할인가 : 89,300원', '소노벨 비발디파크 E (펫동반가능) 정상가 : 388,300원 &gt; 할인가 : 368,885원', '소노펠리체 빌리지 비발디파크 정상가 : 414,000원 &gt; 할인가 : 393,000원', '소노펠리체 비발디파크 정상가 : 374,000원 &gt; 할인가 : 355,300원', '메이힐스 리조트 정상가 : 90,250원 &gt; 할인가 : 85,738원', '인터컨티넨탈 알펜시아 정상가 : 174,191원 &gt; 할인가 : 165,481원', '소노벨 비발디파크 B.C 정상가 : 207,000원 &gt; 할인가 : 196,650원', '하이캐슬리조트 정상가 : 77,280원 &gt; 할인가 : 73,416원', '정선 인투라온 정상가 : 149,900원 &gt; 할인가 : 142,405원', '풀빌라 아마레 정상가 : 320,000원 &gt; 할인가 : 304,000원', '경주 비클래시 키즈풀빌라 불국사점 정상가 : 239,000원 &gt; 할인가 : 277,050원', '가평 코지 키즈 가족 풀빌라 펜션 정상가 : 161,100원 &gt; 할인가 : 153,045원', '포항 그랑모던풀빌라 정상가 : 90,300원 &gt; 할인가 : 85,785원', '경주 머물다풀빌라 정상가 : 179,000원 &gt; 할인가 : 170,050원', '가평 도도키즈풀빌라 정상가 : 130,000원 &gt; 할인가 : 123,500원', '경주 JS애견풀빌라 정상가 : 69,000원 &gt; 할인가 : 65,550원', '남해 파인트리키즈스파펜션 정상가 : 230,000원 &gt; 할인가 : 218,500원', '제이앤파크 호텔 정상가 : 157,000원 &gt; 할인가 : 149,150원', '속초 호텔 더 블루테라 정상가 : 63,049원 &gt; 할인가 : 59,897원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 64,125원', '더클래스300 호텔 정상가 : 92,000원 &gt; 할인가 : 87,400원', '여수 하이락리조트 정상가 : 94,000원 &gt; 할인가 : 89,300원', '디그니티 호텔 정상가 : 89,096원 &gt; 할인가 : 84,641원', '라마다 속초 정상가 : 104,900원 &gt; 할인가 : 99,655원', '오션스위츠 제주 정상가 : 79,001원 &gt; 할인가 : 75,051원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', 'KB국민카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성카드 7만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY 전용] NH농협카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>피코크 12/22(목) 8PM</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>피코크/프레시지 최대 30% 크리스마스 홈파티!</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003421&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>피코크@SSG.LIVE 12/22(목)20:00PM</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2022-12-13</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2022-12-24</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 피코크@SSG.LIVE 12/22(목)20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2022-12-01</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>12월 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~50% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '(카드사할인 12/8-25) 헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Dec 29 01:24:23 UTC 2022
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,22 +473,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023 설 스페셜 혜택전</t>
+          <t>설 선물세트 다함께 공동구매 1탄 _프리미엄</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>단 3일간, 최대 3만원 선물세트 전용쿠폰</t>
+          <t>최대 40%할인 + 목표달성하면 SSG머니 최대 6만원 혜택</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003554</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003545</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023 설 스페셜 혜택전</t>
+          <t>[명절]설 공동구매 1탄</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -498,261 +498,261 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-12-28</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 설 스페셜 혜택전', '스마일클럽', '4종쿠폰', '카드사 청구할인', '명절 종합 선물세트 4종 쿠폰', '      명절 선물 전용 3,000원 쿠폰 (점포명절, 명절)', '      명절 선물 전용 7,000원 쿠폰 (점포명절, 명절)', '      명절 선물 전용 15,000원 쿠폰 (점포명절, 명절)', '      명절 선물 전용 30,000원 쿠폰 (점포명절, 명절)', '쿠폰 발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '[명절] [점포 명절] 엠블렘이 있는 설 명절 기프트 상품 전용 쿠폰입니다.', '[카드 50% 할인]LG 선물 세트)리튠 녹용진액 골드 3종 기획세트', '[SSGPAY머니 증정][1/5(목)이후 순차출고][냉동][오늘의소] 꽃갈비를 품은 블랙앵거스 LA갈비 선물세트 3kg', '[20만원↑구매시3만원쓱머니증정][배송일 해피콜][직접배송][SSG정담][과일愛]프라이빗 과일선물세트 후룻디니뜨 혼합 9호 (샤인머스켓3 / 사과2 / 배2 / 자몽2 - 4.8kg) - 보자기포장', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가', '최대 57% 할인! GC녹십자 설 명절 건강 선물세트', '[백화점라인/국내배송] 폴로 랄프로렌 이태리산 울 100% 시그니처 멀티로고 폴로 머플러 (6color)', '[해외직구] 포켓몬 몬스터볼 변신 피규어 6종세트 무료배송 빠른 출고', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '새해맞이 댕댕이 한복/배변패드/유모차 할인 구경하시개!', '설맞이 설레는 고양이 모래/캣타워/스크래쳐 용품 할인전', '- 삼성카드 청구할인 -']</t>
+          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 1탄', '스마일클럽', '명절 선물세트 7종 최대 40% 할인 + 공동구매 혜택 최대 6만원 적립', '공구 이벤트 기간 : 12월 26일 ~ 1월 1일', '[오메드] 오일 비네거 세트 30% 할인 + 최대 8천원 적립!', '[꽁피튀르] 파리지엥잼 선물세트 30% 할인 + 최대 8천원 적립!', '[SSG 정담] 프리미엄 선물세트 33% 할인 + 최대 8천원 적립!', '프리미엄 망고혼합 선물세트 17% 할인 + 최대 1만원 적립!', '[종근당건강] 6년근 홍삼정업 세트 20% 할인 + 최대 1만원 적립!', '[고려천홍삼] 프리미엄 녹용홍삼 37% 할인 + 최대 8천원 적립!', '호주산 LA갈비 선물세트 28% 할인 + 최대 8천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>설 선물세트 다함께 공동구매 1탄 _프리미엄</t>
+          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 40%할인 + 목표달성하면 SSG머니 최대 6만원 혜택</t>
+          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003545</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[명절]설 공동구매 1탄</t>
+          <t>선물하기로 쓱- 마음을 전하세요</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-12-26</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 1탄', '스마일클럽', '명절 선물세트 7종 최대 40% 할인 + 공동구매 혜택 최대 6만원 적립', '공구 이벤트 기간 : 12월 26일 ~ 1월 1일', '[오메드] 오일 비네거 세트 30% 할인 + 최대 8천원 적립!', '[꽁피튀르] 파리지엥잼 선물세트 30% 할인 + 최대 8천원 적립!', '[SSG 정담] 프리미엄 선물세트 33% 할인 + 최대 8천원 적립!', '프리미엄 망고혼합 선물세트 17% 할인 + 최대 1만원 적립!', '[종근당건강] 6년근 홍삼정업 세트 20% 할인 + 최대 1만원 적립!', '[고려천홍삼] 프리미엄 녹용홍삼 37% 할인 + 최대 8천원 적립!', '호주산 LA갈비 선물세트 28% 할인 + 최대 8천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>선물하기로 쓱- 마음을 전하세요</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '      이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '      카드혜택 + 스마일클럽 혜택', '      이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>연말 홈파티 메뉴 추천</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>최대 30% 할인부터 페이백 이벤트까지</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>Holiday at Home</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>연말 홈파티 메뉴 추천</t>
+          <t>W컨셉 베스트 브랜드 셀렉션</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>최대 30% 할인부터 페이백 이벤트까지</t>
+          <t>13% 쿠폰+모두가 사랑한 브랜드를 한 자리에!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003454</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Holiday at Home</t>
+          <t>[12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-12-26</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION', '스마일클럽', '01) SPECIAL OFFER 13% 쿠폰 바로보기', '01) SPECIAL OFFER 13% 쿠폰 상품 쿠폰', '1만원 이상 구매시 최대 2만원 할인 -기간 내 ID당 4장 발급 가능-', '         쿠폰 발급 및 사용 기간', '         - 1만원 이상 상품 구매 시 13% 할인, 최대 2만원 (기간내 ID당 발급수량 4장)', '         쿠폰 적용 방법', '- 쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>W컨셉 베스트 브랜드 셀렉션</t>
+          <t>스마일클럽 12월의 가입 혜택</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13% 쿠폰+모두가 사랑한 브랜드를 한 자리에!</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003454</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION</t>
+          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-12-26</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION', '스마일클럽', '01) SPECIAL OFFER 13% 쿠폰 바로보기', '01) SPECIAL OFFER 13% 쿠폰 상품 쿠폰', '1만원 이상 구매시 최대 2만원 할인 -기간 내 ID당 4장 발급 가능-', '         쿠폰 발급 및 사용 기간', '         - 1만원 이상 상품 구매 시 13% 할인, 최대 2만원 (기간내 ID당 발급수량 4장)', '         쿠폰 적용 방법', '- 쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>인기브랜드 15% 쿠폰 혜택</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>2023 스마일클럽 건강 프로젝트</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -762,71 +762,71 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '건강 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', '      쿠폰발급 및 사용 기간', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰은 기간 내 ID당 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점, 이마트몰, 새벽배송, 트레이더스몰에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니 쿠폰으로 구매 건 내 해당 브랜드에 적용되며, 3만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '해피라운지★올인원 이뮨 액상 비타민 구매시 콜라겐 구미 증정★', '이마트 선물세트 할인 및 적립 상품권 증정까지 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>[e득라이브] 과일 12/29(목) 11AM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>인기브랜드 15% 쿠폰 혜택</t>
+          <t>딸기/칼밤/레드향/감귤 최대 57% / 이마트 금액권 최대 5만원 증정 행사</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003570</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>[e득라이브] 과일 @SSG.LIVE 12/29(목) 11:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-12-23</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2022-12-29</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '건강 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', '      쿠폰발급 및 사용 기간', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰은 기간 내 ID당 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점, 이마트몰, 새벽배송, 트레이더스몰에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니 쿠폰으로 구매 건 내 해당 브랜드에 적용되며, 3만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '겨울맞이 10% 즉시 할인중♥', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '해피라운지★올인원 이뮨 액상 비타민 구매시 콜라겐 구미 증정★', '이마트 선물세트 할인 및 적립 상품권 증정까지 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; [e득라이브] 과일 @SSG.LIVE 12/29(목) 11:00', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[월간캠핑쇼]  이타카 12/26(월) 7PM</t>
+          <t>12월 BEST 유아동 크리스마스 선물</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>그랑데 스테이션 38만원+코베아 3웨이 구이바다 6.9만원대 핫딜</t>
+          <t>산타가 골라준 홀리데이 장난감</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003558&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[쓱라이브] 이타카 12/26(월) 7PM</t>
+          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-12-21</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -836,116 +836,42 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 이타카 12/26(월) 7PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>포레오 12/27(화) 8PM</t>
+          <t>12월 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>라이브중에만 추가 10% 쿠폰! 쏟아지는 구매인증 선물까지</t>
+          <t>지금 할인 중! ~50% 할인 혜택</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003559&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[신세계라이브쇼핑] 포레오 12/27(화) 8PM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-12-21</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [신세계라이브쇼핑] 포레오 12/27(화) 8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2022-12-01</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>12월 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~50% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Jan  2 01:23:37 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,407 +473,629 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>설 선물세트 다함께 공동구매 1탄 _프리미엄</t>
+          <t>DAY1 하나되어 더 큰 할인</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>최대 40%할인 + 목표달성하면 SSG머니 최대 6만원 혜택</t>
+          <t>쓱배송 10%+라이프스타일 최대 ~12% 3만원 쿠폰</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003545</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003414</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[명절]설 공동구매 1탄</t>
+          <t>Day1 Home - 하나되어 더 큰 할인! 혜택의 대축제</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-12-26</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-04</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 1탄', '스마일클럽', '명절 선물세트 7종 최대 40% 할인 + 공동구매 혜택 최대 6만원 적립', '공구 이벤트 기간 : 12월 26일 ~ 1월 1일', '[오메드] 오일 비네거 세트 30% 할인 + 최대 8천원 적립!', '[꽁피튀르] 파리지엥잼 선물세트 30% 할인 + 최대 8천원 적립!', '[SSG 정담] 프리미엄 선물세트 33% 할인 + 최대 8천원 적립!', '프리미엄 망고혼합 선물세트 17% 할인 + 최대 1만원 적립!', '[종근당건강] 6년근 홍삼정업 세트 20% 할인 + 최대 1만원 적립!', '[고려천홍삼] 프리미엄 녹용홍삼 37% 할인 + 최대 8천원 적립!', '호주산 LA갈비 선물세트 28% 할인 + 최대 8천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; Day1 Home - 하나되어 더 큰 할인! 혜택의 대축제', '스마일클럽', 'Day1 Home - 하나되어 더 큰 할인! 혜택의 대축제', '하나되어 더 큰 할인 DAY1 (현재페이지)', '하나되어 더 큰 할인 DAY1', '새해엔 더 큰 할인! DAY1 혜택 대축제', '01. 매일매일 쓱배송 10% 할인 쿠폰', '선착순 15,000명', '선착순 3만명', '       10% 장바구니 쿠폰', '       쓱배송 상품 전용', '       7만원 이상 구매시, 최대 1만원 할인', '       쿠폰 적용 대상 : 이마트몰, 트레이더스 쓱배송/새벽배송 점포택배 상품 (일부상품 제외)', '쿠폰 받기 -ID당 1일 1회 다운가능-', '       쿠폰 발급 기간', '       매일 오전 9시 선착순 발급', '       쿠폰 사용 기간', '       쿠폰 발급 후 당일 23:59까지 사용', '       쿠폰 사용 조건', '       쿠폰 사용 대상 : 이마트몰, 트레이더스 쓱배송/새벽배송 점포택배 상품 (일부상품 제외)', '       쿠폰 발급 대상', '02. 라이프스타일 최대 12% 최대 3만원 쿠폰', '       7% 장바구니 쿠폰', '       일별 선착순 5만명', '       7만원 이상 구매 시 최대 1만원 할인', '       10만원 이상 구매 시 최대 2만원 할인', '       12% 장바구니 쿠폰', '       15만원 이상 구매 시 최대 3만원 할인', '쿠폰 받기 -기간 내 ID당 1회-', '+ 스마일클럽이라면 특별쿠폰 1장 더!', '       일별 선착순 3,500명', '       10만원 이상 구매 시 최대 3만원 할인', '       쿠폰 발급 후 1/04(수)까지', '       (선착순 수량 종료시 쿠폰 마감될 수 있습니다)', '       본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '+ 카드 청구할인 혜택도 챙겨가세요!', '오늘의 카드 청구할인', '꽝 없는 100% 당첨! 23년도 올해 나의 행운은\xa0', '03. 쓱쓱쓱 스크래치 SSG머니 (일별 선착순 3만명)', '혜택메뉴판 반값다~딜 : 21.12.30 이후 쓱배송 구매 이력이 없는 고객님 대상', '#2. 첫 달은 무료! 스마일클럽 가입해서 혜택받기', '       선착순 1만명', '       5만원 이상 결제 시 최대 3만원 할인', '       쿠폰적용 대상 : 신세계몰 신세계백화점', '       12/31~1/4 기간 중 SSG.COM에서 스마일클럽 멤버십을 최초 신규 가입한 고객 대상', '       신세계몰, 신세계백화점 상품을 5만원 이상 결제시 12% (최대 3만원) 장바구니 할인', '오늘의 초특가 타임딜 &amp; 브랜드 행사', '타임딜 하이라이트', '11시 : 한국금거래소 - 초특가 핫딜 골드바, 토끼 골드바 &amp; S머니 최대 4만원 적립!', '20시 : LG - LG전자 울트라기어 게이밍모니터/일체형PC 역대급 핫딜특가', '21시 : 바디프렌드 - 바디프렌드 A급리퍼 한정수량 선착순', '11시 : 필립스 - 내 집을 홈카페로! 필립스 커피머신 베스트모델 30만8천원대 핫딜~', '19시 : 다이슨 - 다이슨 청소기 Gen5+클리닝키트, V11+거치대 증정, 백화점 상품권&amp;커피쿠폰 추첨']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
+          <t>이마트몰 DAY1 장보기</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
+          <t>쓱배송 10% 할인 + 특별전단 + 반값다딜까지!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003480</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>선물하기로 쓱- 마음을 전하세요</t>
+          <t>DAY1 - 이마트몰 DAY1 장보기</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-04</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽', '첫 선물하기 기념 SSG 머니 페이백 이벤트 바로보기', '모바일쿠폰', '천명에게 쏟아지는 SSG머니 이벤트', '선물하기가 처음이시라면, 쓱머니 이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 모바일 상품 교환권, 모바일 쿠폰, 외식 식사권 등 e쿠폰 선물하기는 해당 이벤트에서 제외 됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; DAY1 - 이마트몰 DAY1 장보기', '스마일클럽', '하나되어 더 큰 할인 DAY1', '01. 새해에는 더 알뜰하게 장보세요! 쓱배송 10% 할인 쿠폰', '선착순 15000명', '선착순 3만장', '       10% 장바구니 쿠폰', '       쓱배송 상품 전용', '       7만원 이상 구매시, 최대 1만원 할인', '       이마트몰, 트레이더스 쓱배송 새벽배송상품 대상', '쿠폰 받기 -ID당 1일 1회 ', '       쿠폰 발급 기간', '       2022년 12/31(토) ~2023년 1/4(수) / 매일 오전 9시 선착순 발급', '       쿠폰 사용 기간', '       쿠폰 발급 당일 사용 가능', '       쿠폰 사용 조건', '       쿠폰 사용 대상 : 이마트몰 트레이더스 쓱배송/새벽배송, 점포 택배 상품 (일부 상품 제외) ', '       쿠폰 발급 대상', '횡성축협한우 최대 40% 할인', '풀무원최대 1+1 행사 및 경품 추첨 이벤트', '남양유업특가행사 최대 30%할인 다다익선 최대 50% 할인', '피코크유기농 최대 30% 할인', '지퍼락단 2일! 지퍼락 전품목 40% 할인', '밀키트 특집2개구매시 50% 단품 최대 40%할인', '조우겨울철 따뜻한 국물 최대 20% 할인', '3MSSG X 3M 단독할인', '롯데제과주유권 추첨 이벤트', '매일유업유제품 &amp; 분유 특가 최대 30%', '청정원X종가집기프티콘 이벤트', '설화수새해맞이 10% 추가 쿠폰', '피코크최대 50% 할인 + 다다익선 최대 50%', '오뚜기행사품목 3만원 이상 5천원 할인', '쓱배송 첫구매 혜택', '반가운 새해, 첫구매는 반값다~딜', '첫구매는 네 개 다 반값! - 딸기, 계란, 떡, 핫초코 모두 반값에 구매하세요', '※ 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매이력이 없는 고객을 포함합니다.', '반값 딸기 - 향도 달콤, 맛도 달콤한 제철딸기(최대할인금액 5천원)', '반값 계란 - 온가족이 좋아하는 우리집 식탁 필수템(최대할인금액 3천원)', '반값 떡 - 간식으로도, 식사로도 간편하고 맛있는 우리떡(최대할인금액 3천원)', '반값 핫초코 - 몸도 마음도 녹여주는 따뜻한 핫초코 한잔(최대할인금액 3천원)', '첫구매는 무료매송!', '첫구매라면 반값으로 구매하고, 무료로 배송받으세요.', '       무료배송', '       첫구매 전용', '       20,000원 이상 구매시 사용가능', '       무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '고객님들의 성원에 힘입어 반값다딜 쿠폰이 조기마감 되었습니다.감사합니다.', '쿠폰 받기 - 기간 내 ID당 1회', '       상품할인쿠폰: 2022년 12/31(토) ~ 2023년 1/4(수)', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 딸기 1개, 계란 1개,, 떡 1개, 핫초코 1개 적용 가능.(ex. 딸기 2개 구매시 1개에만 적용 가능합니다)', '       첫구매 쿠폰 CAT', '       딸기 50% cat', '       계란 50% cat', '       떡 50% cat', '       핫초코 50% cat']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>DAY 1 초특가 타임딜</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>에어팟 프로 2세대&amp;나이키 에어맥스 최대 66% OFF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003478</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>Day1 - 라이프스타일 초특가</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-04</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 한달 내내 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 한달 내내 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 6월 1일 부터 2022년 11월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 6월 1일 부터 2022년 11월 30일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       해당 5% 적립은 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지!', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', 'SSG.COM카드 Edition2는 실물카드 수령 전에도SSGPAY를 통해 바로 결제 가능합니다 (단, 실물카드 수령 전까지 SSG.COM 1회 결제 한도는 100만원으로 제한됨)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; Day1 - 라이프스타일 초특가', '스마일클럽', '하나되어 더 큰 할인 DAY 1', '신세계몰 &amp; 신세계백화점 혜택 축제 라이프스타일 12% 최대 3만원 쿠폰', '7% 장바구니 쿠폰 - 7만원 이상 구매시, 최대 1만원 할인(일별 선착순 5만명, 최대 1만원)', '10% 장바구니 쿠폰 - 10만원 이상 구매시, 최대 2만원 할인(일별 선착순 5만명, 최대 2만원)', '12% 장바구니 쿠폰 - 15만원 이상 구매시, 최대 3만원 할인(일별 선착순 5만명, 최대 3만원)', '쿠폰 발급 기간 : 2022년 12/31(토) ~2023년 1/04(수)', '스마일클럽이라면 특별쿠폰 1장 더!', '12% 장바구니 쿠폰 - 10만원 이상 구매시, 최대 3만원 할인(스마일클럽 전용, 일별 선착순 3,500명)', '아직 스마일클럽 고객이 아니라면\xa0', '쿠폰 발급 기간 : 2022년 12/31(토) ~2023년 1/04(수) (선착순 수량 종료시 쿠폰 마감될 수 있습니다)', '본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '쿠폰 발급 대상 : 본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '+ PLUS 카드 청구할인 혜택도 챙겨가세요!', '매일 오전 9시 열리는 오늘의 초특가 타임딜', '금일 타임딜은 9시에 오픈됩니다!', '타임딜 스케쥴']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>DAY1 메타버쓱 오픈런 한정상품 구매</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>달릴 준비되셨나요? 빠른 자가 갖는다!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003293</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>Day1 - 메타버쓱 오픈런 구매 도전</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-04</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '      이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '      카드혜택 + 스마일클럽 혜택', '      이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%']</t>
+          <t>['이벤트/쿠폰 &gt; Day1 - 메타버쓱 오픈런 구매 도전', '스마일클럽', '역대가 도전 오쏘몰 60일분 (이뮨 정제+드링크) : 148,500원에서 오픈런 가격 : 79,000원 (선착순 150명, 해외직구)', '오픈런이니까 가능한 가격 페이즈 외식 5만원권 정상가 : 50,000원에서 오픈런 가격 : 30,000원 (선착순 400명)', '금시세 파괴 23년 계묘년 토끼 골드바 정상가 : 386,200원에서 오픈런 가격 : 305,304원 (선착순 150명)', '코카콜라 제로 355ml 24CAN 정상가 : 24,500원에서 오픈런 가격 : 10,900원 (선착순 600명, 캔당 450원)', '겨울 캠핑 NO.1 상품 코베아 구이바다 M 아이보리 (+가방세트) 정상가 : 138,000원에서 오픈런 가격 : 45,000원 (선착순 150명)', '믿고 쓰는 수지 파데 랑콤 뗑 이돌 롱라스팅 30ml + 30ml 정품 용량 추가 증정 정상가 : 79,000원 SSG머니 3.5만원 적립 (선착순 200명)', '선착순 당첨 완료(연습을 통해 다음 오픈런을 도전해보세요)', '       선착순에 들었다면', '선착순 당첨자 한정 구매', '선착순 판매완료', '      오전 10시 - 역대가 도전 오쏘몰 60일분(이뮨 정제+드링크) 79,000원(선착순 150명, 해외직구)', '      오후 2시 - 오픈런이니까 가능한 가격 페이즈 외식 5만원권 30,000원(선착순 400명)', '      오전 10시 - 금시세 파괴 23년 계묘년 토끼 골드바 305,304원(선착순 150명)', '      오후 2시 - 캔당 450원 코카콜라 제로 355ml 24CAN 10,900원(선착순 600명)', '      오전 10시 - 겨울 캠핑 NO.1 상품 코베아 구이바다 M 아이보리(+가방세트) 45,000원(선착순 150명)', '      오후 2시 - 믿고 쓰는 수지 파데 랑콤 뗑 이돌 롱라스팅 30ml SSG머니 3.5만원 적립(선착순 200명)', '쉽고 재밌는 메타버쓱 속 보물 찾기! 진짜 순금 골드바 경품 + 선착순 SSG머니 1천원까지']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>연말 홈파티 메뉴 추천</t>
+          <t>DAY1 메타버쓱 재밌는 보물찾기</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>최대 30% 할인부터 페이백 이벤트까지</t>
+          <t>누구나 참여 시 골드바 경품 + SSG머니 증정</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003406</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003294</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Holiday at Home</t>
+          <t>Day1 - 메타버쓱 보물찾기 보물을 찾아라!</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-04</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Holiday at Home', '스마일클럽', '공동 구매 이벤트', ' SSG.COM 안의 작은 카페, Cafe at HOME 입니다. 12월 이벤트 토픽은 ‘홀리데이’에요. 홈파티 상품 할인부터 귀여운굿즈까지 영상으로 소개해드릴게요. ', 'EVENT01 홈파티 인기 상품 공구 이벤트', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸됩니다.', '본 이벤트는 당사의 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '새벽배송을 7만원 이상 주문하면, 카페앳홈의 귀여운 한정판 굿즈를 랜덤으로 알비백 안에 쏙 담아드립니다. 선착순 5백명이니, 서두르시면 좋아요!', '이벤트 기간 내 새벽배송 7만원 이상 주문 시 주문서에 사은품이 자동으로 포함됩니다.', '선착순 수량이 모두 소진되었을 시, 주문서에 사은품이 보이지 않습니다.', '      새벽배송 7만원 이상 주문 시, 선착순 증정', '주문서에 사은품이 보이지 않을 시, 선착순 수량이 모두 소진된 것임을 참고해주세요.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; Day1 - 메타버쓱 보물찾기 보물을 찾아라!', '스마일클럽', '       매일 오전 10시 선착순 5천명', '이벤트 기간 : 2023년 1월 2일 (월) 10:00 ~ 1월 4일 (수) 23:59', '       SSG머니 1천원 응모 버튼 클릭 시 선착순 한정 즉시 지급되며, 지급일로부터 7일간 사용 가능합니다.', '       경품은 이벤트 응모 시 사용한 ID 회원정보 상의 휴대폰 번호와 주소지 기준으로 발송되오니, 개인정보를 꼭 확인해 주세요.', '       이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>W컨셉 베스트 브랜드 셀렉션</t>
+          <t>신세계백화점 쓱페스타</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13% 쿠폰+모두가 사랑한 브랜드를 한 자리에!</t>
+          <t>10% 쿠폰 + 2023분께 경품 혜택까지!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003454</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003546</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION</t>
+          <t>(0102-0108) 신세계백화점 쓱페스타</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-12-26</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-08</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/26~1/1] 2022 W컨셉 BEST BRAND SELECTION', '스마일클럽', '01) SPECIAL OFFER 13% 쿠폰 바로보기', '01) SPECIAL OFFER 13% 쿠폰 상품 쿠폰', '1만원 이상 구매시 최대 2만원 할인 -기간 내 ID당 4장 발급 가능-', '         쿠폰 발급 및 사용 기간', '         - 1만원 이상 상품 구매 시 13% 할인, 최대 2만원 (기간내 ID당 발급수량 4장)', '         쿠폰 적용 방법', '- 쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0108) 신세계백화점 쓱페스타', '스마일클럽', '01. 쓱페스타 10% 쿠폰 바로보기', '03. 신년 맞이 경품 이벤트 바로보기', '01. 쓱페스타 10% 쿠폰', '쿠폰 다운 받기', '쿠폰 마감되었습니다.', "발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다", '03. 2023쓱페스타 구매 이벤트 신세계백화점이 2023명에게 추첨을 통해 새해 맞이 선물을 드립니다!', '경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다', '이벤트 기간 내 경품 응모 후 주문 후 취소/반품하신 고객은 경품 응모 대상에서 제외됩니다', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다', 'DAY1 새해 첫 득템은 SSG.COM에서! 초특가부터 쿠폰까지 하나되어 더 큰 할인 DAY1 바로 가기']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>스마일클럽 12월의 가입 혜택</t>
+          <t>2023 순금 GOLD WEEK</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>새해맞이 순금제품 구매하면 SSG머니 ~4만원</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003057</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003691</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[스마일클럽] 12월 내내 매일매일 스마일</t>
+          <t>2023 순금 GOLD WEEK</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-12-05</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-08</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 12월 내내 매일매일 스마일', '스마일클럽', '[스마일클럽] 12월 내내 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', '스마일클럽 전용 혜택을 잡으세요!', '스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일 클럽 전용 15% 쿠폰으로 건강을 선물해요!', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 순금 GOLD WEEK', '스마일클럽', '구매사은 대상금액은 지정된 구매사은의 실구매금액기준(상품쿠폰/에누리 및 배송비제외) 으로 적용되며 하단 [신청가능내역조회]를 통해 확인가능합니다. ', '이벤트에 응모하시고 결제취소 하셨더라도,\xa0행사 마감 전까지\xa0다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다. ', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우,\xa0이벤트 신청을 완료하셨더라도 이벤트 대상에서 제외됩니다 ', '본 이벤트에 응모하실 경우 개인정보\xa0(회원ID\xa0등)\xa0제공에 동의하신 것으로 간주되며,\xa0제공된 정보는\xa0SSG머니 지급 후 즉시 파기합니다.', "이벤트 참여 후 'MY SSG &gt; 이벤트 참여 현황' 에서 참여여부 확인가능합니다. ", '고순도 999.9% 계묘년 토끼 골드바']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>인기브랜드 15% 쿠폰 혜택</t>
+          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003386</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트</t>
+          <t>선물하기로 쓱- 마음을 전하세요</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트', '스마일클럽', '2023 스마일클럽 건강 프로젝트', '건강 TOP 브랜드 15% 쿠폰', '스마일클럽 회원 전용', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', '      쿠폰발급 및 사용 기간', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #연말연시선물 #새해새다짐 #탑브랜드', '쿠폰은 기간 내 ID당 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점, 이마트몰, 새벽배송, 트레이더스몰에 적용되는 쿠폰입니다.', '본 쿠폰은 장바구니 쿠폰으로 구매 건 내 해당 브랜드에 적용되며, 3만원 이상 주문 시 쿠폰이 적용됩니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰발급 및 사용 기간 :  2022년 12월 19일(월) ~ 12월 31일(토)  ', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '해피라운지★올인원 이뮨 액상 비타민 구매시 콜라겐 구미 증정★', '이마트 선물세트 할인 및 적립 상품권 증정까지 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[e득라이브] 과일 12/29(목) 11AM</t>
+          <t>설 선물도 역시! 선물하기로</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>딸기/칼밤/레드향/감귤 최대 57% / 이마트 금액권 최대 5만원 증정 행사</t>
+          <t>쓱에서 선물하면 내 선물도 쓱-</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003570</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[e득라이브] 과일 @SSG.LIVE 12/29(목) 11:00</t>
+          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-12-23</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022-12-29</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [e득라이브] 과일 @SSG.LIVE 12/29(목) 11:00', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>12월 BEST 유아동 크리스마스 선물</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>산타가 골라준 홀리데이 장난감</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003103</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [12/01-31] 12월의 유아동 매거진 Little SSG X 스타일러', '스마일클럽', '"설레는 마음으로 크리스마스를 준비하는 시즌 스타일러맘과 함께하는 퀵 월간 쇼핑, \'리틀 쓱\'과 함께해요!" 이런저런 고민 없이 클릭 한 번이면 육아템을 빠르게 구매할 수 있는 시대. 기존 \'유아동 전문관\'에서 \'리틀 쓱(Little SSG)\'으로 새롭게 선보이는 SSG닷컴(www.ssg.com)을 만나보세요. 계절에 꼭 필요한 각종 패션 아이템부터 아이와 집 안에서 보내는 시간을 풍요롭게 도와줄 교육 놀잇감, 친환경 육아용품 등 매달 &lt;스타일러&gt; 지면과 함께하는 유아동 기획전을 리틀 쓱 페이지에서도 소개합니다! ‘쓱 배송’은 물론 ‘타임 딜’ 등 수시로 열리는 다양한 이벤트 혜택까지, 현명한 스타일러맘이라면 지금 당장 리틀 쓱 페이지에 접속!']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>12월 맘키즈 PLUS</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>지금 할인 중! ~50% 할인 혜택</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>이달의 맘키즈 PLUS</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2999-12-13</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '콩순이 NEW콩순이냉장고 (N2쓱배송, 전국택배)', '자연나라 세종대왕김 국산 100% 도시락김 5g 36봉', '[맘키즈특가40%할인]서경한우 미경산 암소한우 1++등급  불고기 300g(냉장)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023 스마일클럽 건강 프로젝트_</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-01-22</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송] 정관장 홍삼진황 50ml*20포', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>이번주 월요일은 장보기 더블적립</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DAY1 스마일클럽 전용 할인까지</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-01-02</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2023-01-31</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'DAY 1월 2일 월요일은 스마일클럽 장보기 최대 10% 적립 DAY', '스마일클럽 기본적립 + 추가적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '새해맞이 다 모여 더 큰 할인 DAY1 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>신년 골드바 1/2(월) 11AM</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>초특가 핫딜 골드바 &amp; S머니 최대 4만원적립</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003669&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>순금 골드바@SSG.LIVE 1/2(월)11:00AM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-12-27</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023-01-04</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 순금 골드바@SSG.LIVE 1/2(월)11:00AM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LG전자 1/2(월) 8PM</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>LG전자 울트라기어 게이밍모니터 역대급 핫딜 + 일체형 PC SSG 단독특가</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003616</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>LG전자 @SSG.LIVE 1/2(월) 20:00PM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022-12-26</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2023-01-02</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; LG전자 @SSG.LIVE 1/2(월) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>바디프랜드 1/2(월) 9PM</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>바디프랜드 A급리퍼 한정수량 90만원대~ &amp; 특별사은품 2종</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003639</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>바디프랜드 @SSG.LIVE 1/2(월) 9PM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2022-12-26</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2023-01-02</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 바디프랜드 @SSG.LIVE 1/2(월) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>USM 1/3(화) 8PM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>국내 최초 라이브! 바로배송에 200만원 이상 구매시 10만원 상품권 증정</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003662&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>[쓱라이브] USM 1/3(화) 8PM</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2022-12-27</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2023-01-06</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] USM 1/3(화) 8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Jan  5 01:27:08 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,170 +473,170 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAY1 하나되어 더 큰 할인</t>
+          <t>첫구매는 반값다~딜</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>쓱배송 10%+라이프스타일 최대 ~12% 3만원 쿠폰</t>
+          <t>첫구매는 네 개 다 반값 + 무료배송</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003414</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003710&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Day1 Home - 하나되어 더 큰 할인! 혜택의 대축제</t>
+          <t>첫구매는 네 개 다 반값! 반값다딜 (1/5~11)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Day1 Home - 하나되어 더 큰 할인! 혜택의 대축제', '스마일클럽', 'Day1 Home - 하나되어 더 큰 할인! 혜택의 대축제', '하나되어 더 큰 할인 DAY1 (현재페이지)', '하나되어 더 큰 할인 DAY1', '새해엔 더 큰 할인! DAY1 혜택 대축제', '01. 매일매일 쓱배송 10% 할인 쿠폰', '선착순 15,000명', '선착순 3만명', '       10% 장바구니 쿠폰', '       쓱배송 상품 전용', '       7만원 이상 구매시, 최대 1만원 할인', '       쿠폰 적용 대상 : 이마트몰, 트레이더스 쓱배송/새벽배송 점포택배 상품 (일부상품 제외)', '쿠폰 받기 -ID당 1일 1회 다운가능-', '       쿠폰 발급 기간', '       매일 오전 9시 선착순 발급', '       쿠폰 사용 기간', '       쿠폰 발급 후 당일 23:59까지 사용', '       쿠폰 사용 조건', '       쿠폰 사용 대상 : 이마트몰, 트레이더스 쓱배송/새벽배송 점포택배 상품 (일부상품 제외)', '       쿠폰 발급 대상', '02. 라이프스타일 최대 12% 최대 3만원 쿠폰', '       7% 장바구니 쿠폰', '       일별 선착순 5만명', '       7만원 이상 구매 시 최대 1만원 할인', '       10만원 이상 구매 시 최대 2만원 할인', '       12% 장바구니 쿠폰', '       15만원 이상 구매 시 최대 3만원 할인', '쿠폰 받기 -기간 내 ID당 1회-', '+ 스마일클럽이라면 특별쿠폰 1장 더!', '       일별 선착순 3,500명', '       10만원 이상 구매 시 최대 3만원 할인', '       쿠폰 발급 후 1/04(수)까지', '       (선착순 수량 종료시 쿠폰 마감될 수 있습니다)', '       본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '+ 카드 청구할인 혜택도 챙겨가세요!', '오늘의 카드 청구할인', '꽝 없는 100% 당첨! 23년도 올해 나의 행운은\xa0', '03. 쓱쓱쓱 스크래치 SSG머니 (일별 선착순 3만명)', '혜택메뉴판 반값다~딜 : 21.12.30 이후 쓱배송 구매 이력이 없는 고객님 대상', '#2. 첫 달은 무료! 스마일클럽 가입해서 혜택받기', '       선착순 1만명', '       5만원 이상 결제 시 최대 3만원 할인', '       쿠폰적용 대상 : 신세계몰 신세계백화점', '       12/31~1/4 기간 중 SSG.COM에서 스마일클럽 멤버십을 최초 신규 가입한 고객 대상', '       신세계몰, 신세계백화점 상품을 5만원 이상 결제시 12% (최대 3만원) 장바구니 할인', '오늘의 초특가 타임딜 &amp; 브랜드 행사', '타임딜 하이라이트', '11시 : 한국금거래소 - 초특가 핫딜 골드바, 토끼 골드바 &amp; S머니 최대 4만원 적립!', '20시 : LG - LG전자 울트라기어 게이밍모니터/일체형PC 역대급 핫딜특가', '21시 : 바디프렌드 - 바디프렌드 A급리퍼 한정수량 선착순', '11시 : 필립스 - 내 집을 홈카페로! 필립스 커피머신 베스트모델 30만8천원대 핫딜~', '19시 : 다이슨 - 다이슨 청소기 Gen5+클리닝키트, V11+거치대 증정, 백화점 상품권&amp;커피쿠폰 추첨']</t>
+          <t>['이벤트/쿠폰 &gt; 첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '스마일클럽', '첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '첫구매 전용 프로모션', '반값다~딜 - 50% / 무료배송', '첫구매는 네 개 다 반값!', '※ 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매이력이 없는 고객을 포함합니다.', '반값 귤추운 겨울, 이불 속에서 까먹는 새콤달콤한 별미 (최대 할인금액 5천원)', '반값 떡볶이추운 겨울, 이불 속에서 까먹는 새콤달콤한 별미 (최대 할인금액 5천원)', '반값 과자(파이류)한눈팔면 무한흡입! 폭신폭신 달콤한 파이 과자 (최대 할인금액 3천원)', '반값 과채음료생기를 채워주는 상큼한 과채음료 (최대 할인금액 3천원)', '첫구매는 무료배송!', '첫구매라면 반값으로 구매하고, 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능 - 무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 한번에 받기 - 기간 내 ID당 1회 -', '       쿠폰 사용 기간', '       상품할인쿠폰 : 2023년 1월 5일(목) ~2023년 1월 11일(수)', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 귤 1개, 떡볶이 1개, 과자(파이/케익류) 1개, 과일음료 1개 적용 가능 (ex. 귤 2개 구매시에도 1개에만 적용 가능합니다)', '       ＊첫구매 쿠폰 CAT', '       귤 50% cat (최대 5천원 할인)', '       떡볶이 50% cat (최대 3천원 할인)', '       과자(파이/케익류) 50% cat (최대 3천원 할인)', '       과일음료 50% cat (최대 3천원 할인)', '첫구매 전용 오늘의 상품 보기']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>이마트몰 DAY1 장보기</t>
+          <t>설 선물세트 다함께 공동구매 2탄 _ 가성비상품편</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>쓱배송 10% 할인 + 특별전단 + 반값다딜까지!</t>
+          <t>최대 74%할인 + 목표달성하면 SSG머니 최대 5만원 혜택</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003480</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003656</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DAY1 - 이마트몰 DAY1 장보기</t>
+          <t>[명절]설 공동구매 2탄_가성비상품편</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; DAY1 - 이마트몰 DAY1 장보기', '스마일클럽', '하나되어 더 큰 할인 DAY1', '01. 새해에는 더 알뜰하게 장보세요! 쓱배송 10% 할인 쿠폰', '선착순 15000명', '선착순 3만장', '       10% 장바구니 쿠폰', '       쓱배송 상품 전용', '       7만원 이상 구매시, 최대 1만원 할인', '       이마트몰, 트레이더스 쓱배송 새벽배송상품 대상', '쿠폰 받기 -ID당 1일 1회 ', '       쿠폰 발급 기간', '       2022년 12/31(토) ~2023년 1/4(수) / 매일 오전 9시 선착순 발급', '       쿠폰 사용 기간', '       쿠폰 발급 당일 사용 가능', '       쿠폰 사용 조건', '       쿠폰 사용 대상 : 이마트몰 트레이더스 쓱배송/새벽배송, 점포 택배 상품 (일부 상품 제외) ', '       쿠폰 발급 대상', '횡성축협한우 최대 40% 할인', '풀무원최대 1+1 행사 및 경품 추첨 이벤트', '남양유업특가행사 최대 30%할인 다다익선 최대 50% 할인', '피코크유기농 최대 30% 할인', '지퍼락단 2일! 지퍼락 전품목 40% 할인', '밀키트 특집2개구매시 50% 단품 최대 40%할인', '조우겨울철 따뜻한 국물 최대 20% 할인', '3MSSG X 3M 단독할인', '롯데제과주유권 추첨 이벤트', '매일유업유제품 &amp; 분유 특가 최대 30%', '청정원X종가집기프티콘 이벤트', '설화수새해맞이 10% 추가 쿠폰', '피코크최대 50% 할인 + 다다익선 최대 50%', '오뚜기행사품목 3만원 이상 5천원 할인', '쓱배송 첫구매 혜택', '반가운 새해, 첫구매는 반값다~딜', '첫구매는 네 개 다 반값! - 딸기, 계란, 떡, 핫초코 모두 반값에 구매하세요', '※ 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매이력이 없는 고객을 포함합니다.', '반값 딸기 - 향도 달콤, 맛도 달콤한 제철딸기(최대할인금액 5천원)', '반값 계란 - 온가족이 좋아하는 우리집 식탁 필수템(최대할인금액 3천원)', '반값 떡 - 간식으로도, 식사로도 간편하고 맛있는 우리떡(최대할인금액 3천원)', '반값 핫초코 - 몸도 마음도 녹여주는 따뜻한 핫초코 한잔(최대할인금액 3천원)', '첫구매는 무료매송!', '첫구매라면 반값으로 구매하고, 무료로 배송받으세요.', '       무료배송', '       첫구매 전용', '       20,000원 이상 구매시 사용가능', '       무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '고객님들의 성원에 힘입어 반값다딜 쿠폰이 조기마감 되었습니다.감사합니다.', '쿠폰 받기 - 기간 내 ID당 1회', '       상품할인쿠폰: 2022년 12/31(토) ~ 2023년 1/4(수)', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 딸기 1개, 계란 1개,, 떡 1개, 핫초코 1개 적용 가능.(ex. 딸기 2개 구매시 1개에만 적용 가능합니다)', '       첫구매 쿠폰 CAT', '       딸기 50% cat', '       계란 50% cat', '       떡 50% cat', '       핫초코 50% cat']</t>
+          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 2탄_가성비상품편', '스마일클럽', '명절 선물세트 7종 최대 74% 할인 + 공동구매 혜택 최대 5만원 적립', '공구 이벤트 기간 : 1월 5일 ~ 1월 11일', '[CJ제일제당]특별한선택 O-1호 40% 할인 + 최대 8천원 적립!', '[휴럼] 천년침향환 3.7g*30환 53% 할인 + 최대 8천원 적립!', '[올즙] 타트체리 주스 1000ml 2병 74% 할인 + 최대 4천원 적립!', '[일리] 스틱커피 선물세트 20% 할인 + 최대 8천원 적립!', '[신세계푸드] 월넛 + 잉글리쉬파운드 22% 할인 + 최대 5천원 적립!', '사과배한라봉 혼합 선물세트 2호 29% 할인 + 최대 8천원 적립!', '블랙앵거스 LA갈비 선물세트 3kg 25% 할인 + 최대 9천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DAY 1 초특가 타임딜</t>
+          <t>신세계백화점 쓱페스타</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>에어팟 프로 2세대&amp;나이키 에어맥스 최대 66% OFF</t>
+          <t>10% 쿠폰 + 2023분께 경품 혜택까지!</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003478</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003546</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Day1 - 라이프스타일 초특가</t>
+          <t>(0102-0108) 신세계백화점 쓱페스타</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-01-08</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Day1 - 라이프스타일 초특가', '스마일클럽', '하나되어 더 큰 할인 DAY 1', '신세계몰 &amp; 신세계백화점 혜택 축제 라이프스타일 12% 최대 3만원 쿠폰', '7% 장바구니 쿠폰 - 7만원 이상 구매시, 최대 1만원 할인(일별 선착순 5만명, 최대 1만원)', '10% 장바구니 쿠폰 - 10만원 이상 구매시, 최대 2만원 할인(일별 선착순 5만명, 최대 2만원)', '12% 장바구니 쿠폰 - 15만원 이상 구매시, 최대 3만원 할인(일별 선착순 5만명, 최대 3만원)', '쿠폰 발급 기간 : 2022년 12/31(토) ~2023년 1/04(수)', '스마일클럽이라면 특별쿠폰 1장 더!', '12% 장바구니 쿠폰 - 10만원 이상 구매시, 최대 3만원 할인(스마일클럽 전용, 일별 선착순 3,500명)', '아직 스마일클럽 고객이 아니라면\xa0', '쿠폰 발급 기간 : 2022년 12/31(토) ~2023년 1/04(수) (선착순 수량 종료시 쿠폰 마감될 수 있습니다)', '본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '쿠폰 발급 대상 : 본 쿠폰은 스마일클럽 회원 전용으로 발급되는 쿠폰입니다.', '+ PLUS 카드 청구할인 혜택도 챙겨가세요!', '매일 오전 9시 열리는 오늘의 초특가 타임딜', '금일 타임딜은 9시에 오픈됩니다!', '타임딜 스케쥴']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0108) 신세계백화점 쓱페스타', '스마일클럽', '01. 쓱페스타 10% 쿠폰 바로보기', '03. 신년 맞이 경품 이벤트 바로보기', '01. 쓱페스타 10% 쿠폰', '쿠폰 다운 받기', '쿠폰 마감되었습니다.', "발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다", '03. 2023쓱페스타 구매 이벤트 신세계백화점이 2023명에게 추첨을 통해 새해 맞이 선물을 드립니다!', '경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다', '이벤트 기간 내 경품 응모 후 주문 후 취소/반품하신 고객은 경품 응모 대상에서 제외됩니다', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다', 'DAY1 새해 첫 득템은 SSG.COM에서! 초특가부터 쿠폰까지 하나되어 더 큰 할인 DAY1 바로 가기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DAY1 메타버쓱 오픈런 한정상품 구매</t>
+          <t>2023 순금 GOLD WEEK</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>달릴 준비되셨나요? 빠른 자가 갖는다!</t>
+          <t>새해맞이 순금제품 구매하면 SSG머니 ~4만원</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003293</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003691</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Day1 - 메타버쓱 오픈런 구매 도전</t>
+          <t>2023 순금 GOLD WEEK</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-01-08</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Day1 - 메타버쓱 오픈런 구매 도전', '스마일클럽', '역대가 도전 오쏘몰 60일분 (이뮨 정제+드링크) : 148,500원에서 오픈런 가격 : 79,000원 (선착순 150명, 해외직구)', '오픈런이니까 가능한 가격 페이즈 외식 5만원권 정상가 : 50,000원에서 오픈런 가격 : 30,000원 (선착순 400명)', '금시세 파괴 23년 계묘년 토끼 골드바 정상가 : 386,200원에서 오픈런 가격 : 305,304원 (선착순 150명)', '코카콜라 제로 355ml 24CAN 정상가 : 24,500원에서 오픈런 가격 : 10,900원 (선착순 600명, 캔당 450원)', '겨울 캠핑 NO.1 상품 코베아 구이바다 M 아이보리 (+가방세트) 정상가 : 138,000원에서 오픈런 가격 : 45,000원 (선착순 150명)', '믿고 쓰는 수지 파데 랑콤 뗑 이돌 롱라스팅 30ml + 30ml 정품 용량 추가 증정 정상가 : 79,000원 SSG머니 3.5만원 적립 (선착순 200명)', '선착순 당첨 완료(연습을 통해 다음 오픈런을 도전해보세요)', '       선착순에 들었다면', '선착순 당첨자 한정 구매', '선착순 판매완료', '      오전 10시 - 역대가 도전 오쏘몰 60일분(이뮨 정제+드링크) 79,000원(선착순 150명, 해외직구)', '      오후 2시 - 오픈런이니까 가능한 가격 페이즈 외식 5만원권 30,000원(선착순 400명)', '      오전 10시 - 금시세 파괴 23년 계묘년 토끼 골드바 305,304원(선착순 150명)', '      오후 2시 - 캔당 450원 코카콜라 제로 355ml 24CAN 10,900원(선착순 600명)', '      오전 10시 - 겨울 캠핑 NO.1 상품 코베아 구이바다 M 아이보리(+가방세트) 45,000원(선착순 150명)', '      오후 2시 - 믿고 쓰는 수지 파데 랑콤 뗑 이돌 롱라스팅 30ml SSG머니 3.5만원 적립(선착순 200명)', '쉽고 재밌는 메타버쓱 속 보물 찾기! 진짜 순금 골드바 경품 + 선착순 SSG머니 1천원까지']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 순금 GOLD WEEK', '스마일클럽', '구매사은 대상금액은 지정된 구매사은의 실구매금액기준(상품쿠폰/에누리 및 배송비제외) 으로 적용되며 하단 [신청가능내역조회]를 통해 확인가능합니다. ', '이벤트에 응모하시고 결제취소 하셨더라도,\xa0행사 마감 전까지\xa0다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다. ', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우,\xa0이벤트 신청을 완료하셨더라도 이벤트 대상에서 제외됩니다 ', '본 이벤트에 응모하실 경우 개인정보\xa0(회원ID\xa0등)\xa0제공에 동의하신 것으로 간주되며,\xa0제공된 정보는\xa0SSG머니 지급 후 즉시 파기합니다.', "이벤트 참여 후 'MY SSG &gt; 이벤트 참여 현황' 에서 참여여부 확인가능합니다. ", '고순도 999.9% 계묘년 토끼 골드바']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DAY1 메타버쓱 재밌는 보물찾기</t>
+          <t>설 선물도 역시! 선물하기로</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>누구나 참여 시 골드바 경품 + SSG머니 증정</t>
+          <t>쓱에서 선물하면 내 선물도 쓱-</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003294</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Day1 - 메타버쓱 보물찾기 보물을 찾아라!</t>
+          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -646,150 +646,150 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Day1 - 메타버쓱 보물찾기 보물을 찾아라!', '스마일클럽', '       매일 오전 10시 선착순 5천명', '이벤트 기간 : 2023년 1월 2일 (월) 10:00 ~ 1월 4일 (수) 23:59', '       SSG머니 1천원 응모 버튼 클릭 시 선착순 한정 즉시 지급되며, 지급일로부터 7일간 사용 가능합니다.', '       경품은 이벤트 응모 시 사용한 ID 회원정보 상의 휴대폰 번호와 주소지 기준으로 발송되오니, 개인정보를 꼭 확인해 주세요.', '       이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>신세계백화점 쓱페스타</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10% 쿠폰 + 2023분께 경품 혜택까지!</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003546</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(0102-0108) 신세계백화점 쓱페스타</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-08</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0108) 신세계백화점 쓱페스타', '스마일클럽', '01. 쓱페스타 10% 쿠폰 바로보기', '03. 신년 맞이 경품 이벤트 바로보기', '01. 쓱페스타 10% 쿠폰', '쿠폰 다운 받기', '쿠폰 마감되었습니다.', "발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다", '03. 2023쓱페스타 구매 이벤트 신세계백화점이 2023명에게 추첨을 통해 새해 맞이 선물을 드립니다!', '경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다', '이벤트 기간 내 경품 응모 후 주문 후 취소/반품하신 고객은 경품 응모 대상에서 제외됩니다', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다', 'DAY1 새해 첫 득템은 SSG.COM에서! 초특가부터 쿠폰까지 하나되어 더 큰 할인 DAY1 바로 가기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023 순금 GOLD WEEK</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>새해맞이 순금제품 구매하면 SSG머니 ~4만원</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003691</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023 순금 GOLD WEEK</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-01-08</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 순금 GOLD WEEK', '스마일클럽', '구매사은 대상금액은 지정된 구매사은의 실구매금액기준(상품쿠폰/에누리 및 배송비제외) 으로 적용되며 하단 [신청가능내역조회]를 통해 확인가능합니다. ', '이벤트에 응모하시고 결제취소 하셨더라도,\xa0행사 마감 전까지\xa0다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다. ', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우,\xa0이벤트 신청을 완료하셨더라도 이벤트 대상에서 제외됩니다 ', '본 이벤트에 응모하실 경우 개인정보\xa0(회원ID\xa0등)\xa0제공에 동의하신 것으로 간주되며,\xa0제공된 정보는\xa0SSG머니 지급 후 즉시 파기합니다.', "이벤트 참여 후 'MY SSG &gt; 이벤트 참여 현황' 에서 참여여부 확인가능합니다. ", '고순도 999.9% 계묘년 토끼 골드바']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Happy Holiday 연말엔 선물하기로 쓱-</t>
+          <t>2022 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>선물하기 처음이라면 SSG머니 행운까지!</t>
+          <t>연말 이벤트전</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003313</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>선물하기로 쓱- 마음을 전하세요</t>
+          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 선물하기로 쓱- 마음을 전하세요', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>설 선물도 역시! 선물하기로</t>
+          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>쓱에서 선물하면 내 선물도 쓱-</t>
+          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
+          <t>2023 스마일클럽 건강 프로젝트_</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -799,303 +799,192 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>1월 가입 웰컴 기프트 5천원</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>명절 선물세트 ~15% 2종 할인까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽 혜택보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'DAY 1월 2일 월요일은 스마일클럽 장보기 최대 10% 적립 DAY', '스마일클럽 기본적립 + 추가적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '새해맞이 다 모여 더 큰 할인 DAY1 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>지금 꼭 먹어야 할 건강 밥상 특집</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>겨울 제철 식품 ~40% 특가</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003621</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>건강 밥상 특집</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 건강 밥상 특집', '스마일클럽', '#최대 40% 할인', '최대 40% 할인 제철 음식 장보기 바로보기', '최대 40% 할인! 제철 수산물', '최대 30% 할인! 제철 채소', '최대 40% 할인! 제철 양곡/견과류', '최대 25% 할인! 제철 과일', 'SSG.COM 푸드마켓 인기상품 할인 최대 20% 할인', '쿠폰 사용 전 꼭 확인하세요(레이어팝업 열기)', '할인 적용 기간 : 2023년 1월 5일(목)~11일(수)', '면역력이 쓱! 스마일클럽 건강식품 최대 15% 쿠폰', '상품쿠폰 15% - 7만원 이상 구매시 최대 1만 5천원 할인(smileClub 전용)', '스마일클럽 15% 쿠폰 받으러 가기', '반가우니까, 네 개 다 반값! 최대 50% 할인 반값다 딜', '만두/떡 동시구매시 10% 에누리 조선호텔 곰탕 20% 할인']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+          <t>아베다 1/5(목) 8PM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+          <t>NEW 스칼프솔루션 런칭! 인바티/보태니컬/로즈메리 24%↓</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003617</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트_</t>
+          <t>[SSG.LIVE] 1/4(목) 8PM 아베다</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2022-12-26</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송] 정관장 홍삼진황 50ml*20포', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE] 1/4(목) 8PM 아베다', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>이번주 월요일은 장보기 더블적립</t>
+          <t>올리브데올리브 1/5(목) 9PM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DAY1 스마일클럽 전용 할인까지</t>
+          <t>올리브데올리브 최대 80%할인! 트와이스 나연 착장 숏패딩 99,000원 한정수량</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003670</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>올리브데올리브 @SSG.LIVE 1/5(목) 9PM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2022-12-27</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'DAY 1월 2일 월요일은 스마일클럽 장보기 최대 10% 적립 DAY', '스마일클럽 기본적립 + 추가적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '새해맞이 다 모여 더 큰 할인 DAY1 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 올리브데올리브 @SSG.LIVE 1/5(목) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>신년 골드바 1/2(월) 11AM</t>
+          <t>1월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>초특가 핫딜 골드바 &amp; S머니 최대 4만원적립</t>
+          <t>매월 쏟아지는 맘키즈 특가!</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003669&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>순금 골드바@SSG.LIVE 1/2(월)11:00AM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-12-27</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 순금 골드바@SSG.LIVE 1/2(월)11:00AM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>LG전자 1/2(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>LG전자 울트라기어 게이밍모니터 역대급 핫딜 + 일체형 PC SSG 단독특가</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003616</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>LG전자 @SSG.LIVE 1/2(월) 20:00PM</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2022-12-26</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-01-02</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; LG전자 @SSG.LIVE 1/2(월) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>바디프랜드 1/2(월) 9PM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>바디프랜드 A급리퍼 한정수량 90만원대~ &amp; 특별사은품 2종</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003639</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>바디프랜드 @SSG.LIVE 1/2(월) 9PM</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2022-12-26</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2023-01-02</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 바디프랜드 @SSG.LIVE 1/2(월) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>USM 1/3(화) 8PM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>국내 최초 라이브! 바로배송에 200만원 이상 구매시 10만원 상품권 증정</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003662&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>[쓱라이브] USM 1/3(화) 8PM</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2022-12-27</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2023-01-06</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] USM 1/3(화) 8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Jan  9 00:20:43 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,392 +473,392 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>첫구매는 반값다~딜</t>
+          <t>뷰티 쓱세일 이번주 뷰티 최강 혜택!</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>첫구매는 네 개 다 반값 + 무료배송</t>
+          <t>뷰티 ~15% 쿠폰 + ~10% 청구할인</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003710&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003718</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>첫구매는 네 개 다 반값! 반값다딜 (1/5~11)</t>
+          <t>[0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '스마일클럽', '첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '첫구매 전용 프로모션', '반값다~딜 - 50% / 무료배송', '첫구매는 네 개 다 반값!', '※ 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매이력이 없는 고객을 포함합니다.', '반값 귤추운 겨울, 이불 속에서 까먹는 새콤달콤한 별미 (최대 할인금액 5천원)', '반값 떡볶이추운 겨울, 이불 속에서 까먹는 새콤달콤한 별미 (최대 할인금액 5천원)', '반값 과자(파이류)한눈팔면 무한흡입! 폭신폭신 달콤한 파이 과자 (최대 할인금액 3천원)', '반값 과채음료생기를 채워주는 상큼한 과채음료 (최대 할인금액 3천원)', '첫구매는 무료배송!', '첫구매라면 반값으로 구매하고, 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능 - 무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 한번에 받기 - 기간 내 ID당 1회 -', '       쿠폰 사용 기간', '       상품할인쿠폰 : 2023년 1월 5일(목) ~2023년 1월 11일(수)', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 귤 1개, 떡볶이 1개, 과자(파이/케익류) 1개, 과일음료 1개 적용 가능 (ex. 귤 2개 구매시에도 1개에만 적용 가능합니다)', '       ＊첫구매 쿠폰 CAT', '       귤 50% cat (최대 5천원 할인)', '       떡볶이 50% cat (최대 3천원 할인)', '       과자(파이/케익류) 50% cat (최대 3천원 할인)', '       과일음료 50% cat (최대 3천원 할인)', '첫구매 전용 오늘의 상품 보기']</t>
+          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '스마일클럽', '[0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '       뷰티 쿠폰 최대 9장', '       매일 10시 선착순 타임딜', '뷰티 쓱세일 최대 3만원 할인', '백화점 뷰티 최대 15% 상품쿠폰', '상품쿠폰 15% : 3만원 이상 상품 구매시 최대 2만원 할인', '쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 1월 9일(월) 09시 00분 부터 1월 15일(일) 23시 59분 까지', '본 쿠폰은 신세계백화점몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '쿠폰은 9시 부터 발급됩니다', '트렌드 뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '상품쿠폰 15% : 1만원 이상 상품 구매시 최대 1만원 할인', '상품쿠폰 15% : 7만원 이상 상품 구매시 최대 3만원 할인', '본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 및 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '트렌드 뷰티 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기 보러가기 - 자세히 보기', '누구나 최대 3만원 할인 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 2만원 할인', '스마일클럽 회원은 한장 더!', '장바구니 쿠폰 10% : 7만원 이상 구매시 최대 2만원 할인 (SmileClub 전용) (매일 9시 5000장)', '쿠폰 마감 되었습니다.', 'ID 당 발급 수량 : 7% 장바구니 쿠폰 1장 , 10% 장바구니 쿠폰 1장(멤버십회원 전용)', 'SSG 첫 구매 고객이라면\xa0 15% 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 3만원 할인 (첫 구매 전용) (매일 9시 10000장)', '첫구매 쿠폰 발급 대상 : 2022년 1월 8일 이후 SSG.COM 구매이력이 없는 고객', '혜택의 마무리 카드 청구 할인', 'KB카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '신한카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', 'KB카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '현대카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '신한카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '현대카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '카드 발급 후 스마일클럽 정기결제 카드로 들록하시겠어요\xa0', '월 정기결제 카드 등록시에만 해당 카드의 스마일클럽 정기 결제 금액 3,900원 지원/할인 혜택을 받으실 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>설 선물세트 다함께 공동구매 2탄 _ 가성비상품편</t>
+          <t>뷰티 쓱세일 백화점에서 트렌드뷰티까지</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 74%할인 + 목표달성하면 SSG머니 최대 5만원 혜택</t>
+          <t>디올/로레알 외 TOP 24 브랜드</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003656</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003719</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[명절]설 공동구매 2탄_가성비상품편</t>
+          <t>[0109~0115] 뷰티 쓱세일 _ 백화점/트렌드 뷰티 TOP 브랜드</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 2탄_가성비상품편', '스마일클럽', '명절 선물세트 7종 최대 74% 할인 + 공동구매 혜택 최대 5만원 적립', '공구 이벤트 기간 : 1월 5일 ~ 1월 11일', '[CJ제일제당]특별한선택 O-1호 40% 할인 + 최대 8천원 적립!', '[휴럼] 천년침향환 3.7g*30환 53% 할인 + 최대 8천원 적립!', '[올즙] 타트체리 주스 1000ml 2병 74% 할인 + 최대 4천원 적립!', '[일리] 스틱커피 선물세트 20% 할인 + 최대 8천원 적립!', '[신세계푸드] 월넛 + 잉글리쉬파운드 22% 할인 + 최대 5천원 적립!', '사과배한라봉 혼합 선물세트 2호 29% 할인 + 최대 8천원 적립!', '블랙앵거스 LA갈비 선물세트 3kg 25% 할인 + 최대 9천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 백화점/트렌드 뷰티 TOP 브랜드', '스마일클럽', '혜택 끝판왕 트렌드 뷰티 최대 75 할인', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기', '         설화수 설맞이 베스트셀러 자음2종 외 최대 41% 체감가 + 모든 구매고객 윤조 향초 증정', '         미라클토닝 글로우 세럼&amp;토닝 워터패드 최초 방송 라이브 한정 2 STEP KIT 옐로우컵 증정 이벤트']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>신세계백화점 쓱페스타</t>
+          <t>뷰티 쓱세일 매일 오전 10시! 한정수량 타임딜</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10% 쿠폰 + 2023분께 경품 혜택까지!</t>
+          <t>쓱세일 뷰티 추천템</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003546</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003720</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(0102-0108) 신세계백화점 쓱페스타</t>
+          <t>[0109~0115] 뷰티 쓱세일 _ 매일 오전 10시 타임딜 &amp; 특가</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-08</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0108) 신세계백화점 쓱페스타', '스마일클럽', '01. 쓱페스타 10% 쿠폰 바로보기', '03. 신년 맞이 경품 이벤트 바로보기', '01. 쓱페스타 10% 쿠폰', '쿠폰 다운 받기', '쿠폰 마감되었습니다.', "발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다", '03. 2023쓱페스타 구매 이벤트 신세계백화점이 2023명에게 추첨을 통해 새해 맞이 선물을 드립니다!', '경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다', '이벤트 기간 내 경품 응모 후 주문 후 취소/반품하신 고객은 경품 응모 대상에서 제외됩니다', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기합니다', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다', 'DAY1 새해 첫 득템은 SSG.COM에서! 초특가부터 쿠폰까지 하나되어 더 큰 할인 DAY1 바로 가기']</t>
+          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 매일 오전 10시 타임딜 &amp; 특가', '스마일클럽', '[0109~0115] 뷰티 쓱세일 _ 매일 오전 10시 타임딜 &amp; 특가', '한정수량 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023 순금 GOLD WEEK</t>
+          <t>2023 설 스페셜 혜택전</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>새해맞이 순금제품 구매하면 SSG머니 ~4만원</t>
+          <t>단 3일, 최대 3만원 4종 쿠폰 혜택</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003691</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003791</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023 순금 GOLD WEEK</t>
+          <t>2023 설 스페셜 혜택전</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-08</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 순금 GOLD WEEK', '스마일클럽', '구매사은 대상금액은 지정된 구매사은의 실구매금액기준(상품쿠폰/에누리 및 배송비제외) 으로 적용되며 하단 [신청가능내역조회]를 통해 확인가능합니다. ', '이벤트에 응모하시고 결제취소 하셨더라도,\xa0행사 마감 전까지\xa0다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다. ', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우,\xa0이벤트 신청을 완료하셨더라도 이벤트 대상에서 제외됩니다 ', '본 이벤트에 응모하실 경우 개인정보\xa0(회원ID\xa0등)\xa0제공에 동의하신 것으로 간주되며,\xa0제공된 정보는\xa0SSG머니 지급 후 즉시 파기합니다.', "이벤트 참여 후 'MY SSG &gt; 이벤트 참여 현황' 에서 참여여부 확인가능합니다. ", '고순도 999.9% 계묘년 토끼 골드바']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 설 스페셜 혜택전', '스마일클럽', '단 3일간, 명절선물 전용쿠폰', '#1. 명절 종합 선물세트 4종 쿠폰', '#4. 할인에 할인을 더한 카드사 청구할인', '#1. 감사의 마음을 담은 명절 종합 선물세트 4종 쿠폰', '      쿠폰 발급 후 ‘My SSG &gt; 쿠폰 &gt; 보유쿠폰’ 에서 확인 가능합니다.', '      본 쿠폰은 ‘명절’ ‘점포 명절’ 엠블렘이 있는 설 명절 기프트 상품 전용 쿠폰입니다.', '설 선물도 역시! 선물하기로 쓱 - 선물하기 서비스 이용 시 한우/정관장 경품 이벤트!', '#4. 할인에 할인을 더하다 카드사 청구할인']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>설 선물도 역시! 선물하기로</t>
+          <t>첫구매는 반값다~딜</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>쓱에서 선물하면 내 선물도 쓱-</t>
+          <t>첫구매는 네 개 다 반값 + 무료배송</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003710&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
+          <t>첫구매는 네 개 다 반값! 반값다딜 (1/5~11)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '스마일클럽', '첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '첫구매 전용 프로모션', '반값다~딜 - 50% / 무료배송', '첫구매는 네 개 다 반값!', '※ 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매이력이 없는 고객을 포함합니다.', '반값 귤추운 겨울, 이불 속에서 까먹는 새콤달콤한 별미 (최대 할인금액 5천원)', '반값 떡볶이달달매콤, 말랑찰떡한 한국인의 소울푸드 (최대 할인금액 3천원)', '반값 과자(파이류)한눈팔면 무한흡입! 폭신폭신 달콤한 파이 과자 (최대 할인금액 3천원)', '반값 과채음료생기를 채워주는 상큼한 과채음료 (최대 할인금액 3천원)', '첫구매는 무료배송!', '첫구매라면 반값으로 구매하고, 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능 - 무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 한번에 받기 - 기간 내 ID당 1회 -', '       쿠폰 사용 기간', '       상품할인쿠폰 : 2023년 1월 5일(목) ~2023년 1월 11일(수)', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 귤 1개, 떡볶이 1개, 과자(파이/케익류) 1개, 과일음료 1개 적용 가능 (ex. 귤 2개 구매시에도 1개에만 적용 가능합니다)', '       ＊첫구매 쿠폰 CAT', '       귤 50% cat (최대 5천원 할인)', '       떡볶이 50% cat (최대 3천원 할인)', '       과자(파이/케익류) 50% cat (최대 3천원 할인)', '       과일음료 50% cat (최대 3천원 할인)', '첫구매 전용 오늘의 상품 보기']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>설 선물세트 다함께 공동구매 2탄 _ 가성비상품편</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>최대 74%할인 + 목표달성하면 SSG머니 최대 5만원 혜택</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003656</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[명절]설 공동구매 2탄_가성비상품편</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 2탄_가성비상품편', '스마일클럽', '명절 선물세트 7종 최대 74% 할인 + 공동구매 혜택 최대 5만원 적립', '공구 이벤트 기간 : 1월 5일 ~ 1월 11일', '[CJ제일제당]특별한선택 O-1호 40% 할인 + 최대 8천원 적립!', '[휴럼] 천년침향환 3.7g*30환 53% 할인 + 최대 8천원 적립!', '[올즙] 타트체리 주스 1000ml 2병 74% 할인 + 최대 4천원 적립!', '[일리] 스틱커피 선물세트 20% 할인 + 최대 8천원 적립!', '[신세계푸드] 월넛 + 잉글리쉬파운드 22% 할인 + 최대 5천원 적립!', '사과배한라봉 혼합 선물세트 2호 29% 할인 + 최대 8천원 적립!', '블랙앵거스 LA갈비 선물세트 3kg 25% 할인 + 최대 9천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>SSG 브랜드 스포트라이트: 디올</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>NEW미차 리미티드 에디션부터 다양한 특별 혜택까지</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003632</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG 브랜드 스포트라이트 - 디올</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 디올', '스마일클럽', ' 03. 특정 상품 구매 시, 스페셜 사은품 증정 루즈 디올 - 미차 리미티드 에디션 구매 시, 루즈 디올 립스틱 홀더 증정 ※ 상품 주문수량 당 1개 증정 디올 어딕트 립 아이템 포함, 8만원 이상 구매 시, 어딕트 폰 그립 증정 ※ 디올 어딕트 립 아이템 포함 디올 뷰티 전 상품 8만원 이상 구매시 적용 ※ 어딕트 립 글로우, 어딕트 립스틱, 어딕트 립 틴트, 어딕트 립 맥시마이저, 어딕트 립 글로우 오일 제품 포함 ※ 주문번호 당 1개 증정 ']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2022 대한민국 수산대전</t>
+          <t>설 선물도 역시! 선물하기로</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>연말 이벤트전</t>
+          <t>쓱에서 선물하면 내 선물도 쓱-</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
+          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트_</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1월 가입 웰컴 기프트 5천원</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>명절 선물세트 ~15% 2종 할인까지</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'DAY 1월 2일 월요일은 스마일클럽 장보기 최대 10% 적립 DAY', '스마일클럽 기본적립 + 추가적립', '더블 적립 혜택 최대 10%', '*스마일클럽 혜택 선택 회원님이 장보기(쓱배송/새벽배송/트레이더스) 주문 시 자동 적립됩니다.', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '새해맞이 다 모여 더 큰 할인 DAY1 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>지금 꼭 먹어야 할 건강 밥상 특집</t>
+          <t>2022 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>겨울 제철 식품 ~40% 특가</t>
+          <t>연말 이벤트전</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003621</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>건강 밥상 특집</t>
+          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -868,121 +868,454 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 건강 밥상 특집', '스마일클럽', '#최대 40% 할인', '최대 40% 할인 제철 음식 장보기 바로보기', '최대 40% 할인! 제철 수산물', '최대 30% 할인! 제철 채소', '최대 40% 할인! 제철 양곡/견과류', '최대 25% 할인! 제철 과일', 'SSG.COM 푸드마켓 인기상품 할인 최대 20% 할인', '쿠폰 사용 전 꼭 확인하세요(레이어팝업 열기)', '할인 적용 기간 : 2023년 1월 5일(목)~11일(수)', '면역력이 쓱! 스마일클럽 건강식품 최대 15% 쿠폰', '상품쿠폰 15% - 7만원 이상 구매시 최대 1만 5천원 할인(smileClub 전용)', '스마일클럽 15% 쿠폰 받으러 가기', '반가우니까, 네 개 다 반값! 최대 50% 할인 반값다 딜', '만두/떡 동시구매시 10% 에누리 조선호텔 곰탕 20% 할인']</t>
+          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>아베다 1/5(목) 8PM</t>
+          <t>WINTER : SEASON OFF</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NEW 스칼프솔루션 런칭! 인바티/보태니컬/로즈메리 24%↓</t>
+          <t>인기 브랜드 SEASON OFF 최대 80% + 할인쿠폰 혜택</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003617</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003767</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[SSG.LIVE] 1/4(목) 8PM 아베다</t>
+          <t>(0109-15) WINTER : SEASON OFF</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-12-26</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE] 1/4(목) 8PM 아베다', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; (0109-15) WINTER : SEASON OFF', '스마일클럽', '매일 선착순', '장바구니 쿠폰', '장바구니 쿠폰 8% : 5만원 이상 구매시 최대 1만 (매일 오전 9시) (선착순 1만장)', '쿠폰 발급 받기 - 기간 내 ID당 1회 발급', '쿠폰은 09시부터 다운 가능 합니다.', '오늘의 쿠폰은 마감 되었습니다!', '쿠폰 발급기간23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용기간23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰 발급 기간: 23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간: 23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '몽클레어 : 70주년 역사의 대표 명품 패딩 브랜드, 몽클레어 패셔너블 하면서도 뛰어난 품질을 갖춘 아이템들을 최대 30% 할인 혜택으로 만나보세요.', '슈콤마보니 : 여성을 가장 돋보이게 하는 슈즈 브랜드, 슈콤마보니 본사 + 아울렛 겨울 연합전을 통해 최대 80% 할인가로 만나보세요.', '투미 : 손흥민이 선택한 퍼포먼스 럭셔리 브랜드, 투미 다양한 베스트셀러들을 최대 30% 할인으로 만나보세요.', '나이키 : 전세계의 ATHLETE에게 영감과 혁신을 불어넣는 브랜드 나이키, WINTER SALE 최대 44% 할인 혜택을 놓치지 마세요.', '[마시모두띠 여성] 세일 최대 60% 할인!', '♥백화점 단독 물량♥ 아울렛 최대 52%OFF', '[S.I.VILLAGE] 보브/톰보이 外 ★50종 특가★ 패딩/코트/가디건 外 ~45%', '[쥬크.CC콜렉트.듀엘] SSG 브랜드위크! WINTER BEST ITEM LAST CHANCE ~60% OFF', '[주간BEST] 추위 걱정없는 포근한 겨울팬츠&amp;니트 BEST 새해맞이 무료배송', '테니스/골프웨어 추천♥ 일상룩으로도 활용가능한 FW 최대 50% 할인!', '[공식]위크엔드 막스마라 시즌오프 30% + 23SS 윈터 신상', '[마시모두띠 남성] 세일 최대 60% 할인', '겨울세일 최대 70% 할인! BEST 아이템 모음전', '[브룩스브라더스] 22 F/W 시즌오프 베스트 아이템  최대 30%OFF', '[J.LINDEBERG] 새해롭게 준비하는 골프 + 10% 쿠폰', '무료배송+사은품 마지막 특가 시즌오프! 골프/겨울/방한/모자/워머', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '컬럼비아 브랜드 위크 ~60% OFF', '[레투] 남녀공용 테니스/액티브룩 자켓&amp;상하의SET 최대 60% + 추가쿠폰', '편집샵 브랜드별 22FW SEASON OFF ~40%', '해피 뉴 이어, 패밀리 슈즈 제안 + 시크릿 15% 쿠폰', 'FW 신상슈즈 비밀특가+최대20%쿠폰♥', 'MAJE 22FW 시즌오프20%', '[공식][40프로할인]필드 토트 22 CD720 B4RHR', '[토리버치 공식]시즌오프 베스트 최대 40%세일', '[워치스테이션] 아르마니 BEST 시계 최대 61% SALE']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>올리브데올리브 1/5(목) 9PM</t>
+          <t>Molly's SSG 1주년 감사제</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>올리브데올리브 최대 80%할인! 트와이스 나연 착장 숏패딩 99,000원 한정수량</t>
+          <t>매일 선착순 반려동물 15% 쿠폰</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003670</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003788</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>올리브데올리브 @SSG.LIVE 1/5(목) 9PM</t>
+          <t>Molly's SSG 1주년 감사제</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-12-27</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 올리브데올리브 @SSG.LIVE 1/5(목) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>["이벤트/쿠폰 &gt; Molly's SSG 1주년 감사제", '스마일클럽', '매일 선착순 혜택', '최대 15% 쿠폰', '1주년 타임딜', '매일매일 선착순 혜택', '최대 15% 장바구니 쿠폰', '선착순 쿠폰은 매일 10시 오픈됩니다', '      15% 장바구니 쿠폰', '      매일 500명 선착순', '      최대 1만원 할인', '오늘의 쿠폰이 모두 소진되었습니다', '쿠폰은 1/9 10시 오픈됩니다', '      10% 장바구니 쿠폰', '발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '타임딜은 매일 10시 오픈됩니다', '일룸 캐스터네츠 커스텀캣타워 정상가 619,000원 &gt; 할인가 517,100원 구매하러 가기', '힐스 사이언스다이어트 사료 모음전 정상가 148,000원 &gt; 할인가 108,400원 구매하러 가기', '내추럴발란스 강아지 사료 모음 정상가 88,000원 &gt; 할인가 60,400원 구매하러 가기', '포켄스 윔지스 버라이어티팩 정상가 32,000원 &gt; 할인가 24,000원 구매하러 가기', '웨루바 고양이 캔 12개입 정상가 32,400원 &gt; 할인가 18,900원 구매하러 가기', '야미야미 순살닭가슴살 22g x100개 정상가 26,500원 &gt; 할인가 23,500원 구매하러 가기', '붐 펫드라이룸 정상가 1,090,000원 &gt; 할인가 880,000원 구매하러 가기', '타임딜 스케줄', '[쓱배송] 우리와 ANF 반려견 사료 특가모음', '[로그인쿠폰] 하림펫푸드 더리얼 밥이보약 사료 모음', '쓱배송★ 반려견 프리미엄 영양제 견옥고', '[쓱배송] 새벽배송 내추럴발란스 사료 특가', '[쓱배송] 강아지 오리젠,아카나 사료', '점포/네오에서 쓱배송으로! 펫프렌즈 최대 1+1 특가!', '반려동물 겨울나기 펫용품 쓱 할인전', '럭셔리 애견 용품 Boooh 15% mark-down 단독', '[쓱배송] 챠오츄르 SSG 단독상품 출시! 캣 간식 행사 모음', '밥이보약 30%외 몰리스 고양이 사료/간식 행사', '[고양이] 캐츠랑/프로베스트/이즈칸 대포장사료 ~40%_신세계몰 직발송', '[로그인시 최대20%]하림펫푸드 더리얼/밥이보약 고양이사료', '[쓱배송/새벽배송]프로베스트/ANF/이즈칸 사료 행사', '[쓱배송] 고양이 간식 N+1 , 최대 50% 할인행사', '집사들 주목! 뽀떼/그린웨일 스크래쳐/캣타워/캣워크 할인', '[고양이 왕국] 펫페어 고양이 모래/캣타워/스크래쳐1+1/장난감 할인특가', 'SSG단독 ~40% 할인+사은품']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023 스마일클럽 건강 프로젝트_</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023-01-22</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1월 가입 웰컴 기프트 5천원</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>뷰티쓱세일스마일클럽 전용 할인까지</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-01-02</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2023-01-31</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '매달 달라지는 특급 쇼핑 찬스 뷰티 쓱세일 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>지금 꼭 먹어야 할 건강 밥상 특집</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>겨울 제철 식품 ~40% 특가</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003621</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>건강 밥상 특집</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-01-05</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2023-01-11</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 건강 밥상 특집', '스마일클럽', '#최대 40% 할인', '최대 40% 할인 제철 음식 장보기 바로보기', '최대 40% 할인! 제철 수산물', '최대 30% 할인! 제철 채소', '최대 40% 할인! 제철 양곡/견과류', '최대 25% 할인! 제철 과일', 'SSG.COM 푸드마켓 인기상품 할인 최대 20% 할인', '쿠폰 사용 전 꼭 확인하세요(레이어팝업 열기)', '할인 적용 기간 : 2023년 1월 5일(목)~11일(수)', '면역력이 쓱! 스마일클럽 건강식품 최대 15% 쿠폰', '상품쿠폰 15% - 7만원 이상 구매시 최대 1만 5천원 할인(smileClub 전용)', '스마일클럽 15% 쿠폰 받으러 가기', '반가우니까, 네 개 다 반값! 최대 50% 할인 반값다 딜', '만두/떡 동시구매시 10% 에누리 조선호텔 곰탕 20% 할인']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>프리미엄 아울렛 위크 : 2023 신년 &amp; 설맞이 선물 특가전</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003829</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>[0109-0115] 프리미엄 아울렛 위크</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-01-09</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2023-01-15</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [0109-0115] 프리미엄 아울렛 위크', '스마일클럽', '최대 10% 할인 쿠폰 혜택', '할인율은 최초 정산가격 대비 할인율임', '[여성 패션 - 최대 80% 할인] 아울렛 위크 단독 특가, 시즌오프 BEST 外 보러가기', '[언더웨어 - 최대 73% 할인] 노와이어/심리스 &amp; 드로즈 &amp; 겨울 홈웨어 보러가기', '[해외명품 - 최대 70% 할인] 프라다/메종마르지엘라 外 명품 특가 보러가기', '[패션슈즈 - 최대 73% 할인] SHOES TOP 200 ITEMS 최대 10% 쿠폰 보러가기', '[패션잡화 - 최대 73% 할인] BAG&amp;ACC TOP 200 ITEMS 최대 10% 쿠폰 보러가기', '[키즈패션 - 최대 70% 할인] 유아동 BEST 모음 +최대 10% 쿠폰 보러가기', '[남성 패션 - 최대 70% 할인] 브룩스브라더스 外 남성 겨울 상품 입고 보러가기', '[유니섹스 - 최대 80% 할인] 라코스테/ 뉴에라 外 아웃도어 BEST 보러가기', '[스포츠 - 최대 70% 할인] 노스페이스/ 내셔널지오그래픽 外 BEST 보러가기', '[리빙 - 최대 70% 할인] 주방/식탁용품 BEST 모음 +최대10% 쿠폰 보러가기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>쁘띠엘린 1/9(월) 11AM</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>아이스크림 카트 65,002원 선착순 핫딜! 국민 애착인형 젤리캣 최저가!</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003736&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>[쓱라이브] 쁘띠엘린 1/9(월)11AM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-01-02</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2023-01-11</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 쁘띠엘린 1/9(월)11AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>설화수 1/9(월) 7PM</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>설화수 설맞이 베스트셀러 자음2종 외~ 최대 41% 체감가</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003583</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>[뷰티쓱세일] 설화수 @SSG.LIVE 1/9(월) 7PM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2022-12-22</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2023-01-09</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [뷰티쓱세일] 설화수 @SSG.LIVE 1/9(월) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>르크루제 1/9(월) 8PM</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>최대62% 할인! 소르베 2인 셋트 7P 핫딜 10만원대~</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003810&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>르크루제@SSG.LIVE 1/9(월) 20:00PM</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2023-01-04</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2023-01-11</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 르크루제@SSG.LIVE 1/9(월) 20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>[뷰티쓱세일]랑콤 1/10(화) 11AM</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>제니피끄 아이&amp;래쉬 세럼 선런칭! 베스트셀러 15%</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003588</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>[SSG.LIVE]1/10  11AM 랑콤</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-01-04</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2023-01-10</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]1/10  11AM 랑콤', '스마일클럽', '                    SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>[뷰티쓱세일]키엘 1/10(화) 7PM</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEW 장벽 리페어 크림 출시! 5만 5천원대 선착순 핫딜</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003735&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>[쓱라이브] 키엘 1/10(화) 7PM</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2023-01-02</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2023-01-11</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 키엘 1/10(화) 7PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>1월 맘키즈 플러스</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>매월 쏟아지는 맘키즈 특가!</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>2022-09-01</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>2999-12-13</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Jan 12 00:21:16 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '스마일클럽', '[0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '       뷰티 쿠폰 최대 9장', '       매일 10시 선착순 타임딜', '뷰티 쓱세일 최대 3만원 할인', '백화점 뷰티 최대 15% 상품쿠폰', '상품쿠폰 15% : 3만원 이상 상품 구매시 최대 2만원 할인', '쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 1월 9일(월) 09시 00분 부터 1월 15일(일) 23시 59분 까지', '본 쿠폰은 신세계백화점몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '쿠폰은 9시 부터 발급됩니다', '트렌드 뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '상품쿠폰 15% : 1만원 이상 상품 구매시 최대 1만원 할인', '상품쿠폰 15% : 7만원 이상 상품 구매시 최대 3만원 할인', '본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 및 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '트렌드 뷰티 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기 보러가기 - 자세히 보기', '누구나 최대 3만원 할인 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 2만원 할인', '스마일클럽 회원은 한장 더!', '장바구니 쿠폰 10% : 7만원 이상 구매시 최대 2만원 할인 (SmileClub 전용) (매일 9시 5000장)', '쿠폰 마감 되었습니다.', 'ID 당 발급 수량 : 7% 장바구니 쿠폰 1장 , 10% 장바구니 쿠폰 1장(멤버십회원 전용)', 'SSG 첫 구매 고객이라면\xa0 15% 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 3만원 할인 (첫 구매 전용) (매일 9시 10000장)', '첫구매 쿠폰 발급 대상 : 2022년 1월 8일 이후 SSG.COM 구매이력이 없는 고객', '혜택의 마무리 카드 청구 할인', 'KB카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '신한카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', 'KB카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '현대카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '신한카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '현대카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '카드 발급 후 스마일클럽 정기결제 카드로 들록하시겠어요\xa0', '월 정기결제 카드 등록시에만 해당 카드의 스마일클럽 정기 결제 금액 3,900원 지원/할인 혜택을 받으실 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '스마일클럽', '[0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '       뷰티 쿠폰 최대 9장', '       매일 10시 선착순 타임딜', '뷰티 쓱세일 최대 3만원 할인', '백화점 뷰티 최대 15% 상품쿠폰', '상품쿠폰 15% : 3만원 이상 상품 구매시 최대 2만원 할인', '쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 1월 9일(월) 09시 00분 부터 1월 15일(일) 23시 59분 까지', '본 쿠폰은 신세계백화점몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '트렌드 뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '상품쿠폰 15% : 1만원 이상 상품 구매시 최대 1만원 할인', '상품쿠폰 15% : 7만원 이상 상품 구매시 최대 3만원 할인', '본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 및 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '트렌드 뷰티 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기 보러가기 - 자세히 보기', '누구나 최대 3만원 할인 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 2만원 할인', '스마일클럽 회원은 한장 더!', '장바구니 쿠폰 10% : 7만원 이상 구매시 최대 2만원 할인 (SmileClub 전용) (매일 9시 5000장)', '쿠폰은 9시 부터 발급됩니다', '쿠폰 마감 되었습니다.', 'ID 당 발급 수량 : 7% 장바구니 쿠폰 1장 , 10% 장바구니 쿠폰 1장(멤버십회원 전용)', 'SSG 첫 구매 고객이라면\xa0 15% 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 3만원 할인 (첫 구매 전용) (매일 9시 10000장)', '첫구매 쿠폰 발급 대상 : 2022년 1월 8일 이후 SSG.COM 구매이력이 없는 고객', '혜택의 마무리 카드 청구 할인', 'KB카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '신한카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', 'KB카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '현대카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '신한카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '현대카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '카드 발급 후 스마일클럽 정기결제 카드로 들록하시겠어요\xa0', '월 정기결제 카드 등록시에만 해당 카드의 스마일클럽 정기 결제 금액 3,900원 지원/할인 혜택을 받으실 수 있습니다.']</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>디올/로레알 외 TOP 24 브랜드</t>
+          <t>조 말론 런던/에스티로더 외 TOP 브랜드</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -584,229 +584,229 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023 설 스페셜 혜택전</t>
+          <t>쓱배송 days</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>단 3일, 최대 3만원 4종 쿠폰 혜택</t>
+          <t>10% 장보기 쿠폰 + 최대 7%카드 할인까지</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003791</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003851</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023 설 스페셜 혜택전</t>
+          <t>쓱배송 Days</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-13</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 설 스페셜 혜택전', '스마일클럽', '단 3일간, 명절선물 전용쿠폰', '#1. 명절 종합 선물세트 4종 쿠폰', '#4. 할인에 할인을 더한 카드사 청구할인', '#1. 감사의 마음을 담은 명절 종합 선물세트 4종 쿠폰', '      쿠폰 발급 후 ‘My SSG &gt; 쿠폰 &gt; 보유쿠폰’ 에서 확인 가능합니다.', '      본 쿠폰은 ‘명절’ ‘점포 명절’ 엠블렘이 있는 설 명절 기프트 상품 전용 쿠폰입니다.', '설 선물도 역시! 선물하기로 쓱 - 선물하기 서비스 이용 시 한우/정관장 경품 이벤트!', '#4. 할인에 할인을 더하다 카드사 청구할인']</t>
+          <t>['이벤트/쿠폰 &gt; 쓱배송 Days', '스마일클럽', '쓱배송 Days', '쓱배송DAYS', '10% 장보기 쿠폰 &amp; 최대 7% 카드할인까지', '오늘은 장 보는 날 최대 2만원 할인 쿠폰 &amp; 카드할인 바로보기', '최대 40% 할인부터 최대 50만원 혜택까지 설 선물 원하는 시간에 쓱 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장보기 쿠폰', '10% 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1매 (오전 9시 오픈, 선착순 2만명)', '10% 쿠폰 - 8만원 이상 결제시 최대 2만원 할인 ID당 1매 (오전 9시 오픈, 선착순 5천명, smile club 전용)', '스마일클럽 전용 쿠폰 받기', '       쿠폰발급 및 사용 기간', '       23년 1월 12일/13일 양 일간 (당일 발급된 쿠폰은 당일 한정 사용가능)', '       쿠폰 발급 및 사용일', '       2023년 1월 12일 / 13일 양 일간 진행 (진행간 중 ID당 1일 1회 다운가능하며 당일 발급 쿠폰은 해당일 한정 사용 가능)', '       쿠폰 사용조건', '       대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '       쿠폰 발급 대상', '       스마일클럽 전용 2만원 할인 장바구니 쿠폰 : 스마일클럽 멤버십 가입 회원 전용 (두 쿠폰 모두 이메일주소, SNS 등으로 가입된 간편회원은 제외됩니다)', '       쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '결제할때 한 번더 할인받기 오늘의 청구할인 카드혜택', 'KB카드 최대 10%만원 7% 청구할인 자세히 보기', '[SSGPAY 전용] 삼성카드 최대 10만원 5% 청구할인 자세히 보기', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '쓱배송 첫구매 복 많이 받으세요! 새해 특집 1만원 할인+무료배송', '이벤트 보러가기', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품', '금주의 트레이더스 상품쿠폰 + 특가행사 더보기', '설 명절 선물도 원하는 시간에 쓱 최대 40% 할인부터 최대 50만원 혜택까지!', '쓱배송 명절 선물 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>첫구매는 반값다~딜</t>
+          <t>쓱배송 만원 할인</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>첫구매는 네 개 다 반값 + 무료배송</t>
+          <t>쓱배송 장바구니 1만원 할인쿠폰 + 무료배송 쿠폰</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003710&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003796&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>첫구매는 네 개 다 반값! 반값다딜 (1/5~11)</t>
+          <t>2023 첫 장보기 응원! 쓱배송 만원할인</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-18</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '스마일클럽', '첫구매는 네 개 다 반값! 반값다딜 (1/5~11)', '첫구매 전용 프로모션', '반값다~딜 - 50% / 무료배송', '첫구매는 네 개 다 반값!', '※ 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매이력이 없는 고객을 포함합니다.', '반값 귤추운 겨울, 이불 속에서 까먹는 새콤달콤한 별미 (최대 할인금액 5천원)', '반값 떡볶이달달매콤, 말랑찰떡한 한국인의 소울푸드 (최대 할인금액 3천원)', '반값 과자(파이류)한눈팔면 무한흡입! 폭신폭신 달콤한 파이 과자 (최대 할인금액 3천원)', '반값 과채음료생기를 채워주는 상큼한 과채음료 (최대 할인금액 3천원)', '첫구매는 무료배송!', '첫구매라면 반값으로 구매하고, 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능 - 무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 한번에 받기 - 기간 내 ID당 1회 -', '       쿠폰 사용 기간', '       상품할인쿠폰 : 2023년 1월 5일(목) ~2023년 1월 11일(수)', '       무료배송 쿠폰 : 발급일로부터 30일간 사용 가능', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 귤 1개, 떡볶이 1개, 과자(파이/케익류) 1개, 과일음료 1개 적용 가능 (ex. 귤 2개 구매시에도 1개에만 적용 가능합니다)', '       ＊첫구매 쿠폰 CAT', '       귤 50% cat (최대 5천원 할인)', '       떡볶이 50% cat (최대 3천원 할인)', '       과자(파이/케익류) 50% cat (최대 3천원 할인)', '       과일음료 50% cat (최대 3천원 할인)', '첫구매 전용 오늘의 상품 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 첫 장보기 응원! 쓱배송 만원할인', '스마일클럽', '2023 첫 장보기 응원! 쓱배송 만원할인', '2023 첫장보기 응원 쓱배송 만원할인', '(첫구매 전용 EVENT) 장바구니쿠폰 10,000원', 'WELCOME 쓱배송 첫구매 고객님,1년만에 다시 오신 고객님 1만원 바로 할인 받고 무료배송 받으세요 바로보기', '쓱배송 추천탬 쓱배송 첫구매 고객 인기 아이템 추천', '2023년 첫 장보기 혜택 쓱배송 첫구매 고객 1만원 바로 할인', '(첫 구매 전용)장바구니쿠폰 10,000원 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '(첫 구매 전용)무료배송 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', '첫구매 쿠폰 모두 한번에 받기', '       2022년 1월 11일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매이력이 없는 고객 한정', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰: 쓱배송/새벽배송 상품 2만원 이상 구매시 최대 1만원 할인', '       무료배송 쿠폰: 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용 대상', '       쓱배송, 새벽배송', '       쓱배송 새벽배송 상품에 대해 적용 가능 (일부상품 제외)', '       쿠폰 발급 대상', '쓱배송 첫구매 고객 인기 아이템 추천']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>설 선물세트 다함께 공동구매 2탄 _ 가성비상품편</t>
+          <t>명절 장보기</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>최대 74%할인 + 목표달성하면 SSG머니 최대 5만원 혜택</t>
+          <t>명절 장보고 최대 1만원 할인쿠폰 신청하세요</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003656</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003798&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[명절]설 공동구매 2탄_가성비상품편</t>
+          <t>(1/12~18) 명절 장보기</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-18</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [명절]설 공동구매 2탄_가성비상품편', '스마일클럽', '명절 선물세트 7종 최대 74% 할인 + 공동구매 혜택 최대 5만원 적립', '공구 이벤트 기간 : 1월 5일 ~ 1월 11일', '[CJ제일제당]특별한선택 O-1호 40% 할인 + 최대 8천원 적립!', '[휴럼] 천년침향환 3.7g*30환 53% 할인 + 최대 8천원 적립!', '[올즙] 타트체리 주스 1000ml 2병 74% 할인 + 최대 4천원 적립!', '[일리] 스틱커피 선물세트 20% 할인 + 최대 8천원 적립!', '[신세계푸드] 월넛 + 잉글리쉬파운드 22% 할인 + 최대 5천원 적립!', '사과배한라봉 혼합 선물세트 2호 29% 할인 + 최대 8천원 적립!', '블랙앵거스 LA갈비 선물세트 3kg 25% 할인 + 최대 9천원 적립!', '본 이벤트에 대한 세부사항은 당사 사정에 따라 임의로 변경 혹은 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (1/12~18) 명절 장보기', '스마일클럽', '명절 장보고 신청하면 최대 1만원 할인쿠폰 EVENT 바로보기', '온가족이 함께 즐기는 쓱배송 명절 먹거리 바로보기', '명절에 진심인 분은 쓱배송으로 장을 봅니다.', '쓱배송으로 장보면 최대 1만원 할인쿠폰 증정', '1월 12일 부터 1월 18일 까지 쓱배송으로 10만원 이상 구매고객 대상', '쓱배송 상품 전용 10% 할인쿠폰 (선착순 1만명) (1월 25일 이후 순차 지급)', '이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능) * 배송비, 할인액을 제외한 상품 실결제 금액 기준입니다. * 신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.", '      1/25(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용조건', '      이마트/트레이더스 쓱배송/새벽배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '      쿠폰 사용기간', '      쿠폰 사용대상', '      이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '할인쿠폰 신청하기', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능)", '      배송비, 할인액을 제외한 상품 실결제 금액 기준입니다.', '      신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.', '      쿠폰 발급 예정일', '      1월 25일(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용 조건', '      쿠폰 사용 가능 기간', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '온가족이 함께 즐기는 이마트몰 쓱배송 명절 먹거리', '쓱배송 딱지를 확인하세요!', '이마트몰 쓱배송 명절 먹거리 상품 더 보러가기', '명장이라면, 놓치지마세요 카드 청구할인', 'KB국민카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[명절상품] SSG.COM카드 Ed2 10만원 이상 10% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 7만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', '(1/12~18) 명장 장바구니 10% 쿠폰']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 디올</t>
+          <t>설 선물세트 퀵배송</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NEW미차 리미티드 에디션부터 다양한 특별 혜택까지</t>
+          <t>아직 명절 준비 못했다면, 빠르고 편리하게 마음을 선물하세요</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003632</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003880&amp;previewYn=Y&amp;cacheCmd=expire</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 디올</t>
+          <t>23년 설 배송마감/퀵배송 기획전</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 디올', '스마일클럽', ' 03. 특정 상품 구매 시, 스페셜 사은품 증정 루즈 디올 - 미차 리미티드 에디션 구매 시, 루즈 디올 립스틱 홀더 증정 ※ 상품 주문수량 당 1개 증정 디올 어딕트 립 아이템 포함, 8만원 이상 구매 시, 어딕트 폰 그립 증정 ※ 디올 어딕트 립 아이템 포함 디올 뷰티 전 상품 8만원 이상 구매시 적용 ※ 어딕트 립 글로우, 어딕트 립스틱, 어딕트 립 틴트, 어딕트 립 맥시마이저, 어딕트 립 글로우 오일 제품 포함 ※ 주문번호 당 1개 증정 ']</t>
+          <t>['이벤트/쿠폰 &gt; 23년 설 배송마감/퀵배송 기획전', '스마일클럽', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>설 선물도 역시! 선물하기로</t>
+          <t>SSG 브랜드 스포트라이트: 디올</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>쓱에서 선물하면 내 선물도 쓱-</t>
+          <t>NEW미차 리미티드 에디션부터 다양한 특별 혜택까지</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003632</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
+          <t>SSG 브랜드 스포트라이트 - 디올</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 디올', '스마일클럽', ' 03. 특정 상품 구매 시, 스페셜 사은품 증정 루즈 디올 - 미차 리미티드 에디션 구매 시, 루즈 디올 립스틱 홀더 증정 ※ 상품 주문수량 당 1개 증정 디올 어딕트 립 아이템 포함, 8만원 이상 구매 시, 어딕트 폰 그립 증정 ※ 디올 어딕트 립 아이템 포함 디올 뷰티 전 상품 8만원 이상 구매시 적용 ※ 어딕트 립 글로우, 어딕트 립스틱, 어딕트 립 틴트, 어딕트 립 맥시마이저, 어딕트 립 글로우 오일 제품 포함 ※ 주문번호 당 1개 증정 ']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>설 선물도 역시! 선물하기로</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>쓱에서 선물하면 내 선물도 쓱-</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -836,103 +836,103 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2022 대한민국 수산대전</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>연말 이벤트전</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>WINTER : SEASON OFF</t>
+          <t>2023 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>인기 브랜드 SEASON OFF 최대 80% + 할인쿠폰 혜택</t>
+          <t>설 특별전</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003767</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(0109-15) WINTER : SEASON OFF</t>
+          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0109-15) WINTER : SEASON OFF', '스마일클럽', '매일 선착순', '장바구니 쿠폰', '장바구니 쿠폰 8% : 5만원 이상 구매시 최대 1만 (매일 오전 9시) (선착순 1만장)', '쿠폰 발급 받기 - 기간 내 ID당 1회 발급', '쿠폰은 09시부터 다운 가능 합니다.', '오늘의 쿠폰은 마감 되었습니다!', '쿠폰 발급기간23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용기간23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰 발급 기간: 23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간: 23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '몽클레어 : 70주년 역사의 대표 명품 패딩 브랜드, 몽클레어 패셔너블 하면서도 뛰어난 품질을 갖춘 아이템들을 최대 30% 할인 혜택으로 만나보세요.', '슈콤마보니 : 여성을 가장 돋보이게 하는 슈즈 브랜드, 슈콤마보니 본사 + 아울렛 겨울 연합전을 통해 최대 80% 할인가로 만나보세요.', '투미 : 손흥민이 선택한 퍼포먼스 럭셔리 브랜드, 투미 다양한 베스트셀러들을 최대 30% 할인으로 만나보세요.', '나이키 : 전세계의 ATHLETE에게 영감과 혁신을 불어넣는 브랜드 나이키, WINTER SALE 최대 44% 할인 혜택을 놓치지 마세요.', '[마시모두띠 여성] 세일 최대 60% 할인!', '♥백화점 단독 물량♥ 아울렛 최대 52%OFF', '[S.I.VILLAGE] 보브/톰보이 外 ★50종 특가★ 패딩/코트/가디건 外 ~45%', '[쥬크.CC콜렉트.듀엘] SSG 브랜드위크! WINTER BEST ITEM LAST CHANCE ~60% OFF', '[주간BEST] 추위 걱정없는 포근한 겨울팬츠&amp;니트 BEST 새해맞이 무료배송', '테니스/골프웨어 추천♥ 일상룩으로도 활용가능한 FW 최대 50% 할인!', '[공식]위크엔드 막스마라 시즌오프 30% + 23SS 윈터 신상', '[마시모두띠 남성] 세일 최대 60% 할인', '겨울세일 최대 70% 할인! BEST 아이템 모음전', '[브룩스브라더스] 22 F/W 시즌오프 베스트 아이템  최대 30%OFF', '[J.LINDEBERG] 새해롭게 준비하는 골프 + 10% 쿠폰', '무료배송+사은품 마지막 특가 시즌오프! 골프/겨울/방한/모자/워머', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '컬럼비아 브랜드 위크 ~60% OFF', '[레투] 남녀공용 테니스/액티브룩 자켓&amp;상하의SET 최대 60% + 추가쿠폰', '편집샵 브랜드별 22FW SEASON OFF ~40%', '해피 뉴 이어, 패밀리 슈즈 제안 + 시크릿 15% 쿠폰', 'FW 신상슈즈 비밀특가+최대20%쿠폰♥', 'MAJE 22FW 시즌오프20%', '[공식][40프로할인]필드 토트 22 CD720 B4RHR', '[토리버치 공식]시즌오프 베스트 최대 40%세일', '[워치스테이션] 아르마니 BEST 시계 최대 61% SALE']</t>
+          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Molly's SSG 1주년 감사제</t>
+          <t>WINTER : SEASON OFF</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>매일 선착순 반려동물 15% 쿠폰</t>
+          <t>인기 브랜드 SEASON OFF 최대 80% + 할인쿠폰 혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003788</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003767</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Molly's SSG 1주년 감사제</t>
+          <t>(0109-15) WINTER : SEASON OFF</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -947,118 +947,118 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; Molly's SSG 1주년 감사제", '스마일클럽', '매일 선착순 혜택', '최대 15% 쿠폰', '1주년 타임딜', '매일매일 선착순 혜택', '최대 15% 장바구니 쿠폰', '선착순 쿠폰은 매일 10시 오픈됩니다', '      15% 장바구니 쿠폰', '      매일 500명 선착순', '      최대 1만원 할인', '오늘의 쿠폰이 모두 소진되었습니다', '쿠폰은 1/9 10시 오픈됩니다', '      10% 장바구니 쿠폰', '발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '타임딜은 매일 10시 오픈됩니다', '일룸 캐스터네츠 커스텀캣타워 정상가 619,000원 &gt; 할인가 517,100원 구매하러 가기', '힐스 사이언스다이어트 사료 모음전 정상가 148,000원 &gt; 할인가 108,400원 구매하러 가기', '내추럴발란스 강아지 사료 모음 정상가 88,000원 &gt; 할인가 60,400원 구매하러 가기', '포켄스 윔지스 버라이어티팩 정상가 32,000원 &gt; 할인가 24,000원 구매하러 가기', '웨루바 고양이 캔 12개입 정상가 32,400원 &gt; 할인가 18,900원 구매하러 가기', '야미야미 순살닭가슴살 22g x100개 정상가 26,500원 &gt; 할인가 23,500원 구매하러 가기', '붐 펫드라이룸 정상가 1,090,000원 &gt; 할인가 880,000원 구매하러 가기', '타임딜 스케줄', '[쓱배송] 우리와 ANF 반려견 사료 특가모음', '[로그인쿠폰] 하림펫푸드 더리얼 밥이보약 사료 모음', '쓱배송★ 반려견 프리미엄 영양제 견옥고', '[쓱배송] 새벽배송 내추럴발란스 사료 특가', '[쓱배송] 강아지 오리젠,아카나 사료', '점포/네오에서 쓱배송으로! 펫프렌즈 최대 1+1 특가!', '반려동물 겨울나기 펫용품 쓱 할인전', '럭셔리 애견 용품 Boooh 15% mark-down 단독', '[쓱배송] 챠오츄르 SSG 단독상품 출시! 캣 간식 행사 모음', '밥이보약 30%외 몰리스 고양이 사료/간식 행사', '[고양이] 캐츠랑/프로베스트/이즈칸 대포장사료 ~40%_신세계몰 직발송', '[로그인시 최대20%]하림펫푸드 더리얼/밥이보약 고양이사료', '[쓱배송/새벽배송]프로베스트/ANF/이즈칸 사료 행사', '[쓱배송] 고양이 간식 N+1 , 최대 50% 할인행사', '집사들 주목! 뽀떼/그린웨일 스크래쳐/캣타워/캣워크 할인', '[고양이 왕국] 펫페어 고양이 모래/캣타워/스크래쳐1+1/장난감 할인특가', 'SSG단독 ~40% 할인+사은품']</t>
+          <t>['이벤트/쿠폰 &gt; (0109-15) WINTER : SEASON OFF', '스마일클럽', '매일 선착순', '장바구니 쿠폰', '장바구니 쿠폰 8% : 5만원 이상 구매시 최대 1만 (매일 오전 9시) (선착순 1만장)', '쿠폰 발급 받기 - 기간 내 ID당 1회 발급', '쿠폰은 09시부터 다운 가능 합니다.', '오늘의 쿠폰은 마감 되었습니다!', '쿠폰 발급기간23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용기간23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰 발급 기간: 23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간: 23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '몽클레어 : 70주년 역사의 대표 명품 패딩 브랜드, 몽클레어 패셔너블 하면서도 뛰어난 품질을 갖춘 아이템들을 최대 30% 할인 혜택으로 만나보세요.', '슈콤마보니 : 여성을 가장 돋보이게 하는 슈즈 브랜드, 슈콤마보니 본사 + 아울렛 겨울 연합전을 통해 최대 80% 할인가로 만나보세요.', '투미 : 손흥민이 선택한 퍼포먼스 럭셔리 브랜드, 투미 다양한 베스트셀러들을 최대 30% 할인으로 만나보세요.', '나이키 : 전세계의 ATHLETE에게 영감과 혁신을 불어넣는 브랜드 나이키, WINTER SALE 최대 44% 할인 혜택을 놓치지 마세요.', '[마시모두띠 여성] 세일 최대 60% 할인!', '[빈폴레이디스]♥백화점 단독 물량♥ 아울렛 최대 52%OFF', '[S.I.VILLAGE] 보브/톰보이 外 ★50종 특가★ 패딩/코트/가디건 外 ~45%', '[쥬크.CC콜렉트.듀엘] SSG 브랜드위크! WINTER BEST ITEM LAST CHANCE ~60% OFF', '[주간BEST] 추위 걱정없는 포근한 겨울팬츠&amp;니트 BEST 새해맞이 무료배송', '테니스/골프웨어 추천♥ 일상룩으로도 활용가능한 FW 최대 50% 할인!', '[공식]위크엔드 막스마라 시즌오프 30% + 23SS 윈터 신상', '[마시모두띠 남성] 세일 최대 60% 할인', '겨울세일 최대 70% 할인! BEST 아이템 모음전', '[브룩스브라더스] 22 F/W 시즌오프 베스트 아이템  최대 30%OFF', '[J.LINDEBERG] 새해롭게 준비하는 골프 + 10% 쿠폰', '무료배송+사은품 마지막 특가 시즌오프! 골프/겨울/방한/모자/워머', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '컬럼비아 브랜드 위크 ~60% OFF', '[레투] 남녀공용 테니스/액티브룩 자켓&amp;상하의SET 최대 60% + 추가쿠폰', '편집샵 브랜드별 22FW SEASON OFF ~40%', '해피 뉴 이어, 패밀리 슈즈 제안 + 시크릿 15% 쿠폰', 'FW 신상슈즈 비밀특가+최대20%쿠폰♥', 'MAJE 22FW 시즌오프20%', '[공식][40프로할인]필드 토트 22 CD720 B4RHR', '[토리버치 공식]시즌오프 베스트 최대 40%세일', '[워치스테이션] 아르마니 BEST 시계 최대 61% SALE']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+          <t>Molly's SSG 1주년 감사제</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+          <t>매일 선착순 반려동물 15% 쿠폰</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003788</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트_</t>
+          <t>Molly's SSG 1주년 감사제</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+          <t>["이벤트/쿠폰 &gt; Molly's SSG 1주년 감사제", '스마일클럽', '매일 선착순 혜택', '최대 15% 쿠폰', '1주년 타임딜', '매일매일 선착순 혜택', '최대 15% 장바구니 쿠폰', '선착순 쿠폰은 매일 10시 오픈됩니다', '      15% 장바구니 쿠폰', '      매일 500명 선착순', '      최대 1만원 할인', '오늘의 쿠폰이 모두 소진되었습니다', '쿠폰은 1/9 10시 오픈됩니다', '      10% 장바구니 쿠폰', '타임딜은 매일 10시 오픈됩니다', '일룸 캐스터네츠 커스텀캣타워 정상가 619,000원 &gt; 할인가 517,100원 구매하러 가기', '힐스 사이언스다이어트 사료 모음전 정상가 148,000원 &gt; 할인가 108,400원 구매하러 가기', '내추럴발란스 강아지 사료 모음 정상가 88,000원 &gt; 할인가 60,400원 구매하러 가기', '포켄스 윔지스 버라이어티팩 정상가 32,000원 &gt; 할인가 24,000원 구매하러 가기', '웨루바 고양이 캔 12개입 정상가 32,400원 &gt; 할인가 18,900원 구매하러 가기', '야미야미 순살닭가슴살 22g x100개 정상가 26,500원 &gt; 할인가 23,500원 구매하러 가기', '붐펫 펫드라이룸 정상가 1,090,000원 &gt; 할인가 615,000원 구매하러 가기', '타임딜 스케줄', '[쓱배송] 우리와 ANF 반려견 사료 특가모음', '[로그인쿠폰] 하림펫푸드 더리얼 밥이보약 사료 모음', '쓱배송★ 반려견 프리미엄 영양제 견옥고', '[쓱배송] 새벽배송 내추럴발란스 사료 특가', '[쓱배송] 강아지 오리젠,아카나 사료', '점포/네오에서 쓱배송으로! 펫프렌즈 1+1 특가! (일부품목제외)', '반려동물 겨울나기 펫용품 쓱 할인전', '럭셔리 애견 용품 Boooh 15% mark-down 단독', '[쓱배송] 챠오츄르 SSG 단독상품 출시! 캣 간식 행사 모음', '밥이보약 30%외 몰리스 고양이 사료/간식 행사', '[고양이] 캐츠랑/프로베스트/이즈칸 대포장사료 ~40%_신세계몰 직발송', '[로그인시 최대20%]하림펫푸드 더리얼/밥이보약 고양이사료', '[쓱배송] 고양이 인기 캔/간식 N+1 /한정수량', '집사들 주목! 뽀떼/그린웨일 스크래쳐/캣타워/캣워크 할인', '[고양이 왕국] 펫페어 고양이 모래/캣타워/스크래쳐1+1/장난감 할인특가', 'SSG단독 ~40% 할인+사은품']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1월 가입 웰컴 기프트 5천원</t>
+          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>뷰티쓱세일스마일클럽 전용 할인까지</t>
+          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>2023 스마일클럽 건강 프로젝트_</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '매달 달라지는 특급 쇼핑 찬스 뷰티 쓱세일 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>지금 꼭 먹어야 할 건강 밥상 특집</t>
+          <t>1월 가입 웰컴 기프트 5천원</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>겨울 제철 식품 ~40% 특가</t>
+          <t>뷰티쓱세일스마일클럽 전용 할인까지</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003621</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>건강 밥상 특집</t>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 건강 밥상 특집', '스마일클럽', '#최대 40% 할인', '최대 40% 할인 제철 음식 장보기 바로보기', '최대 40% 할인! 제철 수산물', '최대 30% 할인! 제철 채소', '최대 40% 할인! 제철 양곡/견과류', '최대 25% 할인! 제철 과일', 'SSG.COM 푸드마켓 인기상품 할인 최대 20% 할인', '쿠폰 사용 전 꼭 확인하세요(레이어팝업 열기)', '할인 적용 기간 : 2023년 1월 5일(목)~11일(수)', '면역력이 쓱! 스마일클럽 건강식품 최대 15% 쿠폰', '상품쿠폰 15% - 7만원 이상 구매시 최대 1만 5천원 할인(smileClub 전용)', '스마일클럽 15% 쿠폰 받으러 가기', '반가우니까, 네 개 다 반값! 최대 50% 할인 반값다 딜', '만두/떡 동시구매시 10% 에누리 조선호텔 곰탕 20% 할인']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '매달 달라지는 특급 쇼핑 찬스 뷰티 쓱세일 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
@@ -1102,220 +1102,183 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>쁘띠엘린 1/9(월) 11AM</t>
+          <t>클라랑스 1/12(목) 11AM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>아이스크림 카트 65,002원 선착순 핫딜! 국민 애착인형 젤리캣 최저가!</t>
+          <t>더블세럼 75ml 역대급 구성 핫딜 &amp; 립오일 1+1혜택까지</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003736&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003530</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[쓱라이브] 쁘띠엘린 1/9(월)11AM</t>
+          <t>[뷰티쓱세일] 클라랑스 @SSG.LIVE 1/12(목) 11:00AM</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2022-12-20</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 쁘띠엘린 1/9(월)11AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [뷰티쓱세일] 클라랑스 @SSG.LIVE 1/12(목) 11:00AM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>설화수 1/9(월) 7PM</t>
+          <t>[뷰티쓱세일] 오휘 1/12(목) 7PM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>설화수 설맞이 베스트셀러 자음2종 외~ 최대 41% 체감가</t>
+          <t>최대 15,000원 적립+백화점 상품권 증정 혜택</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003583</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003879</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[뷰티쓱세일] 설화수 @SSG.LIVE 1/9(월) 7PM</t>
+          <t>[SSG.LIVE]1/12(목) 7PM 오휘</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2022-12-22</t>
+          <t>2023-01-10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [뷰티쓱세일] 설화수 @SSG.LIVE 1/9(월) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]1/12(목) 7PM 오휘', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>르크루제 1/9(월) 8PM</t>
+          <t>에스티로더 1/13(금) 11AM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>최대62% 할인! 소르베 2인 셋트 7P 핫딜 10만원대~</t>
+          <t>에스티로더 설 특집! 갈색병 세럼 50ml 구매 시, 45ml 추가 증정</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003810&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003584</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>르크루제@SSG.LIVE 1/9(월) 20:00PM</t>
+          <t>[뷰티쓱세일] 에스티로더 @SSG.LIVE 1/13(금) 11AM</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2022-12-22</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-13</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 르크루제@SSG.LIVE 1/9(월) 20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [뷰티쓱세일] 에스티로더 @SSG.LIVE 1/13(금) 11AM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>[뷰티쓱세일]랑콤 1/10(화) 11AM</t>
+          <t>신세계 No. 1 럭스 뷰티 대전</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>제니피끄 아이&amp;래쉬 세럼 선런칭! 베스트셀러 15%</t>
+          <t>신세계상품권 증정 및 SSG머니 즉시할인 혜택</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003588</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003448&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]1/10  11AM 랑콤</t>
+          <t>[1/9-1/15] 로레알 럭셔리 뷰티 쓱세일</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-01-09</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2023-01-10</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]1/10  11AM 랑콤', '스마일클럽', '                    SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [1/9-1/15] 로레알 럭셔리 뷰티 쓱세일', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>[뷰티쓱세일]키엘 1/10(화) 7PM</t>
+          <t>1월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NEW 장벽 리페어 크림 출시! 5만 5천원대 선착순 핫딜</t>
+          <t>매월 쏟아지는 맘키즈 특가!</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003735&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[쓱라이브] 키엘 1/10(화) 7PM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 키엘 1/10(화) 7PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>1월 맘키즈 플러스</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>매월 쏟아지는 맘키즈 특가!</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Jan 16 00:20:36 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,133 +473,133 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>뷰티 쓱세일 이번주 뷰티 최강 혜택!</t>
+          <t>쓱배송 만원 할인</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>뷰티 ~15% 쿠폰 + ~10% 청구할인</t>
+          <t>쓱배송 장바구니 1만원 할인쿠폰 + 무료배송 쿠폰</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003718</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003796&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택</t>
+          <t>2023 첫 장보기 응원! 쓱배송 만원할인</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-18</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '스마일클럽', '[0109~0115] 뷰티 쓱세일 _ 쿠폰 최대 9장 혜택', '       뷰티 쿠폰 최대 9장', '       매일 10시 선착순 타임딜', '뷰티 쓱세일 최대 3만원 할인', '백화점 뷰티 최대 15% 상품쿠폰', '상품쿠폰 15% : 3만원 이상 상품 구매시 최대 2만원 할인', '쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 1월 9일(월) 09시 00분 부터 1월 15일(일) 23시 59분 까지', '본 쿠폰은 신세계백화점몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '트렌드 뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '상품쿠폰 15% : 1만원 이상 상품 구매시 최대 1만원 할인', '상품쿠폰 15% : 7만원 이상 상품 구매시 최대 3만원 할인', '본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 및 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '트렌드 뷰티 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기 보러가기 - 자세히 보기', '누구나 최대 3만원 할인 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 2만원 할인', '스마일클럽 회원은 한장 더!', '장바구니 쿠폰 10% : 7만원 이상 구매시 최대 2만원 할인 (SmileClub 전용) (매일 9시 5000장)', '쿠폰은 9시 부터 발급됩니다', '쿠폰 마감 되었습니다.', 'ID 당 발급 수량 : 7% 장바구니 쿠폰 1장 , 10% 장바구니 쿠폰 1장(멤버십회원 전용)', 'SSG 첫 구매 고객이라면\xa0 15% 장바구니 쿠폰', '장바구니 쿠폰 7% : 7만원 이상 구매시 최대 3만원 할인 (첫 구매 전용) (매일 9시 10000장)', '첫구매 쿠폰 발급 대상 : 2022년 1월 8일 이후 SSG.COM 구매이력이 없는 고객', '혜택의 마무리 카드 청구 할인', 'KB카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '신한카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '삼성카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', 'KB카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '현대카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '신한카드 [SSGPAY전용] [뷰티쓱세일] : 7만원이상 10% 청구할인 (일 5만원 한) 자세히 보기', '현대카드 [SSGPAY전용] : 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '카드 발급 후 스마일클럽 정기결제 카드로 들록하시겠어요\xa0', '월 정기결제 카드 등록시에만 해당 카드의 스마일클럽 정기 결제 금액 3,900원 지원/할인 혜택을 받으실 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 첫 장보기 응원! 쓱배송 만원할인', '스마일클럽', '2023 첫 장보기 응원! 쓱배송 만원할인', '2023 첫장보기 응원 쓱배송 만원할인', '(첫구매 전용 EVENT) 장바구니쿠폰 10,000원', 'WELCOME 쓱배송 첫구매 고객님,1년만에 다시 오신 고객님 1만원 바로 할인 받고 무료배송 받으세요 바로보기', '쓱배송 추천탬 쓱배송 첫구매 고객 인기 아이템 추천', '2023년 첫 장보기 혜택 쓱배송 첫구매 고객 1만원 바로 할인', '(첫 구매 전용)장바구니쿠폰 10,000원 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '(첫 구매 전용)무료배송 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', '첫구매 쿠폰 모두 한번에 받기', '       2022년 1월 11일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매이력이 없는 고객 한정', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰: 쓱배송/새벽배송 상품 2만원 이상 구매시 최대 1만원 할인', '       무료배송 쿠폰: 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용 대상', '       쓱배송, 새벽배송', '       쓱배송 새벽배송 상품에 대해 적용 가능 (일부상품 제외)', '       쿠폰 발급 대상', '쓱배송 첫구매 고객 인기 아이템 추천']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>뷰티 쓱세일 백화점에서 트렌드뷰티까지</t>
+          <t>2023 설 스페셜 혜택전</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>조 말론 런던/에스티로더 외 TOP 브랜드</t>
+          <t>단 2일간, 장바구니 10% 쿠폰 최대 10만원</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003719</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003651</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[0109~0115] 뷰티 쓱세일 _ 백화점/트렌드 뷰티 TOP 브랜드</t>
+          <t>[1/16-17] 2023 설 스페셜 혜택전</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-17</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 백화점/트렌드 뷰티 TOP 브랜드', '스마일클럽', '혜택 끝판왕 트렌드 뷰티 최대 75 할인', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기', '         설화수 설맞이 베스트셀러 자음2종 외 최대 41% 체감가 + 모든 구매고객 윤조 향초 증정', '         미라클토닝 글로우 세럼&amp;토닝 워터패드 최초 방송 라이브 한정 2 STEP KIT 옐로우컵 증정 이벤트']</t>
+          <t>['이벤트/쿠폰 &gt; [1/16-17] 2023 설 스페셜 혜택전', '스마일클럽', '10% 장바구니 쿠폰받기', '      장바구니 쿠폰 10% 쿠폰 (점포명절, 명절)', '      5만원 이상 구매 시 최대 10만원 할인', '쿠폰 발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '[명절] [점포 명절] 엠블렘이 있는 설 명절 기프트 상품 전용 쿠폰입니다.', '★쇼핑백 증정★ [폴로 랄프로렌]이태리산 울 100% 시그니처 멀티로고 폴로 머플러 3종', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가', '[1월18일 오전10시까지 주문시 명절전배송][수산대전20%][해신수산] 완도 활전복 1kg 外 선물세트 모음전', '베이커리 선물 모음전 (무료배송)', '★ 센트룸 할인 행사 ★', '[쓱배송]CJ 한뿌리 홍삼대보 24입 외 특가행사', '[빈폴멘] 22FW 30% 시즌오프! 실시간 BEST 추천', '신년 주목해야할 브랜드 마리끌레르♥ 프랜치 스타일 베스트 아이템 +추가 쿠폰', '해피 뉴 이어, 패밀리 슈즈 제안 + 시크릿 15% 쿠폰', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', 'FW 남여 의류/용품 최대 40% OFF', '블랙야크/디스커버리 外 인기브랜드 다운/패딩 ~70% OFF', '[나이키코리아공식] 남여 인기 신발 모음 ~45%', '설맞이 설레는 고양이 모래/캣타워/스크래쳐 용품 할인전', '[Boooh] 럭셔리 애견 용품 하네스 모음 (단독 20%)']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>뷰티 쓱세일 매일 오전 10시! 한정수량 타임딜</t>
+          <t>명절 장보기</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>쓱세일 뷰티 추천템</t>
+          <t>명절 장보고 최대 1만원 할인쿠폰 신청하세요</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003720</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003798&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[0109~0115] 뷰티 쓱세일 _ 매일 오전 10시 타임딜 &amp; 특가</t>
+          <t>(1/12~18) 명절 장보기</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-18</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0109~0115] 뷰티 쓱세일 _ 매일 오전 10시 타임딜 &amp; 특가', '스마일클럽', '[0109~0115] 뷰티 쓱세일 _ 매일 오전 10시 타임딜 &amp; 특가', '한정수량 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '뷰티 쓱세일 트렌드 뷰티 쿠폰 참여 협력사 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; (1/12~18) 명절 장보기', '스마일클럽', '명절 장보고 신청하면 최대 1만원 할인쿠폰 EVENT 바로보기', '온가족이 함께 즐기는 쓱배송 명절 먹거리 바로보기', '명절에 진심인 분은 쓱배송으로 장을 봅니다.', '쓱배송으로 장보면 최대 1만원 할인쿠폰 증정', '1월 12일 부터 1월 18일 까지 쓱배송으로 10만원 이상 구매고객 대상', '쓱배송 상품 전용 10% 할인쿠폰 (선착순 1만명) (1월 25일 이후 순차 지급)', '이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능) * 배송비, 할인액을 제외한 상품 실결제 금액 기준입니다. * 신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.", '      1/25(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용조건', '      이마트/트레이더스 쓱배송/새벽배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '      쿠폰 사용기간', '      쿠폰 사용대상', '      이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '할인쿠폰 신청하기', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능)", '      배송비, 할인액을 제외한 상품 실결제 금액 기준입니다.', '      신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.', '      쿠폰 발급 예정일', '      1월 25일(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용 조건', '      쿠폰 사용 가능 기간', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '온가족이 함께 즐기는 이마트몰 쓱배송 명절 먹거리', '쓱배송 딱지를 확인하세요!', '이마트몰 쓱배송 명절 먹거리 상품 더 보러가기', '명장이라면, 놓치지마세요 카드 청구할인', 'KB국민카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[명절상품] SSG.COM카드 Ed2 10만원 이상 10% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 7만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', '(1/12~18) 명장 장바구니 10% 쿠폰']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>쓱배송 days</t>
+          <t>설 선물세트 퀵배송</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10% 장보기 쿠폰 + 최대 7%카드 할인까지</t>
+          <t>아직 명절 준비 못했다면, 빠르고 편리하게 마음을 선물하세요</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003851</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003880&amp;previewYn=Y&amp;cacheCmd=expire</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>쓱배송 Days</t>
+          <t>23년 설 배송마감/퀵배송 기획전</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -609,678 +609,530 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-13</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 쓱배송 Days', '스마일클럽', '쓱배송 Days', '쓱배송DAYS', '10% 장보기 쿠폰 &amp; 최대 7% 카드할인까지', '오늘은 장 보는 날 최대 2만원 할인 쿠폰 &amp; 카드할인 바로보기', '최대 40% 할인부터 최대 50만원 혜택까지 설 선물 원하는 시간에 쓱 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장보기 쿠폰', '10% 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1매 (오전 9시 오픈, 선착순 2만명)', '10% 쿠폰 - 8만원 이상 결제시 최대 2만원 할인 ID당 1매 (오전 9시 오픈, 선착순 5천명, smile club 전용)', '스마일클럽 전용 쿠폰 받기', '       쿠폰발급 및 사용 기간', '       23년 1월 12일/13일 양 일간 (당일 발급된 쿠폰은 당일 한정 사용가능)', '       쿠폰 발급 및 사용일', '       2023년 1월 12일 / 13일 양 일간 진행 (진행간 중 ID당 1일 1회 다운가능하며 당일 발급 쿠폰은 해당일 한정 사용 가능)', '       쿠폰 사용조건', '       대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '       쿠폰 발급 대상', '       스마일클럽 전용 2만원 할인 장바구니 쿠폰 : 스마일클럽 멤버십 가입 회원 전용 (두 쿠폰 모두 이메일주소, SNS 등으로 가입된 간편회원은 제외됩니다)', '       쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '결제할때 한 번더 할인받기 오늘의 청구할인 카드혜택', 'KB카드 최대 10%만원 7% 청구할인 자세히 보기', '[SSGPAY 전용] 삼성카드 최대 10만원 5% 청구할인 자세히 보기', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '쓱배송 첫구매 복 많이 받으세요! 새해 특집 1만원 할인+무료배송', '이벤트 보러가기', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품', '금주의 트레이더스 상품쿠폰 + 특가행사 더보기', '설 명절 선물도 원하는 시간에 쓱 최대 40% 할인부터 최대 50만원 혜택까지!', '쓱배송 명절 선물 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 23년 설 배송마감/퀵배송 기획전', '스마일클럽', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>쓱배송 만원 할인</t>
+          <t>브랜드 스포트라이트 X 트라이온: JJ지고트</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>쓱배송 장바구니 1만원 할인쿠폰 + 무료배송 쿠폰</t>
+          <t>SSG 단독 최대 80% 클리어런스 세일</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003796&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003845</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023 첫 장보기 응원! 쓱배송 만원할인</t>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-01-18</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 첫 장보기 응원! 쓱배송 만원할인', '스마일클럽', '2023 첫 장보기 응원! 쓱배송 만원할인', '2023 첫장보기 응원 쓱배송 만원할인', '(첫구매 전용 EVENT) 장바구니쿠폰 10,000원', 'WELCOME 쓱배송 첫구매 고객님,1년만에 다시 오신 고객님 1만원 바로 할인 받고 무료배송 받으세요 바로보기', '쓱배송 추천탬 쓱배송 첫구매 고객 인기 아이템 추천', '2023년 첫 장보기 혜택 쓱배송 첫구매 고객 1만원 바로 할인', '(첫 구매 전용)장바구니쿠폰 10,000원 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '(첫 구매 전용)무료배송 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', '첫구매 쿠폰 모두 한번에 받기', '       2022년 1월 11일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매이력이 없는 고객 한정', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰: 쓱배송/새벽배송 상품 2만원 이상 구매시 최대 1만원 할인', '       무료배송 쿠폰: 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용 대상', '       쓱배송, 새벽배송', '       쓱배송 새벽배송 상품에 대해 적용 가능 (일부상품 제외)', '       쿠폰 발급 대상', '쓱배송 첫구매 고객 인기 아이템 추천']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트', '스마일클럽', '1 WINTER CLEARANCE 최대 80% OFF', '2 23년 봄 신상 최대 50% OFF', 'SSG 단독! 브랜드 스포트라이트 기간에만 진행하는 특별 할인']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>명절 장보기</t>
+          <t>설 선물도 역시! 선물하기로</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>명절 장보고 최대 1만원 할인쿠폰 신청하세요</t>
+          <t>쓱에서 선물하면 내 선물도 쓱-</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003798&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(1/12~18) 명절 장보기</t>
+          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-18</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/12~18) 명절 장보기', '스마일클럽', '명절 장보고 신청하면 최대 1만원 할인쿠폰 EVENT 바로보기', '온가족이 함께 즐기는 쓱배송 명절 먹거리 바로보기', '명절에 진심인 분은 쓱배송으로 장을 봅니다.', '쓱배송으로 장보면 최대 1만원 할인쿠폰 증정', '1월 12일 부터 1월 18일 까지 쓱배송으로 10만원 이상 구매고객 대상', '쓱배송 상품 전용 10% 할인쿠폰 (선착순 1만명) (1월 25일 이후 순차 지급)', '이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능) * 배송비, 할인액을 제외한 상품 실결제 금액 기준입니다. * 신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.", '      1/25(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용조건', '      이마트/트레이더스 쓱배송/새벽배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '      쿠폰 사용기간', '      쿠폰 사용대상', '      이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '할인쿠폰 신청하기', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능)", '      배송비, 할인액을 제외한 상품 실결제 금액 기준입니다.', '      신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.', '      쿠폰 발급 예정일', '      1월 25일(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용 조건', '      쿠폰 사용 가능 기간', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '온가족이 함께 즐기는 이마트몰 쓱배송 명절 먹거리', '쓱배송 딱지를 확인하세요!', '이마트몰 쓱배송 명절 먹거리 상품 더 보러가기', '명장이라면, 놓치지마세요 카드 청구할인', 'KB국민카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[명절상품] SSG.COM카드 Ed2 10만원 이상 10% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 7만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', '(1/12~18) 명장 장바구니 10% 쿠폰']</t>
+          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>설 선물세트 퀵배송</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>아직 명절 준비 못했다면, 빠르고 편리하게 마음을 선물하세요</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003880&amp;previewYn=Y&amp;cacheCmd=expire</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>23년 설 배송마감/퀵배송 기획전</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 23년 설 배송마감/퀵배송 기획전', '스마일클럽', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 디올</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NEW미차 리미티드 에디션부터 다양한 특별 혜택까지</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003632</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 디올</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 디올', '스마일클럽', ' 03. 특정 상품 구매 시, 스페셜 사은품 증정 루즈 디올 - 미차 리미티드 에디션 구매 시, 루즈 디올 립스틱 홀더 증정 ※ 상품 주문수량 당 1개 증정 디올 어딕트 립 아이템 포함, 8만원 이상 구매 시, 어딕트 폰 그립 증정 ※ 디올 어딕트 립 아이템 포함 디올 뷰티 전 상품 8만원 이상 구매시 적용 ※ 어딕트 립 글로우, 어딕트 립스틱, 어딕트 립 틴트, 어딕트 립 맥시마이저, 어딕트 립 글로우 오일 제품 포함 ※ 주문번호 당 1개 증정 ']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>설 선물도 역시! 선물하기로</t>
+          <t>2023 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>쓱에서 선물하면 내 선물도 쓱-</t>
+          <t>설 특별전</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
+          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>광장시장 K-원조 맛집</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>최대 50% 할인에 페이백 이벤트까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003731</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>힙스토랑 순희네 빈대떡 편</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; 힙스토랑 순희네 빈대떡 편', '스마일클럽', '순희네 빈대떡 간판 메뉴 3종 최대 50% 할인 행사', '맷돌로 직접 간 녹두에 숙주와 김치 듬뿍 순희네 녹두 빈대떡 : 정상가 8,980원 8%할인가 8,262원', '가득한 고기와 야채가 일품인 순희네 고기완자전 : 정상가 7,980원 15%할인가 6,783원', '탱글탱글한 새우와 아삭한 채소의 조화 순희네 새우녹두완자 : 정상가 9,480원 50%할인가 4,740원', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>2023 스마일클럽 건강 프로젝트_</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★설특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전</t>
+          <t>스마일클럽 가입 축하 5천원 기프트</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>설 특별전</t>
+          <t>명절 선물세트 ~15% 2종 할인까지</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>WINTER : SEASON OFF</t>
+          <t>새해 여행 특가</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>인기 브랜드 SEASON OFF 최대 80% + 할인쿠폰 혜택</t>
+          <t>국제선 전 노선 최대 5만원 즉시할인 설 연휴 바로 출발! 해외 패키지 특가</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003767</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003809</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>(0109-15) WINTER : SEASON OFF</t>
+          <t>2023 여행 새해 특가</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0109-15) WINTER : SEASON OFF', '스마일클럽', '매일 선착순', '장바구니 쿠폰', '장바구니 쿠폰 8% : 5만원 이상 구매시 최대 1만 (매일 오전 9시) (선착순 1만장)', '쿠폰 발급 받기 - 기간 내 ID당 1회 발급', '쿠폰은 09시부터 다운 가능 합니다.', '오늘의 쿠폰은 마감 되었습니다!', '쿠폰 발급기간23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용기간23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰 발급 기간: 23/01/09(월) ~ 23/01/15(일) , 매일 오전 9시부터 선착순 발급', '쿠폰 사용 기간: 23/01/09(월) ~ 23/01/15(일) , 발급 후 기간 내 사용', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", ' SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '몽클레어 : 70주년 역사의 대표 명품 패딩 브랜드, 몽클레어 패셔너블 하면서도 뛰어난 품질을 갖춘 아이템들을 최대 30% 할인 혜택으로 만나보세요.', '슈콤마보니 : 여성을 가장 돋보이게 하는 슈즈 브랜드, 슈콤마보니 본사 + 아울렛 겨울 연합전을 통해 최대 80% 할인가로 만나보세요.', '투미 : 손흥민이 선택한 퍼포먼스 럭셔리 브랜드, 투미 다양한 베스트셀러들을 최대 30% 할인으로 만나보세요.', '나이키 : 전세계의 ATHLETE에게 영감과 혁신을 불어넣는 브랜드 나이키, WINTER SALE 최대 44% 할인 혜택을 놓치지 마세요.', '[마시모두띠 여성] 세일 최대 60% 할인!', '[빈폴레이디스]♥백화점 단독 물량♥ 아울렛 최대 52%OFF', '[S.I.VILLAGE] 보브/톰보이 外 ★50종 특가★ 패딩/코트/가디건 外 ~45%', '[쥬크.CC콜렉트.듀엘] SSG 브랜드위크! WINTER BEST ITEM LAST CHANCE ~60% OFF', '[주간BEST] 추위 걱정없는 포근한 겨울팬츠&amp;니트 BEST 새해맞이 무료배송', '테니스/골프웨어 추천♥ 일상룩으로도 활용가능한 FW 최대 50% 할인!', '[공식]위크엔드 막스마라 시즌오프 30% + 23SS 윈터 신상', '[마시모두띠 남성] 세일 최대 60% 할인', '겨울세일 최대 70% 할인! BEST 아이템 모음전', '[브룩스브라더스] 22 F/W 시즌오프 베스트 아이템  최대 30%OFF', '[J.LINDEBERG] 새해롭게 준비하는 골프 + 10% 쿠폰', '무료배송+사은품 마지막 특가 시즌오프! 골프/겨울/방한/모자/워머', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '컬럼비아 브랜드 위크 ~60% OFF', '[레투] 남녀공용 테니스/액티브룩 자켓&amp;상하의SET 최대 60% + 추가쿠폰', '편집샵 브랜드별 22FW SEASON OFF ~40%', '해피 뉴 이어, 패밀리 슈즈 제안 + 시크릿 15% 쿠폰', 'FW 신상슈즈 비밀특가+최대20%쿠폰♥', 'MAJE 22FW 시즌오프20%', '[공식][40프로할인]필드 토트 22 CD720 B4RHR', '[토리버치 공식]시즌오프 베스트 최대 40%세일', '[워치스테이션] 아르마니 BEST 시계 최대 61% SALE']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 여행 새해 특가', '스마일클럽', 'KYTE 선착순 단독 특가', '국제선 ~5만원 할인', '여행 전 상품 ~5만원 할인', '실시간 숙소 ~12% 할인', '카드 청구할인', '사용 방법:행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '소노캄고양 단독PKG 원마운트스노우할인권제공', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '호텔 인 나인 강남 정상가 : 91,958원 &gt; 할인가 : 80,923원', '디어스명동 (충무로) 호텔 정상가 : 81,400원 &gt; 할인가 : 71,632원', '이천 미란다 호텔 정상가 : 59,000원 &gt; 할인가 : 51,920원', '체스터톤스 속초 정상가 : 89,300원 &gt; 할인가 : 78,584원', '그랜드 조선 부산 정상가 : 209,000원 &gt; 할인가 : 183,920원', '모항 해나루 가족호텔 정상가 : 68,970원 &gt; 할인가 : 60,694원', '라마다 프라자 제주 정상가 : 120,000원 &gt; 할인가 : 105,600원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '켄싱턴호텔 여의도 정상가 : 99,900원 &gt; 할인가 : 87,912원', '글래드 마포 정상가 : 93,500원 &gt; 할인가 : 82,280원', '광명 테이크 호텔 정상가 : 125,000원 &gt; 할인가 : 110,000원', '인터컨티넨탈 알펜시아 평창 정상가 : 163,438원 &gt; 할인가 : 143,825원', '솔라리아 니시테츠 부산 정상가 : 65,000원 &gt; 할인가 : 57,200원', '여수 호텔 JCS 정상가 : 130,000원 &gt; 할인가 : 114,400원', '히든 클리프 호텔 앤 네이쳐 정상가 : 171,380원 &gt; 할인가 : 150,814원', '호텔 시리우스 제주 정상가 : 85,138원 &gt; 할인가 : 74,921원', '소노벨 비발디파크 B , C 정상가 : 193,000원 &gt; 할인가 : 169,840원', '휘닉스평창 리조트 정상가 : 209,000원 &gt; 할인가 : 183,920원', '메이힐스 리조트 정상가 : 93,500원 &gt; 할인가 : 82,280원', '하이원 리조트 정상가 : 204,000원 &gt; 할인가 : 179,520원', '용평리조트 정상가 : 193,230원 &gt; 할인가 : 170,042원', '곤지암리조트 정상가 : 196,650원 &gt; 할인가 : 173,052원', '웰리힐리파크 정상가 : 108,480원 &gt; 할인가 : 95,462원', '레고랜드 코리아 리조트 정상가 : 330,000원 &gt; 할인가 : 300,000원', '포항 네이처풀빌라펜션 정상가 : 190,000원 &gt; 할인가 : 167,200원', '여수 해랑호스텔펜션 정상가 : 140,000원 &gt; 할인가 : 123,200원', '포천 포레스트풀빌라(키즈풀빌라보유) 정상가 : 129,000원 &gt; 할인가 : 113,520원', '고성(속초) 코스트하우스펜션 정상가 : 55,000원 &gt; 할인가 : 48,400원', '강릉 더원펜션,더클래식펜션(신축펜션) 정상가 : 80,000원 &gt; 할인가 : 70,400원', '남양주 코지힐펜션(워터슬라이드,무료 스파) 정상가 : 109,000원 &gt; 할인가 : 95,920원', '가평 에이스펜션(대형수영장,스파) 정상가 : 69,000원 &gt; 할인가 : 60,720원', '서귀포 성산오채풀빌라 정상가 : 420,000원 &gt; 할인가 : 390,000원', '네스트 호텔 정상가 : 128,700원 &gt; 할인가 : 113,256원', '강릉 세인트존스호텔 정상가 : 100,000원 &gt; 할인가 : 88,000원', '호텔 탑스텐 정동진 정상가 : 94,910원 &gt; 할인가 : 83,521원', '파라다이스 호텔 부산 정상가 : 272,263원 &gt; 할인가 : 242,263원', '부산 송도 호텔 정상가 : 54,001원 &gt; 할인가 : 47,521원', '여수 유탑 마리나 호텔&amp;리조트 정상가 : 94,887원 &gt; 할인가 : 983,501원', '봄그리고가을 호텔&amp;리조트 정상가 : 57,000원 &gt; 할인가 : 50,160원', '오션 스위츠 제주 호텔 정상가 : 86,203원 &gt; 할인가 : 75,859원', '그랜드 하얏트 후쿠오카 정상가 : 393,562원 &gt; 할인가 : 366,013원', '오리엔탈 호텔 후쿠오카 하카타 스테이션 정상가 : 227,999원 &gt; 할인가 : 212,039원', '도쿄 sequence MIYASHITA PARK 정상가 : 235,651원 &gt; 할인가 : 219,155원', '아고라 플레이스 오사카 남바 정상가 : 109,406원 &gt; 할인가 : 101,748원', '퍼시픽 아일랜드 클럽 괌 정상가 : 360,815원 &gt; 할인가 : 355,558원', '스위소텔 더 스탬퍼드, 싱가포르 정상가 : 515,878원 &gt; 할인가 : 479,767원', '쉐라톤 그란데 수쿰윗, 럭셔리 컬렉션 호텔, 방콕 정상가 : 339,473원 &gt; 할인가 : 315,710원', '빈펄 리조트 &amp; 스파 다낭 정상가 : 552,914원 &gt; 할인가 : 514,210원', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 현대 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기', 'KB 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] NH카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Molly's SSG 1주년 감사제</t>
+          <t>레고 1/16(월) 11AM</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>매일 선착순 반려동물 15% 쿠폰</t>
+          <t>23년 신상품 라이브 단독 10% 적립+5%시청쿠폰 혜택</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003788</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003827</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Molly's SSG 1주년 감사제</t>
+          <t>[SSG.LIVE]1/16 11AM 레고</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; Molly's SSG 1주년 감사제", '스마일클럽', '매일 선착순 혜택', '최대 15% 쿠폰', '1주년 타임딜', '매일매일 선착순 혜택', '최대 15% 장바구니 쿠폰', '선착순 쿠폰은 매일 10시 오픈됩니다', '      15% 장바구니 쿠폰', '      매일 500명 선착순', '      최대 1만원 할인', '오늘의 쿠폰이 모두 소진되었습니다', '쿠폰은 1/9 10시 오픈됩니다', '      10% 장바구니 쿠폰', '타임딜은 매일 10시 오픈됩니다', '일룸 캐스터네츠 커스텀캣타워 정상가 619,000원 &gt; 할인가 517,100원 구매하러 가기', '힐스 사이언스다이어트 사료 모음전 정상가 148,000원 &gt; 할인가 108,400원 구매하러 가기', '내추럴발란스 강아지 사료 모음 정상가 88,000원 &gt; 할인가 60,400원 구매하러 가기', '포켄스 윔지스 버라이어티팩 정상가 32,000원 &gt; 할인가 24,000원 구매하러 가기', '웨루바 고양이 캔 12개입 정상가 32,400원 &gt; 할인가 18,900원 구매하러 가기', '야미야미 순살닭가슴살 22g x100개 정상가 26,500원 &gt; 할인가 23,500원 구매하러 가기', '붐펫 펫드라이룸 정상가 1,090,000원 &gt; 할인가 615,000원 구매하러 가기', '타임딜 스케줄', '[쓱배송] 우리와 ANF 반려견 사료 특가모음', '[로그인쿠폰] 하림펫푸드 더리얼 밥이보약 사료 모음', '쓱배송★ 반려견 프리미엄 영양제 견옥고', '[쓱배송] 새벽배송 내추럴발란스 사료 특가', '[쓱배송] 강아지 오리젠,아카나 사료', '점포/네오에서 쓱배송으로! 펫프렌즈 1+1 특가! (일부품목제외)', '반려동물 겨울나기 펫용품 쓱 할인전', '럭셔리 애견 용품 Boooh 15% mark-down 단독', '[쓱배송] 챠오츄르 SSG 단독상품 출시! 캣 간식 행사 모음', '밥이보약 30%외 몰리스 고양이 사료/간식 행사', '[고양이] 캐츠랑/프로베스트/이즈칸 대포장사료 ~40%_신세계몰 직발송', '[로그인시 최대20%]하림펫푸드 더리얼/밥이보약 고양이사료', '[쓱배송] 고양이 인기 캔/간식 N+1 /한정수량', '집사들 주목! 뽀떼/그린웨일 스크래쳐/캣타워/캣워크 할인', '[고양이 왕국] 펫페어 고양이 모래/캣타워/스크래쳐1+1/장난감 할인특가', 'SSG단독 ~40% 할인+사은품']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]1/16 11AM 레고', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+          <t>하기스 1/16(월) 12PM</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+          <t>하기스&amp;그린핑거 최대 52%할인, 구매인증시 스타벅스 경품 100분 증정</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003723</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트_</t>
+          <t>초특가 하기스&amp;그린핑거 최대 52%할인 @SSG.LIVE 1/16(수) 12PM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★런칭특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+          <t>['이벤트/쿠폰 &gt; 초특가 하기스&amp;그린핑거 최대 52%할인 @SSG.LIVE 1/16(수) 12PM', '스마일클럽', '초특가 하기스&amp;그린핑거 최대 52%할인 @SSG.LIVE 1/16(수) 12PM']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1월 가입 웰컴 기프트 5천원</t>
+          <t>정관장 1/16(월) 8PM</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>뷰티쓱세일스마일클럽 전용 할인까지</t>
+          <t>설명절 GIFT 넘버원 정관장! 선착순 추가 증정품</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003889</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>정관장 @SSG.LIVE 1/16(월) 20:00PM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', 'ONLY 멤버십은 더 큰 할인! BIG SMILE,BIG SALE', '매달 달라지는 특급 쇼핑 찬스 뷰티 쓱세일 스마일클럽 전용 추가 혜택', '쿠폰 받으러 가기', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 정관장 @SSG.LIVE 1/16(월) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛 위크 : 2023 신년 &amp; 설맞이 선물 특가전</t>
+          <t>비쎌  1/17(화) 7PM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
+          <t>습식청소기 16만원대+전용 포뮬라 증정</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003829</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003914&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[0109-0115] 프리미엄 아울렛 위크</t>
+          <t>비쎌@SSG.LIVE 1/17(화)19:00PM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0109-0115] 프리미엄 아울렛 위크', '스마일클럽', '최대 10% 할인 쿠폰 혜택', '할인율은 최초 정산가격 대비 할인율임', '[여성 패션 - 최대 80% 할인] 아울렛 위크 단독 특가, 시즌오프 BEST 外 보러가기', '[언더웨어 - 최대 73% 할인] 노와이어/심리스 &amp; 드로즈 &amp; 겨울 홈웨어 보러가기', '[해외명품 - 최대 70% 할인] 프라다/메종마르지엘라 外 명품 특가 보러가기', '[패션슈즈 - 최대 73% 할인] SHOES TOP 200 ITEMS 최대 10% 쿠폰 보러가기', '[패션잡화 - 최대 73% 할인] BAG&amp;ACC TOP 200 ITEMS 최대 10% 쿠폰 보러가기', '[키즈패션 - 최대 70% 할인] 유아동 BEST 모음 +최대 10% 쿠폰 보러가기', '[남성 패션 - 최대 70% 할인] 브룩스브라더스 外 남성 겨울 상품 입고 보러가기', '[유니섹스 - 최대 80% 할인] 라코스테/ 뉴에라 外 아웃도어 BEST 보러가기', '[스포츠 - 최대 70% 할인] 노스페이스/ 내셔널지오그래픽 外 BEST 보러가기', '[리빙 - 최대 70% 할인] 주방/식탁용품 BEST 모음 +최대10% 쿠폰 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 비쎌@SSG.LIVE 1/17(화)19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>클라랑스 1/12(목) 11AM</t>
+          <t>1월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>더블세럼 75ml 역대급 구성 핫딜 &amp; 립오일 1+1혜택까지</t>
+          <t>매월 쏟아지는 맘키즈 특가!</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003530</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[뷰티쓱세일] 클라랑스 @SSG.LIVE 1/12(목) 11:00AM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2022-12-20</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [뷰티쓱세일] 클라랑스 @SSG.LIVE 1/12(목) 11:00AM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>[뷰티쓱세일] 오휘 1/12(목) 7PM</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>최대 15,000원 적립+백화점 상품권 증정 혜택</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003879</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]1/12(목) 7PM 오휘</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2023-01-10</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2023-01-12</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]1/12(목) 7PM 오휘', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>에스티로더 1/13(금) 11AM</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>에스티로더 설 특집! 갈색병 세럼 50ml 구매 시, 45ml 추가 증정</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003584</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>[뷰티쓱세일] 에스티로더 @SSG.LIVE 1/13(금) 11AM</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2022-12-22</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2023-01-13</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [뷰티쓱세일] 에스티로더 @SSG.LIVE 1/13(금) 11AM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>신세계 No. 1 럭스 뷰티 대전</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>신세계상품권 증정 및 SSG머니 즉시할인 혜택</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003448&amp;domainSiteNo=6005</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>[1/9-1/15] 로레알 럭셔리 뷰티 쓱세일</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2023-01-09</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2023-01-15</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [1/9-1/15] 로레알 럭셔리 뷰티 쓱세일', '스마일클럽']</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>1월 맘키즈 플러스</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>매월 쏟아지는 맘키즈 특가!</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Jan 19 00:20:49 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,664 +473,479 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>쓱배송 만원 할인</t>
+          <t>연휴에도 쓱배송은 ing</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>쓱배송 장바구니 1만원 할인쿠폰 + 무료배송 쿠폰</t>
+          <t>장보기 추천 상품 + 핫플 랜선 투어 ~ 15% 할인</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003796&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003928&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023 첫 장보기 응원! 쓱배송 만원할인</t>
+          <t>연휴에도  쓱배송은 ing</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-18</t>
+          <t>2023-01-24</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 첫 장보기 응원! 쓱배송 만원할인', '스마일클럽', '2023 첫 장보기 응원! 쓱배송 만원할인', '2023 첫장보기 응원 쓱배송 만원할인', '(첫구매 전용 EVENT) 장바구니쿠폰 10,000원', 'WELCOME 쓱배송 첫구매 고객님,1년만에 다시 오신 고객님 1만원 바로 할인 받고 무료배송 받으세요 바로보기', '쓱배송 추천탬 쓱배송 첫구매 고객 인기 아이템 추천', '2023년 첫 장보기 혜택 쓱배송 첫구매 고객 1만원 바로 할인', '(첫 구매 전용)장바구니쿠폰 10,000원 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '(첫 구매 전용)무료배송 이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', '첫구매 쿠폰 모두 한번에 받기', '       2022년 1월 11일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매이력이 없는 고객 한정', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰: 쓱배송/새벽배송 상품 2만원 이상 구매시 최대 1만원 할인', '       무료배송 쿠폰: 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 적용 대상', '       쓱배송, 새벽배송', '       쓱배송 새벽배송 상품에 대해 적용 가능 (일부상품 제외)', '       쿠폰 발급 대상', '쓱배송 첫구매 고객 인기 아이템 추천']</t>
+          <t>['이벤트/쿠폰 &gt; 연휴에도  쓱배송은 ing', '스마일클럽', '연휴에도  쓱배송은 ing', '연휴에도 쓱배송은 ing', '실속있는 장보기 추천 상품 + 핫플 랜선 투어 최대 15% 할인', '연휴 쓱배송 일정 안내 바로보기', '#01 연휴 쓱배송 일정은 어떻게 되나요\xa0', '쓱배송 상품은 명절 연휴 기간에도 배송됩니다. 1/21(토) 오후 2시 전까지 주문하시면 당일 배송 가능!', '*설 당일 1/22(일) 제외 및 일부 점포별 배송 가능 일자가 상이할 수 있습니다.(쓱배송 딱지를 확인하세요)', '쓱배송 가능한 상품만 보여드릴게요 - 쓱배송 매장 보기', '우리 집도 쓱배송 가능한가요\xa0 쓱배송 가능 지역 확인하러 가기', '#신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요', '#3 줄서기 없이 여유롭게 + 다다익선 최대 15% 할인까지!', '아우어베이커리, 노티드, 프��츠 등 인기 베이커리 &amp; 커피 3개 이상 10%, 5개 이상 구매 시 15% 할인!']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023 설 스페셜 혜택전</t>
+          <t>단 하루! 쓱배송데이</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>단 2일간, 장바구니 10% 쿠폰 최대 10만원</t>
+          <t>최대 10% 장바구니 쿠폰 + 카드 혜택</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003651</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003887</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[1/16-17] 2023 설 스페셜 혜택전</t>
+          <t>1/19 단 하루! 쓱배송데이</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-01-16</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-17</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [1/16-17] 2023 설 스페셜 혜택전', '스마일클럽', '10% 장바구니 쿠폰받기', '      장바구니 쿠폰 10% 쿠폰 (점포명절, 명절)', '      5만원 이상 구매 시 최대 10만원 할인', '쿠폰 발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '[명절] [점포 명절] 엠블렘이 있는 설 명절 기프트 상품 전용 쿠폰입니다.', '★쇼핑백 증정★ [폴로 랄프로렌]이태리산 울 100% 시그니처 멀티로고 폴로 머플러 3종', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가', '[1월18일 오전10시까지 주문시 명절전배송][수산대전20%][해신수산] 완도 활전복 1kg 外 선물세트 모음전', '베이커리 선물 모음전 (무료배송)', '★ 센트룸 할인 행사 ★', '[쓱배송]CJ 한뿌리 홍삼대보 24입 외 특가행사', '[빈폴멘] 22FW 30% 시즌오프! 실시간 BEST 추천', '신년 주목해야할 브랜드 마리끌레르♥ 프랜치 스타일 베스트 아이템 +추가 쿠폰', '해피 뉴 이어, 패밀리 슈즈 제안 + 시크릿 15% 쿠폰', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', 'FW 남여 의류/용품 최대 40% OFF', '블랙야크/디스커버리 外 인기브랜드 다운/패딩 ~70% OFF', '[나이키코리아공식] 남여 인기 신발 모음 ~45%', '설맞이 설레는 고양이 모래/캣타워/스크래쳐 용품 할인전', '[Boooh] 럭셔리 애견 용품 하네스 모음 (단독 20%)']</t>
+          <t>['이벤트/쿠폰 &gt; 1/19 단 하루! 쓱배송데이', '스마일클럽', '1/19 단 하루! 쓱배송데이', '할인에 할인을 더하다', '쓱배송데이', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '쓱배송 특가상품 최대 50% 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장보기 쿠폰', '이마트, 트레이더스 쓱배송 및 점포택배/새벽배송', '10% 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1매 (오전 9시 오픈, 선착순 2만명)', '10% 쿠폰 - 8만원 이상 결제시 최대 2만원 할인 ID당 1매 (오전 9시 오픈, 선착순 5천명, smile club 전용)', '스마일클럽 전용 쿠폰 받기', '       쿠폰발급 및 사용 기간', '       2023년 1월 19일 (당일 발급된 쿠폰은 당일 한정 사용가능)', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', 'KB국민카드 7만원 이상 5% 청구할인(일 10만원 한) 자세히 보기', '      쿠폰 발급 및 사용일', '      23년 1월 19일 단 하루! (기간 중 ID당 1일 1회 다운가능, 발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      스마일클럽 전용 2만원 할인 장바구니 쿠폰 : 스마일클럽 멤버십 가입 회원 전용 (두 쿠폰 모두 이메일주소, SNS 등으로 가입된 간편회원은 제외됩니다)', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '최대 50% 쓱배송데이 장보기 특가상품', '1. 점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '2. 가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>명절 장보기</t>
+          <t>2023 설 선물 늦지 않았어요</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>명절 장보고 최대 1만원 할인쿠폰 신청하세요</t>
+          <t>명절 전날까지 이마트몰 쓱-배송</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003798&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003860&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(1/12~18) 명절 장보기</t>
+          <t>[명절] 23년 설 쓱배송/바로배송 선물 준비!</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2023-01-18</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-18</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/12~18) 명절 장보기', '스마일클럽', '명절 장보고 신청하면 최대 1만원 할인쿠폰 EVENT 바로보기', '온가족이 함께 즐기는 쓱배송 명절 먹거리 바로보기', '명절에 진심인 분은 쓱배송으로 장을 봅니다.', '쓱배송으로 장보면 최대 1만원 할인쿠폰 증정', '1월 12일 부터 1월 18일 까지 쓱배송으로 10만원 이상 구매고객 대상', '쓱배송 상품 전용 10% 할인쿠폰 (선착순 1만명) (1월 25일 이후 순차 지급)', '이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능) * 배송비, 할인액을 제외한 상품 실결제 금액 기준입니다. * 신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.", '      1/25(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용조건', '      이마트/트레이더스 쓱배송/새벽배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '      쿠폰 사용기간', '      쿠폰 사용대상', '      이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배 8만원 이상 결제 시 최대 1만원 할인 (ID당 1회)', '할인쿠폰 신청하기', '많은 성원으로 선착순 응모 마감되었습니다. 가족과 함께 따뜻한 명절을 즐기세요:)', "      행사기간 동안 이마트 쓱배송/새벽배송/점포택배, 트레이더스 쓱배송/점포택배로 10만원 이상 구매 후 '신청버튼' 클릭 (구매합산 가능)", '      배송비, 할인액을 제외한 상품 실결제 금액 기준입니다.', '      신청하였으나, 주문취소 등으로 신청 조건을 만족하지 못하였을 경우, 쿠폰 지급 대상에서 제외됩니다.', '      쿠폰 발급 예정일', '      1월 25일(수) 이후 순차적으로 고객님 쿠폰함으로 자동 지급 (마이 쿠폰함 확인)', '      쿠폰 사용 조건', '      쿠폰 사용 가능 기간', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '온가족이 함께 즐기는 이마트몰 쓱배송 명절 먹거리', '쓱배송 딱지를 확인하세요!', '이마트몰 쓱배송 명절 먹거리 상품 더 보러가기', '명장이라면, 놓치지마세요 카드 청구할인', 'KB국민카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 7만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[명절상품] SSG.COM카드 Ed2 10만원 이상 10% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 현대카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 7만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', '(1/12~18) 명장 장바구니 10% 쿠폰']</t>
+          <t>['이벤트/쿠폰 &gt; [명절] 23년 설 쓱배송/바로배송 선물 준비!', '스마일클럽', '[명절] 23년 설 쓱배송/바로배송 선물 준비!', '명절 전날까지 쓱배송 바로보기', '명절 전날까지 쓱배송', '상품상세페이지 쓱배송 마크를 꼭 확인하세요!', '1월 22일 (일) 명절 당일은 쓱배송을 운영하지 않습니다.', '점포에 따라 쓱배송이 조기 마감될 수 있으니 내 점포 배송시간을 미리 확인해 보세요', '쓱배송 배송시간 확인', '쓱배송 주문방법', '담기 전 왼쪽 하단 쓱배송 마크를 꼭 확인해주세요!', '카테고리별 쓱배송 선물세트 확인하기', '쓱배송 마크를 꼭 확인하세요!', '이마트 설 명절 선물세트 행사카드 결제 시 최대 50만원 상품권 증정 or 즉시할인 행사카드로 10만원 이상 구매 시 적용 자세히 보기', '트레이더스 설 명절 선물세트 행사카드 결제 시 최대 50만원 상품권 증정 or 즉시할인 행사카드로 10만원 이상 구매 시 적용 자세히 보기', '설 명절 선물세트 행사카드 결제 시 최대 40% 즉시할인 행사카드로 전액 결제 시, 상품권 증정 제외 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>설 선물세트 퀵배송</t>
+          <t>브랜드 스포트라이트 X 트라이온: JJ지고트</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>아직 명절 준비 못했다면, 빠르고 편리하게 마음을 선물하세요</t>
+          <t>SSG 단독 최대 80% 클리어런스 세일</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003880&amp;previewYn=Y&amp;cacheCmd=expire</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003845</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>23년 설 배송마감/퀵배송 기획전</t>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 23년 설 배송마감/퀵배송 기획전', '스마일클럽', '[냉장][장흥명품한우할인직판장] 구이1호 1.3kg 외 프리미엄 한우 선물세트 특가']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트', '스마일클럽', '1 WINTER CLEARANCE 최대 80% OFF', '2 23년 봄 신상 최대 50% OFF', 'SSG 단독! 브랜드 스포트라이트 기간에만 진행하는 특별 할인']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: JJ지고트</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SSG 단독 최대 80% 클리어런스 세일</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003845</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-01-16</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트', '스마일클럽', '1 WINTER CLEARANCE 최대 80% OFF', '2 23년 봄 신상 최대 50% OFF', 'SSG 단독! 브랜드 스포트라이트 기간에만 진행하는 특별 할인']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>설 선물도 역시! 선물하기로</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>쓱에서 선물하면 내 선물도 쓱-</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003555</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(0102-0122) 설선물도 역시! 선물하기로 쓱-</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0102-0122) 설선물도 역시! 선물하기로 쓱-', '스마일클럽', '선물하기 이벤트 SSG에서 드리는 선물 바로보기', '이벤트 응모하기', '※ 본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '※ 나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외 )', '이벤트 기간(1/2~22) 동안 선물하기 상품 구매 고객을 대상으로 1회 응모 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '본 이벤트는 이벤트는 ID당 1회 응모할수 있으며, 행사기간 중 1회 응모 가능합니다.', '선물왕은 이벤트 기간(1/2~22) ID당 선물하기 주문 건에 대한 총금액을 기준으로 합산되며, 기간 중 구매 건수와 구매금액이 많을수록 선정 확률은 올라갑니다.', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>쓱배송의 세계로 초대합니다</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>첫 구매 쿠폰 받고, 친구 초대하면 혜택이 두 배</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003900</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>1월 쓱배송 친구 초대 이벤트</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 1월 쓱배송 친구 초대 이벤트', '스마일클럽', '1월 쓱배송 친구 초대 이벤트', '5천원 할인에 무료배송', '친구 초대 이벤트', '쓱배송이 처음이라면? 할인에 무료배송', '쓱배송 웰컴 쿠폰', '5,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 2022년 1월 18일 이후 이마트몰, 트레이더스 쓱배송/점포 택배 및 새벽배송 구매 이력이 없는 고객 ', '쿠폰 사용 조건 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매 시 사용 가능', '이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 세가지 배송 모두 한 번도 해본 적 없는 친구에게 나의 초대장 번호를 공유해주세요', '응모 이후 초대받은 친구가 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', 'SSG MONEY 적립 이후 초대받은 친구가 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '본인 스스로 초대한 경우에는 이벤트 참여에서 제외됩니다.', "친구가 전달 준 초대장 번호를 입력하고 '첫 쓱배송 응모하기' 버튼을 눌러주세요 응모 이후, 반드시 이벤트 기간 내 첫 쓱배송 구매를 완료해야만 SSG MONEY가 정상 적립됩니다.", '첫 쓱배송 응모하기', '이벤트 응모여부 확인하기', 'STEP2 첫 쓱배송 배송 주문하기 : 쓱배송 or 쓱배송TRADERS or 새벽배송(* 주문시, 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'STEP3 SSG MONEY적립 : 이벤트 종료 후 2월 10일(금) 이내 SSG MONEY가 일괄 적립됩니다.', '응모 이후 이벤트 기간 내 "쓱배송" 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', '쓱배송이 아닌 다른 배송 유형으로 구매했을 시, 참여 인정되지 않습니다. (반드시 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '이벤트 기간 :  1월 19일(목) 00:00 ~ 1월 31일(화) 23:59', '최근 1년 간 이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 모두 구매 이력이 없는 경우만 쓱배송 첫 구매자로 응모 가능합니다. (2022년 1월 18일 이후 주문 내역이 없는 자)', '이벤트 기간 내 등록할 수 있는 초대자는 한 명입니다.', '본인 스스로 초대/응모한 경우에는 이벤트 참여에서 제외됩니다.', '응모 이후  초대받은 사람이 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 ? 첫 구매 배송 완료)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 추천인과 초대받은 사람 모두 SSG MONEY가 회수될 수 있습니다.', '초대 받은 친구가 탈퇴 후 재가입하여 구매를 하더라도 첫 구매로 인정되지 않으며, SSG MONEY가 지급되지 않습니다.', '본 이벤트를 통해 지급된 SSG MONEY는 지급일로부터 30일 이후 자동 소멸됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 당첨이 취소될 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>2023 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>설 특별전</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전</t>
+          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>설 특별전</t>
+          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
+          <t>2023 스마일클럽 건강 프로젝트_</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송] CJ 한뿌리 홍삼대보 24입 외 특가행사', '[쓱배송][Biopublic]홍삼정 240g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★설특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>광장시장 K-원조 맛집</t>
+          <t>스마일클럽 가입 축하 5천원 기프트</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>최대 50% 할인에 페이백 이벤트까지</t>
+          <t>명절 선물세트 ~15% 2종 할인까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003731</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>힙스토랑 순희네 빈대떡 편</t>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-01-16</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 힙스토랑 순희네 빈대떡 편', '스마일클럽', '순희네 빈대떡 간판 메뉴 3종 최대 50% 할인 행사', '맷돌로 직접 간 녹두에 숙주와 김치 듬뿍 순희네 녹두 빈대떡 : 정상가 8,980원 8%할인가 8,262원', '가득한 고기와 야채가 일품인 순희네 고기완자전 : 정상가 7,980원 15%할인가 6,783원', '탱글탱글한 새우와 아삭한 채소의 조화 순희네 새우녹두완자 : 정상가 9,480원 50%할인가 4,740원', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
+          <t>쓱스럽게 안녕</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
+          <t>See you again, Say Goodbye</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003967</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2023 스마일클럽 건강 프로젝트_</t>
+          <t>쓱스럽게 안녕</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-17</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송]정관장 홍삼정 에브리타임 밸런스 10ml*20포[쇼핑백포함]', '[쓱배송][정관장]홍삼진황 50ml*20포[쇼핑백포함]', '★15%즉시할인★ 종근당건강 BEST 행사 상품', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[쓱배송]셀렉스 코어프로틴 프로 캔 304g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★설특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
+          <t>['이벤트/쿠폰 &gt; 쓱스럽게 안녕', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>스마일클럽 가입 축하 5천원 기프트</t>
+          <t>새해 여행 특가</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>명절 선물세트 ~15% 2종 할인까지</t>
+          <t>국제선 전 노선 최대 5만원 즉시할인 설 연휴 바로 출발! 해외 패키지 특가</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003809</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>2023 여행 새해 특가</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 여행 새해 특가', '스마일클럽', 'KYTE 선착순 단독 특가', '국제선 ~5만원 할인', '여행 전 상품 ~5만원 할인', '실시간 숙소 ~12% 할인', '카드 청구할인', '사용 방법:행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '소노캄고양 단독PKG 원마운트스노우할인권제공', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '호텔 인 나인 강남 정상가 : 91,958원 &gt; 할인가 : 80,923원', '디어스명동 (충무로) 호텔 정상가 : 81,400원 &gt; 할인가 : 71,632원', '이천 미란다 호텔 정상가 : 59,000원 &gt; 할인가 : 51,920원', '체스터톤스 속초 정상가 : 89,300원 &gt; 할인가 : 78,584원', '그랜드 조선 부산 정상가 : 209,000원 &gt; 할인가 : 183,920원', '모항 해나루 가족호텔 정상가 : 68,970원 &gt; 할인가 : 60,694원', '라마다 프라자 제주 정상가 : 120,000원 &gt; 할인가 : 105,600원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '켄싱턴호텔 여의도 정상가 : 99,900원 &gt; 할인가 : 87,912원', '글래드 마포 정상가 : 93,500원 &gt; 할인가 : 82,280원', '광명 테이크 호텔 정상가 : 125,000원 &gt; 할인가 : 110,000원', '인터컨티넨탈 알펜시아 평창 정상가 : 163,438원 &gt; 할인가 : 143,825원', '솔라리아 니시테츠 부산 정상가 : 65,000원 &gt; 할인가 : 57,200원', '여수 호텔 JCS 정상가 : 130,000원 &gt; 할인가 : 114,400원', '히든 클리프 호텔 앤 네이쳐 정상가 : 171,380원 &gt; 할인가 : 150,814원', '호텔 시리우스 제주 정상가 : 85,138원 &gt; 할인가 : 74,921원', '소노벨 비발디파크 B , C 정상가 : 193,000원 &gt; 할인가 : 169,840원', '휘닉스평창 리조트 정상가 : 209,000원 &gt; 할인가 : 183,920원', '메이힐스 리조트 정상가 : 93,500원 &gt; 할인가 : 82,280원', '하이원 리조트 정상가 : 204,000원 &gt; 할인가 : 179,520원', '용평리조트 정상가 : 193,230원 &gt; 할인가 : 170,042원', '곤지암리조트 정상가 : 196,650원 &gt; 할인가 : 173,052원', '웰리힐리파크 정상가 : 108,480원 &gt; 할인가 : 95,462원', '레고랜드 코리아 리조트 정상가 : 330,000원 &gt; 할인가 : 300,000원', '포항 네이처풀빌라펜션 정상가 : 190,000원 &gt; 할인가 : 167,200원', '여수 해랑호스텔펜션 정상가 : 140,000원 &gt; 할인가 : 123,200원', '포천 포레스트풀빌라(키즈풀빌라보유) 정상가 : 129,000원 &gt; 할인가 : 113,520원', '고성(속초) 코스트하우스펜션 정상가 : 55,000원 &gt; 할인가 : 48,400원', '강릉 더원펜션,더클래식펜션(신축펜션) 정상가 : 80,000원 &gt; 할인가 : 70,400원', '남양주 코지힐펜션(워터슬라이드,무료 스파) 정상가 : 109,000원 &gt; 할인가 : 95,920원', '가평 에이스펜션(대형수영장,스파) 정상가 : 69,000원 &gt; 할인가 : 60,720원', '서귀포 성산오채풀빌라 정상가 : 420,000원 &gt; 할인가 : 390,000원', '네스트 호텔 정상가 : 128,700원 &gt; 할인가 : 113,256원', '강릉 세인트존스호텔 정상가 : 100,000원 &gt; 할인가 : 88,000원', '호텔 탑스텐 정동진 정상가 : 94,910원 &gt; 할인가 : 83,521원', '파라다이스 호텔 부산 정상가 : 272,263원 &gt; 할인가 : 242,263원', '부산 송도 호텔 정상가 : 54,001원 &gt; 할인가 : 47,521원', '여수 유탑 마리나 호텔&amp;리조트 정상가 : 94,887원 &gt; 할인가 : 983,501원', '봄그리고가을 호텔&amp;리조트 정상가 : 57,000원 &gt; 할인가 : 50,160원', '오션 스위츠 제주 호텔 정상가 : 86,203원 &gt; 할인가 : 75,859원', '그랜드 하얏트 후쿠오카 정상가 : 393,562원 &gt; 할인가 : 366,013원', '오리엔탈 호텔 후쿠오카 하카타 스테이션 정상가 : 227,999원 &gt; 할인가 : 212,039원', '도쿄 sequence MIYASHITA PARK 정상가 : 235,651원 &gt; 할인가 : 219,155원', '아고라 플레이스 오사카 남바 정상가 : 109,406원 &gt; 할인가 : 101,748원', '퍼시픽 아일랜드 클럽 괌 정상가 : 360,815원 &gt; 할인가 : 355,558원', '스위소텔 더 스탬퍼드, 싱가포르 정상가 : 515,878원 &gt; 할인가 : 479,767원', '쉐라톤 그란데 수쿰윗, 럭셔리 컬렉션 호텔, 방콕 정상가 : 339,473원 &gt; 할인가 : 315,710원', '빈펄 리조트 &amp; 스파 다낭 정상가 : 552,914원 &gt; 할인가 : 514,210원', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 현대 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기', 'KB 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] NH카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>새해 여행 특가</t>
+          <t>1월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>국제선 전 노선 최대 5만원 즉시할인 설 연휴 바로 출발! 해외 패키지 특가</t>
+          <t>매월 쏟아지는 맘키즈 특가!</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003809</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023 여행 새해 특가</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-01-16</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 2023 여행 새해 특가', '스마일클럽', 'KYTE 선착순 단독 특가', '국제선 ~5만원 할인', '여행 전 상품 ~5만원 할인', '실시간 숙소 ~12% 할인', '카드 청구할인', '사용 방법:행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '소노캄고양 단독PKG 원마운트스노우할인권제공', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '호텔 인 나인 강남 정상가 : 91,958원 &gt; 할인가 : 80,923원', '디어스명동 (충무로) 호텔 정상가 : 81,400원 &gt; 할인가 : 71,632원', '이천 미란다 호텔 정상가 : 59,000원 &gt; 할인가 : 51,920원', '체스터톤스 속초 정상가 : 89,300원 &gt; 할인가 : 78,584원', '그랜드 조선 부산 정상가 : 209,000원 &gt; 할인가 : 183,920원', '모항 해나루 가족호텔 정상가 : 68,970원 &gt; 할인가 : 60,694원', '라마다 프라자 제주 정상가 : 120,000원 &gt; 할인가 : 105,600원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '켄싱턴호텔 여의도 정상가 : 99,900원 &gt; 할인가 : 87,912원', '글래드 마포 정상가 : 93,500원 &gt; 할인가 : 82,280원', '광명 테이크 호텔 정상가 : 125,000원 &gt; 할인가 : 110,000원', '인터컨티넨탈 알펜시아 평창 정상가 : 163,438원 &gt; 할인가 : 143,825원', '솔라리아 니시테츠 부산 정상가 : 65,000원 &gt; 할인가 : 57,200원', '여수 호텔 JCS 정상가 : 130,000원 &gt; 할인가 : 114,400원', '히든 클리프 호텔 앤 네이쳐 정상가 : 171,380원 &gt; 할인가 : 150,814원', '호텔 시리우스 제주 정상가 : 85,138원 &gt; 할인가 : 74,921원', '소노벨 비발디파크 B , C 정상가 : 193,000원 &gt; 할인가 : 169,840원', '휘닉스평창 리조트 정상가 : 209,000원 &gt; 할인가 : 183,920원', '메이힐스 리조트 정상가 : 93,500원 &gt; 할인가 : 82,280원', '하이원 리조트 정상가 : 204,000원 &gt; 할인가 : 179,520원', '용평리조트 정상가 : 193,230원 &gt; 할인가 : 170,042원', '곤지암리조트 정상가 : 196,650원 &gt; 할인가 : 173,052원', '웰리힐리파크 정상가 : 108,480원 &gt; 할인가 : 95,462원', '레고랜드 코리아 리조트 정상가 : 330,000원 &gt; 할인가 : 300,000원', '포항 네이처풀빌라펜션 정상가 : 190,000원 &gt; 할인가 : 167,200원', '여수 해랑호스텔펜션 정상가 : 140,000원 &gt; 할인가 : 123,200원', '포천 포레스트풀빌라(키즈풀빌라보유) 정상가 : 129,000원 &gt; 할인가 : 113,520원', '고성(속초) 코스트하우스펜션 정상가 : 55,000원 &gt; 할인가 : 48,400원', '강릉 더원펜션,더클래식펜션(신축펜션) 정상가 : 80,000원 &gt; 할인가 : 70,400원', '남양주 코지힐펜션(워터슬라이드,무료 스파) 정상가 : 109,000원 &gt; 할인가 : 95,920원', '가평 에이스펜션(대형수영장,스파) 정상가 : 69,000원 &gt; 할인가 : 60,720원', '서귀포 성산오채풀빌라 정상가 : 420,000원 &gt; 할인가 : 390,000원', '네스트 호텔 정상가 : 128,700원 &gt; 할인가 : 113,256원', '강릉 세인트존스호텔 정상가 : 100,000원 &gt; 할인가 : 88,000원', '호텔 탑스텐 정동진 정상가 : 94,910원 &gt; 할인가 : 83,521원', '파라다이스 호텔 부산 정상가 : 272,263원 &gt; 할인가 : 242,263원', '부산 송도 호텔 정상가 : 54,001원 &gt; 할인가 : 47,521원', '여수 유탑 마리나 호텔&amp;리조트 정상가 : 94,887원 &gt; 할인가 : 983,501원', '봄그리고가을 호텔&amp;리조트 정상가 : 57,000원 &gt; 할인가 : 50,160원', '오션 스위츠 제주 호텔 정상가 : 86,203원 &gt; 할인가 : 75,859원', '그랜드 하얏트 후쿠오카 정상가 : 393,562원 &gt; 할인가 : 366,013원', '오리엔탈 호텔 후쿠오카 하카타 스테이션 정상가 : 227,999원 &gt; 할인가 : 212,039원', '도쿄 sequence MIYASHITA PARK 정상가 : 235,651원 &gt; 할인가 : 219,155원', '아고라 플레이스 오사카 남바 정상가 : 109,406원 &gt; 할인가 : 101,748원', '퍼시픽 아일랜드 클럽 괌 정상가 : 360,815원 &gt; 할인가 : 355,558원', '스위소텔 더 스탬퍼드, 싱가포르 정상가 : 515,878원 &gt; 할인가 : 479,767원', '쉐라톤 그란데 수쿰윗, 럭셔리 컬렉션 호텔, 방콕 정상가 : 339,473원 &gt; 할인가 : 315,710원', '빈펄 리조트 &amp; 스파 다낭 정상가 : 552,914원 &gt; 할인가 : 514,210원', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 현대 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기', 'KB 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] NH카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>레고 1/16(월) 11AM</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>23년 신상품 라이브 단독 10% 적립+5%시청쿠폰 혜택</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003827</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]1/16 11AM 레고</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2023-01-11</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-01-16</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]1/16 11AM 레고', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>하기스 1/16(월) 12PM</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>하기스&amp;그린핑거 최대 52%할인, 구매인증시 스타벅스 경품 100분 증정</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003723</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>초특가 하기스&amp;그린핑거 최대 52%할인 @SSG.LIVE 1/16(수) 12PM</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2023-01-02</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-01-16</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 초특가 하기스&amp;그린핑거 최대 52%할인 @SSG.LIVE 1/16(수) 12PM', '스마일클럽', '초특가 하기스&amp;그린핑거 최대 52%할인 @SSG.LIVE 1/16(수) 12PM']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>정관장 1/16(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>설명절 GIFT 넘버원 정관장! 선착순 추가 증정품</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003889</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>정관장 @SSG.LIVE 1/16(월) 20:00PM</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2023-01-10</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2023-01-16</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 정관장 @SSG.LIVE 1/16(월) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>비쎌  1/17(화) 7PM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>습식청소기 16만원대+전용 포뮬라 증정</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003914&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>비쎌@SSG.LIVE 1/17(화)19:00PM</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2023-01-11</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2023-01-19</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 비쎌@SSG.LIVE 1/17(화)19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1월 맘키즈 플러스</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>매월 쏟아지는 맘키즈 특가!</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Jan 23 00:19:45 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,212 +510,212 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>단 하루! 쓱배송데이</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 10% 장바구니 쿠폰 + 카드 혜택</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003887</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1/19 단 하루! 쓱배송데이</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 1/19 단 하루! 쓱배송데이', '스마일클럽', '1/19 단 하루! 쓱배송데이', '할인에 할인을 더하다', '쓱배송데이', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '쓱배송 특가상품 최대 50% 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장보기 쿠폰', '이마트, 트레이더스 쓱배송 및 점포택배/새벽배송', '10% 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1매 (오전 9시 오픈, 선착순 2만명)', '10% 쿠폰 - 8만원 이상 결제시 최대 2만원 할인 ID당 1매 (오전 9시 오픈, 선착순 5천명, smile club 전용)', '스마일클럽 전용 쿠폰 받기', '       쿠폰발급 및 사용 기간', '       2023년 1월 19일 (당일 발급된 쿠폰은 당일 한정 사용가능)', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', 'KB국민카드 7만원 이상 5% 청구할인(일 10만원 한) 자세히 보기', '      쿠폰 발급 및 사용일', '      23년 1월 19일 단 하루! (기간 중 ID당 1일 1회 다운가능, 발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      스마일클럽 전용 2만원 할인 장바구니 쿠폰 : 스마일클럽 멤버십 가입 회원 전용 (두 쿠폰 모두 이메일주소, SNS 등으로 가입된 간편회원은 제외됩니다)', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '최대 50% 쓱배송데이 장보기 특가상품', '1. 점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '2. 가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023 설 선물 늦지 않았어요</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>명절 전날까지 이마트몰 쓱-배송</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003860&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[명절] 23년 설 쓱배송/바로배송 선물 준비!</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-01-18</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [명절] 23년 설 쓱배송/바로배송 선물 준비!', '스마일클럽', '[명절] 23년 설 쓱배송/바로배송 선물 준비!', '명절 전날까지 쓱배송 바로보기', '명절 전날까지 쓱배송', '상품상세페이지 쓱배송 마크를 꼭 확인하세요!', '1월 22일 (일) 명절 당일은 쓱배송을 운영하지 않습니다.', '점포에 따라 쓱배송이 조기 마감될 수 있으니 내 점포 배송시간을 미리 확인해 보세요', '쓱배송 배송시간 확인', '쓱배송 주문방법', '담기 전 왼쪽 하단 쓱배송 마크를 꼭 확인해주세요!', '카테고리별 쓱배송 선물세트 확인하기', '쓱배송 마크를 꼭 확인하세요!', '이마트 설 명절 선물세트 행사카드 결제 시 최대 50만원 상품권 증정 or 즉시할인 행사카드로 10만원 이상 구매 시 적용 자세히 보기', '트레이더스 설 명절 선물세트 행사카드 결제 시 최대 50만원 상품권 증정 or 즉시할인 행사카드로 10만원 이상 구매 시 적용 자세히 보기', '설 명절 선물세트 행사카드 결제 시 최대 40% 즉시할인 행사카드로 전액 결제 시, 상품권 증정 제외 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: JJ지고트</t>
+          <t>쓱배송의 세계로 초대합니다</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SSG 단독 최대 80% 클리어런스 세일</t>
+          <t>첫 구매 쿠폰 받고, 친구 초대하면 혜택이 두 배</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003845</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003900</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트</t>
+          <t>1월 쓱배송 친구 초대 이벤트</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-01-16</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - JJ지고트', '스마일클럽', '1 WINTER CLEARANCE 최대 80% OFF', '2 23년 봄 신상 최대 50% OFF', 'SSG 단독! 브랜드 스포트라이트 기간에만 진행하는 특별 할인']</t>
+          <t>['이벤트/쿠폰 &gt; 1월 쓱배송 친구 초대 이벤트', '스마일클럽', '1월 쓱배송 친구 초대 이벤트', '5천원 할인에 무료배송', '친구 초대 이벤트', '쓱배송이 처음이라면? 할인에 무료배송', '쓱배송 웰컴 쿠폰', '5,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 2022년 1월 18일 이후 이마트몰, 트레이더스 쓱배송/점포 택배 및 새벽배송 구매 이력이 없는 고객 ', '쿠폰 사용 조건 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매 시 사용 가능', '이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 세가지 배송 모두 한 번도 해본 적 없는 친구에게 나의 초대장 번호를 공유해주세요', '응모 이후 초대받은 친구가 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', 'SSG MONEY 적립 이후 초대받은 친구가 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '본인 스스로 초대한 경우에는 이벤트 참여에서 제외됩니다.', "친구가 전달 준 초대장 번호를 입력하고 '첫 쓱배송 응모하기' 버튼을 눌러주세요 응모 이후, 반드시 이벤트 기간 내 첫 쓱배송 구매를 완료해야만 SSG MONEY가 정상 적립됩니다.", '첫 쓱배송 응모하기', '이벤트 응모여부 확인하기', 'STEP2 첫 쓱배송 배송 주문하기 : 쓱배송 or 쓱배송TRADERS or 새벽배송(* 주문시, 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'STEP3 SSG MONEY적립 : 이벤트 종료 후 2월 10일(금) 이내 SSG MONEY가 일괄 적립됩니다.', '응모 이후 이벤트 기간 내 "쓱배송" 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', '쓱배송이 아닌 다른 배송 유형으로 구매했을 시, 참여 인정되지 않습니다. (반드시 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '이벤트 기간 :  1월 19일(목) 00:00 ~ 1월 31일(화) 23:59', '최근 1년 간 이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 모두 구매 이력이 없는 경우만 쓱배송 첫 구매자로 응모 가능합니다. (2022년 1월 18일 이후 주문 내역이 없는 자)', '이벤트 기간 내 등록할 수 있는 초대자는 한 명입니다.', '본인 스스로 초대/응모한 경우에는 이벤트 참여에서 제외됩니다.', '응모 이후  초대받은 사람이 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 ? 첫 구매 배송 완료)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 추천인과 초대받은 사람 모두 SSG MONEY가 회수될 수 있습니다.', '초대 받은 친구가 탈퇴 후 재가입하여 구매를 하더라도 첫 구매로 인정되지 않으며, SSG MONEY가 지급되지 않습니다.', '본 이벤트를 통해 지급된 SSG MONEY는 지급일로부터 30일 이후 자동 소멸됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 당첨이 취소될 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>2023 대한민국 수산대전</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>설 특별전</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-05</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>스마일클럽 1월의 가입 혜택</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>쓱배송의 세계로 초대합니다</t>
+          <t>쓱스럽게 안녕</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>첫 구매 쿠폰 받고, 친구 초대하면 혜택이 두 배</t>
+          <t>See you again, Say Goodbye</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003900</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003967</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1월 쓱배송 친구 초대 이벤트</t>
+          <t>쓱스럽게 안녕</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2023-01-17</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -725,227 +725,42 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 1월 쓱배송 친구 초대 이벤트', '스마일클럽', '1월 쓱배송 친구 초대 이벤트', '5천원 할인에 무료배송', '친구 초대 이벤트', '쓱배송이 처음이라면? 할인에 무료배송', '쓱배송 웰컴 쿠폰', '5,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 2022년 1월 18일 이후 이마트몰, 트레이더스 쓱배송/점포 택배 및 새벽배송 구매 이력이 없는 고객 ', '쿠폰 사용 조건 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매 시 사용 가능', '이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 세가지 배송 모두 한 번도 해본 적 없는 친구에게 나의 초대장 번호를 공유해주세요', '응모 이후 초대받은 친구가 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', 'SSG MONEY 적립 이후 초대받은 친구가 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '본인 스스로 초대한 경우에는 이벤트 참여에서 제외됩니다.', "친구가 전달 준 초대장 번호를 입력하고 '첫 쓱배송 응모하기' 버튼을 눌러주세요 응모 이후, 반드시 이벤트 기간 내 첫 쓱배송 구매를 완료해야만 SSG MONEY가 정상 적립됩니다.", '첫 쓱배송 응모하기', '이벤트 응모여부 확인하기', 'STEP2 첫 쓱배송 배송 주문하기 : 쓱배송 or 쓱배송TRADERS or 새벽배송(* 주문시, 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'STEP3 SSG MONEY적립 : 이벤트 종료 후 2월 10일(금) 이내 SSG MONEY가 일괄 적립됩니다.', '응모 이후 이벤트 기간 내 "쓱배송" 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', '쓱배송이 아닌 다른 배송 유형으로 구매했을 시, 참여 인정되지 않습니다. (반드시 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '이벤트 기간 :  1월 19일(목) 00:00 ~ 1월 31일(화) 23:59', '최근 1년 간 이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 모두 구매 이력이 없는 경우만 쓱배송 첫 구매자로 응모 가능합니다. (2022년 1월 18일 이후 주문 내역이 없는 자)', '이벤트 기간 내 등록할 수 있는 초대자는 한 명입니다.', '본인 스스로 초대/응모한 경우에는 이벤트 참여에서 제외됩니다.', '응모 이후  초대받은 사람이 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 ? 첫 구매 배송 완료)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 추천인과 초대받은 사람 모두 SSG MONEY가 회수될 수 있습니다.', '초대 받은 친구가 탈퇴 후 재가입하여 구매를 하더라도 첫 구매로 인정되지 않으며, SSG MONEY가 지급되지 않습니다.', '본 이벤트를 통해 지급된 SSG MONEY는 지급일로부터 30일 이후 자동 소멸됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 당첨이 취소될 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요']</t>
+          <t>['이벤트/쿠폰 &gt; 쓱스럽게 안녕', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전</t>
+          <t>1월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>설 특별전</t>
+          <t>매월 쏟아지는 맘키즈 특가!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2023 스마일클럽 건강 프로젝트 ~ 15% 쿠폰</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>#명절선물세트 #탑브랜드 #건강을선물하세요</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003594</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2023 스마일클럽 건강 프로젝트_</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2023-01-01</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2023-01-22</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 2023 스마일클럽 건강 프로젝트_', '스마일클럽', '2023 스마일클럽 건강 프로젝트_', 'SmlieClub전용 15%상품쿠폰 : 5만원 이상 구매시 최대 1만 5천원 할인', '      쿠폰 발급 대상 및 발급 매수', 'SmlieClub전용 12%장바구니쿠폰 : 3만원 이상 구매시 최대 1만원 할인', '쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요', '스마일클럽 건강 프로젝트 최대 15%쿠폰 #명절선물 #새해새다짐 #탑브랜드', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다. (에누리, 상품 할인 제외)', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '[쓱배송] CJ 한뿌리 홍삼대보 24입 외 특가행사', '[쓱배송][Biopublic]홍삼정 240g 외 특가행사', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '★설특가★[무료배송][공식판매처] 1+1 쏜리서치 영양제 구성 모음! 2/데이,S.A.T 외']</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>스마일클럽 가입 축하 5천원 기프트</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>명절 선물세트 ~15% 2종 할인까지</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2023-01-02</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2023-01-31</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>쓱스럽게 안녕</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>See you again, Say Goodbye</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003967</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>쓱스럽게 안녕</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2023-01-17</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2023-01-31</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 쓱스럽게 안녕', '스마일클럽']</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>새해 여행 특가</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>국제선 전 노선 최대 5만원 즉시할인 설 연휴 바로 출발! 해외 패키지 특가</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003809</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2023 여행 새해 특가</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2023-01-16</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2023-01-22</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 2023 여행 새해 특가', '스마일클럽', 'KYTE 선착순 단독 특가', '국제선 ~5만원 할인', '여행 전 상품 ~5만원 할인', '실시간 숙소 ~12% 할인', '카드 청구할인', '사용 방법:행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '소노캄고양 단독PKG 원마운트스노우할인권제공', '사용 방법 :요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '호텔 인 나인 강남 정상가 : 91,958원 &gt; 할인가 : 80,923원', '디어스명동 (충무로) 호텔 정상가 : 81,400원 &gt; 할인가 : 71,632원', '이천 미란다 호텔 정상가 : 59,000원 &gt; 할인가 : 51,920원', '체스터톤스 속초 정상가 : 89,300원 &gt; 할인가 : 78,584원', '그랜드 조선 부산 정상가 : 209,000원 &gt; 할인가 : 183,920원', '모항 해나루 가족호텔 정상가 : 68,970원 &gt; 할인가 : 60,694원', '라마다 프라자 제주 정상가 : 120,000원 &gt; 할인가 : 105,600원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '켄싱턴호텔 여의도 정상가 : 99,900원 &gt; 할인가 : 87,912원', '글래드 마포 정상가 : 93,500원 &gt; 할인가 : 82,280원', '광명 테이크 호텔 정상가 : 125,000원 &gt; 할인가 : 110,000원', '인터컨티넨탈 알펜시아 평창 정상가 : 163,438원 &gt; 할인가 : 143,825원', '솔라리아 니시테츠 부산 정상가 : 65,000원 &gt; 할인가 : 57,200원', '여수 호텔 JCS 정상가 : 130,000원 &gt; 할인가 : 114,400원', '히든 클리프 호텔 앤 네이쳐 정상가 : 171,380원 &gt; 할인가 : 150,814원', '호텔 시리우스 제주 정상가 : 85,138원 &gt; 할인가 : 74,921원', '소노벨 비발디파크 B , C 정상가 : 193,000원 &gt; 할인가 : 169,840원', '휘닉스평창 리조트 정상가 : 209,000원 &gt; 할인가 : 183,920원', '메이힐스 리조트 정상가 : 93,500원 &gt; 할인가 : 82,280원', '하이원 리조트 정상가 : 204,000원 &gt; 할인가 : 179,520원', '용평리조트 정상가 : 193,230원 &gt; 할인가 : 170,042원', '곤지암리조트 정상가 : 196,650원 &gt; 할인가 : 173,052원', '웰리힐리파크 정상가 : 108,480원 &gt; 할인가 : 95,462원', '레고랜드 코리아 리조트 정상가 : 330,000원 &gt; 할인가 : 300,000원', '포항 네이처풀빌라펜션 정상가 : 190,000원 &gt; 할인가 : 167,200원', '여수 해랑호스텔펜션 정상가 : 140,000원 &gt; 할인가 : 123,200원', '포천 포레스트풀빌라(키즈풀빌라보유) 정상가 : 129,000원 &gt; 할인가 : 113,520원', '고성(속초) 코스트하우스펜션 정상가 : 55,000원 &gt; 할인가 : 48,400원', '강릉 더원펜션,더클래식펜션(신축펜션) 정상가 : 80,000원 &gt; 할인가 : 70,400원', '남양주 코지힐펜션(워터슬라이드,무료 스파) 정상가 : 109,000원 &gt; 할인가 : 95,920원', '가평 에이스펜션(대형수영장,스파) 정상가 : 69,000원 &gt; 할인가 : 60,720원', '서귀포 성산오채풀빌라 정상가 : 420,000원 &gt; 할인가 : 390,000원', '네스트 호텔 정상가 : 128,700원 &gt; 할인가 : 113,256원', '강릉 세인트존스호텔 정상가 : 100,000원 &gt; 할인가 : 88,000원', '호텔 탑스텐 정동진 정상가 : 94,910원 &gt; 할인가 : 83,521원', '파라다이스 호텔 부산 정상가 : 272,263원 &gt; 할인가 : 242,263원', '부산 송도 호텔 정상가 : 54,001원 &gt; 할인가 : 47,521원', '여수 유탑 마리나 호텔&amp;리조트 정상가 : 94,887원 &gt; 할인가 : 983,501원', '봄그리고가을 호텔&amp;리조트 정상가 : 57,000원 &gt; 할인가 : 50,160원', '오션 스위츠 제주 호텔 정상가 : 86,203원 &gt; 할인가 : 75,859원', '그랜드 하얏트 후쿠오카 정상가 : 393,562원 &gt; 할인가 : 366,013원', '오리엔탈 호텔 후쿠오카 하카타 스테이션 정상가 : 227,999원 &gt; 할인가 : 212,039원', '도쿄 sequence MIYASHITA PARK 정상가 : 235,651원 &gt; 할인가 : 219,155원', '아고라 플레이스 오사카 남바 정상가 : 109,406원 &gt; 할인가 : 101,748원', '퍼시픽 아일랜드 클럽 괌 정상가 : 360,815원 &gt; 할인가 : 355,558원', '스위소텔 더 스탬퍼드, 싱가포르 정상가 : 515,878원 &gt; 할인가 : 479,767원', '쉐라톤 그란데 수쿰윗, 럭셔리 컬렉션 호텔, 방콕 정상가 : 339,473원 &gt; 할인가 : 315,710원', '빈펄 리조트 &amp; 스파 다낭 정상가 : 552,914원 &gt; 할인가 : 514,210원', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 현대 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기', 'KB 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] NH카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1월 맘키즈 플러스</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>매월 쏟아지는 맘키즈 특가!</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Jan 26 00:20:26 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,212 +473,212 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>연휴에도 쓱배송은 ing</t>
+          <t>쓱배송 days</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>장보기 추천 상품 + 핫플 랜선 투어 ~ 15% 할인</t>
+          <t>10% 쿠폰 + 카드혜택</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003928&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003979</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>연휴에도  쓱배송은 ing</t>
+          <t>1/26~27 쓱배송DAYS</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2023-01-26</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-24</t>
+          <t>2023-01-27</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 연휴에도  쓱배송은 ing', '스마일클럽', '연휴에도  쓱배송은 ing', '연휴에도 쓱배송은 ing', '실속있는 장보기 추천 상품 + 핫플 랜선 투어 최대 15% 할인', '연휴 쓱배송 일정 안내 바로보기', '#01 연휴 쓱배송 일정은 어떻게 되나요\xa0', '쓱배송 상품은 명절 연휴 기간에도 배송됩니다. 1/21(토) 오후 2시 전까지 주문하시면 당일 배송 가능!', '*설 당일 1/22(일) 제외 및 일부 점포별 배송 가능 일자가 상이할 수 있습니다.(쓱배송 딱지를 확인하세요)', '쓱배송 가능한 상품만 보여드릴게요 - 쓱배송 매장 보기', '우리 집도 쓱배송 가능한가요\xa0 쓱배송 가능 지역 확인하러 가기', '#신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요', '#3 줄서기 없이 여유롭게 + 다다익선 최대 15% 할인까지!', '아우어베이커리, 노티드, 프��츠 등 인기 베이커리 &amp; 커피 3개 이상 10%, 5개 이상 구매 시 15% 할인!']</t>
+          <t>['이벤트/쿠폰 &gt; 1/26~27 쓱배송DAYS', '스마일클럽', '1/26~27 쓱배송DAYS', '할인에 할인을 더하다', '쓱배송DAYS', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '오늘은 장보는 날 쓱배송 특가상품 바로보기', '1. 쓱배송, 새벽배송 모두 쓸 수 있는 10% 장보기 쿠폰', '이마트, 트레이더스 쓱배송 및 점포택배/새벽배송', '10% 장바구니 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1일 1매 (오전 9시 오픈, 선착순 2만명)', '10% 장바구니 쿠폰 - 8만원 이상 결제시 최대 2만원 할인 ID당 1일 1매 (오전 9시 오픈, 선착순 5천명, smile club 전용)', '스마일클럽 전용 쿠폰 받기', '       쿠폰발급 및 사용 기간', '       2023년 1월 26일/27일 양일간 (*당일 발급된 쿠폰은 당일 한정 사용가능)', '       쿠폰 발급 및 사용일', '       23년 1월 26일/27일 양일간 (기간 중 ID당 1일 1회 다운가능, 발급된 쿠폰 당일 한정 사용 가능)', '       쿠폰 사용조건', '       대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '       쿠폰 발급 대상', '       스마일클럽 전용 2만원 할인 장바구니 쿠폰 : 스마일클럽 멤버십 가입 회원 전용 (두 쿠폰 모두 이메일주소, SNS 등으로 가입된 간편회원은 제외됩니다)', '       쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '+ 결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', '[SSGPAY 전용]삼성카드 최대 5만원 5% 청구할인 자세히 보기', '3. 오늘은 장보는 날! 쓱배송데이 장보기 특가상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품', '신세계상품권을 SSG MONEY로 전환하고 SSG.COM에서 쇼핑하세요 바로 가기']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>2023 쇼핑 버킷리스트</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>최대 3만원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003961</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>2023 쇼핑 버킷리스트</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 쇼핑 버킷리스트', '스마일클럽', '올해 첫 합리적 소비를 위한 장바구니쿠폰 2종', '장바구니쿠폰 10% 15만원 이상 최대 3만원', '장바구니쿠폰 7% 10만원 이상 최대 1만원', '쿠폰은 25일 10시에 오픈됩니다.', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[공식] 윈터 세일 최대 50% &amp; 베스트 상품 제안', '★레드하트★한정수량★맨투맨/니트 +)즉시할인쿠폰 바로적용', '★SSG x 템퍼★ 덴마크 프리미엄 TEMPUR ~베개/매트리스 ~30% OFF', '[자라홈] 이불, 쿠션, 러그 등 : 최대 60%할인', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '[즉시할인+카드혜택+사은품 4종] 삼성 갤럭시 워치4  모음', 'SSGX불리 최대 단독 증정 혜택~15%', '안티에이징&amp;기미잡티케어 ~50% 7만이상 구매시 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', '신년맞이 [SSG X 일동제약 퍼스트랩 ] 10종 스킨&amp;헤어케어 ~80%SALE!', '명절 연휴에 추천하는 향수 할인전 / 바이레도, 톰포드, 조말론 외', '트와이스 지효PICK  V리프팅 괄사 + 진정크림 UP TO 37% +무료배송', '♥시즌오프♥FW 인기 아이템 최대 52% OFF', '[에고이스트/랩/플라스틱아일랜드] ~70% OFF! 윈터 클리어런스 외 인기 아이템 쇼핑 위크', '[캠브리지] X SSG 아놀 단독 할인 + best 아이템 UP TO 40% OFF', '★어그 베스트셀러 ~40% 세일★', '[CARLYN]23SS 푸퍼 출시!♥신상&amp;베스트 최대 76% SALE + 추가 쿠폰 혜택까지!', '블랙야크/디스커버리 外 인기브랜드 다운/패딩 ~70% OFF', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[아식스 본사] 최대 82% OFF 다운부터 런닝화까지 베스트템 모음전', '투어360 골프화 50%할인', '[자라홈] 키즈용품, 장난감, 인형 등 : 최대 60%할인', '레고 클리어런스 특가! ★최대 40%할인★ (~2/1일까지)']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>블라썸 위크</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인, 1+1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004037</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>(1/26~2/1) 블라썸위크</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-01-26</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; (1/26~2/1) 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '한정수량! 오늘만! 단 하루 타임딜 바로보기', '최대 50%할인, 1+1, 사은품증정 블라썸관 행사상품/이벤트 바로보기', '한정수량! 오늘만! 단 하루 타임딜', '(오늘 단 하루, 1+1) CJ 비비고 특양지곰탕/특설렁탕 700G : 할인전 14,900원 할인후 개당 7,450원~', '(오늘 단 하루, 50%) 대상 포도씨유 900ml : 할인전 16,900원 할인후 8,450원', '(오늘 단 하루, 1+1) 풀무원 풀무원 모짜렐라 핫도그 5입 : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 31%, 1+1) LG생활건강 테크 실내건조 세탁세제3L : 할인전 15,900원 할인후 개당 5,450원', '(오늘 단 하루, 한정수량 체럼, 41%) 아모레퍼시픽 (체험팩) 스킨유 이노센트 샤워젤/로션 라보에이치 샴푸 : 할인전 4,900원 할인후 2,900원', '(오늘 단 하루, 40%) CJ 헷반 현미/흑미 귀리 곤약밥 150G*12개 : 할인전 35,760원 할인후 21,500원', '(오늘 단 하루, 1+1) CJ 백설 파스타 소스 4종 : 할인전 5,500원 할인후 개당 2,790원 ~', '(오늘 단 하루, 1+1) 풀무원 들기름을 섞어 바삭바삭 고소하게 구워낸 재래김 80g (5g*16) : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 1+1) 풀무원 풀무원 동물복지 수비드 닭가슴살 1150G 3종 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 45%) 아모레퍼시픽 LG생활건강 퍼퓸스튜디오 1L 플로라피치 : 할인전 8,900원 할인후 4,900원', '(오늘 단 하루, 1+1) 대상 청정원 드레싱 2종 : 할인전 3,600원 할인후 개당 1,800원', '(오늘 단 하루, 한정수량, 18%) 매일유업 상하치킨 브리또 6입 : 할인전 20,000원 할인후 16,500원', '(오늘 단 하루, 33%) 풀무원 풀무원 행복한 동물복지유정란 15구 780g : 할인전 8,980원 할인후 5,980원', '(오늘 단 하루, 30%, 한정수량) LG생활건강 피이조겔 지코의 NO.1보습크립 세트 : 할인전 59,800원 할인후 41,860원', '(오늘 단 하루, 60%, 한정수량) 아모레퍼시픽 려 더블이펙터 블랙 샴푸/트리트먼트 543ML : 할인전 39,000원 할인후 15,600원', '(오늘 단 하루, 1+1) 우리동네 떡볶이/고소한 유부초밥 330G : 할인전 4,900원 할인후 개당 2,980원~', '(오늘 단 하루, 1+1) CJ 비비고 진국육수 닭고기/소고기양지 500g : 할인전 3,080원 할인후 개당 1,540원', '(오늘 단 하루, 44%, 한정수량) 매일유업 셀렉스 프로핏 웨ㅐ이프로틴 드링크 초콜릿 2박스 : 할인전 69.900원 할인후 38,900원', '(오늘 단 하루, 1+1) LG생활건강 엘라스틴 5X 샴푸/트리트먼트 : 할인전 16,900원 할인후 개당 8,450원', '(오늘 단 하루, 1+1) LG생활건강 히말라야 핑크솔트 치약 100g*3_아이스카밍 : 할인전 14,900원 할인후 개당 7,450원', '(오늘 단 하루, 1+1) CJ 비비고 사골시래기된장국 460g : 할인전 5,480원 할인후 개당 2,740원', '(오늘 단 하루, 1+1) 풀무원 자연은맛있다 건면 4종 : 할인전 5,450원 할인후 개당 2,725원', '(오늘 단 하루, 1+1) 풀무원 요리육수 3종 1000ML : 할인전 3,980원 할인후 개당 1,990원', '(오늘 단 하루, 2개 구매 시 50%) 유한킴벌리 크리넥스 디럭스미니 카카오230매6입 : 할인전 12,700원 할인후 개당 6,350원', '(오늘 단 하루, 62%, 한정수량) LG생활건강 실크테라피 인리처드 액션 60ML X 4개 : 할인전 79,600원 할인후 29,900원', '(오늘 단 하루, 1+1) CJ 백설 스파게티소스 640G 2종 : 할인전 4,380원 할인후 개당 2,190원', '(오늘 단 하루, 18%, 한정수량) 매일유업 마이카페라떼 마일드로어슈거 220ml 10팩 : 할인전 14,500원 할인후 11,900원', '(오늘 단 하루, 25%, 한정수량) 아모레퍼시픽 일리윤 세라마이드 아토로션/울트라리페어로션 + 일리윤 로션 : 할인전 24,500원 할인후 18,743원', '(오늘 단 하루, 50%, 한정수량) 유한킴벌리 좋은느낌 유기농순면 내추럴코어 슬날대 14X6 : 할인전 35,900원 할인후 17,950원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 그린핑거 판테딘 더마 밴드/팬티 기저귀 : 할인전 30,450원 할인후 개당 15,225원~', '(오늘 단 하루, 1+1) 풀무원 다논 요거톡125G*4입 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 31%, 한정수량) 매일유업 셀렉스 코어프로틴 음료 오리지널 2박스 : 할인전 58,000원 할인후 39,900원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 크리넥스 안심 프리미엄 3겹 키친타올 140매x4롤 : 할인전 9,200원 할인후 개당 4,600원', '(오늘 단 하루, 52%, 한정수량) LG생활건강 세이프 뿌리는 레몬식초 400ml x 3개 : 할인전 22,500원 할인후 10,900원', '(오늘 단 하루, 한정수량 체험, 64%) 아모레퍼시픽 롱테이크 샌달우드 인텐시브 3종 KIT : 할인전 10,800원 할인후 3,900원', '최대 50%할인 / 1+1 / 다다익선 / 사은품증정', '블라썸관 행사상품 및 이벤트', '블라썸관 좋아요 누르면 5% 할인쿠폰', '최대 50% 할인 행사상품', '※ 자세한 내용은 상품 상세페이지 내 이벤트내용을 참고해주세요.', '최대 50%할인 행사상품', '블라썸관 좋아요 누르면 10% 할인쿠폰', '최대 50%할인 행사상품, 기획상품', '최대 50%할인, 1+1 행사상품', '최대 30%할인, 1+1 행사상품', '3만원 이상 구매고객 스타벅스 아메리카노 증정(선착순 1천명)', '최대 30%할인, 1+1 행사상품, SSG단독 상품', '구매왕 응모이벤트 : 1등 건조기(1명), 2등 스타벅스 아메리카노(100명)']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>쓱배송의 세계로 초대합니다</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>첫 구매 쿠폰 받고, 친구 초대하면 혜택이 두 배</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003900</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1월 쓱배송 친구 초대 이벤트</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 1월 쓱배송 친구 초대 이벤트', '스마일클럽', '1월 쓱배송 친구 초대 이벤트', '5천원 할인에 무료배송', '친구 초대 이벤트', '쓱배송이 처음이라면? 할인에 무료배송', '쓱배송 웰컴 쿠폰', '5,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 2022년 1월 18일 이후 이마트몰, 트레이더스 쓱배송/점포 택배 및 새벽배송 구매 이력이 없는 고객 ', '쿠폰 사용 조건 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매 시 사용 가능', '이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 세가지 배송 모두 한 번도 해본 적 없는 친구에게 나의 초대장 번호를 공유해주세요', '응모 이후 초대받은 친구가 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', 'SSG MONEY 적립 이후 초대받은 친구가 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '본인 스스로 초대한 경우에는 이벤트 참여에서 제외됩니다.', "친구가 전달 준 초대장 번호를 입력하고 '첫 쓱배송 응모하기' 버튼을 눌러주세요 응모 이후, 반드시 이벤트 기간 내 첫 쓱배송 구매를 완료해야만 SSG MONEY가 정상 적립됩니다.", '첫 쓱배송 응모하기', '이벤트 응모여부 확인하기', 'STEP2 첫 쓱배송 배송 주문하기 : 쓱배송 or 쓱배송TRADERS or 새벽배송(* 주문시, 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'STEP3 SSG MONEY적립 : 이벤트 종료 후 2월 10일(금) 이내 SSG MONEY가 일괄 적립됩니다.', '응모 이후 이벤트 기간 내 "쓱배송" 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', '쓱배송이 아닌 다른 배송 유형으로 구매했을 시, 참여 인정되지 않습니다. (반드시 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '이벤트 기간 :  1월 19일(목) 00:00 ~ 1월 31일(화) 23:59', '최근 1년 간 이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 모두 구매 이력이 없는 경우만 쓱배송 첫 구매자로 응모 가능합니다. (2022년 1월 18일 이후 주문 내역이 없는 자)', '이벤트 기간 내 등록할 수 있는 초대자는 한 명입니다.', '본인 스스로 초대/응모한 경우에는 이벤트 참여에서 제외됩니다.', '응모 이후  초대받은 사람이 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 ? 첫 구매 배송 완료)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 추천인과 초대받은 사람 모두 SSG MONEY가 회수될 수 있습니다.', '초대 받은 친구가 탈퇴 후 재가입하여 구매를 하더라도 첫 구매로 인정되지 않으며, SSG MONEY가 지급되지 않습니다.', '본 이벤트를 통해 지급된 SSG MONEY는 지급일로부터 30일 이후 자동 소멸됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 당첨이 취소될 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>설 특별전</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(1/5~25) 2023 대한민국 수산대전 - 설 특별전</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-01-05</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/5~25) 2023 대한민국 수산대전 - 설 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 2만원 할인 받으세요!', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 2만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>스마일클럽 1월의 가입 혜택</t>
+          <t>쓱배송의 세계로 초대합니다</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>첫 구매 쿠폰 받고, 친구 초대하면 혜택이 두 배</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003900</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>1월 쓱배송 친구 초대 이벤트</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,34 +688,34 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 1월 쓱배송 친구 초대 이벤트', '스마일클럽', '1월 쓱배송 친구 초대 이벤트', '5천원 할인에 무료배송', '친구 초대 이벤트', '쓱배송이 처음이라면? 할인에 무료배송', '쓱배송 웰컴 쿠폰', '5,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 2022년 1월 18일 이후 이마트몰, 트레이더스 쓱배송/점포 택배 및 새벽배송 구매 이력이 없는 고객 ', '쿠폰 사용 조건 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매 시 사용 가능', '이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 세가지 배송 모두 한 번도 해본 적 없는 친구에게 나의 초대장 번호를 공유해주세요', '응모 이후 초대받은 친구가 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', 'SSG MONEY 적립 이후 초대받은 친구가 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '본인 스스로 초대한 경우에는 이벤트 참여에서 제외됩니다.', "친구가 전달 준 초대장 번호를 입력하고 '첫 쓱배송 응모하기' 버튼을 눌러주세요 응모 이후, 반드시 이벤트 기간 내 첫 쓱배송 구매를 완료해야만 SSG MONEY가 정상 적립됩니다.", '첫 쓱배송 응모하기', '이벤트 응모여부 확인하기', 'STEP2 첫 쓱배송 배송 주문하기 : 쓱배송 or 쓱배송TRADERS or 새벽배송(* 주문시, 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'STEP3 SSG MONEY적립 : 이벤트 종료 후 2월 10일(금) 이내 SSG MONEY가 일괄 적립됩니다.', '응모 이후 이벤트 기간 내 "쓱배송" 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', '쓱배송이 아닌 다른 배송 유형으로 구매했을 시, 참여 인정되지 않습니다. (반드시 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '이벤트 기간 :  1월 19일(목) 00:00 ~ 1월 31일(화) 23:59', '최근 1년 간 이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 모두 구매 이력이 없는 경우만 쓱배송 첫 구매자로 응모 가능합니다. (2022년 1월 18일 이후 주문 내역이 없는 자)', '이벤트 기간 내 등록할 수 있는 초대자는 한 명입니다.', '본인 스스로 초대/응모한 경우에는 이벤트 참여에서 제외됩니다.', '응모 이후  초대받은 사람이 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 ? 첫 구매 배송 완료)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 추천인과 초대받은 사람 모두 SSG MONEY가 회수될 수 있습니다.', '초대 받은 친구가 탈퇴 후 재가입하여 구매를 하더라도 첫 구매로 인정되지 않으며, SSG MONEY가 지급되지 않습니다.', '본 이벤트를 통해 지급된 SSG MONEY는 지급일로부터 30일 이후 자동 소멸됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 당첨이 취소될 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>쓱스럽게 안녕</t>
+          <t>스마일클럽 1월의 가입 혜택</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>See you again, Say Goodbye</t>
+          <t>WELCOME 5천원 할인쿠폰 제공</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003967</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>쓱스럽게 안녕</t>
+          <t>[스마일클럽] 1월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-17</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -725,44 +725,155 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 쓱스럽게 안녕', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1월 맘키즈 플러스</t>
+          <t>쓱스럽게 안녕</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>매월 쏟아지는 맘키즈 특가!</t>
+          <t>See you again, Say Goodbye</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003967</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>이달의 맘키즈 PLUS</t>
+          <t>쓱스럽게 안녕</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
+          <t>2023-01-17</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2999-12-13</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '크리스탈 레진아트 칼라세트(N2 쓱배송, 전국택배)', '뽀로로 코딩컴퓨터(N2 쓱배송, 전국택배)', '미미 어린이병원 (N2쓱배송, 전국택배)']</t>
+          <t>['이벤트/쿠폰 &gt; 쓱스럽게 안녕', '스마일클럽']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>민지의 장바구니-겨울 먹거리편</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003980</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>민지의 장바구니-겨울 먹거리편 (1/26~2/1)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-겨울 먹거리편 (1/26~2/1)', '스마일클럽', 'SSG MONEY 1천원 (500명)', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       - ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       - 이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '최대 2만원 할인 10% 장보기 쿠폰 받고 오세요!', '쓱배송데이 보러가기', '신세계몰 상품권을 SSG MONEY로 전환하고 SSG.COM에서 쇼핑하세요']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>신일전자 1/26(목) 8PM</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>신일 팬히터 1200 아이보리 선착순 핫딜 39만원대 + 전고객 캠핑용 전기그릴 증정</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003983</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>신일 팬히터 선착순 핫딜 39만원대 @SSG.LIVE 1/26(목) 8PM</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-01-19</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 신일 팬히터 선착순 핫딜 39만원대 @SSG.LIVE 1/26(목) 8PM', '스마일클럽', '신일 팬히터 선착순 핫딜 39만원대 @SSG.LIVE 1/26(목) 8PM']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>피코크 1/27(금) 11AM</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>요리가 제일 귀찮을 명절 직후, 피코크 간식/간편식 최대 52%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003986</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>피코크 @SSG.LIVE 1/27(금) 11:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-01-17</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023-01-27</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 피코크 @SSG.LIVE 1/27(금) 11:00', '스마일클럽']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Jan 30 00:18:07 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,37 +473,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>쓱배송 days</t>
+          <t>역대급 디지털 쇼핑 혜택 COMING SOON</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10% 쿠폰 + 카드혜택</t>
+          <t>행운의 쓱세일 퀴즈 미리 풀고 스탠바이미/다이슨 경품 도전!</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003979</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003975</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1/26~27 쓱배송DAYS</t>
+          <t>행운의 쓱세일을 잡아라!</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2023-01-30</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-27</t>
+          <t>2023-02-05</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 1/26~27 쓱배송DAYS', '스마일클럽', '1/26~27 쓱배송DAYS', '할인에 할인을 더하다', '쓱배송DAYS', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '오늘은 장보는 날 쓱배송 특가상품 바로보기', '1. 쓱배송, 새벽배송 모두 쓸 수 있는 10% 장보기 쿠폰', '이마트, 트레이더스 쓱배송 및 점포택배/새벽배송', '10% 장바구니 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1일 1매 (오전 9시 오픈, 선착순 2만명)', '10% 장바구니 쿠폰 - 8만원 이상 결제시 최대 2만원 할인 ID당 1일 1매 (오전 9시 오픈, 선착순 5천명, smile club 전용)', '스마일클럽 전용 쿠폰 받기', '       쿠폰발급 및 사용 기간', '       2023년 1월 26일/27일 양일간 (*당일 발급된 쿠폰은 당일 한정 사용가능)', '       쿠폰 발급 및 사용일', '       23년 1월 26일/27일 양일간 (기간 중 ID당 1일 1회 다운가능, 발급된 쿠폰 당일 한정 사용 가능)', '       쿠폰 사용조건', '       대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '       쿠폰 발급 대상', '       스마일클럽 전용 2만원 할인 장바구니 쿠폰 : 스마일클럽 멤버십 가입 회원 전용 (두 쿠폰 모두 이메일주소, SNS 등으로 가입된 간편회원은 제외됩니다)', '       쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '+ 결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', '[SSGPAY 전용]삼성카드 최대 5만원 5% 청구할인 자세히 보기', '3. 오늘은 장보는 날! 쓱배송데이 장보기 특가상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품', '신세계상품권을 SSG MONEY로 전환하고 SSG.COM에서 쇼핑하세요 바로 가기']</t>
+          <t>['이벤트/쿠폰 &gt; 행운의 쓱세일을 잡아라!', '스마일클럽', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기됩니다.']</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 쇼핑 버킷리스트', '스마일클럽', '올해 첫 합리적 소비를 위한 장바구니쿠폰 2종', '장바구니쿠폰 10% 15만원 이상 최대 3만원', '장바구니쿠폰 7% 10만원 이상 최대 1만원', '쿠폰은 25일 10시에 오픈됩니다.', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[공식] 윈터 세일 최대 50% &amp; 베스트 상품 제안', '★레드하트★한정수량★맨투맨/니트 +)즉시할인쿠폰 바로적용', '★SSG x 템퍼★ 덴마크 프리미엄 TEMPUR ~베개/매트리스 ~30% OFF', '[자라홈] 이불, 쿠션, 러그 등 : 최대 60%할인', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '[즉시할인+카드혜택+사은품 4종] 삼성 갤럭시 워치4  모음', 'SSGX불리 최대 단독 증정 혜택~15%', '안티에이징&amp;기미잡티케어 ~50% 7만이상 구매시 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', '신년맞이 [SSG X 일동제약 퍼스트랩 ] 10종 스킨&amp;헤어케어 ~80%SALE!', '명절 연휴에 추천하는 향수 할인전 / 바이레도, 톰포드, 조말론 외', '트와이스 지효PICK  V리프팅 괄사 + 진정크림 UP TO 37% +무료배송', '♥시즌오프♥FW 인기 아이템 최대 52% OFF', '[에고이스트/랩/플라스틱아일랜드] ~70% OFF! 윈터 클리어런스 외 인기 아이템 쇼핑 위크', '[캠브리지] X SSG 아놀 단독 할인 + best 아이템 UP TO 40% OFF', '★어그 베스트셀러 ~40% 세일★', '[CARLYN]23SS 푸퍼 출시!♥신상&amp;베스트 최대 76% SALE + 추가 쿠폰 혜택까지!', '블랙야크/디스커버리 外 인기브랜드 다운/패딩 ~70% OFF', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[아식스 본사] 최대 82% OFF 다운부터 런닝화까지 베스트템 모음전', '투어360 골프화 50%할인', '[자라홈] 키즈용품, 장난감, 인형 등 : 최대 60%할인', '레고 클리어런스 특가! ★최대 40%할인★ (~2/1일까지)']</t>
+          <t>['이벤트/쿠폰 &gt; 2023 쇼핑 버킷리스트', '스마일클럽', '올해 첫 합리적 소비를 위한 장바구니쿠폰 2종', '장바구니쿠폰 10% 15만원 이상 최대 3만원', '장바구니쿠폰 7% 10만원 이상 최대 1만원', '쿠폰은 25일 10시에 오픈됩니다.', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[LUXURY 가방 BEST 50] 떠오르는 명품 브랜드 자크뮈스/미우미우 外 50종 자체할인 + 추가쿠폰!', '[공식] 윈터 세일 최대 50% &amp; 베스트 상품 제안', '★레드하트★한정수량★맨투맨/니트 +)즉시할인쿠폰 바로적용', '★SSG x 템퍼★ 덴마크 프리미엄 TEMPUR ~베개/매트리스 ~30% OFF', '[자라홈] 이불, 쿠션, 러그 등 : 최대 60%할인', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '[즉시할인+카드혜택+사은품 4종] 삼성 갤럭시 워치4  모음', 'SSGX불리 최대 단독 증정 혜택~15%', '안티에이징&amp;기미잡티케어 ~50% 7만이상 구매시 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', '신년맞이 [SSG X 일동제약 퍼스트랩 ] 10종 스킨&amp;헤어케어 ~80%SALE!', '명절 연휴에 추천하는 향수 할인전 / 바이레도, 톰포드, 조말론 외', '트와이스 지효PICK  V리프팅 괄사 + 진정크림 UP TO 37% +무료배송', '♥시즌오프♥FW 인기 아이템 최대 52% OFF', '[에고이스트/랩/플라스틱아일랜드] ~70% OFF! 윈터 클리어런스 외 인기 아이템 쇼핑 위크', '[캠브리지] X SSG 아놀 단독 할인 + best 아이템 UP TO 40% OFF', '★어그 베스트셀러 ~40% 세일★', '[CARLYN]23SS 푸퍼 출시!♥신상&amp;베스트 최대 76% SALE + 추가 쿠폰 혜택까지!', '블랙야크/디스커버리 外 인기브랜드 다운/패딩 ~70% OFF', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[아식스 본사] 최대 82% OFF 다운부터 런닝화까지 베스트템 모음전', '투어360 골프화 50%할인', '[자라홈] 키즈용품, 장난감, 인형 등 : 최대 60%할인', '레고 클리어런스 특가! ★최대 40%할인★ (~2/1일까지)']</t>
         </is>
       </c>
     </row>
@@ -577,81 +577,81 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/26~2/1) 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '한정수량! 오늘만! 단 하루 타임딜 바로보기', '최대 50%할인, 1+1, 사은품증정 블라썸관 행사상품/이벤트 바로보기', '한정수량! 오늘만! 단 하루 타임딜', '(오늘 단 하루, 1+1) CJ 비비고 특양지곰탕/특설렁탕 700G : 할인전 14,900원 할인후 개당 7,450원~', '(오늘 단 하루, 50%) 대상 포도씨유 900ml : 할인전 16,900원 할인후 8,450원', '(오늘 단 하루, 1+1) 풀무원 풀무원 모짜렐라 핫도그 5입 : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 31%, 1+1) LG생활건강 테크 실내건조 세탁세제3L : 할인전 15,900원 할인후 개당 5,450원', '(오늘 단 하루, 한정수량 체럼, 41%) 아모레퍼시픽 (체험팩) 스킨유 이노센트 샤워젤/로션 라보에이치 샴푸 : 할인전 4,900원 할인후 2,900원', '(오늘 단 하루, 40%) CJ 헷반 현미/흑미 귀리 곤약밥 150G*12개 : 할인전 35,760원 할인후 21,500원', '(오늘 단 하루, 1+1) CJ 백설 파스타 소스 4종 : 할인전 5,500원 할인후 개당 2,790원 ~', '(오늘 단 하루, 1+1) 풀무원 들기름을 섞어 바삭바삭 고소하게 구워낸 재래김 80g (5g*16) : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 1+1) 풀무원 풀무원 동물복지 수비드 닭가슴살 1150G 3종 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 45%) 아모레퍼시픽 LG생활건강 퍼퓸스튜디오 1L 플로라피치 : 할인전 8,900원 할인후 4,900원', '(오늘 단 하루, 1+1) 대상 청정원 드레싱 2종 : 할인전 3,600원 할인후 개당 1,800원', '(오늘 단 하루, 한정수량, 18%) 매일유업 상하치킨 브리또 6입 : 할인전 20,000원 할인후 16,500원', '(오늘 단 하루, 33%) 풀무원 풀무원 행복한 동물복지유정란 15구 780g : 할인전 8,980원 할인후 5,980원', '(오늘 단 하루, 30%, 한정수량) LG생활건강 피이조겔 지코의 NO.1보습크립 세트 : 할인전 59,800원 할인후 41,860원', '(오늘 단 하루, 60%, 한정수량) 아모레퍼시픽 려 더블이펙터 블랙 샴푸/트리트먼트 543ML : 할인전 39,000원 할인후 15,600원', '(오늘 단 하루, 1+1) 우리동네 떡볶이/고소한 유부초밥 330G : 할인전 4,900원 할인후 개당 2,980원~', '(오늘 단 하루, 1+1) CJ 비비고 진국육수 닭고기/소고기양지 500g : 할인전 3,080원 할인후 개당 1,540원', '(오늘 단 하루, 44%, 한정수량) 매일유업 셀렉스 프로핏 웨ㅐ이프로틴 드링크 초콜릿 2박스 : 할인전 69.900원 할인후 38,900원', '(오늘 단 하루, 1+1) LG생활건강 엘라스틴 5X 샴푸/트리트먼트 : 할인전 16,900원 할인후 개당 8,450원', '(오늘 단 하루, 1+1) LG생활건강 히말라야 핑크솔트 치약 100g*3_아이스카밍 : 할인전 14,900원 할인후 개당 7,450원', '(오늘 단 하루, 1+1) CJ 비비고 사골시래기된장국 460g : 할인전 5,480원 할인후 개당 2,740원', '(오늘 단 하루, 1+1) 풀무원 자연은맛있다 건면 4종 : 할인전 5,450원 할인후 개당 2,725원', '(오늘 단 하루, 1+1) 풀무원 요리육수 3종 1000ML : 할인전 3,980원 할인후 개당 1,990원', '(오늘 단 하루, 2개 구매 시 50%) 유한킴벌리 크리넥스 디럭스미니 카카오230매6입 : 할인전 12,700원 할인후 개당 6,350원', '(오늘 단 하루, 62%, 한정수량) LG생활건강 실크테라피 인리처드 액션 60ML X 4개 : 할인전 79,600원 할인후 29,900원', '(오늘 단 하루, 1+1) CJ 백설 스파게티소스 640G 2종 : 할인전 4,380원 할인후 개당 2,190원', '(오늘 단 하루, 18%, 한정수량) 매일유업 마이카페라떼 마일드로어슈거 220ml 10팩 : 할인전 14,500원 할인후 11,900원', '(오늘 단 하루, 25%, 한정수량) 아모레퍼시픽 일리윤 세라마이드 아토로션/울트라리페어로션 + 일리윤 로션 : 할인전 24,500원 할인후 18,743원', '(오늘 단 하루, 50%, 한정수량) 유한킴벌리 좋은느낌 유기농순면 내추럴코어 슬날대 14X6 : 할인전 35,900원 할인후 17,950원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 그린핑거 판테딘 더마 밴드/팬티 기저귀 : 할인전 30,450원 할인후 개당 15,225원~', '(오늘 단 하루, 1+1) 풀무원 다논 요거톡125G*4입 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 31%, 한정수량) 매일유업 셀렉스 코어프로틴 음료 오리지널 2박스 : 할인전 58,000원 할인후 39,900원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 크리넥스 안심 프리미엄 3겹 키친타올 140매x4롤 : 할인전 9,200원 할인후 개당 4,600원', '(오늘 단 하루, 52%, 한정수량) LG생활건강 세이프 뿌리는 레몬식초 400ml x 3개 : 할인전 22,500원 할인후 10,900원', '(오늘 단 하루, 한정수량 체험, 64%) 아모레퍼시픽 롱테이크 샌달우드 인텐시브 3종 KIT : 할인전 10,800원 할인후 3,900원', '최대 50%할인 / 1+1 / 다다익선 / 사은품증정', '블라썸관 행사상품 및 이벤트', '블라썸관 좋아요 누르면 5% 할인쿠폰', '최대 50% 할인 행사상품', '※ 자세한 내용은 상품 상세페이지 내 이벤트내용을 참고해주세요.', '최대 50%할인 행사상품', '블라썸관 좋아요 누르면 10% 할인쿠폰', '최대 50%할인 행사상품, 기획상품', '최대 50%할인, 1+1 행사상품', '최대 30%할인, 1+1 행사상품', '3만원 이상 구매고객 스타벅스 아메리카노 증정(선착순 1천명)', '최대 30%할인, 1+1 행사상품, SSG단독 상품', '구매왕 응모이벤트 : 1등 건조기(1명), 2등 스타벅스 아메리카노(100명)']</t>
+          <t>['이벤트/쿠폰 &gt; (1/26~2/1) 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '한정수량! 오늘만! 단 하루 타임딜 바로보기', '최대 50%할인, 1+1, 사은품증정 블라썸관 행사상품/이벤트 바로보기', '한정수량! 오늘만! 단 하루 타임딜', '(오늘 단 하루, 1+1) CJ 비비고 특양지곰탕/특설렁탕 700G : 할인전 14,900원 할인후 개당 7,450원~', '(오늘 단 하루, 50%) 대상 포도씨유 900ml : 할인전 16,900원 할인후 8,450원', '(오늘 단 하루, 1+1) 풀무원 풀무원 모짜렐라 핫도그 5입 : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 31%, 1+1) LG생활건강 테크 실내건조 세탁세제3L : 할인전 15,900원 할인후 개당 5,450원', '(오늘 단 하루, 한정수량 체럼, 41%) 아모레퍼시픽 (체험팩) 스킨유 이노센트 샤워젤/로션 라보에이치 샴푸 : 할인전 4,900원 할인후 2,900원', '(오늘 단 하루, 40%) CJ 헷반 현미/흑미 귀리 곤약밥 150G*12개 : 할인전 35,760원 할인후 21,500원', '(오늘 단 하루, 1+1) CJ 백설 파스타 소스 4종 : 할인전 5,500원 할인후 개당 2,790원 ~', '(오늘 단 하루, 1+1) 풀무원 들기름을 섞어 바삭바삭 고소하게 구워낸 재래김 80g (5g*16) : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 1+1) 풀무원 풀무원 동물복지 수비드 닭가슴살 1150G 3종 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 22%) LG생활건강 퍼퓸스튜디오 1L 플로라피치 : 할인전 8,900원 할인후 6,900원', '(오늘 단 하루, 1+1) 대상 청정원 드레싱 2종 : 할인전 3,600원 할인후 개당 1,800원', '(오늘 단 하루, 한정수량, 18%) 매일유업 상하치킨 브리또 6입 : 할인전 20,000원 할인후 16,500원', '(오늘 단 하루, 33%) 풀무원 풀무원 행복한 동물복지유정란 15구 780g : 할인전 8,980원 할인후 5,980원', '(오늘 단 하루, 30%, 한정수량) LG생활건강 피이조겔 지코의 NO.1보습크립 세트 : 할인전 59,800원 할인후 41,860원', '(오늘 단 하루, 60%, 한정수량) 아모레퍼시픽 려 더블이펙터 블랙 샴푸/트리트먼트 543ML : 할인전 39,000원 할인후 15,600원', '(오늘 단 하루, 1+1) 우리동네 떡볶이/고소한 유부초밥 330G : 할인전 4,900원 할인후 개당 2,980원~', '(오늘 단 하루, 1+1) CJ 비비고 진국육수 닭고기/소고기양지 500g : 할인전 3,080원 할인후 개당 1,540원', '(오늘 단 하루, 44%, 한정수량) 매일유업 셀렉스 프로핏 웨ㅐ이프로틴 드링크 초콜릿 2박스 : 할인전 69.900원 할인후 38,900원', '(오늘 단 하루, 1+1) LG생활건강 엘라스틴 5X 샴푸/트리트먼트 : 할인전 16,900원 할인후 개당 8,450원', '(오늘 단 하루, 1+1) LG생활건강 히말라야 핑크솔트 치약 100g*3_아이스카밍 : 할인전 14,900원 할인후 개당 7,450원', '(오늘 단 하루, 1+1) CJ 비비고 사골시래기된장국 460g : 할인전 5,480원 할인후 개당 2,740원', '(오늘 단 하루, 1+1) 풀무원 자연은맛있다 건면 4종 : 할인전 5,450원 할인후 개당 2,725원', '(오늘 단 하루, 1+1) 풀무원 요리육수 3종 1000ML : 할인전 3,980원 할인후 개당 1,990원', '(오늘 단 하루, 2개 구매 시 50%) 유한킴벌리 크리넥스 디럭스미니 카카오230매6입 : 할인전 12,700원 할인후 개당 6,350원', '(오늘 단 하루, 65%, 한정수량) LG생활건강 실크테라피 인리처드 액션 60ML X 4개 : 할인전 79,600원 할인후 27,900원', '(오늘 단 하루, 1+1) CJ 백설 스파게티소스 640G 2종 : 할인전 4,380원 할인후 개당 2,190원', '(오늘 단 하루, 18%, 한정수량) 매일유업 마이카페라떼 마일드로어슈거 220ml 10팩 : 할인전 14,500원 할인후 11,900원', '(오늘 단 하루, 53%, 한정수량) 아모레퍼시픽 일리윤 세라마이드 아토로션/울트라리페어로션 + 일리윤 로션 : 할인전 39,900원 할인후 18,810원', '(오늘 단 하루, 두개 구매 시, 50%, 한정수량) 유한킴벌리 좋은느낌 유기농순면 내추럴코어 슬날대 14X6 : 할인전 38,500원 할인후 19,250원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 그린핑거 판테딘 더마 밴드/팬티 기저귀 : 할인전 30,450원 할인후 개당 15,225원~', '(오늘 단 하루, 1+1) 풀무원 다논 요거톡125G*4입 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 31%, 한정수량) 매일유업 셀렉스 코어프로틴 음료 오리지널 2박스 : 할인전 58,000원 할인후 39,900원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 크리넥스 안심 프리미엄 3겹 키친타올 140매x4롤 : 할인전 9,200원 할인후 개당 4,600원', '(오늘 단 하루, 52%, 한정수량) LG생활건강 세이프 뿌리는 레몬식초 400ml x 3개 : 할인전 22,500원 할인후 10,900원', '(오늘 단 하루, 한정수량 체험, 64%) 아모레퍼시픽 롱테이크 샌달우드 인텐시브 3종 KIT : 할인전 10,800원 할인후 3,900원', '최대 50%할인 / 1+1 / 다다익선 / 사은품증정', '블라썸관 행사상품 및 이벤트', '최대 50% 할인 행사상품', '※ 자세한 내용은 블라썸관 및 상품상세페이지 내 이벤트내용을 참고해주세요.', '최대 50%할인 행사상품', '최대 50%할인 행사상품, 기획상품', '최대 50%할인, 1+1 행사상품', "'대상'브랜드 상품 3만 5천원 이상 구매 시 5천원 즉시할인(일부 상품 제외)", '최대 30%할인, 1+1 행사상품', '3만원 이상 구매고객 스타벅스 아메리카노 증정(선착순 1천명)', '최대 30%할인, 1+1 행사상품, SSG단독 상품', '구매왕 응모이벤트 : 1등 건조기(1명), 2등 스타벅스 아메리카노(100명)', '※ 자세한 내용은 상품 상세페이지 내 이벤트내용을 참고해주세요.']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', '쿠폰 발급기간 : 2022.12.01 ~ 2022.12.31', '쿠폰 사용기간 : 2022.12.01 ~ 2022.12.31', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
@@ -806,74 +806,111 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>신일전자 1/26(목) 8PM</t>
+          <t>첫 구매 고객 스페셜 혜택</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>신일 팬히터 1200 아이보리 선착순 핫딜 39만원대 + 전고객 캠핑용 전기그릴 증정</t>
+          <t>메가박스 영화 관람권 5,900원</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003983</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>신일 팬히터 선착순 핫딜 39만원대 @SSG.LIVE 1/26(목) 8PM</t>
+          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2023-01-27</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2023-02-02</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신일 팬히터 선착순 핫딜 39만원대 @SSG.LIVE 1/26(목) 8PM', '스마일클럽', '신일 팬히터 선착순 핫딜 39만원대 @SSG.LIVE 1/26(목) 8PM']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 2일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>피코크 1/27(금) 11AM</t>
+          <t>스테디셀러 명품 1/30(월) 8PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>요리가 제일 귀찮을 명절 직후, 피코크 간식/간편식 최대 52%</t>
+          <t>생로랑/보테가베네타/발렌시아가 外 물량 확보! 한정수량 핫딜 혜택</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003986</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004020</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>피코크 @SSG.LIVE 1/27(금) 11:00</t>
+          <t>[SSG.LIVE]스테디셀러 명품 특집</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-01-17</t>
+          <t>2023-01-23</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-01-27</t>
+          <t>2023-01-30</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 피코크 @SSG.LIVE 1/27(금) 11:00', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]스테디셀러 명품 특집', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>그리스/튀르키예(터키) 여행 1/31(목) 8PM</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[SSG단독 전일정 균일가] 18만원 혜택포함! 그리스/튀르키예(터키) 10일 최저가 120만원대~</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004022</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>튀르키예(터키) 여행 패키지 @SSG.LIVE 1/31(화) 8PM</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-01-18</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-01-31</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 튀르키예(터키) 여행 패키지 @SSG.LIVE 1/31(화) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Feb  2 00:21:24 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,81 +510,81 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023 쇼핑 버킷리스트</t>
+          <t xml:space="preserve">첫구매는 반값다~딜 </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 3만원 할인쿠폰 제공</t>
+          <t>첫구매는 세 개 골라 다~반값 + 무료배송</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003961</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004059&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023 쇼핑 버킷리스트</t>
+          <t>반값다딜 - CJ편 (2/1~8)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-02-08</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2023 쇼핑 버킷리스트', '스마일클럽', '올해 첫 합리적 소비를 위한 장바구니쿠폰 2종', '장바구니쿠폰 10% 15만원 이상 최대 3만원', '장바구니쿠폰 7% 10만원 이상 최대 1만원', '쿠폰은 25일 10시에 오픈됩니다.', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[LUXURY 가방 BEST 50] 떠오르는 명품 브랜드 자크뮈스/미우미우 外 50종 자체할인 + 추가쿠폰!', '[공식] 윈터 세일 최대 50% &amp; 베스트 상품 제안', '★레드하트★한정수량★맨투맨/니트 +)즉시할인쿠폰 바로적용', '★SSG x 템퍼★ 덴마크 프리미엄 TEMPUR ~베개/매트리스 ~30% OFF', '[자라홈] 이불, 쿠션, 러그 등 : 최대 60%할인', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '[즉시할인+카드혜택+사은품 4종] 삼성 갤럭시 워치4  모음', 'SSGX불리 최대 단독 증정 혜택~15%', '안티에이징&amp;기미잡티케어 ~50% 7만이상 구매시 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', '신년맞이 [SSG X 일동제약 퍼스트랩 ] 10종 스킨&amp;헤어케어 ~80%SALE!', '명절 연휴에 추천하는 향수 할인전 / 바이레도, 톰포드, 조말론 외', '트와이스 지효PICK  V리프팅 괄사 + 진정크림 UP TO 37% +무료배송', '♥시즌오프♥FW 인기 아이템 최대 52% OFF', '[에고이스트/랩/플라스틱아일랜드] ~70% OFF! 윈터 클리어런스 외 인기 아이템 쇼핑 위크', '[캠브리지] X SSG 아놀 단독 할인 + best 아이템 UP TO 40% OFF', '★어그 베스트셀러 ~40% 세일★', '[CARLYN]23SS 푸퍼 출시!♥신상&amp;베스트 최대 76% SALE + 추가 쿠폰 혜택까지!', '블랙야크/디스커버리 外 인기브랜드 다운/패딩 ~70% OFF', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[아식스 본사] 최대 82% OFF 다운부터 런닝화까지 베스트템 모음전', '투어360 골프화 50%할인', '[자라홈] 키즈용품, 장난감, 인형 등 : 최대 60%할인', '레고 클리어런스 특가! ★최대 40%할인★ (~2/1일까지)']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다딜 - CJ편 (2/1~8)', '스마일클럽', '첫구매 전용 프로모션', '50% 할인 쿠폰, 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'cj상품 50% 할인 쿠폰 &amp; 첫구매 무료배송 쿠폰', ' 최대 할인 금액 각 5천원 ', '         쿠폰 발급 기간', '         쿠폰 발급 대상', '         2022년 1월 31일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매 이력이 없는 고객 한정', '         상품 할인 쿠폰 적용 방법', '         본 페이지 내 전시된 CJ브랜드 상품 중 3개를 골라 결제 단계에서 쿠폰 적용 (상품당 1개 수량 적용)', '         20,000원 이상 구매시 사용 가능', '         무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 사용 기간', '       상품할인쿠폰/무료배송 쿠폰 : 2023년 2/1(수) ~ 2/8(수) 행사 기간 내 사용', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 총 3장, 할인 적용 가능 상품들에 한해 50% 할인(상품당 최대할인금액 적용)', '       무료배송 쿠폰 : 총 1장, 이마트몰 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       상품당 1개 수량에 쿠폰 적용 가능하며, 동일한 상품 2개 구매시에도 1개에만 적용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>블라썸 위크</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인, 1+1</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004037</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(1/26~2/1) 블라썸위크</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (1/26~2/1) 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '한정수량! 오늘만! 단 하루 타임딜 바로보기', '최대 50%할인, 1+1, 사은품증정 블라썸관 행사상품/이벤트 바로보기', '한정수량! 오늘만! 단 하루 타임딜', '(오늘 단 하루, 1+1) CJ 비비고 특양지곰탕/특설렁탕 700G : 할인전 14,900원 할인후 개당 7,450원~', '(오늘 단 하루, 50%) 대상 포도씨유 900ml : 할인전 16,900원 할인후 8,450원', '(오늘 단 하루, 1+1) 풀무원 풀무원 모짜렐라 핫도그 5입 : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 31%, 1+1) LG생활건강 테크 실내건조 세탁세제3L : 할인전 15,900원 할인후 개당 5,450원', '(오늘 단 하루, 한정수량 체럼, 41%) 아모레퍼시픽 (체험팩) 스킨유 이노센트 샤워젤/로션 라보에이치 샴푸 : 할인전 4,900원 할인후 2,900원', '(오늘 단 하루, 40%) CJ 헷반 현미/흑미 귀리 곤약밥 150G*12개 : 할인전 35,760원 할인후 21,500원', '(오늘 단 하루, 1+1) CJ 백설 파스타 소스 4종 : 할인전 5,500원 할인후 개당 2,790원 ~', '(오늘 단 하루, 1+1) 풀무원 들기름을 섞어 바삭바삭 고소하게 구워낸 재래김 80g (5g*16) : 할인전 8,480원 할인후 개당 4,240원~', '(오늘 단 하루, 1+1) 풀무원 풀무원 동물복지 수비드 닭가슴살 1150G 3종 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 22%) LG생활건강 퍼퓸스튜디오 1L 플로라피치 : 할인전 8,900원 할인후 6,900원', '(오늘 단 하루, 1+1) 대상 청정원 드레싱 2종 : 할인전 3,600원 할인후 개당 1,800원', '(오늘 단 하루, 한정수량, 18%) 매일유업 상하치킨 브리또 6입 : 할인전 20,000원 할인후 16,500원', '(오늘 단 하루, 33%) 풀무원 풀무원 행복한 동물복지유정란 15구 780g : 할인전 8,980원 할인후 5,980원', '(오늘 단 하루, 30%, 한정수량) LG생활건강 피이조겔 지코의 NO.1보습크립 세트 : 할인전 59,800원 할인후 41,860원', '(오늘 단 하루, 60%, 한정수량) 아모레퍼시픽 려 더블이펙터 블랙 샴푸/트리트먼트 543ML : 할인전 39,000원 할인후 15,600원', '(오늘 단 하루, 1+1) 우리동네 떡볶이/고소한 유부초밥 330G : 할인전 4,900원 할인후 개당 2,980원~', '(오늘 단 하루, 1+1) CJ 비비고 진국육수 닭고기/소고기양지 500g : 할인전 3,080원 할인후 개당 1,540원', '(오늘 단 하루, 44%, 한정수량) 매일유업 셀렉스 프로핏 웨ㅐ이프로틴 드링크 초콜릿 2박스 : 할인전 69.900원 할인후 38,900원', '(오늘 단 하루, 1+1) LG생활건강 엘라스틴 5X 샴푸/트리트먼트 : 할인전 16,900원 할인후 개당 8,450원', '(오늘 단 하루, 1+1) LG생활건강 히말라야 핑크솔트 치약 100g*3_아이스카밍 : 할인전 14,900원 할인후 개당 7,450원', '(오늘 단 하루, 1+1) CJ 비비고 사골시래기된장국 460g : 할인전 5,480원 할인후 개당 2,740원', '(오늘 단 하루, 1+1) 풀무원 자연은맛있다 건면 4종 : 할인전 5,450원 할인후 개당 2,725원', '(오늘 단 하루, 1+1) 풀무원 요리육수 3종 1000ML : 할인전 3,980원 할인후 개당 1,990원', '(오늘 단 하루, 2개 구매 시 50%) 유한킴벌리 크리넥스 디럭스미니 카카오230매6입 : 할인전 12,700원 할인후 개당 6,350원', '(오늘 단 하루, 65%, 한정수량) LG생활건강 실크테라피 인리처드 액션 60ML X 4개 : 할인전 79,600원 할인후 27,900원', '(오늘 단 하루, 1+1) CJ 백설 스파게티소스 640G 2종 : 할인전 4,380원 할인후 개당 2,190원', '(오늘 단 하루, 18%, 한정수량) 매일유업 마이카페라떼 마일드로어슈거 220ml 10팩 : 할인전 14,500원 할인후 11,900원', '(오늘 단 하루, 53%, 한정수량) 아모레퍼시픽 일리윤 세라마이드 아토로션/울트라리페어로션 + 일리윤 로션 : 할인전 39,900원 할인후 18,810원', '(오늘 단 하루, 두개 구매 시, 50%, 한정수량) 유한킴벌리 좋은느낌 유기농순면 내추럴코어 슬날대 14X6 : 할인전 38,500원 할인후 19,250원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 그린핑거 판테딘 더마 밴드/팬티 기저귀 : 할인전 30,450원 할인후 개당 15,225원~', '(오늘 단 하루, 1+1) 풀무원 다논 요거톡125G*4입 : 할인전 3,480원 할인후 개당 1,740원', '(오늘 단 하루, 31%, 한정수량) 매일유업 셀렉스 코어프로틴 음료 오리지널 2박스 : 할인전 58,000원 할인후 39,900원', '(오늘 단 하루, 2개 구매 시, 50%) 유한킴벌리 크리넥스 안심 프리미엄 3겹 키친타올 140매x4롤 : 할인전 9,200원 할인후 개당 4,600원', '(오늘 단 하루, 52%, 한정수량) LG생활건강 세이프 뿌리는 레몬식초 400ml x 3개 : 할인전 22,500원 할인후 10,900원', '(오늘 단 하루, 한정수량 체험, 64%) 아모레퍼시픽 롱테이크 샌달우드 인텐시브 3종 KIT : 할인전 10,800원 할인후 3,900원', '최대 50%할인 / 1+1 / 다다익선 / 사은품증정', '블라썸관 행사상품 및 이벤트', '최대 50% 할인 행사상품', '※ 자세한 내용은 블라썸관 및 상품상세페이지 내 이벤트내용을 참고해주세요.', '최대 50%할인 행사상품', '최대 50%할인 행사상품, 기획상품', '최대 50%할인, 1+1 행사상품', "'대상'브랜드 상품 3만 5천원 이상 구매 시 5천원 즉시할인(일부 상품 제외)", '최대 30%할인, 1+1 행사상품', '3만원 이상 구매고객 스타벅스 아메리카노 증정(선착순 1천명)', '최대 30%할인, 1+1 행사상품, SSG단독 상품', '구매왕 응모이벤트 : 1등 건조기(1명), 2등 스타벅스 아메리카노(100명)', '※ 자세한 내용은 상품 상세페이지 내 이벤트내용을 참고해주세요.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -614,177 +614,177 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 7월 1일 부터 2022년 12월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '* 쿠폰할인, 적립금 사용 등 선할인을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>스마일클럽 웰컴 5천원 쿠폰</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>2월의신규가입혜택</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만원 이상 결제 시 사용 가능한 4만 5천원 할인쿠폰 제공', '45,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.01.01 ~ 2023.01.31', '쿠폰 사용기간 : 2023.01.01 ~ 2023.01.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 50,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 고객이라면 9% 장바구니 쿠폰', 'SSG.COM 삼성카드로 100,000원 이상 결제 시 사용 가능(아이디당 1회, 할인한도 20,000원)', 'SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 100,000원 이상이여야 쿠폰을 사용할 수 있습니다.', '쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경할 수 있 습니다.', '현금성 상품, 무형서비스 상품, 초특가 상품 등 일부 상품은 제외됩니다.(쿠폰 적용 제외 상품은 결제 화면에서 쿠폰이 보이지 않음)', '04. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '(1)행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>쓱배송의 세계로 초대합니다</t>
+          <t>첫 구매 고객 스페셜 혜택</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>첫 구매 쿠폰 받고, 친구 초대하면 혜택이 두 배</t>
+          <t>메가박스 영화 관람권 5,900원</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003900</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1월 쓱배송 친구 초대 이벤트</t>
+          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2023-01-27</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 1월 쓱배송 친구 초대 이벤트', '스마일클럽', '1월 쓱배송 친구 초대 이벤트', '5천원 할인에 무료배송', '친구 초대 이벤트', '쓱배송이 처음이라면? 할인에 무료배송', '쓱배송 웰컴 쿠폰', '5,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '이마트몰, 쓱배송/새벽배송 20,000원 이상 구매시 사용 가능', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 2022년 1월 18일 이후 이마트몰, 트레이더스 쓱배송/점포 택배 및 새벽배송 구매 이력이 없는 고객 ', '쿠폰 사용 조건 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매 시 사용 가능', '이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 세가지 배송 모두 한 번도 해본 적 없는 친구에게 나의 초대장 번호를 공유해주세요', '응모 이후 초대받은 친구가 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', 'SSG MONEY 적립 이후 초대받은 친구가 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '본인 스스로 초대한 경우에는 이벤트 참여에서 제외됩니다.', "친구가 전달 준 초대장 번호를 입력하고 '첫 쓱배송 응모하기' 버튼을 눌러주세요 응모 이후, 반드시 이벤트 기간 내 첫 쓱배송 구매를 완료해야만 SSG MONEY가 정상 적립됩니다.", '첫 쓱배송 응모하기', '이벤트 응모여부 확인하기', 'STEP2 첫 쓱배송 배송 주문하기 : 쓱배송 or 쓱배송TRADERS or 새벽배송(* 주문시, 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'STEP3 SSG MONEY적립 : 이벤트 종료 후 2월 10일(금) 이내 SSG MONEY가 일괄 적립됩니다.', '응모 이후 이벤트 기간 내 "쓱배송" 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 - 첫 구매 배송 완료 시점)', '쓱배송이 아닌 다른 배송 유형으로 구매했을 시, 참여 인정되지 않습니다. (반드시 쓱배송 혹은 새벽배송 스티커를 확인해주세요)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 SSG MONEY가 회수될 수 있습니다.', '이벤트 기간 :  1월 19일(목) 00:00 ~ 1월 31일(화) 23:59', '최근 1년 간 이마트몰 쓱배송, 트레이더스 쓱배송, 새벽배송 모두 구매 이력이 없는 경우만 쓱배송 첫 구매자로 응모 가능합니다. (2022년 1월 18일 이후 주문 내역이 없는 자)', '이벤트 기간 내 등록할 수 있는 초대자는 한 명입니다.', '본인 스스로 초대/응모한 경우에는 이벤트 참여에서 제외됩니다.', '응모 이후  초대받은 사람이 이벤트 기간 내 쓱배송 첫 구매를 완료해야만 추천인과 초대받은 사람 모두에게 SSG MONEY 5천원이 적립됩니다. (*첫 구매 완료 기준 ? 첫 구매 배송 완료)', 'SSG MONEY 적립 이후 첫 쓱배송 주문을 전체 반품할 경우, 해당 초대 건에 대하여 추천인과 초대받은 사람 모두 SSG MONEY가 회수될 수 있습니다.', '초대 받은 친구가 탈퇴 후 재가입하여 구매를 하더라도 첫 구매로 인정되지 않으며, SSG MONEY가 지급되지 않습니다.', '본 이벤트를 통해 지급된 SSG MONEY는 지급일로부터 30일 이후 자동 소멸됩니다.', '부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 당첨이 취소될 수 있습니다.', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '신세계상품권을 SSG MONEY로 전환하고, SSG.COM에서 쇼핑하세요']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 9일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>스마일클럽 1월의 가입 혜택</t>
+          <t>폴레드 2/2(목) 11:00AM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>WELCOME 5천원 할인쿠폰 제공</t>
+          <t>국민육아핫템! 폴레드 최대79% 역대급 할인</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003449</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004147</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[스마일클럽] 1월 매일매일 스마일</t>
+          <t>폴레드 @SSG.LIVE 2/2(목) 11:00AM</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-30</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-02-02</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 1월 매일매일 스마일', '스마일클럽', '[스마일클럽] 1월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '한달 내내 막강한 스마일클럽 혜택', 'WELCOME 스마일클럽이 처음이라면 첫달 무료 + 5천원 할인 쿠폰 발급 (5,100원 이상 구매 시 사용 가능)', '본 쿠폰은 1/5(목)~1/31(화) 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다. (단, 마케팅 정보 수신을 비동의 하신 경우 안내 발송이 제한됩니다.)', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', 'SSG.COM 카드 Edition2 매월 스마일클럽 가입비 100% 지원', '장 보는 날에도 멤버십은 더 큰 혜택 쓱배송데이 최대 2만원 10% 할인 쿠폰', '2023년 검은 토끼의 해 맞이 건강 프로젝트 스마일클럽 전용 최대 15% 쿠폰으로 건강을 선물해요', '계속해서 이어질 스마일클럽 전용 혜택을 기대해주세요']</t>
+          <t>['이벤트/쿠폰 &gt; 폴레드 @SSG.LIVE 2/2(목) 11:00AM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>쓱스럽게 안녕</t>
+          <t>톰포드뷰티 2/2(목) 7PM</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>See you again, Say Goodbye</t>
+          <t>톰포드뷰티 발렌타인 선물제안 로즈프릭 에디션 긴급공수 &amp; 상품권 증정</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003967</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004083</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>쓱스럽게 안녕</t>
+          <t>톰포드뷰티 @SSG.LIVE 2/2(목) 7PM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-01-17</t>
+          <t>2023-01-26</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2023-02-02</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 쓱스럽게 안녕', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; 톰포드뷰티 @SSG.LIVE 2/2(목) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>민지의 장바구니-겨울 먹거리편</t>
+          <t>웨스틴조선서울 2/2(목) 8PM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+          <t>주중(일-목) 이그제큐티브룸 구매시 클럽라운지 1인 추가 무료</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003980</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003995</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>민지의 장바구니-겨울 먹거리편 (1/26~2/1)</t>
+          <t>웨스틴조선서울 이그제큐티브 핫딜 29만원대부터~ @SSG.LIVE 2/2(목) 8PM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -794,34 +794,34 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-02-02</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-겨울 먹거리편 (1/26~2/1)', '스마일클럽', 'SSG MONEY 1천원 (500명)', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       - ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       - 이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '최대 2만원 할인 10% 장보기 쿠폰 받고 오세요!', '쓱배송데이 보러가기', '신세계몰 상품권을 SSG MONEY로 전환하고 SSG.COM에서 쇼핑하세요']</t>
+          <t>['이벤트/쿠폰 &gt; 웨스틴조선서울 이그제큐티브 핫딜 29만원대부터~ @SSG.LIVE 2/2(목) 8PM', '스마일클럽', '웨스틴조선서울 이그제큐티브 핫딜 29만원대부터~ @SSG.LIVE 2/2(목) 8PM']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>첫 구매 고객 스페셜 혜택</t>
+          <t>빈폴키즈 2/3(금) 11AM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>메가박스 영화 관람권 5,900원</t>
+          <t>우리아이 조카 선물로 딱! / LIVE에서만 책가방 최대 28% 압도적 혜택</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004084</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
+          <t>빈폴키즈 @SSG.LIVE 2/3(금) 11:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -831,86 +831,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2023-02-03</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 2일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>스테디셀러 명품 1/30(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>생로랑/보테가베네타/발렌시아가 外 물량 확보! 한정수량 핫딜 혜택</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004020</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]스테디셀러 명품 특집</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2023-01-23</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2023-01-30</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]스테디셀러 명품 특집', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>그리스/튀르키예(터키) 여행 1/31(목) 8PM</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>[SSG단독 전일정 균일가] 18만원 혜택포함! 그리스/튀르키예(터키) 10일 최저가 120만원대~</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004022</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>튀르키예(터키) 여행 패키지 @SSG.LIVE 1/31(화) 8PM</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2023-01-18</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2023-01-31</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 튀르키예(터키) 여행 패키지 @SSG.LIVE 1/31(화) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 빈폴키즈 @SSG.LIVE 2/3(금) 11:00', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Feb  6 00:20:11 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,170 +473,170 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>역대급 디지털 쇼핑 혜택 COMING SOON</t>
+          <t>디지털 쓱세일 이번주 디지털 최강 혜택!</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>행운의 쓱세일 퀴즈 미리 풀고 스탠바이미/다이슨 경품 도전!</t>
+          <t>디지털 ~15% 쿠폰 + ~8% 청구할인</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003975</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004222</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>행운의 쓱세일을 잡아라!</t>
+          <t>디지털 쓱세일 _ 혜택 페이지</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-01-30</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-02-05</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 행운의 쓱세일을 잡아라!', '스마일클럽', '이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일 _ 혜택 페이지', '스마일클럽', '       디지털 쿠폰 최대 2장', '디지털 쓱세일 최대 10만원 할인', '디지털 대표 브랜드 최대 15% 상품쿠폰', '쿠폰은 9시 부터 발급됩니다', '최대 10만원 할인 쿠폰 다운 받기', '최대 1만원 항린 쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 2월 6일(월) 09시 00분 부터 2월 12일(일) 23시 59분 까지', '본 쿠폰은 신세계몰/이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '디지털 대표 브랜드 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '백화점 디지털 15% 상품쿠폰', '최대 1만원 할인 쿠폰 다운 받기', 'SSG.COM 첫 구매 고객이라면\xa0 선착순 1만원 장바구니 쿠폰까지', '장바구니 쿠폰 1만원 : 3만원 이상 구매시 1만원 할인 (첫 구매 전용, 디지털가전전용, 선착순 3만명, 일부 특가상품 제외)', '쿠폰 마감 되었습니다.', '쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 2월 6일(월) 09시 00분 ~ 2월 12일(일) 23시 59분', '추가 혜택! 카드 청구 할인', '[SSGPAY전용] 신한카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] 삼성카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 현대카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] KB카드 8만원이상 5%, 10만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] KB카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] 현대카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">첫구매는 반값다~딜 </t>
+          <t>디지털 쓱세일 인기 가전 브랜드 총출동</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>첫구매는 세 개 골라 다~반값 + 무료배송</t>
+          <t>애플/삼성 외 TOP 브랜드</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004059&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004223</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>반값다딜 - CJ편 (2/1~8)</t>
+          <t>디지털 쓱세일_브랜드</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-02-08</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다딜 - CJ편 (2/1~8)', '스마일클럽', '첫구매 전용 프로모션', '50% 할인 쿠폰, 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'cj상품 50% 할인 쿠폰 &amp; 첫구매 무료배송 쿠폰', ' 최대 할인 금액 각 5천원 ', '         쿠폰 발급 기간', '         쿠폰 발급 대상', '         2022년 1월 31일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매 이력이 없는 고객 한정', '         상품 할인 쿠폰 적용 방법', '         본 페이지 내 전시된 CJ브랜드 상품 중 3개를 골라 결제 단계에서 쿠폰 적용 (상품당 1개 수량 적용)', '         20,000원 이상 구매시 사용 가능', '         무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 사용 기간', '       상품할인쿠폰/무료배송 쿠폰 : 2023년 2/1(수) ~ 2/8(수) 행사 기간 내 사용', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 총 3장, 할인 적용 가능 상품들에 한해 50% 할인(상품당 최대할인금액 적용)', '       무료배송 쿠폰 : 총 1장, 이마트몰 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       상품당 1개 수량에 쿠폰 적용 가능하며, 동일한 상품 2개 구매시에도 1개에만 적용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일_브랜드', '스마일클럽', '         브라운 9466cc 올인원 패키지 핫딜']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>디지털 쓱세일 매일 오전 10시! 한정수량 타임딜</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>쓱세일 디지털 추천템</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004224</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>디지털 쓱세일_특가</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일_특가', '스마일클럽', '한정수량 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>Romantic Valentine</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>최대 10% 할인쿠폰팩 + BEST GIFT 추천</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004112</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>(0206-12) Romantic Valentine</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; (0206-12) Romantic Valentine', '스마일클럽', '#최대 10% 할인 쿠폰팩 #BEST GIFT ITEM', '발렌타인 전용 10% 할인 쿠폰팩 바로보기', '발렌타인데이 전용 쿠폰 10% 할인 쿠폰팩', '7% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 7만원 이상 구매시 최대 1만원 할인', '10% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 15만원 이상 구매시 최대 2만원 할인', '오늘의 쿠폰은 마감되었습니다.', '       쿠폰 발급 기간', '       23/02/06(월) ~ 23/02/12(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', 'SSG푸드마켓 스윗 발렌타인 위크 - 프리미엄 초콜릿/디저트/커피 다다익선 할인']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+          <t xml:space="preserve">첫구매는 반값다~딜 </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2월의신규가입혜택</t>
+          <t>첫구매는 세 개 골라 다~반값 + 무료배송</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004059&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>반값다딜 - CJ편 (2/1~8)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -646,197 +646,604 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-08</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다딜 - CJ편 (2/1~8)', '스마일클럽', '첫구매 전용 프로모션', '50% 할인 쿠폰, 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'cj상품 50% 할인 쿠폰 &amp; 첫구매 무료배송 쿠폰', ' 최대 할인 금액 각 5천원 ', '         쿠폰 발급 기간', '         쿠폰 발급 대상', '         2022년 1월 31일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매 이력이 없는 고객 한정', '         상품 할인 쿠폰 적용 방법', '         본 페이지 내 전시된 CJ브랜드 상품 중 3개를 골라 결제 단계에서 쿠폰 적용 (상품당 1개 수량 적용)', '         20,000원 이상 구매시 사용 가능', '         무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 사용 기간', '       상품할인쿠폰/무료배송 쿠폰 : 2023년 2/1(수) ~ 2/8(수) 행사 기간 내 사용', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 총 3장, 할인 적용 가능 상품들에 한해 50% 할인(상품당 최대할인금액 적용)', '       무료배송 쿠폰 : 총 1장, 이마트몰 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       상품당 1개 수량에 쿠폰 적용 가능하며, 동일한 상품 2개 구매시에도 1개에만 적용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>첫 구매 고객 스페셜 혜택</t>
+          <t>브랜드 스포트라이트 X 트라이온: 부가부</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>메가박스 영화 관람권 5,900원</t>
+          <t>최대 10% 할인 및 SSGPAY 추가 즉시할인</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004111</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - 부가부</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-01-27</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 9일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 부가부', '스마일클럽', '       1. 부가부 전 상품 5% 상시 할인', '       1. 부가부 스트롤러 및 스타더스트 10% 할인(※폭스 5, 버터플라이 제외)', '       2. 부가부 스트롤러 SSGPAY 카드로 100만원 이상 결제 시, 7만원 즉시할인', '       3. 부가부 폭스 5 구매 시, 선착순 30명 한정 바스타올 증정']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>폴레드 2/2(목) 11:00AM</t>
+          <t>힙슐랭이 제안하는 발렌타인 가이드</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>국민육아핫템! 폴레드 최대79% 역대급 할인</t>
+          <t>15% 할인과 페이백 이벤트</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004147</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004273</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>폴레드 @SSG.LIVE 2/2(목) 11:00AM</t>
+          <t>힙슐랭 : 발렌타인데이편</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-30</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 폴레드 @SSG.LIVE 2/2(목) 11:00AM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 힙슐랭 : 발렌타인데이편', '스마일클럽', '# 최대 15% 할인', '힙슐랭 베스트 상품 최대 15% 할인 행사', '3개 모두 구매 시, 10% 추가 할인!', ' 감각적인 선물 [트리투바] 밀크/화이트 크로캉 세트 6입 : 정상가 23,080원 10%할인가 20,700원 힙슐랭 comment트리투바는 쇼콜라티에 부부가 직접 만든 초콜릿 전문 브랜드로서, 전 세계 카카오 농장을 직접 찾아 맛보고 연구하여 제품을 생산합니다.신선하면서도 맛있는 감각적인 선물로 추천합니다. ', ' 귀여운 선물 [노티드] 옐로우 밀키팜 틴카라멜 : 정상가 13,980원 10%할인가 12,510원 힙슐랭 comment크림 가득 도넛과 시그니처 패키징으로 새로운 트렌드를 만들어가는 노티드가, 이번엔 귀여운 틴케이스에 달콤한 카라멜을 가득 담아 출시했어요. 먹고 남은 틴케이스는 다양한 용도로 활용해보세요. ', ' 색다른 선물 [구아우쇼콜라] 제주 보리개역 파베초콜릿 16구 : 정상가 22,000원 15%할인가 18,700원 힙슐랭 comment제주도 동쪽 항구마을 김녕에 위치한 초콜릿 숍, 구아우쇼콜라에요. 제주 보리개역을 활용해서 색다른 초콜렛을 만들었어요. 보리개역이란, 제주 지역의 보리를 맷돌에 갈아 분말로 만든 가루라 고소한 마무리가 특징입니다.  ', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>톰포드뷰티 2/2(목) 7PM</t>
+          <t>선물은 사랑을 싣고</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>톰포드뷰티 발렌타인 선물제안 로즈프릭 에디션 긴급공수 &amp; 상품권 증정</t>
+          <t>선물한 사연 댓글달고 경품의 행운까지!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004083</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>톰포드뷰티 @SSG.LIVE 2/2(목) 7PM</t>
+          <t>[0202-0226] 선물은 사랑을 싣고</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 톰포드뷰티 @SSG.LIVE 2/2(목) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [0202-0226] 선물은 사랑을 싣고', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일쿠폰', '모바일쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '로맨틱 발렌타인 - 최대 10% 할인쿠폰팩 + BEST GIFT 추천']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>웨스틴조선서울 2/2(목) 8PM</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>주중(일-목) 이그제큐티브룸 구매시 클럽라운지 1인 추가 무료</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003995</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>웨스틴조선서울 이그제큐티브 핫딜 29만원대부터~ @SSG.LIVE 2/2(목) 8PM</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 웨스틴조선서울 이그제큐티브 핫딜 29만원대부터~ @SSG.LIVE 2/2(목) 8PM', '스마일클럽', '웨스틴조선서울 이그제큐티브 핫딜 29만원대부터~ @SSG.LIVE 2/2(목) 8PM']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>빈폴키즈 2/3(금) 11AM</t>
+          <t>미식구매 할인찬스 피코크 위크</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>우리아이 조카 선물로 딱! / LIVE에서만 책가방 최대 28% 압도적 혜택</t>
+          <t>간편하고 맛있는 피코크로 든든한 하루 ~ 30%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004084</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004175&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>빈폴키즈 @SSG.LIVE 2/3(금) 11:00</t>
+          <t>미식체험 할인찬스 피코크 위크</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>2023-02-03</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2023-02-15</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 미식체험 할인찬스 피코크 위크', '스마일클럽', '미식체험 할인찬스 피코크 위크', '최대 50% / 1+1 / 2+1', '~30%/ 2+1 구매찬스', '[피코크] 피콕분식 신당동식떡볶이 970g 신당동 떡볶이를 간편하게 원가 8,480원 &gt; 할인가 5,936원', '[피코크] 한옥집 김치찜 500g 서대문 맛집의 비법을 그대로 원가 7,980원 &gt; 할인가 5,586원', '~30% 할인특가 대표상품', '피코크 자연치즈를 99% 담은 모짜렐라 슈레드치즈 300g(피자치즈)', '피코크 자연치즈를 99% 담은 고다&amp;체다 슈레드치즈 500g(피자치즈)']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>스윗 홈&amp;리빙</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>새로운 시작의 순간, ~3만원 쿠폰과 스윗 홈을 만들어보세요</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004054</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>(2/6~12) Sweet Home&amp;Living</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023-02-12</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; (2/6~12) Sweet Home&amp;Living', '스마일클럽', '최대 3만원 할인!', '장바구니 쿠폰팩', '3종 장바구니 쿠폰팩', '매일 오전 9시 선착순 5천명', '장바구니 3,000원 쿠폰 - 3만원 이상 구매시 3천원 할인', '장바구니 10,000원 쿠폰 - 10만원 이상 구매시 1만원 할인', '장바구니 30,000원 쿠폰 - 30만원 이상 구매시 3만원 할인', '선착순 쿠폰 Soldout!', '쿠폰 발급 및 사용 기간 : 2023년 2월 6일 (월) 00 : 00 ~ 2023년 2월 12일 (일) 23 : 59 ', '쿠폰은 ID당 기간 내 1회 발급 가능하며, 신세계몰 /신세계백화점몰 상품에만 적용됩니다. ', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM  회원만 쿠폰 발급이 가능합니다.', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '신학기 기념 플로라 BEST 침구 특가 ~50% OFF!', '국민 호텔 수건 170g 10장 세트 (리본선물포장) ★SSG몰내 쿠폰확인★', '연인에게 전하는 기프트 ~32%', '[자라홈] 주방용품, 접시, 컵 등 : 최대 60%할인', '50%', '60%', 'UP TO 60% OFF', '20%', 'SNS 감성 란가구, 신학기 초특가 할인전', '17%', '10%', '조명은 비츠조명! 인기상품 할인전']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2월의신규가입혜택</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>첫 구매 고객 스페셜 혜택</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>메가박스 영화 관람권 5,900원</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>2023-01-27</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2023-02-03</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 빈폴키즈 @SSG.LIVE 2/3(금) 11:00', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2023-02-09</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 9일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-10-26</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>시디즈 2/6(월) 7PM</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>신학기 의자 100개 한정 핫딜 + 구매인증 사은품</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004139</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>시디즈 신학기 의자 100개 한정 핫딜~ @SSG.LIVE 2/6(월) 19PM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 시디즈 신학기 의자 100개 한정 핫딜~ @SSG.LIVE 2/6(월) 19PM', '스마일클럽', '시디즈 신학기 의자 100개 한정 핫딜~ @SSG.LIVE 2/6(월) 19PM', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기', '6. 본 이벤트 경품은 브랜드사 상황에 따라 사전 고지 없이 변경, 대체 될 수 있습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>입생로랑 2/6(월) 8PM</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>엉크르드뽀/메쉬핑크 한정판 쿠션 선런칭 핫딜! +브러쉬 3종 추첨!</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004220&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>입생로랑@SSG.LIVE　2/6(월) 20:00PM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-01-31</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2023-02-08</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 입생로랑@SSG.LIVE\u30002/6(월) 20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>LG노트북 2/6(월) 9PM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>13세대 최신형 라이브 한정 ~19% OFF + 추가사은품</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004127</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>LG노트북 @SSG.LIVE 2/6(월) 9PM</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-01-27</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; LG노트북 @SSG.LIVE 2/6(월) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>갤럭시 S23 사전예약 2/7(화) 10AM</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>할인에 조선호텔 식사권/상품권 추첨까지!</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004101&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>삼성 갤럭시S23@SSG.LIVE　2/7(화) 10:00AM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2023-02-09</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 삼성 갤럭시S23@SSG.LIVE\u30002/7(화) 10:00AM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>[디지털쓱세일] LG전자 2/7(화) 7PM</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>LG전자 식기세척기/인덕션/가습기 파격특가+오브제컬렉션 청소기 역대급 핫딜까지</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004170</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>LG전자 가전 @SSG.LIVE 2/7(화) 19:00PM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; LG전자 가전 @SSG.LIVE 2/7(화) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>데스커 2/7(화) 20PM</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>책상세트&amp;모션데스크 세트 ~32% 할인 +사은품부터 라이브 한정 이벤트까지</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004140</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>데스커 책상세트&amp;모션데스크 세트 ~32% 할인 @SSG.LIVE 2/7(화) 20PM</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 데스커 책상세트&amp;모션데스크 세트 ~32% 할인 @SSG.LIVE 2/7(화) 20PM', '스마일클럽', '데스커 책상세트&amp;모션데스크 세트 ~32% 할인 @SSG.LIVE 2/7(화) 20PM']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2월 맘키즈 PLUS</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>지금 할인 중! ~40% 할인 혜택</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>이달의 맘키즈 PLUS</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2022-09-01</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2999-12-13</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '포켓몬 페이스 피규어 12종 세트 (N2쓱배송, 전국택배)', '헬로카봇 펜타스톰X (N2쓱배송, 전국택배)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)', '뽀로로 스마트 쓰기패드(N2 쓱배송, 전국택배)', '얌얌펫 잼하우스스페셜 (N2쓱배송, 전국택배)', '리틀라이브펫 리틀피쉬 어항세트 (N2쓱배송, 전국택배가능)', '/ 올리키즈 유아동침구 특별 할인전★']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Feb  9 00:21:17 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,103 +577,103 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일_특가', '스마일클럽', '한정수량 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일_특가', '스마일클럽', '한정수량 타임딜', '타임딜은 오전 10시에 시작됩니다!', '오늘의 타임딜이 종료되었습니다.', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Romantic Valentine</t>
+          <t>단 하루! 쓱배송데이</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>최대 10% 할인쿠폰팩 + BEST GIFT 추천</t>
+          <t>10% 쿠폰 + 카드 할인까지</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004112</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004247</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(0206-12) Romantic Valentine</t>
+          <t>2/9  단 하루! 쓱배송DAY</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0206-12) Romantic Valentine', '스마일클럽', '#최대 10% 할인 쿠폰팩 #BEST GIFT ITEM', '발렌타인 전용 10% 할인 쿠폰팩 바로보기', '발렌타인데이 전용 쿠폰 10% 할인 쿠폰팩', '7% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 7만원 이상 구매시 최대 1만원 할인', '10% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 15만원 이상 구매시 최대 2만원 할인', '오늘의 쿠폰은 마감되었습니다.', '       쿠폰 발급 기간', '       23/02/06(월) ~ 23/02/12(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', 'SSG푸드마켓 스윗 발렌타인 위크 - 프리미엄 초콜릿/디저트/커피 다다익선 할인']</t>
+          <t>['이벤트/쿠폰 &gt; 2/9  단 하루! 쓱배송DAY', '스마일클럽', '2/9  단 하루! 쓱배송DAY', '할인에 할인을 더하다', '단 하루! 쓱배송 Day', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '오늘은 장보는 날 쓱배송 특가상품 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 쿠폰', '이마트, 트레이더스 쓱배송 및 점포택배/새벽배송', '10% 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1매 (오전 9시 오픈, 선착순 2만명)', '쿠폰발급 및 사용 기간 2023년 2월 9일 (당일 발급된 쿠폰은 당일 한정 사용가능)', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', 'KB국민카드 8만원 이상 5% 청구할인 / 10만원 이상 7% 청구할인', '      쿠폰 발급 및 사용일', '      23년 2월 9일(기간 중 ID당 1일 1회 다운가능) (발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '2 오늘은 장보는 날! 쓱배송데이 장보기 특가상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">첫구매는 반값다~딜 </t>
+          <t>반값다딜</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>첫구매는 세 개 골라 다~반값 + 무료배송</t>
+          <t>상품쿠폰 50% 할인 3장 , 무료배송쿠폰 1장</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004059&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004143</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>반값다딜 - CJ편 (2/1~8)</t>
+          <t>신규고객 이벤트! 반값다딜</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-08</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다딜 - CJ편 (2/1~8)', '스마일클럽', '첫구매 전용 프로모션', '50% 할인 쿠폰, 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'cj상품 50% 할인 쿠폰 &amp; 첫구매 무료배송 쿠폰', ' 최대 할인 금액 각 5천원 ', '         쿠폰 발급 기간', '         쿠폰 발급 대상', '         2022년 1월 31일 이후 이마트몰, 트레이더스 쓱배송/점포택배 및 새벽배송 구매 이력이 없는 고객 한정', '         상품 할인 쿠폰 적용 방법', '         본 페이지 내 전시된 CJ브랜드 상품 중 3개를 골라 결제 단계에서 쿠폰 적용 (상품당 1개 수량 적용)', '         20,000원 이상 구매시 사용 가능', '         무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰과 함께 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 사용 기간', '       상품할인쿠폰/무료배송 쿠폰 : 2023년 2/1(수) ~ 2/8(수) 행사 기간 내 사용', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 총 3장, 할인 적용 가능 상품들에 한해 50% 할인(상품당 최대할인금액 적용)', '       무료배송 쿠폰 : 총 1장, 이마트몰 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       상품당 1개 수량에 쿠폰 적용 가능하며, 동일한 상품 2개 구매시에도 1개에만 적용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 신규고객 이벤트! 반값다딜', '스마일클럽', '신규고객 이벤트! 반값다딜', '첫구매 전용 달달한 혜택', '50% 할인 쿠폰, 무료배송', '첫 구매는 세개 다~반값! 게다가 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'MENU 50% 할인쿠폰 3장 + 무료배송 쿠폰', '         발렌타인데이 기념 달달한 초콜릿 50% 상품할인쿠폰 1장 (최대 할인금액 5천원)', '         달콤하고 기분 좋은 사탕/카라멜 50% 상품할인쿠폰 1장 (최대 할인금액 2천원)', '         기분좋은 향기로 상쾌하게 칙-칙- 50% 상품할인쿠폰 1장 (최대 할인금액 4천원)', '첫구매는 무료배송! 첫구매라면 반값으로 구매하고 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능', '무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰 3장과 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기 -기간 내 ID당 1회', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 초콜릿 1개, 사탕/카라멜 1개, 섬유탈취제 1개 (ex.초콜릿 2개 구매시에도 1개에만 적용 가능합니다)', '       첫구매 쿠폰 CAT', '        초콜릿 50% cat (최대 5천원 할인) ', '       사탕/카라멜 50% cat (최대 2천원 할인)', '       섬유탈취제 50% cat (최대 4천원 할인)']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: 부가부</t>
+          <t>Romantic Valentine</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>최대 10% 할인 및 SSGPAY 추가 즉시할인</t>
+          <t>최대 10% 할인쿠폰팩 + BEST GIFT 추천</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004111</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004112</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - 부가부</t>
+          <t>(0206-12) Romantic Valentine</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -688,29 +688,29 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 부가부', '스마일클럽', '       1. 부가부 전 상품 5% 상시 할인', '       1. 부가부 스트롤러 및 스타더스트 10% 할인(※폭스 5, 버터플라이 제외)', '       2. 부가부 스트롤러 SSGPAY 카드로 100만원 이상 결제 시, 7만원 즉시할인', '       3. 부가부 폭스 5 구매 시, 선착순 30명 한정 바스타올 증정']</t>
+          <t>['이벤트/쿠폰 &gt; (0206-12) Romantic Valentine', '스마일클럽', '#최대 10% 할인 쿠폰팩 #BEST GIFT ITEM', '발렌타인 전용 10% 할인 쿠폰팩 바로보기', '발렌타인데이 전용 쿠폰 10% 할인 쿠폰팩', '7% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 7만원 이상 구매시 최대 1만원 할인', '10% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 15만원 이상 구매시 최대 2만원 할인', '오늘의 쿠폰은 마감되었습니다.', '       쿠폰 발급 기간', '       23/02/06(월) ~ 23/02/12(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', 'SSG푸드마켓 스윗 발렌타인 위크 - 프리미엄 초콜릿/디저트/커피 다다익선 할인']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>힙슐랭이 제안하는 발렌타인 가이드</t>
+          <t>선물은 사랑을 싣고</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15% 할인과 페이백 이벤트</t>
+          <t>선물한 사연 댓글달고 경품의 행운까지!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004273</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>힙슐랭 : 발렌타인데이편</t>
+          <t>[0202-0226] 선물은 사랑을 싣고</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -720,34 +720,34 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 힙슐랭 : 발렌타인데이편', '스마일클럽', '# 최대 15% 할인', '힙슐랭 베스트 상품 최대 15% 할인 행사', '3개 모두 구매 시, 10% 추가 할인!', ' 감각적인 선물 [트리투바] 밀크/화이트 크로캉 세트 6입 : 정상가 23,080원 10%할인가 20,700원 힙슐랭 comment트리투바는 쇼콜라티에 부부가 직접 만든 초콜릿 전문 브랜드로서, 전 세계 카카오 농장을 직접 찾아 맛보고 연구하여 제품을 생산합니다.신선하면서도 맛있는 감각적인 선물로 추천합니다. ', ' 귀여운 선물 [노티드] 옐로우 밀키팜 틴카라멜 : 정상가 13,980원 10%할인가 12,510원 힙슐랭 comment크림 가득 도넛과 시그니처 패키징으로 새로운 트렌드를 만들어가는 노티드가, 이번엔 귀여운 틴케이스에 달콤한 카라멜을 가득 담아 출시했어요. 먹고 남은 틴케이스는 다양한 용도로 활용해보세요. ', ' 색다른 선물 [구아우쇼콜라] 제주 보리개역 파베초콜릿 16구 : 정상가 22,000원 15%할인가 18,700원 힙슐랭 comment제주도 동쪽 항구마을 김녕에 위치한 초콜릿 숍, 구아우쇼콜라에요. 제주 보리개역을 활용해서 색다른 초콜렛을 만들었어요. 보리개역이란, 제주 지역의 보리를 맷돌에 갈아 분말로 만든 가루라 고소한 마무리가 특징입니다.  ', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [0202-0226] 선물은 사랑을 싣고', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일쿠폰', '모바일쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '로맨틱 발렌타인 - 최대 10% 할인쿠폰팩 + BEST GIFT 추천']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>선물은 사랑을 싣고</t>
+          <t>힙슐랭이 제안하는 발렌타인 가이드</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>선물한 사연 댓글달고 경품의 행운까지!</t>
+          <t>15% 할인과 페이백 이벤트</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004273</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[0202-0226] 선물은 사랑을 싣고</t>
+          <t>힙슐랭 : 발렌타인데이편</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -757,49 +757,49 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0202-0226] 선물은 사랑을 싣고', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일쿠폰', '모바일쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '로맨틱 발렌타인 - 최대 10% 할인쿠폰팩 + BEST GIFT 추천']</t>
+          <t>['이벤트/쿠폰 &gt; 힙슐랭 : 발렌타인데이편', '스마일클럽', '# 최대 15% 할인', '힙슐랭 베스트 상품 최대 15% 할인 행사', '3개 모두 구매 시, 10% 추가 할인!', ' 감각적인 선물 [트리투바] 밀크/화이트 크로캉 세트 6입 : 정상가 23,080원 10%할인가 20,700원 힙슐랭 comment트리투바는 쇼콜라티에 부부가 직접 만든 초콜릿 전문 브랜드로서, 전 세계 카카오 농장을 직접 찾아 맛보고 연구하여 제품을 생산합니다.신선하면서도 맛있는 감각적인 선물로 추천합니다. ', ' 귀여운 선물 [노티드] 옐로우 밀키팜 틴카라멜 : 정상가 13,980원 10%할인가 12,510원 힙슐랭 comment크림 가득 도넛과 시그니처 패키징으로 새로운 트렌드를 만들어가는 노티드가, 이번엔 귀여운 틴케이스에 달콤한 카라멜을 가득 담아 출시했어요. 먹고 남은 틴케이스는 다양한 용도로 활용해보세요. ', ' 색다른 선물 [구아우쇼콜라] 제주 보리개역 파베초콜릿 16구 : 정상가 22,000원 15%할인가 18,700원 힙슐랭 comment제주도 동쪽 항구마을 김녕에 위치한 초콜릿 숍, 구아우쇼콜라에요. 제주 보리개역을 활용해서 색다른 초콜렛을 만들었어요. 보리개역이란, 제주 지역의 보리를 맷돌에 갈아 분말로 만든 가루라 고소한 마무리가 특징입니다.  ', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>든든한 소고기 한 상</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>한우 ~40%할인부터 SSG머니 행운까지</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004312</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022년 7월 1일 부터 년 12월 31일 까지) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; (집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '스마일클럽', '(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '이번 주는 든든하게 소고기 먹고 겨울 마무리! 최대 40할인 한우 행사상품부터 빠르고 손쉬운 소고기 간편식품까지!최애 소고기 요리 댓글달면 SSG머니 행운이!', '최대 40% 할인! 한우/소고기 추천 상품 바로보기', '        My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '        이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '최대 40% 할인!']</t>
         </is>
       </c>
     </row>
@@ -873,251 +873,251 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/6~12) Sweet Home&amp;Living', '스마일클럽', '최대 3만원 할인!', '장바구니 쿠폰팩', '3종 장바구니 쿠폰팩', '매일 오전 9시 선착순 5천명', '장바구니 3,000원 쿠폰 - 3만원 이상 구매시 3천원 할인', '장바구니 10,000원 쿠폰 - 10만원 이상 구매시 1만원 할인', '장바구니 30,000원 쿠폰 - 30만원 이상 구매시 3만원 할인', '선착순 쿠폰 Soldout!', '쿠폰 발급 및 사용 기간 : 2023년 2월 6일 (월) 00 : 00 ~ 2023년 2월 12일 (일) 23 : 59 ', '쿠폰은 ID당 기간 내 1회 발급 가능하며, 신세계몰 /신세계백화점몰 상품에만 적용됩니다. ', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM  회원만 쿠폰 발급이 가능합니다.', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '신학기 기념 플로라 BEST 침구 특가 ~50% OFF!', '국민 호텔 수건 170g 10장 세트 (리본선물포장) ★SSG몰내 쿠폰확인★', '연인에게 전하는 기프트 ~32%', '[자라홈] 주방용품, 접시, 컵 등 : 최대 60%할인', '50%', '60%', 'UP TO 60% OFF', '20%', 'SNS 감성 란가구, 신학기 초특가 할인전', '17%', '10%', '조명은 비츠조명! 인기상품 할인전']</t>
+          <t>['이벤트/쿠폰 &gt; (2/6~12) Sweet Home&amp;Living', '스마일클럽', '최대 3만원 할인!', '장바구니 쿠폰팩', '3종 장바구니 쿠폰팩', '매일 오전 9시 선착순 5천명', '장바구니 3,000원 쿠폰 - 3만원 이상 구매시 3천원 할인', '장바구니 10,000원 쿠폰 - 10만원 이상 구매시 1만원 할인', '장바구니 30,000원 쿠폰 - 30만원 이상 구매시 3만원 할인', '선착순 쿠폰 Soldout!', '쿠폰 발급 및 사용 기간 : 2023년 2월 6일 (월) 00 : 00 ~ 2023년 2월 12일 (일) 23 : 59 ', '쿠폰은 ID당 기간 내 1회 발급 가능하며, 신세계몰 /신세계백화점몰 상품에만 적용됩니다. ', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM  회원만 쿠폰 발급이 가능합니다.', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '소파구매는 지금이 기회! 최대 25%즉시할인+7%쿠폰~2/12', '신학기 기념 플로라 BEST 침구 특가 ~50% OFF!', '국민 호텔 수건 170g 10장 세트 (리본선물포장) ★SSG몰내 쿠폰확인★', '연인에게 전하는 기프트 ~32%', '[자라홈] 주방용품, 접시, 컵 등 : 최대 60%할인', '50%', '60%', 'UP TO 60% OFF', '20%', 'SNS 감성 란가구, 신학기 초특가 할인전', '17%', '10%', '조명은 비츠조명! 인기상품 할인전']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+          <t>2023 대한민국 수산대전 ?2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2월의신규가입혜택</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>첫 구매 고객 스페셜 혜택</t>
+          <t>스마일클럽 웰컴 5천원 쿠폰</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>메가박스 영화 관람권 5,900원</t>
+          <t>2월의신규가입혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-01-27</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 9일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>첫 구매 고객 스페셜 혜택</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>메가박스 영화 관람권 5,900원</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-01-27</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 9일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>시디즈 2/6(월) 7PM</t>
+          <t>브랜드 스포트라이트 X 트라이온: 부가부</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>신학기 의자 100개 한정 핫딜 + 구매인증 사은품</t>
+          <t>최대 10% 할인 및 SSGPAY 추가 즉시할인</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004139</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004111</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>시디즈 신학기 의자 100개 한정 핫딜~ @SSG.LIVE 2/6(월) 19PM</t>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - 부가부</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-01-30</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 시디즈 신학기 의자 100개 한정 핫딜~ @SSG.LIVE 2/6(월) 19PM', '스마일클럽', '시디즈 신학기 의자 100개 한정 핫딜~ @SSG.LIVE 2/6(월) 19PM', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기', '6. 본 이벤트 경품은 브랜드사 상황에 따라 사전 고지 없이 변경, 대체 될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 부가부', '스마일클럽', '       1. 부가부 전 상품 5% 상시 할인', '       1. 부가부 스트롤러 및 스타더스트 10% 할인(※폭스 5, 버터플라이 제외)', '       2. 부가부 스트롤러 SSGPAY 카드로 100만원 이상 결제 시, 7만원 즉시할인', '       3. 부가부 폭스 5 구매 시, 선착순 30명 한정 바스타올 증정']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>입생로랑 2/6(월) 8PM</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>엉크르드뽀/메쉬핑크 한정판 쿠션 선런칭 핫딜! +브러쉬 3종 추첨!</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004220&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>입생로랑@SSG.LIVE　2/6(월) 20:00PM</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-02-08</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 입생로랑@SSG.LIVE\u30002/6(월) 20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LG노트북 2/6(월) 9PM</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>13세대 최신형 라이브 한정 ~19% OFF + 추가사은품</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004127</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>LG노트북 @SSG.LIVE 2/6(월) 9PM</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-01-27</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; LG노트북 @SSG.LIVE 2/6(월) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>갤럭시 S23 사전예약 2/7(화) 10AM</t>
+          <t>발몽 2/9(목) 7PM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>할인에 조선호텔 식사권/상품권 추첨까지!</t>
+          <t>최대 30만원대 기프트 구성 +구매왕 발몽 브라이트닝 팩 정품 증정</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004101&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004106&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>삼성 갤럭시S23@SSG.LIVE　2/7(화) 10:00AM</t>
+          <t>발몽@SSG.LIVE 2/9(목) 19:00PM</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1127,121 +1127,158 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 삼성 갤럭시S23@SSG.LIVE\u30002/7(화) 10:00AM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 발몽@SSG.LIVE 2/9(목) 19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[디지털쓱세일] LG전자 2/7(화) 7PM</t>
+          <t>[월간호캉쓱] 웨스틴 조선 부산2/9(목) 8PM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LG전자 식기세척기/인덕션/가습기 파격특가+오브제컬렉션 청소기 역대급 핫딜까지</t>
+          <t>객실 리뉴얼 기념 압도적 단독특가 / 이규제큐티브 클럽라운지 26만원대~</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004170</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004217</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>LG전자 가전 @SSG.LIVE 2/7(화) 19:00PM</t>
+          <t>웨스틴 조선 부산 @SSG.LIVE 2/9(목) 8PM</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2023-01-30</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; LG전자 가전 @SSG.LIVE 2/7(화) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 웨스틴 조선 부산 @SSG.LIVE 2/9(목) 8PM', '스마일클럽', '                    \xa0\xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>데스커 2/7(화) 20PM</t>
+          <t>삼성전자  2/9(목) 9PM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>책상세트&amp;모션데스크 세트 ~32% 할인 +사은품부터 라이브 한정 이벤트까지</t>
+          <t>삼성 세탁기+건조기 그랑데 패키지 긴급공수! 라이브 한정수량 최대 33% 할인!</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004140</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004130</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>데스커 책상세트&amp;모션데스크 세트 ~32% 할인 @SSG.LIVE 2/7(화) 20PM</t>
+          <t>삼성전자 @SSG.LIVE 2/9(목) 9PM</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2023-01-30</t>
+          <t>2023-01-27</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 데스커 책상세트&amp;모션데스크 세트 ~32% 할인 @SSG.LIVE 2/7(화) 20PM', '스마일클럽', '데스커 책상세트&amp;모션데스크 세트 ~32% 할인 @SSG.LIVE 2/7(화) 20PM']</t>
+          <t>['이벤트/쿠폰 &gt; 삼성전자 @SSG.LIVE 2/9(목) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>다이슨 2/10(금) 7PM</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>기억에 남는 최고의 발렌타인 선물+웨스틴조선호텔 식사권 추첨!</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004103&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>다이슨@SSG.LIVE 2/10(금) 19:00PM</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2023-02-12</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 2/10(금) 19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>2월 맘키즈 PLUS</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>지금 할인 중! ~40% 할인 혜택</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>2022-09-01</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>2999-12-13</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '포켓몬 페이스 피규어 12종 세트 (N2쓱배송, 전국택배)', '헬로카봇 펜타스톰X (N2쓱배송, 전국택배)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)', '뽀로로 스마트 쓰기패드(N2 쓱배송, 전국택배)', '얌얌펫 잼하우스스페셜 (N2쓱배송, 전국택배)', '리틀라이브펫 리틀피쉬 어항세트 (N2쓱배송, 전국택배가능)', '/ 올리키즈 유아동침구 특별 할인전★']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Feb 13 00:21:58 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,814 +473,666 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>디지털 쓱세일 이번주 디지털 최강 혜택!</t>
+          <t>SSG 쇼핑 익스프레스</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>디지털 ~15% 쿠폰 + ~8% 청구할인</t>
+          <t>최대 12% 할인쿠폰+카드 청구할인</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004222</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004232</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>디지털 쓱세일 _ 혜택 페이지</t>
+          <t>SSG 쇼핑 익스프레스</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일 _ 혜택 페이지', '스마일클럽', '       디지털 쿠폰 최대 2장', '디지털 쓱세일 최대 10만원 할인', '디지털 대표 브랜드 최대 15% 상품쿠폰', '쿠폰은 9시 부터 발급됩니다', '최대 10만원 할인 쿠폰 다운 받기', '최대 1만원 항린 쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 2월 6일(월) 09시 00분 부터 2월 12일(일) 23시 59분 까지', '본 쿠폰은 신세계몰/이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '디지털 대표 브랜드 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '백화점 디지털 15% 상품쿠폰', '최대 1만원 할인 쿠폰 다운 받기', 'SSG.COM 첫 구매 고객이라면\xa0 선착순 1만원 장바구니 쿠폰까지', '장바구니 쿠폰 1만원 : 3만원 이상 구매시 1만원 할인 (첫 구매 전용, 디지털가전전용, 선착순 3만명, 일부 특가상품 제외)', '쿠폰 마감 되었습니다.', '쿠폰 다운 받기', '쿠폰발급 및 사용 기간 : 2023년 2월 6일(월) 09시 00분 ~ 2월 12일(일) 23시 59분', '추가 혜택! 카드 청구 할인', '[SSGPAY전용] 신한카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] 삼성카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 현대카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] KB카드 8만원이상 5%, 10만원 이상 7% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] KB카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 7만원이상 8% 청구할인 (일 20만원 한, 디지털쓱세일 전용) 자세히 보기', '[SSGPAY전용] 현대카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 쇼핑 익스프레스', '스마일클럽', '~12% 쿠폰팩', '할인의 완성', '쿠폰 받고 쇼핑열차 출발! 최대 12% 할인 3종 쿠폰', '장바구니쿠폰 7% 10만원 이상 구매 시 최대 1만원 할인', '장바구니쿠폰 10% 15만원 이상 구매 시 최대 2만원 할인', '장바구니쿠폰 12% 20만원 이상 구매 시 최대 3만원 할인', '쿠폰은 13일 10시에 오픈됩니다.', '발급된 쿠폰은 프로모션 기간 중에만 사용 가능하고 이후 소멸됩니다.', '발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '15% OFF+마이크로 에센스 증정', '신학기/봄맞이 최대 44% 세일', '최대 35% + 15% 더블혜택 + 사은품', '인기모델 확보 ~15% OFF', '유아필수품 No.1 +8%OFF', '빠른배송 + ~26%OFF', '[W컨셉] ♥BEST 50♥ 모한/해바이해킴/보카바카 外 ~50% SALE', '[쥬크.CC콜렉트.듀엘] 패밀리세일! 브랜드별 BEST ITEM ~65% OFF + 쿠폰 혜택', '★봄 신상 오픈 + 윈터  클리어런스 ~80% SALE★', '[CARLYN]23SS 푸퍼 출시!♥신상&amp;베스트 최대 76% SALE + 추가 쿠폰 혜택까지!', '★레드하트★한정수량★맨투맨/니트 +)즉시할인쿠폰 바로적용', '탄력과 보습을 한번에! / 최대 91% 할인 + 전구매 사은품', '먼데이문3주년  UP TO 50%+gift', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[라코스테 키즈] 신학기 준비 어패럴/ACC +추가쿠폰!', '★Little SSG★[출산/유아동용품]BEST모음 베이비무브/폴레드/릴리팟/베이비뵨 외 SSG 핫딜!', '믿고 사는 프라이팬+궁중팬 세트 외 할인특가', '★최대32%OFF★덴마크 프리미엄 TEMPUR ! 포토 리뷰 EVENT 스타벅스 기프티콘 증정 !', '[신세계대구점]로라애슐리 신학기 침구할인전', '【해외직구】[애플정품] 애플 에어팟 프로 2세대 맥세이프 충전 케이스  (케이스+스트랩 증정) / 재고보유 / 빠른출고 / H2칩 / 2022년 9월 신제품  / IPX 4 / 관부가세 포함 / 홍콩발송 / 무료배송', '[닥터 브로너스] SSG 단독 할인 +증정 혜택', '[★~71%★]애경 2월의 달콤한 선물(할인+쿠폰+다다익선까지)', '쇼핑익스프레스! SSG 추천하는 고양이 용품 할인 대찬지', '새봄맞이 초특가! 뉴 로제타스톤 (1번 구매로) 24개 언어 무제한 평생 학습권 최대 82% 할인', 'SSG 단독구성 최대 71%할인', '15%할인DAY★1등급 한우 국거리용  400G 외  장조림용/사태/카레용/산적용/불고기용/샤브샤브/다짐육 이유식소고기 골라담기', '- 삼성카드 청구할인 -', '- 현대카드 청구할인 -', '신학기 아이템 전용 10%쿠폰 지급', '뷰티 15% 쿠폰 + 대표 브랜드']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>디지털 쓱세일 인기 가전 브랜드 총출동</t>
+          <t>반값다딜</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>애플/삼성 외 TOP 브랜드</t>
+          <t>상품쿠폰 50% 할인 3장 , 무료배송쿠폰 1장</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004223</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004143</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>디지털 쓱세일_브랜드</t>
+          <t>신규고객 이벤트! 반값다딜</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일_브랜드', '스마일클럽', '         브라운 9466cc 올인원 패키지 핫딜']</t>
+          <t>['이벤트/쿠폰 &gt; 신규고객 이벤트! 반값다딜', '스마일클럽', '신규고객 이벤트! 반값다딜', '첫구매 전용 달달한 혜택', '50% 할인 쿠폰, 무료배송', '첫 구매는 세개 다~반값! 게다가 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'MENU 50% 할인쿠폰 3장 + 무료배송 쿠폰', '         발렌타인데이 기념 달달한 초콜릿 50% 상품할인쿠폰 1장 (최대 할인금액 5천원)', '         달콤하고 기분 좋은 사탕/카라멜 50% 상품할인쿠폰 1장 (최대 할인금액 2천원)', '         기분좋은 향기로 상쾌하게 칙-칙- 50% 상품할인쿠폰 1장 (최대 할인금액 4천원)', '첫구매는 무료배송! 첫구매라면 반값으로 구매하고 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능', '무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰 3장과 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기 -기간 내 ID당 1회', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 초콜릿 1개, 사탕/카라멜 1개, 섬유탈취제 1개 (ex.초콜릿 2개 구매시에도 1개에만 적용 가능합니다)', '       첫구매 쿠폰 CAT', '        초콜릿 50% cat (최대 5천원 할인) ', '       사탕/카라멜 50% cat (최대 2천원 할인)', '       섬유탈취제 50% cat (최대 4천원 할인)']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>디지털 쓱세일 매일 오전 10시! 한정수량 타임딜</t>
+          <t>신학기 페스티벌</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>쓱세일 디지털 추천템</t>
+          <t>매일 10% 쿠폰 + 신학기 준비는 SSG에서</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004224</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004100</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>디지털 쓱세일_특가</t>
+          <t>신학기 FESTIVAL - 신학기 준비는 SSG에서</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 디지털 쓱세일_특가', '스마일클럽', '한정수량 타임딜', '타임딜은 오전 10시에 시작됩니다!', '오늘의 타임딜이 종료되었습니다.', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL - 신학기 준비는 SSG에서', '스마일클럽', '신학기 10% 쿠폰 받고 쇼핑 GO! (현재 페이지)', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '프레드페리 : 프레드페리 S머니 추가 혜택 신학기 패션 고민 끝! SSG 단독 할인', '나이키 : 나이키 공식 스토어 신학기 대전 늘 인기있는 나이키의 신상 운동화/의류 최대 45%off', '오니츠카타이거 : 오니츠카타이거 BEST 모음 프리미엄 인기 슈즈 제안 + 할인 쿠폰 혜택까지', '마리끌레르 : 신학기 선물 SSG 단독 기획 23SS 오픈! 마리끌레르 BEST 단독 추가 쿠폰 할인까지!', '토리버치 : 신학기 BEST 토리버치 선물 토리버치 시즌오프 최대 40% 세일', 'H&amp;M키즈: SSG 단독 유아동 전상품 10% 할인+무배 신학기 맞이! H&amp;M 유아동 전상품 10% 할인+무료배송', '무아스 : 신학기 준비 필수 아이방 꾸미기 인기 홈데코 시계/거울/액자/데코 최대할인', '푸딩이너웨어 : 아이를 위한 편안한 언더웨어 최대 20% 할인 + 사은품 증정', '모윰 : 어린이집 국민육아템 모윰 1DAY 특가전! SSG 단독 최대~60%OFF+사은품 증정!', '아이리스 : 신학기 아이리스 수납 특가전 BEST 1+1 수비르 수납모음 7% 쿠폰 포함', '프라다 : 입학 졸업 선물 명품 구매 찬스! 프라다/생로랑 外 자체 인하 + 즉시할인쿠폰까지', '젠하이저 : 신학기 선물 고민 끝! 젠하이저 IE200 신상품 런칭! 10% 쿠폰 혜택 추가 할인혜택까지', '(특가) 23년 신학기맞이 책가방 행사전 SSG 단독 책가방 포함 ~최대 50% OFF', '(최대 55%) 리바트 공부방 베스트 모음전 최대 할인 혜택+적립+리뷰 이벤트까지', '(최대 35%) 시몬스 인기상품 시크릿 최저가! 최대 35% 즉시할인, 100% 당첨 리뷰이벤트', '(최대 30%) 집중력 높여주는 인기 가드닝템 할인전 싱그러운 향기 가득! 생화/화분/조화 外 할인전', '(최대 50%) 신학기 신상 침구 모음전 신상 침구 ~50% OFF ! 새 이불로 꿀잠 자기', '(최대 65%) 신학기 인기 브랜드 쥬크.CC콜렉트.듀엘.모조에스핀 NEW LOOK &amp; 특가 찬스!', '(이월상품 최대 10%) 믿고 사는 내셔널지오그래픽 아우터, 백팩 23년 S/S 신상 오픈! 이월~10% 할인까지', '(BEST 할인전) 백화점 프리미엄 뉴시즌 페어 신세계백화점 신학기 맞이 스포츠 인기 상품전']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>단 하루! 쓱배송데이</t>
+          <t>Little SSG 베이비페어</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10% 쿠폰 + 카드 할인까지</t>
+          <t>유아동~7% 쿠폰 + BEST 상품 제안</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004247</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004276</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2/9  단 하루! 쓱배송DAY</t>
+          <t>[0213~0219] Little SSG 베이비페어</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2/9  단 하루! 쓱배송DAY', '스마일클럽', '2/9  단 하루! 쓱배송DAY', '할인에 할인을 더하다', '단 하루! 쓱배송 Day', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '오늘은 장보는 날 쓱배송 특가상품 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 쿠폰', '이마트, 트레이더스 쓱배송 및 점포택배/새벽배송', '10% 쿠폰 - 8만원 이상 결제시 최대 1만 5천원 할인 ID당 1매 (오전 9시 오픈, 선착순 2만명)', '쿠폰발급 및 사용 기간 2023년 2월 9일 (당일 발급된 쿠폰은 당일 한정 사용가능)', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', 'KB국민카드 8만원 이상 5% 청구할인 / 10만원 이상 7% 청구할인', '      쿠폰 발급 및 사용일', '      23년 2월 9일(기간 중 ID당 1일 1회 다운가능) (발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '2 오늘은 장보는 날! 쓱배송데이 장보기 특가상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; [0213~0219] Little SSG 베이비페어', '스마일클럽', '유아동~7%쿠폰', '유아동 선착순 ~7% 쿠폰', '7% 상품쿠폰 : 2만원 이상 상품 구매시 최대 7천원 할인(선착순 5만장)', '쿠폰은 09시부터 선착순 발급 됩니다.', '쿠폰발급 및 사용 기간 :  2023년 2월 13일(월) 09시 00분 ~ 2월 19일(일) 23시 59분', '최대 ~40% 할인', '최대 40% 할인', '★블랑101XSSG★파격특가! 세탁세제/섬유유연제 최대 50%할인+ 사은품 증정', '★[엘라바/오케이베이비/와우컵/퓨어닷]★ SSG 스페셜 최대~48%OFF+단독핫딜헤택', '베이비페어 7% 할인찬스', '[닥스키즈/헤지스키즈/피터젠슨] 23SS신상 책가방특가+겨울의류 파이널세일! 최대55%할인', '[빈폴키즈][쿠폰혜택] 23SS 신상 BEST 책가방/상하의/맨투맨/팬츠/세트 모음', '베이비페어 4일간 스트롤러/스타더스트  10% OFF', '완구 네오센터 클리어런스 ★최대 40%특가★', '[5~15%다운쿠폰]후디스 이유식/그릭요거트/두유 브랜드위크', '[쓱배송]킨도 기저귀 모음전']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>반값다딜</t>
+          <t>선물은 사랑을 싣고</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>상품쿠폰 50% 할인 3장 , 무료배송쿠폰 1장</t>
+          <t>선물한 사연 댓글달고 경품의 행운까지!</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004143</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>신규고객 이벤트! 반값다딜</t>
+          <t>[0202-0226] 선물은 사랑을 싣고</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신규고객 이벤트! 반값다딜', '스마일클럽', '신규고객 이벤트! 반값다딜', '첫구매 전용 달달한 혜택', '50% 할인 쿠폰, 무료배송', '첫 구매는 세개 다~반값! 게다가 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'MENU 50% 할인쿠폰 3장 + 무료배송 쿠폰', '         발렌타인데이 기념 달달한 초콜릿 50% 상품할인쿠폰 1장 (최대 할인금액 5천원)', '         달콤하고 기분 좋은 사탕/카라멜 50% 상품할인쿠폰 1장 (최대 할인금액 2천원)', '         기분좋은 향기로 상쾌하게 칙-칙- 50% 상품할인쿠폰 1장 (최대 할인금액 4천원)', '첫구매는 무료배송! 첫구매라면 반값으로 구매하고 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능', '무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰 3장과 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기 -기간 내 ID당 1회', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 초콜릿 1개, 사탕/카라멜 1개, 섬유탈취제 1개 (ex.초콜릿 2개 구매시에도 1개에만 적용 가능합니다)', '       첫구매 쿠폰 CAT', '        초콜릿 50% cat (최대 5천원 할인) ', '       사탕/카라멜 50% cat (최대 2천원 할인)', '       섬유탈취제 50% cat (최대 4천원 할인)']</t>
+          <t>['이벤트/쿠폰 &gt; [0202-0226] 선물은 사랑을 싣고', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일쿠폰', '모바일쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '로맨틱 발렌타인 - 최대 10% 할인쿠폰팩 + BEST GIFT 추천']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Romantic Valentine</t>
+          <t>든든한 소고기 한 상</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>최대 10% 할인쿠폰팩 + BEST GIFT 추천</t>
+          <t>한우 ~40%할인부터 SSG머니 행운까지</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004112</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004312</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(0206-12) Romantic Valentine</t>
+          <t>(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0206-12) Romantic Valentine', '스마일클럽', '#최대 10% 할인 쿠폰팩 #BEST GIFT ITEM', '발렌타인 전용 10% 할인 쿠폰팩 바로보기', '발렌타인데이 전용 쿠폰 10% 할인 쿠폰팩', '7% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 7만원 이상 구매시 최대 1만원 할인', '10% 장바구니 쿠폰 (매일 오전 9시 / 선착순 1만장) - 15만원 이상 구매시 최대 2만원 할인', '오늘의 쿠폰은 마감되었습니다.', '       쿠폰 발급 기간', '       23/02/06(월) ~ 23/02/12(일), 매일 오전 9시부터 선착순 발급', '       쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', 'SSG푸드마켓 스윗 발렌타인 위크 - 프리미엄 초콜릿/디저트/커피 다다익선 할인']</t>
+          <t>['이벤트/쿠폰 &gt; (집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '스마일클럽', '(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '이번 주는 든든하게 소고기 먹고 겨울 마무리! 최대 40할인 한우 행사상품부터 빠르고 손쉬운 소고기 간편식품까지!최애 소고기 요리 댓글달면 SSG머니 행운이!', '최대 40% 할인! 한우/소고기 추천 상품 바로보기', '        My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '        이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '최대 40% 할인!']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>선물은 사랑을 싣고</t>
+          <t>미식구매 할인찬스 피코크 위크</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>선물한 사연 댓글달고 경품의 행운까지!</t>
+          <t>간편하고 맛있는 피코크로 든든한 하루 ~ 30%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004175&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[0202-0226] 선물은 사랑을 싣고</t>
+          <t>미식체험 할인찬스 피코크 위크</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-03</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0202-0226] 선물은 사랑을 싣고', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일쿠폰', '모바일쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '로맨틱 발렌타인 - 최대 10% 할인쿠폰팩 + BEST GIFT 추천']</t>
+          <t>['이벤트/쿠폰 &gt; 미식체험 할인찬스 피코크 위크', '스마일클럽', '미식체험 할인찬스 피코크 위크', '최대 50% / 1+1 / 2+1', '~30%/ 2+1 구매찬스', '[피코크] 피콕분식 신당동식떡볶이 970g 신당동 떡볶이를 간편하게 원가 8,480원 &gt; 할인가 5,936원', '[피코크] 한옥집 김치찜 500g 서대문 맛집의 비법을 그대로 원가 7,980원 &gt; 할인가 5,586원', '~30% 할인특가 대표상품', '피코크 자연치즈를 99% 담은 모짜렐라 슈레드치즈 300g(피자치즈)', '피코크 자연치즈를 99% 담은 고다&amp;체다 슈레드치즈 500g(피자치즈)']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>힙슐랭이 제안하는 발렌타인 가이드</t>
+          <t>2023 대한민국 수산대전 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15% 할인과 페이백 이벤트</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004273</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>힙슐랭 : 발렌타인데이편</t>
+          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 힙슐랭 : 발렌타인데이편', '스마일클럽', '# 최대 15% 할인', '힙슐랭 베스트 상품 최대 15% 할인 행사', '3개 모두 구매 시, 10% 추가 할인!', ' 감각적인 선물 [트리투바] 밀크/화이트 크로캉 세트 6입 : 정상가 23,080원 10%할인가 20,700원 힙슐랭 comment트리투바는 쇼콜라티에 부부가 직접 만든 초콜릿 전문 브랜드로서, 전 세계 카카오 농장을 직접 찾아 맛보고 연구하여 제품을 생산합니다.신선하면서도 맛있는 감각적인 선물로 추천합니다. ', ' 귀여운 선물 [노티드] 옐로우 밀키팜 틴카라멜 : 정상가 13,980원 10%할인가 12,510원 힙슐랭 comment크림 가득 도넛과 시그니처 패키징으로 새로운 트렌드를 만들어가는 노티드가, 이번엔 귀여운 틴케이스에 달콤한 카라멜을 가득 담아 출시했어요. 먹고 남은 틴케이스는 다양한 용도로 활용해보세요. ', ' 색다른 선물 [구아우쇼콜라] 제주 보리개역 파베초콜릿 16구 : 정상가 22,000원 15%할인가 18,700원 힙슐랭 comment제주도 동쪽 항구마을 김녕에 위치한 초콜릿 숍, 구아우쇼콜라에요. 제주 보리개역을 활용해서 색다른 초콜렛을 만들었어요. 보리개역이란, 제주 지역의 보리를 맷돌에 갈아 분말로 만든 가루라 고소한 마무리가 특징입니다.  ', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>든든한 소고기 한 상</t>
+          <t>스마일클럽 웰컴 5천원 쿠폰</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>한우 ~40%할인부터 SSG머니 행운까지</t>
+          <t>2월의신규 가입 혜택</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004312</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '스마일클럽', '(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '이번 주는 든든하게 소고기 먹고 겨울 마무리! 최대 40할인 한우 행사상품부터 빠르고 손쉬운 소고기 간편식품까지!최애 소고기 요리 댓글달면 SSG머니 행운이!', '최대 40% 할인! 한우/소고기 추천 상품 바로보기', '        My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '        이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '최대 40% 할인!']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>미식구매 할인찬스 피코크 위크</t>
+          <t>SSG 브랜드 스포트라이트: 삼성</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>간편하고 맛있는 피코크로 든든한 하루 ~ 30%</t>
+          <t>비스포크 제트 무선청소기 220w ~28% 할인</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004175&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004364</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>미식체험 할인찬스 피코크 위크</t>
+          <t>SSG 브랜드 스포트라이트 - 삼성</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-02-03</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 미식체험 할인찬스 피코크 위크', '스마일클럽', '미식체험 할인찬스 피코크 위크', '최대 50% / 1+1 / 2+1', '~30%/ 2+1 구매찬스', '[피코크] 피콕분식 신당동식떡볶이 970g 신당동 떡볶이를 간편하게 원가 8,480원 &gt; 할인가 5,936원', '[피코크] 한옥집 김치찜 500g 서대문 맛집의 비법을 그대로 원가 7,980원 &gt; 할인가 5,586원', '~30% 할인특가 대표상품', '피코크 자연치즈를 99% 담은 모짜렐라 슈레드치즈 300g(피자치즈)', '피코크 자연치즈를 99% 담은 고다&amp;체다 슈레드치즈 500g(피자치즈)']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 삼성', '스마일클럽', '더 강력하고 더 가벼워진 210W 최경량 청소기 놀랄만큼 강력해진 흡입력으로 더욱 쉽고 효율적이게, 모터는 기존 대비 47% 더 가벼워진 무게로 더욱 빠른 회전 최적의 구조로 에너지 효율을 높여 최고 210W의 강력한 흡입력까지!', '       비스포크 무선 / 로봇 청소기 인기 모델 최대 28% OFF']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>스윗 홈&amp;리빙</t>
+          <t>먼데이문 3rd ANNIVERSARY</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>새로운 시작의 순간, ~3만원 쿠폰과 스윗 홈을 만들어보세요</t>
+          <t>뷰티 전용 ~15% 쿠폰부터 브랜드 특가전, 체험단까지!</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004054</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004305</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>(2/6~12) Sweet Home&amp;Living</t>
+          <t>[0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/6~12) Sweet Home&amp;Living', '스마일클럽', '최대 3만원 할인!', '장바구니 쿠폰팩', '3종 장바구니 쿠폰팩', '매일 오전 9시 선착순 5천명', '장바구니 3,000원 쿠폰 - 3만원 이상 구매시 3천원 할인', '장바구니 10,000원 쿠폰 - 10만원 이상 구매시 1만원 할인', '장바구니 30,000원 쿠폰 - 30만원 이상 구매시 3만원 할인', '선착순 쿠폰 Soldout!', '쿠폰 발급 및 사용 기간 : 2023년 2월 6일 (월) 00 : 00 ~ 2023년 2월 12일 (일) 23 : 59 ', '쿠폰은 ID당 기간 내 1회 발급 가능하며, 신세계몰 /신세계백화점몰 상품에만 적용됩니다. ', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM  회원만 쿠폰 발급이 가능합니다.', '세계 최초 모듈가구 USM, 10%쿠폰 할인', '소파구매는 지금이 기회! 최대 25%즉시할인+7%쿠폰~2/12', '신학기 기념 플로라 BEST 침구 특가 ~50% OFF!', '국민 호텔 수건 170g 10장 세트 (리본선물포장) ★SSG몰내 쿠폰확인★', '연인에게 전하는 기프트 ~32%', '[자라홈] 주방용품, 접시, 컵 등 : 최대 60%할인', '50%', '60%', 'UP TO 60% OFF', '20%', 'SNS 감성 란가구, 신학기 초특가 할인전', '17%', '10%', '조명은 비츠조명! 인기상품 할인전']</t>
+          <t>['이벤트/쿠폰 &gt; [0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY', '스마일클럽', '먼데이문 3주년을 맞아 준비한 최대 15% 상품쿠폰 3종 + 브랜드 특가전 + 체험단', '뷰티 전용 최대 15% 쿠폰 바로보기', '원하는 날 빠르게 뷰티 쓱배송 바로보기', '먼데이문 3주년 기념 쿠폰 3종', '뷰티 최대 15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '3만원 이상 상품 구매시 최대 1만 2천원 할인 (신세계백화점몰/시코르)', '선착순 쿠폰 Soldout!', '트렌드뷰티 최대5% 상품쿠폰', '2만원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '       쿠폰 발급 및 사용 기간', '       쿠폰 사용 조건', '       각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '15% 상품쿠폰', '1원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '케라스타즈케라스타즈 봄 담은 헤어&amp;두피 케어 - 10% 할인&amp;럭셔리 케어 증정 보러가기', '닥터지닥터지 국민크림 블랙스네일 外 - BEST 최대89% SALE + 쿠폰&amp;증정 혜택 보러가기', '더바디샵더바디샵 X 조규성 SELF LOVE - 최대 35% 즉시할인 + 15% 더블쿠폰 + 사은품 증정 보러가기', '베스트셀러 증정 응모 이벤트 등 쏟아지는 혜택', '프란츠프리미엄 안티에이징 프란츠 - 줄기세포 앰플/토너 외 BEST 스킨&amp;선케어 최대35% SALE 보러가기', '삐아삐아 - UP TO 29% + 쿠폰 15% + 사은품 증정 보러가기', '비프리지친 피부에 진정과 수분을 더하는 비프리 - BEST 스킨케어&amp;클렌징 최대 40% + 스타벅스 기프티콘 보러가기', '트리셀나를 더욱 나답게, 라이프스타일 브랜드 트리셀 - 전품목 UP TO 57% + 다다익선 10% + 사은품 증정 보러가기', '뷰티 상품도 쓱배송']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 ?2월 깜짝 특별전</t>
+          <t>봄꽃 여행 특가 위크</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>제주/도쿄/오사카 봄 여행 준비! ~5만원 패키지 즉시 할인 + 항공권 특가</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004326</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
+          <t>봄꽃 여행 특가 위크</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 봄꽃 여행 특가 위크', '스마일클럽', '최대 5만원 할인', '국제선 ~5만원 할인', '12% 단독 할인', '카드 청구 할인', '여행 전 상품 최대 5만원 할인', "프로모션 내용:  SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 4천원/1만원/2만원/5만원 즉시할인", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '사용방법행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '사용 방법:요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '봄 여행, 할인 받고 여기어때?', '해비치 호텔&amp;리조트 정상가 : 209,088원 &gt; 할인가 : 183,997원', '라마다 프라자 제주 호텔 정상가 : 158,119원 &gt; 할인가 : 139,145원', '메종 글래드 제주 정상가 : 134,500원 &gt; 할인가 : 118,360원', '썬앤문 리조트 정상가 : 198,000원 &gt; 할인가 : 174,240원', '제주 나인리조트 정상가 : 90,000원 &gt; 할인가 : 79,200원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 59,400원', '풀빌라 소랑 제주 정상가 : 84,000원 &gt; 할인가 : 73,920원', '탐라스테이 호텔 정상가 : 75,650원 &gt; 할인가 : 66,572원', '시그니엘 부산 정상가 : 321,860원 &gt; 할인가 : 291,860원', '웨스틴 조선 부산 정상가 : 261,360원 &gt; 할인가 : 231,360원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 197,472원', '아난티 힐튼 부산 정상가 : 363,000원 &gt; 할인가 : 333,000원', '펠릭스 by STX 호텔앤스위트 정상가 : 73,600원 &gt; 할인가 : 64,768원', '라마다 앙코르 바이 윈덤 부산 해운대 정상가 : 70,000원 &gt; 할인가 : 61,600원', '부산 코모도호텔 정상가 : 69,000원 &gt; 할인가 : 60,720원', '호텔 아쿠아펠리스 정상가 : 90,000원 &gt; 할인가 : 79,200원', '레고랜드 코리아 리조트 정상가 : 297,000원 &gt; 할인가 : 267,000원', '르네블루 바이 워커힐 정상가 : 190,000원 &gt; 할인가 : 167,200원', '소노캄 델피노 AB동 정상가 : 162,000원 &gt; 할인가 : 142,560원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '금강산콘도 정상가 : 45,650원 &gt; 할인가 : 40,172원', '디그니티 호텔 정상가 : 90,000원 &gt; 할인가 : 79,200원', '아비오 호텔 정상가 : 72,624원 &gt; 할인가 : 63,909원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 79,000원 &gt; 할인가 : 69,520원', '여수 라테라스 리조트 정상가 : 109,000원 &gt; 할인가 : 95,920원', '여수예술랜드 정상가 : 130,000원 &gt; 할인가 : 114,400원', '헤이븐 호텔 정상가 : 56,709원 &gt; 할인가 : 49,904원', '여수 하이락리조트 정상가 : 85,500원 &gt; 할인가 : 75,240원', '쏠비치 진도 리조트 정상가 : 151,000원 &gt; 할인가 : 132,880원', '클럽이에스 제천리조트 정상가 : 135,000원 &gt; 할인가 : 118,800원', '무주 나봄리조트 정상가 : 70,000원 &gt; 할인가 : 61,600원', '목포 어반 호텔 정상가 : 65,000원 &gt; 할인가 : 57,200원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 316,500원', '콘래드 서울 정상가 : 451,000원 &gt; 할인가 : 421,000원', '골든튤립 인천공항 호텔&amp;스위트 정상가 : 83,591원 &gt; 할인가 : 73,560원', '제이앤파크 호텔 정상가 : 147,999원 &gt; 할인가 : 130,239원', '레스케이프 정상가 : 175,248원 &gt; 할인가 : 154,218원', '노보텔 앰배서더 서울 용산 정상가 : 174,000원 &gt; 할인가 : 153,120원', '스위스 그랜드 호텔 정상가 : 205,000원 &gt; 할인가 : 180,400원', 'L7 강남 바이 롯데 정상가 : 148,330원 &gt; 할인가 : 130,530원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Ed2 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+          <t>프리미엄 아울렛 위크  : S/S NEW ARRIVALS</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2월의신규가입혜택</t>
+          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004363</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>[0213-0219] 프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [0213-0219] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 2월 할인 대전', '최대 10% 할인 쿠폰 혜택', '[여성 패션 - 최대 70% 할인] 온앤온/ 나이스클랍/ 랩 브랜드 위크 外 보러가기', '[언더웨어 - 최대 70% 할인] 라페어/ 비너스/ 바바라/ 트라이엄프 특가 外 보러가기', '[명품잡화 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[스포츠 - 최대 70% 할인] 내셔널지오그래픽 등 아웃도어 브랜드 위크 보러가기', '[패션잡화 - 최대 37% 할인] 발렌타인데이 기념 - 전품목 30% OFF 보러가기', '[패션 슈즈 - 최대 80% 할인] 슈즈 판매 랭킹 TOP 300 인기상품 특가 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 80% 할인] 라코스테, 지프 등 캐주얼 특가 外 보러가기', '[키즈패션 - 최대 60% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 70% 할인] 테팔 브랜드위크! 매직핸드 外 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>첫 구매 고객 스페셜 혜택</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>메가박스 영화 관람권 5,900원</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003994</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-01-27</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '스마일클럽', '[쓱- 첫구매 응원 이벤트] 메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택', '메가박스 스페셜 할인 혜택으로 가족&amp;연인과 즐거운 시간 보내세요!', 'SSG.COM 첫구매 응원 이벤트', '쓱닷컴 첫구매 고객님과 1년만에 다시 오신 고객님을 위한 메가박스 전용 특별 할인쿠폰', '       4,000원 할인쿠폰', '       첫 구매 고객 전용 쿠폰 발급 대상', '       쿠폰발급 및 사용기간', '       2023년 1월 27일(금) 10:00시 부터 선착순 발급 및 발급 후 2월 9일(목)23:59까지 사용가능', '       본 쿠폰은 지정된 메가박스 스페셜 할인 2D 영화 관람권에 한하여 적용 가능하며, 1장 당 상품 1개에 적용됩니다.', '       본 이벤트는 당사 사정에 따라 변동 및 조기 종료될 수 있습니다.', '       정상 판매가 : 13,000원 / SSG.COM 스페셜 할인가 : 9,900원']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: 부가부</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>최대 10% 할인 및 SSGPAY 추가 즉시할인</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004111</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - 부가부</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 부가부', '스마일클럽', '       1. 부가부 전 상품 5% 상시 할인', '       1. 부가부 스트롤러 및 스타더스트 10% 할인(※폭스 5, 버터플라이 제외)', '       2. 부가부 스트롤러 SSGPAY 카드로 100만원 이상 결제 시, 7만원 즉시할인', '       3. 부가부 폭스 5 구매 시, 선착순 30명 한정 바스타올 증정']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>괌 여행(롯데관광) 2/13(월) 8PM</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>50만원상당혜택포함 괌 특급 롯데호텔 클럽룸UP 4/5일 초특가</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004320</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>괌 여행(롯데관광) @SSG.LIVE 2/13(화) 8PM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-07</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 괌 여행(롯데관광) @SSG.LIVE 2/13(화) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>캐치티니핑 2/14(화) 10AM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>첫 라이브 기념 ~40% 특가! 100% 증정사은품 까지</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004239&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[쓱라이브] 캐치티니핑 2/14(화)10AM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-17</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 캐치티니핑 2/14(화)10AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>발몽 2/9(목) 7PM</t>
+          <t>아르마니 뷰티 2/14(화) 8PM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>최대 30만원대 기프트 구성 +구매왕 발몽 브라이트닝 팩 정품 증정</t>
+          <t>NEW 립 마에스트로 사틴 최.초.공.개! 듀오세트 핫딜구성&amp;선착순 600명 립 미니어처 증정</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004106&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004270</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>발몽@SSG.LIVE 2/9(목) 19:00PM</t>
+          <t>[SSG.LIVE]2/14(화) 8PM 아르마니뷰티</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2023-02-08</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-02-14</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 발몽@SSG.LIVE 2/9(목) 19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>[월간호캉쓱] 웨스틴 조선 부산2/9(목) 8PM</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>객실 리뉴얼 기념 압도적 단독특가 / 이규제큐티브 클럽라운지 26만원대~</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004217</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>웨스틴 조선 부산 @SSG.LIVE 2/9(목) 8PM</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2023-01-31</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2023-02-09</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 웨스틴 조선 부산 @SSG.LIVE 2/9(목) 8PM', '스마일클럽', '                    \xa0\xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>삼성전자  2/9(목) 9PM</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>삼성 세탁기+건조기 그랑데 패키지 긴급공수! 라이브 한정수량 최대 33% 할인!</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004130</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>삼성전자 @SSG.LIVE 2/9(목) 9PM</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2023-01-27</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2023-02-09</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 삼성전자 @SSG.LIVE 2/9(목) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>다이슨 2/10(금) 7PM</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>기억에 남는 최고의 발렌타인 선물+웨스틴조선호텔 식사권 추첨!</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004103&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>다이슨@SSG.LIVE 2/10(금) 19:00PM</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2023-01-26</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2023-02-12</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 2/10(금) 19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2월 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~40% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '잠깐! 쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰으로 상품별 최대 40%', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '[파스퇴르] 올곧게만든 위드맘 3단계 750g (NEO2 쓱배송, 그외지역 택배)', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '포켓몬 페이스 피규어 12종 세트 (N2쓱배송, 전국택배)', '헬로카봇 펜타스톰X (N2쓱배송, 전국택배)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)', '뽀로로 스마트 쓰기패드(N2 쓱배송, 전국택배)', '얌얌펫 잼하우스스페셜 (N2쓱배송, 전국택배)', '리틀라이브펫 리틀피쉬 어항세트 (N2쓱배송, 전국택배가능)', '/ 올리키즈 유아동침구 특별 할인전★']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]2/14(화) 8PM 아르마니뷰티', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Feb 16 00:21:21 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -473,286 +473,286 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SSG 쇼핑 익스프레스</t>
+          <t>첫구매는 반값다딜</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>최대 12% 할인쿠폰+카드 청구할인</t>
+          <t>첫구매 인기템! 화장지, 밀키트 총 1.5만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004232</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004346&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SSG 쇼핑 익스프레스</t>
+          <t>첫구매는 반값다딜 (2/16~22)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 쇼핑 익스프레스', '스마일클럽', '~12% 쿠폰팩', '할인의 완성', '쿠폰 받고 쇼핑열차 출발! 최대 12% 할인 3종 쿠폰', '장바구니쿠폰 7% 10만원 이상 구매 시 최대 1만원 할인', '장바구니쿠폰 10% 15만원 이상 구매 시 최대 2만원 할인', '장바구니쿠폰 12% 20만원 이상 구매 시 최대 3만원 할인', '쿠폰은 13일 10시에 오픈됩니다.', '발급된 쿠폰은 프로모션 기간 중에만 사용 가능하고 이후 소멸됩니다.', '발급 후 [My SSG] ▶ [쿠폰] ▶ [보유쿠폰] 에서 확인 가능합니다.', '15% OFF+마이크로 에센스 증정', '신학기/봄맞이 최대 44% 세일', '최대 35% + 15% 더블혜택 + 사은품', '인기모델 확보 ~15% OFF', '유아필수품 No.1 +8%OFF', '빠른배송 + ~26%OFF', '[W컨셉] ♥BEST 50♥ 모한/해바이해킴/보카바카 外 ~50% SALE', '[쥬크.CC콜렉트.듀엘] 패밀리세일! 브랜드별 BEST ITEM ~65% OFF + 쿠폰 혜택', '★봄 신상 오픈 + 윈터  클리어런스 ~80% SALE★', '[CARLYN]23SS 푸퍼 출시!♥신상&amp;베스트 최대 76% SALE + 추가 쿠폰 혜택까지!', '★레드하트★한정수량★맨투맨/니트 +)즉시할인쿠폰 바로적용', '탄력과 보습을 한번에! / 최대 91% 할인 + 전구매 사은품', '먼데이문3주년  UP TO 50%+gift', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[라코스테 키즈] 신학기 준비 어패럴/ACC +추가쿠폰!', '★Little SSG★[출산/유아동용품]BEST모음 베이비무브/폴레드/릴리팟/베이비뵨 외 SSG 핫딜!', '믿고 사는 프라이팬+궁중팬 세트 외 할인특가', '★최대32%OFF★덴마크 프리미엄 TEMPUR ! 포토 리뷰 EVENT 스타벅스 기프티콘 증정 !', '[신세계대구점]로라애슐리 신학기 침구할인전', '【해외직구】[애플정품] 애플 에어팟 프로 2세대 맥세이프 충전 케이스  (케이스+스트랩 증정) / 재고보유 / 빠른출고 / H2칩 / 2022년 9월 신제품  / IPX 4 / 관부가세 포함 / 홍콩발송 / 무료배송', '[닥터 브로너스] SSG 단독 할인 +증정 혜택', '[★~71%★]애경 2월의 달콤한 선물(할인+쿠폰+다다익선까지)', '쇼핑익스프레스! SSG 추천하는 고양이 용품 할인 대찬지', '새봄맞이 초특가! 뉴 로제타스톤 (1번 구매로) 24개 언어 무제한 평생 학습권 최대 82% 할인', 'SSG 단독구성 최대 71%할인', '15%할인DAY★1등급 한우 국거리용  400G 외  장조림용/사태/카레용/산적용/불고기용/샤브샤브/다짐육 이유식소고기 골라담기', '- 삼성카드 청구할인 -', '- 현대카드 청구할인 -', '신학기 아이템 전용 10%쿠폰 지급', '뷰티 15% 쿠폰 + 대표 브랜드']</t>
+          <t>['이벤트/쿠폰 &gt; 첫구매는 반값다딜 (2/16~22)', '하기스 50%', '스마일클럽', '첫구매는 반값다딜 (2/16~22)', '화장지,밀키트 총 1.5만원 할인+무료배송', '반값 할인쿠폰팩', '첫구매 전용 특별 메뉴 반값 할인 쿠폰팩', '첫구매 전용특별 메뉴', ' 마침 필요하셨죠? 화장지 선상품 1만원 할인 최대할인금액 1만원 ', ' 오늘 저녁 고민 끝! 밀키트 전상품 5천원 할인 최대할인금액 5천원 ', '반값메뉴는 무료배송으로 즐겨야죠', '상품쿠폰 50% 이마트몰 무료배송', '첫구매 쿠폰팩 받기 -ID당 기간중 1회', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       -상품할인쿠폰, 무료배송쿠폰: 2023년 2월 16일(목) 2023년 2월 22일 (수)', '       쿠폰 적용 대상 상품', '-쓱배송 새벽배송 상품에 한해서 적용 가능', '-화장지 50% cat (최대 1만원 할인) 제지/위생용품, 화장지/물티슈, 화장지', '-밀키트 50% cat (최대 5천원 할인) 밀키트/간편식, 밀키트', '- 상품당 1개 수량에 쿠폰 적용 가능 : 화장지 1개, 밀키트 1개 적용 가능(ex. 화장지 2개 구매시에도 1개에만 적용 가능합니다.)', '       쿠폰 사용 조건', '-상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인 금액 적용', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>반값다딜</t>
+          <t>신학기 페스티벌</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>상품쿠폰 50% 할인 3장 , 무료배송쿠폰 1장</t>
+          <t>매일 10% 쿠폰 + 신학기 준비는 SSG에서</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004143</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004100</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>신규고객 이벤트! 반값다딜</t>
+          <t>신학기 FESTIVAL - 신학기 준비는 SSG에서</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신규고객 이벤트! 반값다딜', '스마일클럽', '신규고객 이벤트! 반값다딜', '첫구매 전용 달달한 혜택', '50% 할인 쿠폰, 무료배송', '첫 구매는 세개 다~반값! 게다가 무료배송', '첫구매는 세 개 골라 반값!', '* 첫구매 고객은 생애 첫 구매 고객과 최근 1년 이내 구매 이력이 없는 고객을 포함합니다.', 'MENU 50% 할인쿠폰 3장 + 무료배송 쿠폰', '         발렌타인데이 기념 달달한 초콜릿 50% 상품할인쿠폰 1장 (최대 할인금액 5천원)', '         달콤하고 기분 좋은 사탕/카라멜 50% 상품할인쿠폰 1장 (최대 할인금액 2천원)', '         기분좋은 향기로 상쾌하게 칙-칙- 50% 상품할인쿠폰 1장 (최대 할인금액 4천원)', '첫구매는 무료배송! 첫구매라면 반값으로 구매하고 무료로 배송받으세요.', '20,000원 이상 구매시 사용가능', '무료배송 쿠폰은 2만원 이상 구매시 사용가능하며, 반값쿠폰 3장과 발급됩니다.', '첫구매 쿠폰 모두 한번에 받기 -기간 내 ID당 1회', '쿠폰 사용 전 꼭 확인하세요!', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       쿠폰 사용 조건', '       상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인금액 적용', '       무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '       쿠폰 적용 대상 상품', '       대상상품 : 쓱배송 새벽배송, 해당 카테고리 상품에 대해서 적용 가능', '       상품당 1개 수량에 쿠폰 적용 가능 : 초콜릿 1개, 사탕/카라멜 1개, 섬유탈취제 1개 (ex.초콜릿 2개 구매시에도 1개에만 적용 가능합니다)', '       첫구매 쿠폰 CAT', '        초콜릿 50% cat (최대 5천원 할인) ', '       사탕/카라멜 50% cat (최대 2천원 할인)', '       섬유탈취제 50% cat (최대 4천원 할인)']</t>
+          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL - 신학기 준비는 SSG에서', '하기스 50%', '스마일클럽', '신학기 10% 쿠폰 받고 쇼핑 GO! (현재 페이지)', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '프레드페리 : 프레드페리 S머니 추가 혜택 신학기 패션 고민 끝! SSG 단독 할인', '나이키 : 나이키 공식 스토어 신학기 대전 늘 인기있는 나이키의 신상 운동화/의류 최대 45%off', '오니츠카타이거 : 오니츠카타이거 BEST 모음 프리미엄 인기 슈즈 제안 + 할인 쿠폰 혜택까지', '마리끌레르 : 신학기 선물 SSG 단독 기획 23SS 오픈! 마리끌레르 BEST 단독 추가 쿠폰 할인까지!', '토리버치 : 신학기 BEST 토리버치 선물 토리버치 시즌오프 최대 40% 세일', 'H&amp;M키즈: SSG 단독 유아동 전상품 10% 할인+무배 신학기 맞이! H&amp;M 유아동 전상품 10% 할인+무료배송', '무아스 : 신학기 준비 필수 아이방 꾸미기 인기 홈데코 시계/거울/액자/데코 최대할인', '푸딩이너웨어 : 아이를 위한 편안한 언더웨어 최대 20% 할인 + 사은품 증정', '모윰 : 어린이집 국민육아템 모윰 1DAY 특가전! SSG 단독 최대~60%OFF+사은품 증정!', '아이리스 : 신학기 아이리스 수납 특가전 BEST 1+1 수비르 수납모음 7% 쿠폰 포함', '프라다 : 입학 졸업 선물 명품 구매 찬스! 프라다/생로랑 外 자체 인하 + 즉시할인쿠폰까지', '젠하이저 : 신학기 선물 고민 끝! 젠하이저 IE200 신상품 런칭! 10% 쿠폰 혜택 추가 할인혜택까지', '(특가) 23년 신학기맞이 책가방 행사전 SSG 단독 책가방 포함 ~최대 50% OFF', '(최대 55%) 리바트 공부방 베스트 모음전 최대 할인 혜택+적립+리뷰 이벤트까지', '(최대 35%) 시몬스 인기상품 시크릿 최저가! 최대 35% 즉시할인, 100% 당첨 리뷰이벤트', '(최대 30%) 집중력 높여주는 인기 가드닝템 할인전 싱그러운 향기 가득! 생화/화분/조화 外 할인전', '(최대 50%) 신학기 신상 침구 모음전 신상 침구 ~50% OFF ! 새 이불로 꿀잠 자기', '(최대 65%) 신학기 인기 브랜드 쥬크.CC콜렉트.듀엘.모조에스핀 NEW LOOK &amp; 특가 찬스!', '(이월상품 최대 10%) 믿고 사는 내셔널지오그래픽 아우터, 백팩 23년 S/S 신상 오픈! 이월~10% 할인까지', '(BEST 할인전) 백화점 프리미엄 뉴시즌 페어 신세계백화점 신학기 맞이 스포츠 인기 상품전']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>신학기 페스티벌</t>
+          <t>새학기 쓱배송으로 준비해 봄</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>매일 10% 쿠폰 + 신학기 준비는 SSG에서</t>
+          <t>간식/준비물부터 장보면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004100</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>신학기 FESTIVAL - 신학기 준비는 SSG에서</t>
+          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL - 신학기 준비는 SSG에서', '스마일클럽', '신학기 10% 쿠폰 받고 쇼핑 GO! (현재 페이지)', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '프레드페리 : 프레드페리 S머니 추가 혜택 신학기 패션 고민 끝! SSG 단독 할인', '나이키 : 나이키 공식 스토어 신학기 대전 늘 인기있는 나이키의 신상 운동화/의류 최대 45%off', '오니츠카타이거 : 오니츠카타이거 BEST 모음 프리미엄 인기 슈즈 제안 + 할인 쿠폰 혜택까지', '마리끌레르 : 신학기 선물 SSG 단독 기획 23SS 오픈! 마리끌레르 BEST 단독 추가 쿠폰 할인까지!', '토리버치 : 신학기 BEST 토리버치 선물 토리버치 시즌오프 최대 40% 세일', 'H&amp;M키즈: SSG 단독 유아동 전상품 10% 할인+무배 신학기 맞이! H&amp;M 유아동 전상품 10% 할인+무료배송', '무아스 : 신학기 준비 필수 아이방 꾸미기 인기 홈데코 시계/거울/액자/데코 최대할인', '푸딩이너웨어 : 아이를 위한 편안한 언더웨어 최대 20% 할인 + 사은품 증정', '모윰 : 어린이집 국민육아템 모윰 1DAY 특가전! SSG 단독 최대~60%OFF+사은품 증정!', '아이리스 : 신학기 아이리스 수납 특가전 BEST 1+1 수비르 수납모음 7% 쿠폰 포함', '프라다 : 입학 졸업 선물 명품 구매 찬스! 프라다/생로랑 外 자체 인하 + 즉시할인쿠폰까지', '젠하이저 : 신학기 선물 고민 끝! 젠하이저 IE200 신상품 런칭! 10% 쿠폰 혜택 추가 할인혜택까지', '(특가) 23년 신학기맞이 책가방 행사전 SSG 단독 책가방 포함 ~최대 50% OFF', '(최대 55%) 리바트 공부방 베스트 모음전 최대 할인 혜택+적립+리뷰 이벤트까지', '(최대 35%) 시몬스 인기상품 시크릿 최저가! 최대 35% 즉시할인, 100% 당첨 리뷰이벤트', '(최대 30%) 집중력 높여주는 인기 가드닝템 할인전 싱그러운 향기 가득! 생화/화분/조화 外 할인전', '(최대 50%) 신학기 신상 침구 모음전 신상 침구 ~50% OFF ! 새 이불로 꿀잠 자기', '(최대 65%) 신학기 인기 브랜드 쥬크.CC콜렉트.듀엘.모조에스핀 NEW LOOK &amp; 특가 찬스!', '(이월상품 최대 10%) 믿고 사는 내셔널지오그래픽 아우터, 백팩 23년 S/S 신상 오픈! 이월~10% 할인까지', '(BEST 할인전) 백화점 프리미엄 뉴시즌 페어 신세계백화점 신학기 맞이 스포츠 인기 상품전']</t>
+          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '하기스 50%', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '신학기 10% 쿠폰 받고 쇼핑 GO!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 간식부터 준비물까지 + 쓱배송 구매하고 응모하면 SSG 머니의 행운까지!', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Little SSG 베이비페어</t>
+          <t>오반장 위크</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>유아동~7% 쿠폰 + BEST 상품 제안</t>
+          <t>오반장 상품 20%쿠폰 5장 지급!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004276</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004407</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[0213~0219] Little SSG 베이비페어</t>
+          <t>(2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0213~0219] Little SSG 베이비페어', '스마일클럽', '유아동~7%쿠폰', '유아동 선착순 ~7% 쿠폰', '7% 상품쿠폰 : 2만원 이상 상품 구매시 최대 7천원 할인(선착순 5만장)', '쿠폰은 09시부터 선착순 발급 됩니다.', '쿠폰발급 및 사용 기간 :  2023년 2월 13일(월) 09시 00분 ~ 2월 19일(일) 23시 59분', '최대 ~40% 할인', '최대 40% 할인', '★블랑101XSSG★파격특가! 세탁세제/섬유유연제 최대 50%할인+ 사은품 증정', '★[엘라바/오케이베이비/와우컵/퓨어닷]★ SSG 스페셜 최대~48%OFF+단독핫딜헤택', '베이비페어 7% 할인찬스', '[닥스키즈/헤지스키즈/피터젠슨] 23SS신상 책가방특가+겨울의류 파이널세일! 최대55%할인', '[빈폴키즈][쿠폰혜택] 23SS 신상 BEST 책가방/상하의/맨투맨/팬츠/세트 모음', '베이비페어 4일간 스트롤러/스타더스트  10% OFF', '완구 네오센터 클리어런스 ★최대 40%특가★', '[5~15%다운쿠폰]후디스 이유식/그릭요거트/두유 브랜드위크', '[쓱배송]킨도 기저귀 모음전']</t>
+          <t>['이벤트/쿠폰 &gt; (2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄', '하기스 50%', '스마일클럽', '오반장 상품 20%쿠폰 X 5장 지급!', '오반장위크 특별혜택! 20% 상품쿠폰 X 5장 바로보기', '오반장 상품 전용 20%쿠폰 x5장', '스마일클럽 전용 / 매일 오전 9시 선착순 2만명 / x5장', '쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '쿠폰 발급 기간 : 2023년 2월 16일(목) ~ 2023년 2월 22일(수)', '쿠폰 사용 기간 : 쿠폰 발급받은 당일 사용 필수', '쿠폰 1장당 대상상품 1개 수량에 한정하여 20% 할인 적용, 최대 3,000원 할인', '발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '  최대 35% \xa0', '  최대 15% \xa0', '  최대 30% \xa0', '  최대 40% \xa0', '  최대 32% \xa0', '  최대 12% \xa0', '  최대 50% \xa0', '  최대 16% \xa0', '  최대 33% \xa0', '  최대 43% \xa0', '  최대 19% \xa0', '  최대 29% \xa0', '  최대 23% \xa0', '  30% \xa0', '  55% \xa0', '  20% \xa0', '  20%/1+1 \xa0', '  최대 70% \xa0', '  최대 10% \xa0', '  최대 34% \xa0', '  최대 28% \xa0', '  최대 45% \xa0', '  25% \xa0', '  34% \xa0', '  최대 60% \xa0', '  최대 20% \xa0', '  40% \xa0', '  최대 36% \xa0', '  최대33% \xa0', '  최대 39% \xa0', '오반장 상품 전용 20%쿠폰 5장이 발급되었습니다. 즐거운 쇼핑 되세요!', '이미 발급된 쿠폰입니다. [MY - 쿠폰]을 확인해보세요.', '멤버십 전용 쿠폰입니다. 스마일클럽에 가입하고 더 많은 혜택을 누려보세요.', '스마일클럽 가입하기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>선물은 사랑을 싣고</t>
+          <t>Little SSG 베이비페어</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>선물한 사연 댓글달고 경품의 행운까지!</t>
+          <t>유아동~7% 쿠폰 + BEST 상품 제안</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004276</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[0202-0226] 선물은 사랑을 싣고</t>
+          <t>[0213~0219] Little SSG 베이비페어</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0202-0226] 선물은 사랑을 싣고', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일쿠폰', '모바일쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '로맨틱 발렌타인 - 최대 10% 할인쿠폰팩 + BEST GIFT 추천']</t>
+          <t>['이벤트/쿠폰 &gt; [0213~0219] Little SSG 베이비페어', '하기스 50%', '스마일클럽', '유아동~7%쿠폰', '유아동 선착순 ~7% 쿠폰', '7% 상품쿠폰 : 2만원 이상 상품 구매시 최대 7천원 할인(선착순 5만장)', '쿠폰은 09시부터 선착순 발급 됩니다.', '쿠폰발급 및 사용 기간 :  2023년 2월 13일(월) 09시 00분 ~ 2월 19일(일) 23시 59분', '최대 ~40% 할인', '최대 40% 할인', '★블랑101XSSG★파격특가! 세탁세제/섬유유연제 최대 50%할인+ 사은품 증정', '★[모윰 1DAY]★ 국민 육아템 디자인 에디션 젖병/치발기/쪽쪽이 외 출산용품 모음전~60%OFF', '★[엘라바/오케이베이비/와우컵/퓨어닷]★ SSG 스페셜 최대~48%OFF+단독핫딜헤택', '베이비페어 7% 할인찬스', '[닥스키즈/헤지스키즈]새학기 책가방특가+봄신상/겨울 의류 파이널세일! 최대55%할인', '[빈폴키즈][쿠폰혜택] 23SS 신상 신학기 책가방/상하의/맨투맨/팬츠/세트 모음', '베이비페어 4일간 스트롤러/스타더스트  10% OFF', '완구 네오센터 클리어런스 ★최대 40%특가★', '[5~15%다운쿠폰]후디스 이유식/그릭요거트/두유 브랜드위크', '[쓱배송]킨도 기저귀 모음전']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>든든한 소고기 한 상</t>
+          <t>쓱-선물로 응원해!</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>한우 ~40%할인부터 SSG머니 행운까지</t>
+          <t>선물한 사연 응모하고 내 선물도 쓱</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004312</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지</t>
+          <t>[0215-0226] 쓱-선물로 응원해!</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '스마일클럽', '(집밥 챌린지 : 소고기편) 든든한 소고기 한 상 _댓글이벤트까지', '이번 주는 든든하게 소고기 먹고 겨울 마무리! 최대 40할인 한우 행사상품부터 빠르고 손쉬운 소고기 간편식품까지!최애 소고기 요리 댓글달면 SSG머니 행운이!', '최대 40% 할인! 한우/소고기 추천 상품 바로보기', '        My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '        이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '최대 40% 할인!']</t>
+          <t>['이벤트/쿠폰 &gt; [0215-0226] 쓱-선물로 응원해!', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일 쿠폰', '모바일 쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>미식구매 할인찬스 피코크 위크</t>
+          <t>민지의 장바구니-곶감 &amp; k-디저트</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>간편하고 맛있는 피코크로 든든한 하루 ~ 30%</t>
+          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004175&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004387</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>미식체험 할인찬스 피코크 위크</t>
+          <t>민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-02-03</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 미식체험 할인찬스 피코크 위크', '스마일클럽', '미식체험 할인찬스 피코크 위크', '최대 50% / 1+1 / 2+1', '~30%/ 2+1 구매찬스', '[피코크] 피콕분식 신당동식떡볶이 970g 신당동 떡볶이를 간편하게 원가 8,480원 &gt; 할인가 5,936원', '[피코크] 한옥집 김치찜 500g 서대문 맛집의 비법을 그대로 원가 7,980원 &gt; 할인가 5,586원', '~30% 할인특가 대표상품', '피코크 자연치즈를 99% 담은 모짜렐라 슈레드치즈 300g(피자치즈)', '피코크 자연치즈를 99% 담은 고다&amp;체다 슈레드치즈 500g(피자치즈)']</t>
+          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)', '하기스 50%', '스마일클럽', 'SSG MONEY 1천원 (500명)', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       - ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       - 이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '라이브 특가 놓쳐서 아쉽다면\xa0 최대 55% 할인!']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 2월 깜짝 특별전</t>
+          <t>만원상점 알쓸쓱템</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>신선&amp;가공식품 ~70%할인</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004412</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
+          <t>만원상점 알뜰쓱템</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -762,103 +762,103 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 만원상점 알뜰쓱템', '하기스 50%', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+          <t>2023 대한민국 수산대전 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2월의신규 가입 혜택</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '하기스 50%', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 삼성</t>
+          <t>스마일클럽 가입 축하 5천원 기프트</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>비스포크 제트 무선청소기 220w ~28% 할인</t>
+          <t>명절 선물세트 ~15% 2종 할인까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004364</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 삼성</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 삼성', '스마일클럽', '더 강력하고 더 가벼워진 210W 최경량 청소기 놀랄만큼 강력해진 흡입력으로 더욱 쉽고 효율적이게, 모터는 기존 대비 47% 더 가벼워진 무게로 더욱 빠른 회전 최적의 구조로 에너지 효율을 높여 최고 210W의 강력한 흡입력까지!', '       비스포크 무선 / 로봇 청소기 인기 모델 최대 28% OFF']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', '쿠폰 받으러 가기']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>먼데이문 3rd ANNIVERSARY</t>
+          <t>SSG 브랜드 스포트라이트: 삼성</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>뷰티 전용 ~15% 쿠폰부터 브랜드 특가전, 체험단까지!</t>
+          <t>비스포크 제트 무선청소기 220w ~28% 할인</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004305</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004364</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY</t>
+          <t>SSG 브랜드 스포트라이트 - 삼성</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -873,66 +873,66 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY', '스마일클럽', '먼데이문 3주년을 맞아 준비한 최대 15% 상품쿠폰 3종 + 브랜드 특가전 + 체험단', '뷰티 전용 최대 15% 쿠폰 바로보기', '원하는 날 빠르게 뷰티 쓱배송 바로보기', '먼데이문 3주년 기념 쿠폰 3종', '뷰티 최대 15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '3만원 이상 상품 구매시 최대 1만 2천원 할인 (신세계백화점몰/시코르)', '선착순 쿠폰 Soldout!', '트렌드뷰티 최대5% 상품쿠폰', '2만원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '       쿠폰 발급 및 사용 기간', '       쿠폰 사용 조건', '       각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '15% 상품쿠폰', '1원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '케라스타즈케라스타즈 봄 담은 헤어&amp;두피 케어 - 10% 할인&amp;럭셔리 케어 증정 보러가기', '닥터지닥터지 국민크림 블랙스네일 外 - BEST 최대89% SALE + 쿠폰&amp;증정 혜택 보러가기', '더바디샵더바디샵 X 조규성 SELF LOVE - 최대 35% 즉시할인 + 15% 더블쿠폰 + 사은품 증정 보러가기', '베스트셀러 증정 응모 이벤트 등 쏟아지는 혜택', '프란츠프리미엄 안티에이징 프란츠 - 줄기세포 앰플/토너 외 BEST 스킨&amp;선케어 최대35% SALE 보러가기', '삐아삐아 - UP TO 29% + 쿠폰 15% + 사은품 증정 보러가기', '비프리지친 피부에 진정과 수분을 더하는 비프리 - BEST 스킨케어&amp;클렌징 최대 40% + 스타벅스 기프티콘 보러가기', '트리셀나를 더욱 나답게, 라이프스타일 브랜드 트리셀 - 전품목 UP TO 57% + 다다익선 10% + 사은품 증정 보러가기', '뷰티 상품도 쓱배송']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 삼성', '하기스 50%', '스마일클럽', '더 강력하고 더 가벼워진 210W 최경량 청소기 놀랄만큼 강력해진 흡입력으로 더욱 쉽고 효율적이게, 모터는 기존 대비 47% 더 가벼워진 무게로 더욱 빠른 회전 최적의 구조로 에너지 효율을 높여 최고 210W의 강력한 흡입력까지!', '       비스포크 무선 / 로봇 청소기 인기 모델 최대 28% OFF']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>봄꽃 여행 특가 위크</t>
+          <t>신세계백화점몰 ~50% 쿠폰</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>제주/도쿄/오사카 봄 여행 준비! ~5만원 패키지 즉시 할인 + 항공권 특가</t>
+          <t>해피반값데이 스페셜 웰컴혜택</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004326</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004356</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>봄꽃 여행 특가 위크</t>
+          <t>[해피반값쿠폰] 신세계백화점 구매 고객님을 위한 스페셜 혜택</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 봄꽃 여행 특가 위크', '스마일클럽', '최대 5만원 할인', '국제선 ~5만원 할인', '12% 단독 할인', '카드 청구 할인', '여행 전 상품 최대 5만원 할인', "프로모션 내용:  SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 4천원/1만원/2만원/5만원 즉시할인", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '사용방법행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '사용 방법:요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '봄 여행, 할인 받고 여기어때?', '해비치 호텔&amp;리조트 정상가 : 209,088원 &gt; 할인가 : 183,997원', '라마다 프라자 제주 호텔 정상가 : 158,119원 &gt; 할인가 : 139,145원', '메종 글래드 제주 정상가 : 134,500원 &gt; 할인가 : 118,360원', '썬앤문 리조트 정상가 : 198,000원 &gt; 할인가 : 174,240원', '제주 나인리조트 정상가 : 90,000원 &gt; 할인가 : 79,200원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 59,400원', '풀빌라 소랑 제주 정상가 : 84,000원 &gt; 할인가 : 73,920원', '탐라스테이 호텔 정상가 : 75,650원 &gt; 할인가 : 66,572원', '시그니엘 부산 정상가 : 321,860원 &gt; 할인가 : 291,860원', '웨스틴 조선 부산 정상가 : 261,360원 &gt; 할인가 : 231,360원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 197,472원', '아난티 힐튼 부산 정상가 : 363,000원 &gt; 할인가 : 333,000원', '펠릭스 by STX 호텔앤스위트 정상가 : 73,600원 &gt; 할인가 : 64,768원', '라마다 앙코르 바이 윈덤 부산 해운대 정상가 : 70,000원 &gt; 할인가 : 61,600원', '부산 코모도호텔 정상가 : 69,000원 &gt; 할인가 : 60,720원', '호텔 아쿠아펠리스 정상가 : 90,000원 &gt; 할인가 : 79,200원', '레고랜드 코리아 리조트 정상가 : 297,000원 &gt; 할인가 : 267,000원', '르네블루 바이 워커힐 정상가 : 190,000원 &gt; 할인가 : 167,200원', '소노캄 델피노 AB동 정상가 : 162,000원 &gt; 할인가 : 142,560원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '금강산콘도 정상가 : 45,650원 &gt; 할인가 : 40,172원', '디그니티 호텔 정상가 : 90,000원 &gt; 할인가 : 79,200원', '아비오 호텔 정상가 : 72,624원 &gt; 할인가 : 63,909원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 79,000원 &gt; 할인가 : 69,520원', '여수 라테라스 리조트 정상가 : 109,000원 &gt; 할인가 : 95,920원', '여수예술랜드 정상가 : 130,000원 &gt; 할인가 : 114,400원', '헤이븐 호텔 정상가 : 56,709원 &gt; 할인가 : 49,904원', '여수 하이락리조트 정상가 : 85,500원 &gt; 할인가 : 75,240원', '쏠비치 진도 리조트 정상가 : 151,000원 &gt; 할인가 : 132,880원', '클럽이에스 제천리조트 정상가 : 135,000원 &gt; 할인가 : 118,800원', '무주 나봄리조트 정상가 : 70,000원 &gt; 할인가 : 61,600원', '목포 어반 호텔 정상가 : 65,000원 &gt; 할인가 : 57,200원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 316,500원', '콘래드 서울 정상가 : 451,000원 &gt; 할인가 : 421,000원', '골든튤립 인천공항 호텔&amp;스위트 정상가 : 83,591원 &gt; 할인가 : 73,560원', '제이앤파크 호텔 정상가 : 147,999원 &gt; 할인가 : 130,239원', '레스케이프 정상가 : 175,248원 &gt; 할인가 : 154,218원', '노보텔 앰배서더 서울 용산 정상가 : 174,000원 &gt; 할인가 : 153,120원', '스위스 그랜드 호텔 정상가 : 205,000원 &gt; 할인가 : 180,400원', 'L7 강남 바이 롯데 정상가 : 148,330원 &gt; 할인가 : 130,530원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Ed2 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 신세계백화점 구매 고객님을 위한 스페셜 혜택', '하기스 50%', '스마일클럽', '[해피반값쿠폰] 신세계백화점 구매 고객님을 위한 스페셜 혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '(신세계 백화점몰 전용)(선착순 3만장) 50% 할인쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 3만명에게 한정 수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직년 1년간(22년 2월 15일 이후 부터 발급시점) SSG.COM 신세계백화점몰 상품 구매 이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 2만원 이상 구매 시 최대 1만원 할인되며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛 위크  : S/S NEW ARRIVALS</t>
+          <t>먼데이문 3rd ANNIVERSARY</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
+          <t>뷰티 전용 ~15% 쿠폰부터 브랜드 특가전, 체험단까지!</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004363</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004305</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[0213-0219] 프리미엄 아울렛 위크</t>
+          <t>[0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -947,192 +947,192 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0213-0219] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 2월 할인 대전', '최대 10% 할인 쿠폰 혜택', '[여성 패션 - 최대 70% 할인] 온앤온/ 나이스클랍/ 랩 브랜드 위크 外 보러가기', '[언더웨어 - 최대 70% 할인] 라페어/ 비너스/ 바바라/ 트라이엄프 특가 外 보러가기', '[명품잡화 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[스포츠 - 최대 70% 할인] 내셔널지오그래픽 등 아웃도어 브랜드 위크 보러가기', '[패션잡화 - 최대 37% 할인] 발렌타인데이 기념 - 전품목 30% OFF 보러가기', '[패션 슈즈 - 최대 80% 할인] 슈즈 판매 랭킹 TOP 300 인기상품 특가 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 80% 할인] 라코스테, 지프 등 캐주얼 특가 外 보러가기', '[키즈패션 - 최대 60% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 70% 할인] 테팔 브랜드위크! 매직핸드 外 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; [0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY', '하기스 50%', '스마일클럽', '먼데이문 3주년을 맞아 준비한 최대 15% 상품쿠폰 3종 + 브랜드 특가전 + 체험단', '뷰티 전용 최대 15% 쿠폰 바로보기', '원하는 날 빠르게 뷰티 쓱배송 바로보기', '먼데이문 3주년 기념 쿠폰 3종', '뷰티 최대 15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '3만원 이상 상품 구매시 최대 1만 2천원 할인 (신세계백화점몰/시코르)', '선착순 쿠폰 Soldout!', '트렌드뷰티 최대5% 상품쿠폰', '2만원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '       쿠폰 발급 및 사용 기간', '       쿠폰 사용 조건', '       각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '15% 상품쿠폰', '1원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '케라스타즈케라스타즈 봄 담은 헤어&amp;두피 케어 - 10% 할인&amp;럭셔리 케어 증정 보러가기', '닥터지닥터지 국민크림 블랙스네일 外 - BEST 최대89% SALE + 쿠폰&amp;증정 혜택 보러가기', '더바디샵더바디샵 X 조규성 SELF LOVE - 최대 35% 즉시할인 + 15% 더블쿠폰 + 사은품 증정 보러가기', '베스트셀러 증정 응모 이벤트 등 쏟아지는 혜택', '프란츠프리미엄 안티에이징 프란츠 - 줄기세포 앰플/토너 외 BEST 스킨&amp;선케어 최대35% SALE 보러가기', '삐아삐아 - UP TO 29% + 쿠폰 15% + 사은품 증정 보러가기', '비프리지친 피부에 진정과 수분을 더하는 비프리 - BEST 스킨케어&amp;클렌징 최대 40% + 스타벅스 기프티콘 보러가기', '트리셀나를 더욱 나답게, 라이프스타일 브랜드 트리셀 - 전품목 UP TO 57% + 다다익선 10% + 사은품 증정 보러가기', '뷰티 상품도 쓱배송']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>봄꽃 여행 특가 위크</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>제주/도쿄/오사카 봄 여행 준비! ~5만원 패키지 즉시 할인 + 항공권 특가</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004326</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>봄꽃 여행 특가 위크</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 봄꽃 여행 특가 위크', '스마일클럽', '최대 5만원 할인', '국제선 ~5만원 할인', '12% 단독 할인', '카드 청구 할인', '여행 전 상품 최대 5만원 할인', "프로모션 내용:  SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 4천원/1만원/2만원/5만원 즉시할인", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '사용방법행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '사용 방법:요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 실시간 호텔 전 상품 1원 이상 구매 시 12% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '봄 여행, 할인 받고 여기어때?', '해비치 호텔&amp;리조트 정상가 : 209,088원 &gt; 할인가 : 183,997원', '라마다 프라자 제주 호텔 정상가 : 158,119원 &gt; 할인가 : 139,145원', '메종 글래드 제주 정상가 : 134,500원 &gt; 할인가 : 118,360원', '썬앤문 리조트 정상가 : 198,000원 &gt; 할인가 : 174,240원', '제주 나인리조트 정상가 : 90,000원 &gt; 할인가 : 79,200원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 59,400원', '풀빌라 소랑 제주 정상가 : 84,000원 &gt; 할인가 : 73,920원', '탐라스테이 호텔 정상가 : 75,650원 &gt; 할인가 : 66,572원', '시그니엘 부산 정상가 : 321,860원 &gt; 할인가 : 291,860원', '웨스틴 조선 부산 정상가 : 261,360원 &gt; 할인가 : 231,360원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 197,472원', '아난티 힐튼 부산 정상가 : 363,000원 &gt; 할인가 : 333,000원', '펠릭스 by STX 호텔앤스위트 정상가 : 73,600원 &gt; 할인가 : 64,768원', '라마다 앙코르 바이 윈덤 부산 해운대 정상가 : 70,000원 &gt; 할인가 : 61,600원', '부산 코모도호텔 정상가 : 69,000원 &gt; 할인가 : 60,720원', '호텔 아쿠아펠리스 정상가 : 90,000원 &gt; 할인가 : 79,200원', '레고랜드 코리아 리조트 정상가 : 297,000원 &gt; 할인가 : 267,000원', '르네블루 바이 워커힐 정상가 : 190,000원 &gt; 할인가 : 167,200원', '소노캄 델피노 AB동 정상가 : 162,000원 &gt; 할인가 : 142,560원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '금강산콘도 정상가 : 45,650원 &gt; 할인가 : 40,172원', '디그니티 호텔 정상가 : 90,000원 &gt; 할인가 : 79,200원', '아비오 호텔 정상가 : 72,624원 &gt; 할인가 : 63,909원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 79,000원 &gt; 할인가 : 69,520원', '여수 라테라스 리조트 정상가 : 109,000원 &gt; 할인가 : 95,920원', '여수예술랜드 정상가 : 130,000원 &gt; 할인가 : 114,400원', '헤이븐 호텔 정상가 : 56,709원 &gt; 할인가 : 49,904원', '여수 하이락리조트 정상가 : 85,500원 &gt; 할인가 : 75,240원', '쏠비치 진도 리조트 정상가 : 151,000원 &gt; 할인가 : 132,880원', '클럽이에스 제천리조트 정상가 : 135,000원 &gt; 할인가 : 118,800원', '무주 나봄리조트 정상가 : 70,000원 &gt; 할인가 : 61,600원', '목포 어반 호텔 정상가 : 65,000원 &gt; 할인가 : 57,200원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 316,500원', '콘래드 서울 정상가 : 451,000원 &gt; 할인가 : 421,000원', '골든튤립 인천공항 호텔&amp;스위트 정상가 : 83,591원 &gt; 할인가 : 73,560원', '제이앤파크 호텔 정상가 : 147,999원 &gt; 할인가 : 130,239원', '레스케이프 정상가 : 175,248원 &gt; 할인가 : 154,218원', '노보텔 앰배서더 서울 용산 정상가 : 174,000원 &gt; 할인가 : 153,120원', '스위스 그랜드 호텔 정상가 : 205,000원 &gt; 할인가 : 180,400원', 'L7 강남 바이 롯데 정상가 : 148,330원 &gt; 할인가 : 130,530원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Ed2 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>프리미엄 아울렛 위크  : S/S NEW ARRIVALS</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004363</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[0213-0219] 프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-02-13</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [0213-0219] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 2월 할인 대전', '최대 10% 할인 쿠폰 혜택', '[여성 패션 - 최대 70% 할인] 온앤온/ 나이스클랍/ 랩 브랜드 위크 外 보러가기', '[언더웨어 - 최대 70% 할인] 라페어/ 비너스/ 바바라/ 트라이엄프 특가 外 보러가기', '[명품잡화 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[스포츠 - 최대 70% 할인] 내셔널지오그래픽 등 아웃도어 브랜드 위크 보러가기', '[패션잡화 - 최대 37% 할인] 발렌타인데이 기념 - 전품목 30% OFF 보러가기', '[패션 슈즈 - 최대 80% 할인] 슈즈 판매 랭킹 TOP 300 인기상품 특가 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 80% 할인] 라코스테, 지프 등 캐주얼 특가 外 보러가기', '[키즈패션 - 최대 60% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 70% 할인] 테팔 브랜드위크! 매직핸드 外 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>괌 여행(롯데관광) 2/13(월) 8PM</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>50만원상당혜택포함 괌 특급 롯데호텔 클럽룸UP 4/5일 초특가</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004320</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>괌 여행(롯데관광) @SSG.LIVE 2/13(화) 8PM</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 괌 여행(롯데관광) @SSG.LIVE 2/13(화) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>캐치티니핑 2/14(화) 10AM</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>첫 라이브 기념 ~40% 특가! 100% 증정사은품 까지</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004239&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[쓱라이브] 캐치티니핑 2/14(화)10AM</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-02-17</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 캐치티니핑 2/14(화)10AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>아르마니 뷰티 2/14(화) 8PM</t>
+          <t>선원규 곶감 2/16(목) 11AM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>NEW 립 마에스트로 사틴 최.초.공.개! 듀오세트 핫딜구성&amp;선착순 600명 립 미니어처 증정</t>
+          <t>명인의 곶감, 선착순 1천개 최대 73% 핫딜</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004270</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004325</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]2/14(화) 8PM 아르마니뷰티</t>
+          <t>선원규 곶감 @SSG.LIVE 2/16(목) 11:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-02-08</t>
+          <t>2023-02-07</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]2/14(화) 8PM 아르마니뷰티', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 선원규 곶감 @SSG.LIVE 2/16(목) 11:00', '스마일클럽', '                    \xa0\xa0 SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Feb 20 00:23:30 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,66 +503,66 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫구매는 반값다딜 (2/16~22)', '하기스 50%', '스마일클럽', '첫구매는 반값다딜 (2/16~22)', '화장지,밀키트 총 1.5만원 할인+무료배송', '반값 할인쿠폰팩', '첫구매 전용 특별 메뉴 반값 할인 쿠폰팩', '첫구매 전용특별 메뉴', ' 마침 필요하셨죠? 화장지 선상품 1만원 할인 최대할인금액 1만원 ', ' 오늘 저녁 고민 끝! 밀키트 전상품 5천원 할인 최대할인금액 5천원 ', '반값메뉴는 무료배송으로 즐겨야죠', '상품쿠폰 50% 이마트몰 무료배송', '첫구매 쿠폰팩 받기 -ID당 기간중 1회', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       -상품할인쿠폰, 무료배송쿠폰: 2023년 2월 16일(목) 2023년 2월 22일 (수)', '       쿠폰 적용 대상 상품', '-쓱배송 새벽배송 상품에 한해서 적용 가능', '-화장지 50% cat (최대 1만원 할인) 제지/위생용품, 화장지/물티슈, 화장지', '-밀키트 50% cat (최대 5천원 할인) 밀키트/간편식, 밀키트', '- 상품당 1개 수량에 쿠폰 적용 가능 : 화장지 1개, 밀키트 1개 적용 가능(ex. 화장지 2개 구매시에도 1개에만 적용 가능합니다.)', '       쿠폰 사용 조건', '-상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인 금액 적용', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상']</t>
+          <t>['이벤트/쿠폰 &gt; 첫구매는 반값다딜 (2/16~22)', '스마일클럽', '첫구매는 반값다딜 (2/16~22)', '화장지,밀키트 총 1.5만원 할인+무료배송', '반값 할인쿠폰팩', '첫구매 전용 특별 메뉴 반값 할인 쿠폰팩', '첫구매 전용특별 메뉴', ' 마침 필요하셨죠? 화장지 선상품 1만원 할인 최대할인금액 1만원 ', ' 오늘 저녁 고민 끝! 밀키트 전상품 5천원 할인 최대할인금액 5천원 ', '반값메뉴는 무료배송으로 즐겨야죠', '상품쿠폰 50% 이마트몰 무료배송', '첫구매 쿠폰팩 받기 -ID당 기간중 1회', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       -상품할인쿠폰, 무료배송쿠폰: 2023년 2월 16일(목) 2023년 2월 22일 (수)', '       쿠폰 적용 대상 상품', '-쓱배송 새벽배송 상품에 한해서 적용 가능', '-화장지 50% cat (최대 1만원 할인) 제지/위생용품, 화장지/물티슈, 화장지', '-밀키트 50% cat (최대 5천원 할인) 밀키트/간편식, 밀키트', '- 상품당 1개 수량에 쿠폰 적용 가능 : 화장지 1개, 밀키트 1개 적용 가능(ex. 화장지 2개 구매시에도 1개에만 적용 가능합니다.)', '       쿠폰 사용 조건', '-상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인 금액 적용', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>신학기 페스티벌</t>
+          <t>새학기 쓱배송으로 준비해 봄</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>매일 10% 쿠폰 + 신학기 준비는 SSG에서</t>
+          <t>간식/준비물부터 장보면 SSG머니 행운까지!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004100</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>신학기 FESTIVAL - 신학기 준비는 SSG에서</t>
+          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL - 신학기 준비는 SSG에서', '하기스 50%', '스마일클럽', '신학기 10% 쿠폰 받고 쇼핑 GO! (현재 페이지)', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '프레드페리 : 프레드페리 S머니 추가 혜택 신학기 패션 고민 끝! SSG 단독 할인', '나이키 : 나이키 공식 스토어 신학기 대전 늘 인기있는 나이키의 신상 운동화/의류 최대 45%off', '오니츠카타이거 : 오니츠카타이거 BEST 모음 프리미엄 인기 슈즈 제안 + 할인 쿠폰 혜택까지', '마리끌레르 : 신학기 선물 SSG 단독 기획 23SS 오픈! 마리끌레르 BEST 단독 추가 쿠폰 할인까지!', '토리버치 : 신학기 BEST 토리버치 선물 토리버치 시즌오프 최대 40% 세일', 'H&amp;M키즈: SSG 단독 유아동 전상품 10% 할인+무배 신학기 맞이! H&amp;M 유아동 전상품 10% 할인+무료배송', '무아스 : 신학기 준비 필수 아이방 꾸미기 인기 홈데코 시계/거울/액자/데코 최대할인', '푸딩이너웨어 : 아이를 위한 편안한 언더웨어 최대 20% 할인 + 사은품 증정', '모윰 : 어린이집 국민육아템 모윰 1DAY 특가전! SSG 단독 최대~60%OFF+사은품 증정!', '아이리스 : 신학기 아이리스 수납 특가전 BEST 1+1 수비르 수납모음 7% 쿠폰 포함', '프라다 : 입학 졸업 선물 명품 구매 찬스! 프라다/생로랑 外 자체 인하 + 즉시할인쿠폰까지', '젠하이저 : 신학기 선물 고민 끝! 젠하이저 IE200 신상품 런칭! 10% 쿠폰 혜택 추가 할인혜택까지', '(특가) 23년 신학기맞이 책가방 행사전 SSG 단독 책가방 포함 ~최대 50% OFF', '(최대 55%) 리바트 공부방 베스트 모음전 최대 할인 혜택+적립+리뷰 이벤트까지', '(최대 35%) 시몬스 인기상품 시크릿 최저가! 최대 35% 즉시할인, 100% 당첨 리뷰이벤트', '(최대 30%) 집중력 높여주는 인기 가드닝템 할인전 싱그러운 향기 가득! 생화/화분/조화 外 할인전', '(최대 50%) 신학기 신상 침구 모음전 신상 침구 ~50% OFF ! 새 이불로 꿀잠 자기', '(최대 65%) 신학기 인기 브랜드 쥬크.CC콜렉트.듀엘.모조에스핀 NEW LOOK &amp; 특가 찬스!', '(이월상품 최대 10%) 믿고 사는 내셔널지오그래픽 아우터, 백팩 23년 S/S 신상 오픈! 이월~10% 할인까지', '(BEST 할인전) 백화점 프리미엄 뉴시즌 페어 신세계백화점 신학기 맞이 스포츠 인기 상품전']</t>
+          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '신학기 10% 쿠폰 받고 쇼핑 GO!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 간식부터 준비물까지 + 쓱배송 구매하고 응모하면 SSG 머니의 행운까지!', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>새학기 쓱배송으로 준비해 봄</t>
+          <t>오반장 위크</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>간식/준비물부터 장보면 SSG머니 행운까지!</t>
+          <t>오반장 상품 20%쿠폰 5장 지급!</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004407</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
+          <t>(2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,145 +572,145 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '하기스 50%', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '신학기 10% 쿠폰 받고 쇼핑 GO!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 간식부터 준비물까지 + 쓱배송 구매하고 응모하면 SSG 머니의 행운까지!', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
+          <t>['이벤트/쿠폰 &gt; (2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄', '스마일클럽', '오반장 상품 20%쿠폰 X 5장 지급!', '오반장위크 특별혜택! 20% 상품쿠폰 X 5장 바로보기', '오반장 상품 전용 20%쿠폰 x5장', '스마일클럽 전용 / 매일 오전 9시 선착순 2만명 / x5장', '쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '쿠폰 발급 기간 : 2023년 2월 16일(목) ~ 2023년 2월 22일(수)', '쿠폰 사용 기간 : 쿠폰 발급받은 당일 사용 필수', '쿠폰 1장당 대상상품 1개 수량에 한정하여 20% 할인 적용, 최대 3,000원 할인', '발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '  최대 35% \xa0', '  최대 15% \xa0', '  최대 30% \xa0', '  최대 40% \xa0', '  최대 32% \xa0', '  최대 12% \xa0', '  최대 50% \xa0', '  최대 16% \xa0', '  최대 33% \xa0', '  최대 43% \xa0', '  최대 19% \xa0', '  최대 29% \xa0', '  최대 23% \xa0', '  30% \xa0', '  55% \xa0', '  20% \xa0', '  20%/1+1 \xa0', '  최대 70% \xa0', '  최대 10% \xa0', '  최대 34% \xa0', '  최대 28% \xa0', '  최대 45% \xa0', '  25% \xa0', '  34% \xa0', '  최대 60% \xa0', '  최대 20% \xa0', '  40% \xa0', '  최대 36% \xa0', '  최대33% \xa0', '  최대 39% \xa0', '오반장 상품 전용 20%쿠폰 5장이 발급되었습니다. 즐거운 쇼핑 되세요!', '이미 발급된 쿠폰입니다. [MY - 쿠폰]을 확인해보세요.', '멤버십 전용 쿠폰입니다. 스마일클럽에 가입하고 더 많은 혜택을 누려보세요.', '스마일클럽 가입하기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>오반장 위크</t>
+          <t>신학기 준비 한번에 끝!</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>오반장 상품 20%쿠폰 5장 지급!</t>
+          <t>입학&amp;졸업 선물부터 신학기 패션까지, 금주의 신학기 페스티벌</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004407</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004304&amp;cacheCmd=pass</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄</t>
+          <t>신학기 FESTIVAL: 3월 새학기 준비 끝!</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-20</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄', '하기스 50%', '스마일클럽', '오반장 상품 20%쿠폰 X 5장 지급!', '오반장위크 특별혜택! 20% 상품쿠폰 X 5장 바로보기', '오반장 상품 전용 20%쿠폰 x5장', '스마일클럽 전용 / 매일 오전 9시 선착순 2만명 / x5장', '쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '쿠폰 발급 기간 : 2023년 2월 16일(목) ~ 2023년 2월 22일(수)', '쿠폰 사용 기간 : 쿠폰 발급받은 당일 사용 필수', '쿠폰 1장당 대상상품 1개 수량에 한정하여 20% 할인 적용, 최대 3,000원 할인', '발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '  최대 35% \xa0', '  최대 15% \xa0', '  최대 30% \xa0', '  최대 40% \xa0', '  최대 32% \xa0', '  최대 12% \xa0', '  최대 50% \xa0', '  최대 16% \xa0', '  최대 33% \xa0', '  최대 43% \xa0', '  최대 19% \xa0', '  최대 29% \xa0', '  최대 23% \xa0', '  30% \xa0', '  55% \xa0', '  20% \xa0', '  20%/1+1 \xa0', '  최대 70% \xa0', '  최대 10% \xa0', '  최대 34% \xa0', '  최대 28% \xa0', '  최대 45% \xa0', '  25% \xa0', '  34% \xa0', '  최대 60% \xa0', '  최대 20% \xa0', '  40% \xa0', '  최대 36% \xa0', '  최대33% \xa0', '  최대 39% \xa0', '오반장 상품 전용 20%쿠폰 5장이 발급되었습니다. 즐거운 쇼핑 되세요!', '이미 발급된 쿠폰입니다. [MY - 쿠폰]을 확인해보세요.', '멤버십 전용 쿠폰입니다. 스마일클럽에 가입하고 더 많은 혜택을 누려보세요.', '스마일클럽 가입하기']</t>
+          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL: 3월 새학기 준비 끝!', '스마일클럽', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '헤지스레이디스 : 헤지스레이디스 23 S/S 신상 인기 스타일 추가 쿠폰 혜택', '허먼밀러 : 허먼밀러 에어론체어 스페셜 제안 최대 15%할인 ', '까사미아 : 까사미아 신학기 가구 특가 최대 최대 30% 할인혜택', '키르시 : 키르시 인기 맨투맨/후드 단독 최대 50% 기간한정 추가 쿠폰 혜택까지!', 'A.P.C : 산뜻한 새출발을 위한 에센셜 명품 A.P.C/오트리/키츠네 외 최대 35%', '올젠 : SS/FW 인기아이템 최대 65% SALE 10% 추가할인 쿠폰 혜택', '내셔널지오그래픽 : 내셔널지오그래픽 키즈 신학기 오픈!! / 이월 최대 10% 쿠폰', '게스시계 : 게스 신학기 인기 워치 추천 SSG 단독 할인전 ~59% OFF', '닥스키즈/헤지스키즈 : 닥스키즈/헤지스키즈 외 우리아이 취향저격 새학기륵, 최대 60% off 행사', '프리즘 : 봄맞이 인기 조명 SALE 오늘 하루만 최대 할인', '나이키/아디다스/뉴발란스 : 봄신상 신학기 기획전 나이키/뉴발란스/아디다스잔스포츠 外 신학기 할인 모음', '나이키 : 나이키 신학기/봄맞이 특가 최대 44% 빅세일', '글라스락 : 글라스락 신학기 필수템 모음전 보관용기/텀블러 최대 65% OFF', '온앤온 : 23 SS 시즌오픈 NEW FASHION SSG 단독 할인 + 쿠폰혜택까지!', '아디다스 : 아디다스 23신상 스포츠가방 러닝화 슬리퍼 특가 아디다스 최대 40% 신학기 특가', '(신세계 단독 상품 특가 30%) 아동패션 TOP 브랜드 연합 책가방 특가전 신세계 단독상품 외 Top브랜드 상품 특가', '(최대 68% 할인!) SSG 유아동 신학기 페스티벌 행사 어린이집 등원준비 필수템 BEST 모음 ', '(최대 25%) 모던하우스 신학기 맞이 학생가구/침구/완구 BIG SALE 책상+의자 SET 구매시 상품권 증정', '(최대 30%) 까사미아 신학기 가구 특가 최대 30% 할인 혜택', '(네이버 최저가 특가) 신학기 맞이 인기 조명 할인전 인기 조명 최대 20% 할인', '(최대 30%) 신학기 맞이 템퍼 특별 할인전 기능성 베개/메트리스 특가+구매상품별 사은품 증정', '(30~50%) 프레드페리 SSG 단독 할인 상품+ 추가혜택!', '(20%) 스포츠 빅브랜드 신학기 기획전 뉴발란스/나이키/반스/디스커버리 外 신학기 할인 모음', '(40%) 토리버치 시즌오프 최대 40%세일 시즌오프 베스트 아이템']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Little SSG 베이비페어</t>
+          <t>쓱-선물로 응원해!</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>유아동~7% 쿠폰 + BEST 상품 제안</t>
+          <t>선물한 사연 응모하고 내 선물도 쓱</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004276</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[0213~0219] Little SSG 베이비페어</t>
+          <t>[0215-0226] 쓱-선물로 응원해!</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0213~0219] Little SSG 베이비페어', '하기스 50%', '스마일클럽', '유아동~7%쿠폰', '유아동 선착순 ~7% 쿠폰', '7% 상품쿠폰 : 2만원 이상 상품 구매시 최대 7천원 할인(선착순 5만장)', '쿠폰은 09시부터 선착순 발급 됩니다.', '쿠폰발급 및 사용 기간 :  2023년 2월 13일(월) 09시 00분 ~ 2월 19일(일) 23시 59분', '최대 ~40% 할인', '최대 40% 할인', '★블랑101XSSG★파격특가! 세탁세제/섬유유연제 최대 50%할인+ 사은품 증정', '★[모윰 1DAY]★ 국민 육아템 디자인 에디션 젖병/치발기/쪽쪽이 외 출산용품 모음전~60%OFF', '★[엘라바/오케이베이비/와우컵/퓨어닷]★ SSG 스페셜 최대~48%OFF+단독핫딜헤택', '베이비페어 7% 할인찬스', '[닥스키즈/헤지스키즈]새학기 책가방특가+봄신상/겨울 의류 파이널세일! 최대55%할인', '[빈폴키즈][쿠폰혜택] 23SS 신상 신학기 책가방/상하의/맨투맨/팬츠/세트 모음', '베이비페어 4일간 스트롤러/스타더스트  10% OFF', '완구 네오센터 클리어런스 ★최대 40%특가★', '[5~15%다운쿠폰]후디스 이유식/그릭요거트/두유 브랜드위크', '[쓱배송]킨도 기저귀 모음전']</t>
+          <t>['이벤트/쿠폰 &gt; [0215-0226] 쓱-선물로 응원해!', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일 쿠폰', '모바일 쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>쓱-선물로 응원해!</t>
+          <t>민지의 장바구니-곶감 &amp; k-디저트</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>선물한 사연 응모하고 내 선물도 쓱</t>
+          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004387</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[0215-0226] 쓱-선물로 응원해!</t>
+          <t>민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0215-0226] 쓱-선물로 응원해!', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일 쿠폰', '모바일 쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)', '스마일클럽', 'SSG MONEY 1천원 (500명)', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       - ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       - 이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '라이브 특가 놓쳐서 아쉽다면\xa0 최대 55% 할인!']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>민지의 장바구니-곶감 &amp; k-디저트</t>
+          <t>만원상점 알뜰쓱템</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+          <t>신선&amp;가공식품 ~70%할인</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004387</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004412</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)</t>
+          <t>만원상점 알뜰쓱템</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -725,34 +725,34 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)', '하기스 50%', '스마일클럽', 'SSG MONEY 1천원 (500명)', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       - ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       - 이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '라이브 특가 놓쳐서 아쉽다면\xa0 최대 55% 할인!']</t>
+          <t>['이벤트/쿠폰 &gt; 만원상점 알뜰쓱템', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>만원상점 알쓸쓱템</t>
+          <t>2023 대한민국 수산대전 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>신선&amp;가공식품 ~70%할인</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004412</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>만원상점 알뜰쓱템</t>
+          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -762,377 +762,229 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 만원상점 알뜰쓱템', '하기스 50%', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 2월 깜짝 특별전</t>
+          <t>오반장위크멤버십 ~20% 추가할인</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>스마일클럽처음이라면? 5천원쿠폰</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '하기스 50%', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', '쿠폰 받으러 가기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>스마일클럽 가입 축하 5천원 기프트</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>명절 선물세트 ~15% 2종 할인까지</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', '쿠폰 받으러 가기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 삼성</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>비스포크 제트 무선청소기 220w ~28% 할인</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004364</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 삼성</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 삼성', '하기스 50%', '스마일클럽', '더 강력하고 더 가벼워진 210W 최경량 청소기 놀랄만큼 강력해진 흡입력으로 더욱 쉽고 효율적이게, 모터는 기존 대비 47% 더 가벼워진 무게로 더욱 빠른 회전 최적의 구조로 에너지 효율을 높여 최고 210W의 강력한 흡입력까지!', '       비스포크 무선 / 로봇 청소기 인기 모델 최대 28% OFF']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>신세계백화점몰 ~50% 쿠폰</t>
+          <t>JJ지고트 2/20(월) 8PM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>해피반값데이 스페셜 웰컴혜택</t>
+          <t>JJ지고트 봄 신상&amp;이월 상품 ~87%OFF</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004356</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004465&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[해피반값쿠폰] 신세계백화점 구매 고객님을 위한 스페셜 혜택</t>
+          <t>JJ지고트 @SSG.LIVE 2/20(월) 8PM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-14</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-20</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 신세계백화점 구매 고객님을 위한 스페셜 혜택', '하기스 50%', '스마일클럽', '[해피반값쿠폰] 신세계백화점 구매 고객님을 위한 스페셜 혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '(신세계 백화점몰 전용)(선착순 3만장) 50% 할인쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 3만명에게 한정 수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직년 1년간(22년 2월 15일 이후 부터 발급시점) SSG.COM 신세계백화점몰 상품 구매 이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 2만원 이상 구매 시 최대 1만원 할인되며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; JJ지고트 @SSG.LIVE 2/20(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>먼데이문 3rd ANNIVERSARY</t>
+          <t>스타우브 2/21(화) 8PM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>뷰티 전용 ~15% 쿠폰부터 브랜드 특가전, 체험단까지!</t>
+          <t>원형 꼬꼬떼 22cm 22만원대 한정수량 선착순 핫딜</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004305</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004459&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY</t>
+          <t>[쓱라이브] 스타우브 2/21(화)8PM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-25</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0213-0219] SSG 뷰티전문관 먼데이문 3rd ANNIVERSARY', '하기스 50%', '스마일클럽', '먼데이문 3주년을 맞아 준비한 최대 15% 상품쿠폰 3종 + 브랜드 특가전 + 체험단', '뷰티 전용 최대 15% 쿠폰 바로보기', '원하는 날 빠르게 뷰티 쓱배송 바로보기', '먼데이문 3주년 기념 쿠폰 3종', '뷰티 최대 15% 쿠폰', '럭셔리뷰티 최대 12% 상품쿠폰', '3만원 이상 상품 구매시 최대 1만 2천원 할인 (신세계백화점몰/시코르)', '선착순 쿠폰 Soldout!', '트렌드뷰티 최대5% 상품쿠폰', '2만원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '       쿠폰 발급 및 사용 기간', '       쿠폰 사용 조건', '       각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 최대 15% 상품쿠폰', '15% 상품쿠폰', '1원 이상 상품 구매시 최대 7천원 할인 (신세계몰/이마트몰)', '케라스타즈케라스타즈 봄 담은 헤어&amp;두피 케어 - 10% 할인&amp;럭셔리 케어 증정 보러가기', '닥터지닥터지 국민크림 블랙스네일 外 - BEST 최대89% SALE + 쿠폰&amp;증정 혜택 보러가기', '더바디샵더바디샵 X 조규성 SELF LOVE - 최대 35% 즉시할인 + 15% 더블쿠폰 + 사은품 증정 보러가기', '베스트셀러 증정 응모 이벤트 등 쏟아지는 혜택', '프란츠프리미엄 안티에이징 프란츠 - 줄기세포 앰플/토너 외 BEST 스킨&amp;선케어 최대35% SALE 보러가기', '삐아삐아 - UP TO 29% + 쿠폰 15% + 사은품 증정 보러가기', '비프리지친 피부에 진정과 수분을 더하는 비프리 - BEST 스킨케어&amp;클렌징 최대 40% + 스타벅스 기프티콘 보러가기', '트리셀나를 더욱 나답게, 라이프스타일 브랜드 트리셀 - 전품목 UP TO 57% + 다다익선 10% + 사은품 증정 보러가기', '뷰티 상품도 쓱배송']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 스타우브 2/21(화)8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>봄꽃 여행 특가 위크</t>
+          <t>2023 뷰티 미리 '봄'</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>제주/도쿄/오사카 봄 여행 준비! ~5만원 패키지 즉시 할인 + 항공권 특가</t>
+          <t>봄맞이 화사함을 더해줄, 럭셔리 뷰티 아이템</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004326</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004454</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>봄꽃 여행 특가 위크</t>
+          <t>[2/20-26] 2023 명품화장품 쓱- 미리 '봄'</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-02-20</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-02-19</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 봄꽃 여행 특가 위크', '스마일클럽', '최대 5만원 할인', '국제선 ~5만원 할인', '12% 단독 할인', '카드 청구 할인', '여행 전 상품 최대 5만원 할인', "프로모션 내용:  SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 4천원/1만원/2만원/5만원 즉시할인", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '사용방법행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', "할인 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '사용 방법:요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 실시간 호텔 전 상품 1원 이상 구매 시 12% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '봄 여행, 할인 받고 여기어때?', '해비치 호텔&amp;리조트 정상가 : 209,088원 &gt; 할인가 : 183,997원', '라마다 프라자 제주 호텔 정상가 : 158,119원 &gt; 할인가 : 139,145원', '메종 글래드 제주 정상가 : 134,500원 &gt; 할인가 : 118,360원', '썬앤문 리조트 정상가 : 198,000원 &gt; 할인가 : 174,240원', '제주 나인리조트 정상가 : 90,000원 &gt; 할인가 : 79,200원', '브라운스위트 제주 호텔 정상가 : 67,500원 &gt; 할인가 : 59,400원', '풀빌라 소랑 제주 정상가 : 84,000원 &gt; 할인가 : 73,920원', '탐라스테이 호텔 정상가 : 75,650원 &gt; 할인가 : 66,572원', '시그니엘 부산 정상가 : 321,860원 &gt; 할인가 : 291,860원', '웨스틴 조선 부산 정상가 : 261,360원 &gt; 할인가 : 231,360원', '그랜드 조선 부산 정상가 : 224,400원 &gt; 할인가 : 197,472원', '아난티 힐튼 부산 정상가 : 363,000원 &gt; 할인가 : 333,000원', '펠릭스 by STX 호텔앤스위트 정상가 : 73,600원 &gt; 할인가 : 64,768원', '라마다 앙코르 바이 윈덤 부산 해운대 정상가 : 70,000원 &gt; 할인가 : 61,600원', '부산 코모도호텔 정상가 : 69,000원 &gt; 할인가 : 60,720원', '호텔 아쿠아펠리스 정상가 : 90,000원 &gt; 할인가 : 79,200원', '레고랜드 코리아 리조트 정상가 : 297,000원 &gt; 할인가 : 267,000원', '르네블루 바이 워커힐 정상가 : 190,000원 &gt; 할인가 : 167,200원', '소노캄 델피노 AB동 정상가 : 162,000원 &gt; 할인가 : 142,560원', '오크밸리리조트 정상가 : 241,500원 &gt; 할인가 : 212,520원', '금강산콘도 정상가 : 45,650원 &gt; 할인가 : 40,172원', '디그니티 호텔 정상가 : 90,000원 &gt; 할인가 : 79,200원', '아비오 호텔 정상가 : 72,624원 &gt; 할인가 : 63,909원', '양양 더 앤 리조트 호텔&amp;스파 정상가 : 79,000원 &gt; 할인가 : 69,520원', '여수 라테라스 리조트 정상가 : 109,000원 &gt; 할인가 : 95,920원', '여수예술랜드 정상가 : 130,000원 &gt; 할인가 : 114,400원', '헤이븐 호텔 정상가 : 56,709원 &gt; 할인가 : 49,904원', '여수 하이락리조트 정상가 : 85,500원 &gt; 할인가 : 75,240원', '쏠비치 진도 리조트 정상가 : 151,000원 &gt; 할인가 : 132,880원', '클럽이에스 제천리조트 정상가 : 135,000원 &gt; 할인가 : 118,800원', '무주 나봄리조트 정상가 : 70,000원 &gt; 할인가 : 61,600원', '목포 어반 호텔 정상가 : 65,000원 &gt; 할인가 : 57,200원', '소피텔 앰배서더 서울 정상가 : 346,500원 &gt; 할인가 : 316,500원', '콘래드 서울 정상가 : 451,000원 &gt; 할인가 : 421,000원', '골든튤립 인천공항 호텔&amp;스위트 정상가 : 83,591원 &gt; 할인가 : 73,560원', '제이앤파크 호텔 정상가 : 147,999원 &gt; 할인가 : 130,239원', '레스케이프 정상가 : 175,248원 &gt; 할인가 : 154,218원', '노보텔 앰배서더 서울 용산 정상가 : 174,000원 &gt; 할인가 : 153,120원', '스위스 그랜드 호텔 정상가 : 205,000원 &gt; 할인가 : 180,400원', 'L7 강남 바이 롯데 정상가 : 148,330원 &gt; 할인가 : 130,530원', '오늘의 카드 청구할인', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Ed2 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5% 청구할인 (일 20만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 8%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한 7만원이상 5%청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 하나카드 7% 선할인 (상품당 2만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM삼성 7만원이상 7%청구할인 (일 10만원 한) 자세히 보기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>프리미엄 아울렛 위크  : S/S NEW ARRIVALS</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004363</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[0213-0219] 프리미엄 아울렛 위크</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2023-02-13</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-02-19</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [0213-0219] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 2월 할인 대전', '최대 10% 할인 쿠폰 혜택', '[여성 패션 - 최대 70% 할인] 온앤온/ 나이스클랍/ 랩 브랜드 위크 外 보러가기', '[언더웨어 - 최대 70% 할인] 라페어/ 비너스/ 바바라/ 트라이엄프 특가 外 보러가기', '[명품잡화 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[스포츠 - 최대 70% 할인] 내셔널지오그래픽 등 아웃도어 브랜드 위크 보러가기', '[패션잡화 - 최대 37% 할인] 발렌타인데이 기념 - 전품목 30% OFF 보러가기', '[패션 슈즈 - 최대 80% 할인] 슈즈 판매 랭킹 TOP 300 인기상품 특가 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 80% 할인] 라코스테, 지프 등 캐주얼 특가 外 보러가기', '[키즈패션 - 최대 60% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 70% 할인] 테팔 브랜드위크! 매직핸드 外 보러가기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2022-10-26</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2025-10-25</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>최대 5만원 혜택</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2022-07-08</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2023-06-28</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>선원규 곶감 2/16(목) 11AM</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>명인의 곶감, 선착순 1천개 최대 73% 핫딜</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004325</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>선원규 곶감 @SSG.LIVE 2/16(목) 11:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2023-02-07</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2023-02-16</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 선원규 곶감 @SSG.LIVE 2/16(목) 11:00', '스마일클럽', '                    \xa0\xa0 SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>["이벤트/쿠폰 &gt; [2/20-26] 2023 명품화장품 쓱- 미리 '봄'", '스마일클럽', '전구매시, 미니립스틱+향수 샘플 증정', '전품목 15% OFF + SSG 머니 5% 추가 할인!', 'NO.1더블세럼 구매시, 샘플x3 트리플 단독증정!', '[몰튼 브라운] 인기 세트 구매시, 1주일 특별 증정']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Feb 23 00:21:17 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,138 +473,138 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>첫구매는 반값다딜</t>
+          <t>쓱배송 데이</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>첫구매 인기템! 화장지, 밀키트 총 1.5만원 할인 + 무료배송</t>
+          <t>선착순 쿠폰 10% + 카드 할인</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004346&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004457</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>첫구매는 반값다딜 (2/16~22)</t>
+          <t>2/23  단 하루! 쓱배송DAY</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫구매는 반값다딜 (2/16~22)', '스마일클럽', '첫구매는 반값다딜 (2/16~22)', '화장지,밀키트 총 1.5만원 할인+무료배송', '반값 할인쿠폰팩', '첫구매 전용 특별 메뉴 반값 할인 쿠폰팩', '첫구매 전용특별 메뉴', ' 마침 필요하셨죠? 화장지 선상품 1만원 할인 최대할인금액 1만원 ', ' 오늘 저녁 고민 끝! 밀키트 전상품 5천원 할인 최대할인금액 5천원 ', '반값메뉴는 무료배송으로 즐겨야죠', '상품쿠폰 50% 이마트몰 무료배송', '첫구매 쿠폰팩 받기 -ID당 기간중 1회', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       -상품할인쿠폰, 무료배송쿠폰: 2023년 2월 16일(목) 2023년 2월 22일 (수)', '       쿠폰 적용 대상 상품', '-쓱배송 새벽배송 상품에 한해서 적용 가능', '-화장지 50% cat (최대 1만원 할인) 제지/위생용품, 화장지/물티슈, 화장지', '-밀키트 50% cat (최대 5천원 할인) 밀키트/간편식, 밀키트', '- 상품당 1개 수량에 쿠폰 적용 가능 : 화장지 1개, 밀키트 1개 적용 가능(ex. 화장지 2개 구매시에도 1개에만 적용 가능합니다.)', '       쿠폰 사용 조건', '-상품할인 쿠폰 : 해당 카테고리 쓱배송 상품 구매시 50% 할인 적용. 각 카테고리별 최대할인 금액 적용', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상']</t>
+          <t>['이벤트/쿠폰 &gt; 2/23  단 하루! 쓱배송DAY', '스마일클럽', '2/23  단 하루! 쓱배송DAY', '할인에 할인을 더하다 쓱배송 DAY', '단 하루! 장바구니쿠폰 10%', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '쓱배송 라이프의 모든 것 쇼핑 꿀팁 안내 바로보기', '오늘은 장보는 날 쓱배송 특가상품 바로보기', '1 쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 쿠폰', '       이마트, 트레이더스 쓱배송 및 점포택배 / 새벽배송', '(오전 9시 오픈)(선착순 2만명) 장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만 5천원 할인 (ID당 1일 1매)', '+ 결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', 'KB국민카드 8만원 이상 5% 청구할인 / 10만원 이상 7% 청구할인 자세히 보기', '      쿠폰 발급 및 사용일', '      23년 2월 23일(기간 중 ID당 1일 1회 다운가능) (발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '2 오늘은 장보는 날! 쓱배송데이 장보기 특가상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>새학기 쓱배송으로 준비해 봄</t>
+          <t>첫 구매는 50% 반값다딜</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>간식/준비물부터 장보면 SSG머니 행운까지!</t>
+          <t>최대 2만원 할인에 무료배송</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004572</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
+          <t>첫 구매는 반값다딜 - 대상편</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-03-01</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '신학기 10% 쿠폰 받고 쇼핑 GO!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 간식부터 준비물까지 + 쓱배송 구매하고 응모하면 SSG 머니의 행운까지!', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
+          <t>['이벤트/쿠폰 &gt; 첫 구매는 반값다딜 - 대상편', '스마일클럽', '웰컴 쿠폰 받기', '최근 1년 간 쓱배송이 처음이라면,', '50% 할인에 무료배송 쿠폰팩을 드립니다', '무료배송 1장 - 쓱/새벽배송 2만원 이상 구매시', 'DAESANG 50% 상품쿠폰 3장 - 최대 1만원 할인 쿠폰 1장, 최대 5천원 할인 쿠폰 2장', '발급 대상 : 최근 1년 간 쓱배송 및 새벽배송 구매 이력이 없는 고객 ', '사용 방법 : 아래 소개된 상품 중 3개를 골라 결제 단계에서 쿠폰을 적용해주세요 ', '반 값에 무료배송으로 받아보세요', '      호밍스 - 낙곱새 저골 800g (50%, 무료배송)', '      정가 : 16,900원 / 할인가 8,450원', '      종가집 - 썰어담은 맛김치 900g (50%, 무료배송, 1+1)', '      정가 : 13,900원 / 할인가 6,950원', '      청정원 - 태양초 찰고추장 1Kg (50%, 무료배송)', '      정가 : 16,830원 / 할인가 8,415원', '      안주야 - 논현동포차 붊박창 160g (50%, 무료배송)', '      정가 : 9,280원 / 할인가 4,640원', '할인 상품 한 눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>오반장 위크</t>
+          <t>신학기 준비 한번에 끝!</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>오반장 상품 20%쿠폰 5장 지급!</t>
+          <t>입학&amp;졸업 선물부터 신학기 패션까지, 금주의 신학기 페스티벌</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004407</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004304&amp;cacheCmd=pass</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄</t>
+          <t>신학기 FESTIVAL: 3월 새학기 준비 끝!</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/16~22) 오반장위크_GOOD BYE 겨울, HELLO 봄', '스마일클럽', '오반장 상품 20%쿠폰 X 5장 지급!', '오반장위크 특별혜택! 20% 상품쿠폰 X 5장 바로보기', '오반장 상품 전용 20%쿠폰 x5장', '스마일클럽 전용 / 매일 오전 9시 선착순 2만명 / x5장', '쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '쿠폰 발급 기간 : 2023년 2월 16일(목) ~ 2023년 2월 22일(수)', '쿠폰 사용 기간 : 쿠폰 발급받은 당일 사용 필수', '쿠폰 1장당 대상상품 1개 수량에 한정하여 20% 할인 적용, 최대 3,000원 할인', '발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '  최대 35% \xa0', '  최대 15% \xa0', '  최대 30% \xa0', '  최대 40% \xa0', '  최대 32% \xa0', '  최대 12% \xa0', '  최대 50% \xa0', '  최대 16% \xa0', '  최대 33% \xa0', '  최대 43% \xa0', '  최대 19% \xa0', '  최대 29% \xa0', '  최대 23% \xa0', '  30% \xa0', '  55% \xa0', '  20% \xa0', '  20%/1+1 \xa0', '  최대 70% \xa0', '  최대 10% \xa0', '  최대 34% \xa0', '  최대 28% \xa0', '  최대 45% \xa0', '  25% \xa0', '  34% \xa0', '  최대 60% \xa0', '  최대 20% \xa0', '  40% \xa0', '  최대 36% \xa0', '  최대33% \xa0', '  최대 39% \xa0', '오반장 상품 전용 20%쿠폰 5장이 발급되었습니다. 즐거운 쇼핑 되세요!', '이미 발급된 쿠폰입니다. [MY - 쿠폰]을 확인해보세요.', '멤버십 전용 쿠폰입니다. 스마일클럽에 가입하고 더 많은 혜택을 누려보세요.', '스마일클럽 가입하기']</t>
+          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL: 3월 새학기 준비 끝!', '스마일클럽', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '헤지스레이디스 : 헤지스레이디스 23 S/S 신상 인기 스타일 추가 쿠폰 혜택', '허먼밀러 : 허먼밀러 에어론체어 스페셜 제안 최대 15%할인 ', '까사미아 : 까사미아 신학기 가구 특가 최대 최대 30% 할인혜택', '키르시 : 키르시 인기 맨투맨/후드 단독 최대 50% 기간한정 추가 쿠폰 혜택까지!', 'A.P.C : 산뜻한 새출발을 위한 에센셜 명품 A.P.C/오트리/키츠네 외 최대 35%', '올젠 : SS/FW 인기아이템 최대 65% SALE 10% 추가할인 쿠폰 혜택', '내셔널지오그래픽 : 내셔널지오그래픽 키즈 신학기 오픈!! / 이월 최대 10% 쿠폰', '게스시계 : 게스 신학기 인기 워치 추천 SSG 단독 할인전 ~59% OFF', '닥스키즈/헤지스키즈 : 닥스키즈/헤지스키즈 외 우리아이 취향저격 새학기륵, 최대 60% off 행사', '프리즘 : 봄맞이 인기 조명 SALE 오늘 하루만 최대 할인', '나이키/아디다스/뉴발란스 : 봄신상 신학기 기획전 나이키/뉴발란스/아디다스잔스포츠 外 신학기 할인 모음', '나이키 : 나이키 신학기/봄맞이 특가 최대 44% 빅세일', '글라스락 : 글라스락 신학기 필수템 모음전 보관용기/텀블러 최대 65% OFF', '온앤온 : 23 SS 시즌오픈 NEW FASHION SSG 단독 할인 + 쿠폰혜택까지!', '아디다스 : 아디다스 23신상 스포츠가방 러닝화 슬리퍼 특가 아디다스 최대 40% 신학기 특가', '(신세계 단독 상품 특가 30%) 아동패션 TOP 브랜드 연합 책가방 특가전 신세계 단독상품 외 Top브랜드 상품 특가', '(최대 68% 할인!) SSG 유아동 신학기 페스티벌 행사 어린이집 등원준비 필수템 BEST 모음 ', '(최대 25%) 모던하우스 신학기 맞이 학생가구/침구/완구 BIG SALE 책상+의자 SET 구매시 상품권 증정', '(최대 30%) 까사미아 신학기 가구 특가 최대 30% 할인 혜택', '(네이버 최저가 특가) 신학기 맞이 인기 조명 할인전 인기 조명 최대 20% 할인', '(최대 30%) 신학기 맞이 템퍼 특별 할인전 기능성 베개/메트리스 특가+구매상품별 사은품 증정', '(30~50%) 프레드페리 SSG 단독 할인 상품+ 추가혜택!', '(20%) 스포츠 빅브랜드 신학기 기획전 뉴발란스/나이키/반스/디스커버리 外 신학기 할인 모음', '(40%) 토리버치 시즌오프 최대 40%세일 시즌오프 베스트 아이템']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>신학기 준비 한번에 끝!</t>
+          <t>쓱-선물로 응원해!</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>입학&amp;졸업 선물부터 신학기 패션까지, 금주의 신학기 페스티벌</t>
+          <t>선물한 사연 응모하고 내 선물도 쓱</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004304&amp;cacheCmd=pass</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>신학기 FESTIVAL: 3월 새학기 준비 끝!</t>
+          <t>[0215-0226] 쓱-선물로 응원해!</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-20</t>
+          <t>2023-02-06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -614,377 +614,303 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL: 3월 새학기 준비 끝!', '스마일클럽', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '헤지스레이디스 : 헤지스레이디스 23 S/S 신상 인기 스타일 추가 쿠폰 혜택', '허먼밀러 : 허먼밀러 에어론체어 스페셜 제안 최대 15%할인 ', '까사미아 : 까사미아 신학기 가구 특가 최대 최대 30% 할인혜택', '키르시 : 키르시 인기 맨투맨/후드 단독 최대 50% 기간한정 추가 쿠폰 혜택까지!', 'A.P.C : 산뜻한 새출발을 위한 에센셜 명품 A.P.C/오트리/키츠네 외 최대 35%', '올젠 : SS/FW 인기아이템 최대 65% SALE 10% 추가할인 쿠폰 혜택', '내셔널지오그래픽 : 내셔널지오그래픽 키즈 신학기 오픈!! / 이월 최대 10% 쿠폰', '게스시계 : 게스 신학기 인기 워치 추천 SSG 단독 할인전 ~59% OFF', '닥스키즈/헤지스키즈 : 닥스키즈/헤지스키즈 외 우리아이 취향저격 새학기륵, 최대 60% off 행사', '프리즘 : 봄맞이 인기 조명 SALE 오늘 하루만 최대 할인', '나이키/아디다스/뉴발란스 : 봄신상 신학기 기획전 나이키/뉴발란스/아디다스잔스포츠 外 신학기 할인 모음', '나이키 : 나이키 신학기/봄맞이 특가 최대 44% 빅세일', '글라스락 : 글라스락 신학기 필수템 모음전 보관용기/텀블러 최대 65% OFF', '온앤온 : 23 SS 시즌오픈 NEW FASHION SSG 단독 할인 + 쿠폰혜택까지!', '아디다스 : 아디다스 23신상 스포츠가방 러닝화 슬리퍼 특가 아디다스 최대 40% 신학기 특가', '(신세계 단독 상품 특가 30%) 아동패션 TOP 브랜드 연합 책가방 특가전 신세계 단독상품 외 Top브랜드 상품 특가', '(최대 68% 할인!) SSG 유아동 신학기 페스티벌 행사 어린이집 등원준비 필수템 BEST 모음 ', '(최대 25%) 모던하우스 신학기 맞이 학생가구/침구/완구 BIG SALE 책상+의자 SET 구매시 상품권 증정', '(최대 30%) 까사미아 신학기 가구 특가 최대 30% 할인 혜택', '(네이버 최저가 특가) 신학기 맞이 인기 조명 할인전 인기 조명 최대 20% 할인', '(최대 30%) 신학기 맞이 템퍼 특별 할인전 기능성 베개/메트리스 특가+구매상품별 사은품 증정', '(30~50%) 프레드페리 SSG 단독 할인 상품+ 추가혜택!', '(20%) 스포츠 빅브랜드 신학기 기획전 뉴발란스/나이키/반스/디스커버리 外 신학기 할인 모음', '(40%) 토리버치 시즌오프 최대 40%세일 시즌오프 베스트 아이템']</t>
+          <t>['이벤트/쿠폰 &gt; [0215-0226] 쓱-선물로 응원해!', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일 쿠폰', '모바일 쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>쓱-선물로 응원해!</t>
+          <t>새학기 쓱배송으로 준비해 봄</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>선물한 사연 응모하고 내 선물도 쓱</t>
+          <t>간식/준비물 쓱-장보고 SSG머니 5천원 행운</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[0215-0226] 쓱-선물로 응원해!</t>
+          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0215-0226] 쓱-선물로 응원해!', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일 쿠폰', '모바일 쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', '      My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>민지의 장바구니-곶감 &amp; k-디저트</t>
+          <t>블라썸위크</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+          <t>장보기 대표브랜드 최대 50%할인, 1+1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004387</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004565</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)</t>
+          <t>블라썸위크</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-03-01</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-곶감&amp;k-디저트편 (2/16~2/22)', '스마일클럽', 'SSG MONEY 1천원 (500명)', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       - ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       - 이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '라이브 특가 놓쳐서 아쉽다면\xa0 최대 55% 할인!']</t>
+          <t>['이벤트/쿠폰 &gt; 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '오늘만 할인해봄 한정수량 타임딜 바로보기', '봄맞이 세일해봄 최대 50% 할인 + 사은품 바로보기', '딱 하루만 한정수량 타임딜', '브랜드별 최대 50% 할인+사은품 이벤트', '한정수량 타임딜', '브랜드별 할인 + 사은품 혜택', '첫 구매 반값다딜 50%', '종가집 반찬 단독 최대 30%', '간장 1.5만원 구매시 3천원 할인', '비비고 브랜드 좋아요 5%쿠폰 받으러 가기', '최대 50% 할인', '행사상품 1.5만 이상 구매시 1천원 할인', '신상품 체험단 이벤트', '2개 구매시 50% 할인', '다다익선 2,4,5만이상 구매 시 5,7,10%할인', 'LG생활건강 브랜드 좋아요 5% 쿠폰 받으러 가기', '최대 38%', '다다익선 10%', '구매왕 이벤트 LG공기청정기 증정 외', '아모레퍼시픽 브랜드 좋아요 5% 쿠폰 받으러 가기']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>만원상점 알뜰쓱템</t>
+          <t>스마일클럽 웰컴 5천원 쿠폰</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>신선&amp;가공식품 ~70%할인</t>
+          <t>2월의신규 가입 혜택</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004412</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>만원상점 알뜰쓱템</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 만원상점 알뜰쓱템', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 2월 깜짝 특별전</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004294</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (2/9~22) 2023 대한민국 수산대전 - 2월 깜짝 특별전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 차수별 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>오반장위크멤버십 ~20% 추가할인</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>스마일클럽처음이라면? 5천원쿠폰</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.', '쿠폰 받으러 가기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>신세계인터내셔날 럭셔리 2/23(목) 8PM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>톰브라운/발렌시아가/보테가베네타外 파격 특가</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004499&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SIV명품 @SSG.LIVE 2/23(목) 20:00PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-02-15</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SIV명품 @SSG.LIVE 2/23(목) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>2023 뷰티 미리 '봄'</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>봄맞이 화사함을 더해줄, 럭셔리 뷰티 아이템</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004454</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[2/20-26] 2023 명품화장품 쓱- 미리 '봄'</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-20</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-26</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '[카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 결제시 적용(상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>["이벤트/쿠폰 &gt; [2/20-26] 2023 명품화장품 쓱- 미리 '봄'", '스마일클럽', '전구매시, 미니립스틱+향수 샘플 증정', '전품목 15% 할인', '[몰튼 브라운] 달콤한 향기를 선물하세요 UP TO 35%']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>JJ지고트 2/20(월) 8PM</t>
+          <t>2월 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>JJ지고트 봄 신상&amp;이월 상품 ~87%OFF</t>
+          <t>지금 할인 중! ~40% 할인 혜택</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004465&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>JJ지고트 @SSG.LIVE 2/20(월) 8PM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-02-20</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; JJ지고트 @SSG.LIVE 2/20(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>스타우브 2/21(화) 8PM</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>원형 꼬꼬떼 22cm 22만원대 한정수량 선착순 핫딜</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004459&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[쓱라이브] 스타우브 2/21(화)8PM</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2023-02-14</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2023-02-25</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 스타우브 2/21(화)8PM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2023 뷰티 미리 '봄'</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>봄맞이 화사함을 더해줄, 럭셔리 뷰티 아이템</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004454</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[2/20-26] 2023 명품화장품 쓱- 미리 '봄'</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2023-02-20</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-02-26</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>["이벤트/쿠폰 &gt; [2/20-26] 2023 명품화장품 쓱- 미리 '봄'", '스마일클럽', '전구매시, 미니립스틱+향수 샘플 증정', '전품목 15% OFF + SSG 머니 5% 추가 할인!', 'NO.1더블세럼 구매시, 샘플x3 트리플 단독증정!', '[몰튼 브라운] 인기 세트 구매시, 1주일 특별 증정']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '헬로카봇 펜타스톰X (N2쓱배송, 전국택배)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)', '뽀로로 스마트 쓰기패드(N2 쓱배송, 전국택배)', '얌얌펫 잼하우스스페셜 (N2쓱배송, 전국택배)', '리틀라이브펫 리틀피쉬 어항세트 (N2쓱배송, 전국택배가능)', '/ 올리키즈 유아동침구 특별 할인전★']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Feb 27 00:22:03 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,37 +473,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>쓱배송 데이</t>
+          <t>SPRING WEEK 봄격쇼핑 신상세일</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>선착순 쿠폰 10% + 카드 할인</t>
+          <t>패션/뷰티, 홈스타일링 봄맞이 인기상품</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004457</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004521</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2/23  단 하루! 쓱배송DAY</t>
+          <t>봄격쇼핑 신상세일 SPRING WEEK</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-03-05</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2/23  단 하루! 쓱배송DAY', '스마일클럽', '2/23  단 하루! 쓱배송DAY', '할인에 할인을 더하다 쓱배송 DAY', '단 하루! 장바구니쿠폰 10%', '최대 10% 장바구니 쿠폰 &amp; 카드할인 바로보기', '쓱배송 라이프의 모든 것 쇼핑 꿀팁 안내 바로보기', '오늘은 장보는 날 쓱배송 특가상품 바로보기', '1 쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 쿠폰', '       이마트, 트레이더스 쓱배송 및 점포택배 / 새벽배송', '(오전 9시 오픈)(선착순 2만명) 장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만 5천원 할인 (ID당 1일 1매)', '+ 결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', 'KB국민카드 8만원 이상 5% 청구할인 / 10만원 이상 7% 청구할인 자세히 보기', '      쿠폰 발급 및 사용일', '      23년 2월 23일(기간 중 ID당 1일 1회 다운가능) (발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '2 오늘은 장보는 날! 쓱배송데이 장보기 특가상품', '점포의 신선함을 그대로 간직한 이마트몰 쓱배송 추천상품', '가성비 챙기고 대용량 장보기 트레이더스 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; 봄격쇼핑 신상세일 SPRING WEEK', '스마일클럽', '+PLUS 카드 청구할인 혜택도 챙겨가세요!']</t>
         </is>
       </c>
     </row>
@@ -547,101 +547,101 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>신학기 준비 한번에 끝!</t>
+          <t>새학기 쓱배송으로 준비해 봄</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>입학&amp;졸업 선물부터 신학기 패션까지, 금주의 신학기 페스티벌</t>
+          <t>간식/준비물 쓱-장보고 SSG머니 5천원 행운</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004304&amp;cacheCmd=pass</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>신학기 FESTIVAL: 3월 새학기 준비 끝!</t>
+          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-02-20</t>
+          <t>2023-02-16</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신학기 FESTIVAL: 3월 새학기 준비 끝!', '스마일클럽', '다가오는 신학기 준비는 SSG에서! 10% 장바구니 쿠폰 + 신학기 BEST 브랜드 특별전', '#1 매일 선착순 최대 1.5만원 쿠폰', '#1 오늘 받아 바로 쓰는 신학기 10% 부터 최대 1.5마원 쿠폰', '쿠폰이 모두 소진되었습니다! 성원에 감사드립니다.', '쿠폰 사용 전 꼭 확인하세요!', '      쿠폰 사용 기간', '      쿠폰 사용 조건', 'SSG.COM +PLUS 카드 청구할인 혜택도 챙겨가세요! 자세히 보기', '헤지스레이디스 : 헤지스레이디스 23 S/S 신상 인기 스타일 추가 쿠폰 혜택', '허먼밀러 : 허먼밀러 에어론체어 스페셜 제안 최대 15%할인 ', '까사미아 : 까사미아 신학기 가구 특가 최대 최대 30% 할인혜택', '키르시 : 키르시 인기 맨투맨/후드 단독 최대 50% 기간한정 추가 쿠폰 혜택까지!', 'A.P.C : 산뜻한 새출발을 위한 에센셜 명품 A.P.C/오트리/키츠네 외 최대 35%', '올젠 : SS/FW 인기아이템 최대 65% SALE 10% 추가할인 쿠폰 혜택', '내셔널지오그래픽 : 내셔널지오그래픽 키즈 신학기 오픈!! / 이월 최대 10% 쿠폰', '게스시계 : 게스 신학기 인기 워치 추천 SSG 단독 할인전 ~59% OFF', '닥스키즈/헤지스키즈 : 닥스키즈/헤지스키즈 외 우리아이 취향저격 새학기륵, 최대 60% off 행사', '프리즘 : 봄맞이 인기 조명 SALE 오늘 하루만 최대 할인', '나이키/아디다스/뉴발란스 : 봄신상 신학기 기획전 나이키/뉴발란스/아디다스잔스포츠 外 신학기 할인 모음', '나이키 : 나이키 신학기/봄맞이 특가 최대 44% 빅세일', '글라스락 : 글라스락 신학기 필수템 모음전 보관용기/텀블러 최대 65% OFF', '온앤온 : 23 SS 시즌오픈 NEW FASHION SSG 단독 할인 + 쿠폰혜택까지!', '아디다스 : 아디다스 23신상 스포츠가방 러닝화 슬리퍼 특가 아디다스 최대 40% 신학기 특가', '(신세계 단독 상품 특가 30%) 아동패션 TOP 브랜드 연합 책가방 특가전 신세계 단독상품 외 Top브랜드 상품 특가', '(최대 68% 할인!) SSG 유아동 신학기 페스티벌 행사 어린이집 등원준비 필수템 BEST 모음 ', '(최대 25%) 모던하우스 신학기 맞이 학생가구/침구/완구 BIG SALE 책상+의자 SET 구매시 상품권 증정', '(최대 30%) 까사미아 신학기 가구 특가 최대 30% 할인 혜택', '(네이버 최저가 특가) 신학기 맞이 인기 조명 할인전 인기 조명 최대 20% 할인', '(최대 30%) 신학기 맞이 템퍼 특별 할인전 기능성 베개/메트리스 특가+구매상품별 사은품 증정', '(30~50%) 프레드페리 SSG 단독 할인 상품+ 추가혜택!', '(20%) 스포츠 빅브랜드 신학기 기획전 뉴발란스/나이키/반스/디스커버리 外 신학기 할인 모음', '(40%) 토리버치 시즌오프 최대 40%세일 시즌오프 베스트 아이템']</t>
+          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', '      My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>쓱-선물로 응원해!</t>
+          <t>블라썸위크</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>선물한 사연 응모하고 내 선물도 쓱</t>
+          <t>장보기 대표브랜드 최대 50%할인, 1+1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004089</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004565</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[0215-0226] 쓱-선물로 응원해!</t>
+          <t>블라썸위크</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2023-03-01</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0215-0226] 쓱-선물로 응원해!', '스마일클럽', '&lt;선물하기&gt; 이벤트 선물은 사랑을 싣고 바로보기', '모바일 쿠폰', '모바일 쿠폰 상품 더 보기', '#3 &lt;선물하기&gt; 이벤트', '       행사기간동안 쓱 선물하기를 통해 선물한 사연을 댓글로 달아주세요. ID당 이벤트 기간 내 1일 1회, 댓글 참여가 가능하며, 댓글에 사연과 SNS로 이벤트를 공유한 링크를 함께 남기면 당첨 확률이 쑥쑥!!', '       선물하기 이벤트 기간', '본 이벤트에 대한 세부 사항은 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.', '나에게 선물하는 경우는 해당 이벤트에서 제외 됩니다. (상품 구매 건 중 구매하는 분과 받는분의 회원정보 중 이름, ID, 휴대폰 번호 중 1개 이상 정보 중복시 이벤트 제외)', '본 이벤트는 ID당 일별 1회 응모할수 있으며, 행사기간 중 중복 응모 가능합니다. 부정한 방법으로 참여한 것이 발견될 경우 응모와 당첨이 취소될 수 있습니다.', '쓱 선물하기를 통해 선물한 사연과 해당 이벤트를 SNS, 블로그 등을 통해 공유한 링크를 함께 댓글로 남겨주신분들은 당첨 확률이 올라갑니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. - 개인정보 위탁업체 : (주)젤라블루코리아, - 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '오늘만 할인해봄 한정수량 타임딜 바로보기', '봄맞이 세일해봄 최대 50% 할인 + 사은품 바로보기', '딱 하루만 한정수량 타임딜', '브랜드별 최대 50% 할인+사은품 이벤트', '한정수량 타임딜', '브랜드별 할인 + 사은품 혜택', '첫 구매 반값다딜 50%', '종가집 반찬 단독 최대 30%', '간장 1.5만원 구매시 3천원 할인', '비비고 브랜드 좋아요 5%쿠폰 받으러 가기', '최대 50% 할인', '행사상품 1.5만 이상 구매시 1천원 할인', '신상품 체험단 이벤트', '2개 구매시 50% 할인', '다다익선 2,4,5만이상 구매 시 5,7,10%할인', 'LG생활건강 브랜드 좋아요 5% 쿠폰 받으러 가기', '최대 38%', '다다익선 10%', '구매왕 이벤트 LG공기청정기 증정 외', '아모레퍼시픽 브랜드 좋아요 5% 쿠폰 받으러 가기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>새학기 쓱배송으로 준비해 봄</t>
+          <t>스마일클럽 웰컴 5천원 쿠폰</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>간식/준비물 쓱-장보고 SSG머니 5천원 행운</t>
+          <t>2월의신규 가입 혜택</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
+          <t>[스마일클럽] 2월 매일매일 스마일</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-02-01</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -651,266 +651,192 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', '      My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
+          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>블라썸위크</t>
+          <t>최대 8만원 혜택</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>장보기 대표브랜드 최대 50%할인, 1+1</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004565</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>블라썸위크</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '오늘만 할인해봄 한정수량 타임딜 바로보기', '봄맞이 세일해봄 최대 50% 할인 + 사은품 바로보기', '딱 하루만 한정수량 타임딜', '브랜드별 최대 50% 할인+사은품 이벤트', '한정수량 타임딜', '브랜드별 할인 + 사은품 혜택', '첫 구매 반값다딜 50%', '종가집 반찬 단독 최대 30%', '간장 1.5만원 구매시 3천원 할인', '비비고 브랜드 좋아요 5%쿠폰 받으러 가기', '최대 50% 할인', '행사상품 1.5만 이상 구매시 1천원 할인', '신상품 체험단 이벤트', '2개 구매시 50% 할인', '다다익선 2,4,5만이상 구매 시 5,7,10%할인', 'LG생활건강 브랜드 좋아요 5% 쿠폰 받으러 가기', '최대 38%', '다다익선 10%', '구매왕 이벤트 LG공기청정기 증정 외', '아모레퍼시픽 브랜드 좋아요 5% 쿠폰 받으러 가기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2월의신규 가입 혜택</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>다이슨 조명 2/27(월) 7PM</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>다이슨 솔라사이클 모프 조명 역대급 할인! 조명 구매고객 대상 상품권 추첨 이벤트까지</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004575&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>다이슨 @SSG.LIVE 2/27(월) 19:00PM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-02-21</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; 다이슨 @SSG.LIVE 2/27(월) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>르메르디앙&amp;목시 서울 명동 2/27(월) 8PM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>르메르디앙 서울 명동 199,000원~ , 목시 서울 명동 99,000원~</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004554</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>르메르디앙&amp;목시 서울 명동 @SSG.LIVE 2/27(월) 20:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-20</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 르메르디앙&amp;목시 서울 명동 @SSG.LIVE 2/27(월) 20:00', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>신세계인터내셔날 럭셔리 2/23(목) 8PM</t>
+          <t>블랙라벨 오렌지 2/28(화) 11AM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>톰브라운/발렌시아가/보테가베네타外 파격 특가</t>
+          <t>핫딜! 중소과 20과 1만1천원대 완판 시 1과 더!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004499&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004604&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SIV명품 @SSG.LIVE 2/23(목) 20:00PM</t>
+          <t>[쓱라이브] 블랙라벨 오렌지 2/28(화)11AM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-02-21</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-03-03</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SIV명품 @SSG.LIVE 2/23(목) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2023 뷰티 미리 '봄'</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>봄맞이 화사함을 더해줄, 럭셔리 뷰티 아이템</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004454</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[2/20-26] 2023 명품화장품 쓱- 미리 '봄'</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2023-02-20</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2023-02-26</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>["이벤트/쿠폰 &gt; [2/20-26] 2023 명품화장품 쓱- 미리 '봄'", '스마일클럽', '전구매시, 미니립스틱+향수 샘플 증정', '전품목 15% 할인', '[몰튼 브라운] 달콤한 향기를 선물하세요 UP TO 35%']</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2월 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~40% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '[파스퇴르] 올곧게만든 위드맘 2단계 750g (NEO2 쓱배송, 그외지역 택배)', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '헬로카봇 펜타스톰X (N2쓱배송, 전국택배)', '헬로카봇 하이퍼캅스(N2쓱배송, 전국택배가능)', '뽀로로 스마트 쓰기패드(N2 쓱배송, 전국택배)', '얌얌펫 잼하우스스페셜 (N2쓱배송, 전국택배)', '리틀라이브펫 리틀피쉬 어항세트 (N2쓱배송, 전국택배가능)', '/ 올리키즈 유아동침구 특별 할인전★']</t>
+          <t>['이벤트/쿠폰 &gt; [쓱라이브] 블랙라벨 오렌지 2/28(화)11AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Mar  2 00:23:01 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,244 +510,244 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>첫 구매는 50% 반값다딜</t>
+          <t>패션명품 쓱세일 COMING SOON</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 2만원 할인에 무료배송</t>
+          <t>SSG머니 100% 페이백!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004572</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004758</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>첫 구매는 반값다딜 - 대상편</t>
+          <t>(3/2~5) 패션명품 쓱세일 COMING SOON</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
+          <t>2023-03-05</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫 구매는 반값다딜 - 대상편', '스마일클럽', '웰컴 쿠폰 받기', '최근 1년 간 쓱배송이 처음이라면,', '50% 할인에 무료배송 쿠폰팩을 드립니다', '무료배송 1장 - 쓱/새벽배송 2만원 이상 구매시', 'DAESANG 50% 상품쿠폰 3장 - 최대 1만원 할인 쿠폰 1장, 최대 5천원 할인 쿠폰 2장', '발급 대상 : 최근 1년 간 쓱배송 및 새벽배송 구매 이력이 없는 고객 ', '사용 방법 : 아래 소개된 상품 중 3개를 골라 결제 단계에서 쿠폰을 적용해주세요 ', '반 값에 무료배송으로 받아보세요', '      호밍스 - 낙곱새 저골 800g (50%, 무료배송)', '      정가 : 16,900원 / 할인가 8,450원', '      종가집 - 썰어담은 맛김치 900g (50%, 무료배송, 1+1)', '      정가 : 13,900원 / 할인가 6,950원', '      청정원 - 태양초 찰고추장 1Kg (50%, 무료배송)', '      정가 : 16,830원 / 할인가 8,415원', '      안주야 - 논현동포차 붊박창 160g (50%, 무료배송)', '      정가 : 9,280원 / 할인가 4,640원', '할인 상품 한 눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; (3/2~5) 패션명품 쓱세일 COMING SOON', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>새학기 쓱배송으로 준비해 봄</t>
+          <t>첫구매는 반값다딜 &lt;풀무원 편&gt;</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>간식/준비물 쓱-장보고 SSG머니 5천원 행운</t>
+          <t>풀무원 상품 4개 골라 최대 2만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004430</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004661&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(이벤트) 새학기 쓱배송으로 준비해 봄!</t>
+          <t>반값다딜 - 풀무원 편 (3/2~12)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (이벤트) 새학기 쓱배송으로 준비해 봄!', '스마일클럽', '(이벤트) 새학기 쓱배송으로 준비해 봄!', '새학기 쓱배송으로 준비해 봄', '쓱배송으로 장 봄 #4', 'SSG MONEY 5천원 (200명)', '이마트몰 쓱배송/새벽배송으로 3만원 이상 구매 후 하단의 신청하기 버튼을 눌러주세요. 추첨을 통해서 200분에게 SSG머니 5천원 페이백!', '      My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '이벤트에 응모하시고 결제취소 하셨더라도, 행사 마감 전까지 다시 응모조건 금액을 충족해주시면 정상적으로 이벤트 대상에 포함됩니다.', '주문취소 및 단순반품으로 인해 신청조건 금액을 달성하지 못할 경우, 이벤트 대상에서 제외됩니다.', '본 이벤트에 응모하실 경우 개인정보 (회원ID 등) 제공에 동의하신 것으로 간주되며, 제공된 정보는 SSG머니 지급 후 즉시 파기합니다.', '본 이벤트는 당사 사정에 따라 사전고지 없이 임의로 변경 혹은 조기 종료될 수 있습니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다딜 - 풀무원 편 (3/2~12)', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'Pulmuone 상품쿠폰 50% 4장, 개별 쿠폰 당 최대 5천원 할인', 'Pulmuone 상품쿠폰 무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 2023년 3월 2일(목)~ 2023년 3월 12일 (일)', '       쿠폰 사용 조건', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '(50%, 무료배송) [풀무원] 얇은피 꽉찬속 김치만두 400gx2 할인전 : 9,480원 할인후 : 4,740원', '(50%, 무료배송) [풀무원] 국산콩 투컵 두부 600g 할인전 : 5,480원 할인후 : 2,740원', '(50%, 무료배송) [풀무원] 바릴라 캠핑 기획팩 2,700G 할인전 : 29,800원 할인후 : 14,900원', '(50%, 무료배송) [풀무원] 새콤달콤 유부초밥 330g 할인전 : 5,680원 할인후 : 2,840원', '(50%, 무료배송) [풀무원] 행복한 동물복지유정란 15구 780g : 8,980원 할인후 : 4,490원', '할인 상품 한 눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>블라썸위크</t>
+          <t>어서와 봄, 할인상품 득템해 봄</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>장보기 대표브랜드 최대 50%할인, 1+1</t>
+          <t>창고 대개방! 반짝할인 놓치지 말고 득템하세요</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004565</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004717</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>블라썸위크</t>
+          <t>(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 블라썸위크', '스마일클럽', 'CJ/유한킴벌리 등 장보기 대표브랜드 최대 50%할인 및 이벤트', '오늘만 할인해봄 한정수량 타임딜 바로보기', '봄맞이 세일해봄 최대 50% 할인 + 사은품 바로보기', '딱 하루만 한정수량 타임딜', '브랜드별 최대 50% 할인+사은품 이벤트', '한정수량 타임딜', '브랜드별 할인 + 사은품 혜택', '첫 구매 반값다딜 50%', '종가집 반찬 단독 최대 30%', '간장 1.5만원 구매시 3천원 할인', '비비고 브랜드 좋아요 5%쿠폰 받으러 가기', '최대 50% 할인', '행사상품 1.5만 이상 구매시 1천원 할인', '신상품 체험단 이벤트', '2개 구매시 50% 할인', '다다익선 2,4,5만이상 구매 시 5,7,10%할인', 'LG생활건강 브랜드 좋아요 5% 쿠폰 받으러 가기', '최대 38%', '다다익선 10%', '구매왕 이벤트 LG공기청정기 증정 외', '아모레퍼시픽 브랜드 좋아요 5% 쿠폰 받으러 가기']</t>
+          <t>['이벤트/쿠폰 &gt; (3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄', '스마일클럽', '(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>스마일클럽 웰컴 5천원 쿠폰</t>
+          <t>최대 7.2만원 혜택</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2월의신규 가입 혜택</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000003992</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[스마일클럽] 2월 매일매일 스마일</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [스마일클럽] 2월 매일매일 스마일', '스마일클럽', '[스마일클럽] 2월 매일매일 스마일', ' 지금 스마일클럽 가입하고 모든 혜택 받기 ', '본 쿠폰은 이벤트 기간 내 SSG.COM에서 스마일클럽에 최초 신규 가입한 고객님에 한해 ID당 1회 발급됩니다.', '쿠폰은 가입 차주 금요일 이내 자동 지급되며, 앱푸시나 문자메시지 등을 통해 별도 안내 예정입니다.', '본 쿠폰은 5,100원 이상 구매 시 5,000원 할인됩니다. (할인액 및 배송비 제외한 구매 금액 기준으로 쿠폰 적용됨)', '일부 상품 및 브랜드는 쿠폰 적용 제외될 수 있습니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '본 이벤트는 당사 사정으로 내용이 변경되거나 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 8월 1일 부터 2023년 1월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '4. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>SK-II 3/2(목) 8PM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>극광 에센스 리뉴얼 최초 공개! 선착순 핫딜 20만원대+백화점 상품권 증정+선물포장</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004573&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>[SSG.LIVE]3/2(목) SK-II</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.02.01 ~ 2023.02.28', '쿠폰 사용기간 : 2023.02.01 ~ 2023.02.28', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/2(목) SK-II', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>다이슨 조명 2/27(월) 7PM</t>
+          <t>보라카이(하나투어) 3/2(목) 9PM</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>다이슨 솔라사이클 모프 조명 역대급 할인! 조명 구매고객 대상 상품권 추첨 이벤트까지</t>
+          <t>보라카이 베스트셀러 헤난가든 초특가 4/5일</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004575&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004579&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>다이슨 @SSG.LIVE 2/27(월) 19:00PM</t>
+          <t>보라카이 여행(하나투어) @SSG.LIVE 3/2(목) 9PM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -757,86 +757,49 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 다이슨 @SSG.LIVE 2/27(월) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 보라카이 여행(하나투어) @SSG.LIVE 3/2(목) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>르메르디앙&amp;목시 서울 명동 2/27(월) 8PM</t>
+          <t>3월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>르메르디앙 서울 명동 199,000원~ , 목시 서울 명동 99,000원~</t>
+          <t>지금 할인 중! ~40% 할인 혜택</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004554</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>르메르디앙&amp;목시 서울 명동 @SSG.LIVE 2/27(월) 20:00</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-02-20</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 르메르디앙&amp;목시 서울 명동 @SSG.LIVE 2/27(월) 20:00', '스마일클럽']</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>블랙라벨 오렌지 2/28(화) 11AM</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>핫딜! 중소과 20과 1만1천원대 완판 시 1과 더!</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004604&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[쓱라이브] 블랙라벨 오렌지 2/28(화)11AM</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2023-02-21</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2023-03-03</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [쓱라이브] 블랙라벨 오렌지 2/28(화)11AM', '스마일클럽', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '시크릿쥬쥬 베스트프렌즈마고 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈스쿨백세트 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈리나 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈쥬쥬 (N2쓱배송, 전국택배)', '베스트프렌즈시크릿프렌즈폰 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈미니사물함 (N2쓱배송, 전국택배)', '★금주의 할인딜★ KIDS 침구 / 어린이집 낮잠이불']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Mar  6 00:22:07 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,101 +473,101 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SPRING WEEK 봄격쇼핑 신상세일</t>
+          <t>패션명품 쓱세일 NEW SPRING, NEW ITEM</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>패션/뷰티, 홈스타일링 봄맞이 인기상품</t>
+          <t>최대15% 할인 쿠폰팩 + 청구할인 혜택</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004521</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004551</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>봄격쇼핑 신상세일 SPRING WEEK</t>
+          <t>(0306~12) 패션명품 쓱세일 - 혜택</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-05</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 봄격쇼핑 신상세일 SPRING WEEK', '스마일클럽', '+PLUS 카드 청구할인 혜택도 챙겨가세요!']</t>
+          <t>['이벤트/쿠폰 &gt; (0306~12) 패션명품 쓱세일 - 혜택', '스마일클럽', '#혜택 01 패션의류/잡화 전용 할인 혜택 바로보기', '#혜택 02 명품 전용 할인 혜택 바로보기', '#혜택 04 매일매일 카드청구할인 바로보기', '최대 15% 할인! 패션의류/잡화 전용 할인 혜택', '패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 2만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장(패션명품 쓱세일)', '쿠폰 받기(기간 내 ID당 1회)', '       상품별 15% 할인', '       2만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '       쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다.(동일상품 복수 개 구매 시 1개 수량에만 적용)', '* 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세에서 쿠폰을 다운 받으실 수 없습니다.', '패션의류/잡화 대표 브랜드 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '백화점 패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 5만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장', '       5만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '최대 15만원 할인! 명품 전용 할인 혜택', '상품쿠폰 7% - 10만원 이상 상품 구매 시 7% 할인, 최대 10만원', '상품쿠폰 8% - 30만원 이상 상품 구매 시 8% 할인, 최대 15만원', '더 많은 상품을 담아 최대 8% 할인 받는 장바구니 쿠폰', '* 타 사이트를 통해 방문하신 고객의 경우, 상품 구매 시 쿠폰이 적용되지 않습니다.', '장바구니쿠폰 8% - 7만원 이상 구매 시 최대 3만원 할인(ID당 1장 발급)', '쿠폰 받기', 'W컨셉 SPRING SHOP 15% 쿠폰과 함께 W컨셉의 감성을 담은 봄 패션 아이템을 만나보세요!', '신세계백화점몰&amp;신세계몰 첫구매 고객이라면\xa0 BONUS 쿠폰 하나 더!', '* 신세계백화점몰 및 신세계몰 첫구매 고객 대상으로 발급되는 쿠폰입니다.', '장바구니쿠폰 12% - 7만원 이상 구매 시 최대 2만원 할인 ID당 1장 발급(첫구매 전용, 패션/명품 전용, 선착순 1만명)', '선착순 쿠폰이 마감되었습니다.', '카드 혜택도 놓치지 마세요! 매일매일 카드 청구할인', '[SSGPAY전용] 삼성카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 결제 시 10% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기', '[SSGPAY전용] KB국민카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일 COMING SOON</t>
+          <t>패션명품 쓱세일 23 S/S BEST BRAND FOR U</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SSG머니 100% 페이백!</t>
+          <t>마시모두띠/칼린 외 TOP 브랜드</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004758</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004552</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(3/2~5) 패션명품 쓱세일 COMING SOON</t>
+          <t>(0306~12) 패션명품 쓱세일 - 브랜드</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-03-05</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/2~5) 패션명품 쓱세일 COMING SOON', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; (0306~12) 패션명품 쓱세일 - 브랜드', '스마일클럽', '알도 - 그랜드오픈 기념 단독특가 + 15% 쿠폰 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>첫구매는 반값다딜 &lt;풀무원 편&gt;</t>
+          <t>패션명품 쓱세일 매일 오전 10시, 한정수량 타임딜!</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>풀무원 상품 4개 골라 최대 2만원 할인 + 무료배송</t>
+          <t>쓱세일 봄 스타일링 추천템</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004661&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004555</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>반값다딜 - 풀무원 편 (3/2~12)</t>
+          <t>(0306~12) 패션명품 쓱세일 - 특가</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -577,229 +577,636 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다딜 - 풀무원 편 (3/2~12)', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'Pulmuone 상품쿠폰 50% 4장, 개별 쿠폰 당 최대 5천원 할인', 'Pulmuone 상품쿠폰 무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 2023년 3월 2일(목)~ 2023년 3월 12일 (일)', '       쿠폰 사용 조건', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '(50%, 무료배송) [풀무원] 얇은피 꽉찬속 김치만두 400gx2 할인전 : 9,480원 할인후 : 4,740원', '(50%, 무료배송) [풀무원] 국산콩 투컵 두부 600g 할인전 : 5,480원 할인후 : 2,740원', '(50%, 무료배송) [풀무원] 바릴라 캠핑 기획팩 2,700G 할인전 : 29,800원 할인후 : 14,900원', '(50%, 무료배송) [풀무원] 새콤달콤 유부초밥 330g 할인전 : 5,680원 할인후 : 2,840원', '(50%, 무료배송) [풀무원] 행복한 동물복지유정란 15구 780g : 8,980원 할인후 : 4,490원', '할인 상품 한 눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; (0306~12) 패션명품 쓱세일 - 특가', '스마일클럽', '#혜택 01 매일 오전 10시 초특가 타임딜 바로보기', '한정수량 타임딜', '타임딜은 오전 10시에 시작됩니다!', '오늘의 타임딜이 종료되었습니다.', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '3/6(월) 오후 7시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/7(화) 오후 7시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 8시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 9시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/8(수) 오후 8시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/10(금) 오후 6시, 데카브&amp;CC콜렉트 봄 아우터 한정수량 특 무료배송/무료반품 &amp; 추첨 사은품 증정']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>어서와 봄, 할인상품 득템해 봄</t>
+          <t>패션 명품 쓱세일  라이브 커머스 혜택</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>창고 대개방! 반짝할인 놓치지 말고 득템하세요</t>
+          <t>쓱세일 기간 동안 라이브 보고  경품 받기</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004593</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄</t>
+          <t>[패션명품 쓱세일] SSG.LIVE 라이브 구매 이벤트 + 라이브 캘린더 까지</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄', '스마일클럽', '(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄']</t>
+          <t>['이벤트/쿠폰 &gt; [패션명품 쓱세일] SSG.LIVE 라이브 구매 이벤트 + 라이브 캘린더 까지', '스마일클럽', '[패션명품 쓱세일] SSG.LIVE 라이브 구매 이벤트 + 라이브 캘린더 까지', '[쓱라이브 이벤트 주의사항]', '-\xa0패션쓱\xa0SSG.LIVE\xa0에서 패션쓱\xa0SSG.LIVE\xa0제품 구매시\xa0이벤트 응모한 것으로 간주됩니다.', '-\xa0이벤트는 모두 주문번호\xa01개 기준 집계 및 증정됩니다.', '-\xa0구매 취소시 이벤트 당첨은 모두 취소됩니다.', '-\xa0이벤트에 응모하시는 경우,\xa0아래 개인정보 제공에 동의하신 것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다.', '-\xa0사은품 지급 및 이벤트 혜택 제공', '-\xa0사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기', '6.\xa0본 이벤트 경품은 브랜드사 상황에 따라 사전 고지 없이 변경,\xa0대체 될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>최대 7.2만원 혜택</t>
+          <t>어서와 봄, 할인상품 득템해 봄</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>창고대개방! 봄 맞이 할인 놓치지 마세요.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004717</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; (3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄', '스마일클럽', '(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>첫구매는 반값다딜 &lt;풀무원 편&gt;</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>풀무원 상품 4개 골라 최대 2만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004661&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>반값다딜 - 풀무원 편 (3/2~12)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다딜 - 풀무원 편 (3/2~12)', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'Pulmuone 상품쿠폰 50% 4장, 개별 쿠폰 당 최대 5천원 할인', 'Pulmuone 상품쿠폰 무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 2023년 3월 2일(목)~ 2023년 3월 12일 (일)', '       쿠폰 사용 조건', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '(50%, 무료배송) [풀무원] 얇은피 꽉찬속 김치만두 400gx2 할인전 : 9,480원 할인후 : 4,740원', '(50%, 무료배송) [풀무원] 국산콩 투컵 두부 600g 할인전 : 5,480원 할인후 : 2,740원', '(50%, 무료배송) [풀무원] 바릴라 캠핑 기획팩 2,700G 할인전 : 29,800원 할인후 : 24,800원', '(50%, 무료배송) [풀무원] 새콤달콤 유부초밥 330g 할인전 : 5,680원 할인후 : 2,840원', '(50%, 무료배송) [풀무원] 행복한 동물복지유정란 15구 780g : 8,980원 할인후 : 4,490원', '할인 상품 한 눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SK-II 3/2(목) 8PM</t>
+          <t>Romantic 화이트데이</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>극광 에센스 리뉴얼 최초 공개! 선착순 핫딜 20만원대+백화점 상품권 증정+선물포장</t>
+          <t>장바구니 10% 쿠폰+ 달콤한 사랑을 전하세요</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004573&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004520</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]3/2(목) SK-II</t>
+          <t>Romantic 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/2(목) SK-II', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; Romantic 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!', '스마일클럽', '화이트데이 10% 쿠폰 받고 쇼핑 GO! 바로보기', '#10% 장바구니 쿠폰', '사탕만큼 달콤한 10% 할인 쿠폰 바로보기', '10% 장바구니 할인 쿠폰', '10% 결제쿠폰 (매일 오전 9시 / 선착순 1만명) - 15만원 이상 구매시 최대 1.5만원 할인', '      쿠폰 발급 기간', '      23/03/06(월) ~ 23/03/12(일), 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용 조건', '+PLUS 카드 청구할인 혜택도 챙겨가세요!', '구호사계절 프리미엄 버킷백, 구호 SSG 단독특가 최대 10%', '프라다 外화이트데이 BEST 명품/잡화 프라다/키플링/빅토리아/스톤헨지 外 인기브랜드 ~ 70% 특가!', '스와로브스키스와로브스키 주얼리 기프트 추천 크리스탈처럼 반짝이는 주얼리 일부 품목 20%']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>보라카이(하나투어) 3/2(목) 9PM</t>
+          <t>SSG 스포츠페어</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>보라카이 베스트셀러 헤난가든 초특가 4/5일</t>
+          <t>매일 오전 9시 선착순 10%쿠폰</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004579&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004731</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>보라카이 여행(하나투어) @SSG.LIVE 3/2(목) 9PM</t>
+          <t>SSG 스포츠페어</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-02-21</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 보라카이 여행(하나투어) @SSG.LIVE 3/2(목) 9PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 스포츠페어', '스마일클럽', '10% 할인쿠폰', '할인의 완성', '매일 오전 9시 선착순 1만명', '스포츠페어 10% 상품쿠폰', '상품쿠폰 10% (매일 오전 9시) (선착순 1만명)', '쿠폰은 매일 오전 9시 발급됩니다.', "발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '23SS UP TO 44%', '최대 20% 할인혜택', '쿠폰할인 대전', '31% OFF', '23SS NEW ARRIVAL 자켓/맨투맨/하의 최대 ~10% OFF', '23SS NEW 스쿨룩 UPTO~20%★', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[나이키코리아공식] 남여 인기 신발 모음 ~45%', '조던/런닝/트레이닝룩 ~44% SALE!', 'CLEARENCE 기획전 ~70% OFF + 15% 쿠폰', '23 SPRING 점퍼/티셔츠/니트 외 30%OFF 50종 택1', '티셔츠/팬츠/스커트 등 신상~이월 최대50%', 'F/W 최대 40% 할인 특집', '[빈폴골프] 남녀 BEST 50 라운딩웨어☆ + SSG 특별 혜택★ + 최대할인쿠폰★', '골프존커머스 BEST 클럽/용품 모음전! 23년 신상부터 이월상품 최대할인까지', '인도어화 할인전']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3월 맘키즈 플러스</t>
+          <t>생필품 특가 위크 10% 선착순 할인 쿠폰</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>지금 할인 중! ~40% 할인 혜택</t>
+          <t>화장지부터 세제까지 우리집 필수템 알뜰 쇼핑</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004597</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>이달의 맘키즈 PLUS</t>
+          <t>생필품 특가 위크</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2999-12-13</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '시크릿쥬쥬 베스트프렌즈마고 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈스쿨백세트 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈리나 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈쥬쥬 (N2쓱배송, 전국택배)', '베스트프렌즈시크릿프렌즈폰 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈미니사물함 (N2쓱배송, 전국택배)', '★금주의 할인딜★ KIDS 침구 / 어린이집 낮잠이불']</t>
+          <t>['이벤트/쿠폰 &gt; 생필품 특가 위크', '스마일클럽', '10% 할인 쿠폰', '금주의 할인 특가', '      쿠폰 적용 대상', '매일 9시 3만명 선착순 상품쿠폰 10% SSG.COM', '2만원 이상 구매 시 최대 1만원 할인', '금일 쿠폰은 모두 소진 되었습니다.', '쿠폰은 매일 오전 9시 발급됩니다', '       쿠폰 발급 및 사용기간', "       쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '       쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '♥[모나리자] 생필품 ~20% 할인♥ 휴지/키친타올/미용티슈/물티슈/각티슈/마스크', '오슬림밴드/에어팬츠 기저귀 ~2개50%(맘키즈회원전용)', '★브랜드할인★ 센트라린 캡슐세탁세제 모음전(아로퓸/카포드/엘에이/향기부스터)', '[★40% SALE★]애경 3월 봄이 왔나봄 할인+쿠폰+다다익선+증정', '엘경유켈. 세제 4대 브랜드 대통합 할인', '[웰라] 프리미엄 살롱 헤어케어 최대 70% off / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '★생필품 특가위크★ 헤어/바디 브랜드별 BEST 단독 할인전', '★생필품 특가 위크★헤어케어 1+1/2개이상10% 모음', '[쓱배송] 3배 빨라진 새치샴푸 런칭 특가전★(함께살수록 할인)', '★천만개 판매돌파★ 지아자/크나이프 SSG 단독할인', '닥터 브로너스 SSG 할인 +증정혜택', '★단독구성+10%쿠폰★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '★생필품 특가 위크★바디케어 1+1/2개이상10% 모음', '세타필 바디로션, 크림  할인 행사', '★단독사은품+최대46%할인가★ 리스테린 쿨민트/그린티 외 250ml&amp;750ml 모음전', '[서인국마스크][5%다운쿠폰]38년 필터 기업이 만든 귀가 편한 시노텍스 마스크', '1+1 / 다다익선 할인 혜택', '세제/헤어/바디 ~40% 할인+적립', '~30% OFF + 다다익선  + 증정품', '인기 제품&amp;기획SET 최대 ~30% OFF', '★배송비특가★헤어플러스 브랜드 위크+할인쿠폰+사은품까지!', '리뷰이벤트 단독 SSGX살롱클리닉 청담 살롱 새치 ALL 커버 셀프 염색약 전 상품 특가 15% 쿠폰 할인까지', '기획전★ 구매왕+다다익선 10%+구매사은품', '도브 바디로션 런칭기념행사 [최대~50%할인]']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SPRING IS COMING</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>다가오는 봄, 나에게 주는 선물부터 달콤한 봄 GIFT까지!</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004736</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>SPRING IS COMING</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-03-06</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2023-03-19</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SPRING IS COMING', '스마일클럽']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SSG 브랜드 스포트라이트: 코치</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SSG단독 10% 할인 + 구매 사은품 증정</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004624</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>SSG 브랜드 스포트라이트 - 코치</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-03-06</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023-03-12</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 코치', '스마일클럽', '상위 20%의 엄선된 고품질 가죽으로 제작된 코치만의 가죽 지갑 최소한의 가공으로 원가죽 무늬와 느낌을 살린 똑같은 가죽이 아닌 하나 뿐인 고유한 상품', '      01 SSG 단독 브랜드 스포트라이트 기간 중 10% 할인 혜택']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>W컨셉 SPRING SHOP#</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>모한, 르니나 外 봄 아이템 추천 + 15% 쿠폰 혜택</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004587</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>(0306~0312) W컨셉 SPRING SHOP#</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-03-06</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-03-12</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; (0306~0312) W컨셉 SPRING SHOP#', '스마일클럽', 'SPECIAL OFFER 15% 쿠폰 바로보기', 'SPECIAL OFFER 15% 상품 쿠폰', '15% 상품쿠폰 - 2만원 이상 구매시 최대 2만원 할인', '         쿠폰 발급 및 사용 기간', '         2만원 이상 상품 구매 시 15% 할인, 최대 2만원 (기간내 ID당 발급수량 2장)', '         쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에도 상품 상세에서 쿠폰을 다운받으실 수 없습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>민지의 장바구니-화이트데이편</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004754&amp;domainSiteNo=7018</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>민지의 장바구니-화이트데이편 (3/6~3/12)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-03-06</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2023-03-12</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-화이트데이편 (3/6~3/12)', '스마일클럽', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>최대 7.2만원 혜택</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-07-08</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023-06-28</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022-10-26</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '최대 2% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>프레드페리 3/6(월) 7PM</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>우븐트랙자켓 단독 발매+S머니 할인! 봄신상 &amp; 이월 최대 56%</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004605&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>프레드페리@SSG.LIVE 3/6(월) 19:00PM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2023-03-09</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 프레드페리@SSG.LIVE 3/6(월) 19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>[월간호캉쓱] 파라다이스 시티 3/6(월) 8PM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1박 + 6만 리조트머니 27만원대~, 2박 + 조식 + 3만 리조트 머니 54만원대~</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004712&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>파라다이스 시티 @SSG.LIVE 3/6(월) 20:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2023-03-06</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 파라다이스 시티 @SSG.LIVE 3/6(월) 20:00', '스마일클럽']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>킨록by킨록앤더슨 3/7(화) 19PM</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>신상 30% 선할인&amp;이월 ~30% 할인 라이브 한정 특가 진행</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004588&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>킨록by 라이브 동안 신상품 30% 할인 @SSG.LIVE 3//7(화) 19PM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2023-03-07</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 킨록by 라이브 동안 신상품 30% 할인 @SSG.LIVE 3//7(화) 19PM', '스마일클럽', '킨록by 라이브 동안 신상품 30% 할인 @SSG.LIVE 3//7(화) 19PM']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>[패션명품 쓱세일] 구해줘명품즈 시즌2 3/7(화) 8PM</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>골든구스/보테가베네타/마르지엘라 외 SS명품 한정수량 역대급 파격 특가</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004703&amp;domainSiteNo=6005</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>구해줘명품즈2 @SSG.LIVE 3/7(화) 20:00PM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2023-03-07</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 구해줘명품즈2 @SSG.LIVE 3/7(화) 20:00PM', '스마일클럽', '                    SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>온앤온 3/7(화) 9PM</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>봄 신상 &amp; 이월 최대 67%! 싱글 투버튼 자켓 선착순 9만9천원 핫딜</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004705&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>온앤온 @SSG.LIVE 3/7(화) 9PM</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2023-03-08</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 온앤온 @SSG.LIVE 3/7(화) 9PM', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Mar  9 00:21:54 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(0306~12) 패션명품 쓱세일 - 혜택</t>
+          <t>패션명품 쓱세일</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0306~12) 패션명품 쓱세일 - 혜택', '스마일클럽', '#혜택 01 패션의류/잡화 전용 할인 혜택 바로보기', '#혜택 02 명품 전용 할인 혜택 바로보기', '#혜택 04 매일매일 카드청구할인 바로보기', '최대 15% 할인! 패션의류/잡화 전용 할인 혜택', '패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 2만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장(패션명품 쓱세일)', '쿠폰 받기(기간 내 ID당 1회)', '       상품별 15% 할인', '       2만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '       쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다.(동일상품 복수 개 구매 시 1개 수량에만 적용)', '* 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세에서 쿠폰을 다운 받으실 수 없습니다.', '패션의류/잡화 대표 브랜드 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '백화점 패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 5만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장', '       5만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '최대 15만원 할인! 명품 전용 할인 혜택', '상품쿠폰 7% - 10만원 이상 상품 구매 시 7% 할인, 최대 10만원', '상품쿠폰 8% - 30만원 이상 상품 구매 시 8% 할인, 최대 15만원', '더 많은 상품을 담아 최대 8% 할인 받는 장바구니 쿠폰', '* 타 사이트를 통해 방문하신 고객의 경우, 상품 구매 시 쿠폰이 적용되지 않습니다.', '장바구니쿠폰 8% - 7만원 이상 구매 시 최대 3만원 할인(ID당 1장 발급)', '쿠폰 받기', 'W컨셉 SPRING SHOP 15% 쿠폰과 함께 W컨셉의 감성을 담은 봄 패션 아이템을 만나보세요!', '신세계백화점몰&amp;신세계몰 첫구매 고객이라면\xa0 BONUS 쿠폰 하나 더!', '* 신세계백화점몰 및 신세계몰 첫구매 고객 대상으로 발급되는 쿠폰입니다.', '장바구니쿠폰 12% - 7만원 이상 구매 시 최대 2만원 할인 ID당 1장 발급(첫구매 전용, 패션/명품 전용, 선착순 1만명)', '선착순 쿠폰이 마감되었습니다.', '카드 혜택도 놓치지 마세요! 매일매일 카드 청구할인', '[SSGPAY전용] 삼성카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 결제 시 10% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기', '[SSGPAY전용] KB국민카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 패션명품 쓱세일', '스마일클럽', '#혜택 01 패션의류/잡화 전용 할인 혜택 바로보기', '#혜택 02 명품 전용 할인 혜택 바로보기', '#혜택 04 매일매일 카드청구할인 바로보기', '최대 15% 할인! 패션의류/잡화 전용 할인 혜택', '패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 2만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장(패션명품 쓱세일)', '쿠폰 받기(기간 내 ID당 1회)', '       상품별 15% 할인', '       2만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '       쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다.(동일상품 복수 개 구매 시 1개 수량에만 적용)', '* 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세에서 쿠폰을 다운 받으실 수 없습니다.', '패션의류/잡화 대표 브랜드 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '백화점 패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 5만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장', '       5만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '최대 15만원 할인! 명품 전용 할인 혜택', '상품쿠폰 7% - 10만원 이상 상품 구매 시 7% 할인, 최대 10만원', '상품쿠폰 8% - 30만원 이상 상품 구매 시 8% 할인, 최대 15만원', '더 많은 상품을 담아 최대 8% 할인 받는 장바구니 쿠폰', '* 타 사이트를 통해 방문하신 고객의 경우, 상품 구매 시 쿠폰이 적용되지 않습니다.', '장바구니쿠폰 8% - 7만원 이상 구매 시 최대 3만원 할인(ID당 1장 발급)', '쿠폰 받기', 'W컨셉 SPRING SHOP 15% 쿠폰과 함께 W컨셉의 감성을 담은 봄 패션 아이템을 만나보세요!', '신세계백화점몰&amp;신세계몰 첫구매 고객이라면\xa0 BONUS 쿠폰 하나 더!', '* 신세계백화점몰 및 신세계몰 첫구매 고객 대상으로 발급되는 쿠폰입니다.', '장바구니쿠폰 12% - 7만원 이상 구매 시 최대 2만원 할인 ID당 1장 발급(첫구매 전용, 패션/명품 전용, 선착순 1만명)', '선착순 쿠폰이 마감되었습니다.', '카드 혜택도 놓치지 마세요! 매일매일 카드 청구할인', '[SSGPAY전용] 삼성카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 결제 시 10% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기', '[SSGPAY전용] KB국민카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기']</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(0306~12) 패션명품 쓱세일 - 브랜드</t>
+          <t>패션명품 쓱세일</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0306~12) 패션명품 쓱세일 - 브랜드', '스마일클럽', '알도 - 그랜드오픈 기념 단독특가 + 15% 쿠폰 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 패션명품 쓱세일', '스마일클럽', '알도 - 그랜드오픈 기념 단독특가 + 15% 쿠폰 자세히 보기']</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(0306~12) 패션명품 쓱세일 - 특가</t>
+          <t>패션명품 쓱세일</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0306~12) 패션명품 쓱세일 - 특가', '스마일클럽', '#혜택 01 매일 오전 10시 초특가 타임딜 바로보기', '한정수량 타임딜', '타임딜은 오전 10시에 시작됩니다!', '오늘의 타임딜이 종료되었습니다.', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '3/6(월) 오후 7시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/7(화) 오후 7시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 8시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 9시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/8(수) 오후 8시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/10(금) 오후 6시, 데카브&amp;CC콜렉트 봄 아우터 한정수량 특 무료배송/무료반품 &amp; 추첨 사은품 증정']</t>
+          <t>['이벤트/쿠폰 &gt; 패션명품 쓱세일', '스마일클럽', '#혜택 01 매일 오전 10시 초특가 타임딜 바로보기', '한정수량 타임딜', '타임딜은 오전 10시에 시작됩니다!', '오늘의 타임딜이 종료되었습니다.', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '3/6(월) 오후 7시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/7(화) 오후 7시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 8시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 9시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/8(수) 오후 8시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/10(금) 오후 6시, 데카브&amp;CC콜렉트 봄 아우터 한정수량 특 무료배송/무료반품 &amp; 추첨 사은품 증정']</t>
         </is>
       </c>
     </row>
@@ -621,22 +621,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>어서와 봄, 할인상품 득템해 봄</t>
+          <t>첫구매는 반값다딜 &lt;풀무원 편&gt;</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>창고대개방! 봄 맞이 할인 놓치지 마세요.</t>
+          <t>풀무원 상품 4개 골라 최대 2만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004717</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004661&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄</t>
+          <t>반값다딜 - 풀무원 편 (3/2~12)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -646,56 +646,56 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄', '스마일클럽', '(3/2~31) 창고대개방! 어서 와 봄, 할인상품 득템해 봄']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다딜 - 풀무원 편 (3/2~12)', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'Pulmuone 상품쿠폰 50% 4장, 개별 쿠폰 당 최대 5천원 할인', 'Pulmuone 상품쿠폰 무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 2023년 3월 2일(목)~ 2023년 3월 12일 (일)', '       쿠폰 사용 조건', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '(50%, 무료배송) [풀무원] 얇은피 꽉찬속 김치만두 400gx2 할인전 : 9,480원 할인후 : 4,740원', '(50%, 무료배송) [풀무원] 국산콩 투컵 두부 600g 할인전 : 5,480원 할인후 : 2,740원', '(50%, 무료배송) [풀무원] 바릴라 캠핑 기획팩 2,700G 할인전 : 29,800원 할인후 : 24,800원', '(50%, 무료배송) [풀무원] 새콤달콤 유부초밥 330g 할인전 : 5,680원 할인후 : 2,840원', '(50%, 무료배송) [풀무원] 행복한 동물복지유정란 15구 780g : 8,980원 할인후 : 4,490원', '할인 상품 한 눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>첫구매는 반값다딜 &lt;풀무원 편&gt;</t>
+          <t>2023 대한민국 수산대전 ? 봄 맞이전</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>풀무원 상품 4개 골라 최대 2만원 할인 + 무료배송</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004661&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004679</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>반값다딜 - 풀무원 편 (3/2~12)</t>
+          <t>(3/9~15) 2023 대한민국 수산대전 - 봄 맞이전</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-15</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다딜 - 풀무원 편 (3/2~12)', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'Pulmuone 상품쿠폰 50% 4장, 개별 쿠폰 당 최대 5천원 할인', 'Pulmuone 상품쿠폰 무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 2023년 3월 2일(목)~ 2023년 3월 12일 (일)', '       쿠폰 사용 조건', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '(50%, 무료배송) [풀무원] 얇은피 꽉찬속 김치만두 400gx2 할인전 : 9,480원 할인후 : 4,740원', '(50%, 무료배송) [풀무원] 국산콩 투컵 두부 600g 할인전 : 5,480원 할인후 : 2,740원', '(50%, 무료배송) [풀무원] 바릴라 캠핑 기획팩 2,700G 할인전 : 29,800원 할인후 : 24,800원', '(50%, 무료배송) [풀무원] 새콤달콤 유부초밥 330g 할인전 : 5,680원 할인후 : 2,840원', '(50%, 무료배송) [풀무원] 행복한 동물복지유정란 15구 780g : 8,980원 할인후 : 4,490원', '할인 상품 한 눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; (3/9~15) 2023 대한민국 수산대전 - 봄 맞이전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Romantic 화이트데이</t>
+          <t>러블리 화이트데이</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Romantic 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!</t>
+          <t>러블리 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Romantic 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!', '스마일클럽', '화이트데이 10% 쿠폰 받고 쇼핑 GO! 바로보기', '#10% 장바구니 쿠폰', '사탕만큼 달콤한 10% 할인 쿠폰 바로보기', '10% 장바구니 할인 쿠폰', '10% 결제쿠폰 (매일 오전 9시 / 선착순 1만명) - 15만원 이상 구매시 최대 1.5만원 할인', '      쿠폰 발급 기간', '      23/03/06(월) ~ 23/03/12(일), 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용 조건', '+PLUS 카드 청구할인 혜택도 챙겨가세요!', '구호사계절 프리미엄 버킷백, 구호 SSG 단독특가 최대 10%', '프라다 外화이트데이 BEST 명품/잡화 프라다/키플링/빅토리아/스톤헨지 外 인기브랜드 ~ 70% 특가!', '스와로브스키스와로브스키 주얼리 기프트 추천 크리스탈처럼 반짝이는 주얼리 일부 품목 20%']</t>
+          <t>['이벤트/쿠폰 &gt; 러블리 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!', '스마일클럽', '화이트데이 10% 쿠폰 받고 쇼핑 GO! 바로보기', '#10% 장바구니 쿠폰', '사탕만큼 달콤한 10% 할인 쿠폰 바로보기', '10% 장바구니 할인 쿠폰', '10% 결제쿠폰 (매일 오전 9시 / 선착순 1만명) - 15만원 이상 구매시 최대 1.5만원 할인', '      쿠폰 발급 기간', '      23/03/06(월) ~ 23/03/12(일), 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용 조건', '+PLUS 카드 청구할인 혜택도 챙겨가세요!', '구호사계절 프리미엄 버킷백, 구호 SSG 단독특가 최대 15%', '프라다 外화이트데이 BEST 명품/잡화 프라다/키플링/빅토리아/스톤헨지 外 인기브랜드 ~ 70% 특가!', '스와로브스키스와로브스키 주얼리 기프트 추천 크리스탈처럼 반짝이는 주얼리 일부 품목 20%']</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 생필품 특가 위크', '스마일클럽', '10% 할인 쿠폰', '금주의 할인 특가', '      쿠폰 적용 대상', '매일 9시 3만명 선착순 상품쿠폰 10% SSG.COM', '2만원 이상 구매 시 최대 1만원 할인', '금일 쿠폰은 모두 소진 되었습니다.', '쿠폰은 매일 오전 9시 발급됩니다', '       쿠폰 발급 및 사용기간', "       쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '       쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '♥[모나리자] 생필품 ~20% 할인♥ 휴지/키친타올/미용티슈/물티슈/각티슈/마스크', '오슬림밴드/에어팬츠 기저귀 ~2개50%(맘키즈회원전용)', '★브랜드할인★ 센트라린 캡슐세탁세제 모음전(아로퓸/카포드/엘에이/향기부스터)', '[★40% SALE★]애경 3월 봄이 왔나봄 할인+쿠폰+다다익선+증정', '엘경유켈. 세제 4대 브랜드 대통합 할인', '[웰라] 프리미엄 살롱 헤어케어 최대 70% off / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '★생필품 특가위크★ 헤어/바디 브랜드별 BEST 단독 할인전', '★생필품 특가 위크★헤어케어 1+1/2개이상10% 모음', '[쓱배송] 3배 빨라진 새치샴푸 런칭 특가전★(함께살수록 할인)', '★천만개 판매돌파★ 지아자/크나이프 SSG 단독할인', '닥터 브로너스 SSG 할인 +증정혜택', '★단독구성+10%쿠폰★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '★생필품 특가 위크★바디케어 1+1/2개이상10% 모음', '세타필 바디로션, 크림  할인 행사', '★단독사은품+최대46%할인가★ 리스테린 쿨민트/그린티 외 250ml&amp;750ml 모음전', '[서인국마스크][5%다운쿠폰]38년 필터 기업이 만든 귀가 편한 시노텍스 마스크', '1+1 / 다다익선 할인 혜택', '세제/헤어/바디 ~40% 할인+적립', '~30% OFF + 다다익선  + 증정품', '인기 제품&amp;기획SET 최대 ~30% OFF', '★배송비특가★헤어플러스 브랜드 위크+할인쿠폰+사은품까지!', '리뷰이벤트 단독 SSGX살롱클리닉 청담 살롱 새치 ALL 커버 셀프 염색약 전 상품 특가 15% 쿠폰 할인까지', '기획전★ 구매왕+다다익선 10%+구매사은품', '도브 바디로션 런칭기념행사 [최대~50%할인]']</t>
+          <t>['이벤트/쿠폰 &gt; 생필품 특가 위크', '스마일클럽', '10% 할인 쿠폰', '금주의 할인 특가', '      쿠폰 적용 대상', '매일 9시 3만명 선착순 상품쿠폰 10% SSG.COM', '2만원 이상 구매 시 최대 1만원 할인', '금일 쿠폰은 모두 소진 되었습니다.', '쿠폰은 매일 오전 9시 발급됩니다', '       쿠폰 발급 및 사용기간', "       쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '       쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '♥[모나리자] 생필품 ~20% 할인♥ 휴지/키친타올/미용티슈/물티슈/각티슈/마스크', '오슬림밴드/에어팬츠 기저귀 ~2개50%(맘키즈회원전용)', '★브랜드할인★ 센트라린 캡슐세탁세제 모음전(아로퓸/카포드/엘에이/향기부스터)', '[★40% SALE★]애경 3월 봄이 왔나봄 할인+쿠폰+다다익선+증정', '[쓱배송]때가 쏙 비트 세탁세제&amp;참그린 주방세제 최대 1+1 모음전', '[쓱배송]피죤 생필품 1+1 특가전', '엘경유켈. 세제 4대 브랜드 대통합 할인', '[웰라] 프리미엄 살롱 헤어케어 최대 70% off / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '[쓱배송] 3배 빨라진 새치샴푸 런칭 특가전★(함께살수록 할인)', '★천만개 판매돌파★ 지아자/크나이프 SSG 단독할인', '최대~36%할인 +구매별 60ml 증정 혜택', '★단독구성+10%쿠폰★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '★생필품 특가 위크★바디케어 1+1/2개이상10% 모음', '세타필 바디로션, 크림  할인 행사', '★단독사은품+최대46%할인가★ 리스테린 쿨민트/그린티 외 250ml&amp;750ml 모음전', '[서인국마스크][5%다운쿠폰]38년 필터 기업이 만든 귀가 편한 시노텍스 마스크', '1+1 / 다다익선 할인 혜택', '세제/헤어/바디 ~40% 할인+적립', '~30% OFF + 다다익선  + 증정품', '인기 제품&amp;기획SET 최대 ~30% OFF', '★배송비특가★헤어플러스 브랜드 위크+할인쿠폰+사은품까지!', '★SSG단독 특가★  살롱클리닉 새치 ALL 커버 셀프 염색약 전 상품 특가 (할인+쿠폰+15%추가 쿠폰+증정품까지)', '기획전★ 구매왕+다다익선 10%+구매사은품', '도브 바디로션 런칭기념행사 [최대~50%할인]']</t>
         </is>
       </c>
     </row>
@@ -880,59 +880,59 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>W컨셉 SPRING SHOP#</t>
+          <t>3월 로맨틱 다이닝 도전 홈스토랑 파스타</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>모한, 르니나 外 봄 아이템 추천 + 15% 쿠폰 혜택</t>
+          <t>소스 1+1 구성부터 SSG머니 이벤트 행운까지!</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004587</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004777</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(0306~0312) W컨셉 SPRING SHOP#</t>
+          <t>집 밥 챌린지 - 파스타편</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-15</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (0306~0312) W컨셉 SPRING SHOP#', '스마일클럽', 'SPECIAL OFFER 15% 쿠폰 바로보기', 'SPECIAL OFFER 15% 상품 쿠폰', '15% 상품쿠폰 - 2만원 이상 구매시 최대 2만원 할인', '         쿠폰 발급 및 사용 기간', '         2만원 이상 상품 구매 시 15% 할인, 최대 2만원 (기간내 ID당 발급수량 2장)', '         쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에도 상품 상세에서 쿠폰을 다운받으실 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 파스타편', '스마일클럽', '이번 주는 특별하게, 파스타로 홈스토랑 셰프가 되어보세요. 소스 최대 1+1부터, 샐러드/파스타/스테이크 할인 취향 투표하면 SSG머니 행운이!', '최대 1+1 할인 파스타 소스 추천 상품', "        당첨자 발표 일정: 2023년 3월 20일 발표 예정 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요’", '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '올리브오일 최대 40% 할인 - 다양한 요리유의 세계 확인하기', '해산물/채소 할인']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>민지의 장바구니-화이트데이편</t>
+          <t>W컨셉 SPRING SHOP#</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+          <t>모한, 르니나 外 봄 아이템 추천 + 15% 쿠폰 혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004754&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004587</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>민지의 장바구니-화이트데이편 (3/6~3/12)</t>
+          <t>W컨셉 SPRING SHOP#</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -947,214 +947,214 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-화이트데이편 (3/6~3/12)', '스마일클럽', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; W컨셉 SPRING SHOP#', '스마일클럽', 'SPECIAL OFFER 15% 쿠폰 바로보기', 'SPECIAL OFFER 15% 상품 쿠폰', '15% 상품쿠폰 - 2만원 이상 구매시 최대 2만원 할인', '         쿠폰 발급 및 사용 기간', '         2만원 이상 상품 구매 시 15% 할인, 최대 2만원 (기간내 ID당 발급수량 2장)', '         쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에도 상품 상세에서 쿠폰을 다운받으실 수 없습니다.']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>최대 7.2만원 혜택</t>
+          <t>민지의 장바구니-화이트데이편</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004754&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>민지의 장바구니-화이트데이편 (3/6~3/12)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-03-12</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-화이트데이편 (3/6~3/12)', '스마일클럽', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '쓱배송 8만원 이상 구매시, 응모필수! 오늘 단 하루, SSG머니 5천원 100% 페이백']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>최대 7.2만원 혜택</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '최대 2% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>프레드페리 3/6(월) 7PM</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>우븐트랙자켓 단독 발매+S머니 할인! 봄신상 &amp; 이월 최대 56%</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004605&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>프레드페리@SSG.LIVE 3/6(월) 19:00PM</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 프레드페리@SSG.LIVE 3/6(월) 19:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[월간호캉쓱] 파라다이스 시티 3/6(월) 8PM</t>
+          <t>[공동판매구역] 세이펜 3/9(목) 11AM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1박 + 6만 리조트머니 27만원대~, 2박 + 조식 + 3만 리조트 머니 54만원대~</t>
+          <t>우리아이 교육 필수품 역대급 혜택LIVE!</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004712&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004755&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>파라다이스 시티 @SSG.LIVE 3/6(월) 20:00</t>
+          <t>[SSG.LIVE]3/9(목) 세이펜</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 파라다이스 시티 @SSG.LIVE 3/6(월) 20:00', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/9(목) 세이펜', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>킨록by킨록앤더슨 3/7(화) 19PM</t>
+          <t>명품대전 3/9(목) 8PM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>신상 30% 선할인&amp;이월 ~30% 할인 라이브 한정 특가 진행</t>
+          <t>프라다/보테가베네타/오트리/메종키츠네/멀버리/발렌티노/아미 외~</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004588&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004598&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>킨록by 라이브 동안 신상품 30% 할인 @SSG.LIVE 3//7(화) 19PM</t>
+          <t>명품대전 @SSG.LIVE 3/9(목) 8PM</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-03-07</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 킨록by 라이브 동안 신상품 30% 할인 @SSG.LIVE 3//7(화) 19PM', '스마일클럽', '킨록by 라이브 동안 신상품 30% 할인 @SSG.LIVE 3//7(화) 19PM']</t>
+          <t>['이벤트/쿠폰 &gt; 명품대전 @SSG.LIVE 3/9(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[패션명품 쓱세일] 구해줘명품즈 시즌2 3/7(화) 8PM</t>
+          <t>데카브&amp;CC콜렉트 3/10(금) 6PM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>골든구스/보테가베네타/마르지엘라 외 SS명품 한정수량 역대급 파격 특가</t>
+          <t>[패션명품 쓱세일] 데카브&amp;CC콜렉트 2023년 신상&amp;이월 최대 81% 할인</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004703&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004600&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>구해줘명품즈2 @SSG.LIVE 3/7(화) 20:00PM</t>
+          <t>[패션명품 쓱세일] 데카브&amp;CC콜렉트 @SSG.LIVE 3/10(금) 6PM</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1164,49 +1164,49 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023-03-07</t>
+          <t>2023-03-10</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 구해줘명품즈2 @SSG.LIVE 3/7(화) 20:00PM', '스마일클럽', '                    SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [패션명품 쓱세일] 데카브&amp;CC콜렉트 @SSG.LIVE 3/10(금) 6PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>온앤온 3/7(화) 9PM</t>
+          <t>3월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>봄 신상 &amp; 이월 최대 67%! 싱글 투버튼 자켓 선착순 9만9천원 핫딜</t>
+          <t>지금 할인 중! ~40% 할인 혜택</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004705&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>온앤온 @SSG.LIVE 3/7(화) 9PM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-03-08</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 온앤온 @SSG.LIVE 3/7(화) 9PM', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '시크릿쥬쥬 베스트프렌즈마고 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈스쿨백세트 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈리나 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈쥬쥬 (N2쓱배송, 전국택배)', '베스트프렌즈시크릿프렌즈폰 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈미니사물함 (N2쓱배송, 전국택배)', '★금주의 할인딜★ KIDS 침구 / 어린이집 낮잠이불']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Mar 13 00:21:01 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,360 +473,360 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일 NEW SPRING, NEW ITEM</t>
+          <t>SSG 창립 4주년 쓱배송데이</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>최대15% 할인 쿠폰팩 + 청구할인 혜택</t>
+          <t>하루 두 번 10% 선착순 쿠폰 + 카드 할인</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004551</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004809</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일</t>
+          <t>3/13  창립 기념 쓱배송데이</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 패션명품 쓱세일', '스마일클럽', '#혜택 01 패션의류/잡화 전용 할인 혜택 바로보기', '#혜택 02 명품 전용 할인 혜택 바로보기', '#혜택 04 매일매일 카드청구할인 바로보기', '최대 15% 할인! 패션의류/잡화 전용 할인 혜택', '패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 2만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장(패션명품 쓱세일)', '쿠폰 받기(기간 내 ID당 1회)', '       상품별 15% 할인', '       2만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '       쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다.(동일상품 복수 개 구매 시 1개 수량에만 적용)', '* 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세에서 쿠폰을 다운 받으실 수 없습니다.', '패션의류/잡화 대표 브랜드 쿠폰 대상 상품은 검색결과에서도 쉽게 보여요!', '백화점 패션의류/잡화 대표 브랜드 15% 상품쿠폰', '상품쿠폰 15% - 5만원 이상 상품 구매 시 15% 할인, 최대 3만원 2장', '       5만원 이상 상품 구매 시 15% 할인, 최대 3만원 (ID당 발급수량 2장)', '최대 15만원 할인! 명품 전용 할인 혜택', '상품쿠폰 7% - 10만원 이상 상품 구매 시 7% 할인, 최대 10만원', '상품쿠폰 8% - 30만원 이상 상품 구매 시 8% 할인, 최대 15만원', '더 많은 상품을 담아 최대 8% 할인 받는 장바구니 쿠폰', '* 타 사이트를 통해 방문하신 고객의 경우, 상품 구매 시 쿠폰이 적용되지 않습니다.', '장바구니쿠폰 8% - 7만원 이상 구매 시 최대 3만원 할인(ID당 1장 발급)', '쿠폰 받기', 'W컨셉 SPRING SHOP 15% 쿠폰과 함께 W컨셉의 감성을 담은 봄 패션 아이템을 만나보세요!', '신세계백화점몰&amp;신세계몰 첫구매 고객이라면\xa0 BONUS 쿠폰 하나 더!', '* 신세계백화점몰 및 신세계몰 첫구매 고객 대상으로 발급되는 쿠폰입니다.', '장바구니쿠폰 12% - 7만원 이상 구매 시 최대 2만원 할인 ID당 1장 발급(첫구매 전용, 패션/명품 전용, 선착순 1만명)', '선착순 쿠폰이 마감되었습니다.', '카드 혜택도 놓치지 마세요! 매일매일 카드 청구할인', '[SSGPAY전용] 삼성카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 결제 시 10% 청구할인 (일 10만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기', '[SSGPAY전용] KB국민카드 8만원 이상 결제 시 8% 청구할인 (일 10만원 ) 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 3/13  창립 기념 쓱배송데이', '스마일클럽', '3/13  창립 기념 쓱배송데이', 'SSG 창립 4주년 감사대축제 쓱배송데이', '10% 쿠폰 + 5천원 적립 + 카드혜택', '쓱배송 DAY 남은 시간', '10% 쿠폰 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오전 쿠폰', '      이마트, 트레이더스 쓱배송 및 점포택배 / 새벽배송', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만원 할인 오전 또는 오후 쿠폰 ID당 1일 1매 다운(오전 9시 오픈, 선착순 2만명)', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오후 쿠폰', '      쿠폰 발급 및 사용일', '      23년 3월 13일(오전 또는 오후 쿠폰 ID당 1일 1매 다운)(발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', '[SSGPAY전용] 삼성카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] KB국민카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 8만원이상 8% 청구할인 (일 5만원 한) 자세히보기', '인기상품 1+1, 최대 50% 할인 쓱배송데이 장보기 특가상품', '오늘 원하는 시간에 받고 싶다면, 이마트몰 쓱배송 추천상품', '대용량 쟁여두기가 필요할 땐, 트레이더스 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일 23 S/S BEST BRAND FOR U</t>
+          <t>SSG 창립4주년 감사대축제 'Thanks 4U'</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>마시모두띠/칼린 외 TOP 브랜드</t>
+          <t>누구나 6종 쿠폰팩 + 매일 오전 10시 선착순 타임딜 + 브랜드 갈라쇼</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004552</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004808</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일</t>
+          <t>SSG 창립 4주년 감사대축제 'Thanks 4 U'</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 패션명품 쓱세일', '스마일클럽', '알도 - 그랜드오픈 기념 단독특가 + 15% 쿠폰 자세히 보기']</t>
+          <t>["이벤트/쿠폰 &gt; SSG 창립 4주년 감사대축제 'Thanks 4 U'", '스마일클럽', '누구나 10% 할인 쿠폰 6매 / 최대 2만 5천원 할인', '6종 쿠폰 바로보기', '선착순 타임딜 바로보기', '한 시간 한정 최대 3만원 장바구니 쿠폰 발급 중!', '지금 바로! 장바구니 게릴라 쿠폰 놓치지 말고 받아가세요!', '장바구니 쿠폰 10% 8만원 이상 구매시 최대 3만원 할인', '※ 타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '딱 한시간만! 최대 3만원 장바구니 쿠폰 발급 중!', '쿠폰 발급 시간 : 2023년 3월 13일(월) 10시 00분 부터 3월 13일(월) 10시 59분 까지', '쿠폰 발급 시간 : 2023년 3월 15일(수) 10시 00분 부터 3월 15일(수) 10시 59분 까지', '타 사이트를 통해 방문하신 고객의 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '10% 할인 쿠폰 6매 누구나 최대 2만 5천원 할인!', '상품쿠폰 10% X 6', '6종 쿠폰팩 한번에 다운 받기', '쿠폰 할인 대상 및 사용 안내(레이어팝업 열기)', '※ 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '쿠폰 이용안내', '할인 대상', '      10% 상품쿠폰 2매 (1만원 이상 상품 구매시 ~3천원 할인 / 4만원 이상 상품 구매시 ~5천원 할인)', '      10% 상품쿠폰 2매 (1만원 이상 상품 구매시 ~3천원 할인 / 7만원 이상 상품 구매시 ~8천원 할인)', '      10% 상품쿠폰 2매 (10만원 이상 상품 구매시 ~1만 5천원 할인, 20만원 이상 상품 구매시 ~2만 5천원 할인)', '쿠폰은 신세계몰, 신세계백화점몰 각 해당 카테고리에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '신세계몰&amp;신세계백화점몰 첫구매 고객님이신가요\xa0', '첫구매 응원 최대 12% 장바구니 쿠폰', '매일 오전 07시 선착순 1만장 장바구니 쿠폰 12% 8민원 이상 구매시 최대 2만원 할인', '신세계백화점몰 및 신세계몰 첫구매 고객 대상 으로 발급되는 쿠폰 입니다.', '타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '쿠폰 마감 되었습니다.', '쿠폰발급 대상 : 2022년 3월 12일 이후로 신세계몰, 신세계백화점몰 구매 이력이 없는 고객', '타사이트를 통해 방문하신 경우 결제시 장바구니 쿠폰이 적용되지 않습니다.', '매일 오전 10시! 선착순 타임딜', '망설이명 품절! 핫딜로 구매하세요', '타임딜 행사는 SSG 모바일로 확인해주세요', '       타임딜 진행시간', '타임딜 대표 상품 미리보기', '3월 15일(화) : ★타임딜★ [립프로그] 아이스크림카트 디럭스(한영버전) 핑크, [SSG][2박스]팸퍼스 베이비드라이 팬티 8팩 기저귀', '3월 17일(화) : [블랑101] 1L세탁세제 2개+유연제 2개 택1 + 정품 사은품증정(품목 미정/본품으로 구성예정), [독일직구무료배송] 힙분유 Pre,1단계, 2단계, 2단계무전분, 3단계', '나이키 정기세일 UP TO 44% 신상품까지 할인! 쿠폰 더블혜택', 'SSG 창립4주년 한정! LG전자 라이프스타일 쇼핑 대축제 올레드TV, 오브제냉장고, 휘센에어컨, 그램PC 등 BEST상품 할인혜택', '내셔널지오그래픽 23SS 신상 오픈 적립 혜택! 이월 가격인하 + 추가 쿠폰 혜택까지', '쇼핑의 마무리 카드 청구 할인', '[SSGPAY전용]삼성카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 10% 청구할인 (일 5만원 한)', '[SSGPAY전용] 신한카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]KB카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]SSG.COM 삼성카드 8만원 이상 8% 청구할인 (일 5만원 한)', '[SSGPAY전용]비씨카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]신한카드 8만원 이상 5% 청구할인 (일 5만원 한)', '해피라운지 매일 오전 9시! 핫딜의 신세계']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일 매일 오전 10시, 한정수량 타임딜!</t>
+          <t>SSG 창립 4주년 장보기 혜택</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>쓱세일 봄 스타일링 추천템</t>
+          <t>최대 50% 할인부터 S머니 5천원 페이백!</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004555</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004812</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>패션명품 쓱세일</t>
+          <t>SSG.COM 창립 4주년 기념 장보기</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 패션명품 쓱세일', '스마일클럽', '#혜택 01 매일 오전 10시 초특가 타임딜 바로보기', '한정수량 타임딜', '타임딜은 오전 10시에 시작됩니다!', '오늘의 타임딜이 종료되었습니다.', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '3/6(월) 오후 7시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/7(화) 오후 7시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 8시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/7(화) 오후 9시, 라이브 동안만 신상품 30%, 이월상품 25~30% 할인, 구매 사은품 증정까지', '3/8(수) 오후 8시, SSG 단독 발매! 우븐트랙자켓 2종 S머니 추가혜택+이월상품 최대할인 전 구매고객 대상 사은품 까지', '3/10(금) 오후 6시, 데카브&amp;CC콜렉트 봄 아우터 한정수량 특 무료배송/무료반품 &amp; 추첨 사은품 증정']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM 창립 4주년 기념 장보기', '스마일클럽', '최대 50% 할인', '단 하루 PLUS+ 혜택! 쓱배송데이! 종료까지', '미슐랭 2스타 셰프가 만든 케이크 50% 할인', '정식당으로 유명한 임정식 셰프가 운영중인 정식카페가 만든 케이크 50% 할인 받아보세요!', '장보기 특가 최대 50% 할인', '50% 할인', '대상 상품 : 쓱배송, 새벽배송 상품', '적립금 : SSG MONEY 5,000원 적립금 (30일내 사용가능)', '본 행사는 쓱배송 및 새벽배송 상품 10만원 이상 구매 시 응모 가능합니다. (트레이더스 상품 제외 / 기간 중 1회 기준이며 구매 금액 합산되지 않습니다)', '이벤트페이지에서 &lt;응모하기&gt;버튼을 눌러 신청하신 고객에 한해 해당 ID로 적립됩니다.', '쓱배송 만원 할인에 무료배송', '장바구니 쿠폰 10,000원 - 첫 구매 전용', '쓱배송/새벽배송 무료배송 - 첫 구매 전용', '쓱배송/새벽배송 2만원 이상 구매 시 사용 가능', '첫 구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '첫 구매 쿠폰 모두 받으러 가기', 'SSG 창립 4주년 장보기 최대 50% 할인 오반장 위크']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>패션 명품 쓱세일  라이브 커머스 혜택</t>
+          <t>디즈니와 함께하는 SSG.COM 4주년 생일파티</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>쓱세일 기간 동안 라이브 보고  경품 받기</t>
+          <t>4가지의 놀라운 혜택</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004593</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004821</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[패션명품 쓱세일] SSG.LIVE 라이브 구매 이벤트 + 라이브 캘린더 까지</t>
+          <t>디즈니와 함께하는 SSG 4주년 생일파티</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [패션명품 쓱세일] SSG.LIVE 라이브 구매 이벤트 + 라이브 캘린더 까지', '스마일클럽', '[패션명품 쓱세일] SSG.LIVE 라이브 구매 이벤트 + 라이브 캘린더 까지', '[쓱라이브 이벤트 주의사항]', '-\xa0패션쓱\xa0SSG.LIVE\xa0에서 패션쓱\xa0SSG.LIVE\xa0제품 구매시\xa0이벤트 응모한 것으로 간주됩니다.', '-\xa0이벤트는 모두 주문번호\xa01개 기준 집계 및 증정됩니다.', '-\xa0구매 취소시 이벤트 당첨은 모두 취소됩니다.', '-\xa0이벤트에 응모하시는 경우,\xa0아래 개인정보 제공에 동의하신 것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다.', '-\xa0사은품 지급 및 이벤트 혜택 제공', '-\xa0사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기', '6.\xa0본 이벤트 경품은 브랜드사 상황에 따라 사전 고지 없이 변경,\xa0대체 될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 디즈니와 함께하는 SSG 4주년 생일파티', '스마일클럽', '추가 사은 이벤트 바로보기', '아이콘 클릭하여 친구들에게 공유하고 자동으로 이벤트 응모하기', ' 참여 방법 : 행사 기간 내 SSG.COM 로그인 후 인스타그램 또는 카카오톡 아이콘 클릭하여 이벤트 공유', '디즈니 브랜드관 구매 고객 추가 사은 이벤트']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>첫구매는 반값다딜 &lt;풀무원 편&gt;</t>
+          <t>오반장위크</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>풀무원 상품 4개 골라 최대 2만원 할인 + 무료배송</t>
+          <t>SSG 창립 4주년 장보기 최대 50%할인</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004661&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004791</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>반값다딜 - 풀무원 편 (3/2~12)</t>
+          <t>(3/13~19)  오반장위크_SSG창립 4주년 기념</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다딜 - 풀무원 편 (3/2~12)', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'Pulmuone 상품쿠폰 50% 4장, 개별 쿠폰 당 최대 5천원 할인', 'Pulmuone 상품쿠폰 무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '       쿠폰 발급 기간', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 2023년 3월 2일(목)~ 2023년 3월 12일 (일)', '       쿠폰 사용 조건', '-무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '(50%, 무료배송) [풀무원] 얇은피 꽉찬속 김치만두 400gx2 할인전 : 9,480원 할인후 : 4,740원', '(50%, 무료배송) [풀무원] 국산콩 투컵 두부 600g 할인전 : 5,480원 할인후 : 2,740원', '(50%, 무료배송) [풀무원] 바릴라 캠핑 기획팩 2,700G 할인전 : 29,800원 할인후 : 24,800원', '(50%, 무료배송) [풀무원] 새콤달콤 유부초밥 330g 할인전 : 5,680원 할인후 : 2,840원', '(50%, 무료배송) [풀무원] 행복한 동물복지유정란 15구 780g : 8,980원 할인후 : 4,490원', '할인 상품 한 눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; (3/13~19)  오반장위크_SSG창립 4주년 기념', '스마일클럽', 'SSG 창립 4주년 장보기 최대 50%할인', '매일 오전 9시, 최대 50%할인 오반장 PICK 오반장템 바로보기', '매일 오전 9시, 최대 50% 할인 놓치지 마세요!', '초콜릿/캔디/카라멜/젤리 브랜드별 최대 1+1, 54%할인', '한우바로구이 3종, 파머스픽 참외 1.2kg 최대 50%할인', '오반장상품으로 쓱배송/새벽배송 10만원 이상 장보고 SSG MONEY 5천원 페이백! SSG 창립 4주년 감사대축제 THANKS 4U!']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 ? 봄 맞이전</t>
+          <t>만원 할인에 무료배송</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>창립 기념 쓱배송 첫 구매 혜택</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004679</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004699</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(3/9~15) 2023 대한민국 수산대전 - 봄 맞이전</t>
+          <t>쓱배송 첫 구매 만원 할인</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-03-15</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/9~15) 2023 대한민국 수산대전 - 봄 맞이전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 쓱배송 첫 구매 만원 할인', '스마일클럽', '쓱배송 첫 구매 만원 할인', '최근 1년간 쓱배송이 처음이라면', '쓱배송 만원 할인에 무료배송', '10,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '쓱배송/새벽배송 2만원 이상 구매 시 사용 가능', '첫 구매 쿠폰 모두 받기', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 최근 1년 간 쓱배송 및 새벽배송 구매 이력이 없는 고객', '사용 조건 : 쓱배송 및 새벽배송 상품 2만원 이상 구매 시 사용 가능 ', '적용 대상 : 쓱배송 및 새벽배송 상품 한정 (일부 상품 제외)', '쓱배송 인기 아이템 추천', '믿고 사는 쓱배송 TOP RANKING', '쓱배송 라이프 즐기는 법']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>러블리 화이트데이</t>
+          <t>2023 대한민국 수산대전 봄 맞이전</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>장바구니 10% 쿠폰+ 달콤한 사랑을 전하세요</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004520</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004679</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>러블리 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!</t>
+          <t>(3/9~15) 2023 대한민국 수산대전 - 봄 맞이전</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-15</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 러블리 화이트데이 - 달콤한 사랑을 마음 가득 담아 전하세요!', '스마일클럽', '화이트데이 10% 쿠폰 받고 쇼핑 GO! 바로보기', '#10% 장바구니 쿠폰', '사탕만큼 달콤한 10% 할인 쿠폰 바로보기', '10% 장바구니 할인 쿠폰', '10% 결제쿠폰 (매일 오전 9시 / 선착순 1만명) - 15만원 이상 구매시 최대 1.5만원 할인', '      쿠폰 발급 기간', '      23/03/06(월) ~ 23/03/12(일), 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '      쿠폰 사용 조건', '+PLUS 카드 청구할인 혜택도 챙겨가세요!', '구호사계절 프리미엄 버킷백, 구호 SSG 단독특가 최대 15%', '프라다 外화이트데이 BEST 명품/잡화 프라다/키플링/빅토리아/스톤헨지 外 인기브랜드 ~ 70% 특가!', '스와로브스키스와로브스키 주얼리 기프트 추천 크리스탈처럼 반짝이는 주얼리 일부 품목 20%']</t>
+          <t>['이벤트/쿠폰 &gt; (3/9~15) 2023 대한민국 수산대전 - 봄 맞이전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SSG 스포츠페어</t>
+          <t>브랜드 스포트라이트 X 트라이온: 마리끌레르</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>매일 오전 9시 선착순 10%쿠폰</t>
+          <t>최대 52% 할인부터 사은품 및 특별 라이브까지!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004731</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004860</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG 스포츠페어</t>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 스포츠페어', '스마일클럽', '10% 할인쿠폰', '할인의 완성', '매일 오전 9시 선착순 1만명', '스포츠페어 10% 상품쿠폰', '상품쿠폰 10% (매일 오전 9시) (선착순 1만명)', '쿠폰은 매일 오전 9시 발급됩니다.', "발급 후 'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '23SS UP TO 44%', '최대 20% 할인혜택', '쿠폰할인 대전', '31% OFF', '23SS NEW ARRIVAL 자켓/맨투맨/하의 최대 ~10% OFF', '23SS NEW 스쿨룩 UPTO~20%★', '풋웨어 BEST 에어맥스97/데이브레이크 ~44%', '[나이키코리아공식] 남여 인기 신발 모음 ~45%', '조던/런닝/트레이닝룩 ~44% SALE!', 'CLEARENCE 기획전 ~70% OFF + 15% 쿠폰', '23 SPRING 점퍼/티셔츠/니트 외 30%OFF 50종 택1', '티셔츠/팬츠/스커트 등 신상~이월 최대50%', 'F/W 최대 40% 할인 특집', '[빈폴골프] 남녀 BEST 50 라운딩웨어☆ + SSG 특별 혜택★ + 최대할인쿠폰★', '골프존커머스 BEST 클럽/용품 모음전! 23년 신상부터 이월상품 최대할인까지', '인도어화 할인전']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르', '스마일클럽', '오피스룩 맞춤형 셔츠 스타일 뒷면 요크라인을 따라 일정한 간격의 플리츠 주름을 블록하여 포인트를 주며 면 100% 소재로 쾌적한 착용감 여유있는 사이즈로 체형 커버에 용이합니다.', '       행사기간 마리끌레르 전 상품, 최대 52% 할인', '       행사상품 20만원 이상 구매 시, 볼캡 선착순 50명 증정', '       ※ 이벤트 페이지 상단에 모델 촬영한 8개 상품만 해당됩니다.', '       ※ 할인액을 제외한 최종 결제금액 기준입니다.', '       ※ 3/15 (수) SSG.LIVE 방송 볼캡 선착순 100개 증정과는 별개의 이벤트로 라이브 방송 시간 외 구매한 건을 대상으로 합니다.', '       라이브 방송 1분 시청 시, 10% 시청쿠폰 발급', '       ※ 시청쿠폰은 당일 자정까지만 사용 가능합니다.', '       마리끌레르 2개 상품 한정수량 핫딜', '       라이브 방송 한정 20만원 이상 구매 시, 볼캡 선착순 100명 증정', '       ※ 브랜드 스포트라이트 혜택인 볼캡 50개 선착순 증정과는 별개의 이벤트입니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>생필품 특가 위크 10% 선착순 할인 쿠폰</t>
+          <t>3월 로맨틱 다이닝 도전 홈스토랑 파스타</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>화장지부터 세제까지 우리집 필수템 알뜰 쇼핑</t>
+          <t>소스 1+1 구성부터 SSG머니 이벤트 행운까지!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004597</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004777</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>생필품 특가 위크</t>
+          <t>집 밥 챌린지 - 파스타편</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-15</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 생필품 특가 위크', '스마일클럽', '10% 할인 쿠폰', '금주의 할인 특가', '      쿠폰 적용 대상', '매일 9시 3만명 선착순 상품쿠폰 10% SSG.COM', '2만원 이상 구매 시 최대 1만원 할인', '금일 쿠폰은 모두 소진 되었습니다.', '쿠폰은 매일 오전 9시 발급됩니다', '       쿠폰 발급 및 사용기간', "       쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '       쿠폰은 SSG.COM 회원만 다운 가능하며(간편가입 포함), 비회원 주문시 쿠폰은 적용할 수 없습니다.', '♥[모나리자] 생필품 ~20% 할인♥ 휴지/키친타올/미용티슈/물티슈/각티슈/마스크', '오슬림밴드/에어팬츠 기저귀 ~2개50%(맘키즈회원전용)', '★브랜드할인★ 센트라린 캡슐세탁세제 모음전(아로퓸/카포드/엘에이/향기부스터)', '[★40% SALE★]애경 3월 봄이 왔나봄 할인+쿠폰+다다익선+증정', '[쓱배송]때가 쏙 비트 세탁세제&amp;참그린 주방세제 최대 1+1 모음전', '[쓱배송]피죤 생필품 1+1 특가전', '엘경유켈. 세제 4대 브랜드 대통합 할인', '[웰라] 프리미엄 살롱 헤어케어 최대 70% off / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '[쓱배송] 3배 빨라진 새치샴푸 런칭 특가전★(함께살수록 할인)', '★천만개 판매돌파★ 지아자/크나이프 SSG 단독할인', '최대~36%할인 +구매별 60ml 증정 혜택', '★단독구성+10%쿠폰★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '★생필품 특가 위크★바디케어 1+1/2개이상10% 모음', '세타필 바디로션, 크림  할인 행사', '★단독사은품+최대46%할인가★ 리스테린 쿨민트/그린티 외 250ml&amp;750ml 모음전', '[서인국마스크][5%다운쿠폰]38년 필터 기업이 만든 귀가 편한 시노텍스 마스크', '1+1 / 다다익선 할인 혜택', '세제/헤어/바디 ~40% 할인+적립', '~30% OFF + 다다익선  + 증정품', '인기 제품&amp;기획SET 최대 ~30% OFF', '★배송비특가★헤어플러스 브랜드 위크+할인쿠폰+사은품까지!', '★SSG단독 특가★  살롱클리닉 새치 ALL 커버 셀프 염색약 전 상품 특가 (할인+쿠폰+15%추가 쿠폰+증정품까지)', '기획전★ 구매왕+다다익선 10%+구매사은품', '도브 바디로션 런칭기념행사 [최대~50%할인]']</t>
+          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 파스타편', '스마일클럽', '이번 주는 특별하게, 파스타로 홈스토랑 셰프가 되어보세요. 소스 최대 1+1부터, 샐러드/파스타/스테이크 할인 취향 투표하면 SSG머니 행운이!', '최대 1+1 할인 파스타 소스 추천 상품', "        당첨자 발표 일정: 2023년 3월 20일 발표 예정 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요’", '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '올리브오일 최대 40% 할인 - 다양한 요리유의 세계 확인하기', '해산물/채소 할인']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SPRING IS COMING</t>
+          <t>먼데이문 SPRING WEEK</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>다가오는 봄, 나에게 주는 선물부터 달콤한 봄 GIFT까지!</t>
+          <t>봄맞이 취향맞춤 메이크업은 SSG에서!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004736</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004862</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SPRING IS COMING</t>
+          <t>먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -836,103 +836,103 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SPRING IS COMING', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어', '스마일클럽', '~10% 쿠폰', '뷰티 10%쿠폰 ~5천원 할인', '- Thanks 4 U 쿠폰과 동일 -', '[클리오/페리페라 外] 3월 뷰티위크 UP TO 50%/1+1/사은혜택까지', '다운타우너 콜라보 스페셜 특가 최대40% 글로우픽수상', '베스트 무료배송 (블러워터틴트,멀티아이팔레트,페이스블러쉬,소프트매트립,뉴테이크 외)', '단독 기획, 최대 30% OFF', 'UP TO ~50% + 스팟 패치 증정', '스크래치 쿠폰받고 에어팟 맥스 GET!', '한정수량 체험특가 + ~60% OFF', '최대 39% 세일 + 퍼프/틴트 外', '갈색병 세럼 할인+사은품', 'BEST ~39% 할인+상품권', 'UP TO 40% / 메이크업은 키스미!', '[닥터지] 스프링 SUN 페스타 BEST&amp;NEW 1+1 ~89%할인/구매사은품혜택♥', '[아떼] 7일만! 어센틱 립밤 SSG 단독 특가 / 선&amp;비비 한정수량 50%OFF + BEST 제안', '셀퓨전씨 봄볕 자외선 밀착 차단! + 구금사 + 무료배송!', 'SSG 3월 기획전 최대 51%할인', '화이트데이 기프트 특가 및 적립행사 ~50%/구매금액별 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', '고현정의 피부 비결, 코이 인기상품모음 ~20%OFF', '[AHC] SSG 단독 구성 &amp; BEST 스킨/선케어 ~62%OFF + 사은품 증정', '봄맞이 최대 75% 세일! 룸스프레이/핸드/바디/구강 모음전 + 사은품 증정', '[UP TO 60%] 바이탈뷰티 특집전!']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 코치</t>
+          <t>최대 7.2만원 혜택</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SSG단독 10% 할인 + 구매 사은품 증정</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004624</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 코치</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 코치', '스마일클럽', '상위 20%의 엄선된 고품질 가죽으로 제작된 코치만의 가죽 지갑 최소한의 가공으로 원가죽 무늬와 느낌을 살린 똑같은 가죽이 아닌 하나 뿐인 고유한 상품', '      01 SSG 단독 브랜드 스포트라이트 기간 중 10% 할인 혜택']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3월 로맨틱 다이닝 도전 홈스토랑 파스타</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>소스 1+1 구성부터 SSG머니 이벤트 행운까지!</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004777</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>집 밥 챌린지 - 파스타편</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-03-15</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 파스타편', '스마일클럽', '이번 주는 특별하게, 파스타로 홈스토랑 셰프가 되어보세요. 소스 최대 1+1부터, 샐러드/파스타/스테이크 할인 취향 투표하면 SSG머니 행운이!', '최대 1+1 할인 파스타 소스 추천 상품', "        당첨자 발표 일정: 2023년 3월 20일 발표 예정 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요’", '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '올리브오일 최대 40% 할인 - 다양한 요리유의 세계 확인하기', '해산물/채소 할인']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '최대 3% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>W컨셉 SPRING SHOP#</t>
+          <t>스토케  3/13(월) 11AM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>모한, 르니나 外 봄 아이템 추천 + 15% 쿠폰 혜택</t>
+          <t>스토케 구매시 SSG머니 적립 페이백&amp;구매사은품 증정 단독 라이브</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004587</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004775&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>W컨셉 SPRING SHOP#</t>
+          <t>휴대용 유모차 스토케 YOYO @SSG.LIVE 3/13(월) 11AM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -942,34 +942,34 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; W컨셉 SPRING SHOP#', '스마일클럽', 'SPECIAL OFFER 15% 쿠폰 바로보기', 'SPECIAL OFFER 15% 상품 쿠폰', '15% 상품쿠폰 - 2만원 이상 구매시 최대 2만원 할인', '         쿠폰 발급 및 사용 기간', '         2만원 이상 상품 구매 시 15% 할인, 최대 2만원 (기간내 ID당 발급수량 2장)', '         쿠폰 적용 방법', '쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '상품 상세에서 이미 쿠폰을 다운 받으신 경우 행사 페이지에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에도 상품 상세에서 쿠폰을 다운받으실 수 없습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 휴대용 유모차 스토케 YOYO @SSG.LIVE 3/13(월) 11AM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기', '6. 본 이벤트 경품은 브랜드사 상황에 따라 사전 고지 없이 변경, 대체 될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>민지의 장바구니-화이트데이편</t>
+          <t>헤라 3/13(월) 7PM</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>디저트 레시피 영상보고 댓글 달면 SSG머니 추첨 증정</t>
+          <t>이사배X헤라 실키 파운데이션 시연 라이브! 전구매고객 사은품 外 브랜드 연중 최대 혜택</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004754&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004813&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>민지의 장바구니-화이트데이편 (3/6~3/12)</t>
+          <t>[SSG.LIVE]3/13(월)헤라</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -979,232 +979,158 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-03-12</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 민지의 장바구니-화이트데이편 (3/6~3/12)', '스마일클럽', '       My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요', '       ID당 이벤트 기간 내 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '       이벤트 성격과 다른 내용이거나 불쾌감을 줄 수 있는 댓글은 사전 고지 없이 삭제될 수 있습니다.', '쓱배송 8만원 이상 구매시, 응모필수! 오늘 단 하루, SSG머니 5천원 100% 페이백']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/13(월)헤라', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>최대 7.2만원 혜택</t>
+          <t>오키나와 여행(모두투어) 3/13(월) 8PM</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>오키나와 힐링 패키지 [비치리조트 오션뷰UP+3대특식+핵심관광] VS 가성비 자유여행 4일</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004801&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>오키나와 여행(모두투어) @SSG.LIVE 3/13(월) 8PM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-03-03</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; 오키나와 여행(모두투어) @SSG.LIVE 3/13(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>다이슨 3/14(화) 7PM</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>499천원+5%할인+2만5천원 적립!(방송시)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004835&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>다이슨@SSG.LIVE 3/14(화) 7:00PM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-03-07</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-03-17</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 3/14(화) 7:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[공동판매구역] 세이펜 3/9(목) 11AM</t>
+          <t>[월간호캉쓱] 롯데리조트 속초, 부여 3/14(화) 8PM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>우리아이 교육 필수품 역대급 혜택LIVE!</t>
+          <t>선착순 최대 76% 핫딜가+ 캐릭터룸 최초 공개</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004755&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004766&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]3/9(목) 세이펜</t>
+          <t>롯데리조트 속초, 부여 @SSG.LIVE 3/4(화) 8PM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-02-28</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2023-03-17</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/9(목) 세이펜', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 롯데리조트 속초, 부여 @SSG.LIVE 3/4(화) 8PM', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>명품대전 3/9(목) 8PM</t>
+          <t>3월 맘키즈 플러스</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>프라다/보테가베네타/오트리/메종키츠네/멀버리/발렌티노/아미 외~</t>
+          <t>지금 할인 중! ~40% 할인 혜택</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004598&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>명품대전 @SSG.LIVE 3/9(목) 8PM</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2999-12-13</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 명품대전 @SSG.LIVE 3/9(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>데카브&amp;CC콜렉트 3/10(금) 6PM</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[패션명품 쓱세일] 데카브&amp;CC콜렉트 2023년 신상&amp;이월 최대 81% 할인</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004600&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>[패션명품 쓱세일] 데카브&amp;CC콜렉트 @SSG.LIVE 3/10(금) 6PM</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2023-02-27</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2023-03-10</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [패션명품 쓱세일] 데카브&amp;CC콜렉트 @SSG.LIVE 3/10(금) 6PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>3월 맘키즈 플러스</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~40% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '시크릿쥬쥬 베스트프렌즈마고 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈스쿨백세트 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈리나 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈쥬쥬 (N2쓱배송, 전국택배)', '베스트프렌즈시크릿프렌즈폰 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈미니사물함 (N2쓱배송, 전국택배)', '★금주의 할인딜★ KIDS 침구 / 어린이집 낮잠이불']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Mar 16 00:21:56 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,27 +483,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004809</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004810</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3/13  창립 기념 쓱배송데이</t>
+          <t>3/16  창립 4주년 감사 대축제 쓱배송데이</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-16</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-16</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 3/13  창립 기념 쓱배송데이', '스마일클럽', '3/13  창립 기념 쓱배송데이', 'SSG 창립 4주년 감사대축제 쓱배송데이', '10% 쿠폰 + 5천원 적립 + 카드혜택', '쓱배송 DAY 남은 시간', '10% 쿠폰 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오전 쿠폰', '      이마트, 트레이더스 쓱배송 및 점포택배 / 새벽배송', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만원 할인 오전 또는 오후 쿠폰 ID당 1일 1매 다운(오전 9시 오픈, 선착순 2만명)', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오후 쿠폰', '      쿠폰 발급 및 사용일', '      23년 3월 13일(오전 또는 오후 쿠폰 ID당 1일 1매 다운)(발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', '[SSGPAY전용] 삼성카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] KB국민카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 8만원이상 8% 청구할인 (일 5만원 한) 자세히보기', '인기상품 1+1, 최대 50% 할인 쓱배송데이 장보기 특가상품', '오늘 원하는 시간에 받고 싶다면, 이마트몰 쓱배송 추천상품', '대용량 쟁여두기가 필요할 땐, 트레이더스 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; 3/16  창립 4주년 감사 대축제 쓱배송데이', '스마일클럽', '3/16  창립 4주년 감사 대축제 쓱배송데이', 'SSG 창립 4주년 감사대축제 쓱배송데이', '10% 쿠폰 + 5천원 적립 + 카드혜택', '쓱배송 DAY 남은 시간', '10% 쿠폰 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오전 쿠폰', '      이마트, 트레이더스 쓱배송 및 점포택배 / 새벽배송', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만원 할인 오전 또는 오후 쿠폰 ID당 1일 1매 다운(오전 9시 오픈, 선착순 2만명)', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오후 쿠폰', '      쿠폰 발급 및 사용일', '      23년 3월 16일(오전 또는 오후 쿠폰 ID당 1일 1매 다운)(발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', '[SSGPAY전용] 삼성카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] KB국민카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 8만원이상 8% 청구할인 (일 5만원 한) 자세히보기', '인기상품 1+1, 최대 50% 할인 쓱배송데이 장보기 특가상품', '오늘 원하는 시간에 받고 싶다면, 이마트몰 쓱배송 추천상품']</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; SSG 창립 4주년 감사대축제 'Thanks 4 U'", '스마일클럽', '누구나 10% 할인 쿠폰 6매 / 최대 2만 5천원 할인', '6종 쿠폰 바로보기', '선착순 타임딜 바로보기', '한 시간 한정 최대 3만원 장바구니 쿠폰 발급 중!', '지금 바로! 장바구니 게릴라 쿠폰 놓치지 말고 받아가세요!', '장바구니 쿠폰 10% 8만원 이상 구매시 최대 3만원 할인', '※ 타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '딱 한시간만! 최대 3만원 장바구니 쿠폰 발급 중!', '쿠폰 발급 시간 : 2023년 3월 13일(월) 10시 00분 부터 3월 13일(월) 10시 59분 까지', '쿠폰 발급 시간 : 2023년 3월 15일(수) 10시 00분 부터 3월 15일(수) 10시 59분 까지', '타 사이트를 통해 방문하신 고객의 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '10% 할인 쿠폰 6매 누구나 최대 2만 5천원 할인!', '상품쿠폰 10% X 6', '6종 쿠폰팩 한번에 다운 받기', '쿠폰 할인 대상 및 사용 안내(레이어팝업 열기)', '※ 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '쿠폰 이용안내', '할인 대상', '      10% 상품쿠폰 2매 (1만원 이상 상품 구매시 ~3천원 할인 / 4만원 이상 상품 구매시 ~5천원 할인)', '      10% 상품쿠폰 2매 (1만원 이상 상품 구매시 ~3천원 할인 / 7만원 이상 상품 구매시 ~8천원 할인)', '      10% 상품쿠폰 2매 (10만원 이상 상품 구매시 ~1만 5천원 할인, 20만원 이상 상품 구매시 ~2만 5천원 할인)', '쿠폰은 신세계몰, 신세계백화점몰 각 해당 카테고리에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '신세계몰&amp;신세계백화점몰 첫구매 고객님이신가요\xa0', '첫구매 응원 최대 12% 장바구니 쿠폰', '매일 오전 07시 선착순 1만장 장바구니 쿠폰 12% 8민원 이상 구매시 최대 2만원 할인', '신세계백화점몰 및 신세계몰 첫구매 고객 대상 으로 발급되는 쿠폰 입니다.', '타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '쿠폰 마감 되었습니다.', '쿠폰발급 대상 : 2022년 3월 12일 이후로 신세계몰, 신세계백화점몰 구매 이력이 없는 고객', '타사이트를 통해 방문하신 경우 결제시 장바구니 쿠폰이 적용되지 않습니다.', '매일 오전 10시! 선착순 타임딜', '망설이명 품절! 핫딜로 구매하세요', '타임딜 행사는 SSG 모바일로 확인해주세요', '       타임딜 진행시간', '타임딜 대표 상품 미리보기', '3월 15일(화) : ★타임딜★ [립프로그] 아이스크림카트 디럭스(한영버전) 핑크, [SSG][2박스]팸퍼스 베이비드라이 팬티 8팩 기저귀', '3월 17일(화) : [블랑101] 1L세탁세제 2개+유연제 2개 택1 + 정품 사은품증정(품목 미정/본품으로 구성예정), [독일직구무료배송] 힙분유 Pre,1단계, 2단계, 2단계무전분, 3단계', '나이키 정기세일 UP TO 44% 신상품까지 할인! 쿠폰 더블혜택', 'SSG 창립4주년 한정! LG전자 라이프스타일 쇼핑 대축제 올레드TV, 오브제냉장고, 휘센에어컨, 그램PC 등 BEST상품 할인혜택', '내셔널지오그래픽 23SS 신상 오픈 적립 혜택! 이월 가격인하 + 추가 쿠폰 혜택까지', '쇼핑의 마무리 카드 청구 할인', '[SSGPAY전용]삼성카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 10% 청구할인 (일 5만원 한)', '[SSGPAY전용] 신한카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]KB카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]SSG.COM 삼성카드 8만원 이상 8% 청구할인 (일 5만원 한)', '[SSGPAY전용]비씨카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]신한카드 8만원 이상 5% 청구할인 (일 5만원 한)', '해피라운지 매일 오전 9시! 핫딜의 신세계']</t>
+          <t>["이벤트/쿠폰 &gt; SSG 창립 4주년 감사대축제 'Thanks 4 U'", '스마일클럽', '누구나 10% 할인 쿠폰 6매 / 최대 2만 5천원 할인', '6종 쿠폰 바로보기', '선착순 타임딜 바로보기', '한 시간 한정 최대 3만원 장바구니 쿠폰 발급 중!', '지금 바로! 장바구니 게릴라 쿠폰 놓치지 말고 받아가세요!', '장바구니 쿠폰 10% 8만원 이상 구매시 최대 3만원 할인', '※ 타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '딱 한시간만! 최대 3만원 장바구니 쿠폰 발급 중!', '쿠폰 발급 시간 : 2023년 3월 13일(월) 10시 00분 부터 3월 13일(월) 10시 59분 까지', '쿠폰 발급 시간 : 2023년 3월 15일(수) 10시 00분 부터 3월 15일(수) 10시 59분 까지', '타 사이트를 통해 방문하신 고객의 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '10% 할인 쿠폰 6매 누구나 최대 2만 5천원 할인!', '상품쿠폰 10% X 6', '6종 쿠폰팩 한번에 다운 받기', '쿠폰 할인 대상 및 사용 안내(레이어팝업 열기)', '※ 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '쿠폰 이용안내', '할인 대상', '      10% 상품쿠폰 2매 1만원 이상 최대 3천원 1매, 4만원 이상 최대 5천원 1매', '      10% 상품쿠폰 2매 1만원 이상 최대 3천원 1매, 7만원 이상 최대 8천원 1매', '      10% 상품쿠폰 2매 10만원 이상 최대 1만 5천원 1매, 20만원 이상 최대 2만 5천원 1매', '쿠폰은 신세계몰, 신세계백화점몰 각 해당 카테고리에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '신세계몰&amp;신세계백화점몰 첫구매 고객님이신가요\xa0', '첫구매 응원 최대 12% 장바구니 쿠폰', '매일 오전 07시 선착순 1만장 장바구니 쿠폰 12% 8민원 이상 구매시 최대 2만원 할인', '신세계백화점몰 및 신세계몰 첫구매 고객 대상 으로 발급되는 쿠폰 입니다.', '타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '쿠폰 마감 되었습니다.', '쿠폰발급 대상 : 2022년 3월 12일 이후로 신세계몰, 신세계백화점몰 구매 이력이 없는 고객', '타사이트를 통해 방문하신 경우 결제시 장바구니 쿠폰이 적용되지 않습니다.', '매일 오전 10시! 선착순 타임딜', '망설이명 품절! 핫딜로 구매하세요', '타임딜 행사는 SSG 모바일로 확인해주세요', '       타임딜 진행시간', '타임딜 대표 상품 미리보기', '3월 15일(화) : ★타임딜★ [립프로그] 아이스크림카트 디럭스(한영버전) 핑크, [SSG][2박스]팸퍼스 베이비드라이 팬티 8팩 기저귀', '3월 17일(화) : [블랑101] 1L세탁세제 2개+유연제 2개 택1 + 정품 사은품증정(품목 미정/본품으로 구성예정), [독일직구무료배송] 힙분유 Pre,1단계, 2단계, 2단계무전분, 3단계', '나이키 정기세일 UP TO 50% 신상품까지 할인! 쿠폰 더블혜택', 'SSG 창립4주년 한정! LG전자 라이프스타일 쇼핑 대축제 올레드TV, 오브제냉장고, 휘센에어컨, 그램PC 등 BEST상품 할인혜택', '내셔널지오그래픽 23SS 신상 오픈 적립 혜택! 이월 가격인하 + 추가 쿠폰 혜택까지', '쇼핑의 마무리 카드 청구 할인', '[SSGPAY전용]삼성카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 10% 청구할인 (일 5만원 한)', '[SSGPAY전용] 신한카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]KB카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]SSG.COM 삼성카드 8만원 이상 8% 청구할인 (일 5만원 한)', '[SSGPAY전용]비씨카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]신한카드 8만원 이상 5% 청구할인 (일 5만원 한)', '해피라운지 매일 오전 9시! 핫딜의 신세계']</t>
         </is>
       </c>
     </row>
@@ -695,59 +695,59 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 봄 맞이전</t>
+          <t>브랜드 스포트라이트 X 트라이온: 마리끌레르</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>최대 52% 할인부터 사은품 및 특별 라이브까지!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004679</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004860</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>(3/9~15) 2023 대한민국 수산대전 - 봄 맞이전</t>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-03-15</t>
+          <t>2023-03-19</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/9~15) 2023 대한민국 수산대전 - 봄 맞이전', '스마일클럽', '20% 장바구니 쿠폰', '여러 개 담으시고 최대 1만원 할인 받으세요', '업체택배 상품 : 본 페이지 20% 장바구니 쿠폰 사용 가능 ID당 1매 발급, 최대 1만원 할인', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르', '스마일클럽', '오피스룩 맞춤형 셔츠 스타일 뒷면 요크라인을 따라 일정한 간격의 플리츠 주름을 블록하여 포인트를 주며 면 100% 소재로 쾌적한 착용감 여유있는 사이즈로 체형 커버에 용이합니다.', '       행사기간 마리끌레르 전 상품, 최대 52% 할인', '       행사상품 20만원 이상 구매 시, 볼캡 선착순 50명 증정', '       ※ 이벤트 페이지 상단에 모델 촬영한 8개 상품만 해당됩니다.', '       ※ 할인액을 제외한 최종 결제금액 기준입니다.', '       ※ 3/15 (수) SSG.LIVE 방송 볼캡 선착순 100개 증정과는 별개의 이벤트로 라이브 방송 시간 외 구매한 건을 대상으로 합니다.', '       라이브 방송 1분 시청 시, 10% 시청쿠폰 발급', '       ※ 시청쿠폰은 당일 자정까지만 사용 가능합니다.', '       마리끌레르 2개 상품 한정수량 핫딜', '       라이브 방송 한정 20만원 이상 구매 시, 볼캡 선착순 100명 증정', '       ※ 브랜드 스포트라이트 혜택인 볼캡 50개 선착순 증정과는 별개의 이벤트입니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: 마리끌레르</t>
+          <t>먼데이문 SPRING WEEK</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>최대 52% 할인부터 사은품 및 특별 라이브까지!</t>
+          <t>봄맞이 취향맞춤 메이크업은 SSG에서!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004860</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004862</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르</t>
+          <t>먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -762,377 +762,192 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르', '스마일클럽', '오피스룩 맞춤형 셔츠 스타일 뒷면 요크라인을 따라 일정한 간격의 플리츠 주름을 블록하여 포인트를 주며 면 100% 소재로 쾌적한 착용감 여유있는 사이즈로 체형 커버에 용이합니다.', '       행사기간 마리끌레르 전 상품, 최대 52% 할인', '       행사상품 20만원 이상 구매 시, 볼캡 선착순 50명 증정', '       ※ 이벤트 페이지 상단에 모델 촬영한 8개 상품만 해당됩니다.', '       ※ 할인액을 제외한 최종 결제금액 기준입니다.', '       ※ 3/15 (수) SSG.LIVE 방송 볼캡 선착순 100개 증정과는 별개의 이벤트로 라이브 방송 시간 외 구매한 건을 대상으로 합니다.', '       라이브 방송 1분 시청 시, 10% 시청쿠폰 발급', '       ※ 시청쿠폰은 당일 자정까지만 사용 가능합니다.', '       마리끌레르 2개 상품 한정수량 핫딜', '       라이브 방송 한정 20만원 이상 구매 시, 볼캡 선착순 100명 증정', '       ※ 브랜드 스포트라이트 혜택인 볼캡 50개 선착순 증정과는 별개의 이벤트입니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어', '스마일클럽', '~10% 쿠폰', '뷰티 10%쿠폰 ~5천원 할인', '- Thanks 4 U 쿠폰과 동일 -', 'BEST 아이섀도우 최대 15% OFF 및 추가 샘플 증정', '[클리오/페리페라 外] 3월 뷰티위크 UP TO 50%/1+1/사은혜택까지', '다운타우너 콜라보 스페셜 특가 최대40% 글로우픽수상', '베스트 무료배송 (블러워터틴트,멀티아이팔레트,페이스블러쉬,소프트매트립,뉴테이크 외)', '단독 기획, 최대 30% OFF', 'UP TO ~50% + 스팟 패치 증정', '스크래치 쿠폰받고 에어팟 맥스 GET!', '한정수량 체험특가 + ~60% OFF', '갈색병 세럼 할인+사은품', 'BEST ~39% 할인+상품권', '셀퓨전씨 봄볕 자외선 밀착 차단! 매일 18시 선착순 특가!', '[아떼] 7일만! 어센틱 립밤 SSG 단독 특가 / 선&amp;비비 한정수량 50%OFF + BEST 제안', '[닥터지] 스프링 SUN 페스타 BEST&amp;NEW 1+1 ~89%할인/구매사은품혜택♥', 'UP TO 40% / 메이크업은 키스미!', 'No.1더블세럼, 정품증정 이벤트', '[AHC] SSG 단독 구성 &amp; BEST 스킨/선케어 ~62%OFF + 사은품 증정', '고현정의 피부 비결, 코이 인기상품모음 ~20%OFF', '화이트데이 기프트 특가 및 적립행사 ~50%/구매금액별 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', 'SSG 3월 기획전 최대 51%할인', '[UP TO 60%] 바이탈뷰티 특집전!', '봄맞이 최대 75% 세일! 룸스프레이/핸드/바디/구강 모음전 + 사은품 증정']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3월 로맨틱 다이닝 도전 홈스토랑 파스타</t>
+          <t>최대 10.2만원 혜택</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>소스 1+1 구성부터 SSG머니 이벤트 행운까지!</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004777</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>집 밥 챌린지 - 파스타편</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-03-15</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 파스타편', '스마일클럽', '이번 주는 특별하게, 파스타로 홈스토랑 셰프가 되어보세요. 소스 최대 1+1부터, 샐러드/파스타/스테이크 할인 취향 투표하면 SSG머니 행운이!', '최대 1+1 할인 파스타 소스 추천 상품', "        당첨자 발표 일정: 2023년 3월 20일 발표 예정 'My SSG &gt; 이벤트 현황 &gt; 이벤트 참여내역에서 확인해주세요’", '        ID당 이벤트 기간 내 1일 1회 응모 가능하며, 당첨은 기간 내 ID 당 1회만 가능합니다.', '올리브오일 최대 40% 할인 - 다양한 요리유의 세계 확인하기', '해산물/채소 할인']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>봄맞이 취향맞춤 메이크업은 SSG에서!</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004862</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어', '스마일클럽', '~10% 쿠폰', '뷰티 10%쿠폰 ~5천원 할인', '- Thanks 4 U 쿠폰과 동일 -', '[클리오/페리페라 外] 3월 뷰티위크 UP TO 50%/1+1/사은혜택까지', '다운타우너 콜라보 스페셜 특가 최대40% 글로우픽수상', '베스트 무료배송 (블러워터틴트,멀티아이팔레트,페이스블러쉬,소프트매트립,뉴테이크 외)', '단독 기획, 최대 30% OFF', 'UP TO ~50% + 스팟 패치 증정', '스크래치 쿠폰받고 에어팟 맥스 GET!', '한정수량 체험특가 + ~60% OFF', '최대 39% 세일 + 퍼프/틴트 外', '갈색병 세럼 할인+사은품', 'BEST ~39% 할인+상품권', 'UP TO 40% / 메이크업은 키스미!', '[닥터지] 스프링 SUN 페스타 BEST&amp;NEW 1+1 ~89%할인/구매사은품혜택♥', '[아떼] 7일만! 어센틱 립밤 SSG 단독 특가 / 선&amp;비비 한정수량 50%OFF + BEST 제안', '셀퓨전씨 봄볕 자외선 밀착 차단! + 구금사 + 무료배송!', 'SSG 3월 기획전 최대 51%할인', '화이트데이 기프트 특가 및 적립행사 ~50%/구매금액별 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', '고현정의 피부 비결, 코이 인기상품모음 ~20%OFF', '[AHC] SSG 단독 구성 &amp; BEST 스킨/선케어 ~62%OFF + 사은품 증정', '봄맞이 최대 75% 세일! 룸스프레이/핸드/바디/구강 모음전 + 사은품 증정', '[UP TO 60%] 바이탈뷰티 특집전!']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '최대 2% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '      이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '      카드혜택 + 스마일클럽 혜택', '      이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>최대 7.2만원 혜택</t>
+          <t>SSG푸드마켓 3/16(목) 11AM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>고당도 오렌지, 성주 참외 선착순 1,000개 9,900원 핫딜</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004834&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG푸드마켓 @SSG.LIVE 3/16(목) 11:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-03-08</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-03-16</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 7.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 *단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시 실물카드 수령 후 결제 가능', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG푸드마켓 @SSG.LIVE 3/16(목) 11:00', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>프리메라 3/16(목) 7PM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>프리메라 BEST 최대 39% 할인! PRMR 비타티놀 세럼 구매시, 상품권 증정!</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004882&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>프리메라 @SSG.LIVE 3/16(목) 7PM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-03-08</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-03-16</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 3% 즉시할인', '최대 3% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 프리메라 @SSG.LIVE 3/16(목) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>스토케  3/13(월) 11AM</t>
+          <t>일룸 쿠시노 3/16(목) 20PM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>스토케 구매시 SSG머니 적립 페이백&amp;구매사은품 증정 단독 라이브</t>
+          <t>침대/패드 최대 30%할인 +저상형 침대 3종 핫딜 75만원~ 디즈니 안전거울 증정</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004775&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004837&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>휴대용 유모차 스토케 YOYO @SSG.LIVE 3/13(월) 11AM</t>
+          <t>일룸 쿠시노@SSG.LIVE 3/16(목) 20:00PM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-07</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-17</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 휴대용 유모차 스토케 YOYO @SSG.LIVE 3/13(월) 11AM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기', '6. 본 이벤트 경품은 브랜드사 상황에 따라 사전 고지 없이 변경, 대체 될 수 있습니다.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>헤라 3/13(월) 7PM</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>이사배X헤라 실키 파운데이션 시연 라이브! 전구매고객 사은품 外 브랜드 연중 최대 혜택</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004813&amp;domainSiteNo=6005</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]3/13(월)헤라</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2023-03-06</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-03-13</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/13(월)헤라', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>오키나와 여행(모두투어) 3/13(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>오키나와 힐링 패키지 [비치리조트 오션뷰UP+3대특식+핵심관광] VS 가성비 자유여행 4일</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004801&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>오키나와 여행(모두투어) @SSG.LIVE 3/13(월) 8PM</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2023-03-03</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-03-13</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 오키나와 여행(모두투어) @SSG.LIVE 3/13(월) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>다이슨 3/14(화) 7PM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>499천원+5%할인+2만5천원 적립!(방송시)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004835&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>다이슨@SSG.LIVE 3/14(화) 7:00PM</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2023-03-07</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2023-03-17</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 3/14(화) 7:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>[월간호캉쓱] 롯데리조트 속초, 부여 3/14(화) 8PM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>선착순 최대 76% 핫딜가+ 캐릭터룸 최초 공개</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004766&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>롯데리조트 속초, 부여 @SSG.LIVE 3/4(화) 8PM</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2023-02-28</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2023-03-17</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 롯데리조트 속초, 부여 @SSG.LIVE 3/4(화) 8PM', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>3월 맘키즈 플러스</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>지금 할인 중! ~40% 할인 혜택</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>이달의 맘키즈 PLUS</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2999-12-13</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '맘키즈 에누리 쿠폰', '행사대상 상품별 최대 40% 할인', '맘키즈 상품 에누리 쿠폰', '맘키즈 클럽 회원이라면 로그인 후 각 상품 상세페이지에서도 쿠폰을 받으실 수 있습니다.', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리 쿠폰 ~40%', '5無키즈 100% 유기농 망고오렌지 500ml (100mlx5포)', '5無 100% 국산 배도라지즙 400ml (100mlx4)', '시크릿쥬쥬 베스트프렌즈마고 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈스쿨백세트 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈리나 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈쥬쥬 (N2쓱배송, 전국택배)', '베스트프렌즈시크릿프렌즈폰 (N2쓱배송, 전국택배)', '시크릿쥬쥬 베스트프렌즈미니사물함 (N2쓱배송, 전국택배)', '★금주의 할인딜★ KIDS 침구 / 어린이집 낮잠이불']</t>
+          <t>['이벤트/쿠폰 &gt; 일룸 쿠시노@SSG.LIVE 3/16(목) 20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Mar 20 00:21:46 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,296 +473,296 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SSG 창립 4주년 쓱배송데이</t>
+          <t xml:space="preserve">첫구매는 반값다딜 </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>하루 두 번 10% 선착순 쿠폰 + 카드 할인</t>
+          <t>다우니, 페브리즈 등 인기브랜드 최대 2만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004810</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004966&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3/16  창립 4주년 감사 대축제 쓱배송데이</t>
+          <t>반값다~딜 - P&amp;G편</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-16</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-16</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 3/16  창립 4주년 감사 대축제 쓱배송데이', '스마일클럽', '3/16  창립 4주년 감사 대축제 쓱배송데이', 'SSG 창립 4주년 감사대축제 쓱배송데이', '10% 쿠폰 + 5천원 적립 + 카드혜택', '쓱배송 DAY 남은 시간', '10% 쿠폰 바로보기', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오전 쿠폰', '      이마트, 트레이더스 쓱배송 및 점포택배 / 새벽배송', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만원 할인 오전 또는 오후 쿠폰 ID당 1일 1매 다운(오전 9시 오픈, 선착순 2만명)', '쓱배송, 새벽배송 모두 쓸 수 있는 10% 장바구니 오후 쿠폰', '      쿠폰 발급 및 사용일', '      23년 3월 16일(오전 또는 오후 쿠폰 ID당 1일 1매 다운)(발급된 쿠폰 당일 한정 사용 가능)', '      쿠폰 사용 조건', '      대상상품 : 이마트몰 쓱배송 / 트레이더스몰 쓱배송 및 점포택배 / 새벽배송 상품', '      쿠폰 발급 대상', '      쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '결제할 때 한 번 더 할인받기 오늘의 청구할인 카드혜택', '[SSGPAY전용] 삼성카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] KB국민카드 8만원이상 7% 청구할인 (일 5만원 한) 자세히보기', '[SSGPAY전용] SSG.COM 삼성카드 8만원이상 8% 청구할인 (일 5만원 한) 자세히보기', '인기상품 1+1, 최대 50% 할인 쓱배송데이 장보기 특가상품', '오늘 원하는 시간에 받고 싶다면, 이마트몰 쓱배송 추천상품']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다~딜 - P&amp;G편', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'P&amp;G 상품쿠폰 50% 3장, 개별 쿠폰 당 최대 5천원 할인', '무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '      쿠폰 발급 기간', '      쿠폰 사용 기간', '      상품할인쿠폰, 무료배송쿠폰: 2023년 3월 20일(월)~ 2023년 3월 26일(일)', '      쿠폰 사용 조건', '      무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '      쿠폰 발급 대상', '(50%, 무료배송) 헤드앤숄더 퍼퓸 프레쉬 샴푸 750mL 할인전 : 15,900원 할인후 : 7,950원', '(50%, 무료배송) 다우니 섬유유연제 2L(레몬그라스&amp;라일락) 할인전 : 14,800원 할인후 : 7,400원', '(50%, 무료배송, 1+1) 오랄비 칫솔 벨벳 초미세모 초소형헤드 3개입 할인전 : 11,900원 할인후 : 9,900원', '(50%, 무료배송) 질레트 퓨전 프로글라이드 플렉스볼 매뉴얼 면도기 2UP (기1+날2) 할인전 : 19,900원 할인후 : 9,950원', '(50%, 무료배송) 페브리즈 항균플러스 섬유탈취제 370ML (깨끗한향) 할인전 : 7,600원 할인후 : 3,800원', '할인 상품 한 눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SSG 창립4주년 감사대축제 'Thanks 4U'</t>
+          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>누구나 6종 쿠폰팩 + 매일 오전 10시 선착순 타임딜 + 브랜드 갈라쇼</t>
+          <t>응원 댓글 달고 스카이박스 &amp; 응원지정석 티켓 받자</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004808</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004957</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SSG 창립 4주년 감사대축제 'Thanks 4 U'</t>
+          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; SSG 창립 4주년 감사대축제 'Thanks 4 U'", '스마일클럽', '누구나 10% 할인 쿠폰 6매 / 최대 2만 5천원 할인', '6종 쿠폰 바로보기', '선착순 타임딜 바로보기', '한 시간 한정 최대 3만원 장바구니 쿠폰 발급 중!', '지금 바로! 장바구니 게릴라 쿠폰 놓치지 말고 받아가세요!', '장바구니 쿠폰 10% 8만원 이상 구매시 최대 3만원 할인', '※ 타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '딱 한시간만! 최대 3만원 장바구니 쿠폰 발급 중!', '쿠폰 발급 시간 : 2023년 3월 13일(월) 10시 00분 부터 3월 13일(월) 10시 59분 까지', '쿠폰 발급 시간 : 2023년 3월 15일(수) 10시 00분 부터 3월 15일(수) 10시 59분 까지', '타 사이트를 통해 방문하신 고객의 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '10% 할인 쿠폰 6매 누구나 최대 2만 5천원 할인!', '상품쿠폰 10% X 6', '6종 쿠폰팩 한번에 다운 받기', '쿠폰 할인 대상 및 사용 안내(레이어팝업 열기)', '※ 상품 상세에서 이미 쿠폰을 다운 받으신 경우 본 행사 페이지 에서는 쿠폰을 다운 받으실 수 없으며, 본 행사 페이지에서 이미 쿠폰을 다운 받으신 경우에는 상품 상세 에서 쿠폰을 다운 받으실 수 없습니다.', '쿠폰 이용안내', '할인 대상', '      10% 상품쿠폰 2매 1만원 이상 최대 3천원 1매, 4만원 이상 최대 5천원 1매', '      10% 상품쿠폰 2매 1만원 이상 최대 3천원 1매, 7만원 이상 최대 8천원 1매', '      10% 상품쿠폰 2매 10만원 이상 최대 1만 5천원 1매, 20만원 이상 최대 2만 5천원 1매', '쿠폰은 신세계몰, 신세계백화점몰 각 해당 카테고리에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다.', '신세계몰&amp;신세계백화점몰 첫구매 고객님이신가요\xa0', '첫구매 응원 최대 12% 장바구니 쿠폰', '매일 오전 07시 선착순 1만장 장바구니 쿠폰 12% 8민원 이상 구매시 최대 2만원 할인', '신세계백화점몰 및 신세계몰 첫구매 고객 대상 으로 발급되는 쿠폰 입니다.', '타 사이트를 통해 방문하신 경우, 결제시 장바구니 쿠폰이 적용되지 않습니다.', '쿠폰 마감 되었습니다.', '쿠폰발급 대상 : 2022년 3월 12일 이후로 신세계몰, 신세계백화점몰 구매 이력이 없는 고객', '타사이트를 통해 방문하신 경우 결제시 장바구니 쿠폰이 적용되지 않습니다.', '매일 오전 10시! 선착순 타임딜', '망설이명 품절! 핫딜로 구매하세요', '타임딜 행사는 SSG 모바일로 확인해주세요', '       타임딜 진행시간', '타임딜 대표 상품 미리보기', '3월 15일(화) : ★타임딜★ [립프로그] 아이스크림카트 디럭스(한영버전) 핑크, [SSG][2박스]팸퍼스 베이비드라이 팬티 8팩 기저귀', '3월 17일(화) : [블랑101] 1L세탁세제 2개+유연제 2개 택1 + 정품 사은품증정(품목 미정/본품으로 구성예정), [독일직구무료배송] 힙분유 Pre,1단계, 2단계, 2단계무전분, 3단계', '나이키 정기세일 UP TO 50% 신상품까지 할인! 쿠폰 더블혜택', 'SSG 창립4주년 한정! LG전자 라이프스타일 쇼핑 대축제 올레드TV, 오브제냉장고, 휘센에어컨, 그램PC 등 BEST상품 할인혜택', '내셔널지오그래픽 23SS 신상 오픈 적립 혜택! 이월 가격인하 + 추가 쿠폰 혜택까지', '쇼핑의 마무리 카드 청구 할인', '[SSGPAY전용]삼성카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용] SSG.COM카드 Edition2 8만원 이상 10% 청구할인 (일 5만원 한)', '[SSGPAY전용] 신한카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]KB카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]SSG.COM 삼성카드 8만원 이상 8% 청구할인 (일 5만원 한)', '[SSGPAY전용]비씨카드 8만원 이상 7% 청구할인 (일 5만원 한)', '[SSGPAY전용]신한카드 8만원 이상 5% 청구할인 (일 5만원 한)', '해피라운지 매일 오전 9시! 핫딜의 신세계']</t>
+          <t>['이벤트/쿠폰 &gt; 23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '스마일클럽', '23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '직관 이벤트 바로보기', '* 이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기됩니다. ※ 개인정보 위탁업체 : (주)젤라블루코리아 / 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호. 주소', '* 부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '* 이벤트에 대한 세부사항 및 경품내용은 당사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '맛과 가격 모두 완벽, 노브랜드 버거 핫딜', '         랜더스위크 스페셜 라이브에서 구매하고 랜더스 경품 GET(야구공, 유니폼), 자세한 이벤트 내용은 랜더스위크 스페셜 라이브 예고페이지를 참고해주세요!']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SSG 창립 4주년 장보기 혜택</t>
+          <t>Hopeful New Start</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>최대 50% 할인부터 S머니 5천원 페이백!</t>
+          <t>새 출발을 앞둔 모두에게 따듯한 마음을 선물하세요</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004812</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004908</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SSG.COM 창립 4주년 기념 장보기</t>
+          <t>Hopeful New start</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM 창립 4주년 기념 장보기', '스마일클럽', '최대 50% 할인', '단 하루 PLUS+ 혜택! 쓱배송데이! 종료까지', '미슐랭 2스타 셰프가 만든 케이크 50% 할인', '정식당으로 유명한 임정식 셰프가 운영중인 정식카페가 만든 케이크 50% 할인 받아보세요!', '장보기 특가 최대 50% 할인', '50% 할인', '대상 상품 : 쓱배송, 새벽배송 상품', '적립금 : SSG MONEY 5,000원 적립금 (30일내 사용가능)', '본 행사는 쓱배송 및 새벽배송 상품 10만원 이상 구매 시 응모 가능합니다. (트레이더스 상품 제외 / 기간 중 1회 기준이며 구매 금액 합산되지 않습니다)', '이벤트페이지에서 &lt;응모하기&gt;버튼을 눌러 신청하신 고객에 한해 해당 ID로 적립됩니다.', '쓱배송 만원 할인에 무료배송', '장바구니 쿠폰 10,000원 - 첫 구매 전용', '쓱배송/새벽배송 무료배송 - 첫 구매 전용', '쓱배송/새벽배송 2만원 이상 구매 시 사용 가능', '첫 구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '첫 구매 쿠폰 모두 받으러 가기', 'SSG 창립 4주년 장보기 최대 50% 할인 오반장 위크']</t>
+          <t>['이벤트/쿠폰 &gt; Hopeful New start', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>디즈니와 함께하는 SSG.COM 4주년 생일파티</t>
+          <t>집에서 즐기는 호텔 레시피</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4가지의 놀라운 혜택</t>
+          <t>최대 25% 할인과 5천원 페이백 이벤트</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004821</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004967</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>디즈니와 함께하는 SSG 4주년 생일파티</t>
+          <t>힙슐랭 가이드 : 집에서 즐기는 호텔 레시피</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 디즈니와 함께하는 SSG 4주년 생일파티', '스마일클럽', '추가 사은 이벤트 바로보기', '아이콘 클릭하여 친구들에게 공유하고 자동으로 이벤트 응모하기', ' 참여 방법 : 행사 기간 내 SSG.COM 로그인 후 인스타그램 또는 카카오톡 아이콘 클릭하여 이벤트 공유', '디즈니 브랜드관 구매 고객 추가 사은 이벤트']</t>
+          <t>['이벤트/쿠폰 &gt; 힙슐랭 가이드 : 집에서 즐기는 호텔 레시피', '스마일클럽', '# 최대 24% 할인', '최대 25% 할인 행사', '조식 [조선호텔] 생식빵 정상가 6,400원 10%할인가 5,760원 힙슐랭 comment조선델리의 인기 상품 생식빵입니다. 르방을 사용한 저온 장시간 발효법으로 우유의 진한 풍미와 촉촉함이 느껴집니다.', '디너 [조선호텔] 함박스테이크 정상가 12,900원 25%할인가 9,675원 힙슐랭 comment추억의 맛에 조선 호텔만의 노하우를 담은 함박스테이크입니다. 고기의 황금비율로 부드러운 식감에 진하게 끓여낸 데미그라스 소스로 풍미를 더했습니다.', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>오반장위크</t>
+          <t>먼데이문 SPRING WEEK</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SSG 창립 4주년 장보기 최대 50%할인</t>
+          <t>~15% 쿠폰으로 미세먼지/황사 토탈케어!</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004791</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005006</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(3/13~19)  오반장위크_SSG창립 4주년 기념</t>
+          <t>먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/13~19)  오반장위크_SSG창립 4주년 기념', '스마일클럽', 'SSG 창립 4주년 장보기 최대 50%할인', '매일 오전 9시, 최대 50%할인 오반장 PICK 오반장템 바로보기', '매일 오전 9시, 최대 50% 할인 놓치지 마세요!', '초콜릿/캔디/카라멜/젤리 브랜드별 최대 1+1, 54%할인', '한우바로구이 3종, 파머스픽 참외 1.2kg 최대 50%할인', '오반장상품으로 쓱배송/새벽배송 10만원 이상 장보고 SSG MONEY 5천원 페이백! SSG 창립 4주년 감사대축제 THANKS 4U!']</t>
+          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어', '스마일클럽', '봄맞이 뷰티 최대 15% 할인', '선착순4만명', '상품쿠폰', '%', '3만원 이상 상품 구매 시, 최대 1만2천원 할인', '선착순3만명', '2만원 이상 상품 구매 시, 최대 7천원 할인', '■ 쿠폰 발급 및 사용 기간 : 2023년 3월 20일 (월) 09시 00분 ~ 3월 26일 (일) 23시 59분', '■ 쿠폰 사용 조건 :', '- 각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 15% 상품쿠폰', '- 쿠폰 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '상품쿠폰 15% 선착순 3.5만명', '3만원 이상 상품 구매시 최대 1만 2천원 할인', '■ 쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '3월 먼데이문 UP TO 60% + 15%추가 할인쿠폰', '장영란 모공/기미케어 BEST ~71%OFF + 핑크톤업썬 단독구성!', 'SSG 3월 기획전 할인+쿠폰 중복할인까지', '[이동욱 PICK! 더마펌] 베스트 기초템&amp;선케어&amp;스페셜 홈케어 최대 68% OFF+사은품 증정', '클렌징&amp;스킨케어 BEST 최대 60% + 15% 쿠폰 / 구매금액별 사은품증정', '[우르오스 스프링위크] 피부보습 한통에 다 담다! BEST 최대15% 할인♥', '풍성한 볼륨업 케어 10% 할인&amp;기프트 증정', '[LIVE쇼핑] 홈쇼핑 헤어케어 ~25% OFF', '[웰라] 프리미엄 살롱 헤어케어 최대 50% 할인 + 10% 추가할인쿠폰 / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '★먼데이문15%쿠폰+다다익선10%할인★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '♥더바디샵X먼데이문♥ 최대35%쿠폰+추가할인혜택', '★창립기념★ 닥터브로너스 최대~36%할인 +구매별 60ml 증정 찬스', '피토가닉&amp;딥모이스처&amp;힐링포스 50%+ 1리터 대용량', '[몰튼 브라운] 헤븐리 진저릴리 리미티드 출시! 세트 특별 할인', '피부 광채 100% 충전', '에센스로션 구매시 스킨 100ml 증정', '1+1 &amp; BEST ~50% OFF', '붙이는 더마패드 UP TO 30%', '미니어쳐 증정 + UP TO 40%', '[시코르 화이트데이 추천] UP TO 30%', '★SSG 단독구성&amp;증정★  캐스키드슨 핸드&amp;바디케어템 (바디세트/핸드크림/립밤/바디미스트/손세정제/향수)~72%', '(15%쿠폰)봄맞이빅세일♥네이처리퍼블릭', '스프링 스킨케어 &amp; 클렌징 대전 5% 할인! + 전구매고객 사섀5종증정', '[바이오더마 촉촉 보습템!] 최대 40% OFF', '★단독★ SSG 4주년 기념 단독 NEW 출시 1+50%세트', '미세먼지 없애는 클렌징 DAY 최대 60% 세일! 핸드/바디/구강 모음전 + 사은품 증정', '뷰티 상품도 쓱배송', '[스킨케어 쓱배송] 셀퓨전씨/마녀공장/AHC  BEST 선제품 특가전', '아이크림/앰플/세럼/크림/클렌징 1+1 특가! 최대 30% / 한자플라스트(풋데오드란트&amp;풋크림)', '바이탈뷰티 슈퍼콜라겐/메타그린 예뻐지는 이너뷰티 ~50%', '~48% OFF 핫딜 및 1+1 혜택']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>만원 할인에 무료배송</t>
+          <t>3월 할인대전'사이먼위크</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>창립 기념 쓱배송 첫 구매 혜택</t>
+          <t>~10% 즉시할인 + 10% 카드청구할인</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004699</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005011</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>쓱배송 첫 구매 만원 할인</t>
+          <t>[0320-0326] 프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 쓱배송 첫 구매 만원 할인', '스마일클럽', '쓱배송 첫 구매 만원 할인', '최근 1년간 쓱배송이 처음이라면', '쓱배송 만원 할인에 무료배송', '10,000원 장바구니 쿠폰 - 첫구매 전용', '무료배송 - 첫구매 전용', '쓱배송/새벽배송 2만원 이상 구매 시 사용 가능', '첫 구매 쿠폰 모두 받기', '첫구매 쿠폰이 모두 소진되었습니다. 더 좋은 혜택으로 찾아뵙겠습니다.', '발급 대상 : 최근 1년 간 쓱배송 및 새벽배송 구매 이력이 없는 고객', '사용 조건 : 쓱배송 및 새벽배송 상품 2만원 이상 구매 시 사용 가능 ', '적용 대상 : 쓱배송 및 새벽배송 상품 한정 (일부 상품 제외)', '쓱배송 인기 아이템 추천', '믿고 사는 쓱배송 TOP RANKING', '쓱배송 라이프 즐기는 법']</t>
+          <t>['이벤트/쿠폰 &gt; [0320-0326] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 3월 할인 대전', '쿠폰 혜택 할인쿠폰 최대10%', '혜택에 할인을 더 10% 카드청구할인', '        10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 S/S 행사 둘러보기 - SPRING NEW PROMOTION *할인율은 정상가 기준 할인율임', '[스포츠 - 최대 70% 할인] 나이키골프/볼빅 골프 브랜드위크 外 보러가기', '[해외명품 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[여성패션 - 최대 80% 할인] 쟈딕앤볼테르 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[패션슈즈 - 최대 80% 할인] 슈즈 시즌 선입고 TOP 300 보러가기', '[패션잡화 - 최대 37% 할인] 쥬얼리 GIFT 추가할인 상품전 보러가기', '[언더웨어 - 최대 51% 할인] 라페어 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 81% 할인] 챔피온, 폴햄 특가 外 보러가기', '[키즈패션 - 최대 70% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 30% 할인] 웨지우드, 헹켈 外 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: 마리끌레르</t>
+          <t>봄 여행 준비 A to Z</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>최대 52% 할인부터 사은품 및 특별 라이브까지!</t>
+          <t>~5만원 할인+여행용품 10% 쿠폰 신세계면세점 쇼핑지원금 혜택</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004860</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004996</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르</t>
+          <t>봄 여행 준비 A to Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 마리끌레르', '스마일클럽', '오피스룩 맞춤형 셔츠 스타일 뒷면 요크라인을 따라 일정한 간격의 플리츠 주름을 블록하여 포인트를 주며 면 100% 소재로 쾌적한 착용감 여유있는 사이즈로 체형 커버에 용이합니다.', '       행사기간 마리끌레르 전 상품, 최대 52% 할인', '       행사상품 20만원 이상 구매 시, 볼캡 선착순 50명 증정', '       ※ 이벤트 페이지 상단에 모델 촬영한 8개 상품만 해당됩니다.', '       ※ 할인액을 제외한 최종 결제금액 기준입니다.', '       ※ 3/15 (수) SSG.LIVE 방송 볼캡 선착순 100개 증정과는 별개의 이벤트로 라이브 방송 시간 외 구매한 건을 대상으로 합니다.', '       라이브 방송 1분 시청 시, 10% 시청쿠폰 발급', '       ※ 시청쿠폰은 당일 자정까지만 사용 가능합니다.', '       마리끌레르 2개 상품 한정수량 핫딜', '       라이브 방송 한정 20만원 이상 구매 시, 볼캡 선착순 100명 증정', '       ※ 브랜드 스포트라이트 혜택인 볼캡 50개 선착순 증정과는 별개의 이벤트입니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 봄 여행 준비 A to Z', '스마일클럽', '최대 5만원 할인', '10% 추가 쿠폰', '7% 국내숙소 할인', 'KYTE 선착순 특가', '국제선 ~5만원 할인', '여행 전 상품 최대 5만원 할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '10% 장바구니 쿠폰', '      쿠폰 발급 조건', '장바구니 쿠폰 10% 2만원 이상 구매 시 최대 1만원 할인 (신세계몰/이마트몰/새벽배송)(반려동물,여행용 가방,자동차용품, 티켓, 입장권)', '상품 상세 페이지에서 쿠폰 적용 대상을 확인하세요! 전 상품 최대 5만원 할인+여행용품 10% 쿠폰 봄 여행 준비 A to Z', '쿠폰은 오전 9시부터 발급됩니다.', "신세계면세점 이벤트 페이지에서 '응모하기'를 완료하셔야 정상 응모처리 됩니다.", '국내 숙소 전 상품 7% 할인', '사용 방법요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 / 야놀자 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '따뜻할때 할인받고 떠나야죠! 봄 맞춤 숙소 추천', '행사 내용국제선 타이드스퀘어 항공권 선착순 100명 한정 5만원/2만원/1만원 추가 할인', '사용방법: 행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.2.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK</t>
+          <t>첫 구매 고객 해피반값쿠폰</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>봄맞이 취향맞춤 메이크업은 SSG에서!</t>
+          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004862</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어</t>
+          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-03-19</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄맞이 메이크업&amp;스킨케어', '스마일클럽', '~10% 쿠폰', '뷰티 10%쿠폰 ~5천원 할인', '- Thanks 4 U 쿠폰과 동일 -', 'BEST 아이섀도우 최대 15% OFF 및 추가 샘플 증정', '[클리오/페리페라 外] 3월 뷰티위크 UP TO 50%/1+1/사은혜택까지', '다운타우너 콜라보 스페셜 특가 최대40% 글로우픽수상', '베스트 무료배송 (블러워터틴트,멀티아이팔레트,페이스블러쉬,소프트매트립,뉴테이크 외)', '단독 기획, 최대 30% OFF', 'UP TO ~50% + 스팟 패치 증정', '스크래치 쿠폰받고 에어팟 맥스 GET!', '한정수량 체험특가 + ~60% OFF', '갈색병 세럼 할인+사은품', 'BEST ~39% 할인+상품권', '셀퓨전씨 봄볕 자외선 밀착 차단! 매일 18시 선착순 특가!', '[아떼] 7일만! 어센틱 립밤 SSG 단독 특가 / 선&amp;비비 한정수량 50%OFF + BEST 제안', '[닥터지] 스프링 SUN 페스타 BEST&amp;NEW 1+1 ~89%할인/구매사은품혜택♥', 'UP TO 40% / 메이크업은 키스미!', 'No.1더블세럼, 정품증정 이벤트', '[AHC] SSG 단독 구성 &amp; BEST 스킨/선케어 ~62%OFF + 사은품 증정', '고현정의 피부 비결, 코이 인기상품모음 ~20%OFF', '화이트데이 기프트 특가 및 적립행사 ~50%/구매금액별 신세계상품권 증정! 아이크림/나이트크림/기미잡티앰플/에센스', 'SSG 3월 기획전 최대 51%할인', '[UP TO 60%] 바이탈뷰티 특집전!', '봄맞이 최대 75% 세일! 룸스프레이/핸드/바디/구강 모음전 + 사은품 증정']</t>
+          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
         </is>
       </c>
     </row>
@@ -836,118 +836,155 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 2% 즉시할인', '최대 2% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '      이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '      카드혜택 + 스마일클럽 혜택', '      이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SSG푸드마켓 3/16(목) 11AM</t>
+          <t>V&amp;A 3/20(월) 7PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>고당도 오렌지, 성주 참외 선착순 1,000개 9,900원 핫딜</t>
+          <t>압도적 투명 광채 항산화앰플 핫딜 ~48%OFF!</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004834&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004932&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG푸드마켓 @SSG.LIVE 3/16(목) 11:00</t>
+          <t>[SSG.LIVE]3/20(월) V&amp;A</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-03-08</t>
+          <t>2023-03-14</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-03-16</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG푸드마켓 @SSG.LIVE 3/16(목) 11:00', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/20(월) V&amp;A', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>프리메라 3/16(목) 7PM</t>
+          <t>다이슨 3/20(월) 8PM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>프리메라 BEST 최대 39% 할인! PRMR 비타티놀 세럼 구매시, 상품권 증정!</t>
+          <t>에어랩 컴플리트 빈카블루 입고! 컴플리트 롱/슈퍼소닉 신상 외</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004882&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004835&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>프리메라 @SSG.LIVE 3/16(목) 7PM</t>
+          <t>다이슨@SSG.LIVE 3/20(월) 8:00PM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-08</t>
+          <t>2023-03-07</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-03-16</t>
+          <t>2023-03-22</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 프리메라 @SSG.LIVE 3/16(목) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 3/20(월) 8:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>일룸 쿠시노 3/16(목) 20PM</t>
+          <t>바이탈뷰티 3/21(화) 7PM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>침대/패드 최대 30%할인 +저상형 침대 3종 핫딜 75만원~ 디즈니 안전거울 증정</t>
+          <t>바이탈뷰티 SSG 슈퍼콜라겐 런칭 &amp; 메타그린 역대급 혜택</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004837&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004979&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>일룸 쿠시노@SSG.LIVE 3/16(목) 20:00PM</t>
+          <t>바이탈뷰티 @SSG.LIVE 3/21(화) 19:00PM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-03-07</t>
+          <t>2023-03-14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-03-17</t>
+          <t>2023-03-21</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 일룸 쿠시노@SSG.LIVE 3/16(목) 20:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 바이탈뷰티 @SSG.LIVE 3/21(화) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>쿠첸 3/21(화) 8PM</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>최대 47% 할인 라이브, 121플러스 모델 선착순 적립금 페이백</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004955&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>쿠첸 최대 47% 할인 라이브 @SSG.LIVE 3/21(화) 20PM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-03-13</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023-03-21</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 쿠첸 최대 47% 할인 라이브 @SSG.LIVE 3/21(화) 20PM', '스마일클럽', '쿠첸 최대 47% 할인 라이브 @SSG.LIVE 3/21(화) 20PM']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Mar 23 00:20:48 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,59 +473,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">첫구매는 반값다딜 </t>
+          <t>e장날</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>다우니, 페브리즈 등 인기브랜드 최대 2만원 할인 + 무료배송</t>
+          <t>오늘 단 하루! 오전/오후 10%쿠폰 선착순 발급</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004966&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005084</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>반값다~딜 - P&amp;G편</t>
+          <t>(3/23) e장날_10% 장바구니 쿠폰</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다~딜 - P&amp;G편', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'P&amp;G 상품쿠폰 50% 3장, 개별 쿠폰 당 최대 5천원 할인', '무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '      쿠폰 발급 기간', '      쿠폰 사용 기간', '      상품할인쿠폰, 무료배송쿠폰: 2023년 3월 20일(월)~ 2023년 3월 26일(일)', '      쿠폰 사용 조건', '      무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '      쿠폰 발급 대상', '(50%, 무료배송) 헤드앤숄더 퍼퓸 프레쉬 샴푸 750mL 할인전 : 15,900원 할인후 : 7,950원', '(50%, 무료배송) 다우니 섬유유연제 2L(레몬그라스&amp;라일락) 할인전 : 14,800원 할인후 : 7,400원', '(50%, 무료배송, 1+1) 오랄비 칫솔 벨벳 초미세모 초소형헤드 3개입 할인전 : 11,900원 할인후 : 9,900원', '(50%, 무료배송) 질레트 퓨전 프로글라이드 플렉스볼 매뉴얼 면도기 2UP (기1+날2) 할인전 : 19,900원 할인후 : 9,950원', '(50%, 무료배송) 페브리즈 항균플러스 섬유탈취제 370ML (깨끗한향) 할인전 : 7,600원 할인후 : 3,800원', '할인 상품 한 눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; (3/23) e장날_10% 장바구니 쿠폰', '스마일클럽', '(3/23) e장날_10% 장바구니 쿠폰', '       10% 선착순 쿠폰!', '10% 쿠폰 바로보기', '이마트몰, 새벽배송몰, 트레이더스몰 상품대상 10% 장바구니 쿠폰', '      이마트/트레이더스 쓱배송 및 점포택배, 새벽배송, 택배배송 상품', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만5천원 할인(오전 9시부터, 선착순 6만명)', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만5천원 할인(오후 2시부터, 선착순 6만명)', '쿠폰발급 및 사용 기간 2023년 3월 23일 목요일 단 하루(발급된 쿠폰은 당일 한정 사용가능) * 현금성 상품, 순금, 무형서비스 상품, 초특가 상품 등 일부 상품 제외됩니다.', '      쿠폰 발급 및 사용일', '      2023년 3월 23일 목요일 단 하루(발급된 쿠폰 당일 한정 사용 가능)', '      ID당 오전/오후 쿠폰 중 1매만 다운 가능', '      이마트몰/트레이더스몰/새벽배송몰 상품 대상(이마트/트레이더스 쓱배송 및 점포택배, 새벽배송, 택배배송 상품)', '      쿠폰 발급 대상', '발급된 쿠폰은 MY&gt;쿠폰&gt;보유쿠폰에서 확인 가능합니다.', '최대 5만원! 결제할 때 한 번 더 쏠쏠한 추가 할인 청구할인 카드혜택', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한도) 자세히 보기', 'KB국민카드 7만원 이상 5% 청구할인 (일 5만원 한도) 자세히 보기', '최대 57% 할인 단하루 특가 e장날 대표상품', '글로벌한 맛! 미국산 꽃갈비살 최대 36% 할인부터 노르웨이산 연어까지', '첫구매는\xa0반값다딜 P&amp;G편 다우니, 페브리즈 등 인기브랜드\xa0최대\xa02만원 할인 + 무료배송', '3월 나들이 도시락 한 상 김밥 VS 샌드위치 취향투표부터 쓱배송 과자 최대 1+1까지']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
+          <t>굿바이 미세먼지</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>응원 댓글 달고 스카이박스 &amp; 응원지정석 티켓 받자</t>
+          <t>한번에 구매하는 미세먼지 철벽 방어 아이템</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004957</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005094</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
+          <t>굿바이 미세먼지</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,34 +535,34 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '스마일클럽', '23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '직관 이벤트 바로보기', '* 이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기됩니다. ※ 개인정보 위탁업체 : (주)젤라블루코리아 / 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호. 주소', '* 부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '* 이벤트에 대한 세부사항 및 경품내용은 당사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '맛과 가격 모두 완벽, 노브랜드 버거 핫딜', '         랜더스위크 스페셜 라이브에서 구매하고 랜더스 경품 GET(야구공, 유니폼), 자세한 이벤트 내용은 랜더스위크 스페셜 라이브 예고페이지를 참고해주세요!']</t>
+          <t>['이벤트/쿠폰 &gt; 굿바이 미세먼지', '스마일클럽', '+ PLUS 카드 청구할인 혜택도 챙겨가세요!']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hopeful New Start</t>
+          <t xml:space="preserve">첫구매는 반값다딜 </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>새 출발을 앞둔 모두에게 따듯한 마음을 선물하세요</t>
+          <t>다우니, 페브리즈 등 인기브랜드 최대 2만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004908</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004966&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hopeful New start</t>
+          <t>반값다~딜 - P&amp;G편</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,34 +572,34 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Hopeful New start', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; 반값다~딜 - P&amp;G편', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'P&amp;G 상품쿠폰 50% 3장, 최대 할인금액 1만원(1장) 5천원(2장)', '무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '      쿠폰 발급 기간', '      쿠폰 사용 기간', '      상품할인쿠폰, 무료배송쿠폰: 2023년 3월 20일(월)~ 2023년 3월 26일(일)', '      쿠폰 사용 조건', '      무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '      쿠폰 발급 대상', '(50%, 무료배송) 헤드앤숄더 퍼퓸 프레쉬 샴푸 750mL 할인전 : 15,900원 할인후 : 7,950원', '(50%, 무료배송) 다우니 섬유유연제 2L(레몬그라스&amp;라일락) 할인전 : 12,500원 할인후 : 6,250원', '(50%, 무료배송, 1+1) 오랄비 칫솔 벨벳 초미세모 초소형헤드 3개입 할인전 : 9,900원 할인후 : 4,950원', '(50%, 무료배송) 질레트 퓨전 프로글라이드 플렉스볼 매뉴얼 면도기 2UP (기1+날2) 할인전 : 19,900원 할인후 : 9,950원', '(50%, 무료배송) 페브리즈 항균플러스 섬유탈취제 370ML (깨끗한향) 할인전 : 7,600원 할인후 : 3,800원', '할인 상품 한 눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>집에서 즐기는 호텔 레시피</t>
+          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>최대 25% 할인과 5천원 페이백 이벤트</t>
+          <t>응원 댓글 달고 스카이박스 &amp; 응원지정석 티켓 받자</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004967</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004957</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>힙슐랭 가이드 : 집에서 즐기는 호텔 레시피</t>
+          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -609,71 +609,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 힙슐랭 가이드 : 집에서 즐기는 호텔 레시피', '스마일클럽', '# 최대 24% 할인', '최대 25% 할인 행사', '조식 [조선호텔] 생식빵 정상가 6,400원 10%할인가 5,760원 힙슐랭 comment조선델리의 인기 상품 생식빵입니다. 르방을 사용한 저온 장시간 발효법으로 우유의 진한 풍미와 촉촉함이 느껴집니다.', '디너 [조선호텔] 함박스테이크 정상가 12,900원 25%할인가 9,675원 힙슐랭 comment추억의 맛에 조선 호텔만의 노하우를 담은 함박스테이크입니다. 고기의 황금비율로 부드러운 식감에 진하게 끓여낸 데미그라스 소스로 풍미를 더했습니다.', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '스마일클럽', '23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '직관 이벤트 바로보기', '* 이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기됩니다. ※ 개인정보 위탁업체 : (주)젤라블루코리아 / 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호. 주소', '* 부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '* 이벤트에 대한 세부사항 및 경품내용은 당사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '맛과 가격 모두 완벽, 노브랜드 버거 핫딜', '         랜더스위크 스페셜 라이브에서 구매하고 랜더스 경품 GET(야구공, 유니폼), 자세한 이벤트 내용은 랜더스위크 스페셜 라이브 예고페이지를 참고해주세요!']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK</t>
+          <t>3월 나들이 도시락 한 상</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>~15% 쿠폰으로 미세먼지/황사 토탈케어!</t>
+          <t>김밥 VS 샌드위치 취향투표부터 쓱배송 과자 최대 1+1까지</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005006</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005078</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어</t>
+          <t>집 밥 챌린지 - 도시락편</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-03-29</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어', '스마일클럽', '봄맞이 뷰티 최대 15% 할인', '선착순4만명', '상품쿠폰', '%', '3만원 이상 상품 구매 시, 최대 1만2천원 할인', '선착순3만명', '2만원 이상 상품 구매 시, 최대 7천원 할인', '■ 쿠폰 발급 및 사용 기간 : 2023년 3월 20일 (월) 09시 00분 ~ 3월 26일 (일) 23시 59분', '■ 쿠폰 사용 조건 :', '- 각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 15% 상품쿠폰', '- 쿠폰 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '상품쿠폰 15% 선착순 3.5만명', '3만원 이상 상품 구매시 최대 1만 2천원 할인', '■ 쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '3월 먼데이문 UP TO 60% + 15%추가 할인쿠폰', '장영란 모공/기미케어 BEST ~71%OFF + 핑크톤업썬 단독구성!', 'SSG 3월 기획전 할인+쿠폰 중복할인까지', '[이동욱 PICK! 더마펌] 베스트 기초템&amp;선케어&amp;스페셜 홈케어 최대 68% OFF+사은품 증정', '클렌징&amp;스킨케어 BEST 최대 60% + 15% 쿠폰 / 구매금액별 사은품증정', '[우르오스 스프링위크] 피부보습 한통에 다 담다! BEST 최대15% 할인♥', '풍성한 볼륨업 케어 10% 할인&amp;기프트 증정', '[LIVE쇼핑] 홈쇼핑 헤어케어 ~25% OFF', '[웰라] 프리미엄 살롱 헤어케어 최대 50% 할인 + 10% 추가할인쿠폰 / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '★먼데이문15%쿠폰+다다익선10%할인★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '♥더바디샵X먼데이문♥ 최대35%쿠폰+추가할인혜택', '★창립기념★ 닥터브로너스 최대~36%할인 +구매별 60ml 증정 찬스', '피토가닉&amp;딥모이스처&amp;힐링포스 50%+ 1리터 대용량', '[몰튼 브라운] 헤븐리 진저릴리 리미티드 출시! 세트 특별 할인', '피부 광채 100% 충전', '에센스로션 구매시 스킨 100ml 증정', '1+1 &amp; BEST ~50% OFF', '붙이는 더마패드 UP TO 30%', '미니어쳐 증정 + UP TO 40%', '[시코르 화이트데이 추천] UP TO 30%', '★SSG 단독구성&amp;증정★  캐스키드슨 핸드&amp;바디케어템 (바디세트/핸드크림/립밤/바디미스트/손세정제/향수)~72%', '(15%쿠폰)봄맞이빅세일♥네이처리퍼블릭', '스프링 스킨케어 &amp; 클렌징 대전 5% 할인! + 전구매고객 사섀5종증정', '[바이오더마 촉촉 보습템!] 최대 40% OFF', '★단독★ SSG 4주년 기념 단독 NEW 출시 1+50%세트', '미세먼지 없애는 클렌징 DAY 최대 60% 세일! 핸드/바디/구강 모음전 + 사은품 증정', '뷰티 상품도 쓱배송', '[스킨케어 쓱배송] 셀퓨전씨/마녀공장/AHC  BEST 선제품 특가전', '아이크림/앰플/세럼/크림/클렌징 1+1 특가! 최대 30% / 한자플라스트(풋데오드란트&amp;풋크림)', '바이탈뷰티 슈퍼콜라겐/메타그린 예뻐지는 이너뷰티 ~50%', '~48% OFF 핫딜 및 1+1 혜택']</t>
+          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 도시락편', '스마일클럽', '쓱배송 과자 최대 1+1까지', '다우니, 페브리즈 등 인기브랜드 최대 2만원 할인 + 무료배송 첫구매는 반값다딜 ']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3월 할인대전'사이먼위크</t>
+          <t>Hopeful New Start</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>~10% 즉시할인 + 10% 카드청구할인</t>
+          <t>새 출발을 앞둔 모두에게 따듯한 마음을 선물하세요</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005011</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004908</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[0320-0326] 프리미엄 아울렛 위크</t>
+          <t>Hopeful New start</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -683,34 +683,34 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0320-0326] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 3월 할인 대전', '쿠폰 혜택 할인쿠폰 최대10%', '혜택에 할인을 더 10% 카드청구할인', '        10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 S/S 행사 둘러보기 - SPRING NEW PROMOTION *할인율은 정상가 기준 할인율임', '[스포츠 - 최대 70% 할인] 나이키골프/볼빅 골프 브랜드위크 外 보러가기', '[해외명품 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[여성패션 - 최대 80% 할인] 쟈딕앤볼테르 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[패션슈즈 - 최대 80% 할인] 슈즈 시즌 선입고 TOP 300 보러가기', '[패션잡화 - 최대 37% 할인] 쥬얼리 GIFT 추가할인 상품전 보러가기', '[언더웨어 - 최대 51% 할인] 라페어 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 81% 할인] 챔피온, 폴햄 특가 外 보러가기', '[키즈패션 - 최대 70% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 30% 할인] 웨지우드, 헹켈 外 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; Hopeful New start', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>봄 여행 준비 A to Z</t>
+          <t>집에서 즐기는 호텔 레시피</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>~5만원 할인+여행용품 10% 쿠폰 신세계면세점 쇼핑지원금 혜택</t>
+          <t>최대 25% 할인과 5천원 페이백 이벤트</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004996</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004967</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>봄 여행 준비 A to Z</t>
+          <t>힙슐랭 가이드 : 집에서 즐기는 호텔 레시피</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -725,29 +725,29 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 봄 여행 준비 A to Z', '스마일클럽', '최대 5만원 할인', '10% 추가 쿠폰', '7% 국내숙소 할인', 'KYTE 선착순 특가', '국제선 ~5만원 할인', '여행 전 상품 최대 5만원 할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '10% 장바구니 쿠폰', '      쿠폰 발급 조건', '장바구니 쿠폰 10% 2만원 이상 구매 시 최대 1만원 할인 (신세계몰/이마트몰/새벽배송)(반려동물,여행용 가방,자동차용품, 티켓, 입장권)', '상품 상세 페이지에서 쿠폰 적용 대상을 확인하세요! 전 상품 최대 5만원 할인+여행용품 10% 쿠폰 봄 여행 준비 A to Z', '쿠폰은 오전 9시부터 발급됩니다.', "신세계면세점 이벤트 페이지에서 '응모하기'를 완료하셔야 정상 응모처리 됩니다.", '국내 숙소 전 상품 7% 할인', '사용 방법요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 / 야놀자 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '따뜻할때 할인받고 떠나야죠! 봄 맞춤 숙소 추천', '행사 내용국제선 타이드스퀘어 항공권 선착순 100명 한정 5만원/2만원/1만원 추가 할인', '사용방법: 행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.2.']</t>
+          <t>['이벤트/쿠폰 &gt; 힙슐랭 가이드 : 집에서 즐기는 호텔 레시피', '스마일클럽', '# 최대 24% 할인', '최대 25% 할인 행사', '조식 [조선호텔] 생식빵 정상가 6,400원 10%할인가 5,760원 힙슐랭 comment조선델리의 인기 상품 생식빵입니다. 르방을 사용한 저온 장시간 발효법으로 우유의 진한 풍미와 촉촉함이 느껴집니다.', '디너 [조선호텔] 함박스테이크 정상가 12,900원 25%할인가 9,675원 힙슐랭 comment추억의 맛에 조선 호텔만의 노하우를 담은 함박스테이크입니다. 고기의 황금비율로 부드러운 식감에 진하게 끓여낸 데미그라스 소스로 풍미를 더했습니다.', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>첫 구매 고객 해피반값쿠폰</t>
+          <t>먼데이문 SPRING WEEK</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
+          <t>~15% 쿠폰으로 미세먼지/황사 토탈케어!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005006</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
+          <t>먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -762,229 +762,266 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어', '스마일클럽', '봄맞이 뷰티 최대 15% 할인', '선착순4만명', '상품쿠폰', '%', '3만원 이상 상품 구매 시, 최대 1만2천원 할인', '선착순3만명', '2만원 이상 상품 구매 시, 최대 7천원 할인', '■ 쿠폰 발급 및 사용 기간 : 2023년 3월 20일 (월) 09시 00분 ~ 3월 26일 (일) 23시 59분', '■ 쿠폰 사용 조건 :', '- 각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 15% 상품쿠폰', '- 쿠폰 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '상품쿠폰 15% 선착순 3.5만명', '3만원 이상 상품 구매시 최대 1만 2천원 할인', '■ 쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '3월 먼데이문 UP TO 60% + 15%추가 할인쿠폰', '장영란 모공/기미케어 BEST ~71%OFF + 핑크톤업썬 단독구성!', 'SSG 3월 기획전 할인+쿠폰 중복할인까지', '[이동욱 PICK! 더마펌] 베스트 기초템&amp;선케어&amp;스페셜 홈케어 최대 68% OFF+사은품 증정', '클렌징&amp;스킨케어 BEST 최대 60% + 15% 쿠폰 / 구매금액별 사은품증정', '[우르오스 스프링위크] 피부보습 한통에 다 담다! BEST 최대15% 할인♥', '풍성한 볼륨업 케어 10% 할인&amp;기프트 증정', '[LIVE쇼핑] 홈쇼핑 헤어케어 ~25% OFF', '[웰라] 프리미엄 살롱 헤어케어 최대 50% 할인 + 10% 추가할인쿠폰 / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '★먼데이문15%쿠폰★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '♥더바디샵X먼데이문♥ 최대35%쿠폰+추가할인혜택', '★먼문위크★ 닥터브로너스  여행용60ml 증정+추가쿠폰', '피토가닉&amp;딥모이스처&amp;힐링포스 50%+ 1리터 대용량', '금주 한정 바디케어 20% OFF', '피부 광채 100% 충전', '에센스로션 구매시 스킨 100ml 증정', '1+1 &amp; BEST ~50% OFF', '붙이는 더마패드 UP TO 30%', '미니어쳐 증정 + UP TO 40%', '[시코르 추천] 인기 뷰티템 UP TO 30%', '★SSG 단독구성&amp;증정★  캐스키드슨 핸드&amp;바디케어템 (바디세트/핸드크림/립밤/바디미스트/손세정제/향수)~72%', '(15%쿠폰)봄맞이빅세일♥네이처리퍼블릭', '스프링 스킨케어 &amp; 클렌징 대전 5% 할인! + 전구매고객 사섀5종증정', '[바이오더마 촉촉 보습템!] 최대 40% OFF', '★단독★ SSG 4주년 기념 단독 NEW 출시 1+50%세트', '미세먼지 없애는 클렌징 DAY 최대 60% 세일! 핸드/바디/구강 모음전 + 사은품 증정', '뷰티 상품도 쓱배송', '[스킨케어 쓱배송] 셀퓨전씨/마녀공장/AHC  BEST 선제품 특가전', '아이크림/앰플/세럼/크림/클렌징 1+1 특가! 최대 30% / 한자플라스트(풋데오드란트&amp;풋크림)', '바이탈뷰티 슈퍼콜라겐/메타그린 예뻐지는 이너뷰티 ~50%', '~48% OFF 핫딜 및 1+1 혜택']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>최대 10.2만원 혜택</t>
+          <t>3월 할인대전'사이먼위크</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>~10% 즉시할인 + 10% 카드청구할인</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005011</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>[0320-0326] 프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; [0320-0326] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 3월 할인 대전', '쿠폰 혜택 할인쿠폰 최대10%', '혜택에 할인을 더 10% 카드청구할인', '        10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 S/S 행사 둘러보기 - SPRING NEW PROMOTION *할인율은 정상가 기준 할인율임', '[스포츠 - 최대 70% 할인] 나이키골프/볼빅 골프 브랜드위크 外 보러가기', '[해외명품 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[여성패션 - 최대 80% 할인] 쟈딕앤볼테르 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[패션슈즈 - 최대 80% 할인] 슈즈 시즌 선입고 TOP 300 보러가기', '[패션잡화 - 최대 37% 할인] 쥬얼리 GIFT 추가할인 상품전 보러가기', '[언더웨어 - 최대 51% 할인] 라페어 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 81% 할인] 챔피온, 폴햄 특가 外 보러가기', '[키즈패션 - 최대 70% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 30% 할인] 웨지우드, 헹켈 外 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>봄 여행 준비 A to Z</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>~5만원 할인+여행용품 10% 쿠폰 신세계면세점 쇼핑지원금 혜택</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004996</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>봄 여행 준비 A to Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 봄 여행 준비 A to Z', '스마일클럽', '최대 5만원 할인', '10% 추가 쿠폰', '7% 국내숙소 할인', 'KYTE 선착순 특가', '국제선 ~5만원 할인', '여행 전 상품 최대 5만원 할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '10% 장바구니 쿠폰', '      쿠폰 발급 조건', '장바구니 쿠폰 10% 2만원 이상 구매 시 최대 1만원 할인 (신세계몰/이마트몰/새벽배송)(반려동물,여행용 가방,자동차용품, 티켓, 입장권)', '상품 상세 페이지에서 쿠폰 적용 대상을 확인하세요! 전 상품 최대 5만원 할인+여행용품 10% 쿠폰 봄 여행 준비 A to Z', '쿠폰은 오전 9시부터 발급됩니다.', "신세계면세점 이벤트 페이지에서 '응모하기'를 완료하셔야 정상 응모처리 됩니다.", '국내 숙소 전 상품 7% 할인', '사용 방법요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 / 야놀자 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '따뜻할때 할인받고 떠나야죠! 봄 맞춤 숙소 추천', '행사 내용국제선 타이드스퀘어 항공권 선착순 100명 한정 5만원/2만원/1만원 추가 할인', '사용방법: 행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.2.']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>V&amp;A 3/20(월) 7PM</t>
+          <t>첫 구매 고객 해피반값쿠폰</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>압도적 투명 광채 항산화앰플 핫딜 ~48%OFF!</t>
+          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004932&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[SSG.LIVE]3/20(월) V&amp;A</t>
+          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-03-14</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-26</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/20(월) V&amp;A', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>다이슨 3/20(월) 8PM</t>
+          <t>최대 10.2만원 혜택</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>에어랩 컴플리트 빈카블루 입고! 컴플리트 롱/슈퍼소닉 신상 외</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004835&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>다이슨@SSG.LIVE 3/20(월) 8:00PM</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-07</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-03-22</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 3/20(월) 8:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>바이탈뷰티 3/21(화) 7PM</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>바이탈뷰티 SSG 슈퍼콜라겐 런칭 &amp; 메타그린 역대급 혜택</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004979&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>바이탈뷰티 @SSG.LIVE 3/21(화) 19:00PM</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-03-14</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-03-21</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 바이탈뷰티 @SSG.LIVE 3/21(화) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>쿠첸 3/21(화) 8PM</t>
+          <t>데코르테 3/23(목) 7PM</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>최대 47% 할인 라이브, 121플러스 모델 선착순 적립금 페이백</t>
+          <t>리포솜 세럼 세트 역대급 30% 핫딜! 12만원대 선착순</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004955&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005004&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>쿠첸 최대 47% 할인 라이브 @SSG.LIVE 3/21(화) 20PM</t>
+          <t>데코르테 @SSG.LIVE 3/23(목) 7PM</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-03-14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-03-21</t>
+          <t>2023-03-25</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 쿠첸 최대 47% 할인 라이브 @SSG.LIVE 3/21(화) 20PM', '스마일클럽', '쿠첸 최대 47% 할인 라이브 @SSG.LIVE 3/21(화) 20PM']</t>
+          <t>['이벤트/쿠폰 &gt; 데코르테 @SSG.LIVE 3/23(목) 7PM', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>덴프스 3/23(목) 8PM</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>공유가 선택한 탁! 소리나는 유산균 덴프스 라이브 최대 71% 할인특가</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004993&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>덴프스 @SSG.LIVE 3/23(목) 8PM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-03-14</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2023-03-23</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 덴프스 @SSG.LIVE 3/23(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Mar 27 00:20:02 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,138 +473,138 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>e장날</t>
+          <t>랜더스데이 기대평 EVENT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>오늘 단 하루! 오전/오후 10%쿠폰 선착순 발급</t>
+          <t>기대평 작성하고 상품권 받아가세요!</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005084</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005139</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(3/23) e장날_10% 장바구니 쿠폰</t>
+          <t>랜더스데이 기대평 EVENT</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (3/23) e장날_10% 장바구니 쿠폰', '스마일클럽', '(3/23) e장날_10% 장바구니 쿠폰', '       10% 선착순 쿠폰!', '10% 쿠폰 바로보기', '이마트몰, 새벽배송몰, 트레이더스몰 상품대상 10% 장바구니 쿠폰', '      이마트/트레이더스 쓱배송 및 점포택배, 새벽배송, 택배배송 상품', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만5천원 할인(오전 9시부터, 선착순 6만명)', '장바구니쿠폰 10% : 8만원 이상 결제시 최대 1만5천원 할인(오후 2시부터, 선착순 6만명)', '쿠폰발급 및 사용 기간 2023년 3월 23일 목요일 단 하루(발급된 쿠폰은 당일 한정 사용가능) * 현금성 상품, 순금, 무형서비스 상품, 초특가 상품 등 일부 상품 제외됩니다.', '      쿠폰 발급 및 사용일', '      2023년 3월 23일 목요일 단 하루(발급된 쿠폰 당일 한정 사용 가능)', '      ID당 오전/오후 쿠폰 중 1매만 다운 가능', '      이마트몰/트레이더스몰/새벽배송몰 상품 대상(이마트/트레이더스 쓱배송 및 점포택배, 새벽배송, 택배배송 상품)', '      쿠폰 발급 대상', '발급된 쿠폰은 MY&gt;쿠폰&gt;보유쿠폰에서 확인 가능합니다.', '최대 5만원! 결제할 때 한 번 더 쏠쏠한 추가 할인 청구할인 카드혜택', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한도) 자세히 보기', 'KB국민카드 7만원 이상 5% 청구할인 (일 5만원 한도) 자세히 보기', '최대 57% 할인 단하루 특가 e장날 대표상품', '글로벌한 맛! 미국산 꽃갈비살 최대 36% 할인부터 노르웨이산 연어까지', '첫구매는\xa0반값다딜 P&amp;G편 다우니, 페브리즈 등 인기브랜드\xa0최대\xa02만원 할인 + 무료배송', '3월 나들이 도시락 한 상 김밥 VS 샌드위치 취향투표부터 쓱배송 과자 최대 1+1까지']</t>
+          <t>['이벤트/쿠폰 &gt; 랜더스데이 기대평 EVENT', '스마일클럽', '스타벅스 e-gift 쿠폰 1만원 - 3명', '       경품발송을 위해 입력하신 경품발송정보가 이벤트 진행 대행업체에 제공되며, 경품 증정 후 즉시 파기합니다. (개인정보 위탁업체 : 젤라블루 / 제공범위 : 성명, 휴대전화 번호, 주소 등)', '       본 이벤트에 대한 세부사항은 그룹사 사정에 따라 임의로 변경, 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>굿바이 미세먼지</t>
+          <t>[첫구매 이벤트] 피코크 반값다딜</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>한번에 구매하는 미세먼지 철벽 방어 아이템</t>
+          <t>피코크 전상품 최대 2만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005094</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005097&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>굿바이 미세먼지</t>
+          <t>[첫구매 이벤트] 피코크 반값다딜</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 굿바이 미세먼지', '스마일클럽', '+ PLUS 카드 청구할인 혜택도 챙겨가세요!']</t>
+          <t>['이벤트/쿠폰 &gt; [첫구매 이벤트] 피코크 반값다딜', '스마일클럽', '[첫구매 이벤트] 피코크 반값다딜', '반가운 반값쿠폰팩 받기', 'STEP1 최근 1년간 쓱배송이 처음이라면, 피코크 전상품 50% 할인을 무료배송으로', 'PEACOCK 상품쿠폰 50% 3장, 최대할인금액 1만원 (1장), 5천원 (2장)', '무료배송 1장', '■ 쿠폰 발급 기간 : 2023년 3월 27일(월) ~2023년 3월 31(금)', '■ 쿠폰 사용 기간 : 상품할인쿠폰, 무료배송쿠폰: 2023년 3월 27일(월) ~2023년 3월 31(금)', '■ 쿠폰 사용 조건 :', '-상품할인 쿠폰 :  쓱배송/새벽배송 피코크 브랜드 상품 50% 할인. (최대할인금액 각 1만원, 5천원)', '-무료배송 쿠폰 :  이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '따끈따끈한 피코크 신상품을 한번에 ※할인가는 최대 1만원 할인쿠폰 적용 기준', '(50%, 무료배송) 프리미엄 고래사 종합 어묵이 들어간 뜨끈한 우동전골, 피코크 김치어묵전골 804g 할인전 : 14,800원 할인후 : 7,400원', ' 피코크 마라볶음면510g, 기존가 7,980원, 할인가 3,990원 ', ' 피코크 통살닭다리구이 매콤한맛 420g, 기존가 9,086원, 할인가 4,543원 ', ' 피코크 케이준프라이 감자튀김700g, 기존가 8,980원, 할인가 4,490원 ', ' 피코크 매콤양념 무뼈닭발 180g, 기존가 7,980원, 할인가 3,990원 ', ' 피코크 통살닭다리구이 매콤한맛 420g, 기존가 12,980원, 할인가 6,490원 ', '(50%, 무료배송) 광장시장 대표 K-맛집 순희네 빈대떡을 집에서 그맛 그대로, 순희네 녹두 빈대떡 400g 할인전 : 8,980원 할인후 : 4,490원', ' 피코크 신락원 해물누룽지탕 600g, 기존가 12,980원, 할인가 6,490원 ', ' [피코크X리북방] 순대전골 1,100g (4인분), 기존가 19,980원, 할인가 9,900원 ', ' [피코크]잭슨피자 시카코 페퍼로니 535g, 기존가 9,980원, 할인가 4,490원 ', ' [피코크] 초마짬뽕1,240g, 기존가 9,480원, 할인가 4,740원 ', '(50%, 무료배송) 갓 구운 겉바속촉 크로와상, 15분만에 뚝딱 완성, 피코크 미니크로와상300g(생지) 할인전 : 8,480원 할인후 : 4,240원', ' 피코크 바스크치즈케익 220g, 기존가 5,980원, 할인가 2,990원 ', ' 피코크 에이 클래스 그릭요거트 450g, 기존가 4,680원, 할인가 2,340원 ', ' [피코크]초콜릿 샌드위치 비스킷 135g, 기존가 2,980원, 할인가 1,490원 ', ' [피코크]과테말라 에스에이치비 핸드드립백10g X 10개 (원두커피), 기존가 7,680원, 할인가 3,840원 ', ' [피코크]과테말라 에스에이치비 핸드드립백10g X 10개 (원두커피), 기존가 5,376원, 할인가 2,688원 ']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">첫구매는 반값다딜 </t>
+          <t>3월 나들이 도시락 한 상</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>다우니, 페브리즈 등 인기브랜드 최대 2만원 할인 + 무료배송</t>
+          <t>김밥 VS 샌드위치 취향투표부터 쓱배송 과자 최대 1+1까지</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004966&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005078</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>반값다~딜 - P&amp;G편</t>
+          <t>집 밥 챌린지 - 도시락편</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-03-29</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 반값다~딜 - P&amp;G편', '스마일클럽', 'STEP1 최근 1년간 쓱배송이 처음이라면, 웰컴 쿠폰 받기', 'P&amp;G 상품쿠폰 50% 3장, 최대 할인금액 1만원(1장) 5천원(2장)', '무료배송 1장, 쓱/새벽배송 2만원 이상 구매 시', '      최근 1년 간 이마트몰, 트레이더스 쓱배송/점보택배 및 새벽배송 구매 이력이 없는 고객', '      쿠폰 발급 기간', '      쿠폰 사용 기간', '      상품할인쿠폰, 무료배송쿠폰: 2023년 3월 20일(월)~ 2023년 3월 26일(일)', '      쿠폰 사용 조건', '      무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '      쿠폰 발급 대상', '(50%, 무료배송) 헤드앤숄더 퍼퓸 프레쉬 샴푸 750mL 할인전 : 15,900원 할인후 : 7,950원', '(50%, 무료배송) 다우니 섬유유연제 2L(레몬그라스&amp;라일락) 할인전 : 12,500원 할인후 : 6,250원', '(50%, 무료배송, 1+1) 오랄비 칫솔 벨벳 초미세모 초소형헤드 3개입 할인전 : 9,900원 할인후 : 4,950원', '(50%, 무료배송) 질레트 퓨전 프로글라이드 플렉스볼 매뉴얼 면도기 2UP (기1+날2) 할인전 : 19,900원 할인후 : 9,950원', '(50%, 무료배송) 페브리즈 항균플러스 섬유탈취제 370ML (깨끗한향) 할인전 : 7,600원 할인후 : 3,800원', '할인 상품 한 눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 도시락편', '스마일클럽', '쓱배송 과자 최대 1+1까지']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
+          <t>프리미엄 리빙관 1주년 기념 이벤트</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>응원 댓글 달고 스카이박스 &amp; 응원지정석 티켓 받자</t>
+          <t>20만원 이상 구매시 2만원 페이백</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004957</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005102</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>23년 시즌 개막 기념 SSG랜더스 응원 이벤트</t>
+          <t>프리미엄 리빙 전문관 1주년 기념 행사</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -614,71 +614,71 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '스마일클럽', '23년 시즌 개막 기념 SSG랜더스 응원 이벤트', '직관 이벤트 바로보기', '* 이벤트에 응모하실 경우 개인정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품발송 완료 후 즉시 파기됩니다. ※ 개인정보 위탁업체 : (주)젤라블루코리아 / 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰 번호. 주소', '* 부정한 방법으로 이벤트에 참여한 것이 발견될 경우, 발표일 이후에도 당첨이 취소될 수 있습니다.', '* 이벤트에 대한 세부사항 및 경품내용은 당사 사정에 의해 조기 종료 및 변경될 수 있습니다.', '맛과 가격 모두 완벽, 노브랜드 버거 핫딜', '         랜더스위크 스페셜 라이브에서 구매하고 랜더스 경품 GET(야구공, 유니폼), 자세한 이벤트 내용은 랜더스위크 스페셜 라이브 예고페이지를 참고해주세요!']</t>
+          <t>['이벤트/쿠폰 &gt; 프리미엄 리빙 전문관 1주년 기념 행사', '스마일클럽', '선착순 SSG머니 2만원 페이백', '프리미엄 리빙관에서 20만원 이상 구매시 SSG머니 2만원을 드려요! (선착순 1,000명)', '      프리미엄 리빙관 상품 20만원 이상 구매시', '      2023년 4월 10일(월) 순차 지급. MY SSG - SSG MONEY에서 확인 가능', '      SSG MONEY 사용기한', '이벤트 페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한해 해당 ID로 적립됩니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 20000원']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3월 나들이 도시락 한 상</t>
+          <t>2030 부산세계박람회 유치 응원이벤트</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>김밥 VS 샌드위치 취향투표부터 쓱배송 과자 최대 1+1까지</t>
+          <t>최대 5만원 SSGMONEY 제공</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005078</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005077</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>집 밥 챌린지 - 도시락편</t>
+          <t>2030 부산세계박람회 응원이벤트</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-03-29</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 도시락편', '스마일클럽', '쓱배송 과자 최대 1+1까지', '다우니, 페브리즈 등 인기브랜드 최대 2만원 할인 + 무료배송 첫구매는 반값다딜 ']</t>
+          <t>['이벤트/쿠폰 &gt; 2030 부산세계박람회 응원이벤트', '스마일클럽', '2030 부산세계박람회 응원이벤트']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hopeful New Start</t>
+          <t>신세계 골프대전</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>새 출발을 앞둔 모두에게 따듯한 마음을 선물하세요</t>
+          <t>연중 최대 백화점 골프 행사를 만나보세요</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004908</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004939</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hopeful New start</t>
+          <t>신세계 골프페어</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,29 +688,29 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Hopeful New start', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; 신세계 골프페어', '스마일클럽', '스페셜 쿠폰 10% 바로보기', '스페셜 쿠폰 10% 혜택', '      쿠폰 발급 및 사용 기간', '      쿠폰 발급은 당사 사정에 따라 선착순 조기 마감될 수 있습니다.', '      쿠폰 발급 대상', '      경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다. ', '제이린드버그 50만원 이상 구매시 썬패치 증정', '나이키골프 인기 ITEM SSG 단독 40%OFF', 'WAAC 23 S/S 단독 10%할인 특가', '제이미웨스트 최대 70% 할인 (골프 가방, ACC 외)', '게리앤프레키 최대 50% 할인 및 구매 고객 대상 사은품 증정', 'LYF 23SS 신상품 최대 15%, 이월 최대 30% 할인 및 사은품 증정', '쿠폰은 오전 9시에 오픈됩니다:)', '쿠폰이 마감되었습니다!']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>집에서 즐기는 호텔 레시피</t>
+          <t>첫 구매 고객 해피반값쿠폰</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>최대 25% 할인과 5천원 페이백 이벤트</t>
+          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004967</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>힙슐랭 가이드 : 집에서 즐기는 호텔 레시피</t>
+          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -720,145 +720,145 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 힙슐랭 가이드 : 집에서 즐기는 호텔 레시피', '스마일클럽', '# 최대 24% 할인', '최대 25% 할인 행사', '조식 [조선호텔] 생식빵 정상가 6,400원 10%할인가 5,760원 힙슐랭 comment조선델리의 인기 상품 생식빵입니다. 르방을 사용한 저온 장시간 발효법으로 우유의 진한 풍미와 촉촉함이 느껴집니다.', '디너 [조선호텔] 함박스테이크 정상가 12,900원 25%할인가 9,675원 힙슐랭 comment추억의 맛에 조선 호텔만의 노하우를 담은 함박스테이크입니다. 고기의 황금비율로 부드러운 식감에 진하게 끓여낸 데미그라스 소스로 풍미를 더했습니다.', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK</t>
+          <t>최대 10.2만원 혜택</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>~15% 쿠폰으로 미세먼지/황사 토탈케어!</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005006</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 먼데이문 SPRING WEEK : 봄철 미세먼지/황사 토탈케어', '스마일클럽', '봄맞이 뷰티 최대 15% 할인', '선착순4만명', '상품쿠폰', '%', '3만원 이상 상품 구매 시, 최대 1만2천원 할인', '선착순3만명', '2만원 이상 상품 구매 시, 최대 7천원 할인', '■ 쿠폰 발급 및 사용 기간 : 2023년 3월 20일 (월) 09시 00분 ~ 3월 26일 (일) 23시 59분', '■ 쿠폰 사용 조건 :', '- 각 쿠폰별 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '트렌드뷰티 대표 브랜드 상품 15% 상품쿠폰', '- 쿠폰 대상몰 및 적용 카테고리는 SSG.COM 사이트 기준', '상품쿠폰 15% 선착순 3.5만명', '3만원 이상 상품 구매시 최대 1만 2천원 할인', '■ 쿠폰 발급 대상 : 스마일클럽 멤버십 가입회원 전용', '3월 먼데이문 UP TO 60% + 15%추가 할인쿠폰', '장영란 모공/기미케어 BEST ~71%OFF + 핑크톤업썬 단독구성!', 'SSG 3월 기획전 할인+쿠폰 중복할인까지', '[이동욱 PICK! 더마펌] 베스트 기초템&amp;선케어&amp;스페셜 홈케어 최대 68% OFF+사은품 증정', '클렌징&amp;스킨케어 BEST 최대 60% + 15% 쿠폰 / 구매금액별 사은품증정', '[우르오스 스프링위크] 피부보습 한통에 다 담다! BEST 최대15% 할인♥', '풍성한 볼륨업 케어 10% 할인&amp;기프트 증정', '[LIVE쇼핑] 홈쇼핑 헤어케어 ~25% OFF', '[웰라] 프리미엄 살롱 헤어케어 최대 50% 할인 + 10% 추가할인쿠폰 / 샴푸/ 컨디셔너/트리트먼트/헤어팩/헤어오일', '★먼데이문15%쿠폰★ 뉴트로지나/아비노/존슨즈베이비/아비노베이비/클린앤클리어 BEST 특가', '♥더바디샵X먼데이문♥ 최대35%쿠폰+추가할인혜택', '★먼문위크★ 닥터브로너스  여행용60ml 증정+추가쿠폰', '피토가닉&amp;딥모이스처&amp;힐링포스 50%+ 1리터 대용량', '금주 한정 바디케어 20% OFF', '피부 광채 100% 충전', '에센스로션 구매시 스킨 100ml 증정', '1+1 &amp; BEST ~50% OFF', '붙이는 더마패드 UP TO 30%', '미니어쳐 증정 + UP TO 40%', '[시코르 추천] 인기 뷰티템 UP TO 30%', '★SSG 단독구성&amp;증정★  캐스키드슨 핸드&amp;바디케어템 (바디세트/핸드크림/립밤/바디미스트/손세정제/향수)~72%', '(15%쿠폰)봄맞이빅세일♥네이처리퍼블릭', '스프링 스킨케어 &amp; 클렌징 대전 5% 할인! + 전구매고객 사섀5종증정', '[바이오더마 촉촉 보습템!] 최대 40% OFF', '★단독★ SSG 4주년 기념 단독 NEW 출시 1+50%세트', '미세먼지 없애는 클렌징 DAY 최대 60% 세일! 핸드/바디/구강 모음전 + 사은품 증정', '뷰티 상품도 쓱배송', '[스킨케어 쓱배송] 셀퓨전씨/마녀공장/AHC  BEST 선제품 특가전', '아이크림/앰플/세럼/크림/클렌징 1+1 특가! 최대 30% / 한자플라스트(풋데오드란트&amp;풋크림)', '바이탈뷰티 슈퍼콜라겐/메타그린 예뻐지는 이너뷰티 ~50%', '~48% OFF 핫딜 및 1+1 혜택']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3월 할인대전'사이먼위크</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>~10% 즉시할인 + 10% 카드청구할인</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005011</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[0320-0326] 프리미엄 아울렛 위크</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0320-0326] 프리미엄 아울렛 위크', '스마일클럽', '프리미엄 아울렛 3월 할인 대전', '쿠폰 혜택 할인쿠폰 최대10%', '혜택에 할인을 더 10% 카드청구할인', '        10% 청구할인 *10만원 이상 구매 시 일 최대 10만원 한도', 'EVENT 03 아울렛 S/S 행사 둘러보기 - SPRING NEW PROMOTION *할인율은 정상가 기준 할인율임', '[스포츠 - 최대 70% 할인] 나이키골프/볼빅 골프 브랜드위크 外 보러가기', '[해외명품 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[여성패션 - 최대 80% 할인] 쟈딕앤볼테르 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[패션슈즈 - 최대 80% 할인] 슈즈 시즌 선입고 TOP 300 보러가기', '[패션잡화 - 최대 37% 할인] 쥬얼리 GIFT 추가할인 상품전 보러가기', '[언더웨어 - 최대 51% 할인] 라페어 브랜드 위크 특가 &amp; 쿠폰 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/간트/브룩스브라더스 특가 外 보러가기', '[유니섹스 - 최대 81% 할인] 챔피온, 폴햄 특가 外 보러가기', '[키즈패션 - 최대 70% 할인] 게스키즈/ 아디다스 키즈 브랜드 위크 外 보러가기', '[리빙 - 최대 30% 할인] 웨지우드, 헹켈 外 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>봄 여행 준비 A to Z</t>
+          <t>아이오페  3/27(월) 7PM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>~5만원 할인+여행용품 10% 쿠폰 신세계면세점 쇼핑지원금 혜택</t>
+          <t>핫딜가+선착순 추가 적립부터 구매금액별 사은품까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004996</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005142&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>봄 여행 준비 A to Z</t>
+          <t>아이오페 슈퍼바이탈 래디언트 스틱  @SSG.LIVE 3/27(월) 19PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-03-21</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 봄 여행 준비 A to Z', '스마일클럽', '최대 5만원 할인', '10% 추가 쿠폰', '7% 국내숙소 할인', 'KYTE 선착순 특가', '국제선 ~5만원 할인', '여행 전 상품 최대 5만원 할인', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '10% 장바구니 쿠폰', '      쿠폰 발급 조건', '장바구니 쿠폰 10% 2만원 이상 구매 시 최대 1만원 할인 (신세계몰/이마트몰/새벽배송)(반려동물,여행용 가방,자동차용품, 티켓, 입장권)', '상품 상세 페이지에서 쿠폰 적용 대상을 확인하세요! 전 상품 최대 5만원 할인+여행용품 10% 쿠폰 봄 여행 준비 A to Z', '쿠폰은 오전 9시부터 발급됩니다.', "신세계면세점 이벤트 페이지에서 '응모하기'를 완료하셔야 정상 응모처리 됩니다.", '국내 숙소 전 상품 7% 할인', '사용 방법요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '사용 방법: 요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  여기어때 / 야놀자 실시간 호텔 전 상품 1원 이상 구매 시 5% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '따뜻할때 할인받고 떠나야죠! 봄 맞춤 숙소 추천', '행사 내용국제선 타이드스퀘어 항공권 선착순 100명 한정 5만원/2만원/1만원 추가 할인', '사용방법: 행사 대상 항공권 결제 시 자동적용으로 선착순 마감 시 자동 종료', '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.2.']</t>
+          <t>['이벤트/쿠폰 &gt; 아이오페 슈퍼바이탈 래디언트 스틱  @SSG.LIVE 3/27(월) 19PM', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>첫 구매 고객 해피반값쿠폰</t>
+          <t>제주항공 3/27(월) 8PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
+          <t>해외 인기 10대노선 특가! 일본/동남아 편도 최저 8만원대~</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005090&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
+          <t>[SSG.LIVE]3/27(월) 제주항공</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -868,160 +868,86 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-03-26</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/27(월) 제주항공', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>최대 10.2만원 혜택</t>
+          <t>남도장터 3/28(화) 11AM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>한돈 1등급 목살 500g 6천원대~, 삼겹살 500g 8천원대~ 선착순 핫딜</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005169&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>남도장터 @SSG.LIVE 3/28(화) 11AM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023-03-22</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-03-28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; 남도장터 @SSG.LIVE 3/28(화) 11AM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>쓱직구 베스트템 연합전</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>패션부터 식품까지 대방출</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005135</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>그랜드 조선 부산 X SSG.COM X 또떠남</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>데코르테 3/23(목) 7PM</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>리포솜 세럼 세트 역대급 30% 핫딜! 12만원대 선착순</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005004&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>데코르테 @SSG.LIVE 3/23(목) 7PM</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2023-03-14</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-03-25</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 데코르테 @SSG.LIVE 3/23(목) 7PM', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>덴프스 3/23(목) 8PM</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>공유가 선택한 탁! 소리나는 유산균 덴프스 라이브 최대 71% 할인특가</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004993&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>덴프스 @SSG.LIVE 3/23(목) 8PM</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2023-03-14</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-03-23</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 덴프스 @SSG.LIVE 3/23(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 그랜드 조선 부산 X SSG.COM X 또떠남', '스마일클럽']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Mar 30 00:20:13 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,59 +547,59 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3월 나들이 도시락 한 상</t>
+          <t>프리미엄 리빙관 1주년 기념 이벤트</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>김밥 VS 샌드위치 취향투표부터 쓱배송 과자 최대 1+1까지</t>
+          <t>20만원 이상 구매시 2만원 페이백</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005078</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005102</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>집 밥 챌린지 - 도시락편</t>
+          <t>프리미엄 리빙 전문관 1주년 기념 행사</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-03-29</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 집 밥 챌린지 - 도시락편', '스마일클럽', '쓱배송 과자 최대 1+1까지']</t>
+          <t>['이벤트/쿠폰 &gt; 프리미엄 리빙 전문관 1주년 기념 행사', '스마일클럽', '선착순 SSG머니 2만원 페이백', '프리미엄 리빙관에서 20만원 이상 구매시 SSG머니 2만원을 드려요! (선착순 1,000명)', '      프리미엄 리빙관 상품 20만원 이상 구매시', '      2023년 4월 10일(월) 순차 지급. MY SSG - SSG MONEY에서 확인 가능', '      SSG MONEY 사용기한', '이벤트 페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한해 해당 ID로 적립됩니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 20000원']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>프리미엄 리빙관 1주년 기념 이벤트</t>
+          <t>2030 부산세계박람회 유치 응원이벤트</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>20만원 이상 구매시 2만원 페이백</t>
+          <t>최대 5만원 SSGMONEY 제공</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005102</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005077</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>프리미엄 리빙 전문관 1주년 기념 행사</t>
+          <t>2030 부산세계박람회 응원이벤트</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -614,34 +614,34 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 프리미엄 리빙 전문관 1주년 기념 행사', '스마일클럽', '선착순 SSG머니 2만원 페이백', '프리미엄 리빙관에서 20만원 이상 구매시 SSG머니 2만원을 드려요! (선착순 1,000명)', '      프리미엄 리빙관 상품 20만원 이상 구매시', '      2023년 4월 10일(월) 순차 지급. MY SSG - SSG MONEY에서 확인 가능', '      SSG MONEY 사용기한', '이벤트 페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한해 해당 ID로 적립됩니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 20000원']</t>
+          <t>['이벤트/쿠폰 &gt; 2030 부산세계박람회 응원이벤트', '스마일클럽', '2030 부산세계박람회 응원이벤트']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2030 부산세계박람회 유치 응원이벤트</t>
+          <t>신세계 골프대전</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>최대 5만원 SSGMONEY 제공</t>
+          <t>연중 최대 백화점 골프 행사를 만나보세요</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005077</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004939</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2030 부산세계박람회 응원이벤트</t>
+          <t>신세계 골프페어</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-27</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -651,301 +651,190 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2030 부산세계박람회 응원이벤트', '스마일클럽', '2030 부산세계박람회 응원이벤트']</t>
+          <t>['이벤트/쿠폰 &gt; 신세계 골프페어', '스마일클럽', '스페셜 쿠폰 10% 바로보기', '스페셜 쿠폰 10% 혜택', '      쿠폰 발급 및 사용 기간', '      쿠폰 발급은 당사 사정에 따라 선착순 조기 마감될 수 있습니다.', '      쿠폰 발급 대상', '      경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다. ', '제이린드버그 50만원 이상 구매시 썬패치 증정', '나이키골프 인기 ITEM SSG 단독 40%OFF', 'WAAC 23 S/S 단독 10%할인 특가', '제이미웨스트 최대 70% 할인 (골프 가방, ACC 외)', '게리앤프레키 최대 50% 할인 및 구매 고객 대상 사은품 증정', 'LYF 23SS 신상품 최대 15%, 이월 최대 30% 할인 및 사은품 증정', '쿠폰은 오전 9시에 오픈됩니다:)', '쿠폰이 마감되었습니다!']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>신세계 골프대전</t>
+          <t>첫 구매 고객 해피반값쿠폰</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>연중 최대 백화점 골프 행사를 만나보세요</t>
+          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004939</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>신세계 골프페어</t>
+          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신세계 골프페어', '스마일클럽', '스페셜 쿠폰 10% 바로보기', '스페셜 쿠폰 10% 혜택', '      쿠폰 발급 및 사용 기간', '      쿠폰 발급은 당사 사정에 따라 선착순 조기 마감될 수 있습니다.', '      쿠폰 발급 대상', '      경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다. ', '제이린드버그 50만원 이상 구매시 썬패치 증정', '나이키골프 인기 ITEM SSG 단독 40%OFF', 'WAAC 23 S/S 단독 10%할인 특가', '제이미웨스트 최대 70% 할인 (골프 가방, ACC 외)', '게리앤프레키 최대 50% 할인 및 구매 고객 대상 사은품 증정', 'LYF 23SS 신상품 최대 15%, 이월 최대 30% 할인 및 사은품 증정', '쿠폰은 오전 9시에 오픈됩니다:)', '쿠폰이 마감되었습니다!']</t>
+          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>첫 구매 고객 해피반값쿠폰</t>
+          <t>최대 10.2만원 혜택</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>최대 10.2만원 혜택</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>크리니크 3/30(목) 8PM</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>치크팝 단독특가 &amp; 마스카라/수분크림 대용량 1+1 기획</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005157&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>크리니크 @SSG.LIVE 3/30(목) 20:00PM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023-03-22</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023-03-30</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 크리니크 @SSG.LIVE 3/30(목) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>아이오페  3/27(월) 7PM</t>
+          <t>그랜드조선부산 X 또떠남</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>핫딜가+선착순 추가 적립부터 구매금액별 사은품까지</t>
+          <t>해운대 오션뷰 객실 단독특가 + 청구혜택까지</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005142&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005135</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>아이오페 슈퍼바이탈 래디언트 스틱  @SSG.LIVE 3/27(월) 19PM</t>
+          <t>그랜드 조선 부산 X SSG.COM X 또떠남</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-03-21</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-03-27</t>
+          <t>2023-04-02</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 아이오페 슈퍼바이탈 래디언트 스틱  @SSG.LIVE 3/27(월) 19PM', '스마일클럽']</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>제주항공 3/27(월) 8PM</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>해외 인기 10대노선 특가! 일본/동남아 편도 최저 8만원대~</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005090&amp;domainSiteNo=6005</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]3/27(월) 제주항공</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2023-03-20</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2023-03-27</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]3/27(월) 제주항공', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>남도장터 3/28(화) 11AM</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>한돈 1등급 목살 500g 6천원대~, 삼겹살 500g 8천원대~ 선착순 핫딜</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005169&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>남도장터 @SSG.LIVE 3/28(화) 11AM</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2023-03-22</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2023-03-28</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 남도장터 @SSG.LIVE 3/28(화) 11AM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>쓱직구 베스트템 연합전</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>패션부터 식품까지 대방출</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005135</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>그랜드 조선 부산 X SSG.COM X 또떠남</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2023-03-24</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2023-04-02</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
         <is>
           <t>['이벤트/쿠폰 &gt; 그랜드 조선 부산 X SSG.COM X 또떠남', '스마일클럽']</t>
         </is>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Apr 13 00:18:23 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,370 +473,629 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>랜더스데이 기대평 EVENT</t>
+          <t>오늘은 장보는 날, 쓱배송데이</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기대평 작성하고 상품권 받아가세요!</t>
+          <t>오늘 단 하루! 00시/오전/오후 10%쿠폰 선착순 발급</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005139</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005473</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>랜더스데이 기대평 EVENT</t>
+          <t>오늘은 장보는 날, 쓱배송데이</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023.04.13</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023.04.13</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 랜더스데이 기대평 EVENT', '스마일클럽', '스타벅스 e-gift 쿠폰 1만원 - 3명', '       경품발송을 위해 입력하신 경품발송정보가 이벤트 진행 대행업체에 제공되며, 경품 증정 후 즉시 파기합니다. (개인정보 위탁업체 : 젤라블루 / 제공범위 : 성명, 휴대전화 번호, 주소 등)', '       본 이벤트에 대한 세부사항은 그룹사 사정에 따라 임의로 변경, 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 오늘은 장보는 날, 쓱배송데이', '스마일클럽', '오늘은 장보는 날, 쓱배송데이', '오늘은 장보는날 쓱배송 DAY', '10% 선착순 쿠폰! 오늘 단 하루 00시/09시/14시 딱 3번의 기회', '선착순 10%쿠폰 바로보기', '추가 5% 카드혜택 바로보기', '최대 50% 특가 상품 바로보기', '10% 장바구니 쿠폰', '00시 쿠폰', '00시 오픈, 선착순 2만명 장바구니 10% 쿠폰 : 7만원 이상 결제시 최대 1만원 할인', '오전 9시 쿠폰', '           이마트몰/새벽배송몰/트레이더스몰 상품 대상 (이마트/트레이더스 쓱배송 및 점포택배, 새벽배송, 택배배송상품)', '오전 9시 오픈, 선착순 2만명 장바구니 10% 쿠폰 : 7만원 이상 결제시 최대 1만원 할인', '오후 2시 쿠폰', '오후 2시 오픈, 선착순 2만명 장바구니 10% 쿠폰 : 7만원 이상 결제시 최대 1만원 할인', '쓱배송, 새벽배송, 트레이더스쓱배송 및 점포택배 상품 대상', '        쿠폰 발급 및 사용 기간', '       쿠폰 발급 기간', '       쿠폰 사용 조건', '       대상상품 : 이마트/트레이더스 쓱배송 및 점포택배, 새벽배송상품 대상', '       쿠폰 발급 대상', '       발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '최대 5% 결제할 때 한 번 더 추가 할인', '청구할인 카드혜택', 'KB 국민카드 8만원 이상 5% 청구할인 (일 5만원 한도) 자세히보기', 'KB 국민카드 8만원 이상 5% 청구할인 (일 5만원 한도)', '최대 50%할인, 1+1 쓱배송 대표상품']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[첫구매 이벤트] 피코크 반값다딜</t>
+          <t>SPRING FESTIVAL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>피코크 전상품 최대 2만원 할인 + 무료배송</t>
+          <t>누구나 최대 10% 할인쿠폰 + 봄나들이 필수 아이템</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005097&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005376</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[첫구매 이벤트] 피코크 반값다딜</t>
+          <t>SPRING FESTIVAL : 나들이 쇼핑위크</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-03-27</t>
+          <t>2023.04.10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023.04.16</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [첫구매 이벤트] 피코크 반값다딜', '스마일클럽', '[첫구매 이벤트] 피코크 반값다딜', '반가운 반값쿠폰팩 받기', 'STEP1 최근 1년간 쓱배송이 처음이라면, 피코크 전상품 50% 할인을 무료배송으로', 'PEACOCK 상품쿠폰 50% 3장, 최대할인금액 1만원 (1장), 5천원 (2장)', '무료배송 1장', '■ 쿠폰 발급 기간 : 2023년 3월 27일(월) ~2023년 3월 31(금)', '■ 쿠폰 사용 기간 : 상품할인쿠폰, 무료배송쿠폰: 2023년 3월 27일(월) ~2023년 3월 31(금)', '■ 쿠폰 사용 조건 :', '-상품할인 쿠폰 :  쓱배송/새벽배송 피코크 브랜드 상품 50% 할인. (최대할인금액 각 1만원, 5천원)', '-무료배송 쿠폰 :  이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '따끈따끈한 피코크 신상품을 한번에 ※할인가는 최대 1만원 할인쿠폰 적용 기준', '(50%, 무료배송) 프리미엄 고래사 종합 어묵이 들어간 뜨끈한 우동전골, 피코크 김치어묵전골 804g 할인전 : 14,800원 할인후 : 7,400원', ' 피코크 마라볶음면510g, 기존가 7,980원, 할인가 3,990원 ', ' 피코크 통살닭다리구이 매콤한맛 420g, 기존가 9,086원, 할인가 4,543원 ', ' 피코크 케이준프라이 감자튀김700g, 기존가 8,980원, 할인가 4,490원 ', ' 피코크 매콤양념 무뼈닭발 180g, 기존가 7,980원, 할인가 3,990원 ', ' 피코크 통살닭다리구이 매콤한맛 420g, 기존가 12,980원, 할인가 6,490원 ', '(50%, 무료배송) 광장시장 대표 K-맛집 순희네 빈대떡을 집에서 그맛 그대로, 순희네 녹두 빈대떡 400g 할인전 : 8,980원 할인후 : 4,490원', ' 피코크 신락원 해물누룽지탕 600g, 기존가 12,980원, 할인가 6,490원 ', ' [피코크X리북방] 순대전골 1,100g (4인분), 기존가 19,980원, 할인가 9,900원 ', ' [피코크]잭슨피자 시카코 페퍼로니 535g, 기존가 9,980원, 할인가 4,490원 ', ' [피코크] 초마짬뽕1,240g, 기존가 9,480원, 할인가 4,740원 ', '(50%, 무료배송) 갓 구운 겉바속촉 크로와상, 15분만에 뚝딱 완성, 피코크 미니크로와상300g(생지) 할인전 : 8,480원 할인후 : 4,240원', ' 피코크 바스크치즈케익 220g, 기존가 5,980원, 할인가 2,990원 ', ' 피코크 에이 클래스 그릭요거트 450g, 기존가 4,680원, 할인가 2,340원 ', ' [피코크]초콜릿 샌드위치 비스킷 135g, 기존가 2,980원, 할인가 1,490원 ', ' [피코크]과테말라 에스에이치비 핸드드립백10g X 10개 (원두커피), 기존가 7,680원, 할인가 3,840원 ', ' [피코크]과테말라 에스에이치비 핸드드립백10g X 10개 (원두커피), 기존가 5,376원, 할인가 2,688원 ']</t>
+          <t>['이벤트/쿠폰 &gt; SPRING FESTIVAL : 나들이 쇼핑위크', '스마일클럽', '누구나 최대 10% 할인 쿠폰 봄나들이 필수 상품&amp;브랜드', '최대 10% 쿠폰 바로보기', '누구나 최대 10% 할인 피크닉 전용 선착순 쿠폰', '장바구니 쿠폰 10% - 8만원 이상 구매시 최대 1만원 할인(매일 오전 9시, 선착순 1만장)', '장바구니 쿠폰 10% - 8만원 이상 구매시 최대 1만원 할인(매일 오전 9시, 선착순 15,000장)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 발급 받기(기간 내 ID당 1회 발급)', '      쿠폰 발급 기간', '      23/04/10(월) ~ 23/04/16(일), 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '쿠폰은 매일 선착순 15,000장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '프레드페리 - 브랜드데이 15% 혜택 보러가기', '올리브데올리브 - SSG 단독 신상+이월 SPRING SALE 60% 할인 보러가기', '나이키 - 4월 정기세일 UP TO 48% 할인 보러가기', '레페토 - 명품/잡화 봄맞이 베스트 브랜드 연합전 12% 할인 보러가기', '랑콜 - 봄철 피부 관리, 랑콤 UV 정품용량 증정 15% 할인 보러가기', '크록스 - 23 S/S 봄맞이 인기 크록스 대량 입고 80% 할인 보러가기', '룰루레몬 - Spring Favourites 신제품 기획전 SSG 머니 5% 적립 보러가기', '캉골키즈 - SSG 단독 상품 입고 10% 할인 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>프리미엄 리빙관 1주년 기념 이벤트</t>
+          <t>유아동 쓱세일 COMING SOON</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>20만원 이상 구매시 2만원 페이백</t>
+          <t>사전행사 특별 혜택 SSG머니 2천원 놓치지 마세요</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005102</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005088</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>프리미엄 리빙 전문관 1주년 기념 행사</t>
+          <t>유아동 쓱세일 COMING SOON</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-27</t>
+          <t>2023.04.13</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023.04.16</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 프리미엄 리빙 전문관 1주년 기념 행사', '스마일클럽', '선착순 SSG머니 2만원 페이백', '프리미엄 리빙관에서 20만원 이상 구매시 SSG머니 2만원을 드려요! (선착순 1,000명)', '      프리미엄 리빙관 상품 20만원 이상 구매시', '      2023년 4월 10일(월) 순차 지급. MY SSG - SSG MONEY에서 확인 가능', '      SSG MONEY 사용기한', '이벤트 페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한해 해당 ID로 적립됩니다.', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 20000원']</t>
+          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일 COMING SOON', '스마일클럽', '4월 17일 역대급 유아동 쇼핑 행사가 찾아옵니다. 사전 이벤트 참여하시고, SSG머니 100% 페이백 챙겨가세요!', '공유하기 - 클릭 하면 자동 이벤트 응모', 'STEP.1 유아동 쓱세일 사전 이벤트 공유하고 위 [공유하기] 버튼 클릭 필수!', '      MY SSG - SSG MONEY에서 확인 가능', '01. 혜택최대 15% 강력한 할인 쿠폰팩!', '02. 선착순 타임딜매일 오전 10시 한정수량 타임딜', '05. 카드 혜택매일매일 카드 청구 할인', '우리 아이를 가장 잘 아는 공간 Little SSG 유아동의 모든것 총집합 #핫딜 #타임딜 #생생리뷰 #테마랭킹']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2030 부산세계박람회 유치 응원이벤트</t>
+          <t>Luxury Gift Week</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>최대 5만원 SSGMONEY 제공</t>
+          <t>선착순 ~15만원 할인 쿠폰 가정의 달 럭셔리 선물</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005077</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005287</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2030 부산세계박람회 응원이벤트</t>
+          <t>Luxury Gift Week</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-03-27</t>
+          <t>2023.04.10</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023.04.16</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 2030 부산세계박람회 응원이벤트', '스마일클럽', '2030 부산세계박람회 응원이벤트']</t>
+          <t>['이벤트/쿠폰 &gt; Luxury Gift Week', '스마일클럽', '선착순 최대15만원 쿠폰', '혜택 플러스 알파 카드 청구할인', '금주의 쇼핑 혜택 최대 15만원 할인쿠폰', '상품쿠폰 8% - 30만원 이상 구매 시, 최대 15만원 할인(매일 선착순 8천명)', '오늘의 쿠폰은 마감되었습니다.', '럭셔리 기프트 위크, 단 7일! 최대 15만원 할인 쿠폰, 쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요!', '오전 09시부터 쿠폰 발급이 시작됩니다.', '쿠폰 발급 및 사용기간: 4월 10일 (월) 09:00 - 4월 16일 (일) 23:59', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰 대상 상품은 상품 상세 배너를 확인 부탁드립니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '4월 12일 저녁 8시 COMING SOON, 여름 명품 미리 준비, 방송 중 골든구스/마르지엘라/키츠네 등71%', '혜택에 혜택을 더해요 오늘의 카드 청구할인', 'KB 8만원 이상 5% 청구할인 (일 5만원 한) 2023.04.10', '[SSGPAY전용] SSG.COM삼성 8만원 이상 7% 청구할인 (일 5만원 한) 2023.04.10', '[SSGPAY전용] 삼성 8만원이상 5% 청구할인 (일 5만원 한) 2023.04.11 - 12', 'KB 8만원이상 5%청구할인 (일 5만원 한) 2023.04.13', '[SSGPAY전용] 하나카드 8만원 이상 7% 특정카드 할인 (5만원 한) 2023.04.14']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>신세계 골프대전</t>
+          <t>Molly’s SSG 스프링 위크</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>연중 최대 백화점 골프 행사를 만나보세요</t>
+          <t>~15% 장바구니 쿠폰 + SSG머니 5천원 페이백!</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004939</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005103</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>신세계 골프페어</t>
+          <t>Molly's SSG 스프링 위크</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023.04.10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023.04.16</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신세계 골프페어', '스마일클럽', '스페셜 쿠폰 10% 바로보기', '스페셜 쿠폰 10% 혜택', '      쿠폰 발급 및 사용 기간', '      쿠폰 발급은 당사 사정에 따라 선착순 조기 마감될 수 있습니다.', '      쿠폰 발급 대상', '      경품 응모 대상금액은 백화점 상품 실 구매금액 기준 (상품할인쿠폰/에누리 및 배송비 제외)으로 적용됩니다. ', '제이린드버그 50만원 이상 구매시 썬패치 증정', '나이키골프 인기 ITEM SSG 단독 40%OFF', 'WAAC 23 S/S 단독 10%할인 특가', '제이미웨스트 최대 70% 할인 (골프 가방, ACC 외)', '게리앤프레키 최대 50% 할인 및 구매 고객 대상 사은품 증정', 'LYF 23SS 신상품 최대 15%, 이월 최대 30% 할인 및 사은품 증정', '쿠폰은 오전 9시에 오픈됩니다:)', '쿠폰이 마감되었습니다!']</t>
+          <t>["이벤트/쿠폰 &gt; Molly's SSG 스프링 위크", '스마일클럽', '~15% 쿠폰', '~15% 쿠폰까지!', '~15% 장바구니 쿠폰', '선착순  1천명', '장바구니쿠폰', '%', '3만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 사용 기간: 발급 시점 ~ 2023년 4월 16일 (일) 23 : 59', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '이벤트 응모대상 :  반려 카테고리 상품을 5만원 이상 구매하신 고객님 (배송비/쿠폰, 즉시할인 등의 할인금액 제외)', "이벤트 참여 후 'MY SSG &gt; 자주찾는 메뉴 &gt; 이벤트현황'에서 참여 여부 확인이 가능합니다.", '[펫스프링위크] 캐나다 펫큐리언 now/go! 사료 20%', '[펫스프링위크] 힐스 사이언스 강아지 사료 10% 행사가+ 10% 추가 할인!', '[펫스프링위크] 네츄럴코어 강아지 사료/간식 ~20% 할인', '[펫스프링위크] 로얄캐닌 강아지 사료 추가 4%', '[브랜바인] 미국 수의사 개발, 직구 반려동물 영양제 브랜바인 고양이 호흡기 영양제1+1外 ~25%', '[펫스프링위크] 요요쉬 外 강아지 배변패드 ~25% 할인!', '[펫스프링위크] 강아지 밀리옹 이동가방/카시트 ~20% 할인!', '[펫스프링위크] 바잇미 장난감 30% &amp; 1+1 까지', '[펫스프링위크] ★펫토리아 인기 상품 5% 추가할인!', '[펫스프링위크] 로얄테일즈 강아지 유모차 10% 할인! (로그인쿠폰)', '[펫스프링위크] 낫쏘빅 강아지 유모차 3~7% 즉시할인! (로그인쿠폰)', '[펫스프링위크] 프로베스트 고양이 사료/캔 최대 30%', '[펫스프링위크] 오리젠 캣 사료 20%', '[펫스프링위크] 로얄캐닌 고양이 건식사료 5%할인+사은품증정', '[펫스프링위크] 우다다냥이 이나바 챠오츄르 행사 가격할인적용', '[펫스프링위크] 기호성과 가성비 캐츠랑 17kg 출시! 전라인업 재고확보~15%', '[펫스프링위크] MD추천! 경제적이고 응고력 좋은 두부모래 ~7%_빠른출고', '[펫스프링위크] 일룸 캣타워 7%쿠폰 외 펫가구딜 (모넬로/뽀떼/헬로망치)', '[펫스프링위크] 한국고양이모래연구소 미스터리 두부모래 5% 행사', '[펫스프링위크] [LG유니참] 데오토일렛 모래/패드/탈취제 ~19%', '10% 쿠폰', '[펫스프링위크] 포켄스 간식 10% 로그인쿠폰', '~30%  할인', '[펫스프링위크] 생활공작소 펫 필수템 ~30% 행사가 (15,000원 이상 무료배송)', '~25%  할인', '[직구] 몰리쓱 스프링위크 SSG 단독X브랜바인 고양이 호흡기 1+1, 유산균 외 필수 영양제 ~25%', '단독 할인', '더리얼/밥이보약 최대 30% 할인', 'SSG 단독 15% 할인', '로그인 시 10% 특별할인', '미국 수의사개발 영양제 ~25%OFF', 'ANF/프로베스트/이즈칸 ~20%', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>첫 구매 고객 해피반값쿠폰</t>
+          <t>백화점 선물하기 SPRING GIFT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
+          <t>나들이 필수템 GIFT 준비는 백화점 선물하기로!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000004845</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005258</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
+          <t>신세계백화점 SPRING GIFT</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023.04.03</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피반값쿠폰] 3월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피반값쿠폰', '해피반값쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 3월 20일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 8,000원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 3월 20일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만 5천원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 신세계백화점 SPRING GIFT', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>최대 10.2만원 혜택</t>
+          <t>첫 구매는 50% 할인에 무료배송</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t xml:space="preserve">아이스크림 취향대로 골라담기 </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005406</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>첫 구매는 아이스크림 반값에 무료배송</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2023.04.08</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023.04.16</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 10.2만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 5.2만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 5.2만원 할인', '      직전 6개월간 (2022년 9월 1일 부터 2023년 2월 28일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 5만 3천원 이상 첫 결제 시 5.2만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.08.01~2023.01.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 5만 3천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; 첫 구매는 아이스크림 반값에 무료배송', '스마일클럽', '첫 구매는 아이스크림 반값에 무료배송', '최근 1년간 쓱배송이 처음이라면, 아이스크림 반 값에 무료배송', '쓱배송/새벽배송 무료배송 1장', '아이스크림 할인 쿠폰 50%, 최대할인금액 1만원 (1장), 5천원 (2장)', '웰컴 쿠폰으로', '쓱배송의 시간대 지정 서비스를 통해 ', '따끈따끈한 피코크 신상품을 한번에 ※할인가는 최대 1만원 할인쿠폰 적용 기준', '(50%, 무료배송) 장바구니 담기 &gt; 하겐다즈 커피 아이스크림 파인트 할인전 : 15,500원 할인후 : 7,750원', ' 상하목장 유기농 밀크, 기존가 9,450원, 할인가 4,725원 ', ' 나뚜루 녹차 파인트, 기존가 9,840원, 할인가 4,920원 ', ' 서울우유 딸기우유 아이스크림 474ml, 기존가 9,900원, 할인가 4,950원 ', ' 피코크 욜로우 초코, 기존가 5,980원, 할인가 2,990원 ', '(50%, 무료배송) 장바구니 담기&gt; 빙그레 수퍼콘 바닐라쿠앤크 혼합 할인전 : 6,500원 할인후 : 3,250원', ' 하겐다즈 그린티 아몬드 멀티바, 기존가 15,500원, 할인가 7,750 원 ', ' 롯데 월드콘 초코멀티, 기존가 6,280원, 할인가 3,140원 ', ' 롯데 셀렉션 아이스크림, 기존가 6,280원, 할인가 3,140원 ', ' 해태 부라보콘 화이트바닐라, 기존가 6,280원, 할인가 3,140원 ', '(50%, 무료배송) 장바구니 담기&gt; 빙그레 더 엑셀런트 오리지널 할인전 : 8,280원 할인후 : 4,140원', ' 롯데 티코 딸기, 기존가 6,280원, 할인가 3,140원 ', ' 롯데 빠삐코, 기존가 4,980원, 할인가 2,490원 ', ' 롯데 조안나바, 기존가 6,280원, 할인가 3,140원 ', ' 빙그레 떡붕어싸만코, 기존가 6,000원, 할인가 3,000원 ', '할인 상품 한눈에 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
+          <t>2023 대한민국 수산대전 4월특별전</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005323</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+          <t>(4/6~19) 2023 대한민국 수산대전 - 4월특별전</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2023.04.06</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2023.04.19</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 5천원 이상 결제 시 사용 가능한 5만원 할인쿠폰 제공', '50,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.03.01 ~ 2023.03.31', '쿠폰 사용기간 : 2023.03.01 ~ 2023.03.31', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 55,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '03. 스마일클럽 월 이용료 결제 카드로 SSG.COM 삼성카드 등록 시 SSG머니 3,900원 적립', '행사기간 동안 SSG.COM 삼성카드를 통해 스마일클럽 자동 가입 시 SSG머니 3,900원 즉시 적립', '적립시점까지 스마일클럽 월 이용료 정기결제 수단에 SSG.COM 삼성카드를 등록해야 혜택을 받을 수 있습니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (4/6~19) 2023 대한민국 수산대전 - 4월특별전', '스마일클럽', '장바구니쿠폰', '%', '여러 개 담으시고 최대 1만원 할인 받으세요', '쓱배송 상품 더 보기']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>크리니크 3/30(목) 8PM</t>
+          <t>호주로 떠나는 미식여행</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>치크팝 단독특가 &amp; 마스카라/수분크림 대용량 1+1 기획</t>
+          <t>최대 40% 할인과 시드니 항공권 증정 이벤트</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005157&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005457</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>크리니크 @SSG.LIVE 3/30(목) 20:00PM</t>
+          <t>호주로 떠나는 미식여행</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-03-22</t>
+          <t>2023.04.13</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-03-30</t>
+          <t>2023.04.26</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 크리니크 @SSG.LIVE 3/30(목) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 호주로 떠나는 미식여행', '스마일클럽', '와규 꽃갈비살 구이 (30%할인)정상가 38,600원&gt;할인가 27,020원', 'The 담백한 생연어회 필렛 (20%할인)정상가 26,800원&gt;할인가 21,440원', '[분다버그] 핑크자몽 (10%할인)정상가 17,490원&gt;할인가 15,741원', '호주 왕복 항공권 증정 이벤트', '이벤트 기간 동안 호주산 식재료 구매 금액이 가장 큰 ', '이벤트 기간2023년 4월 13일(목) ~ 26일(수)', '이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다.', '이벤트 참여를 위해 작성한 정보가 부정확할 경우 당첨이 취소될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>그랜드조선부산 X 또떠남</t>
+          <t>SPRING BEAUTY FESTA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>해운대 오션뷰 객실 단독특가 + 청구혜택까지</t>
+          <t>럭셔리&amp;트렌드 뷰티 ~15% 쿠폰 SSG머니 응모 혜택</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005135</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005387</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>그랜드 조선 부산 X SSG.COM X 또떠남</t>
+          <t>[먼데이문] SPRING BEAUTY FESTA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023.04.10</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-04-02</t>
+          <t>2023.04.16</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 그랜드 조선 부산 X SSG.COM X 또떠남', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; [먼데이문] SPRING BEAUTY FESTA', '스마일클럽', '뷰티~15% 쿠폰', '봄맞이 뷰티 ~15% 쿠폰', '선착순4만장', '상품쿠폰', '%', '럭셔리뷰티 ~10% 상품쿠폰', '4만원 이상 상품 구매시 최대 1만원 할인', '선착순3만장', '트렌드뷰티 ~5% 상품쿠폰', '2만원 이상 상품 구매시 최대 5천원 할인', '발급 수량 : 럭셔리뷰티 10% 상품쿠폰 - 선착순 4만장, 트렌드뷰티 5% 상품쿠폰 - 선착순 3만장', '10% 상품쿠폰은 신세계백화점몰, 시코르몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용 됩니다.', '5% 상품쿠폰은 신세계몰, 이마트몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용됩니다. ', '트렌드뷰티 대표 브랜드 상품 15% 상품쿠폰', ' 본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다. ', '15% 쿠폰&amp;다다익선 더블혜택', '최대50%할인 + 대용량기획', '비건 선케어 45% &amp;BEST 상품전', '프로페셔널 스칼프 솔루션 10% 할인&amp;두피 세럼 증정', '차앤박 SUN 넘는 특가 ~47% (+호텔 숙박권 포토 후기 이벤트)', '광채&amp;탄력&amp;미백 트리플케어! 슈퍼세럼30ML 20% + BEST ~57%', '[먼데이문위크] 웰라 프리미엄 살롱 헤어케어 / SP 라인 [1+1 ]+ 추가 할인/ 최대 70% 할인 + 먼데이문 추가 쿠폰 [샴푸/컨디셔너/트리트먼트/헤어오일]', '봄맞이 메이크업 최대 30% OFF', '단4일, 최대 20%할인 및 최대구성! 놓치지마세요', '랩 시리즈 맥스 듀오 구매시, 15만원 상당 사은품 &amp; 파우치 증정', 'SSG 단독 기획 세트+구매 사은 이벤트', '[10% 쿠폰]미스트,클렌징,로션 외 최대 ~62%+SSG 단독 증정', '장영란 NEW 모공선크림 외 모공/기미케어 BEST ~71%OFF', '[우르오스 스프링위크] 피부보습 한통에 다 담다! BEST 최대15% 할인♥', '[문상민 PICK! 아임프롬] 봄맞이 케어 대전 ~40% + 전구매사은품', '베스트 전품목 할인+무료배송 (블러워터틴트,멀티아이팔레트,페이스블러쉬,소프트매트립,뉴테이크 외)', '[삐아&amp;어바웃톤] 먼데이문위크 최대 44% 할인', '[UP TO 60%] 바이탈뷰티 특집전!', '4월 먼데이문 UP TO 56% + 15%추가 할인쿠폰', '매끈매끈 제모준비해 봄,제모기 최대 40% 할인', '★1년에 단 2번★ 지아자/크나이프 상반기 빅세일! UP TO 80%~', '★단독★ THANN 더블 할인 혜택', '당첨 조건 및 당첨 인원 : 이벤트 기간 내 뷰티 1만원 이상 구매 후 응모한 고객  중 500명 추첨 후 SSG머니 2,000원 지급', '해당 조건 1만원 이상 구매 후 이벤트페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한하여 당첨자 추첨 후 해당 ID로 적립됩니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>브랜드 스포트라이트 X 트라이온: 롱샴</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SSG 단독 최대 10% 할인 혜택!</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005333</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>SSG 브랜드 스포트라이트 x 트라이온 - 롱샴</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023.04.10</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023.04.16</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 롱샴', '스마일클럽', 'SSG 단독 롱샴 BEST 상품 최대 10% 할인 혜택(위 상품들 중 에퓌르 버킷백 화이트, 브라운 포함 일부 상품)']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>현실육아 참견라이브 with 정주리</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>정주리와 육아전쟁 사진 공유하고 상품권 5만원 찬스!</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005425</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>[현실육아 참견라이브] 사전 이벤트</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023.04.10</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023.04.16</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [현실육아 참견라이브] 사전 이벤트', '스마일클럽', '[현실육아 참견라이브] 사전 이벤트', '라이브 알림신청 이벤트', '육아전쟁 이미지 댓글 이벤트', '경품 발송을 위해 고객정보가 이벤트 진해애 대행업체에 제공되며, 경품 증정 후 즉시 파기합니다.(개인정보 위탁업체: 젤라블루 / 제공범위: 성명, 휴대전화 번호, 주소)', '본 이벤트에 대한 세부사항은 그룹사 사정에 따라 임의로 변경, 조기 종료될 수 있습니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>첫구매 고객 최대 99% 할인 쿠폰 증정</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005244</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>[해피99쿠폰] 4월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023.04.11</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2023.04.23</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [해피99쿠폰] 4월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피99쿠폰] 4월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피99쿠폰', '신세계몰, 신세계백화점몰 최대 99% 할인 쇼핑 찬스', '해피99쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 4월 11일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 9,900원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 4월 11일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>최대 8만원 혜택</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022.07.08</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023.06.28</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 10월 1일 부터 2023년 3월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.10.01~2023.03.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '3. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022.10.26</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025.10.25</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>LG시네빔 4/13(목) 7PM</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>오직 방송중에만! 23년 신제품 런칭 &amp; 역대급 사은품 증정 혜택</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005437&amp;domainSiteNo=6005</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>LG전자 시네빔 @SSG.LIVE 4/13(목) 19:00PM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023.04.05</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2023.04.13</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; LG전자 시네빔 @SSG.LIVE 4/13(목) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>라테라스 여수 4/13(목) 8PM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>여수라테라스&amp;워터파크 혜택가득 풀캉쓱! 최대 69% 할인!</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005430&amp;siteNo=6005</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>라테라스 여수 @SSG.LIVE 4/13(목) 8PM</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023.04.04</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2023.04.13</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 라테라스 여수 @SSG.LIVE 4/13(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Apr 20 00:18:36 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,185 +473,185 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>오늘은 장보는 날, 쓱배송데이</t>
+          <t>푸드 쓱세일</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>오늘 단 하루! 00시/오전/오후 10%쿠폰 선착순 발급</t>
+          <t>오늘이 마지막! 쿠폰 2장 + 타임딜/초특가</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005473</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005336</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>오늘은 장보는 날, 쓱배송데이</t>
+          <t>푸드쓱세일</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023.04.13</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023.04.13</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 오늘은 장보는 날, 쓱배송데이', '스마일클럽', '오늘은 장보는 날, 쓱배송데이', '오늘은 장보는날 쓱배송 DAY', '10% 선착순 쿠폰! 오늘 단 하루 00시/09시/14시 딱 3번의 기회', '선착순 10%쿠폰 바로보기', '추가 5% 카드혜택 바로보기', '최대 50% 특가 상품 바로보기', '10% 장바구니 쿠폰', '00시 쿠폰', '00시 오픈, 선착순 2만명 장바구니 10% 쿠폰 : 7만원 이상 결제시 최대 1만원 할인', '오전 9시 쿠폰', '           이마트몰/새벽배송몰/트레이더스몰 상품 대상 (이마트/트레이더스 쓱배송 및 점포택배, 새벽배송, 택배배송상품)', '오전 9시 오픈, 선착순 2만명 장바구니 10% 쿠폰 : 7만원 이상 결제시 최대 1만원 할인', '오후 2시 쿠폰', '오후 2시 오픈, 선착순 2만명 장바구니 10% 쿠폰 : 7만원 이상 결제시 최대 1만원 할인', '쓱배송, 새벽배송, 트레이더스쓱배송 및 점포택배 상품 대상', '        쿠폰 발급 및 사용 기간', '       쿠폰 발급 기간', '       쿠폰 사용 조건', '       대상상품 : 이마트/트레이더스 쓱배송 및 점포택배, 새벽배송상품 대상', '       쿠폰 발급 대상', '       발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '최대 5% 결제할 때 한 번 더 추가 할인', '청구할인 카드혜택', 'KB 국민카드 8만원 이상 5% 청구할인 (일 5만원 한도) 자세히보기', 'KB 국민카드 8만원 이상 5% 청구할인 (일 5만원 한도)', '최대 50%할인, 1+1 쓱배송 대표상품']</t>
+          <t>['이벤트/쿠폰 &gt; 푸드쓱세일', '스마일클럽', '할인쿠폰 매일 최대 2장 + 타임딜/오늘의초특가', '할인 쿠폰 바로보기', '선착순 타임딜 바로보기', '매일 1장, 선착순 9만명! 푸드 10% 장바구니쿠폰', '이마트몰/트레이더스몰/새벽배송몰 쓱배송/새벽배송/택배배송 전체 카테고리 상품', '오전 0시 쿠폰 선착순 2만명', '장바구니 쿠폰 10% 6만원 이상 구매 시 최대 1만원 할인 쿠폰받기', '오전 9시 쿠폰 선착순 2만명', '오후 2시 쿠폰 선착순 2만명', '쿠폰 발급 기간 : 2023년 4월 17일(월) 부터 4월 20일(목) 까지', 'ID당 1일 1장, 오전0시/오전9시/오후2시 쿠폰 중 1매만 다운 가능(기간중 최대 4장까지 발급 가능)', '쿠폰 사용 기간 : 쿠폰 발급받은 당일 한정 사용 가능', '      쿠폰 발급 기간', '      2023년 4월 17일(월) ~ 4월 20일(목) ID당 1일 1장, 오전0시/오전9시/오후2시 쿠폰 중 1매만 다운 가능 (기간 중 최대 4장까지 발급 가능)', '      쿠폰 사용 기간', '      쿠폰 발급받은 당일 한정 사용 가능', '      이마트몰/새벽배송몰/트레이더스몰 전체 카테고리 상품(이마트/트레이더스 쓱배송, 새벽배송, 택배배송상품) * 현금성/무형서비스/초특가 상품, 명품/가전 카테고리 상품 등 일부 제외', '      쿠폰 발급 대상', '      발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '매일 1장, 선착순 10만명! 푸드 15% 상품쿠폰', '상품 쿠폰 15% 오늘의 초특가 상품 50개 최대 3천원 할인 (일부상품 제외) 쿠폰받기', '쿠폰 발급 기간 : 2023년 4월 17일~4월 20일', '      푸드쓱세일 오늘의핫딜 상품 50개 *일부상품 제외 쿠폰 1장당 대상상품 1개 수량에 한정하여 15% 할인 적용, 최대 3천원 할인', '쓱배송', '15% 상품쿠폰 적용 오늘의 핫딜 더 보러가기', '선착순 타임딜', '오전 9시 타임딜, 오후 2시 타임딜', '타임딜 스캐쥴', '피코크 피코크 신상품부터 할인행사까지 다양하게 만나기', 'CJ 햇반/비비고 대표상품 ~50%할인', '대상 김치/간편식/조미료등 최대 50%할인', "'이날 아무때나' 쓱배송 선택 시 다음 장보기 배송비 지원! 배송비 반값", "'이날 아무때나' 쓱배송 선택 시 SSG MONEY 적립 1,500원", "응모가 완료되었다고 해도, 실제 '이날 아무때나' 선택하여 쓱배송 주문하지 않았다면 응모가 취소됩니다.", '최종 &lt;응모하기&gt; 버튼 완료 후 결제취소 하셨더라도, 이벤트 마감 전까지 다시 응모조건을 충족해주시면 정상적으로 SSG MONEY 지급 대상에 포함됩니다.', '&lt;응모하기&gt; 버튼을 클릭하여 신청한 후에도, 주문 취소 및 단순반품 등으로 인해 응모조건을 충족하지 못 하는 경우 SSG MONEY 지급대상에 포함되지 않습니다.', "1. 쓱배송 상품을 장바구니에 담고 배송시간 선택 시, '이날 아무때나'를 선택해주세요.", '      이벤트 기간', '      SSG MONEY 적립 예정일', '최대 50% 할인 푸드쓱세일에는 한우데이 보러가기', '최대 00만원! 결제할 때 한 번 더 쏠쏠한 추가 할인 청구할인 카드혜택', 'SSGPAY-신한카드 SSGPAY 전용 7만원 이상 5% 청구할인 (일 5만원 한도)', 'SSGPAY-비씨카드 SSGPAY 전용 7만원 이상 5% 청구할인 (일 5만원 한도)', 'SSG.COM카드 Edition1 &amp; Edition2 SSGPAY 전용 7만원 이상 8% 청구할인 (일 5만원 한도)', '카카오페이-KB국민카드 카카오페이 전용 7만원 이상 5% 청구할인 (일 5만원 한도)', 'SSGPAY-삼성카드 SSGPAY 전용 7만원 이상 5% 청구할인 (일 5만원 한도)']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SPRING FESTIVAL</t>
+          <t>유아동 쓱세일 어린이날 선물대전</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>누구나 최대 10% 할인쿠폰 + 봄나들이 필수 아이템</t>
+          <t>최대 15% 쿠폰 + 엄마아빠 사주세요</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005376</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005087</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SPRING FESTIVAL : 나들이 쇼핑위크</t>
+          <t>유아동 쓱세일</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023.04.10</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SPRING FESTIVAL : 나들이 쇼핑위크', '스마일클럽', '누구나 최대 10% 할인 쿠폰 봄나들이 필수 상품&amp;브랜드', '최대 10% 쿠폰 바로보기', '누구나 최대 10% 할인 피크닉 전용 선착순 쿠폰', '장바구니 쿠폰 10% - 8만원 이상 구매시 최대 1만원 할인(매일 오전 9시, 선착순 1만장)', '장바구니 쿠폰 10% - 8만원 이상 구매시 최대 1만원 할인(매일 오전 9시, 선착순 15,000장)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 발급 받기(기간 내 ID당 1회 발급)', '      쿠폰 발급 기간', '      23/04/10(월) ~ 23/04/16(일), 매일 오전 9시부터 선착순 발급', '      쿠폰 사용 기간', '쿠폰은 매일 선착순 1만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '본 쿠폰은 신세계몰, 신세계백화점 특정 카테고리 상품에 적용되는 카테고리 쿠폰입니다.', '할인액 및 배송비 제외한 금액 기준으로 쿠폰이 적용됩니다.', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '쿠폰은 매일 선착순 15,000장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '프레드페리 - 브랜드데이 15% 혜택 보러가기', '올리브데올리브 - SSG 단독 신상+이월 SPRING SALE 60% 할인 보러가기', '나이키 - 4월 정기세일 UP TO 48% 할인 보러가기', '레페토 - 명품/잡화 봄맞이 베스트 브랜드 연합전 12% 할인 보러가기', '랑콜 - 봄철 피부 관리, 랑콤 UV 정품용량 증정 15% 할인 보러가기', '크록스 - 23 S/S 봄맞이 인기 크록스 대량 입고 80% 할인 보러가기', '룰루레몬 - Spring Favourites 신제품 기획전 SSG 머니 5% 적립 보러가기', '캉골키즈 - SSG 단독 상품 입고 10% 할인 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일', '스마일클럽', '1천여종 완구/패션/유아동 용품 다 모였다! 어린이날 BIG 혜택 15% 최대 2만원 쿠폰+선물 가이드', '유아동 쿠폰 바로보기', '선착순 타임딜 바로보기', '유아동 쓱세일 X4 상품쿠폰 15% 2만원 이상 구매 시, 최대 1만원 할인 10만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기', '쿠폰 받기 클릭 시 총 4장 발급 (ID당 기간 내 1회)', '쿠폰 적용 대상 : 유아동 쓱세일 로고를 확인하세요', '       쿠폰 발급 및 사용 기간', '       쿠폰 적용 방법', '       쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '15% 쿠폰 적용가능 상품은 검색해서 쉽게 볼 수 있어요!', '쿠폰은 대상 상품 상세 페이지에서 편리하게 다운 가능해요!', '상품쿠폰 7% X2 3만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기 클릭 시 총 2장 발급 (ID당 기간 내 1회) ', '      쿠폰 발급 및 사용 기간', '      쿠폰 적용 방법', '      본 쿠폰은 신세계백화점몰 유아동 카테고리 상품에 한하여 적용 가능합니다.', '      쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '장바구니 쿠폰 7% 선착순 쿠폰 7만원 이상 구매 시, 최대 2만원 할인', '장바구니 쿠폰 12% 첫 구매 전용, 유아동 전용, 일별 선착순 1만명 5만원 이상 구매 시, 최대 2만원 할인', '혜택의 마무리 카드 청구 할인', '삼성카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] 7만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '삼성카드 [SSGPAY전용] 7만원 이상 결제 시 5% 청구할인 (일 5만원 한)', '신한카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 10% 청구할인 (일 5만원 한)', 'KB국민카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '매일 오전 10시! 오늘의 선착순 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '타임딜 스캐쥴', '(최대 15%) 남양유업 : 분유 특가 맘키즈 할인+추가 쿠폰', '(최대 35%) 또봇/메카드볼 : 인기 남아완구 특가', '(최대 66%) 네파키즈 : 23 S/S 신상품 반팔세트 등', '(최대 50%) 플레이도 : 인기 상품 원데이 특가', '(최대 15%) 베베숲 : No.1 스테디셀러 물티슈 단 하루 특가', '(쿠폰) H&amp;M : 봄 시즌오프 + 추가 쿠폰', '(최대 10%) 라코스테 : 인기의류 라코스테 키즈 PK 할인', '(최대 18%) 브라이텍스 : 브라이텍스 BEST 쉿! ONLY SSG 단독', '(최대 15%) 하기스 기저귀 : No.1 유한킴벌리 육아 필수품', '(최대 51%) 쁘띠엘린 : 원데이 특가 립프로그 등 인기 특가', '(최대 59%) 휠라키즈 : 23 S/S 신상입고! 신발, 의류 특가', '킨도 : 킨도 기저귀 할인부터 쿠폰까지', '압타밀 : 핫딜 도전 독일 BEST 분유 압타밀', 'S/S 슈즈 ~40% 할인', 'S/S 슈즈 ~40% 할인 상품 더 보러가기', '쿠폰 또는 적립금 혜택까지 실속있게 챙겨가세요 구매 시 쿠폰, 적립 금액을 확인하세요', '              하기스 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 라이브 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 완구 선물 라이브 : 어린이날 기념 SSG단독 완구 최대 49% 특가 및 사은품, 핫딜까지!', '              레고 : [이상훈의 레고네고] 역대급 핫딜/사은품 혜택', '              파크론 : 파크론/아소방 최대 61% 할인 + 쓱라이브 단독사은!', '              탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '          탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '혼자만 알기 아까운 유아동 쓱세일 #쿠폰 받고 같이 쇼핑해요! #오늘의 타임딜, 특가 사고 싶은게 너무 많아! 공유하기']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>유아동 쓱세일 COMING SOON</t>
+          <t>유아동 쓱세일 타임딜</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>사전행사 특별 혜택 SSG머니 2천원 놓치지 마세요</t>
+          <t>득템은 선착순! 놓치지 마세요</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005088</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005087#evtAnchor03</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>유아동 쓱세일 COMING SOON</t>
+          <t>유아동 쓱세일</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023.04.13</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일 COMING SOON', '스마일클럽', '4월 17일 역대급 유아동 쇼핑 행사가 찾아옵니다. 사전 이벤트 참여하시고, SSG머니 100% 페이백 챙겨가세요!', '공유하기 - 클릭 하면 자동 이벤트 응모', 'STEP.1 유아동 쓱세일 사전 이벤트 공유하고 위 [공유하기] 버튼 클릭 필수!', '      MY SSG - SSG MONEY에서 확인 가능', '01. 혜택최대 15% 강력한 할인 쿠폰팩!', '02. 선착순 타임딜매일 오전 10시 한정수량 타임딜', '05. 카드 혜택매일매일 카드 청구 할인', '우리 아이를 가장 잘 아는 공간 Little SSG 유아동의 모든것 총집합 #핫딜 #타임딜 #생생리뷰 #테마랭킹']</t>
+          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일', '스마일클럽', '1천여종 완구/패션/유아동 용품 다 모였다! 어린이날 BIG 혜택 15% 최대 2만원 쿠폰+선물 가이드', '유아동 쿠폰 바로보기', '선착순 타임딜 바로보기', '유아동 쓱세일 X4 상품쿠폰 15% 2만원 이상 구매 시, 최대 1만원 할인 10만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기', '쿠폰 받기 클릭 시 총 4장 발급 (ID당 기간 내 1회)', '쿠폰 적용 대상 : 유아동 쓱세일 로고를 확인하세요', '       쿠폰 발급 및 사용 기간', '       쿠폰 적용 방법', '       쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '15% 쿠폰 적용가능 상품은 검색해서 쉽게 볼 수 있어요!', '쿠폰은 대상 상품 상세 페이지에서 편리하게 다운 가능해요!', '상품쿠폰 7% X2 3만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기 클릭 시 총 2장 발급 (ID당 기간 내 1회) ', '      쿠폰 발급 및 사용 기간', '      쿠폰 적용 방법', '      본 쿠폰은 신세계백화점몰 유아동 카테고리 상품에 한하여 적용 가능합니다.', '      쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '장바구니 쿠폰 7% 선착순 쿠폰 7만원 이상 구매 시, 최대 2만원 할인', '장바구니 쿠폰 12% 첫 구매 전용, 유아동 전용, 일별 선착순 1만명 5만원 이상 구매 시, 최대 2만원 할인', '혜택의 마무리 카드 청구 할인', '삼성카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] 7만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '삼성카드 [SSGPAY전용] 7만원 이상 결제 시 5% 청구할인 (일 5만원 한)', '신한카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 10% 청구할인 (일 5만원 한)', 'KB국민카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '매일 오전 10시! 오늘의 선착순 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '타임딜 스캐쥴', '(최대 15%) 남양유업 : 분유 특가 맘키즈 할인+추가 쿠폰', '(최대 35%) 또봇/메카드볼 : 인기 남아완구 특가', '(최대 66%) 네파키즈 : 23 S/S 신상품 반팔세트 등', '(최대 50%) 플레이도 : 인기 상품 원데이 특가', '(최대 15%) 베베숲 : No.1 스테디셀러 물티슈 단 하루 특가', '(쿠폰) H&amp;M : 봄 시즌오프 + 추가 쿠폰', '(최대 10%) 라코스테 : 인기의류 라코스테 키즈 PK 할인', '(최대 18%) 브라이텍스 : 브라이텍스 BEST 쉿! ONLY SSG 단독', '(최대 15%) 하기스 기저귀 : No.1 유한킴벌리 육아 필수품', '(최대 51%) 쁘띠엘린 : 원데이 특가 립프로그 등 인기 특가', '(최대 59%) 휠라키즈 : 23 S/S 신상입고! 신발, 의류 특가', '킨도 : 킨도 기저귀 할인부터 쿠폰까지', '압타밀 : 핫딜 도전 독일 BEST 분유 압타밀', 'S/S 슈즈 ~40% 할인', 'S/S 슈즈 ~40% 할인 상품 더 보러가기', '쿠폰 또는 적립금 혜택까지 실속있게 챙겨가세요 구매 시 쿠폰, 적립 금액을 확인하세요', '              하기스 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 라이브 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 완구 선물 라이브 : 어린이날 기념 SSG단독 완구 최대 49% 특가 및 사은품, 핫딜까지!', '              레고 : [이상훈의 레고네고] 역대급 핫딜/사은품 혜택', '              파크론 : 파크론/아소방 최대 61% 할인 + 쓱라이브 단독사은!', '              탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '          탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '혼자만 알기 아까운 유아동 쓱세일 #쿠폰 받고 같이 쇼핑해요! #오늘의 타임딜, 특가 사고 싶은게 너무 많아! 공유하기']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Luxury Gift Week</t>
+          <t>유아동 쓱세일 대표 브랜드</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>선착순 ~15만원 할인 쿠폰 가정의 달 럭셔리 선물</t>
+          <t>더 커진 브랜드 혜택 + 인기 상품</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005287</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005087#evtAnchor05</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Luxury Gift Week</t>
+          <t>유아동 쓱세일</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023.04.10</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Luxury Gift Week', '스마일클럽', '선착순 최대15만원 쿠폰', '혜택 플러스 알파 카드 청구할인', '금주의 쇼핑 혜택 최대 15만원 할인쿠폰', '상품쿠폰 8% - 30만원 이상 구매 시, 최대 15만원 할인(매일 선착순 8천명)', '오늘의 쿠폰은 마감되었습니다.', '럭셔리 기프트 위크, 단 7일! 최대 15만원 할인 쿠폰, 쿠폰 대상 상품은 상품상세에서 다음 엠블럼을 확인해주세요!', '오전 09시부터 쿠폰 발급이 시작됩니다.', '쿠폰 발급 및 사용기간: 4월 10일 (월) 09:00 - 4월 16일 (일) 23:59', "쿠폰 발급 후 'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '쿠폰 대상 상품은 상품 상세 배너를 확인 부탁드립니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.', '4월 12일 저녁 8시 COMING SOON, 여름 명품 미리 준비, 방송 중 골든구스/마르지엘라/키츠네 등71%', '혜택에 혜택을 더해요 오늘의 카드 청구할인', 'KB 8만원 이상 5% 청구할인 (일 5만원 한) 2023.04.10', '[SSGPAY전용] SSG.COM삼성 8만원 이상 7% 청구할인 (일 5만원 한) 2023.04.10', '[SSGPAY전용] 삼성 8만원이상 5% 청구할인 (일 5만원 한) 2023.04.11 - 12', 'KB 8만원이상 5%청구할인 (일 5만원 한) 2023.04.13', '[SSGPAY전용] 하나카드 8만원 이상 7% 특정카드 할인 (5만원 한) 2023.04.14']</t>
+          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일', '스마일클럽', '1천여종 완구/패션/유아동 용품 다 모였다! 어린이날 BIG 혜택 15% 최대 2만원 쿠폰+선물 가이드', '유아동 쿠폰 바로보기', '선착순 타임딜 바로보기', '유아동 쓱세일 X4 상품쿠폰 15% 2만원 이상 구매 시, 최대 1만원 할인 10만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기', '쿠폰 받기 클릭 시 총 4장 발급 (ID당 기간 내 1회)', '쿠폰 적용 대상 : 유아동 쓱세일 로고를 확인하세요', '       쿠폰 발급 및 사용 기간', '       쿠폰 적용 방법', '       쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '15% 쿠폰 적용가능 상품은 검색해서 쉽게 볼 수 있어요!', '쿠폰은 대상 상품 상세 페이지에서 편리하게 다운 가능해요!', '상품쿠폰 7% X2 3만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기 클릭 시 총 2장 발급 (ID당 기간 내 1회) ', '      쿠폰 발급 및 사용 기간', '      쿠폰 적용 방법', '      본 쿠폰은 신세계백화점몰 유아동 카테고리 상품에 한하여 적용 가능합니다.', '      쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '장바구니 쿠폰 7% 선착순 쿠폰 7만원 이상 구매 시, 최대 2만원 할인', '장바구니 쿠폰 12% 첫 구매 전용, 유아동 전용, 일별 선착순 1만명 5만원 이상 구매 시, 최대 2만원 할인', '혜택의 마무리 카드 청구 할인', '삼성카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] 7만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '삼성카드 [SSGPAY전용] 7만원 이상 결제 시 5% 청구할인 (일 5만원 한)', '신한카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 10% 청구할인 (일 5만원 한)', 'KB국민카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '매일 오전 10시! 오늘의 선착순 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '타임딜 스캐쥴', '(최대 15%) 남양유업 : 분유 특가 맘키즈 할인+추가 쿠폰', '(최대 35%) 또봇/메카드볼 : 인기 남아완구 특가', '(최대 66%) 네파키즈 : 23 S/S 신상품 반팔세트 등', '(최대 50%) 플레이도 : 인기 상품 원데이 특가', '(최대 15%) 베베숲 : No.1 스테디셀러 물티슈 단 하루 특가', '(쿠폰) H&amp;M : 봄 시즌오프 + 추가 쿠폰', '(최대 10%) 라코스테 : 인기의류 라코스테 키즈 PK 할인', '(최대 18%) 브라이텍스 : 브라이텍스 BEST 쉿! ONLY SSG 단독', '(최대 15%) 하기스 기저귀 : No.1 유한킴벌리 육아 필수품', '(최대 51%) 쁘띠엘린 : 원데이 특가 립프로그 등 인기 특가', '(최대 59%) 휠라키즈 : 23 S/S 신상입고! 신발, 의류 특가', '킨도 : 킨도 기저귀 할인부터 쿠폰까지', '압타밀 : 핫딜 도전 독일 BEST 분유 압타밀', 'S/S 슈즈 ~40% 할인', 'S/S 슈즈 ~40% 할인 상품 더 보러가기', '쿠폰 또는 적립금 혜택까지 실속있게 챙겨가세요 구매 시 쿠폰, 적립 금액을 확인하세요', '              하기스 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 라이브 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 완구 선물 라이브 : 어린이날 기념 SSG단독 완구 최대 49% 특가 및 사은품, 핫딜까지!', '              레고 : [이상훈의 레고네고] 역대급 핫딜/사은품 혜택', '              파크론 : 파크론/아소방 최대 61% 할인 + 쓱라이브 단독사은!', '              탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '          탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '혼자만 알기 아까운 유아동 쓱세일 #쿠폰 받고 같이 쇼핑해요! #오늘의 타임딜, 특가 사고 싶은게 너무 많아! 공유하기']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Molly’s SSG 스프링 위크</t>
+          <t>오늘의 초특가 상품</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>~15% 장바구니 쿠폰 + SSG머니 5천원 페이백!</t>
+          <t>푸드 쓱세일 15% 추가할인</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005103</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005596</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Molly's SSG 스프링 위크</t>
+          <t>푸드 쓱세일 초특가 상품 15% 할인</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023.04.10</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>["이벤트/쿠폰 &gt; Molly's SSG 스프링 위크", '스마일클럽', '~15% 쿠폰', '~15% 쿠폰까지!', '~15% 장바구니 쿠폰', '선착순  1천명', '장바구니쿠폰', '%', '3만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 사용 기간: 발급 시점 ~ 2023년 4월 16일 (일) 23 : 59', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '이벤트 응모대상 :  반려 카테고리 상품을 5만원 이상 구매하신 고객님 (배송비/쿠폰, 즉시할인 등의 할인금액 제외)', "이벤트 참여 후 'MY SSG &gt; 자주찾는 메뉴 &gt; 이벤트현황'에서 참여 여부 확인이 가능합니다.", '[펫스프링위크] 캐나다 펫큐리언 now/go! 사료 20%', '[펫스프링위크] 힐스 사이언스 강아지 사료 10% 행사가+ 10% 추가 할인!', '[펫스프링위크] 네츄럴코어 강아지 사료/간식 ~20% 할인', '[펫스프링위크] 로얄캐닌 강아지 사료 추가 4%', '[브랜바인] 미국 수의사 개발, 직구 반려동물 영양제 브랜바인 고양이 호흡기 영양제1+1外 ~25%', '[펫스프링위크] 요요쉬 外 강아지 배변패드 ~25% 할인!', '[펫스프링위크] 강아지 밀리옹 이동가방/카시트 ~20% 할인!', '[펫스프링위크] 바잇미 장난감 30% &amp; 1+1 까지', '[펫스프링위크] ★펫토리아 인기 상품 5% 추가할인!', '[펫스프링위크] 로얄테일즈 강아지 유모차 10% 할인! (로그인쿠폰)', '[펫스프링위크] 낫쏘빅 강아지 유모차 3~7% 즉시할인! (로그인쿠폰)', '[펫스프링위크] 프로베스트 고양이 사료/캔 최대 30%', '[펫스프링위크] 오리젠 캣 사료 20%', '[펫스프링위크] 로얄캐닌 고양이 건식사료 5%할인+사은품증정', '[펫스프링위크] 우다다냥이 이나바 챠오츄르 행사 가격할인적용', '[펫스프링위크] 기호성과 가성비 캐츠랑 17kg 출시! 전라인업 재고확보~15%', '[펫스프링위크] MD추천! 경제적이고 응고력 좋은 두부모래 ~7%_빠른출고', '[펫스프링위크] 일룸 캣타워 7%쿠폰 외 펫가구딜 (모넬로/뽀떼/헬로망치)', '[펫스프링위크] 한국고양이모래연구소 미스터리 두부모래 5% 행사', '[펫스프링위크] [LG유니참] 데오토일렛 모래/패드/탈취제 ~19%', '10% 쿠폰', '[펫스프링위크] 포켄스 간식 10% 로그인쿠폰', '~30%  할인', '[펫스프링위크] 생활공작소 펫 필수템 ~30% 행사가 (15,000원 이상 무료배송)', '~25%  할인', '[직구] 몰리쓱 스프링위크 SSG 단독X브랜바인 고양이 호흡기 1+1, 유산균 외 필수 영양제 ~25%', '단독 할인', '더리얼/밥이보약 최대 30% 할인', 'SSG 단독 15% 할인', '로그인 시 10% 특별할인', '미국 수의사개발 영양제 ~25%OFF', 'ANF/프로베스트/이즈칸 ~20%', '조건에 맞는 회원님의 이벤트 신청 가능 내역을 조회합니다.', '이벤트 신청 가능 내역', 'SSG MONEY 5000원']</t>
+          <t>['이벤트/쿠폰 &gt; 푸드 쓱세일 초특가 상품 15% 할인', '스마일클럽', '푸드 쓱세일 초특가 상품 15% 할인', '푸드 쓱세일 BEST 상품 15% 추가할인', '상품 상세 페이지에서 오늘의 쿠폰 받으세요', '푸드 15% 상품쿠폰', '쿠폰 적용 대상 : 오늘의 초특가 상품 (일부상품 제외)', '쿠폰이 모두 소진되었습니다. 내일 오전0시를 기대해주세요!', '쿠폰이 모두 소진되었습니다. 많음 참여에 감사드립니다', '* 쿠폰 발급 기간 : 2023년 4월 17일(월) ~ 4월 20일(목)', '* 쿠폰 사용 기간 : 쿠폰 발급 받은 당일 한정 사용 가능', '전시되어 있는 오늘의 초특가 상품 15% 쿠폰 받으세요']</t>
         </is>
       </c>
     </row>
@@ -695,101 +695,101 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>첫 구매는 50% 할인에 무료배송</t>
+          <t>에어서울 국제선 초특가</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">아이스크림 취향대로 골라담기 </t>
+          <t>일본 항공권 5만원대~, 동남아 8만원대부터!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005406</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005477</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>첫 구매는 아이스크림 반값에 무료배송</t>
+          <t>에어서울 국제선 선착순 핫딜 위크</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023.04.08</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 첫 구매는 아이스크림 반값에 무료배송', '스마일클럽', '첫 구매는 아이스크림 반값에 무료배송', '최근 1년간 쓱배송이 처음이라면, 아이스크림 반 값에 무료배송', '쓱배송/새벽배송 무료배송 1장', '아이스크림 할인 쿠폰 50%, 최대할인금액 1만원 (1장), 5천원 (2장)', '웰컴 쿠폰으로', '쓱배송의 시간대 지정 서비스를 통해 ', '따끈따끈한 피코크 신상품을 한번에 ※할인가는 최대 1만원 할인쿠폰 적용 기준', '(50%, 무료배송) 장바구니 담기 &gt; 하겐다즈 커피 아이스크림 파인트 할인전 : 15,500원 할인후 : 7,750원', ' 상하목장 유기농 밀크, 기존가 9,450원, 할인가 4,725원 ', ' 나뚜루 녹차 파인트, 기존가 9,840원, 할인가 4,920원 ', ' 서울우유 딸기우유 아이스크림 474ml, 기존가 9,900원, 할인가 4,950원 ', ' 피코크 욜로우 초코, 기존가 5,980원, 할인가 2,990원 ', '(50%, 무료배송) 장바구니 담기&gt; 빙그레 수퍼콘 바닐라쿠앤크 혼합 할인전 : 6,500원 할인후 : 3,250원', ' 하겐다즈 그린티 아몬드 멀티바, 기존가 15,500원, 할인가 7,750 원 ', ' 롯데 월드콘 초코멀티, 기존가 6,280원, 할인가 3,140원 ', ' 롯데 셀렉션 아이스크림, 기존가 6,280원, 할인가 3,140원 ', ' 해태 부라보콘 화이트바닐라, 기존가 6,280원, 할인가 3,140원 ', '(50%, 무료배송) 장바구니 담기&gt; 빙그레 더 엑셀런트 오리지널 할인전 : 8,280원 할인후 : 4,140원', ' 롯데 티코 딸기, 기존가 6,280원, 할인가 3,140원 ', ' 롯데 빠삐코, 기존가 4,980원, 할인가 2,490원 ', ' 롯데 조안나바, 기존가 6,280원, 할인가 3,140원 ', ' 빙그레 떡붕어싸만코, 기존가 6,000원, 할인가 3,000원 ', '할인 상품 한눈에 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 에어서울 국제선 선착순 핫딜 위크', '스마일클럽', '에어서울 국제선 선착순 핫딜 위크', '~5만원 할인', '7% 쿠폰', '카드 할인', '선착순 한정 수량', '매일 오전 10시, 국제선 편도당 5천원 즉시 할인', '매일 선착순 120개 한정 핫딜', '즉시할인 에어서울 일본 항공권 나리타/오사카/후쿠오카/다카마쓰 최저가 83,900원 ~', '즉시할인 에어서울 일본 항공권 나리타/오사카/후쿠오카/다카마쓰 최저가 55,900원부터', '즉시할인 에어서울 동남아 항공권 보라카이/나트랑/다낭 최저가 89,900원부터', '일본 편도 최저가 60,900원 &gt; 5천원 쿠폰 반영시 55,900원~', '동남아 최저가 94,000원 %gt; 5천원 쿠폰 반영시 89,900원~', '할인 금액70만원 이상 결제시 5만원 / 30만원 이상 결제시 2만원 / 15만원 이상 결제시 1만원 / 5만원 이상 결제시 4천원 할인', "프로모션 내용:  SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 즉시할인 ", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '사용 방법요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  익스피디아 실시간 호텔 전 상품 1원 이상 구매 시 7% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '게이오 플라자 호텔 도쿄 정상가 : 283,140원 &gt; 할인가 : 263,320원', 'sequence MIYASHITA PARK 정상가 : 237,803원 &gt; 할인가 : 221,157원', '스위소텔 난카이 오사카 정상가 : 79,277원 &gt; 할인가 : 73,728원', '남바 오리엔탈 호텔 정상가 : 254,264원 &gt; 할인가 : 236,466원', '이비스 스타일스 오사카 남바 정상가 : 303,717원 &gt; 할인가 : 282,457원', '솔라리아 니시테츠 호텔 후쿠오카 정상가 : 120,000원 &gt; 할인가 : 111,600원', '오리엔탈 호텔 후쿠오카 하카타 스테이션 정상가 : 172,754원 &gt; 할인가 : 142,754원', '삿포로 그랜드 호텔 정상가 : 198,000 &gt; 할인가 : 184,140원', '두짓 타니 괌 리조트 : 421,850원 &gt; 할인가 : 391,850원', '롯데 호텔 괌 : 265,342원 &gt; 할인가 : 246,768원', '호텔 닛코 괌 : 263,380원 &gt; 할인가 : 244,943원', '퍼시픽 아일랜드 클럽 괌 : 304,453원 &gt; 할인가 : 283,141원', '하얏트 리젠시 괌 : 355,366원 &gt; 할인가 : 330,490원', '더 츠바키 타워 : 473,461원 &gt; 할인가 : 443,461원', '하얏트 리젠시 사이판 : 245,199원 &gt; 할인가 : 228,035원', '사이판 월드 리조트 : 438,248원 &gt; 할인가 : 408,248원', '쉐라톤 그란데 수쿰윗, 럭셔리 컬렉션 호텔, 방콕 정상가 : 287,277원 &gt; 할인가 : 287,277원', '더 쇼어 앳 까따타니 - SHA Extra Plus 정상가 : 548,827원 &gt; 할인가 : 518,827원', '빈펄 리조트 &amp; 스파 다낭 정상가 : 450,982원 &gt; 할인가 : 420,982원', '신라모노그램 다낭 정상가 : 228,067원 &gt; 할인가 : 212,102원', '더 리츠칼튼, 밀레니아 싱가포르(SG Clean) 정상가 : 666,808원 &gt; 할인가 : 666,808원', '샹그릴라 호텔, 싱가포르(SG Clean) 정상가 : 351,325원 &gt; 할인가 : 326,732 원', '퓨전 리조트 푸꾸옥 정상가 : 321,210원 &gt; 할인가 : 298,725 원', '퓨전 리조트 깜 라인 정상가 : 334,424원 &gt; 할인가 : 311,014 원', '하얏트 리젠시 와이키키 비치 리조트 &amp; 스파 : 423,295원 &gt; 할인가 : 393,664원', '힐튼 하와이안 빌리지 와이키키 비치 리조트 : 321,455원 &gt; 할인가 : 298,953원', '윈 라스베이거스 : 293,103원 &gt; 할인가 : 272,586원', '더 코스모폴리탄 오브 라스베이거스 : 148,363원 &gt; 할인가 : 137,978원', '풀먼 파리 타워 에펠 : 609,943원 &gt; 할인가 : 579,943원', '시타딘 아파트호텔 생제르망 데 프레 파리 : 517,849원 &gt; 할인가 : 487,849원', '호텔 레지나 : 224,416원 &gt; 할인가 : 208,707원', '마리팀 호텔 프랑크푸르트 : 320,417원 &gt; 할인가 : 297,988원', '서울 신라호텔 정상가 : 506,000원 &gt; 할인가 : 476,000원', '파라다이스시티 정상가 : 352,000원 &gt; 할인가 : 327,360원', '그랜드 조선 제주 정상가 : 351,999원 &gt; 할인가 : 327,359원', '아난티 힐튼 부산 정상가 : 341,000원 &gt; 할인가 : 317,130원', '파라다이스 호텔 부산 정상가 : 278,300원 &gt; 할인가 : 258,819원', '힐튼 경주 정상가 : 272,251원 &gt; 할인가 : 253,193원', '롯데리조트속초 정상가 : 294,000원 &gt; 할인가 : 273,420원', '소노캄 여수 정상가 : 202,364원 &gt; 할인가 : 188,199원', '[SSGPAY전용] 신한카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Ed1&amp;Ed2 7만원 이상 8% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드Ed1&amp;Ed2 7만원 이상 8% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023 대한민국 수산대전 4월특별전</t>
+          <t>[첫구매 이벤트] 반값다딜- 동원 편</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20% 장바구니쿠폰(최대 1만원 할인)</t>
+          <t>첫구매라면, 동원 인기상품 최대 1.6만원 할인 + 무료배송</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005323</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005206&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(4/6~19) 2023 대한민국 수산대전 - 4월특별전</t>
+          <t>[첫구매이벤트] 반값다~딜 - 동원 편</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023.04.06</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023.04.19</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (4/6~19) 2023 대한민국 수산대전 - 4월특별전', '스마일클럽', '장바구니쿠폰', '%', '여러 개 담으시고 최대 1만원 할인 받으세요', '쓱배송 상품 더 보기']</t>
+          <t>['이벤트/쿠폰 &gt; [첫구매이벤트] 반값다~딜 - 동원 편', '스마일클럽', '[첫구매이벤트] 반값다~딜 - 동원 편', 'STEP1 반가운 반값쿠폰팩 받기 바로보기', '최근 1년간 쓱배송이 처음이라면, 동원 상품 50% 할인에 무료배송', '동원 상품쿠폰 50% 4장, 최대 할인 금액 5천원(2장), 3천원(2장), 본 페이지와 하단 기획전에 진열된 상품에 적용 가능', '무료배송 1장, 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 사용 가능', '쿠폰 발급/사용 기간 : 2023년 4월 17일(월) ~2023년 4월 23일(일)', '- 쿠폰 사용 조건 :', '1) 상품할인 쿠폰 :  쓱배송/새벽배송 동원 브랜드 상품 50% 할인. (최대할인금액 각 5천원, 3천원)', '2) 무료배송 쿠폰 :  이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '(50%, 무료배송) 자극적인 짠맛은 줄이고 돈육 본연의 맛은 살린 리챔 오리지널 300gX4 할인전 : 16,800원 할인후 : 11,800원', ' 동원 고추참치 90g*4, 기존가 9,480원, 할인가 4,480원 ', ' 동원 야채참치 90g*4, 기존가 9,480원, 할인가 4,740원 ', ' 리챔 오리지널 340gX4, 기존가 18,800원, 할인가 13,800원 ', ' 동원 을지로골뱅이 300g, 기존가 8,380원, 할인가 4,190원 ', '(50%, 무료배송) 부드러운 한우 사태가 들어가 더욱 깊고 진한 수라 한우소고기죽 287.5g 할인전 : 5,180원 할인후 : 2,590원', ' 수라 완도전복내장죽 287.5g, 기존가 5,180원, 할인가 2,590 원 ', ' 동원 양반 수라 돼지고기 김치찌개, 기존가 6,980원, 할인가 3,490원 ', ' 동원 양반 소고기미역국, 기존가 5,480원, 할인가 2,740원 ', ' 동원 양반 수라 우거지감자탕 460g, 기존가 8,980원, 할인가 4,490원 ', '(50%, 무료배송) 담백한 육즙이 가득 탱글탱글한 비엔나 동원 통그릴 비엔나 300g*2 할인전 : 8,380원 할인후 : 4,190원', ' 동원 그릴리 델리햄 김밥용 150g, 기존가 2,480원, 할인가 1,240원 ', ' 삼각유부초밥 340g, 기존가 5,180원, 할인가 2,590원 ', ' 개성 얇은피 김치만두 400gx2, 기존가 9,800원, 할인가 4,900원 ', ' 감자 물만두 600gx2, 기존가 10,800원, 할인가 5,800원 ']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>호주로 떠나는 미식여행</t>
+          <t>집밥챌린지 - 보양식</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>최대 40% 할인과 시드니 항공권 증정 이벤트</t>
+          <t>나만의 최애 보양식 투표하고 쓱배송으로 보양식 한번에 준비해요!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005457</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005330</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>호주로 떠나는 미식여행</t>
+          <t>(4/20~26) 집밥챌린지_보양식 편</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023.04.13</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -799,145 +799,145 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 호주로 떠나는 미식여행', '스마일클럽', '와규 꽃갈비살 구이 (30%할인)정상가 38,600원&gt;할인가 27,020원', 'The 담백한 생연어회 필렛 (20%할인)정상가 26,800원&gt;할인가 21,440원', '[분다버그] 핑크자몽 (10%할인)정상가 17,490원&gt;할인가 15,741원', '호주 왕복 항공권 증정 이벤트', '이벤트 기간 동안 호주산 식재료 구매 금액이 가장 큰 ', '이벤트 기간2023년 4월 13일(목) ~ 26일(수)', '이벤트에 응모하실 경우 개인 정보 제공에 동의하신 것으로 간주되며, 제공된 정보는 경품 발송 완료 후 즉시 파기합니다.', '이벤트 참여를 위해 작성한 정보가 부정확할 경우 당첨이 취소될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; (4/20~26) 집밥챌린지_보양식 편', '스마일클럽', '보양식 재료부터 손쉬운 간편식품까지 쓱배송으로 준비해요!', '        하단 투표 이벤트도 잊지마세요!', '쓱배송으로 보양식']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SPRING BEAUTY FESTA</t>
+          <t>백화점 캠핑&amp;아웃도어 대전</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>럭셔리&amp;트렌드 뷰티 ~15% 쿠폰 SSG머니 응모 혜택</t>
+          <t>힐링 액티비티 인기 상품전</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005387</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005489</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[먼데이문] SPRING BEAUTY FESTA</t>
+          <t>자연과 함께하는 힐링 액티비티</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023.04.10</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [먼데이문] SPRING BEAUTY FESTA', '스마일클럽', '뷰티~15% 쿠폰', '봄맞이 뷰티 ~15% 쿠폰', '선착순4만장', '상품쿠폰', '%', '럭셔리뷰티 ~10% 상품쿠폰', '4만원 이상 상품 구매시 최대 1만원 할인', '선착순3만장', '트렌드뷰티 ~5% 상품쿠폰', '2만원 이상 상품 구매시 최대 5천원 할인', '발급 수량 : 럭셔리뷰티 10% 상품쿠폰 - 선착순 4만장, 트렌드뷰티 5% 상품쿠폰 - 선착순 3만장', '10% 상품쿠폰은 신세계백화점몰, 시코르몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용 됩니다.', '5% 상품쿠폰은 신세계몰, 이마트몰 뷰티 카테고리 대상으로 적용되며 쿠폰 1장 당 상품 1개에 적용됩니다. ', '트렌드뷰티 대표 브랜드 상품 15% 상품쿠폰', ' 본 쿠폰은 신세계몰, 이마트몰 해당 브랜드 상품에 한하여 적용 가능하며 1장 당 상품 1개에 적용 됩니다. ', '15% 쿠폰&amp;다다익선 더블혜택', '최대50%할인 + 대용량기획', '비건 선케어 45% &amp;BEST 상품전', '프로페셔널 스칼프 솔루션 10% 할인&amp;두피 세럼 증정', '차앤박 SUN 넘는 특가 ~47% (+호텔 숙박권 포토 후기 이벤트)', '광채&amp;탄력&amp;미백 트리플케어! 슈퍼세럼30ML 20% + BEST ~57%', '[먼데이문위크] 웰라 프리미엄 살롱 헤어케어 / SP 라인 [1+1 ]+ 추가 할인/ 최대 70% 할인 + 먼데이문 추가 쿠폰 [샴푸/컨디셔너/트리트먼트/헤어오일]', '봄맞이 메이크업 최대 30% OFF', '단4일, 최대 20%할인 및 최대구성! 놓치지마세요', '랩 시리즈 맥스 듀오 구매시, 15만원 상당 사은품 &amp; 파우치 증정', 'SSG 단독 기획 세트+구매 사은 이벤트', '[10% 쿠폰]미스트,클렌징,로션 외 최대 ~62%+SSG 단독 증정', '장영란 NEW 모공선크림 외 모공/기미케어 BEST ~71%OFF', '[우르오스 스프링위크] 피부보습 한통에 다 담다! BEST 최대15% 할인♥', '[문상민 PICK! 아임프롬] 봄맞이 케어 대전 ~40% + 전구매사은품', '베스트 전품목 할인+무료배송 (블러워터틴트,멀티아이팔레트,페이스블러쉬,소프트매트립,뉴테이크 외)', '[삐아&amp;어바웃톤] 먼데이문위크 최대 44% 할인', '[UP TO 60%] 바이탈뷰티 특집전!', '4월 먼데이문 UP TO 56% + 15%추가 할인쿠폰', '매끈매끈 제모준비해 봄,제모기 최대 40% 할인', '★1년에 단 2번★ 지아자/크나이프 상반기 빅세일! UP TO 80%~', '★단독★ THANN 더블 할인 혜택', '당첨 조건 및 당첨 인원 : 이벤트 기간 내 뷰티 1만원 이상 구매 후 응모한 고객  중 500명 추첨 후 SSG머니 2,000원 지급', '해당 조건 1만원 이상 구매 후 이벤트페이지에서 &lt;응모하기&gt; 버튼을 눌러 신청하신 고객에 한하여 당첨자 추첨 후 해당 ID로 적립됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 자연과 함께하는 힐링 액티비티', '스마일클럽', '10% 쿠폰 혜택 바로보기', '10% 쿠폰 혜택', '      쿠폰 발급 및 사용 기간', '      쿠폰 발급은 당사 사정에 따라 선착순 조기 마감될 수 있습니다.', '      쿠폰 발급 대상', '나이키 4월 정기세일 UP TO 48%', '아디다스 SS신상 &amp; 베스트 스포츠웨어/슈즈 모음전 + 추가즉시할인혜택', '코오롱스포츠 프리미엄 아웃도어 봄 기획전 + 상품별 할인쿠폰 혜택', '반스 스니커즈 UP TP 50% + 추가즉시할인혜택', '쿠폰은 오전 9시에 오픈됩니다:)', '쿠폰이 마감되었습니다!']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>브랜드 스포트라이트 X 트라이온: 롱샴</t>
+          <t>프리미엄 아울렛 위크 : 미리 준비하는 가정의달</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SSG 단독 최대 10% 할인 혜택!</t>
+          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005333</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005557</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 x 트라이온 - 롱샴</t>
+          <t>[0417-0423] 프리미엄 아울렛 위크</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023.04.10</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 x 트라이온 - 롱샴', '스마일클럽', 'SSG 단독 롱샴 BEST 상품 최대 10% 할인 혜택(위 상품들 중 에퓌르 버킷백 화이트, 브라운 포함 일부 상품)']</t>
+          <t>['이벤트/쿠폰 &gt; [0417-0423] 프리미엄 아울렛 위크', '스마일클럽', '쿠폰 혜택 할인쿠폰 최대10%', 'EVENT 03 미리 준비하는 가정의달 - FAMILY WEEK *할인율은 정상가 기준 할인율임', '[키즈패션 - 최대 70% 할인] 유아동 인기 브랜드 총모음 BIG SALE 보러가기', '[리빙 - 최대 50% 할인] 빌레로이앤보흐, 웨지우드 등 특가 + 쿠폰 보러가기', '[스포츠 - 최대 60% 할인] 골프 BEST 특가 모음전 + 쿠폰혜택 보러가기', '[해외명품 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[여성패션 - 최대 70% 할인] BEST 50 &amp; 아울렛 위크 특가 外 보러가기', '[패션슈즈 - 최대 80% 할인] 슈즈잡화쥬얼리 시즌 BEST 특별전 보러가기', '[패션잡화 - 최대 20% 할인] 로우로우 백팩/ 캐리어 신상 물량 입고! 보러가기', '[언더웨어 - 최대 51% 할인] 라페어 브랜드 위크 언더/이제웨어 특가 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/브룩스브라더스 外 보러가기', '[유니섹스 - 최대 79% 할인] 라코스테, 폴햄 등 봄 캐주얼의류 신규입고 보러가기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>현실육아 참견라이브 with 정주리</t>
+          <t>SSG 브랜드 스포트라이트: 영실업</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>정주리와 육아전쟁 사진 공유하고 상품권 5만원 찬스!</t>
+          <t>이번 어린이날 선물로 딱! 또봇 단독 사은품 증정</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005425</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005546</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[현실육아 참견라이브] 사전 이벤트</t>
+          <t>SSG 브랜드 스포트라이트 - 영실업</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023.04.10</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023.04.16</t>
+          <t>2023.04.23</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [현실육아 참견라이브] 사전 이벤트', '스마일클럽', '[현실육아 참견라이브] 사전 이벤트', '라이브 알림신청 이벤트', '육아전쟁 이미지 댓글 이벤트', '경품 발송을 위해 고객정보가 이벤트 진해애 대행업체에 제공되며, 경품 증정 후 즉시 파기합니다.(개인정보 위탁업체: 젤라블루 / 제공범위: 성명, 휴대전화 번호, 주소)', '본 이벤트에 대한 세부사항은 그룹사 사정에 따라 임의로 변경, 조기 종료될 수 있습니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 영실업', '스마일클럽']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>첫구매 고객 최대 99% 할인 쿠폰 증정</t>
+          <t>집에서 즐기는 미쉐린 레스토랑</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>신세계몰, 신세계백화점몰 스페셜 쇼핑 혜택</t>
+          <t>최대 20% 할인에 5천원 페이백</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005244</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005451</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[해피99쿠폰] 4월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택</t>
+          <t>집에서 즐기는 미쉐린 레스토랑</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023.04.11</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -947,14 +947,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [해피99쿠폰] 4월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '스마일클럽', '[해피99쿠폰] 4월 신세계몰/신세계백화점몰 스페셜 쇼핑혜택', '해피99쿠폰', '신세계몰, 신세계백화점몰 최대 99% 할인 쇼핑 찬스', '해피99쿠폰 대상', '2. 신세계몰, 신세계백화점몰 상품 이벤트 직전 1년 이상 미구매 고객 (22년 4월 11일 이후 신세계몰, 신세계백화점몰 구매 이력이 없는 고객)', '(선착순 1만장) 장바구니 쿠폰 9,900원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '해당 쿠폰은 이벤트 대상 고객 선착순 1만명에게 한정수량으로 발급되며, 소진 시 조기 종료됩니다.', '해당 쿠폰은 기간 내 이벤트 직전 1년간(2022년 4월 11일 이후 ~ 발급시점) SSG.COM 신세계몰과 신세계백화점몰 상품 모두에서 구매이력이 없는 고객에게 제공되는 혜택이며 기간 내 1인 1매 발급이 가능합니다.', '해당 쿠폰은 1만원 이상 구매 시 사용 가능하며, 구매 금액은 할인액 및 배송비를 제외한 상품 구매 금액 기준으로 산정됩니다.', 'SSG.COM의 쿠폰은 결제 시 최적 할인에 의해 자동 설정되며, 직접 변경이 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; 집에서 즐기는 미쉐린 레스토랑', '스마일클럽', '# 최대 20% 할인', '생면 파스타 최대 20% 할인 행사', '정상가 9,800원&gt; 할인가 7,840원 (20%할인)', '정상가 8,900원&gt; 할인가 7,120원 (20%할인)', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>최대 8만원 혜택</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -984,7 +984,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 8만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. 횟수 제한 없이 8% 즉시 할인 (대상 상품당, 최대 3만원) 바로보기', '이달의 혜택 02. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. 횟수 제한 없이 8% 즉시할인', 'SSG.COM에서 SSG.COM카드 Edition2로 상품상세 내 [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품 결제 시 (대상 상품당, 최대 3만원 할인)', '현대카드 또는 SSG.COM카드 Edition2 청구할인일에는 진행되지 않습니다.', '8% 즉시할인', '② [카드 혜택가 &gt; SSG.COM카드 Edition2 더보기 &gt; 즉시할인가] 대상상품결제 시 적용 (대상 상품당, 최대 3만원 할인)', '      본 혜택은 SSG.COM카드 Edition2 즉시할인 상품 결제시에만 적용 가능', '      즉시할인 상품 확인 방법 : [상품상세 내 &gt; 카드혜택가 &gt; SSG.COM카드 Edition2 행사 더보기]에서 확인', '      카드혜택가가 노출되지 않는다면 혜택 적용 제외 상품이며, 현대카드 청구할인일에는 본 혜택이 진행되지 않음', '      이벤트 기간 및 혜택 제공 시점에 SSG.COM카드 Edition2를 정상 보유한 회원에 한해 혜택 제공', '이달의 혜택 02. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 10월 1일 부터 2023년 3월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.10.01~2023.03.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '3. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 10월 1일 부터 2023년 3월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.10.01~2023.03.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '3. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
@@ -1021,81 +1021,155 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '최대 5% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LG시네빔 4/13(목) 7PM</t>
+          <t>파크론 4/20(목) 11AM</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>오직 방송중에만! 23년 신제품 런칭 &amp; 역대급 사은품 증정 혜택</t>
+          <t>파크론 부터 아소방까지 라이브 최대 65%할인</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005437&amp;domainSiteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005341&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>LG전자 시네빔 @SSG.LIVE 4/13(목) 19:00PM</t>
+          <t>[유아동특집] 파크론 최대 65%할인 @SSG.LIVE 4/20(목) 11AM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023.04.05</t>
+          <t>2023.03.31</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023.04.13</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; LG전자 시네빔 @SSG.LIVE 4/13(목) 19:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [유아동특집] 파크론 최대 65%할인 @SSG.LIVE 4/20(목) 11AM', '스마일클럽', '[유아동특집] 파크론 최대 65%할인 @SSG.LIVE 4/20(목) 11AM']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>라테라스 여수 4/13(목) 8PM</t>
+          <t>카누 캡슐 커피머신  4/20(목) 7PM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>여수라테라스&amp;워터파크 혜택가득 풀캉쓱! 최대 69% 할인!</t>
+          <t>전문 바리스타의 기술을 그대로, 카누 캡슐 커피머신! 최신상 5만원 즉시할인</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005430&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005575&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>라테라스 여수 @SSG.LIVE 4/13(목) 8PM</t>
+          <t>카누 캡슐 커피머신 @SSG.LIVE 4/20(목) 7PM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023.04.04</t>
+          <t>2023.04.12</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023.04.13</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 라테라스 여수 @SSG.LIVE 4/13(목) 8PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 카누 캡슐 커피머신 @SSG.LIVE 4/20(목) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>[유아동특집] 탑텐키즈 4/21(금) 11AM</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>간절기 특가 총출동 ~81% OFF 우리아이 래쉬가드세트 9천원대 특급 핫딜까지!</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005449&amp;domainSiteNo=6005</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>[SSG.LIVE]4/21(금) 11AM  탑텐키즈</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023.04.14</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2023.04.21</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]4/21(금) 11AM  탑텐키즈', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>웨딩 리빙 FESTA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>가구부터 프리미엄 주방, 침구까지 한번에 득템</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005502</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>웨딩리빙페스타</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023.04.14</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2023.04.24</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['이벤트/쿠폰 &gt; 웨딩리빙페스타', '스마일클럽', '할인쿠폰 최대 35%', ' 시몬스시몬스 인기상품 비밀 최저가 최대 35% 할인+정품 사은품 증정', ' 알로소소파, 그 이상 Alloso 봄맞이 시즌 소파 최대 15% OFF', '일룸일룸 신혼 맞춤 가구 제안 최대 20만원 쿠폰 혜택', '리바트리바트 혼수 리빙 FESTA 적립/할인 최대 혜택!', '한샘한샘 신혼 공간별 가구 제안 포토 상품평 이벤트', ' 글라스락100% 국내생산 No.1 유리 밀폐용기 남들과는 다른 특별한 신혼살림 글라스락', ' 르크루제르크루제 봄맞이 식기 대전 기간 한정 추가 쿠폰 + 최대 50% OFF', ' 테팔테팔 BEST 모음전 팬/냄비 외 쿡웨어 최대할인', ' 휘슬러휘슬러 쇼핑위크 최대 40% OFF &amp; 일부 품목 15% 쿠폰', ' 클래식패브릭쿨쿨구스 런칭 기념 특가 전 제품 20% OFF', '알레르망 스핑크스알러지프리 원단과 8천개의 핏으로 내몸에 맞춘 침대 해리슨스핑크스 창립 183주년 기념 웨딩리빙 FESTA 초특가할인 기획전 보러가기', '덴비영국 프리미엄 테이블웨어 스프링\xa0페스티벌 최대\xa070%할인\xa0혜택! 기획전 보러가기', '케노샤홈[시몬스] 프리미엄 침구 브랜드 최대 ~29% 즉시할인 ! 기획전 보러가기']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Mon Apr 24 00:20:01 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,703 +473,518 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>푸드 쓱세일</t>
+          <t>마음특송 선물위크</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>오늘이 마지막! 쿠폰 2장 + 타임딜/초특가</t>
+          <t>최대 10% 할인쿠폰 + 조선 팰리스 숙박권의 행운까지</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005336</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005588</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>푸드쓱세일</t>
+          <t>[4/24-30] 마음특송 선물위크</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023.04.20</t>
+          <t>2023.04.30</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 푸드쓱세일', '스마일클럽', '할인쿠폰 매일 최대 2장 + 타임딜/오늘의초특가', '할인 쿠폰 바로보기', '선착순 타임딜 바로보기', '매일 1장, 선착순 9만명! 푸드 10% 장바구니쿠폰', '이마트몰/트레이더스몰/새벽배송몰 쓱배송/새벽배송/택배배송 전체 카테고리 상품', '오전 0시 쿠폰 선착순 2만명', '장바구니 쿠폰 10% 6만원 이상 구매 시 최대 1만원 할인 쿠폰받기', '오전 9시 쿠폰 선착순 2만명', '오후 2시 쿠폰 선착순 2만명', '쿠폰 발급 기간 : 2023년 4월 17일(월) 부터 4월 20일(목) 까지', 'ID당 1일 1장, 오전0시/오전9시/오후2시 쿠폰 중 1매만 다운 가능(기간중 최대 4장까지 발급 가능)', '쿠폰 사용 기간 : 쿠폰 발급받은 당일 한정 사용 가능', '      쿠폰 발급 기간', '      2023년 4월 17일(월) ~ 4월 20일(목) ID당 1일 1장, 오전0시/오전9시/오후2시 쿠폰 중 1매만 다운 가능 (기간 중 최대 4장까지 발급 가능)', '      쿠폰 사용 기간', '      쿠폰 발급받은 당일 한정 사용 가능', '      이마트몰/새벽배송몰/트레이더스몰 전체 카테고리 상품(이마트/트레이더스 쓱배송, 새벽배송, 택배배송상품) * 현금성/무형서비스/초특가 상품, 명품/가전 카테고리 상품 등 일부 제외', '      쿠폰 발급 대상', '      발급된 쿠폰은 [MY &gt; 쿠폰 &gt; 보유쿠폰]에서 확인 가능합니다.', '매일 1장, 선착순 10만명! 푸드 15% 상품쿠폰', '상품 쿠폰 15% 오늘의 초특가 상품 50개 최대 3천원 할인 (일부상품 제외) 쿠폰받기', '쿠폰 발급 기간 : 2023년 4월 17일~4월 20일', '      푸드쓱세일 오늘의핫딜 상품 50개 *일부상품 제외 쿠폰 1장당 대상상품 1개 수량에 한정하여 15% 할인 적용, 최대 3천원 할인', '쓱배송', '15% 상품쿠폰 적용 오늘의 핫딜 더 보러가기', '선착순 타임딜', '오전 9시 타임딜, 오후 2시 타임딜', '타임딜 스캐쥴', '피코크 피코크 신상품부터 할인행사까지 다양하게 만나기', 'CJ 햇반/비비고 대표상품 ~50%할인', '대상 김치/간편식/조미료등 최대 50%할인', "'이날 아무때나' 쓱배송 선택 시 다음 장보기 배송비 지원! 배송비 반값", "'이날 아무때나' 쓱배송 선택 시 SSG MONEY 적립 1,500원", "응모가 완료되었다고 해도, 실제 '이날 아무때나' 선택하여 쓱배송 주문하지 않았다면 응모가 취소됩니다.", '최종 &lt;응모하기&gt; 버튼 완료 후 결제취소 하셨더라도, 이벤트 마감 전까지 다시 응모조건을 충족해주시면 정상적으로 SSG MONEY 지급 대상에 포함됩니다.', '&lt;응모하기&gt; 버튼을 클릭하여 신청한 후에도, 주문 취소 및 단순반품 등으로 인해 응모조건을 충족하지 못 하는 경우 SSG MONEY 지급대상에 포함되지 않습니다.', "1. 쓱배송 상품을 장바구니에 담고 배송시간 선택 시, '이날 아무때나'를 선택해주세요.", '      이벤트 기간', '      SSG MONEY 적립 예정일', '최대 50% 할인 푸드쓱세일에는 한우데이 보러가기', '최대 00만원! 결제할 때 한 번 더 쏠쏠한 추가 할인 청구할인 카드혜택', 'SSGPAY-신한카드 SSGPAY 전용 7만원 이상 5% 청구할인 (일 5만원 한도)', 'SSGPAY-비씨카드 SSGPAY 전용 7만원 이상 5% 청구할인 (일 5만원 한도)', 'SSG.COM카드 Edition1 &amp; Edition2 SSGPAY 전용 7만원 이상 8% 청구할인 (일 5만원 한도)', '카카오페이-KB국민카드 카카오페이 전용 7만원 이상 5% 청구할인 (일 5만원 한도)', 'SSGPAY-삼성카드 SSGPAY 전용 7만원 이상 5% 청구할인 (일 5만원 한도)']</t>
+          <t>['이벤트/쿠폰 &gt; [4/24-30] 마음특송 선물위크', '스마일클럽', '선물위크 쿠폰 바로보기', '쓱-넣어드리는 선물위크 쿠폰', '10% 장바구니쿠폰', '7만원 이상 구매 시 최대 1.5만원 할인 (매일 오전 9시 선착순 2만장)', '오늘의 쿠폰은 마감되었습니다.', '쿠폰 발급 받기 -기간 내 ID당 1회 발급-', '7% 상품쿠폰', '1만원 이상 구매 시 최대 1만원 할인', '      쿠폰 발급 및 사용 기간', "쿠폰 발급 후'My SSG &gt; 쿠폰 &gt; 보유쿠폰' 에서 확인 가능합니다.", '10% 장바구니쿠폰은 매일 선착순 2만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '7% 상품쿠폰은 1만원 이상 구매 시 최대 1만원 할인되며, ID당 기간 내1회 발급 가능합니다. ', '일부 특가 및 브랜드, 기프티콘, 순금/귀금속, 현금성 상품은 쿠폰 할인이 적용되지 않습니다.', '이벤트 기간(4/24~30) 동안 SSG 선물하기 상품 구매 고객을 대상으로, 기간 중 1회 참여 가능하며, 기간 중 선물하기 실구매 내역이 없거나 구매 후 취소된 경우 추첨에서 제외됩니다.', '구매 금액에 상관없이 SSG 선물하기 구매 횟수 기준에 따라 응모 가능하며, 선물하기 챌린지를 완료하였더라도 이벤트에 응모하지 않으시면 당첨에서 제외됩니다. ', '경품은 이벤트 응모시 사용한 ID 회원정보상의 휴대폰 번호와 주소지 기준으로 발송됩니다.', '이벤트에 응모하실 경우 개인정보 제공에 동의하신것으로 간주되며 제공된 정보는 경품 발송후 즉시 파기합니다. (개인정보 위탁업체 : (주)젤라블루코리아 / 제공되는 개인정보 범위 : 성명, 회원ID, 휴대폰번호, 주소)', '본 이벤트는 당사 사정에 따라 임의로 변경 혹은 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>유아동 쓱세일 어린이날 선물대전</t>
+          <t>선물의 고수되기, 신백 선물하기</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>최대 15% 쿠폰 + 엄마아빠 사주세요</t>
+          <t>신백 선물관 리뉴얼 OPEN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005087</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005587</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>유아동 쓱세일</t>
+          <t>[4/24-5/14] 선물의 고수되기, 신백 선물하기</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.05.14</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일', '스마일클럽', '1천여종 완구/패션/유아동 용품 다 모였다! 어린이날 BIG 혜택 15% 최대 2만원 쿠폰+선물 가이드', '유아동 쿠폰 바로보기', '선착순 타임딜 바로보기', '유아동 쓱세일 X4 상품쿠폰 15% 2만원 이상 구매 시, 최대 1만원 할인 10만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기', '쿠폰 받기 클릭 시 총 4장 발급 (ID당 기간 내 1회)', '쿠폰 적용 대상 : 유아동 쓱세일 로고를 확인하세요', '       쿠폰 발급 및 사용 기간', '       쿠폰 적용 방법', '       쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '15% 쿠폰 적용가능 상품은 검색해서 쉽게 볼 수 있어요!', '쿠폰은 대상 상품 상세 페이지에서 편리하게 다운 가능해요!', '상품쿠폰 7% X2 3만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기 클릭 시 총 2장 발급 (ID당 기간 내 1회) ', '      쿠폰 발급 및 사용 기간', '      쿠폰 적용 방법', '      본 쿠폰은 신세계백화점몰 유아동 카테고리 상품에 한하여 적용 가능합니다.', '      쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '장바구니 쿠폰 7% 선착순 쿠폰 7만원 이상 구매 시, 최대 2만원 할인', '장바구니 쿠폰 12% 첫 구매 전용, 유아동 전용, 일별 선착순 1만명 5만원 이상 구매 시, 최대 2만원 할인', '혜택의 마무리 카드 청구 할인', '삼성카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] 7만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '삼성카드 [SSGPAY전용] 7만원 이상 결제 시 5% 청구할인 (일 5만원 한)', '신한카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 10% 청구할인 (일 5만원 한)', 'KB국민카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '매일 오전 10시! 오늘의 선착순 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '타임딜 스캐쥴', '(최대 15%) 남양유업 : 분유 특가 맘키즈 할인+추가 쿠폰', '(최대 35%) 또봇/메카드볼 : 인기 남아완구 특가', '(최대 66%) 네파키즈 : 23 S/S 신상품 반팔세트 등', '(최대 50%) 플레이도 : 인기 상품 원데이 특가', '(최대 15%) 베베숲 : No.1 스테디셀러 물티슈 단 하루 특가', '(쿠폰) H&amp;M : 봄 시즌오프 + 추가 쿠폰', '(최대 10%) 라코스테 : 인기의류 라코스테 키즈 PK 할인', '(최대 18%) 브라이텍스 : 브라이텍스 BEST 쉿! ONLY SSG 단독', '(최대 15%) 하기스 기저귀 : No.1 유한킴벌리 육아 필수품', '(최대 51%) 쁘띠엘린 : 원데이 특가 립프로그 등 인기 특가', '(최대 59%) 휠라키즈 : 23 S/S 신상입고! 신발, 의류 특가', '킨도 : 킨도 기저귀 할인부터 쿠폰까지', '압타밀 : 핫딜 도전 독일 BEST 분유 압타밀', 'S/S 슈즈 ~40% 할인', 'S/S 슈즈 ~40% 할인 상품 더 보러가기', '쿠폰 또는 적립금 혜택까지 실속있게 챙겨가세요 구매 시 쿠폰, 적립 금액을 확인하세요', '              하기스 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 라이브 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 완구 선물 라이브 : 어린이날 기념 SSG단독 완구 최대 49% 특가 및 사은품, 핫딜까지!', '              레고 : [이상훈의 레고네고] 역대급 핫딜/사은품 혜택', '              파크론 : 파크론/아소방 최대 61% 할인 + 쓱라이브 단독사은!', '              탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '          탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '혼자만 알기 아까운 유아동 쓱세일 #쿠폰 받고 같이 쇼핑해요! #오늘의 타임딜, 특가 사고 싶은게 너무 많아! 공유하기']</t>
+          <t>['이벤트/쿠폰 &gt; [4/24-5/14] 선물의 고수되기, 신백 선물하기', '스마일클럽', '백화점 특별 쿠폰 바로보기', '선물위크 쿠폰', '장바구니 쿠폰 10% - 7만원 이상 구매 시 최대 1.5만원 할인(매일 오전 9시, 선착순 2만장)', '상품쿠폰 7% - 1만원 이상 구매 시 최대 1만원 할인', '쿠폰 발급 및 사용 기간 : 발급시점~ 2023년 4월 30일 (일) 23:59', '쿠폰 발급 후’My SSG &gt; 쿠폰 &gt; 보유쿠폰’ 에서 확인 가능합니다.', '10% 장바구니 쿠폰은 매일 선착순 2만장 한정으로 발급되며 ID당 기간 내 1회 발급 가능합니다.', '7% 상품쿠폰은 1만원 이상 구매 시 최대 1만원 할인되며, ID당 기간 내 1회 발급 가능합니다. ', '일부 특가 및 브랜드, 기프티콘, 순금/귀금속, 현금성 상품은 쿠폰 할인이 적용되지 않습니다. ', '선물의 의미, 그 이상의 가치! 신세계백화점 선물하기 경품 이벤트', '       선물하기 이벤트 기간 ', '연락처 등 개인정보 오입력으로 발송 오류 및 미수령에 대해서는 책임지지 않습니다. 경품 발송을 위해 입력하신 경품 발송 정보가 이벤트 진행 대행업체에 제공되며, 경품 증정 후 즉시 파기합니다.(개인정보 위탁업체 : 젤라블루 / 제공범위 : 성명, 휴대전화 번호)', '본 이벤트에 대한 세부사항은 그룹사 사정에 따라 임의로 변경, 조기 종료될 수 있습니다.']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>유아동 쓱세일 타임딜</t>
+          <t>Little SSG 어린이날 선물 대전</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>득템은 선착순! 놓치지 마세요</t>
+          <t>유아동 20% 쿠폰 오늘의 특가 상품 바로가기</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005087#evtAnchor03</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005705</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>유아동 쓱세일</t>
+          <t>Little SSG 어린이날 선물대전</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.30</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일', '스마일클럽', '1천여종 완구/패션/유아동 용품 다 모였다! 어린이날 BIG 혜택 15% 최대 2만원 쿠폰+선물 가이드', '유아동 쿠폰 바로보기', '선착순 타임딜 바로보기', '유아동 쓱세일 X4 상품쿠폰 15% 2만원 이상 구매 시, 최대 1만원 할인 10만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기', '쿠폰 받기 클릭 시 총 4장 발급 (ID당 기간 내 1회)', '쿠폰 적용 대상 : 유아동 쓱세일 로고를 확인하세요', '       쿠폰 발급 및 사용 기간', '       쿠폰 적용 방법', '       쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '15% 쿠폰 적용가능 상품은 검색해서 쉽게 볼 수 있어요!', '쿠폰은 대상 상품 상세 페이지에서 편리하게 다운 가능해요!', '상품쿠폰 7% X2 3만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기 클릭 시 총 2장 발급 (ID당 기간 내 1회) ', '      쿠폰 발급 및 사용 기간', '      쿠폰 적용 방법', '      본 쿠폰은 신세계백화점몰 유아동 카테고리 상품에 한하여 적용 가능합니다.', '      쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '장바구니 쿠폰 7% 선착순 쿠폰 7만원 이상 구매 시, 최대 2만원 할인', '장바구니 쿠폰 12% 첫 구매 전용, 유아동 전용, 일별 선착순 1만명 5만원 이상 구매 시, 최대 2만원 할인', '혜택의 마무리 카드 청구 할인', '삼성카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] 7만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '삼성카드 [SSGPAY전용] 7만원 이상 결제 시 5% 청구할인 (일 5만원 한)', '신한카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 10% 청구할인 (일 5만원 한)', 'KB국민카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '매일 오전 10시! 오늘의 선착순 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '타임딜 스캐쥴', '(최대 15%) 남양유업 : 분유 특가 맘키즈 할인+추가 쿠폰', '(최대 35%) 또봇/메카드볼 : 인기 남아완구 특가', '(최대 66%) 네파키즈 : 23 S/S 신상품 반팔세트 등', '(최대 50%) 플레이도 : 인기 상품 원데이 특가', '(최대 15%) 베베숲 : No.1 스테디셀러 물티슈 단 하루 특가', '(쿠폰) H&amp;M : 봄 시즌오프 + 추가 쿠폰', '(최대 10%) 라코스테 : 인기의류 라코스테 키즈 PK 할인', '(최대 18%) 브라이텍스 : 브라이텍스 BEST 쉿! ONLY SSG 단독', '(최대 15%) 하기스 기저귀 : No.1 유한킴벌리 육아 필수품', '(최대 51%) 쁘띠엘린 : 원데이 특가 립프로그 등 인기 특가', '(최대 59%) 휠라키즈 : 23 S/S 신상입고! 신발, 의류 특가', '킨도 : 킨도 기저귀 할인부터 쿠폰까지', '압타밀 : 핫딜 도전 독일 BEST 분유 압타밀', 'S/S 슈즈 ~40% 할인', 'S/S 슈즈 ~40% 할인 상품 더 보러가기', '쿠폰 또는 적립금 혜택까지 실속있게 챙겨가세요 구매 시 쿠폰, 적립 금액을 확인하세요', '              하기스 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 라이브 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 완구 선물 라이브 : 어린이날 기념 SSG단독 완구 최대 49% 특가 및 사은품, 핫딜까지!', '              레고 : [이상훈의 레고네고] 역대급 핫딜/사은품 혜택', '              파크론 : 파크론/아소방 최대 61% 할인 + 쓱라이브 단독사은!', '              탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '          탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '혼자만 알기 아까운 유아동 쓱세일 #쿠폰 받고 같이 쇼핑해요! #오늘의 타임딜, 특가 사고 싶은게 너무 많아! 공유하기']</t>
+          <t>['이벤트/쿠폰 &gt; Little SSG 어린이날 선물대전', '스마일클럽', '20% 쿠폰', '멤버십 전용 유아동 20% 쿠폰', '선착순 4만장 SmileClub전용 상품쿠폰 20%', '3만원 이상 상품 구매시 최대 7천원 할인, 일부 특가상품 적용 제외, 신세계백화점, 신세계몰, 이마트몰', '쿠폰은 25일 10시에 오픈됩니다.', '선착순 쿠폰 마감 되었습니다. 감사합니다', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[ 미미월드 ] 미리준비하는 어린이날 미미/ 똘똘이/ 뽀로로 외 최대 30%할인', '실바니안패밀리 브레드이발소 산리오 외 세트특가할인', '★어린이날★ 산리오/몰랑 완구 모음전 최대 30%할인', '최대 30% 특가', '[해즈브로] 플레이도 /슈퍼소커/ 마이리틀포니 특가할인', '할인이 쓱쓱 인기 여아캐릭터 완구 모음전 미미월드 토이트론 외', '★쓱세일★ 해즈브로 인기 브랜드 할인모음', '시크릿쥬쥬/ LOL/ 미미 최대 30% 할인', '[쁘띠엘린] 완구 특가 립프로그/젤리캣 할인', '[꼬미마녀라라 외] 인기 신상완구 특가 할인!']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>유아동 쓱세일 대표 브랜드</t>
+          <t>맛잘알을 위한 피코크 먹킷리스트</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>더 커진 브랜드 혜택 + 인기 상품</t>
+          <t>피코크 15% 할인쿠폰 + BEST 상품 추천 + 첫구매 해피딜</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005087#evtAnchor05</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005701&amp;domainSiteNo=7018</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>유아동 쓱세일</t>
+          <t>피코크 먹킷리스트</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.30</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 유아동 쓱세일', '스마일클럽', '1천여종 완구/패션/유아동 용품 다 모였다! 어린이날 BIG 혜택 15% 최대 2만원 쿠폰+선물 가이드', '유아동 쿠폰 바로보기', '선착순 타임딜 바로보기', '유아동 쓱세일 X4 상품쿠폰 15% 2만원 이상 구매 시, 최대 1만원 할인 10만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기', '쿠폰 받기 클릭 시 총 4장 발급 (ID당 기간 내 1회)', '쿠폰 적용 대상 : 유아동 쓱세일 로고를 확인하세요', '       쿠폰 발급 및 사용 기간', '       쿠폰 적용 방법', '       쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '15% 쿠폰 적용가능 상품은 검색해서 쉽게 볼 수 있어요!', '쿠폰은 대상 상품 상세 페이지에서 편리하게 다운 가능해요!', '상품쿠폰 7% X2 3만원 이상 구매 시, 최대 2만원 할인', '쿠폰 받기 클릭 시 총 2장 발급 (ID당 기간 내 1회) ', '      쿠폰 발급 및 사용 기간', '      쿠폰 적용 방법', '      본 쿠폰은 신세계백화점몰 유아동 카테고리 상품에 한하여 적용 가능합니다.', '      쿠폰은 적용상품 수량 1개에 대해 적용됩니다. (동일상품 복수 개 구매 시 1개 수량에만 적용)', '장바구니 쿠폰 7% 선착순 쿠폰 7만원 이상 구매 시, 최대 2만원 할인', '장바구니 쿠폰 12% 첫 구매 전용, 유아동 전용, 일별 선착순 1만명 5만원 이상 구매 시, 최대 2만원 할인', '혜택의 마무리 카드 청구 할인', '삼성카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] 7만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '삼성카드 [SSGPAY전용] 7만원 이상 결제 시 5% 청구할인 (일 5만원 한)', '신한카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', 'SSG.COM카드 ED1 &amp; ED2 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 10% 청구할인 (일 5만원 한)', 'KB국민카드 [SSGPAY전용] [유아동쓱세일전용] 8만원 이상 결제 시 8% 청구할인 (일 5만원 한)', '매일 오전 10시! 오늘의 선착순 타임딜', '타임딜은 10시에 오픈됩니다!', '금일 타임딜이 종료되었습니다. 감사합니다.', '타임딜 스캐쥴', '(최대 15%) 남양유업 : 분유 특가 맘키즈 할인+추가 쿠폰', '(최대 35%) 또봇/메카드볼 : 인기 남아완구 특가', '(최대 66%) 네파키즈 : 23 S/S 신상품 반팔세트 등', '(최대 50%) 플레이도 : 인기 상품 원데이 특가', '(최대 15%) 베베숲 : No.1 스테디셀러 물티슈 단 하루 특가', '(쿠폰) H&amp;M : 봄 시즌오프 + 추가 쿠폰', '(최대 10%) 라코스테 : 인기의류 라코스테 키즈 PK 할인', '(최대 18%) 브라이텍스 : 브라이텍스 BEST 쉿! ONLY SSG 단독', '(최대 15%) 하기스 기저귀 : No.1 유한킴벌리 육아 필수품', '(최대 51%) 쁘띠엘린 : 원데이 특가 립프로그 등 인기 특가', '(최대 59%) 휠라키즈 : 23 S/S 신상입고! 신발, 의류 특가', '킨도 : 킨도 기저귀 할인부터 쿠폰까지', '압타밀 : 핫딜 도전 독일 BEST 분유 압타밀', 'S/S 슈즈 ~40% 할인', 'S/S 슈즈 ~40% 할인 상품 더 보러가기', '쿠폰 또는 적립금 혜택까지 실속있게 챙겨가세요 구매 시 쿠폰, 적립 금액을 확인하세요', '              하기스 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 라이브 : 기저귀/제지/생리대 52% + 3.5만이상 구매시 5천원 추가 할인 추첨', '              유아동 쓱세일 완구 선물 라이브 : 어린이날 기념 SSG단독 완구 최대 49% 특가 및 사은품, 핫딜까지!', '              레고 : [이상훈의 레고네고] 역대급 핫딜/사은품 혜택', '              파크론 : 파크론/아소방 최대 61% 할인 + 쓱라이브 단독사은!', '              탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '          탑텐키즈 : 탑텐키즈 간절기 특가전! 래쉬가드세트 핫딜 9천원대', '혼자만 알기 아까운 유아동 쓱세일 #쿠폰 받고 같이 쇼핑해요! #오늘의 타임딜, 특가 사고 싶은게 너무 많아! 공유하기']</t>
+          <t>['이벤트/쿠폰 &gt; 피코크 먹킷리스트', '스마일클럽', '피코크 15% 할인쿠폰', '첫구매 피코크 해피딜', '피코크 할인받고 GET!', '피코크 쓱배송/새벽배송/점포택배 상품', '선착순 1.2만명', '상품쿠폰', '%', '1천원 이상 구매시 최대 3천원 할인', '■ 쿠폰 발급 기간 : 2023년 4월 24일(월) ~ 30일(일)', '쿠폰 발급 및 사용일: 23년 4월 24일(월)~30일(일) (ID당 1일 1회 다운가능)', '쿠폰 사용조건:  이마트몰 쓱배송 / 새벽배송 / 점포택배 피코크 상품 1천원 이상 구매시 사용가능 (최대할인금액 3천원, 일부 상품 제외)', '쿠폰 적용 제외 상품은 구매금액에 합산되지 않습니다.', '장보기 첫구매라면, 해피 90%딜 쿠폰팩받고 피코크 인기상품을 더 저렴하게', '상품쿠폰 90% (선착순 3만장) 해피 90%딜 상품 중 1개에 한하여 최대 1만원 이상 구매시 사용가능', '무료배송 (선착순 3만장)', '쿠폰 다운받으러 가기', '      SSG 가입 후 또는 직전 1년 간(2022년 4월 24일 이후) 이마트몰, 트레이더스쓱배송/점포택배 및 새벽배송 구매 이력이 없는 고객', '      하단 해피 90%딜 적용상품 중 1개를 골라 결제단계에서 쿠폰을 적용해주세요.']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>오늘의 초특가 상품</t>
+          <t>피코크 인기상품 해피 90%딜</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>푸드 쓱세일 15% 추가할인</t>
+          <t>장보기 첫구매 고객님께만 최대 90%할인 + 무료배송</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005596</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005660</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>푸드 쓱세일 초특가 상품 15% 할인</t>
+          <t>첫 장보기 고객님께만 해피 90%딜</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023.04.20</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023.04.20</t>
+          <t>2023.04.30</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 푸드 쓱세일 초특가 상품 15% 할인', '스마일클럽', '푸드 쓱세일 초특가 상품 15% 할인', '푸드 쓱세일 BEST 상품 15% 추가할인', '상품 상세 페이지에서 오늘의 쿠폰 받으세요', '푸드 15% 상품쿠폰', '쿠폰 적용 대상 : 오늘의 초특가 상품 (일부상품 제외)', '쿠폰이 모두 소진되었습니다. 내일 오전0시를 기대해주세요!', '쿠폰이 모두 소진되었습니다. 많음 참여에 감사드립니다', '* 쿠폰 발급 기간 : 2023년 4월 17일(월) ~ 4월 20일(목)', '* 쿠폰 사용 기간 : 쿠폰 발급 받은 당일 한정 사용 가능', '전시되어 있는 오늘의 초특가 상품 15% 쿠폰 받으세요']</t>
+          <t>['이벤트/쿠폰 &gt; 첫 장보기 고객님께만 해피 90%딜', '스마일클럽', '첫 장보기 고객님께만 해피 90%딜', '장보기 첫구매 고객님께만 드리는', '해피 90%딜', '피코크 인기상품 최대 90% 할인 + 무료배송까지!', '최근 1년간 쓱배송이 처음이라면,', '해피 90%딜 쿠폰팩 다운받고 피코크 인기상품을 저렴하게 만나보세요', '상품쿠폰 90% 선착순 3만장, ※해피 90%딜 상품 중 1개에 한하여 최대 1만원까지 할인 적용됩니다.', '무료배송 선착순 3만장', '(선착순 2만장) 장바구니 쿠폰 9,900원 쿠폰 발급받기', '선착순 쿠폰이 마감되었습니다.', '       쿠폰 발급', '       쿠폰 사용 기간', '       상품할인쿠폰, 무료배송쿠폰: 20203년 4월 24일(월)~2023년 4월 30일(일)', '       쿠폰 사용 조건', '무료배송 쿠폰 : 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '       쿠폰 발급 대상', '      SSG 가입 후 또는 직전 1년간(2022년 4월 24일 이후) 이마트몰, 트레이더스쓱배송/점포택배 및 새벽배송 구매 이력이 없는 고객', '      하단 해피 90%딜 적용상품 1개를 골라 결제단계에서 쿠폰을 적용해주세요.', '해피 90%딜 적용상품을 확인하세요!']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>백화점 선물하기 SPRING GIFT</t>
+          <t>집밥챌린지 - 보양식</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>나들이 필수템 GIFT 준비는 백화점 선물하기로!</t>
+          <t>나만의 최애 보양식 투표하고 쓱배송으로 보양식 한번에 준비해요!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005258</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005330</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>신세계백화점 SPRING GIFT</t>
+          <t>(4/20~26) 집밥챌린지_보양식 편</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023.04.03</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.26</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 신세계백화점 SPRING GIFT', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; (4/20~26) 집밥챌린지_보양식 편', '스마일클럽', '보양식 재료부터 손쉬운 간편식품까지 쓱배송으로 준비해요!', '        하단 투표 이벤트도 잊지마세요!', '쓱배송으로 보양식']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>에어서울 국제선 초특가</t>
+          <t>바이오퍼블릭 기프트 위크</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>일본 항공권 5만원대~, 동남아 8만원대부터!</t>
+          <t>15% 쿠폰으로 건강을 선물하세요!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005477</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005633</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>에어서울 국제선 선착순 핫딜 위크</t>
+          <t>바이오퍼블릭 기프트 위크</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.30</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 에어서울 국제선 선착순 핫딜 위크', '스마일클럽', '에어서울 국제선 선착순 핫딜 위크', '~5만원 할인', '7% 쿠폰', '카드 할인', '선착순 한정 수량', '매일 오전 10시, 국제선 편도당 5천원 즉시 할인', '매일 선착순 120개 한정 핫딜', '즉시할인 에어서울 일본 항공권 나리타/오사카/후쿠오카/다카마쓰 최저가 83,900원 ~', '즉시할인 에어서울 일본 항공권 나리타/오사카/후쿠오카/다카마쓰 최저가 55,900원부터', '즉시할인 에어서울 동남아 항공권 보라카이/나트랑/다낭 최저가 89,900원부터', '일본 편도 최저가 60,900원 &gt; 5천원 쿠폰 반영시 55,900원~', '동남아 최저가 94,000원 %gt; 5천원 쿠폰 반영시 89,900원~', '할인 금액70만원 이상 결제시 5만원 / 30만원 이상 결제시 2만원 / 15만원 이상 결제시 1만원 / 5만원 이상 결제시 4천원 할인', "프로모션 내용:  SSG.COM,신세계몰,이마트몰,트립몰 내 '여행' 일반 상품 구매 시 금액대별 즉시할인 ", '해당 이벤트는 사전 고지 없이 혜택 변경 및 조기 종료될 수 있습니다.', 'SSG머니 즉시할인이 적용되지 않는다면 할인 혜택이 종료된 것으로, 즉시할인 금액을 제외한 최종가로 결제됩니다.', '사용 방법요금 할인은 호텔 상세 페이지에서 쿠폰 다운받은 후 적용 가능합니다.', '쿠폰 내용:  익스피디아 실시간 호텔 전 상품 1원 이상 구매 시 7% 할인 ', "쿠폰 변경 적용 시 '혜택 직접 선택하기'로 변경해 주시길 바랍니다.", '게이오 플라자 호텔 도쿄 정상가 : 283,140원 &gt; 할인가 : 263,320원', 'sequence MIYASHITA PARK 정상가 : 237,803원 &gt; 할인가 : 221,157원', '스위소텔 난카이 오사카 정상가 : 79,277원 &gt; 할인가 : 73,728원', '남바 오리엔탈 호텔 정상가 : 254,264원 &gt; 할인가 : 236,466원', '이비스 스타일스 오사카 남바 정상가 : 303,717원 &gt; 할인가 : 282,457원', '솔라리아 니시테츠 호텔 후쿠오카 정상가 : 120,000원 &gt; 할인가 : 111,600원', '오리엔탈 호텔 후쿠오카 하카타 스테이션 정상가 : 172,754원 &gt; 할인가 : 142,754원', '삿포로 그랜드 호텔 정상가 : 198,000 &gt; 할인가 : 184,140원', '두짓 타니 괌 리조트 : 421,850원 &gt; 할인가 : 391,850원', '롯데 호텔 괌 : 265,342원 &gt; 할인가 : 246,768원', '호텔 닛코 괌 : 263,380원 &gt; 할인가 : 244,943원', '퍼시픽 아일랜드 클럽 괌 : 304,453원 &gt; 할인가 : 283,141원', '하얏트 리젠시 괌 : 355,366원 &gt; 할인가 : 330,490원', '더 츠바키 타워 : 473,461원 &gt; 할인가 : 443,461원', '하얏트 리젠시 사이판 : 245,199원 &gt; 할인가 : 228,035원', '사이판 월드 리조트 : 438,248원 &gt; 할인가 : 408,248원', '쉐라톤 그란데 수쿰윗, 럭셔리 컬렉션 호텔, 방콕 정상가 : 287,277원 &gt; 할인가 : 287,277원', '더 쇼어 앳 까따타니 - SHA Extra Plus 정상가 : 548,827원 &gt; 할인가 : 518,827원', '빈펄 리조트 &amp; 스파 다낭 정상가 : 450,982원 &gt; 할인가 : 420,982원', '신라모노그램 다낭 정상가 : 228,067원 &gt; 할인가 : 212,102원', '더 리츠칼튼, 밀레니아 싱가포르(SG Clean) 정상가 : 666,808원 &gt; 할인가 : 666,808원', '샹그릴라 호텔, 싱가포르(SG Clean) 정상가 : 351,325원 &gt; 할인가 : 326,732 원', '퓨전 리조트 푸꾸옥 정상가 : 321,210원 &gt; 할인가 : 298,725 원', '퓨전 리조트 깜 라인 정상가 : 334,424원 &gt; 할인가 : 311,014 원', '하얏트 리젠시 와이키키 비치 리조트 &amp; 스파 : 423,295원 &gt; 할인가 : 393,664원', '힐튼 하와이안 빌리지 와이키키 비치 리조트 : 321,455원 &gt; 할인가 : 298,953원', '윈 라스베이거스 : 293,103원 &gt; 할인가 : 272,586원', '더 코스모폴리탄 오브 라스베이거스 : 148,363원 &gt; 할인가 : 137,978원', '풀먼 파리 타워 에펠 : 609,943원 &gt; 할인가 : 579,943원', '시타딘 아파트호텔 생제르망 데 프레 파리 : 517,849원 &gt; 할인가 : 487,849원', '호텔 레지나 : 224,416원 &gt; 할인가 : 208,707원', '마리팀 호텔 프랑크푸르트 : 320,417원 &gt; 할인가 : 297,988원', '서울 신라호텔 정상가 : 506,000원 &gt; 할인가 : 476,000원', '파라다이스시티 정상가 : 352,000원 &gt; 할인가 : 327,360원', '그랜드 조선 제주 정상가 : 351,999원 &gt; 할인가 : 327,359원', '아난티 힐튼 부산 정상가 : 341,000원 &gt; 할인가 : 317,130원', '파라다이스 호텔 부산 정상가 : 278,300원 &gt; 할인가 : 258,819원', '힐튼 경주 정상가 : 272,251원 &gt; 할인가 : 253,193원', '롯데리조트속초 정상가 : 294,000원 &gt; 할인가 : 273,420원', '소노캄 여수 정상가 : 202,364원 &gt; 할인가 : 188,199원', '[SSGPAY전용] 신한카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 비씨카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드 Ed1&amp;Ed2 7만원 이상 8% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 신한카드 7만원 이상 5% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] SSG.COM카드Ed1&amp;Ed2 7만원 이상 8% 청구할인 (일 5만원 한) 자세히 보기', '[SSGPAY전용] 삼성카드 7만원이상 5% 청구할인 (일 5만원 한) 자세히 보기']</t>
+          <t>['이벤트/쿠폰 &gt; 바이오퍼블릭 기프트 위크', '스마일클럽', '+카드청구할인', '~15%쿠폰', '50%~, 1+1', '건강식품 ~15%쿠폰', '카드청구할인까지', '선착순  1천명', '장바구니쿠폰', '%', '5만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 사용 기간: 발급 당일', '3만원 이상 구매 시 최대 1만 5천원 할인', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '[SSGPAY전용] 신한카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', 'SSG.COM 삼성카드 [SSGPAY전용] 8만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '국민카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '비씨카드[SSGPAY전용] 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '~15%쿠폰으로 건강 선물하기', '[오쏘몰] 프리미엄 종합 비타민 특별할인 무료배송 및 ~17% OFF!', '[Biopublic]100% 식물성 프로틴 케어 350g(25g*14포)', '[이마트해외직구] 신타6 아이솔레이트 단백질파우더 1.82kg 1+1 모음 , 무료배송 1+1', '50%~,  1+1 득템 찬스', '50%~ 할인 상품', '50% 할인', '[함소아제약 외]건강식품 50%이상 할인된 가격', '[기프트위크](50%할인) 휴럼 건강식품 반값행사', '순홍삼(풍기) 50mlx30 1세트+쇼핑백 外 50% 할인특가', '[기프트위크][쓱배송]건강식품 반값행사', '50% 할인. 콤비타', '[쏜리서치] 공식판매처! 인기 영양제 1+1 구성 특가! 2/데이,S.A.T 외 무료배송', '[독일직구][무료배송] 오쏘몰 이뮨 30일 1+1 2박스 드링크 정제 멀티비타민 orthomol / 최신제조일자 / 빠른배송 / 독일현지배송', '[쓱배송]홍삼 기프트 특가', '[최대40%할인] 건강식품 선물하기', '[쓱배송]락티브 비타민 가격할인', '어린이 멀티비타민 유산균 오메가3 백화점 선물세트 [사은품증정이벤트]', '트리플러스50+/90캡슐 x 3개 [사은품증정이벤트]', '[쓱배송]루테인 초특가', '[쓱배송][정관장]홍삼진본 40ml*20포[쇼핑백포함]', '[15% 즉시할인][세노비스] 키즈 멀티비타민미네랄 (1.5g*90정*2통/총90일분) ★미니 멀티비타민 2개 증정★', '[15% 즉시할인][세노비스] 트리플러스 맨 (90캡슐) + 트리플러스 우먼 (90캡슐) (커플세트) ★미니 트리플러스 맨+우먼 증정★', '★139,000→69,500[쓱배송] 휴럼 천년침향환(3.7g*60환)[쇼핑백 동봉]', '★ 레이델 특가상품 모음★ 레이델 폴리코사놀/비즈왁스알코올 셀100  外~ 사은품 + 쿠폰☆', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[무료배송][오쏘몰] 이뮨(immun) 드링크+정제 30일분 3개묶음 / 독일직배송 / 최신제조일자 / 본사 공식', '30% + 5% SSG머니할인', '10% 할인 + 쇼핑백증정', '최대 54% 할인', '1+1 특가 + 추가 4% 즉시할인', '2+1 증정 이벤트']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[첫구매 이벤트] 반값다딜- 동원 편</t>
+          <t>최대 5만원 혜택</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>첫구매라면, 동원 인기상품 최대 1.6만원 할인 + 무료배송</t>
+          <t>+ 쓸 때마다 최대 12% 적립</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005206&amp;domainSiteNo=7018</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[첫구매이벤트] 반값다~딜 - 동원 편</t>
+          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2022.07.08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.06.28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [첫구매이벤트] 반값다~딜 - 동원 편', '스마일클럽', '[첫구매이벤트] 반값다~딜 - 동원 편', 'STEP1 반가운 반값쿠폰팩 받기 바로보기', '최근 1년간 쓱배송이 처음이라면, 동원 상품 50% 할인에 무료배송', '동원 상품쿠폰 50% 4장, 최대 할인 금액 5천원(2장), 3천원(2장), 본 페이지와 하단 기획전에 진열된 상품에 적용 가능', '무료배송 1장, 이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 사용 가능', '쿠폰 발급/사용 기간 : 2023년 4월 17일(월) ~2023년 4월 23일(일)', '- 쿠폰 사용 조건 :', '1) 상품할인 쿠폰 :  쓱배송/새벽배송 동원 브랜드 상품 50% 할인. (최대할인금액 각 5천원, 3천원)', '2) 무료배송 쿠폰 :  이마트 쓱배송/새벽배송 상품 2만원 이상 구매시 무료배송', '(50%, 무료배송) 자극적인 짠맛은 줄이고 돈육 본연의 맛은 살린 리챔 오리지널 300gX4 할인전 : 16,800원 할인후 : 11,800원', ' 동원 고추참치 90g*4, 기존가 9,480원, 할인가 4,480원 ', ' 동원 야채참치 90g*4, 기존가 9,480원, 할인가 4,740원 ', ' 리챔 오리지널 340gX4, 기존가 18,800원, 할인가 13,800원 ', ' 동원 을지로골뱅이 300g, 기존가 8,380원, 할인가 4,190원 ', '(50%, 무료배송) 부드러운 한우 사태가 들어가 더욱 깊고 진한 수라 한우소고기죽 287.5g 할인전 : 5,180원 할인후 : 2,590원', ' 수라 완도전복내장죽 287.5g, 기존가 5,180원, 할인가 2,590 원 ', ' 동원 양반 수라 돼지고기 김치찌개, 기존가 6,980원, 할인가 3,490원 ', ' 동원 양반 소고기미역국, 기존가 5,480원, 할인가 2,740원 ', ' 동원 양반 수라 우거지감자탕 460g, 기존가 8,980원, 할인가 4,490원 ', '(50%, 무료배송) 담백한 육즙이 가득 탱글탱글한 비엔나 동원 통그릴 비엔나 300g*2 할인전 : 8,380원 할인후 : 4,190원', ' 동원 그릴리 델리햄 김밥용 150g, 기존가 2,480원, 할인가 1,240원 ', ' 삼각유부초밥 340g, 기존가 5,180원, 할인가 2,590원 ', ' 개성 얇은피 김치만두 400gx2, 기존가 9,800원, 할인가 4,900원 ', ' 감자 물만두 600gx2, 기존가 10,800원, 할인가 5,800원 ']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 10월 1일 부터 2023년 3월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.10.01~2023.03.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '3. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>집밥챌린지 - 보양식</t>
+          <t>더 강력해진 SSG.COM 삼성카드</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>나만의 최애 보양식 투표하고 쓱배송으로 보양식 한번에 준비해요!</t>
+          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005330</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(4/20~26) 집밥챌린지_보양식 편</t>
+          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023.04.20</t>
+          <t>2022.10.26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023.04.26</t>
+          <t>2025.10.25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (4/20~26) 집밥챌린지_보양식 편', '스마일클럽', '보양식 재료부터 손쉬운 간편식품까지 쓱배송으로 준비해요!', '        하단 투표 이벤트도 잊지마세요!', '쓱배송으로 보양식']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '최대 5% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>백화점 캠핑&amp;아웃도어 대전</t>
+          <t>유세린 4/24(월) 7PM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>힐링 액티비티 인기 상품전</t>
+          <t>흔적케어 UV세럼/톤업 선크림 2만9천원 핫딜!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005489</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005780</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>자연과 함께하는 힐링 액티비티</t>
+          <t>유세린@SSG.LIVE 4/27(수) 7:00PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.29</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 자연과 함께하는 힐링 액티비티', '스마일클럽', '10% 쿠폰 혜택 바로보기', '10% 쿠폰 혜택', '      쿠폰 발급 및 사용 기간', '      쿠폰 발급은 당사 사정에 따라 선착순 조기 마감될 수 있습니다.', '      쿠폰 발급 대상', '나이키 4월 정기세일 UP TO 48%', '아디다스 SS신상 &amp; 베스트 스포츠웨어/슈즈 모음전 + 추가즉시할인혜택', '코오롱스포츠 프리미엄 아웃도어 봄 기획전 + 상품별 할인쿠폰 혜택', '반스 스니커즈 UP TP 50% + 추가즉시할인혜택', '쿠폰은 오전 9시에 오픈됩니다:)', '쿠폰이 마감되었습니다!']</t>
+          <t>['이벤트/쿠폰 &gt; 유세린@SSG.LIVE 4/27(수) 7:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>프리미엄 아울렛 위크 : 미리 준비하는 가정의달</t>
+          <t>사이판 PIC 4/24(월) 8PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>기획전 전시 상품 대상 ~10% 즉시할인</t>
+          <t>올인원 패키지! 2+2 패밀리팩 51만원대~ 선착순 핫딜</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005557</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005649&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[0417-0423] 프리미엄 아울렛 위크</t>
+          <t>노랑풍선 사이판 PIC @SSG.LIVE 4/24(월) 20:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.14</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.29</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [0417-0423] 프리미엄 아울렛 위크', '스마일클럽', '쿠폰 혜택 할인쿠폰 최대10%', 'EVENT 03 미리 준비하는 가정의달 - FAMILY WEEK *할인율은 정상가 기준 할인율임', '[키즈패션 - 최대 70% 할인] 유아동 인기 브랜드 총모음 BIG SALE 보러가기', '[리빙 - 최대 50% 할인] 빌레로이앤보흐, 웨지우드 등 특가 + 쿠폰 보러가기', '[스포츠 - 최대 60% 할인] 골프 BEST 특가 모음전 + 쿠폰혜택 보러가기', '[해외명품 - 최대 70% 할인] 프라다/발렌시아가 外 병행수입 명품 특가 보러가기', '[여성패션 - 최대 70% 할인] BEST 50 &amp; 아울렛 위크 특가 外 보러가기', '[패션슈즈 - 최대 80% 할인] 슈즈잡화쥬얼리 시즌 BEST 특별전 보러가기', '[패션잡화 - 최대 20% 할인] 로우로우 백팩/ 캐리어 신상 물량 입고! 보러가기', '[언더웨어 - 최대 51% 할인] 라페어 브랜드 위크 언더/이제웨어 특가 보러가기', '[남성패션 - 최대 70% 할인] 송지오옴므/브룩스브라더스 外 보러가기', '[유니섹스 - 최대 79% 할인] 라코스테, 폴햄 등 봄 캐주얼의류 신규입고 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 노랑풍선 사이판 PIC @SSG.LIVE 4/24(월) 20:00', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트: 영실업</t>
+          <t>설화수 4/25(화) 7PM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>이번 어린이날 선물로 딱! 또봇 단독 사은품 증정</t>
+          <t>어버이날 선물 준비완료 + 설화수 지함보 세트 핫딜 선착순 적립금 추가지급</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005546</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005742&amp;siteNo=6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SSG 브랜드 스포트라이트 - 영실업</t>
+          <t>설화수 @SSG.LIVE 4/25(화) 7PM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.04.19</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.04.25</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG 브랜드 스포트라이트 - 영실업', '스마일클럽']</t>
+          <t>['이벤트/쿠폰 &gt; 설화수 @SSG.LIVE 4/25(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>집에서 즐기는 미쉐린 레스토랑</t>
+          <t>SSG 럭셔리 더 뷰티 가정의 달 GIFT</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>최대 20% 할인에 5천원 페이백</t>
+          <t>SSG에서만 만나볼수 있는 베스트셀러 부터 신상품 까지</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005451</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005535</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>집에서 즐기는 미쉐린 레스토랑</t>
+          <t>[4/24~30 ] 럭셔리 더 뷰티 가정의 달 GIFT</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023.04.17</t>
+          <t>2023.03.30</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023.04.23</t>
+          <t>2023.05.14</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 집에서 즐기는 미쉐린 레스토랑', '스마일클럽', '# 최대 20% 할인', '생면 파스타 최대 20% 할인 행사', '정상가 9,800원&gt; 할인가 7,840원 (20%할인)', '정상가 8,900원&gt; 할인가 7,120원 (20%할인)', '지급된 SSG MONEY는 지급일로부터 30일간 사용 가능하며 기간 경과 후에는 소멸 됩니다.', '반드시 [페이백 신청하기] 버튼을 클릭하셔야 SSG MONEY가 정상 지급됩니다.']</t>
+          <t>['이벤트/쿠폰 &gt; [4/24~30 ] 럭셔리 더 뷰티 가정의 달 GIFT', '스마일클럽', '15%', '10%', '기획상품10% 할인 전구매 고객 두피세럼 증정', '[시코르 추천] 인기 뷰티템 UP TO 30%', '자연의 작품, 연작   카밍 앤 컴포팅라인 20% 할인 + 쓱단독 사은품 증정', '[몰튼 브라운]SSG 단독 선물포장+UP TO 35%', '예비맘 뷰티루틴, 15%쿠폰&amp;상품권 증정']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>최대 5만원 혜택</t>
+          <t>4월 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>+ 쓸 때마다 최대 12% 적립</t>
+          <t>지금 할인 중! ~40% 할인 혜택</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000000858&amp;siteNo=6005&amp;recruitmentPath=L6007001&amp;eventCode=HPG02</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000001665</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SSG.COM카드 Edition 2 이벤트 안내 페이지</t>
+          <t>이달의 맘키즈 PLUS</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2022.07.08</t>
+          <t>2022.09.01</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023.06.28</t>
+          <t>2022.09.01</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM카드 Edition 2 이벤트 안내 페이지', '스마일클럽', 'SSG.COM카드 Edition 2 이벤트 안내 페이지', 'SSG.COM카드 Edition2는 SSG.COM에서 최대 5만원 혜택 + 쓸 때마다 최대 12% 적립', '이달의 혜택 01. SSG.COM카드 Edition2 첫결제 시 1만원 쿠폰 할인 바로보기', '혜택 01. SSG머니 최대 12% 적립 바로보기', '혜택 02. 매월 스마일클럽 가입비 3,900원 지원 바로보기', '이달의 혜택 01. SSG.COM에서 SSG.COM카드 Edition2 첫 결제 시 1만원 할인', '      직전 6개월간 (2022년 10월 1일 부터 2023년 3월 31일) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한함', '첫 결제 쿠폰 이용 방법', '② SSGPAY에 등록된 SSG.COM카드 Edition2로', '③ SSG.COM에서 기간 내 1만 1천원 이상 첫 결제 시 1만원 쿠폰 할인', '      본 혜택은 SSG.COM카드 및 SSG.COM카드 Edition2 로 SSG.COM(이마트몰, 신세계몰, 신세계백화점몰 등)에서 직전 6개월간 (2022.10.01~2023.03.31) SSG.COM카드 및 SSG.COM카드 Edition2로 결제 이력이 없고 &amp; SSGPAY에 등록된 현대카드가 없는 회원에 한해 제공됨', "      본 혜택은 결제 시 [결제방법 &gt; SSGPAY카드] 내 SSG.COM카드 Edition2 선택 시, '카드할인 최적가' 추천에 의해 할인 금액이 자동 적용됨. 단, 1만 1천원 이상 첫 결제 시 적용)", '다운받은 쿠폰은 SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '쿠폰 사용하러 가기', 'SSGPAY에 등록된 SSG.COM카드 Edition2로 SSG.COM에서 바로 결제 시 사용 가능합니다.', '3. SSG.COM에서 기간 내 2만원 이상 첫 결제 시 제공 *쿠폰할인, 적립금 사용(SSG머니, 신세계포인트 등), 상품권 등 선할인 및 일부상품(상품권 등 현금성 상품, 무형서비스 상품, 초특가 상품, 특정 브랜드 상품 등)을 제외한 카드 최종 결제금액이 2만원 이상인 경우에 한해 혜택 적용', '혜택 01. 장 볼 때마다 SSG머니 최대 12% 적립', 'SSG.COM에서 최대 12%', '       스마일클럽으로 5% 적립', '       쓱·새벽·트레이더스 구매 시 (구매 전 스마일클럽 적립 아이콘을 꼭 확인해주세요)', '       SSG.COM 카드 Edition2로 7% 적립', '어디서나 한도없이 0.5%', 'SSG.COM카드 Edition2로 어디서나 한도없이 0.5% 적립 (SSG.COM 외 모든 가맹점)', 'SSG Money 최대 12% 적립', '스마일클럽 5% 적립 + SSG.COM카드 Edition2 최대 7% 적립', '      스마일클럽 5% 적립은 쓱·새벽배송·트레이더스 이용 시에 한함', '      SSG.COM카드 Edition2 최대 7% 적립', '      SSG.COM에서 결제 시 7%(1만 쓱머니 한도), 그 외 가맹점 0.5% 적립(적립한도 제한 없음)', '      무이자 할부 및 현대카드에서 제공하는 다른 할인 서비스 이용 시 적립 제외', '스마일클럽 가입비 3,900원 매월 100% 지원', '      1. 스마일클럽 자동 가입에', '      2. SSGPAY 내 카드 자동 등록', '      3. 스마일클럽 정기결제수단 자동 등록 및 월 이용료 3,900원 지원까지! (단, 해당 카드를 월 정기결제 수단에 등록한 경우에 한함)', 'SSG.COM카드 Edition2를 스마일클럽 월 정기결제 수단에 등록 및 전월 이용금액 30만원 이상 시 혜택 제공', 'TIP. 스마일클럽 가입 시 SSG.COM 혜택', '(SSG 가입 시) 15,000원만 담아도 쓱 · 새벽배송 무료배송', '쓱 · 새벽배송 · 트레이더스 SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '스마일클럽 단독 혜택 스타벅스 상품 전용 딜', '스마일클럽 가입비 매월 3,900원 지원', '월 1회, 매달 스마일클럽 정기결제일에 혜택 제공', 'SSG.COM카드 Edition2는 최초 발급 시, 스마일클럽 월 정기결제 수단에 자동 등록 됨', '전월 이용금액 30만원 미만 시, SSG.COM카드 Edition2로 스마일클럽 정기 결제 금액이 자동 결제됨', '스마일클럽 무료 이용 기간이라면 정기결제 금액 지원 대신 SSG머니 3,900원 제공', '      스타벅스 자동 충전, 생활요금(통신요금, 아파트관리비 등) 정기결제 신청 및 이체 시 최대 1만원 청구 할인', '      2. 스타벅스 자동 충전 또는 생활요금 정기결제 신청(각 항목당 할인한도 5천원, 최대 1만원 할인)', '      이용금액이 혜택금액보다 적을 경우, 이용 금액만큼 할인 적용', '      정기결제 신청 후 카드 결제일에 따라 매출 발생 다음 달 또는 다다음 달 청구 할인 혜택 적용', '      단, 청구 할인 제공 일정은 당사 또는 신청인 사정에 의해 상이할 수 있음', '      3. 쏘카 1만원 할인쿠폰', '      쿠폰은 등록일 포함 30일간 이용 가능', '실물 SSG.COM카드 Edition2 수령 전 SSGPAY로 결제 시 건당 100만원 이하 결제 가능 (단, 본인 확인(신분증 확인 및 1원 인증) 완료한 경우에 한하며, 건당 100만원 초과 시\xa0실물카드 수령 후 결제 가능)', 'SSG머니 최대 적립 12%에서 5%는 SSG.COM에서 제공하는 멤버십 서비스로 SSG.COM 사정에 따라 변경 가능함', '카드 이용대금 연체 시 약정금리 + 연체가산금리 3%의 연체이자율이 적용됩니다. (회원별, 이용 상품별 차등적용 / 법정 최고금리 20% 이내) 단, 연체 발생시점에 약정금리가 없는 경우 아래와 같이 적용', '일시불 : 거래 발생시점 기준 최소 기간 (2개월)의 유이자 할부 약정금리 + 연체가산금리 3%', '무이자할부 : 거래발생시점 기준 동일한 할부 계약 기간의 유이자할부 약정금리 + 연체가산금리 3%']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>더 강력해진 SSG.COM 삼성카드</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>SSG MONEY 최대 15% 적립 + 스마일클럽 월이용료 할인</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000002385&amp;recruitmentPath=SSG</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2022.10.26</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2025.10.25</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '최대 5% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>파크론 4/20(목) 11AM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>파크론 부터 아소방까지 라이브 최대 65%할인</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005341&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[유아동특집] 파크론 최대 65%할인 @SSG.LIVE 4/20(목) 11AM</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2023.03.31</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2023.04.20</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [유아동특집] 파크론 최대 65%할인 @SSG.LIVE 4/20(목) 11AM', '스마일클럽', '[유아동특집] 파크론 최대 65%할인 @SSG.LIVE 4/20(목) 11AM']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>카누 캡슐 커피머신  4/20(목) 7PM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>전문 바리스타의 기술을 그대로, 카누 캡슐 커피머신! 최신상 5만원 즉시할인</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005575&amp;siteNo=6005</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>카누 캡슐 커피머신 @SSG.LIVE 4/20(목) 7PM</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2023.04.12</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2023.04.20</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 카누 캡슐 커피머신 @SSG.LIVE 4/20(목) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>[유아동특집] 탑텐키즈 4/21(금) 11AM</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>간절기 특가 총출동 ~81% OFF 우리아이 래쉬가드세트 9천원대 특급 핫딜까지!</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005449&amp;domainSiteNo=6005</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>[SSG.LIVE]4/21(금) 11AM  탑텐키즈</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2023.04.14</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2023.04.21</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]4/21(금) 11AM  탑텐키즈', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>웨딩 리빙 FESTA</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>가구부터 프리미엄 주방, 침구까지 한번에 득템</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005502</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>웨딩리빙페스타</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2023.04.14</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2023.04.24</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['이벤트/쿠폰 &gt; 웨딩리빙페스타', '스마일클럽', '할인쿠폰 최대 35%', ' 시몬스시몬스 인기상품 비밀 최저가 최대 35% 할인+정품 사은품 증정', ' 알로소소파, 그 이상 Alloso 봄맞이 시즌 소파 최대 15% OFF', '일룸일룸 신혼 맞춤 가구 제안 최대 20만원 쿠폰 혜택', '리바트리바트 혼수 리빙 FESTA 적립/할인 최대 혜택!', '한샘한샘 신혼 공간별 가구 제안 포토 상품평 이벤트', ' 글라스락100% 국내생산 No.1 유리 밀폐용기 남들과는 다른 특별한 신혼살림 글라스락', ' 르크루제르크루제 봄맞이 식기 대전 기간 한정 추가 쿠폰 + 최대 50% OFF', ' 테팔테팔 BEST 모음전 팬/냄비 외 쿡웨어 최대할인', ' 휘슬러휘슬러 쇼핑위크 최대 40% OFF &amp; 일부 품목 15% 쿠폰', ' 클래식패브릭쿨쿨구스 런칭 기념 특가 전 제품 20% OFF', '알레르망 스핑크스알러지프리 원단과 8천개의 핏으로 내몸에 맞춘 침대 해리슨스핑크스 창립 183주년 기념 웨딩리빙 FESTA 초특가할인 기획전 보러가기', '덴비영국 프리미엄 테이블웨어 스프링\xa0페스티벌 최대\xa070%할인\xa0혜택! 기획전 보러가기', '케노샤홈[시몬스] 프리미엄 침구 브랜드 최대 ~29% 즉시할인 ! 기획전 보러가기']</t>
+          <t>['이벤트/쿠폰 &gt; 이달의 맘키즈 PLUS', '스마일클럽', '맘키즈 ~40% 쿠폰상품', '지금 할인 중!', '※ 할인 금액은 상품 별로 상이하니 각 상품페이지를 꼭 참조하세요', '행사대상 상품별 최대 40% 할인', '쿠폰이 적용되지 않는다면?', '맘키즈 에누리  ~40% 상품 상세의 혜택을 꼭 확인하세요!', '앱솔루트 유기농 궁 2 800g (NEO2 쓱배송, 그외지역 택배)', '레고 10698클래식라지조립박스[클래식] 레고 공식 (N2쓱배송, 전국택배가능', '레고 10970 소방서와 헬리콥터   [듀플로] 레고 공식(N2쓱배송, 전국택배가능)']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GH ACTION Headlines Thu Apr 27 00:20:51 UTC 2023
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -577,7 +577,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; Little SSG 어린이날 선물대전', '스마일클럽', '20% 쿠폰', '멤버십 전용 유아동 20% 쿠폰', '선착순 4만장 SmileClub전용 상품쿠폰 20%', '3만원 이상 상품 구매시 최대 7천원 할인, 일부 특가상품 적용 제외, 신세계백화점, 신세계몰, 이마트몰', '쿠폰은 25일 10시에 오픈됩니다.', '선착순 쿠폰 마감 되었습니다. 감사합니다', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[ 미미월드 ] 미리준비하는 어린이날 미미/ 똘똘이/ 뽀로로 외 최대 30%할인', '실바니안패밀리 브레드이발소 산리오 외 세트특가할인', '★어린이날★ 산리오/몰랑 완구 모음전 최대 30%할인', '최대 30% 특가', '[해즈브로] 플레이도 /슈퍼소커/ 마이리틀포니 특가할인', '할인이 쓱쓱 인기 여아캐릭터 완구 모음전 미미월드 토이트론 외', '★쓱세일★ 해즈브로 인기 브랜드 할인모음', '시크릿쥬쥬/ LOL/ 미미 최대 30% 할인', '[쁘띠엘린] 완구 특가 립프로그/젤리캣 할인', '[꼬미마녀라라 외] 인기 신상완구 특가 할인!']</t>
+          <t>['이벤트/쿠폰 &gt; Little SSG 어린이날 선물대전', '스마일클럽', '20% 쿠폰', '멤버십 전용 유아동 20% 쿠폰', '선착순 4만장 SmileClub전용 상품쿠폰 20%', '3만원 이상 상품 구매시 최대 7천원 할인, 일부 특가상품 적용 제외, 신세계백화점, 신세계몰, 이마트몰', '쿠폰은 25일 10시에 오픈됩니다.', '선착순 쿠폰 마감 되었습니다. 감사합니다', '발급 후 [My SSG] &gt; [쿠폰] &gt; [보유쿠폰] 에서 확인 가능합니다.', '[ 미미월드 ] 미리준비하는 어린이날 미미/ 똘똘이/ 뽀로로 외 최대 30%할인', '어린이날 실바니안패밀리 브레드이발소 산리오 외 세트특가할인', '★어린이날★ 산리오/몰랑 완구 모음전 최대 30%할인', '최대 30% 특가', '[해즈브로] 플레이도 3만원 이상 구매시 매트 증정 *소진시 행사종료*', '할인이 쓱쓱 인기 여아캐릭터 완구 모음전 미미월드 토이트론 외', '★쓱세일★ 해즈브로 인기 브랜드 할인모음', '시크릿쥬쥬/ LOL/ 미미 최대 30% 할인', '[쁘띠엘린] 완구 특가 립프로그/젤리캣/하퍼스테이블 할인', '[꼬미마녀라라 외] 인기 신상완구 특가 할인!']</t>
         </is>
       </c>
     </row>
@@ -658,74 +658,74 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>집밥챌린지 - 보양식</t>
+          <t>바이오퍼블릭 기프트 위크</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>나만의 최애 보양식 투표하고 쓱배송으로 보양식 한번에 준비해요!</t>
+          <t>15% 쿠폰으로 건강을 선물하세요!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005330</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005633</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(4/20~26) 집밥챌린지_보양식 편</t>
+          <t>바이오퍼블릭 기프트 위크</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023.04.20</t>
+          <t>2023.04.24</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023.04.26</t>
+          <t>2023.04.30</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; (4/20~26) 집밥챌린지_보양식 편', '스마일클럽', '보양식 재료부터 손쉬운 간편식품까지 쓱배송으로 준비해요!', '        하단 투표 이벤트도 잊지마세요!', '쓱배송으로 보양식']</t>
+          <t>['이벤트/쿠폰 &gt; 바이오퍼블릭 기프트 위크', '스마일클럽', '+카드청구할인', '~15%쿠폰', '50%~, 1+1', '건강식품 ~15%쿠폰', '카드청구할인까지', '선착순  1천명', '장바구니쿠폰', '%', '5만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 사용 기간: 발급 당일', '3만원 이상 구매 시 최대 1만 5천원 할인', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '[SSGPAY전용] 신한카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', 'SSG.COM 삼성카드 [SSGPAY전용] 8만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '국민카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '비씨카드[SSGPAY전용] 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '~15%쿠폰으로 건강 선물하기', '[오쏘몰] 프리미엄 종합 비타민 특별할인 무료배송 및 ~17% OFF!', '[Biopublic]100% 식물성 프로틴 케어 350g(25g*14포)', '[이마트해외직구] 신타6 아이솔레이트 단백질파우더 1.82kg 1+1 모음 , 무료배송 1+1', '50%~,  1+1 득템 찬스', '50%~ 할인 상품', '50% 할인', '[함소아제약 외]건강식품 50%이상 할인된 가격', '[기프트위크](50%할인) 휴럼 건강식품 반값행사', '홍삼정스틱네이처 10mlx28 1세트+쇼핑백 外 50% 할인특가', '50% 할인. 콤비타', '[기프트위크][쓱배송]건강식품 반값행사', '[쏜리서치] 공식판매처! 인기 영양제 1+1 구성 특가! 2/데이,S.A.T 외 무료배송', '[2개 세트][무료배송] 오쏘몰 Orthomol 이뮨 드링크 + 정제 30일분', '[독일직구][무료배송] 오쏘몰 이뮨 30일 1+1 2박스 드링크 정제 멀티비타민 orthomol / 최신제조일자 / 빠른배송 / 독일현지배송', '[최대40%할인] 건강식품 선물하기', '[쓱배송]락티브 비타민 가격할인', '어린이 멀티비타민 유산균 오메가3 백화점 선물세트 [사은품증정이벤트]', '트리플러스50+/90캡슐 x 3개 [사은품증정이벤트]', '[쓱배송]루테인 초특가', '[쓱배송][정관장]홍삼진본 40ml*20포[쇼핑백포함]', '[15% 즉시할인][세노비스] 키즈 멀티비타민미네랄 (1.5g*90정*2통/총90일분) ★미니 멀티비타민 2개 증정★', '[15% 즉시할인][세노비스] 트리플러스 맨 (90캡슐) + 트리플러스 우먼 (90캡슐) (커플세트) ★미니 트리플러스 맨+우먼 증정★', '★139,000→69,500[쓱배송] 휴럼 천년침향환(3.7g*60환)[쇼핑백 동봉]', '★ 레이델 특가상품 모음★ 레이델 폴리코사놀/비즈왁스알코올 셀100  外~ 사은품 + 쿠폰☆', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[무료배송][오쏘몰] 이뮨(immun) 드링크+정제 30일분 3개묶음 / 독일직배송 / 최신제조일자 / 본사 공식', '최대 20%쿠폰  + 청구할인', '~15% 쿠폰가능 + 청구할인', '10%할인 + 쇼핑백증정', '최대 54% 할인', '30% + 5% SSG머니 할인', '1+1특가 + 추가 4% 즉시할인', '2+1 증정 이벤트']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>바이오퍼블릭 기프트 위크</t>
+          <t>SSG.COM 앰배서더 SSG 메이트 모집</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15% 쿠폰으로 건강을 선물하세요!</t>
+          <t>SSG 메이트가 되어 믿고 사는 즐거움을 누려보세요</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005633</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005708</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>바이오퍼블릭 기프트 위크</t>
+          <t>[SSG.COM 앰배서더] SSG 메이트 모집</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023.04.24</t>
+          <t>2023.04.27</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023.04.30</t>
+          <t>2023.05.10</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 바이오퍼블릭 기프트 위크', '스마일클럽', '+카드청구할인', '~15%쿠폰', '50%~, 1+1', '건강식품 ~15%쿠폰', '카드청구할인까지', '선착순  1천명', '장바구니쿠폰', '%', '5만원 이상 구매 시 최대 1만 5천원 할인', '쿠폰 사용 기간: 발급 당일', '3만원 이상 구매 시 최대 1만 5천원 할인', "쿠폰 발급 후'My SSG ▶ 쿠폰 ▶ 보유쿠폰' 에서 확인 가능합니다.", '[SSGPAY전용] 신한카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '[SSGPAY전용] 삼성카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', 'SSG.COM 삼성카드 [SSGPAY전용] 8만원 이상 7% 청구할인 (일 10만원 한) 자세히보기', '국민카드 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '비씨카드[SSGPAY전용] 8만원 이상 5% 청구할인 (일 10만원 한) 자세히보기', '~15%쿠폰으로 건강 선물하기', '[오쏘몰] 프리미엄 종합 비타민 특별할인 무료배송 및 ~17% OFF!', '[Biopublic]100% 식물성 프로틴 케어 350g(25g*14포)', '[이마트해외직구] 신타6 아이솔레이트 단백질파우더 1.82kg 1+1 모음 , 무료배송 1+1', '50%~,  1+1 득템 찬스', '50%~ 할인 상품', '50% 할인', '[함소아제약 외]건강식품 50%이상 할인된 가격', '[기프트위크](50%할인) 휴럼 건강식품 반값행사', '순홍삼(풍기) 50mlx30 1세트+쇼핑백 外 50% 할인특가', '[기프트위크][쓱배송]건강식품 반값행사', '50% 할인. 콤비타', '[쏜리서치] 공식판매처! 인기 영양제 1+1 구성 특가! 2/데이,S.A.T 외 무료배송', '[독일직구][무료배송] 오쏘몰 이뮨 30일 1+1 2박스 드링크 정제 멀티비타민 orthomol / 최신제조일자 / 빠른배송 / 독일현지배송', '[쓱배송]홍삼 기프트 특가', '[최대40%할인] 건강식품 선물하기', '[쓱배송]락티브 비타민 가격할인', '어린이 멀티비타민 유산균 오메가3 백화점 선물세트 [사은품증정이벤트]', '트리플러스50+/90캡슐 x 3개 [사은품증정이벤트]', '[쓱배송]루테인 초특가', '[쓱배송][정관장]홍삼진본 40ml*20포[쇼핑백포함]', '[15% 즉시할인][세노비스] 키즈 멀티비타민미네랄 (1.5g*90정*2통/총90일분) ★미니 멀티비타민 2개 증정★', '[15% 즉시할인][세노비스] 트리플러스 맨 (90캡슐) + 트리플러스 우먼 (90캡슐) (커플세트) ★미니 트리플러스 맨+우먼 증정★', '★139,000→69,500[쓱배송] 휴럼 천년침향환(3.7g*60환)[쇼핑백 동봉]', '★ 레이델 특가상품 모음★ 레이델 폴리코사놀/비즈왁스알코올 셀100  外~ 사은품 + 쿠폰☆', '[쓱배송][종근당건강] 6년근홍삼정업 2개입세트(240g*2병)[쇼핑백 동봉]', '[무료배송][오쏘몰] 이뮨(immun) 드링크+정제 30일분 3개묶음 / 독일직배송 / 최신제조일자 / 본사 공식', '30% + 5% SSG머니할인', '10% 할인 + 쇼핑백증정', '최대 54% 할인', '1+1 특가 + 추가 4% 즉시할인', '2+1 증정 이벤트']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.COM 앰배서더] SSG 메이트 모집', '스마일클럽']</t>
         </is>
       </c>
     </row>
@@ -799,29 +799,29 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '01. 5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '02. 삼성카드 결제일할인 행사일에는 최대 5% 즉시할인', '최대 5% 즉시할인 : [카드혜택가 &gt; SSG.COM 삼성카드 행사 더보기] 내 즉시할인가가 표시된 상품 구매 시 혜택을 받을 수 있습니다. (상품별 할인한도 30,000원)', '삼성카드 결제일할인 행사일에만 적용됩니다.', '삼성카드 할인이 적용된 결제건은 SSG머니 적립 대상에서 제외됩니다.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
+          <t>['이벤트/쿠폰 &gt; SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', '스마일클럽', 'SSG.COM삼성카드 리뉴얼 이벤트 안내 페이지', 'SSG머니 최대 15% 적립', '스마일클럽 월 이용료 3,900원 결제일 할인', '최대 15% SSG머니 적립 중 5%는 SSG.COM에서 제공하는 서비스로 자세한 내용은 SSG.COM 확인바람.', '01. SSG MONEY 최대 15% 적립!', '       이용실적 관계없이 적립 : 1 % + 이용실적 충족 시 적립 4% = 적립 가능한 최대 SSG머니 5%', '       카드혜택 + 스마일클럽 혜택', '       이용실적 관계없이 적립 1% + 이용실적 충족 시 적립 9% + 쓱배송/쓱배송 traders/새벽배송 상품 구매 시 5% = 적립 가능한 최대 SSG머니 15%', '최대 15% SSG MONEY 적립', 'SSG.COM 삼성카드 최대 10% 적립+스마일클럽 5% 적립', 'SSG.COM 삼성카드 최대 10% 적립(1% 적립+9% 추가 적립)', '1% 적립(전월 실적 조건 및 적립한도 없음)', '9% 추가 적립', '삼성카드 할인이 적용된 일시불 및 할부 이용금액은 제외됩니다.', '스마일클럽 5% 적립', '쓱배송/쓱배송 traders/새벽배송 상품 결제건에 한해 혜택을 받을 수 있습니다.', '02. 스마일클럽 월이용료 매월 3,900원 결제일 할인', '15,000원만 담아도 쓱 새벽배송 무료배송(SSG가입시)', '1쓱 새벽배송 트레이더 - SSG머니 최대 5% 적립', '장바구니 최대 10% 할인쿠폰', '스마일클럽 단독 혜택 - 스타벅스 상품 전용 딜', '매월 4장씩 최대 12% 할인쿠폰', '스마일배송 1만 5천원 이상 무제한 무료배송', '스마일배송 상품 스마일캐시 1% 적립', '카드 할인 혜택 자세히보기 (레이어팝업 열기)', '2022.10.26부터, SSG.COM 삼성카드 발급 시 스마일클럽에 자동 가입됩니다.', 'G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우 혜택을 받을 수 없습니다.', 'SSG.COM 삼성카드로 스마일클럽 월 이용료(3,900원) 정기결제 시 혜택이 제공됩니다.(월 1회)', 'SSG.COM을 통한 스마일클럽 가입건에 한해 혜택이 제공됩니다.', '결제금액이 할인금액보다 적을 경우, 결제금액만큼 할인이 적용됩니다.(결제금액이 없는 경우 할인 대상에서 제외)', '5만 6천원 이상 결제 시 사용 가능한 5만 5천원 할인쿠폰 제공', '55,000원 할인쿠폰 - SSGPAY 바로결제 이용 시 사용 가능', '쿠폰 발급기간 : 2023.04.01 ~ 2023.04.30', '쿠폰 사용기간 : 2023.04.01 ~ 2023.04.30', 'SSGPAY 바로결제 이용 이력이 없는 회원', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제해야 쿠폰을 사용할 수 있습니다.', '배송비 등을 제외한 최종 결제금액이 56,000원 이상이여야 쿠폰을 사용할 수 있습니다.', 'SSGPAY 바로결제에 등록된 SSG.COM 삼성카드로 결제하셔야 쿠폰을 사용할 수 있습니다.', '쿠폰은 통합 회원 본인 명의의 SSG.COM 삼성카드로 결제 시 사용 가능하며, 다른 부정적인 방법으로 사용한 경우에는 주문이 취소될 수 있습니다.', '쿠폰은 결제 화면에서 자동으로 적용됩니다.', '결제 화면에서 쿠폰 변경을 원할 경우 ‘쿠폰선택’을 눌러주세요.', '본 상품 발급 및 SSGPAY앱 설치시 바로결제에 자동 등록 됩니다.', 'SSG MONEY는 매월 1일~말일까지 매출전표가 접수된 금액에 대해 다음달 25일 SSG.COM 계정으로 적립됩니다.', '적립된 SSG MONEY는 SSGPAY 회원가입 후 조회 및 사용 가능합니다. 단, SSG.COM 에서는 SSG.COM만 가입해도 사용 가능합니다.', '연체이자율 : 회원별/이용상품별 정상이자율+3.0%p(최고 연 20.0%)', '이미 SSG.COM 삼성카드를 가지고 계시네요!스마일클럽 가입하고 모든 혜택 누리세요', '이미 SSG.COM 삼성카드를 가지고 계시네요!G마켓 또는 옥션을 통해 스마일클럽에 가입한 경우, 월 이용료 결제일할인 혜택을 받을 수 없습니다.', '쿠폰 다운되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.', '이벤트 쿠폰이 이미 발급되었습니다.다운받은 쿠폰은 SSG.COM 삼성카드 발급 후 바로 사용 가능합니다.']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>유세린 4/24(월) 7PM</t>
+          <t>다이슨 에어랩 컴플리트 4/27(목) 7PM</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>흔적케어 UV세럼/톤업 선크림 2만9천원 핫딜!</t>
+          <t>롱배럴(20/40mm) 추가 증정+7만원 적립! 인기컬러 구매 전.고.객. 모두 증정!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005780</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005778</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>유세린@SSG.LIVE 4/27(수) 7:00PM</t>
+          <t>다이슨@SSG.LIVE 4/27(수) 7:00PM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -836,81 +836,81 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 유세린@SSG.LIVE 4/27(수) 7:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 다이슨@SSG.LIVE 4/27(수) 7:00PM', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>사이판 PIC 4/24(월) 8PM</t>
+          <t>사봉 4/27(목) 8PM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>올인원 패키지! 2+2 패밀리팩 51만원대~ 선착순 핫딜</t>
+          <t>방송중에만! 원더오브자스민外 연중 최대할인 &amp; 전구매고객 단독사은품 증정</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005649&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005664&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>노랑풍선 사이판 PIC @SSG.LIVE 4/24(월) 20:00</t>
+          <t>사봉 @SSG.LIVE 4/27(목) 20:00PM</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023.04.14</t>
+          <t>2023.04.17</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023.04.29</t>
+          <t>2023.04.27</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 노랑풍선 사이판 PIC @SSG.LIVE 4/24(월) 20:00', '스마일클럽', '[SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항]', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; 사봉 @SSG.LIVE 4/27(목) 20:00PM', '스마일클럽', '                    \xa0SSG.LIVE 사은품 지급 및 이벤트 혜택 당첨 주의사항', '\xa0- 사은품 지급 및 이벤트 혜택 제공', '\xa0- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>설화수 4/25(화) 7PM</t>
+          <t>[공동판매구역] 맛젤 4/28(금) 11AM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>어버이날 선물 준비완료 + 설화수 지함보 세트 핫딜 선착순 적립금 추가지급</t>
+          <t>제스프리 썬골드키위 시즌 컴백! 핫딜가 19,900원 &amp; 구매 시 스푼 100% 증정</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005742&amp;siteNo=6005</t>
+          <t>https://event.ssg.com/eventDetail.ssg?nevntId=1000000005691&amp;domainSiteNo=6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>설화수 @SSG.LIVE 4/25(화) 7PM</t>
+          <t>[SSG.LIVE]4/28(금) 11AM 제스프리 골드키위</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023.04.19</t>
+          <t>2023.04.20</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023.04.25</t>
+          <t>2023.04.28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; 설화수 @SSG.LIVE 4/25(화) 7PM', '스마일클럽', '이벤트 혜택 당첨 주의사항', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
+          <t>['이벤트/쿠폰 &gt; [SSG.LIVE]4/28(금) 11AM 제스프리 골드키위', '스마일클럽', '- 사은품 지급 및 이벤트 혜택 제공', '- 사은품 지급 및 이벤트 혜택 제공 관련 업무 종료 후 즉시 파기']</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['이벤트/쿠폰 &gt; [4/24~30 ] 럭셔리 더 뷰티 가정의 달 GIFT', '스마일클럽', '15%', '10%', '기획상품10% 할인 전구매 고객 두피세럼 증정', '[시코르 추천] 인기 뷰티템 UP TO 30%', '자연의 작품, 연작   카밍 앤 컴포팅라인 20% 할인 + 쓱단독 사은품 증정', '[몰튼 브라운]SSG 단독 선물포장+UP TO 35%', '예비맘 뷰티루틴, 15%쿠폰&amp;상품권 증정']</t>
+          <t>['이벤트/쿠폰 &gt; [4/24~30 ] 럭셔리 더 뷰티 가정의 달 GIFT', '스마일클럽', '15%', '10%', '기획상품10% 할인 전구매 고객 두피세럼 증정', '[시코르 추천] 인기 뷰티템 UP TO 30%', '자연의 작품, 연작   카밍 앤 컴포팅라인 20% 할인 + 쓱단독 사은품 증정', '[몰튼 브라운]SSG 단독 선물포장+UP TO 35%']</t>
         </is>
       </c>
     </row>

</xml_diff>